<commit_message>
updated CP list from new official guide
</commit_message>
<xml_diff>
--- a/aws-services-crib-sheet.xlsx
+++ b/aws-services-crib-sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corbuno/WorkDocs/courses/aws-services-crib-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4703290F-9C04-0447-836F-91C803BBEDE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E616C40-EC32-974A-B744-AB9BC348FC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23200" yWindow="-23500" windowWidth="38400" windowHeight="23500" xr2:uid="{8DC9DE24-CECC-4748-B90E-52259685D84E}"/>
+    <workbookView xWindow="1000" yWindow="500" windowWidth="27800" windowHeight="17500" xr2:uid="{8DC9DE24-CECC-4748-B90E-52259685D84E}"/>
   </bookViews>
   <sheets>
     <sheet name="AWS Services" sheetId="1" r:id="rId1"/>
@@ -226,9 +226,6 @@
     <t>ElastiCache</t>
   </si>
   <si>
-    <t>EventBridge</t>
-  </si>
-  <si>
     <t>Forecast</t>
   </si>
   <si>
@@ -1013,6 +1010,9 @@
   </si>
   <si>
     <t>Redshift Data Sharing</t>
+  </si>
+  <si>
+    <t>EventBridge (CloudWatch Events)</t>
   </si>
 </sst>
 </file>
@@ -1782,7 +1782,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1808,53 +1808,53 @@
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D1" s="44" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="44" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F1" s="44" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G1" s="50" t="s">
+        <v>165</v>
+      </c>
+      <c r="H1" s="51" t="s">
         <v>166</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="I1" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="J1" s="51" t="s">
+        <v>231</v>
+      </c>
+      <c r="K1" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="I1" s="51" t="s">
-        <v>231</v>
-      </c>
-      <c r="J1" s="51" t="s">
+      <c r="L1" s="52" t="s">
         <v>232</v>
       </c>
-      <c r="K1" s="52" t="s">
+      <c r="M1" s="53" t="s">
+        <v>170</v>
+      </c>
+      <c r="N1" s="53" t="s">
+        <v>233</v>
+      </c>
+      <c r="O1" s="53" t="s">
         <v>168</v>
       </c>
-      <c r="L1" s="52" t="s">
-        <v>233</v>
-      </c>
-      <c r="M1" s="53" t="s">
-        <v>171</v>
-      </c>
-      <c r="N1" s="53" t="s">
+      <c r="P1" s="53" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q1" s="53" t="s">
         <v>234</v>
-      </c>
-      <c r="O1" s="53" t="s">
-        <v>169</v>
-      </c>
-      <c r="P1" s="53" t="s">
-        <v>170</v>
-      </c>
-      <c r="Q1" s="53" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
@@ -1870,7 +1870,9 @@
       <c r="D2" s="45"/>
       <c r="E2" s="45"/>
       <c r="F2" s="45"/>
-      <c r="G2" s="17"/>
+      <c r="G2" s="17">
+        <v>1</v>
+      </c>
       <c r="H2" s="17">
         <v>1</v>
       </c>
@@ -1896,7 +1898,7 @@
         <v>52</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D3" s="45"/>
       <c r="E3" s="45"/>
@@ -1921,7 +1923,7 @@
         <v>52</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D4" s="45"/>
       <c r="E4" s="45"/>
@@ -1952,7 +1954,7 @@
         <v>52</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D5" s="45"/>
       <c r="E5" s="45"/>
@@ -1979,7 +1981,7 @@
         <v>52</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D6" s="45"/>
       <c r="E6" s="45"/>
@@ -2031,7 +2033,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D8" s="45"/>
       <c r="E8" s="45"/>
@@ -2058,7 +2060,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D9" s="45"/>
       <c r="E9" s="45"/>
@@ -2083,7 +2085,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D10" s="45"/>
       <c r="E10" s="45"/>
@@ -2108,7 +2110,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D11" s="45"/>
       <c r="E11" s="45"/>
@@ -2135,7 +2137,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D12" s="45"/>
       <c r="E12" s="45"/>
@@ -2160,7 +2162,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D13" s="45"/>
       <c r="E13" s="45"/>
@@ -2185,12 +2187,14 @@
         <v>52</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D14" s="45"/>
       <c r="E14" s="45"/>
       <c r="F14" s="45"/>
-      <c r="G14" s="17"/>
+      <c r="G14" s="17">
+        <v>1</v>
+      </c>
       <c r="H14" s="17">
         <v>1</v>
       </c>
@@ -2218,12 +2222,14 @@
         <v>52</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D15" s="45"/>
       <c r="E15" s="45"/>
       <c r="F15" s="45"/>
-      <c r="G15" s="17"/>
+      <c r="G15" s="17">
+        <v>1</v>
+      </c>
       <c r="H15" s="17">
         <v>1</v>
       </c>
@@ -2251,12 +2257,14 @@
         <v>52</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D16" s="45"/>
       <c r="E16" s="45"/>
       <c r="F16" s="45"/>
-      <c r="G16" s="17"/>
+      <c r="G16" s="17">
+        <v>1</v>
+      </c>
       <c r="H16" s="17">
         <v>1</v>
       </c>
@@ -2284,7 +2292,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D17" s="45"/>
       <c r="E17" s="45"/>
@@ -2311,7 +2319,7 @@
         <v>52</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D18" s="45"/>
       <c r="E18" s="45"/>
@@ -2338,12 +2346,14 @@
         <v>52</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" s="45"/>
       <c r="E19" s="45"/>
       <c r="F19" s="45"/>
-      <c r="G19" s="17"/>
+      <c r="G19" s="17">
+        <v>1</v>
+      </c>
       <c r="H19" s="17"/>
       <c r="I19" s="17"/>
       <c r="J19" s="17"/>
@@ -2365,12 +2375,14 @@
         <v>52</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" s="45"/>
       <c r="E20" s="45"/>
       <c r="F20" s="45"/>
-      <c r="G20" s="17"/>
+      <c r="G20" s="17">
+        <v>1</v>
+      </c>
       <c r="H20" s="17">
         <v>1</v>
       </c>
@@ -2400,7 +2412,7 @@
         <v>52</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D21" s="45"/>
       <c r="E21" s="45"/>
@@ -2435,7 +2447,7 @@
         <v>52</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D22" s="45"/>
       <c r="E22" s="45"/>
@@ -2470,7 +2482,7 @@
         <v>52</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D23" s="45"/>
       <c r="E23" s="45"/>
@@ -2505,7 +2517,7 @@
         <v>52</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D24" s="45"/>
       <c r="E24" s="45"/>
@@ -2540,7 +2552,7 @@
         <v>52</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D25" s="45"/>
       <c r="E25" s="45"/>
@@ -2569,7 +2581,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>52</v>
@@ -2594,7 +2606,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>6</v>
@@ -2619,18 +2631,20 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>65</v>
+        <v>327</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="45"/>
       <c r="F28" s="45"/>
-      <c r="G28" s="17"/>
+      <c r="G28" s="17">
+        <v>1</v>
+      </c>
       <c r="H28" s="17"/>
       <c r="I28" s="17"/>
       <c r="J28" s="17"/>
@@ -2644,13 +2658,13 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D29" s="45"/>
       <c r="E29" s="45"/>
@@ -2669,13 +2683,13 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B30" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D30" s="45"/>
       <c r="E30" s="45"/>
@@ -2694,13 +2708,13 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B31" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D31" s="45"/>
       <c r="E31" s="45"/>
@@ -2741,13 +2755,13 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D32" s="45"/>
       <c r="E32" s="45"/>
@@ -2788,13 +2802,13 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B33" s="12" t="s">
         <v>52</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D33" s="45"/>
       <c r="E33" s="45"/>
@@ -2813,13 +2827,13 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D34" s="45"/>
       <c r="E34" s="45"/>
@@ -2844,13 +2858,13 @@
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
+        <v>187</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="16" t="s">
         <v>188</v>
-      </c>
-      <c r="B35" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>189</v>
       </c>
       <c r="D35" s="45"/>
       <c r="E35" s="45"/>
@@ -2871,11 +2885,11 @@
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B36" s="38"/>
       <c r="C36" s="39" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D36" s="45"/>
       <c r="E36" s="45"/>
@@ -2894,7 +2908,7 @@
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B37" s="38" t="s">
         <v>6</v>
@@ -2919,7 +2933,7 @@
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B38" s="38" t="s">
         <v>52</v>
@@ -2944,13 +2958,13 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B39" s="38" t="s">
         <v>52</v>
       </c>
       <c r="C39" s="39" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D39" s="45"/>
       <c r="E39" s="45"/>
@@ -2969,13 +2983,13 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B40" s="38" t="s">
         <v>52</v>
       </c>
       <c r="C40" s="39" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D40" s="45"/>
       <c r="E40" s="45"/>
@@ -2994,13 +3008,13 @@
     </row>
     <row r="41" spans="1:17" ht="19" x14ac:dyDescent="0.2">
       <c r="A41" s="37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B41" s="38" t="s">
         <v>52</v>
       </c>
       <c r="C41" s="39" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D41" s="45"/>
       <c r="E41" s="46"/>
@@ -3030,7 +3044,9 @@
       <c r="D42" s="45"/>
       <c r="E42" s="45"/>
       <c r="F42" s="45"/>
-      <c r="G42" s="17"/>
+      <c r="G42" s="17">
+        <v>1</v>
+      </c>
       <c r="H42" s="17">
         <v>1</v>
       </c>
@@ -3056,7 +3072,7 @@
         <v>52</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D43" s="45"/>
       <c r="E43" s="45"/>
@@ -3103,7 +3119,7 @@
         <v>6</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D44" s="45"/>
       <c r="E44" s="45"/>
@@ -3132,7 +3148,7 @@
         <v>52</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D45" s="45"/>
       <c r="E45" s="45"/>
@@ -3226,12 +3242,14 @@
         <v>52</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D47" s="45"/>
       <c r="E47" s="45"/>
       <c r="F47" s="45"/>
-      <c r="G47" s="17"/>
+      <c r="G47" s="17">
+        <v>1</v>
+      </c>
       <c r="H47" s="17"/>
       <c r="I47" s="17"/>
       <c r="J47" s="17"/>
@@ -3282,7 +3300,7 @@
         <v>6</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D49" s="45"/>
       <c r="E49" s="45"/>
@@ -3330,7 +3348,7 @@
         <v>6</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D51" s="45"/>
       <c r="E51" s="45"/>
@@ -3349,13 +3367,13 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B52" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D52" s="45"/>
       <c r="E52" s="45"/>
@@ -3374,13 +3392,13 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B53" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D53" s="45"/>
       <c r="E53" s="45"/>
@@ -3399,11 +3417,11 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B54" s="15"/>
       <c r="C54" s="16" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D54" s="45"/>
       <c r="E54" s="45"/>
@@ -3422,13 +3440,13 @@
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B55" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="B55" s="15" t="s">
+      <c r="C55" s="16" t="s">
         <v>174</v>
-      </c>
-      <c r="C55" s="16" t="s">
-        <v>175</v>
       </c>
       <c r="D55" s="45"/>
       <c r="E55" s="45"/>
@@ -3447,20 +3465,18 @@
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B56" s="15" t="s">
         <v>52</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D56" s="45"/>
       <c r="E56" s="45"/>
       <c r="F56" s="45"/>
-      <c r="G56" s="17">
-        <v>1</v>
-      </c>
+      <c r="G56" s="17"/>
       <c r="H56" s="17">
         <v>1</v>
       </c>
@@ -3484,13 +3500,13 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B57" s="15" t="s">
         <v>52</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D57" s="45"/>
       <c r="E57" s="45"/>
@@ -3521,13 +3537,13 @@
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B58" s="15" t="s">
         <v>52</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D58" s="45"/>
       <c r="E58" s="45"/>
@@ -3558,7 +3574,7 @@
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B59" s="15" t="s">
         <v>6</v>
@@ -3595,13 +3611,13 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B60" s="15" t="s">
         <v>52</v>
       </c>
       <c r="C60" s="16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D60" s="45"/>
       <c r="E60" s="45"/>
@@ -3620,7 +3636,7 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B61" s="15" t="s">
         <v>6</v>
@@ -3645,11 +3661,11 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B62" s="15"/>
       <c r="C62" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D62" s="45"/>
       <c r="E62" s="45"/>
@@ -3668,7 +3684,7 @@
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B63" s="12" t="s">
         <v>6</v>
@@ -3695,18 +3711,20 @@
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B64" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D64" s="45"/>
       <c r="E64" s="45"/>
       <c r="F64" s="45"/>
-      <c r="G64" s="17"/>
+      <c r="G64" s="17">
+        <v>1</v>
+      </c>
       <c r="H64" s="17"/>
       <c r="I64" s="17"/>
       <c r="J64" s="17"/>
@@ -3720,13 +3738,13 @@
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" s="11" t="s">
+        <v>183</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" s="13" t="s">
         <v>184</v>
-      </c>
-      <c r="B65" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C65" s="13" t="s">
-        <v>185</v>
       </c>
       <c r="D65" s="45"/>
       <c r="E65" s="45"/>
@@ -3747,13 +3765,13 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B66" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C66" s="13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D66" s="45"/>
       <c r="E66" s="45"/>
@@ -3774,11 +3792,11 @@
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B67" s="12"/>
       <c r="C67" s="13" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D67" s="45"/>
       <c r="E67" s="45"/>
@@ -3803,13 +3821,13 @@
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B68" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C68" s="21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D68" s="45"/>
       <c r="E68" s="45"/>
@@ -3828,7 +3846,7 @@
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B69" s="20" t="s">
         <v>6</v>
@@ -3853,18 +3871,20 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B70" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C70" s="21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D70" s="45"/>
       <c r="E70" s="45"/>
       <c r="F70" s="45"/>
-      <c r="G70" s="17"/>
+      <c r="G70" s="17">
+        <v>1</v>
+      </c>
       <c r="H70" s="17"/>
       <c r="I70" s="17"/>
       <c r="J70" s="17"/>
@@ -3878,7 +3898,7 @@
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B71" s="20" t="s">
         <v>6</v>
@@ -3905,13 +3925,13 @@
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B72" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C72" s="21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D72" s="45"/>
       <c r="E72" s="45"/>
@@ -3930,7 +3950,7 @@
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B73" s="20" t="s">
         <v>6</v>
@@ -3957,13 +3977,13 @@
     </row>
     <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B74" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C74" s="21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D74" s="45"/>
       <c r="E74" s="45"/>
@@ -3982,7 +4002,7 @@
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B75" s="20" t="s">
         <v>52</v>
@@ -3993,7 +4013,9 @@
       <c r="D75" s="45"/>
       <c r="E75" s="45"/>
       <c r="F75" s="45"/>
-      <c r="G75" s="17"/>
+      <c r="G75" s="17">
+        <v>1</v>
+      </c>
       <c r="H75" s="17"/>
       <c r="I75" s="17"/>
       <c r="J75" s="17"/>
@@ -4007,13 +4029,13 @@
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B76" s="20" t="s">
         <v>52</v>
       </c>
       <c r="C76" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D76" s="45"/>
       <c r="E76" s="45"/>
@@ -4032,13 +4054,13 @@
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B77" s="20" t="s">
         <v>52</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D77" s="45"/>
       <c r="E77" s="45"/>
@@ -4102,7 +4124,7 @@
         <v>52</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D79" s="45"/>
       <c r="E79" s="45"/>
@@ -4215,7 +4237,7 @@
         <v>52</v>
       </c>
       <c r="C82" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D82" s="45"/>
       <c r="E82" s="45"/>
@@ -4242,7 +4264,7 @@
         <v>52</v>
       </c>
       <c r="C83" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D83" s="45"/>
       <c r="E83" s="45"/>
@@ -4271,7 +4293,7 @@
         <v>52</v>
       </c>
       <c r="C84" s="21" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D84" s="45"/>
       <c r="E84" s="45"/>
@@ -4300,7 +4322,7 @@
         <v>52</v>
       </c>
       <c r="C85" s="21" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D85" s="45"/>
       <c r="E85" s="45"/>
@@ -4325,7 +4347,7 @@
         <v>52</v>
       </c>
       <c r="C86" s="21" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D86" s="45"/>
       <c r="E86" s="45"/>
@@ -4358,7 +4380,7 @@
         <v>52</v>
       </c>
       <c r="C87" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D87" s="45"/>
       <c r="E87" s="45"/>
@@ -4379,7 +4401,7 @@
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A88" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B88" s="20" t="s">
         <v>6</v>
@@ -4404,13 +4426,13 @@
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B89" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C89" s="21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D89" s="45"/>
       <c r="E89" s="45"/>
@@ -4429,7 +4451,7 @@
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A90" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B90" s="20" t="s">
         <v>6</v>
@@ -4454,13 +4476,13 @@
     </row>
     <row r="91" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A91" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B91" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C91" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D91" s="45"/>
       <c r="E91" s="45"/>
@@ -4479,7 +4501,7 @@
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A92" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B92" s="20" t="s">
         <v>6</v>
@@ -4504,7 +4526,7 @@
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A93" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B93" s="20" t="s">
         <v>6</v>
@@ -4515,7 +4537,9 @@
       <c r="D93" s="45"/>
       <c r="E93" s="45"/>
       <c r="F93" s="45"/>
-      <c r="G93" s="17"/>
+      <c r="G93" s="17">
+        <v>1</v>
+      </c>
       <c r="H93" s="17"/>
       <c r="I93" s="17">
         <v>1</v>
@@ -4531,7 +4555,7 @@
     </row>
     <row r="94" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A94" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B94" s="20" t="s">
         <v>6</v>
@@ -4542,7 +4566,9 @@
       <c r="D94" s="45"/>
       <c r="E94" s="45"/>
       <c r="F94" s="45"/>
-      <c r="G94" s="17"/>
+      <c r="G94" s="17">
+        <v>1</v>
+      </c>
       <c r="H94" s="17"/>
       <c r="I94" s="17">
         <v>1</v>
@@ -4558,7 +4584,7 @@
     </row>
     <row r="95" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A95" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B95" s="20" t="s">
         <v>6</v>
@@ -4569,7 +4595,9 @@
       <c r="D95" s="45"/>
       <c r="E95" s="45"/>
       <c r="F95" s="45"/>
-      <c r="G95" s="17"/>
+      <c r="G95" s="17">
+        <v>1</v>
+      </c>
       <c r="H95" s="17"/>
       <c r="I95" s="17">
         <v>1</v>
@@ -4585,7 +4613,7 @@
     </row>
     <row r="96" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A96" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B96" s="20" t="s">
         <v>52</v>
@@ -4610,7 +4638,7 @@
     </row>
     <row r="97" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A97" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B97" s="20" t="s">
         <v>6</v>
@@ -4621,7 +4649,9 @@
       <c r="D97" s="45"/>
       <c r="E97" s="45"/>
       <c r="F97" s="45"/>
-      <c r="G97" s="17"/>
+      <c r="G97" s="17">
+        <v>1</v>
+      </c>
       <c r="H97" s="17"/>
       <c r="I97" s="17">
         <v>1</v>
@@ -4637,7 +4667,7 @@
     </row>
     <row r="98" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A98" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B98" s="20" t="s">
         <v>6</v>
@@ -4648,7 +4678,9 @@
       <c r="D98" s="45"/>
       <c r="E98" s="45"/>
       <c r="F98" s="45"/>
-      <c r="G98" s="17"/>
+      <c r="G98" s="17">
+        <v>1</v>
+      </c>
       <c r="H98" s="17"/>
       <c r="I98" s="17"/>
       <c r="J98" s="17"/>
@@ -4662,13 +4694,13 @@
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A99" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B99" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D99" s="45"/>
       <c r="E99" s="45"/>
@@ -4689,13 +4721,13 @@
     </row>
     <row r="100" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A100" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="B100" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C100" s="21" t="s">
         <v>215</v>
-      </c>
-      <c r="B100" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C100" s="21" t="s">
-        <v>216</v>
       </c>
       <c r="D100" s="45"/>
       <c r="E100" s="45"/>
@@ -4714,13 +4746,13 @@
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A101" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B101" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C101" s="21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D101" s="45"/>
       <c r="E101" s="45"/>
@@ -4739,13 +4771,13 @@
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A102" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B102" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C102" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D102" s="45"/>
       <c r="E102" s="45"/>
@@ -4764,13 +4796,13 @@
     </row>
     <row r="103" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A103" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B103" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C103" s="21" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D103" s="45"/>
       <c r="E103" s="45"/>
@@ -4789,13 +4821,13 @@
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A104" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B104" s="20" t="s">
         <v>52</v>
       </c>
       <c r="C104" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D104" s="45"/>
       <c r="E104" s="45"/>
@@ -4814,13 +4846,13 @@
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A105" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B105" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C105" s="21" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D105" s="45"/>
       <c r="E105" s="45"/>
@@ -4839,13 +4871,13 @@
     </row>
     <row r="106" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A106" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B106" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C106" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D106" s="45"/>
       <c r="E106" s="45"/>
@@ -4864,7 +4896,7 @@
     </row>
     <row r="107" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A107" s="19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B107" s="20" t="s">
         <v>6</v>
@@ -4891,13 +4923,13 @@
     </row>
     <row r="108" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A108" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="B108" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C108" s="22" t="s">
         <v>222</v>
-      </c>
-      <c r="B108" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C108" s="22" t="s">
-        <v>223</v>
       </c>
       <c r="D108" s="45"/>
       <c r="E108" s="45"/>
@@ -4916,13 +4948,13 @@
     </row>
     <row r="109" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A109" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B109" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C109" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D109" s="45"/>
       <c r="E109" s="45"/>
@@ -4941,18 +4973,20 @@
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B110" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C110" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D110" s="45"/>
       <c r="E110" s="45"/>
       <c r="F110" s="45"/>
-      <c r="G110" s="17"/>
+      <c r="G110" s="17">
+        <v>1</v>
+      </c>
       <c r="H110" s="17"/>
       <c r="I110" s="17"/>
       <c r="J110" s="17"/>
@@ -4966,13 +5000,13 @@
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A111" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B111" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C111" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D111" s="45"/>
       <c r="E111" s="45"/>
@@ -4991,13 +5025,13 @@
     </row>
     <row r="112" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A112" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B112" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C112" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D112" s="45"/>
       <c r="E112" s="45"/>
@@ -5016,13 +5050,13 @@
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A113" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B113" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D113" s="45"/>
       <c r="E113" s="45"/>
@@ -5070,7 +5104,7 @@
         <v>6</v>
       </c>
       <c r="C115" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D115" s="45"/>
       <c r="E115" s="45"/>
@@ -5095,7 +5129,7 @@
         <v>6</v>
       </c>
       <c r="C116" s="27" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D116" s="45"/>
       <c r="E116" s="45"/>
@@ -5120,7 +5154,7 @@
         <v>6</v>
       </c>
       <c r="C117" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D117" s="45"/>
       <c r="E117" s="45"/>
@@ -5145,7 +5179,7 @@
         <v>6</v>
       </c>
       <c r="C118" s="27" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D118" s="45"/>
       <c r="E118" s="45"/>
@@ -5170,7 +5204,7 @@
         <v>6</v>
       </c>
       <c r="C119" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D119" s="45"/>
       <c r="E119" s="45"/>
@@ -5195,7 +5229,7 @@
         <v>6</v>
       </c>
       <c r="C120" s="27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D120" s="45"/>
       <c r="E120" s="45"/>
@@ -5220,7 +5254,7 @@
         <v>6</v>
       </c>
       <c r="C121" s="27" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D121" s="45"/>
       <c r="E121" s="45"/>
@@ -5245,7 +5279,7 @@
         <v>6</v>
       </c>
       <c r="C122" s="27" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D122" s="45"/>
       <c r="E122" s="45"/>
@@ -5270,7 +5304,7 @@
         <v>6</v>
       </c>
       <c r="C123" s="27" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D123" s="45"/>
       <c r="E123" s="45"/>
@@ -5295,7 +5329,7 @@
         <v>52</v>
       </c>
       <c r="C124" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D124" s="45"/>
       <c r="E124" s="45"/>
@@ -5314,13 +5348,13 @@
     </row>
     <row r="125" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A125" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B125" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C125" s="24" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D125" s="45"/>
       <c r="E125" s="45"/>
@@ -5341,7 +5375,7 @@
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A126" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B126" s="23" t="s">
         <v>52</v>
@@ -5368,13 +5402,13 @@
     </row>
     <row r="127" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A127" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B127" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C127" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D127" s="45"/>
       <c r="E127" s="45"/>
@@ -5395,13 +5429,13 @@
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A128" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B128" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C128" s="24" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D128" s="45"/>
       <c r="E128" s="45"/>
@@ -5422,13 +5456,13 @@
     </row>
     <row r="129" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A129" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B129" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C129" s="24" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D129" s="45"/>
       <c r="E129" s="45"/>
@@ -5447,13 +5481,13 @@
     </row>
     <row r="130" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A130" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B130" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C130" s="24" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D130" s="45"/>
       <c r="E130" s="45"/>
@@ -5472,13 +5506,13 @@
     </row>
     <row r="131" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A131" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B131" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C131" s="24" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D131" s="45"/>
       <c r="E131" s="45"/>
@@ -5497,13 +5531,13 @@
     </row>
     <row r="132" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A132" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B132" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C132" s="24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D132" s="45"/>
       <c r="E132" s="45"/>
@@ -5524,13 +5558,13 @@
     </row>
     <row r="133" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A133" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B133" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C133" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D133" s="45"/>
       <c r="E133" s="45"/>
@@ -5551,13 +5585,13 @@
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A134" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B134" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C134" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D134" s="45"/>
       <c r="E134" s="45"/>
@@ -5578,13 +5612,13 @@
     </row>
     <row r="135" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A135" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B135" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C135" s="24" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D135" s="45"/>
       <c r="E135" s="45"/>
@@ -5605,13 +5639,13 @@
     </row>
     <row r="136" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A136" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B136" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C136" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D136" s="45"/>
       <c r="E136" s="45"/>
@@ -5630,13 +5664,13 @@
     </row>
     <row r="137" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A137" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B137" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C137" s="24" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D137" s="45"/>
       <c r="E137" s="45"/>
@@ -5655,13 +5689,13 @@
     </row>
     <row r="138" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A138" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B138" s="23" t="s">
         <v>6</v>
       </c>
       <c r="C138" s="24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D138" s="45"/>
       <c r="E138" s="45"/>
@@ -5680,13 +5714,13 @@
     </row>
     <row r="139" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A139" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B139" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C139" s="24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D139" s="45"/>
       <c r="E139" s="45"/>
@@ -5707,13 +5741,13 @@
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A140" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B140" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C140" s="24" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D140" s="45"/>
       <c r="E140" s="45"/>
@@ -5734,13 +5768,13 @@
     </row>
     <row r="141" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A141" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B141" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C141" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D141" s="45"/>
       <c r="E141" s="45"/>
@@ -5761,13 +5795,13 @@
     </row>
     <row r="142" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A142" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B142" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C142" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D142" s="45"/>
       <c r="E142" s="45"/>
@@ -5788,13 +5822,13 @@
     </row>
     <row r="143" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A143" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B143" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C143" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D143" s="45"/>
       <c r="E143" s="45"/>
@@ -5815,13 +5849,13 @@
     </row>
     <row r="144" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A144" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B144" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C144" s="24" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D144" s="45"/>
       <c r="E144" s="45"/>
@@ -5842,13 +5876,13 @@
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A145" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B145" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C145" s="24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D145" s="45"/>
       <c r="E145" s="45"/>
@@ -5869,13 +5903,13 @@
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A146" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B146" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C146" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D146" s="45"/>
       <c r="E146" s="45"/>
@@ -5896,13 +5930,13 @@
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A147" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B147" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C147" s="24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D147" s="45"/>
       <c r="E147" s="45"/>
@@ -5923,13 +5957,13 @@
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A148" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B148" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C148" s="24" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D148" s="45"/>
       <c r="E148" s="45"/>
@@ -5950,13 +5984,13 @@
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A149" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B149" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C149" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D149" s="45"/>
       <c r="E149" s="45"/>
@@ -5977,13 +6011,13 @@
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A150" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B150" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C150" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D150" s="45"/>
       <c r="E150" s="45"/>
@@ -6004,13 +6038,13 @@
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A151" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B151" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C151" s="24" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D151" s="45"/>
       <c r="E151" s="45"/>
@@ -6031,13 +6065,13 @@
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A152" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B152" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C152" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D152" s="45"/>
       <c r="E152" s="45"/>
@@ -6058,13 +6092,13 @@
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A153" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B153" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C153" s="24" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D153" s="45"/>
       <c r="E153" s="45"/>
@@ -6085,13 +6119,13 @@
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A154" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B154" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C154" s="24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D154" s="45"/>
       <c r="E154" s="45"/>
@@ -6112,13 +6146,13 @@
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A155" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B155" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C155" s="24" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D155" s="45"/>
       <c r="E155" s="45"/>
@@ -6139,13 +6173,13 @@
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A156" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B156" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C156" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D156" s="45"/>
       <c r="E156" s="45"/>
@@ -6166,13 +6200,13 @@
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A157" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B157" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C157" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D157" s="45"/>
       <c r="E157" s="45"/>
@@ -6193,13 +6227,13 @@
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A158" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B158" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C158" s="24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D158" s="45"/>
       <c r="E158" s="45"/>
@@ -6220,13 +6254,13 @@
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A159" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B159" s="23" t="s">
         <v>52</v>
       </c>
       <c r="C159" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D159" s="45"/>
       <c r="E159" s="45"/>
@@ -6253,12 +6287,14 @@
         <v>6</v>
       </c>
       <c r="C160" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D160" s="45"/>
       <c r="E160" s="45"/>
       <c r="F160" s="45"/>
-      <c r="G160" s="17"/>
+      <c r="G160" s="17">
+        <v>1</v>
+      </c>
       <c r="H160" s="17">
         <v>1</v>
       </c>
@@ -6287,7 +6323,9 @@
       <c r="D161" s="45"/>
       <c r="E161" s="45"/>
       <c r="F161" s="45"/>
-      <c r="G161" s="17"/>
+      <c r="G161" s="17">
+        <v>1</v>
+      </c>
       <c r="H161" s="17"/>
       <c r="I161" s="17"/>
       <c r="J161" s="17"/>
@@ -6436,7 +6474,7 @@
         <v>6</v>
       </c>
       <c r="C165" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D165" s="45"/>
       <c r="E165" s="45"/>
@@ -6466,7 +6504,9 @@
       <c r="D166" s="45"/>
       <c r="E166" s="45"/>
       <c r="F166" s="45"/>
-      <c r="G166" s="17"/>
+      <c r="G166" s="17">
+        <v>1</v>
+      </c>
       <c r="H166" s="17">
         <v>1</v>
       </c>
@@ -6490,7 +6530,7 @@
         <v>6</v>
       </c>
       <c r="C167" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D167" s="45"/>
       <c r="E167" s="45"/>
@@ -6515,7 +6555,7 @@
         <v>6</v>
       </c>
       <c r="C168" s="31" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D168" s="45"/>
       <c r="E168" s="45"/>
@@ -6540,12 +6580,14 @@
         <v>6</v>
       </c>
       <c r="C169" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D169" s="45"/>
       <c r="E169" s="45"/>
       <c r="F169" s="45"/>
-      <c r="G169" s="17"/>
+      <c r="G169" s="17">
+        <v>1</v>
+      </c>
       <c r="H169" s="17"/>
       <c r="I169" s="17"/>
       <c r="J169" s="17"/>
@@ -6565,7 +6607,7 @@
         <v>52</v>
       </c>
       <c r="C170" s="31" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D170" s="45"/>
       <c r="E170" s="45"/>
@@ -6590,7 +6632,7 @@
         <v>6</v>
       </c>
       <c r="C171" s="31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D171" s="45"/>
       <c r="E171" s="45"/>
@@ -6617,7 +6659,7 @@
         <v>6</v>
       </c>
       <c r="C172" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D172" s="45"/>
       <c r="E172" s="45"/>
@@ -6648,7 +6690,7 @@
         <v>6</v>
       </c>
       <c r="C173" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D173" s="45"/>
       <c r="E173" s="45"/>
@@ -6679,7 +6721,7 @@
         <v>6</v>
       </c>
       <c r="C174" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D174" s="45"/>
       <c r="E174" s="45"/>
@@ -6741,7 +6783,7 @@
         <v>6</v>
       </c>
       <c r="C176" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D176" s="45"/>
       <c r="E176" s="45"/>
@@ -6768,7 +6810,7 @@
         <v>6</v>
       </c>
       <c r="C177" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D177" s="45"/>
       <c r="E177" s="45"/>
@@ -6793,7 +6835,7 @@
         <v>6</v>
       </c>
       <c r="C178" s="31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D178" s="45"/>
       <c r="E178" s="45"/>
@@ -6824,7 +6866,7 @@
         <v>6</v>
       </c>
       <c r="C179" s="31" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D179" s="45"/>
       <c r="E179" s="45"/>
@@ -6853,7 +6895,7 @@
         <v>6</v>
       </c>
       <c r="C180" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D180" s="45"/>
       <c r="E180" s="45"/>
@@ -6882,7 +6924,7 @@
         <v>6</v>
       </c>
       <c r="C181" s="31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D181" s="45"/>
       <c r="E181" s="45"/>
@@ -6911,7 +6953,7 @@
         <v>6</v>
       </c>
       <c r="C182" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D182" s="45"/>
       <c r="E182" s="45"/>
@@ -6940,7 +6982,7 @@
         <v>6</v>
       </c>
       <c r="C183" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D183" s="45"/>
       <c r="E183" s="45"/>
@@ -6969,7 +7011,7 @@
         <v>6</v>
       </c>
       <c r="C184" s="31" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D184" s="45"/>
       <c r="E184" s="45"/>
@@ -6998,7 +7040,7 @@
         <v>6</v>
       </c>
       <c r="C185" s="31" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D185" s="45"/>
       <c r="E185" s="45"/>
@@ -7027,7 +7069,7 @@
         <v>6</v>
       </c>
       <c r="C186" s="31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D186" s="45"/>
       <c r="E186" s="45"/>
@@ -7056,7 +7098,7 @@
         <v>6</v>
       </c>
       <c r="C187" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D187" s="45"/>
       <c r="E187" s="45"/>
@@ -7085,7 +7127,7 @@
         <v>6</v>
       </c>
       <c r="C188" s="31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D188" s="45"/>
       <c r="E188" s="45"/>
@@ -7114,7 +7156,7 @@
         <v>6</v>
       </c>
       <c r="C189" s="31" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D189" s="47"/>
       <c r="E189" s="47"/>
@@ -7143,13 +7185,17 @@
         <v>6</v>
       </c>
       <c r="C190" s="31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D190" s="45"/>
       <c r="E190" s="45"/>
       <c r="F190" s="45"/>
-      <c r="G190" s="17"/>
-      <c r="H190" s="17"/>
+      <c r="G190" s="17">
+        <v>1</v>
+      </c>
+      <c r="H190" s="17">
+        <v>1</v>
+      </c>
       <c r="I190" s="17"/>
       <c r="J190" s="17">
         <v>1</v>
@@ -7172,7 +7218,7 @@
         <v>6</v>
       </c>
       <c r="C191" s="31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D191" s="45"/>
       <c r="E191" s="45"/>
@@ -7201,7 +7247,7 @@
         <v>6</v>
       </c>
       <c r="C192" s="31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D192" s="45"/>
       <c r="E192" s="45"/>
@@ -7230,7 +7276,7 @@
         <v>6</v>
       </c>
       <c r="C193" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D193" s="45"/>
       <c r="E193" s="45"/>
@@ -7259,7 +7305,7 @@
         <v>6</v>
       </c>
       <c r="C194" s="31" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D194" s="45"/>
       <c r="E194" s="45"/>
@@ -7288,12 +7334,14 @@
         <v>6</v>
       </c>
       <c r="C195" s="31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D195" s="45"/>
       <c r="E195" s="45"/>
       <c r="F195" s="45"/>
-      <c r="G195" s="17"/>
+      <c r="G195" s="17">
+        <v>1</v>
+      </c>
       <c r="H195" s="17">
         <v>1</v>
       </c>
@@ -7323,7 +7371,7 @@
         <v>6</v>
       </c>
       <c r="C196" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D196" s="45"/>
       <c r="E196" s="45"/>
@@ -7350,7 +7398,7 @@
         <v>6</v>
       </c>
       <c r="C197" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D197" s="45"/>
       <c r="E197" s="45"/>
@@ -7369,13 +7417,13 @@
     </row>
     <row r="198" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A198" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B198" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C198" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D198" s="45"/>
       <c r="E198" s="45"/>
@@ -7394,13 +7442,13 @@
     </row>
     <row r="199" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A199" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B199" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C199" s="16" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D199" s="45"/>
       <c r="E199" s="45"/>
@@ -7419,13 +7467,13 @@
     </row>
     <row r="200" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A200" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B200" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C200" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D200" s="45"/>
       <c r="E200" s="45"/>
@@ -7444,13 +7492,13 @@
     </row>
     <row r="201" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A201" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B201" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C201" s="16" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D201" s="45"/>
       <c r="E201" s="45"/>
@@ -7469,13 +7517,13 @@
     </row>
     <row r="202" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A202" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B202" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C202" s="16" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D202" s="45"/>
       <c r="E202" s="45"/>
@@ -7494,13 +7542,13 @@
     </row>
     <row r="203" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A203" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B203" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C203" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D203" s="45"/>
       <c r="E203" s="45"/>
@@ -7519,13 +7567,13 @@
     </row>
     <row r="204" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A204" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B204" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C204" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D204" s="45"/>
       <c r="E204" s="45"/>
@@ -7544,13 +7592,13 @@
     </row>
     <row r="205" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A205" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B205" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C205" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D205" s="45"/>
       <c r="E205" s="45"/>
@@ -7569,13 +7617,13 @@
     </row>
     <row r="206" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A206" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B206" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C206" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D206" s="45"/>
       <c r="E206" s="45"/>
@@ -7594,13 +7642,13 @@
     </row>
     <row r="207" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A207" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B207" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C207" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D207" s="45"/>
       <c r="E207" s="45"/>
@@ -7619,13 +7667,13 @@
     </row>
     <row r="208" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A208" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B208" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C208" s="16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D208" s="45"/>
       <c r="E208" s="45"/>
@@ -7644,13 +7692,13 @@
     </row>
     <row r="209" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A209" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B209" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C209" s="16" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D209" s="45"/>
       <c r="E209" s="45"/>
@@ -7669,13 +7717,13 @@
     </row>
     <row r="210" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A210" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B210" s="15" t="s">
         <v>52</v>
       </c>
       <c r="C210" s="16" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D210" s="45"/>
       <c r="E210" s="45"/>
@@ -7694,13 +7742,13 @@
     </row>
     <row r="211" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A211" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B211" s="15" t="s">
         <v>52</v>
       </c>
       <c r="C211" s="16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D211" s="45"/>
       <c r="E211" s="45"/>
@@ -7721,13 +7769,13 @@
     </row>
     <row r="212" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A212" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="B212" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C212" s="16" t="s">
         <v>294</v>
-      </c>
-      <c r="B212" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C212" s="16" t="s">
-        <v>295</v>
       </c>
       <c r="D212" s="45"/>
       <c r="E212" s="45"/>
@@ -7746,13 +7794,13 @@
     </row>
     <row r="213" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A213" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B213" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C213" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D213" s="45"/>
       <c r="E213" s="45"/>
@@ -7771,13 +7819,13 @@
     </row>
     <row r="214" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A214" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B214" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C214" s="16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D214" s="45"/>
       <c r="E214" s="45"/>
@@ -7796,13 +7844,13 @@
     </row>
     <row r="215" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A215" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B215" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C215" s="16" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D215" s="45"/>
       <c r="E215" s="45"/>
@@ -7821,13 +7869,13 @@
     </row>
     <row r="216" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A216" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B216" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C216" s="16" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D216" s="45"/>
       <c r="E216" s="45"/>
@@ -7846,13 +7894,13 @@
     </row>
     <row r="217" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A217" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B217" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C217" s="16" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D217" s="45"/>
       <c r="E217" s="45"/>
@@ -7871,13 +7919,13 @@
     </row>
     <row r="218" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A218" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B218" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C218" s="16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D218" s="45"/>
       <c r="E218" s="45"/>
@@ -7902,7 +7950,7 @@
         <v>6</v>
       </c>
       <c r="C219" s="24" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D219" s="45"/>
       <c r="E219" s="45"/>
@@ -7950,7 +7998,7 @@
         <v>6</v>
       </c>
       <c r="C221" s="24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D221" s="45"/>
       <c r="E221" s="45"/>
@@ -7975,7 +8023,7 @@
         <v>6</v>
       </c>
       <c r="C222" s="24" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D222" s="45"/>
       <c r="E222" s="45"/>
@@ -8004,7 +8052,7 @@
         <v>6</v>
       </c>
       <c r="C223" s="24" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D223" s="45"/>
       <c r="E223" s="45"/>
@@ -8064,7 +8112,7 @@
         <v>6</v>
       </c>
       <c r="C225" s="24" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D225" s="45"/>
       <c r="E225" s="45"/>
@@ -8095,7 +8143,7 @@
       </c>
       <c r="B226" s="23"/>
       <c r="C226" s="24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D226" s="45"/>
       <c r="E226" s="45"/>
@@ -8120,7 +8168,7 @@
         <v>6</v>
       </c>
       <c r="C227" s="24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D227" s="45"/>
       <c r="E227" s="45"/>
@@ -8145,7 +8193,7 @@
         <v>6</v>
       </c>
       <c r="C228" s="24" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D228" s="45"/>
       <c r="E228" s="45"/>
@@ -8203,7 +8251,7 @@
         <v>6</v>
       </c>
       <c r="C230" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D230" s="45"/>
       <c r="E230" s="45"/>
@@ -8261,7 +8309,7 @@
         <v>6</v>
       </c>
       <c r="C232" s="24" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D232" s="45"/>
       <c r="E232" s="45"/>
@@ -8280,18 +8328,20 @@
     </row>
     <row r="233" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A233" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B233" s="34" t="s">
         <v>52</v>
       </c>
       <c r="C233" s="35" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D233" s="45"/>
       <c r="E233" s="45"/>
       <c r="F233" s="45"/>
-      <c r="G233" s="17"/>
+      <c r="G233" s="17">
+        <v>1</v>
+      </c>
       <c r="H233" s="17">
         <v>1</v>
       </c>
@@ -8319,13 +8369,13 @@
     </row>
     <row r="234" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A234" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B234" s="34" t="s">
         <v>6</v>
       </c>
       <c r="C234" s="35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D234" s="45"/>
       <c r="E234" s="45"/>
@@ -8346,13 +8396,13 @@
     </row>
     <row r="235" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A235" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B235" s="34" t="s">
         <v>6</v>
       </c>
       <c r="C235" s="35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D235" s="45"/>
       <c r="E235" s="45"/>
@@ -8373,7 +8423,7 @@
     </row>
     <row r="236" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A236" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B236" s="34" t="s">
         <v>52</v>
@@ -8410,13 +8460,13 @@
     </row>
     <row r="237" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A237" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B237" s="34" t="s">
         <v>6</v>
       </c>
       <c r="C237" s="35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D237" s="45"/>
       <c r="E237" s="45"/>
@@ -8443,7 +8493,7 @@
     </row>
     <row r="238" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A238" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B238" s="36"/>
       <c r="C238" s="35" t="s">
@@ -8488,13 +8538,13 @@
     </row>
     <row r="239" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A239" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B239" s="34" t="s">
         <v>6</v>
       </c>
       <c r="C239" s="35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D239" s="45"/>
       <c r="E239" s="45"/>
@@ -8515,13 +8565,13 @@
     </row>
     <row r="240" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A240" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B240" s="34" t="s">
         <v>6</v>
       </c>
       <c r="C240" s="35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D240" s="45"/>
       <c r="E240" s="45"/>
@@ -8542,7 +8592,7 @@
     </row>
     <row r="241" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A241" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B241" s="34" t="s">
         <v>6</v>
@@ -8571,13 +8621,13 @@
     </row>
     <row r="242" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A242" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B242" s="34" t="s">
         <v>52</v>
       </c>
       <c r="C242" s="35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D242" s="45"/>
       <c r="E242" s="45"/>
@@ -8610,13 +8660,13 @@
     </row>
     <row r="243" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A243" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B243" s="34" t="s">
         <v>6</v>
       </c>
       <c r="C243" s="35" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D243" s="45"/>
       <c r="E243" s="45"/>
@@ -8639,13 +8689,13 @@
     </row>
     <row r="244" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A244" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B244" s="34" t="s">
         <v>52</v>
       </c>
       <c r="C244" s="35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D244" s="45"/>
       <c r="E244" s="45"/>
@@ -8686,7 +8736,7 @@
     </row>
     <row r="245" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A245" s="33" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B245" s="34" t="s">
         <v>6</v>
@@ -8719,13 +8769,13 @@
     </row>
     <row r="246" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A246" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B246" s="15" t="s">
         <v>52</v>
       </c>
       <c r="C246" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D246" s="45"/>
       <c r="E246" s="45"/>
@@ -8744,7 +8794,7 @@
     </row>
     <row r="247" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A247" s="37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B247" s="38" t="s">
         <v>6</v>
@@ -8769,13 +8819,13 @@
     </row>
     <row r="248" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A248" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B248" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C248" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D248" s="45"/>
       <c r="E248" s="45"/>
@@ -8829,7 +8879,7 @@
         <v>6</v>
       </c>
       <c r="C250" s="39" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D250" s="45"/>
       <c r="E250" s="45"/>
@@ -8856,12 +8906,14 @@
         <v>6</v>
       </c>
       <c r="C251" s="39" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D251" s="45"/>
       <c r="E251" s="45"/>
       <c r="F251" s="45"/>
-      <c r="G251" s="17"/>
+      <c r="G251" s="17">
+        <v>1</v>
+      </c>
       <c r="H251" s="17"/>
       <c r="I251" s="17"/>
       <c r="J251" s="17"/>
@@ -8883,7 +8935,7 @@
         <v>52</v>
       </c>
       <c r="C252" s="39" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D252" s="45"/>
       <c r="E252" s="45"/>
@@ -8915,7 +8967,9 @@
       <c r="D253" s="45"/>
       <c r="E253" s="45"/>
       <c r="F253" s="45"/>
-      <c r="G253" s="17"/>
+      <c r="G253" s="17">
+        <v>1</v>
+      </c>
       <c r="H253" s="17">
         <v>1</v>
       </c>
@@ -8946,7 +9000,9 @@
       <c r="D254" s="45"/>
       <c r="E254" s="45"/>
       <c r="F254" s="45"/>
-      <c r="G254" s="17"/>
+      <c r="G254" s="17">
+        <v>1</v>
+      </c>
       <c r="H254" s="17">
         <v>1</v>
       </c>
@@ -8979,7 +9035,9 @@
       <c r="D255" s="45"/>
       <c r="E255" s="45"/>
       <c r="F255" s="45"/>
-      <c r="G255" s="17"/>
+      <c r="G255" s="17">
+        <v>1</v>
+      </c>
       <c r="H255" s="17"/>
       <c r="I255" s="17"/>
       <c r="J255" s="17"/>
@@ -9001,7 +9059,7 @@
         <v>6</v>
       </c>
       <c r="C256" s="39" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D256" s="45"/>
       <c r="E256" s="45"/>
@@ -9030,7 +9088,7 @@
         <v>6</v>
       </c>
       <c r="C257" s="39" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D257" s="45"/>
       <c r="E257" s="45"/>
@@ -9057,7 +9115,7 @@
         <v>6</v>
       </c>
       <c r="C258" s="39" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D258" s="45"/>
       <c r="E258" s="45"/>
@@ -9084,7 +9142,7 @@
         <v>6</v>
       </c>
       <c r="C259" s="39" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D259" s="45"/>
       <c r="E259" s="45"/>
@@ -9111,7 +9169,7 @@
         <v>6</v>
       </c>
       <c r="C260" s="39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D260" s="45"/>
       <c r="E260" s="45"/>
@@ -9138,7 +9196,7 @@
         <v>52</v>
       </c>
       <c r="C261" s="39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D261" s="45"/>
       <c r="E261" s="45"/>
@@ -9167,7 +9225,7 @@
         <v>6</v>
       </c>
       <c r="C262" s="39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D262" s="45"/>
       <c r="E262" s="45"/>
@@ -9214,7 +9272,7 @@
         <v>52</v>
       </c>
       <c r="C263" s="39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D263" s="45"/>
       <c r="E263" s="45"/>
@@ -9243,7 +9301,7 @@
         <v>6</v>
       </c>
       <c r="C264" s="39" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D264" s="45"/>
       <c r="E264" s="45"/>
@@ -9282,12 +9340,14 @@
         <v>52</v>
       </c>
       <c r="C265" s="39" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D265" s="45"/>
       <c r="E265" s="45"/>
       <c r="F265" s="45"/>
-      <c r="G265" s="17"/>
+      <c r="G265" s="17">
+        <v>1</v>
+      </c>
       <c r="H265" s="17"/>
       <c r="I265" s="17"/>
       <c r="J265" s="17"/>
@@ -9309,12 +9369,14 @@
         <v>6</v>
       </c>
       <c r="C266" s="39" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D266" s="45"/>
       <c r="E266" s="45"/>
       <c r="F266" s="45"/>
-      <c r="G266" s="17"/>
+      <c r="G266" s="17">
+        <v>1</v>
+      </c>
       <c r="H266" s="17"/>
       <c r="I266" s="17"/>
       <c r="J266" s="17"/>
@@ -9338,7 +9400,7 @@
         <v>6</v>
       </c>
       <c r="C267" s="39" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D267" s="45"/>
       <c r="E267" s="45"/>
@@ -9398,7 +9460,7 @@
         <v>6</v>
       </c>
       <c r="C269" s="39" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D269" s="45"/>
       <c r="E269" s="45"/>
@@ -9483,7 +9545,7 @@
         <v>52</v>
       </c>
       <c r="C272" s="13" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D272" s="45"/>
       <c r="E272" s="45"/>
@@ -9512,7 +9574,7 @@
         <v>52</v>
       </c>
       <c r="C273" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D273" s="45"/>
       <c r="E273" s="45"/>
@@ -9543,7 +9605,7 @@
         <v>6</v>
       </c>
       <c r="C274" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D274" s="45"/>
       <c r="E274" s="45"/>
@@ -9568,7 +9630,7 @@
         <v>52</v>
       </c>
       <c r="C275" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D275" s="45"/>
       <c r="E275" s="45"/>
@@ -9593,7 +9655,7 @@
         <v>52</v>
       </c>
       <c r="C276" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D276" s="45"/>
       <c r="E276" s="45"/>
@@ -9622,7 +9684,7 @@
         <v>52</v>
       </c>
       <c r="C277" s="13" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D277" s="45"/>
       <c r="E277" s="45"/>
@@ -9669,7 +9731,7 @@
         <v>52</v>
       </c>
       <c r="C278" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D278" s="45"/>
       <c r="E278" s="45"/>
@@ -9716,7 +9778,7 @@
         <v>52</v>
       </c>
       <c r="C279" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D279" s="45"/>
       <c r="E279" s="45"/>
@@ -9763,12 +9825,14 @@
         <v>6</v>
       </c>
       <c r="C280" s="56" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D280" s="48"/>
       <c r="E280" s="48"/>
       <c r="F280" s="48"/>
-      <c r="G280" s="54"/>
+      <c r="G280" s="54">
+        <v>1</v>
+      </c>
       <c r="H280" s="54">
         <v>1</v>
       </c>
@@ -9794,7 +9858,7 @@
         <v>6</v>
       </c>
       <c r="C281" s="57" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D281" s="48"/>
       <c r="E281" s="48"/>
@@ -9825,7 +9889,7 @@
         <v>6</v>
       </c>
       <c r="C282" s="57" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D282" s="48"/>
       <c r="E282" s="48"/>
@@ -9856,7 +9920,7 @@
         <v>6</v>
       </c>
       <c r="C283" s="57" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D283" s="48"/>
       <c r="E283" s="48"/>
@@ -9887,7 +9951,7 @@
         <v>6</v>
       </c>
       <c r="C284" s="57" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D284" s="48"/>
       <c r="E284" s="48"/>
@@ -9918,7 +9982,7 @@
         <v>6</v>
       </c>
       <c r="C285" s="57" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D285" s="48"/>
       <c r="E285" s="48"/>
@@ -10255,10 +10319,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="23" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>270</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CART, MRA, MPA added
</commit_message>
<xml_diff>
--- a/aws-services-crib-sheet.xlsx
+++ b/aws-services-crib-sheet.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corbuno/WorkDocs/courses/aws-services-crib-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5920A0-4B46-5C43-89F1-3C55172B2BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B9F697-3480-E842-A51A-D758DFD666FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="500" windowWidth="27860" windowHeight="17500" xr2:uid="{8DC9DE24-CECC-4748-B90E-52259685D84E}"/>
+    <workbookView xWindow="-15340" yWindow="-23500" windowWidth="27800" windowHeight="17500" xr2:uid="{8DC9DE24-CECC-4748-B90E-52259685D84E}"/>
   </bookViews>
   <sheets>
     <sheet name="AWS Services" sheetId="1" r:id="rId1"/>
     <sheet name="source" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AWS Services'!$A$1:$Q$298</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AWS Services'!$A$1:$Q$301</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="907" uniqueCount="344">
   <si>
     <t>CloudEndure Disaster Recovery</t>
   </si>
@@ -1052,6 +1052,15 @@
   </si>
   <si>
     <t>IoT Device SDK for Embedded C (C-SDK)</t>
+  </si>
+  <si>
+    <t>Migration Portfolio Assessment (MPA)</t>
+  </si>
+  <si>
+    <t>Migration Readiness Assessment (MRA)</t>
+  </si>
+  <si>
+    <t>Cloud Adoption Readiness Tool (CART)</t>
   </si>
 </sst>
 </file>
@@ -1817,11 +1826,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00D01EA-5C3E-F64B-8B7F-2EE6141A689A}">
-  <dimension ref="A1:Q298"/>
+  <dimension ref="A1:Q301"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D228" sqref="D228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -8317,7 +8326,7 @@
         <v>6</v>
       </c>
       <c r="C229" s="24" t="s">
-        <v>92</v>
+        <v>343</v>
       </c>
       <c r="D229" s="45"/>
       <c r="E229" s="45"/>
@@ -8342,25 +8351,21 @@
         <v>6</v>
       </c>
       <c r="C230" s="24" t="s">
-        <v>265</v>
+        <v>92</v>
       </c>
       <c r="D230" s="45"/>
       <c r="E230" s="45"/>
       <c r="F230" s="45"/>
       <c r="G230" s="17"/>
       <c r="H230" s="17"/>
-      <c r="I230" s="17">
-        <v>1</v>
-      </c>
+      <c r="I230" s="17"/>
       <c r="J230" s="17"/>
       <c r="K230" s="17"/>
       <c r="L230" s="17"/>
       <c r="M230" s="17"/>
       <c r="N230" s="17"/>
       <c r="O230" s="17"/>
-      <c r="P230" s="17">
-        <v>1</v>
-      </c>
+      <c r="P230" s="17"/>
       <c r="Q230" s="17"/>
     </row>
     <row r="231" spans="1:17" x14ac:dyDescent="0.2">
@@ -8371,22 +8376,18 @@
         <v>6</v>
       </c>
       <c r="C231" s="24" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="D231" s="45"/>
       <c r="E231" s="45"/>
       <c r="F231" s="45"/>
-      <c r="G231" s="17">
-        <v>1</v>
-      </c>
-      <c r="H231" s="17">
-        <v>1</v>
-      </c>
-      <c r="I231" s="17"/>
+      <c r="G231" s="17"/>
+      <c r="H231" s="17"/>
+      <c r="I231" s="17">
+        <v>1</v>
+      </c>
       <c r="J231" s="17"/>
-      <c r="K231" s="17">
-        <v>1</v>
-      </c>
+      <c r="K231" s="17"/>
       <c r="L231" s="17"/>
       <c r="M231" s="17"/>
       <c r="N231" s="17"/>
@@ -8394,9 +8395,7 @@
       <c r="P231" s="17">
         <v>1</v>
       </c>
-      <c r="Q231" s="17">
-        <v>1</v>
-      </c>
+      <c r="Q231" s="17"/>
     </row>
     <row r="232" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A232" s="22" t="s">
@@ -8406,19 +8405,19 @@
         <v>6</v>
       </c>
       <c r="C232" s="24" t="s">
-        <v>26</v>
+        <v>276</v>
       </c>
       <c r="D232" s="45"/>
       <c r="E232" s="45"/>
       <c r="F232" s="45"/>
-      <c r="G232" s="17"/>
+      <c r="G232" s="17">
+        <v>1</v>
+      </c>
       <c r="H232" s="17">
         <v>1</v>
       </c>
       <c r="I232" s="17"/>
-      <c r="J232" s="17">
-        <v>1</v>
-      </c>
+      <c r="J232" s="17"/>
       <c r="K232" s="17">
         <v>1</v>
       </c>
@@ -8429,7 +8428,9 @@
       <c r="P232" s="17">
         <v>1</v>
       </c>
-      <c r="Q232" s="17"/>
+      <c r="Q232" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="233" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A233" s="22" t="s">
@@ -8439,19 +8440,19 @@
         <v>6</v>
       </c>
       <c r="C233" s="24" t="s">
-        <v>277</v>
+        <v>26</v>
       </c>
       <c r="D233" s="45"/>
       <c r="E233" s="45"/>
       <c r="F233" s="45"/>
-      <c r="G233" s="17">
-        <v>1</v>
-      </c>
+      <c r="G233" s="17"/>
       <c r="H233" s="17">
         <v>1</v>
       </c>
       <c r="I233" s="17"/>
-      <c r="J233" s="17"/>
+      <c r="J233" s="17">
+        <v>1</v>
+      </c>
       <c r="K233" s="17">
         <v>1</v>
       </c>
@@ -8459,56 +8460,60 @@
       <c r="M233" s="17"/>
       <c r="N233" s="17"/>
       <c r="O233" s="17"/>
-      <c r="P233" s="17"/>
-      <c r="Q233" s="17">
-        <v>1</v>
-      </c>
+      <c r="P233" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q233" s="17"/>
     </row>
     <row r="234" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A234" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B234" s="23"/>
+      <c r="B234" s="23" t="s">
+        <v>6</v>
+      </c>
       <c r="C234" s="24" t="s">
-        <v>222</v>
+        <v>277</v>
       </c>
       <c r="D234" s="45"/>
       <c r="E234" s="45"/>
       <c r="F234" s="45"/>
-      <c r="G234" s="17"/>
-      <c r="H234" s="17"/>
+      <c r="G234" s="17">
+        <v>1</v>
+      </c>
+      <c r="H234" s="17">
+        <v>1</v>
+      </c>
       <c r="I234" s="17"/>
       <c r="J234" s="17"/>
-      <c r="K234" s="17"/>
+      <c r="K234" s="17">
+        <v>1</v>
+      </c>
       <c r="L234" s="17"/>
       <c r="M234" s="17"/>
       <c r="N234" s="17"/>
       <c r="O234" s="17"/>
       <c r="P234" s="17"/>
-      <c r="Q234" s="17"/>
+      <c r="Q234" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="235" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A235" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B235" s="23" t="s">
-        <v>6</v>
-      </c>
+      <c r="B235" s="23"/>
       <c r="C235" s="24" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="D235" s="45"/>
       <c r="E235" s="45"/>
       <c r="F235" s="45"/>
       <c r="G235" s="17"/>
-      <c r="H235" s="17">
-        <v>1</v>
-      </c>
+      <c r="H235" s="17"/>
       <c r="I235" s="17"/>
       <c r="J235" s="17"/>
-      <c r="K235" s="17">
-        <v>1</v>
-      </c>
+      <c r="K235" s="17"/>
       <c r="L235" s="17"/>
       <c r="M235" s="17"/>
       <c r="N235" s="17"/>
@@ -8524,7 +8529,7 @@
         <v>6</v>
       </c>
       <c r="C236" s="24" t="s">
-        <v>120</v>
+        <v>221</v>
       </c>
       <c r="D236" s="45"/>
       <c r="E236" s="45"/>
@@ -8553,29 +8558,21 @@
         <v>6</v>
       </c>
       <c r="C237" s="24" t="s">
-        <v>45</v>
+        <v>341</v>
       </c>
       <c r="D237" s="45"/>
       <c r="E237" s="45"/>
       <c r="F237" s="45"/>
-      <c r="G237" s="17">
-        <v>1</v>
-      </c>
-      <c r="H237" s="17">
-        <v>1</v>
-      </c>
+      <c r="G237" s="17"/>
+      <c r="H237" s="17"/>
       <c r="I237" s="17"/>
       <c r="J237" s="17"/>
-      <c r="K237" s="17">
-        <v>1</v>
-      </c>
+      <c r="K237" s="17"/>
       <c r="L237" s="17"/>
       <c r="M237" s="17"/>
       <c r="N237" s="17"/>
       <c r="O237" s="17"/>
-      <c r="P237" s="17">
-        <v>1</v>
-      </c>
+      <c r="P237" s="17"/>
       <c r="Q237" s="17"/>
     </row>
     <row r="238" spans="1:17" x14ac:dyDescent="0.2">
@@ -8586,14 +8583,12 @@
         <v>6</v>
       </c>
       <c r="C238" s="24" t="s">
-        <v>226</v>
+        <v>342</v>
       </c>
       <c r="D238" s="45"/>
       <c r="E238" s="45"/>
       <c r="F238" s="45"/>
-      <c r="G238" s="17">
-        <v>1</v>
-      </c>
+      <c r="G238" s="17"/>
       <c r="H238" s="17"/>
       <c r="I238" s="17"/>
       <c r="J238" s="17"/>
@@ -8613,14 +8608,12 @@
         <v>6</v>
       </c>
       <c r="C239" s="24" t="s">
-        <v>46</v>
+        <v>120</v>
       </c>
       <c r="D239" s="45"/>
       <c r="E239" s="45"/>
       <c r="F239" s="45"/>
-      <c r="G239" s="17">
-        <v>1</v>
-      </c>
+      <c r="G239" s="17"/>
       <c r="H239" s="17">
         <v>1</v>
       </c>
@@ -8644,19 +8637,19 @@
         <v>6</v>
       </c>
       <c r="C240" s="24" t="s">
-        <v>125</v>
+        <v>45</v>
       </c>
       <c r="D240" s="45"/>
       <c r="E240" s="45"/>
       <c r="F240" s="45"/>
-      <c r="G240" s="17"/>
+      <c r="G240" s="17">
+        <v>1</v>
+      </c>
       <c r="H240" s="17">
         <v>1</v>
       </c>
       <c r="I240" s="17"/>
-      <c r="J240" s="17">
-        <v>1</v>
-      </c>
+      <c r="J240" s="17"/>
       <c r="K240" s="17">
         <v>1</v>
       </c>
@@ -8670,14 +8663,14 @@
       <c r="Q240" s="17"/>
     </row>
     <row r="241" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A241" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="B241" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="C241" s="35" t="s">
-        <v>129</v>
+      <c r="A241" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B241" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C241" s="24" t="s">
+        <v>226</v>
       </c>
       <c r="D241" s="45"/>
       <c r="E241" s="45"/>
@@ -8685,83 +8678,79 @@
       <c r="G241" s="17">
         <v>1</v>
       </c>
-      <c r="H241" s="17">
-        <v>1</v>
-      </c>
-      <c r="I241" s="17">
-        <v>1</v>
-      </c>
+      <c r="H241" s="17"/>
+      <c r="I241" s="17"/>
       <c r="J241" s="17"/>
-      <c r="K241" s="17">
-        <v>1</v>
-      </c>
-      <c r="L241" s="17">
-        <v>1</v>
-      </c>
-      <c r="M241" s="17">
-        <v>1</v>
-      </c>
-      <c r="N241" s="17">
-        <v>1</v>
-      </c>
+      <c r="K241" s="17"/>
+      <c r="L241" s="17"/>
+      <c r="M241" s="17"/>
+      <c r="N241" s="17"/>
       <c r="O241" s="17"/>
-      <c r="P241" s="17">
-        <v>1</v>
-      </c>
+      <c r="P241" s="17"/>
       <c r="Q241" s="17"/>
     </row>
     <row r="242" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A242" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="B242" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C242" s="35" t="s">
-        <v>86</v>
+      <c r="A242" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B242" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C242" s="24" t="s">
+        <v>46</v>
       </c>
       <c r="D242" s="45"/>
       <c r="E242" s="45"/>
       <c r="F242" s="45"/>
-      <c r="G242" s="17"/>
-      <c r="H242" s="17"/>
+      <c r="G242" s="17">
+        <v>1</v>
+      </c>
+      <c r="H242" s="17">
+        <v>1</v>
+      </c>
       <c r="I242" s="17"/>
       <c r="J242" s="17"/>
-      <c r="K242" s="17"/>
+      <c r="K242" s="17">
+        <v>1</v>
+      </c>
       <c r="L242" s="17"/>
       <c r="M242" s="17"/>
-      <c r="N242" s="17">
-        <v>1</v>
-      </c>
+      <c r="N242" s="17"/>
       <c r="O242" s="17"/>
       <c r="P242" s="17"/>
       <c r="Q242" s="17"/>
     </row>
     <row r="243" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A243" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="B243" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C243" s="35" t="s">
-        <v>336</v>
+      <c r="A243" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B243" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C243" s="24" t="s">
+        <v>125</v>
       </c>
       <c r="D243" s="45"/>
       <c r="E243" s="45"/>
       <c r="F243" s="45"/>
       <c r="G243" s="17"/>
-      <c r="H243" s="17"/>
+      <c r="H243" s="17">
+        <v>1</v>
+      </c>
       <c r="I243" s="17"/>
       <c r="J243" s="17">
         <v>1</v>
       </c>
-      <c r="K243" s="17"/>
+      <c r="K243" s="17">
+        <v>1</v>
+      </c>
       <c r="L243" s="17"/>
       <c r="M243" s="17"/>
       <c r="N243" s="17"/>
       <c r="O243" s="17"/>
-      <c r="P243" s="17"/>
+      <c r="P243" s="17">
+        <v>1</v>
+      </c>
       <c r="Q243" s="17"/>
     </row>
     <row r="244" spans="1:17" x14ac:dyDescent="0.2">
@@ -8769,26 +8758,40 @@
         <v>169</v>
       </c>
       <c r="B244" s="34" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C244" s="35" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="D244" s="45"/>
       <c r="E244" s="45"/>
       <c r="F244" s="45"/>
-      <c r="G244" s="17"/>
-      <c r="H244" s="17"/>
-      <c r="I244" s="17"/>
+      <c r="G244" s="17">
+        <v>1</v>
+      </c>
+      <c r="H244" s="17">
+        <v>1</v>
+      </c>
+      <c r="I244" s="17">
+        <v>1</v>
+      </c>
       <c r="J244" s="17"/>
-      <c r="K244" s="17"/>
-      <c r="L244" s="17"/>
-      <c r="M244" s="17"/>
+      <c r="K244" s="17">
+        <v>1</v>
+      </c>
+      <c r="L244" s="17">
+        <v>1</v>
+      </c>
+      <c r="M244" s="17">
+        <v>1</v>
+      </c>
       <c r="N244" s="17">
         <v>1</v>
       </c>
       <c r="O244" s="17"/>
-      <c r="P244" s="17"/>
+      <c r="P244" s="17">
+        <v>1</v>
+      </c>
       <c r="Q244" s="17"/>
     </row>
     <row r="245" spans="1:17" x14ac:dyDescent="0.2">
@@ -8796,33 +8799,21 @@
         <v>169</v>
       </c>
       <c r="B245" s="34" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C245" s="35" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="D245" s="45"/>
       <c r="E245" s="45"/>
       <c r="F245" s="45"/>
-      <c r="G245" s="17">
-        <v>1</v>
-      </c>
-      <c r="H245" s="17">
-        <v>1</v>
-      </c>
-      <c r="I245" s="17">
-        <v>1</v>
-      </c>
-      <c r="J245" s="17">
-        <v>1</v>
-      </c>
-      <c r="K245" s="17">
-        <v>1</v>
-      </c>
+      <c r="G245" s="17"/>
+      <c r="H245" s="17"/>
+      <c r="I245" s="17"/>
+      <c r="J245" s="17"/>
+      <c r="K245" s="17"/>
       <c r="L245" s="17"/>
-      <c r="M245" s="17">
-        <v>1</v>
-      </c>
+      <c r="M245" s="17"/>
       <c r="N245" s="17">
         <v>1</v>
       </c>
@@ -8838,96 +8829,74 @@
         <v>6</v>
       </c>
       <c r="C246" s="35" t="s">
-        <v>93</v>
+        <v>336</v>
       </c>
       <c r="D246" s="45"/>
       <c r="E246" s="45"/>
       <c r="F246" s="45"/>
-      <c r="G246" s="17">
-        <v>1</v>
-      </c>
-      <c r="H246" s="17">
-        <v>1</v>
-      </c>
+      <c r="G246" s="17"/>
+      <c r="H246" s="17"/>
       <c r="I246" s="17"/>
-      <c r="J246" s="17"/>
-      <c r="K246" s="17">
-        <v>1</v>
-      </c>
+      <c r="J246" s="17">
+        <v>1</v>
+      </c>
+      <c r="K246" s="17"/>
       <c r="L246" s="17"/>
       <c r="M246" s="17"/>
-      <c r="N246" s="17">
-        <v>1</v>
-      </c>
+      <c r="N246" s="17"/>
       <c r="O246" s="17"/>
-      <c r="P246" s="17">
-        <v>1</v>
-      </c>
+      <c r="P246" s="17"/>
       <c r="Q246" s="17"/>
     </row>
     <row r="247" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A247" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="B247" s="36"/>
+      <c r="B247" s="34" t="s">
+        <v>6</v>
+      </c>
       <c r="C247" s="35" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
       <c r="D247" s="45"/>
       <c r="E247" s="45"/>
       <c r="F247" s="45"/>
-      <c r="G247" s="17">
-        <v>1</v>
-      </c>
-      <c r="H247" s="17">
-        <v>1</v>
-      </c>
-      <c r="I247" s="17">
-        <v>1</v>
-      </c>
-      <c r="J247" s="17">
-        <v>1</v>
-      </c>
-      <c r="K247" s="17">
-        <v>1</v>
-      </c>
-      <c r="L247" s="17">
-        <v>1</v>
-      </c>
-      <c r="M247" s="17">
-        <v>1</v>
-      </c>
+      <c r="G247" s="17"/>
+      <c r="H247" s="17"/>
+      <c r="I247" s="17"/>
+      <c r="J247" s="17"/>
+      <c r="K247" s="17"/>
+      <c r="L247" s="17"/>
+      <c r="M247" s="17"/>
       <c r="N247" s="17">
         <v>1</v>
       </c>
-      <c r="O247" s="17">
-        <v>1</v>
-      </c>
-      <c r="P247" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q247" s="17">
-        <v>1</v>
-      </c>
+      <c r="O247" s="17"/>
+      <c r="P247" s="17"/>
+      <c r="Q247" s="17"/>
     </row>
     <row r="248" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A248" s="33" t="s">
         <v>169</v>
       </c>
       <c r="B248" s="34" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C248" s="35" t="s">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="D248" s="45"/>
       <c r="E248" s="45"/>
       <c r="F248" s="45"/>
-      <c r="G248" s="17"/>
+      <c r="G248" s="17">
+        <v>1</v>
+      </c>
       <c r="H248" s="17">
         <v>1</v>
       </c>
-      <c r="I248" s="17"/>
+      <c r="I248" s="17">
+        <v>1</v>
+      </c>
       <c r="J248" s="17">
         <v>1</v>
       </c>
@@ -8935,7 +8904,9 @@
         <v>1</v>
       </c>
       <c r="L248" s="17"/>
-      <c r="M248" s="17"/>
+      <c r="M248" s="17">
+        <v>1</v>
+      </c>
       <c r="N248" s="17">
         <v>1</v>
       </c>
@@ -8951,70 +8922,92 @@
         <v>6</v>
       </c>
       <c r="C249" s="35" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="D249" s="45"/>
       <c r="E249" s="45"/>
       <c r="F249" s="45"/>
-      <c r="G249" s="17"/>
-      <c r="H249" s="17"/>
+      <c r="G249" s="17">
+        <v>1</v>
+      </c>
+      <c r="H249" s="17">
+        <v>1</v>
+      </c>
       <c r="I249" s="17"/>
       <c r="J249" s="17"/>
-      <c r="K249" s="17"/>
+      <c r="K249" s="17">
+        <v>1</v>
+      </c>
       <c r="L249" s="17"/>
       <c r="M249" s="17"/>
       <c r="N249" s="17">
         <v>1</v>
       </c>
       <c r="O249" s="17"/>
-      <c r="P249" s="17"/>
+      <c r="P249" s="17">
+        <v>1</v>
+      </c>
       <c r="Q249" s="17"/>
     </row>
     <row r="250" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A250" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="B250" s="34" t="s">
-        <v>6</v>
-      </c>
+      <c r="B250" s="36"/>
       <c r="C250" s="35" t="s">
-        <v>40</v>
+        <v>2</v>
       </c>
       <c r="D250" s="45"/>
       <c r="E250" s="45"/>
       <c r="F250" s="45"/>
-      <c r="G250" s="17"/>
-      <c r="H250" s="17"/>
-      <c r="I250" s="17"/>
-      <c r="J250" s="17"/>
+      <c r="G250" s="17">
+        <v>1</v>
+      </c>
+      <c r="H250" s="17">
+        <v>1</v>
+      </c>
+      <c r="I250" s="17">
+        <v>1</v>
+      </c>
+      <c r="J250" s="17">
+        <v>1</v>
+      </c>
       <c r="K250" s="17">
         <v>1</v>
       </c>
-      <c r="L250" s="17"/>
-      <c r="M250" s="17"/>
+      <c r="L250" s="17">
+        <v>1</v>
+      </c>
+      <c r="M250" s="17">
+        <v>1</v>
+      </c>
       <c r="N250" s="17">
         <v>1</v>
       </c>
-      <c r="O250" s="17"/>
-      <c r="P250" s="17"/>
-      <c r="Q250" s="17"/>
+      <c r="O250" s="17">
+        <v>1</v>
+      </c>
+      <c r="P250" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q250" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="251" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A251" s="33" t="s">
         <v>169</v>
       </c>
       <c r="B251" s="34" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C251" s="35" t="s">
-        <v>154</v>
+        <v>100</v>
       </c>
       <c r="D251" s="45"/>
       <c r="E251" s="45"/>
       <c r="F251" s="45"/>
-      <c r="G251" s="17">
-        <v>1</v>
-      </c>
+      <c r="G251" s="17"/>
       <c r="H251" s="17">
         <v>1</v>
       </c>
@@ -9025,9 +9018,7 @@
       <c r="K251" s="17">
         <v>1</v>
       </c>
-      <c r="L251" s="17">
-        <v>1</v>
-      </c>
+      <c r="L251" s="17"/>
       <c r="M251" s="17"/>
       <c r="N251" s="17">
         <v>1</v>
@@ -9044,7 +9035,7 @@
         <v>6</v>
       </c>
       <c r="C252" s="35" t="s">
-        <v>337</v>
+        <v>112</v>
       </c>
       <c r="D252" s="45"/>
       <c r="E252" s="45"/>
@@ -9056,7 +9047,9 @@
       <c r="K252" s="17"/>
       <c r="L252" s="17"/>
       <c r="M252" s="17"/>
-      <c r="N252" s="17"/>
+      <c r="N252" s="17">
+        <v>1</v>
+      </c>
       <c r="O252" s="17"/>
       <c r="P252" s="17"/>
       <c r="Q252" s="17"/>
@@ -9069,19 +9062,15 @@
         <v>6</v>
       </c>
       <c r="C253" s="35" t="s">
-        <v>126</v>
+        <v>40</v>
       </c>
       <c r="D253" s="45"/>
       <c r="E253" s="45"/>
       <c r="F253" s="45"/>
       <c r="G253" s="17"/>
-      <c r="H253" s="17">
-        <v>1</v>
-      </c>
+      <c r="H253" s="17"/>
       <c r="I253" s="17"/>
-      <c r="J253" s="17">
-        <v>1</v>
-      </c>
+      <c r="J253" s="17"/>
       <c r="K253" s="17">
         <v>1</v>
       </c>
@@ -9102,7 +9091,7 @@
         <v>51</v>
       </c>
       <c r="C254" s="35" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="D254" s="45"/>
       <c r="E254" s="45"/>
@@ -9113,9 +9102,7 @@
       <c r="H254" s="17">
         <v>1</v>
       </c>
-      <c r="I254" s="17">
-        <v>1</v>
-      </c>
+      <c r="I254" s="17"/>
       <c r="J254" s="17">
         <v>1</v>
       </c>
@@ -9125,31 +9112,23 @@
       <c r="L254" s="17">
         <v>1</v>
       </c>
-      <c r="M254" s="17">
-        <v>1</v>
-      </c>
+      <c r="M254" s="17"/>
       <c r="N254" s="17">
         <v>1</v>
       </c>
-      <c r="O254" s="17">
-        <v>1</v>
-      </c>
-      <c r="P254" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q254" s="17">
-        <v>1</v>
-      </c>
+      <c r="O254" s="17"/>
+      <c r="P254" s="17"/>
+      <c r="Q254" s="17"/>
     </row>
     <row r="255" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A255" s="33" t="s">
         <v>169</v>
       </c>
       <c r="B255" s="34" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C255" s="35" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D255" s="45"/>
       <c r="E255" s="45"/>
@@ -9157,9 +9136,7 @@
       <c r="G255" s="17"/>
       <c r="H255" s="17"/>
       <c r="I255" s="17"/>
-      <c r="J255" s="17">
-        <v>1</v>
-      </c>
+      <c r="J255" s="17"/>
       <c r="K255" s="17"/>
       <c r="L255" s="17"/>
       <c r="M255" s="17"/>
@@ -9176,19 +9153,19 @@
         <v>6</v>
       </c>
       <c r="C256" s="35" t="s">
-        <v>49</v>
+        <v>126</v>
       </c>
       <c r="D256" s="45"/>
       <c r="E256" s="45"/>
       <c r="F256" s="45"/>
-      <c r="G256" s="17">
-        <v>1</v>
-      </c>
+      <c r="G256" s="17"/>
       <c r="H256" s="17">
         <v>1</v>
       </c>
       <c r="I256" s="17"/>
-      <c r="J256" s="17"/>
+      <c r="J256" s="17">
+        <v>1</v>
+      </c>
       <c r="K256" s="17">
         <v>1</v>
       </c>
@@ -9202,39 +9179,61 @@
       <c r="Q256" s="17"/>
     </row>
     <row r="257" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A257" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B257" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C257" s="16" t="s">
-        <v>179</v>
+      <c r="A257" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="B257" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C257" s="35" t="s">
+        <v>161</v>
       </c>
       <c r="D257" s="45"/>
       <c r="E257" s="45"/>
       <c r="F257" s="45"/>
-      <c r="G257" s="17"/>
-      <c r="H257" s="17"/>
-      <c r="I257" s="17"/>
-      <c r="J257" s="17"/>
-      <c r="K257" s="17"/>
-      <c r="L257" s="17"/>
-      <c r="M257" s="17"/>
-      <c r="N257" s="17"/>
-      <c r="O257" s="17"/>
-      <c r="P257" s="17"/>
-      <c r="Q257" s="17"/>
+      <c r="G257" s="17">
+        <v>1</v>
+      </c>
+      <c r="H257" s="17">
+        <v>1</v>
+      </c>
+      <c r="I257" s="17">
+        <v>1</v>
+      </c>
+      <c r="J257" s="17">
+        <v>1</v>
+      </c>
+      <c r="K257" s="17">
+        <v>1</v>
+      </c>
+      <c r="L257" s="17">
+        <v>1</v>
+      </c>
+      <c r="M257" s="17">
+        <v>1</v>
+      </c>
+      <c r="N257" s="17">
+        <v>1</v>
+      </c>
+      <c r="O257" s="17">
+        <v>1</v>
+      </c>
+      <c r="P257" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q257" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="258" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A258" s="37" t="s">
-        <v>223</v>
-      </c>
-      <c r="B258" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="C258" s="39" t="s">
-        <v>42</v>
+      <c r="A258" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="B258" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C258" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="D258" s="45"/>
       <c r="E258" s="45"/>
@@ -9242,7 +9241,9 @@
       <c r="G258" s="17"/>
       <c r="H258" s="17"/>
       <c r="I258" s="17"/>
-      <c r="J258" s="17"/>
+      <c r="J258" s="17">
+        <v>1</v>
+      </c>
       <c r="K258" s="17"/>
       <c r="L258" s="17"/>
       <c r="M258" s="17"/>
@@ -9252,70 +9253,72 @@
       <c r="Q258" s="17"/>
     </row>
     <row r="259" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A259" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="B259" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C259" s="21" t="s">
-        <v>101</v>
+      <c r="A259" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="B259" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C259" s="35" t="s">
+        <v>49</v>
       </c>
       <c r="D259" s="45"/>
       <c r="E259" s="45"/>
       <c r="F259" s="45"/>
-      <c r="G259" s="17"/>
-      <c r="H259" s="17"/>
+      <c r="G259" s="17">
+        <v>1</v>
+      </c>
+      <c r="H259" s="17">
+        <v>1</v>
+      </c>
       <c r="I259" s="17"/>
       <c r="J259" s="17"/>
-      <c r="K259" s="17"/>
+      <c r="K259" s="17">
+        <v>1</v>
+      </c>
       <c r="L259" s="17"/>
       <c r="M259" s="17"/>
-      <c r="N259" s="17"/>
+      <c r="N259" s="17">
+        <v>1</v>
+      </c>
       <c r="O259" s="17"/>
       <c r="P259" s="17"/>
       <c r="Q259" s="17"/>
     </row>
     <row r="260" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A260" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B260" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="C260" s="39" t="s">
-        <v>9</v>
+      <c r="A260" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B260" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C260" s="16" t="s">
+        <v>179</v>
       </c>
       <c r="D260" s="45"/>
       <c r="E260" s="45"/>
       <c r="F260" s="45"/>
-      <c r="G260" s="17">
-        <v>1</v>
-      </c>
+      <c r="G260" s="17"/>
       <c r="H260" s="17"/>
       <c r="I260" s="17"/>
       <c r="J260" s="17"/>
       <c r="K260" s="17"/>
       <c r="L260" s="17"/>
-      <c r="M260" s="17">
-        <v>1</v>
-      </c>
+      <c r="M260" s="17"/>
       <c r="N260" s="17"/>
       <c r="O260" s="17"/>
-      <c r="P260" s="17">
-        <v>1</v>
-      </c>
+      <c r="P260" s="17"/>
       <c r="Q260" s="17"/>
     </row>
     <row r="261" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A261" s="37" t="s">
-        <v>43</v>
+        <v>223</v>
       </c>
       <c r="B261" s="38" t="s">
         <v>6</v>
       </c>
       <c r="C261" s="39" t="s">
-        <v>87</v>
+        <v>42</v>
       </c>
       <c r="D261" s="45"/>
       <c r="E261" s="45"/>
@@ -9326,49 +9329,35 @@
       <c r="J261" s="17"/>
       <c r="K261" s="17"/>
       <c r="L261" s="17"/>
-      <c r="M261" s="17">
-        <v>1</v>
-      </c>
+      <c r="M261" s="17"/>
       <c r="N261" s="17"/>
       <c r="O261" s="17"/>
       <c r="P261" s="17"/>
       <c r="Q261" s="17"/>
     </row>
     <row r="262" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A262" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B262" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="C262" s="39" t="s">
-        <v>225</v>
+      <c r="A262" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="B262" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C262" s="21" t="s">
+        <v>101</v>
       </c>
       <c r="D262" s="45"/>
       <c r="E262" s="45"/>
       <c r="F262" s="45"/>
-      <c r="G262" s="17">
-        <v>1</v>
-      </c>
-      <c r="H262" s="17">
-        <v>1</v>
-      </c>
+      <c r="G262" s="17"/>
+      <c r="H262" s="17"/>
       <c r="I262" s="17"/>
-      <c r="J262" s="17">
-        <v>1</v>
-      </c>
-      <c r="K262" s="17">
-        <v>1</v>
-      </c>
+      <c r="J262" s="17"/>
+      <c r="K262" s="17"/>
       <c r="L262" s="17"/>
-      <c r="M262" s="17">
-        <v>1</v>
-      </c>
+      <c r="M262" s="17"/>
       <c r="N262" s="17"/>
       <c r="O262" s="17"/>
-      <c r="P262" s="17">
-        <v>1</v>
-      </c>
+      <c r="P262" s="17"/>
       <c r="Q262" s="17"/>
     </row>
     <row r="263" spans="1:17" x14ac:dyDescent="0.2">
@@ -9376,15 +9365,17 @@
         <v>43</v>
       </c>
       <c r="B263" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C263" s="39" t="s">
-        <v>131</v>
+        <v>9</v>
       </c>
       <c r="D263" s="45"/>
       <c r="E263" s="45"/>
       <c r="F263" s="45"/>
-      <c r="G263" s="17"/>
+      <c r="G263" s="17">
+        <v>1</v>
+      </c>
       <c r="H263" s="17"/>
       <c r="I263" s="17"/>
       <c r="J263" s="17"/>
@@ -9395,7 +9386,9 @@
       </c>
       <c r="N263" s="17"/>
       <c r="O263" s="17"/>
-      <c r="P263" s="17"/>
+      <c r="P263" s="17">
+        <v>1</v>
+      </c>
       <c r="Q263" s="17"/>
     </row>
     <row r="264" spans="1:17" x14ac:dyDescent="0.2">
@@ -9406,31 +9399,23 @@
         <v>6</v>
       </c>
       <c r="C264" s="39" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="D264" s="45"/>
       <c r="E264" s="45"/>
       <c r="F264" s="45"/>
-      <c r="G264" s="17">
-        <v>1</v>
-      </c>
-      <c r="H264" s="17">
-        <v>1</v>
-      </c>
+      <c r="G264" s="17"/>
+      <c r="H264" s="17"/>
       <c r="I264" s="17"/>
       <c r="J264" s="17"/>
-      <c r="K264" s="17">
-        <v>1</v>
-      </c>
+      <c r="K264" s="17"/>
       <c r="L264" s="17"/>
       <c r="M264" s="17">
         <v>1</v>
       </c>
       <c r="N264" s="17"/>
       <c r="O264" s="17"/>
-      <c r="P264" s="17">
-        <v>1</v>
-      </c>
+      <c r="P264" s="17"/>
       <c r="Q264" s="17"/>
     </row>
     <row r="265" spans="1:17" x14ac:dyDescent="0.2">
@@ -9438,10 +9423,10 @@
         <v>43</v>
       </c>
       <c r="B265" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C265" s="39" t="s">
-        <v>59</v>
+        <v>225</v>
       </c>
       <c r="D265" s="45"/>
       <c r="E265" s="45"/>
@@ -9452,10 +9437,10 @@
       <c r="H265" s="17">
         <v>1</v>
       </c>
-      <c r="I265" s="17">
-        <v>1</v>
-      </c>
-      <c r="J265" s="17"/>
+      <c r="I265" s="17"/>
+      <c r="J265" s="17">
+        <v>1</v>
+      </c>
       <c r="K265" s="17">
         <v>1</v>
       </c>
@@ -9478,19 +9463,15 @@
         <v>51</v>
       </c>
       <c r="C266" s="39" t="s">
-        <v>61</v>
+        <v>131</v>
       </c>
       <c r="D266" s="45"/>
       <c r="E266" s="45"/>
       <c r="F266" s="45"/>
-      <c r="G266" s="17">
-        <v>1</v>
-      </c>
+      <c r="G266" s="17"/>
       <c r="H266" s="17"/>
       <c r="I266" s="17"/>
-      <c r="J266" s="17">
-        <v>1</v>
-      </c>
+      <c r="J266" s="17"/>
       <c r="K266" s="17"/>
       <c r="L266" s="17"/>
       <c r="M266" s="17">
@@ -9509,19 +9490,19 @@
         <v>6</v>
       </c>
       <c r="C267" s="39" t="s">
-        <v>94</v>
+        <v>16</v>
       </c>
       <c r="D267" s="45"/>
       <c r="E267" s="45"/>
       <c r="F267" s="45"/>
-      <c r="G267" s="17"/>
+      <c r="G267" s="17">
+        <v>1</v>
+      </c>
       <c r="H267" s="17">
         <v>1</v>
       </c>
       <c r="I267" s="17"/>
-      <c r="J267" s="17">
-        <v>1</v>
-      </c>
+      <c r="J267" s="17"/>
       <c r="K267" s="17">
         <v>1</v>
       </c>
@@ -9531,7 +9512,9 @@
       </c>
       <c r="N267" s="17"/>
       <c r="O267" s="17"/>
-      <c r="P267" s="17"/>
+      <c r="P267" s="17">
+        <v>1</v>
+      </c>
       <c r="Q267" s="17"/>
     </row>
     <row r="268" spans="1:17" x14ac:dyDescent="0.2">
@@ -9539,28 +9522,36 @@
         <v>43</v>
       </c>
       <c r="B268" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C268" s="39" t="s">
-        <v>271</v>
+        <v>59</v>
       </c>
       <c r="D268" s="45"/>
       <c r="E268" s="45"/>
       <c r="F268" s="45"/>
-      <c r="G268" s="17"/>
+      <c r="G268" s="17">
+        <v>1</v>
+      </c>
       <c r="H268" s="17">
         <v>1</v>
       </c>
-      <c r="I268" s="17"/>
+      <c r="I268" s="17">
+        <v>1</v>
+      </c>
       <c r="J268" s="17"/>
       <c r="K268" s="17">
         <v>1</v>
       </c>
       <c r="L268" s="17"/>
-      <c r="M268" s="17"/>
+      <c r="M268" s="17">
+        <v>1</v>
+      </c>
       <c r="N268" s="17"/>
       <c r="O268" s="17"/>
-      <c r="P268" s="17"/>
+      <c r="P268" s="17">
+        <v>1</v>
+      </c>
       <c r="Q268" s="17"/>
     </row>
     <row r="269" spans="1:17" x14ac:dyDescent="0.2">
@@ -9568,25 +9559,27 @@
         <v>43</v>
       </c>
       <c r="B269" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C269" s="39" t="s">
-        <v>270</v>
+        <v>61</v>
       </c>
       <c r="D269" s="45"/>
       <c r="E269" s="45"/>
       <c r="F269" s="45"/>
-      <c r="G269" s="17"/>
-      <c r="H269" s="17">
-        <v>1</v>
-      </c>
+      <c r="G269" s="17">
+        <v>1</v>
+      </c>
+      <c r="H269" s="17"/>
       <c r="I269" s="17"/>
-      <c r="J269" s="17"/>
-      <c r="K269" s="17">
-        <v>1</v>
-      </c>
+      <c r="J269" s="17">
+        <v>1</v>
+      </c>
+      <c r="K269" s="17"/>
       <c r="L269" s="17"/>
-      <c r="M269" s="17"/>
+      <c r="M269" s="17">
+        <v>1</v>
+      </c>
       <c r="N269" s="17"/>
       <c r="O269" s="17"/>
       <c r="P269" s="17"/>
@@ -9600,7 +9593,7 @@
         <v>6</v>
       </c>
       <c r="C270" s="39" t="s">
-        <v>272</v>
+        <v>94</v>
       </c>
       <c r="D270" s="45"/>
       <c r="E270" s="45"/>
@@ -9610,12 +9603,16 @@
         <v>1</v>
       </c>
       <c r="I270" s="17"/>
-      <c r="J270" s="17"/>
+      <c r="J270" s="17">
+        <v>1</v>
+      </c>
       <c r="K270" s="17">
         <v>1</v>
       </c>
       <c r="L270" s="17"/>
-      <c r="M270" s="17"/>
+      <c r="M270" s="17">
+        <v>1</v>
+      </c>
       <c r="N270" s="17"/>
       <c r="O270" s="17"/>
       <c r="P270" s="17"/>
@@ -9629,22 +9626,22 @@
         <v>6</v>
       </c>
       <c r="C271" s="39" t="s">
-        <v>99</v>
+        <v>271</v>
       </c>
       <c r="D271" s="45"/>
       <c r="E271" s="45"/>
       <c r="F271" s="45"/>
       <c r="G271" s="17"/>
-      <c r="H271" s="17"/>
+      <c r="H271" s="17">
+        <v>1</v>
+      </c>
       <c r="I271" s="17"/>
-      <c r="J271" s="17">
-        <v>1</v>
-      </c>
-      <c r="K271" s="17"/>
+      <c r="J271" s="17"/>
+      <c r="K271" s="17">
+        <v>1</v>
+      </c>
       <c r="L271" s="17"/>
-      <c r="M271" s="17">
-        <v>1</v>
-      </c>
+      <c r="M271" s="17"/>
       <c r="N271" s="17"/>
       <c r="O271" s="17"/>
       <c r="P271" s="17"/>
@@ -9655,31 +9652,25 @@
         <v>43</v>
       </c>
       <c r="B272" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C272" s="39" t="s">
-        <v>66</v>
+        <v>270</v>
       </c>
       <c r="D272" s="45"/>
       <c r="E272" s="45"/>
       <c r="F272" s="45"/>
-      <c r="G272" s="17">
-        <v>1</v>
-      </c>
+      <c r="G272" s="17"/>
       <c r="H272" s="17">
         <v>1</v>
       </c>
       <c r="I272" s="17"/>
-      <c r="J272" s="17">
-        <v>1</v>
-      </c>
+      <c r="J272" s="17"/>
       <c r="K272" s="17">
         <v>1</v>
       </c>
       <c r="L272" s="17"/>
-      <c r="M272" s="17">
-        <v>1</v>
-      </c>
+      <c r="M272" s="17"/>
       <c r="N272" s="17"/>
       <c r="O272" s="17"/>
       <c r="P272" s="17"/>
@@ -9693,18 +9684,20 @@
         <v>6</v>
       </c>
       <c r="C273" s="39" t="s">
-        <v>339</v>
+        <v>272</v>
       </c>
       <c r="D273" s="45"/>
       <c r="E273" s="45"/>
       <c r="F273" s="45"/>
       <c r="G273" s="17"/>
-      <c r="H273" s="17"/>
+      <c r="H273" s="17">
+        <v>1</v>
+      </c>
       <c r="I273" s="17"/>
-      <c r="J273" s="17">
-        <v>1</v>
-      </c>
-      <c r="K273" s="17"/>
+      <c r="J273" s="17"/>
+      <c r="K273" s="17">
+        <v>1</v>
+      </c>
       <c r="L273" s="17"/>
       <c r="M273" s="17"/>
       <c r="N273" s="17"/>
@@ -9720,44 +9713,26 @@
         <v>6</v>
       </c>
       <c r="C274" s="39" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D274" s="45"/>
       <c r="E274" s="45"/>
       <c r="F274" s="45"/>
-      <c r="G274" s="17">
-        <v>1</v>
-      </c>
-      <c r="H274" s="17">
-        <v>1</v>
-      </c>
-      <c r="I274" s="17">
-        <v>1</v>
-      </c>
+      <c r="G274" s="17"/>
+      <c r="H274" s="17"/>
+      <c r="I274" s="17"/>
       <c r="J274" s="17">
         <v>1</v>
       </c>
-      <c r="K274" s="17">
-        <v>1</v>
-      </c>
-      <c r="L274" s="17">
-        <v>1</v>
-      </c>
+      <c r="K274" s="17"/>
+      <c r="L274" s="17"/>
       <c r="M274" s="17">
         <v>1</v>
       </c>
-      <c r="N274" s="17">
-        <v>1</v>
-      </c>
-      <c r="O274" s="17">
-        <v>1</v>
-      </c>
-      <c r="P274" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q274" s="17">
-        <v>1</v>
-      </c>
+      <c r="N274" s="17"/>
+      <c r="O274" s="17"/>
+      <c r="P274" s="17"/>
+      <c r="Q274" s="17"/>
     </row>
     <row r="275" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A275" s="37" t="s">
@@ -9767,7 +9742,7 @@
         <v>51</v>
       </c>
       <c r="C275" s="39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D275" s="45"/>
       <c r="E275" s="45"/>
@@ -9802,37 +9777,23 @@
         <v>6</v>
       </c>
       <c r="C276" s="39" t="s">
-        <v>312</v>
+        <v>339</v>
       </c>
       <c r="D276" s="45"/>
       <c r="E276" s="45"/>
       <c r="F276" s="45"/>
-      <c r="G276" s="17">
-        <v>1</v>
-      </c>
-      <c r="H276" s="17">
-        <v>1</v>
-      </c>
-      <c r="I276" s="17">
-        <v>1</v>
-      </c>
+      <c r="G276" s="17"/>
+      <c r="H276" s="17"/>
+      <c r="I276" s="17"/>
       <c r="J276" s="17">
         <v>1</v>
       </c>
-      <c r="K276" s="17">
-        <v>1</v>
-      </c>
-      <c r="L276" s="17">
-        <v>1</v>
-      </c>
-      <c r="M276" s="17">
-        <v>1</v>
-      </c>
+      <c r="K276" s="17"/>
+      <c r="L276" s="17"/>
+      <c r="M276" s="17"/>
       <c r="N276" s="17"/>
       <c r="O276" s="17"/>
-      <c r="P276" s="17">
-        <v>1</v>
-      </c>
+      <c r="P276" s="17"/>
       <c r="Q276" s="17"/>
     </row>
     <row r="277" spans="1:17" x14ac:dyDescent="0.2">
@@ -9840,10 +9801,10 @@
         <v>43</v>
       </c>
       <c r="B277" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C277" s="39" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
       <c r="D277" s="45"/>
       <c r="E277" s="45"/>
@@ -9854,31 +9815,43 @@
       <c r="H277" s="17">
         <v>1</v>
       </c>
-      <c r="I277" s="17"/>
-      <c r="J277" s="17"/>
+      <c r="I277" s="17">
+        <v>1</v>
+      </c>
+      <c r="J277" s="17">
+        <v>1</v>
+      </c>
       <c r="K277" s="17">
         <v>1</v>
       </c>
-      <c r="L277" s="17"/>
+      <c r="L277" s="17">
+        <v>1</v>
+      </c>
       <c r="M277" s="17">
         <v>1</v>
       </c>
-      <c r="N277" s="17"/>
-      <c r="O277" s="17"/>
+      <c r="N277" s="17">
+        <v>1</v>
+      </c>
+      <c r="O277" s="17">
+        <v>1</v>
+      </c>
       <c r="P277" s="17">
         <v>1</v>
       </c>
-      <c r="Q277" s="17"/>
+      <c r="Q277" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="278" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A278" s="37" t="s">
         <v>43</v>
       </c>
       <c r="B278" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C278" s="39" t="s">
-        <v>118</v>
+        <v>67</v>
       </c>
       <c r="D278" s="45"/>
       <c r="E278" s="45"/>
@@ -9902,9 +9875,7 @@
       </c>
       <c r="N278" s="17"/>
       <c r="O278" s="17"/>
-      <c r="P278" s="17">
-        <v>1</v>
-      </c>
+      <c r="P278" s="17"/>
       <c r="Q278" s="17"/>
     </row>
     <row r="279" spans="1:17" x14ac:dyDescent="0.2">
@@ -9915,25 +9886,37 @@
         <v>6</v>
       </c>
       <c r="C279" s="39" t="s">
-        <v>119</v>
+        <v>312</v>
       </c>
       <c r="D279" s="45"/>
       <c r="E279" s="45"/>
       <c r="F279" s="45"/>
-      <c r="G279" s="17"/>
-      <c r="H279" s="17"/>
-      <c r="I279" s="17"/>
+      <c r="G279" s="17">
+        <v>1</v>
+      </c>
+      <c r="H279" s="17">
+        <v>1</v>
+      </c>
+      <c r="I279" s="17">
+        <v>1</v>
+      </c>
       <c r="J279" s="17">
         <v>1</v>
       </c>
-      <c r="K279" s="17"/>
-      <c r="L279" s="17"/>
+      <c r="K279" s="17">
+        <v>1</v>
+      </c>
+      <c r="L279" s="17">
+        <v>1</v>
+      </c>
       <c r="M279" s="17">
         <v>1</v>
       </c>
       <c r="N279" s="17"/>
       <c r="O279" s="17"/>
-      <c r="P279" s="17"/>
+      <c r="P279" s="17">
+        <v>1</v>
+      </c>
       <c r="Q279" s="17"/>
     </row>
     <row r="280" spans="1:17" x14ac:dyDescent="0.2">
@@ -9941,10 +9924,10 @@
         <v>43</v>
       </c>
       <c r="B280" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C280" s="39" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="D280" s="45"/>
       <c r="E280" s="45"/>
@@ -9956,9 +9939,7 @@
         <v>1</v>
       </c>
       <c r="I280" s="17"/>
-      <c r="J280" s="17">
-        <v>1</v>
-      </c>
+      <c r="J280" s="17"/>
       <c r="K280" s="17">
         <v>1</v>
       </c>
@@ -9968,7 +9949,9 @@
       </c>
       <c r="N280" s="17"/>
       <c r="O280" s="17"/>
-      <c r="P280" s="17"/>
+      <c r="P280" s="17">
+        <v>1</v>
+      </c>
       <c r="Q280" s="17"/>
     </row>
     <row r="281" spans="1:17" x14ac:dyDescent="0.2">
@@ -9979,17 +9962,21 @@
         <v>6</v>
       </c>
       <c r="C281" s="39" t="s">
-        <v>269</v>
+        <v>118</v>
       </c>
       <c r="D281" s="45"/>
       <c r="E281" s="45"/>
       <c r="F281" s="45"/>
-      <c r="G281" s="17"/>
+      <c r="G281" s="17">
+        <v>1</v>
+      </c>
       <c r="H281" s="17">
         <v>1</v>
       </c>
       <c r="I281" s="17"/>
-      <c r="J281" s="17"/>
+      <c r="J281" s="17">
+        <v>1</v>
+      </c>
       <c r="K281" s="17">
         <v>1</v>
       </c>
@@ -10012,24 +9999,18 @@
         <v>6</v>
       </c>
       <c r="C282" s="39" t="s">
-        <v>324</v>
+        <v>119</v>
       </c>
       <c r="D282" s="45"/>
       <c r="E282" s="45"/>
       <c r="F282" s="45"/>
-      <c r="G282" s="17">
-        <v>1</v>
-      </c>
-      <c r="H282" s="17">
-        <v>1</v>
-      </c>
+      <c r="G282" s="17"/>
+      <c r="H282" s="17"/>
       <c r="I282" s="17"/>
       <c r="J282" s="17">
         <v>1</v>
       </c>
-      <c r="K282" s="17">
-        <v>1</v>
-      </c>
+      <c r="K282" s="17"/>
       <c r="L282" s="17"/>
       <c r="M282" s="17">
         <v>1</v>
@@ -10040,62 +10021,82 @@
       <c r="Q282" s="17"/>
     </row>
     <row r="283" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A283" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B283" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C283" s="13" t="s">
-        <v>330</v>
+      <c r="A283" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B283" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C283" s="39" t="s">
+        <v>44</v>
       </c>
       <c r="D283" s="45"/>
       <c r="E283" s="45"/>
       <c r="F283" s="45"/>
-      <c r="G283" s="17"/>
-      <c r="H283" s="17"/>
+      <c r="G283" s="17">
+        <v>1</v>
+      </c>
+      <c r="H283" s="17">
+        <v>1</v>
+      </c>
       <c r="I283" s="17"/>
-      <c r="J283" s="17"/>
-      <c r="K283" s="17"/>
+      <c r="J283" s="17">
+        <v>1</v>
+      </c>
+      <c r="K283" s="17">
+        <v>1</v>
+      </c>
       <c r="L283" s="17"/>
-      <c r="M283" s="17"/>
+      <c r="M283" s="17">
+        <v>1</v>
+      </c>
       <c r="N283" s="17"/>
       <c r="O283" s="17"/>
       <c r="P283" s="17"/>
       <c r="Q283" s="17"/>
     </row>
     <row r="284" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A284" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B284" s="40"/>
-      <c r="C284" s="13" t="s">
-        <v>0</v>
+      <c r="A284" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B284" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C284" s="39" t="s">
+        <v>269</v>
       </c>
       <c r="D284" s="45"/>
       <c r="E284" s="45"/>
       <c r="F284" s="45"/>
       <c r="G284" s="17"/>
-      <c r="H284" s="17"/>
+      <c r="H284" s="17">
+        <v>1</v>
+      </c>
       <c r="I284" s="17"/>
       <c r="J284" s="17"/>
-      <c r="K284" s="17"/>
+      <c r="K284" s="17">
+        <v>1</v>
+      </c>
       <c r="L284" s="17"/>
-      <c r="M284" s="17"/>
+      <c r="M284" s="17">
+        <v>1</v>
+      </c>
       <c r="N284" s="17"/>
       <c r="O284" s="17"/>
-      <c r="P284" s="17"/>
+      <c r="P284" s="17">
+        <v>1</v>
+      </c>
       <c r="Q284" s="17"/>
     </row>
     <row r="285" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A285" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B285" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C285" s="13" t="s">
-        <v>135</v>
+      <c r="A285" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B285" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C285" s="39" t="s">
+        <v>324</v>
       </c>
       <c r="D285" s="45"/>
       <c r="E285" s="45"/>
@@ -10114,7 +10115,9 @@
         <v>1</v>
       </c>
       <c r="L285" s="17"/>
-      <c r="M285" s="17"/>
+      <c r="M285" s="17">
+        <v>1</v>
+      </c>
       <c r="N285" s="17"/>
       <c r="O285" s="17"/>
       <c r="P285" s="17"/>
@@ -10128,24 +10131,16 @@
         <v>51</v>
       </c>
       <c r="C286" s="13" t="s">
-        <v>139</v>
+        <v>330</v>
       </c>
       <c r="D286" s="45"/>
       <c r="E286" s="45"/>
       <c r="F286" s="45"/>
-      <c r="G286" s="17">
-        <v>1</v>
-      </c>
-      <c r="H286" s="17">
-        <v>1</v>
-      </c>
+      <c r="G286" s="17"/>
+      <c r="H286" s="17"/>
       <c r="I286" s="17"/>
-      <c r="J286" s="17">
-        <v>1</v>
-      </c>
-      <c r="K286" s="17">
-        <v>1</v>
-      </c>
+      <c r="J286" s="17"/>
+      <c r="K286" s="17"/>
       <c r="L286" s="17"/>
       <c r="M286" s="17"/>
       <c r="N286" s="17"/>
@@ -10157,11 +10152,9 @@
       <c r="A287" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B287" s="12" t="s">
-        <v>6</v>
-      </c>
+      <c r="B287" s="40"/>
       <c r="C287" s="13" t="s">
-        <v>240</v>
+        <v>0</v>
       </c>
       <c r="D287" s="45"/>
       <c r="E287" s="45"/>
@@ -10186,12 +10179,14 @@
         <v>51</v>
       </c>
       <c r="C288" s="13" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="D288" s="45"/>
       <c r="E288" s="45"/>
       <c r="F288" s="45"/>
-      <c r="G288" s="17"/>
+      <c r="G288" s="17">
+        <v>1</v>
+      </c>
       <c r="H288" s="17">
         <v>1</v>
       </c>
@@ -10217,12 +10212,14 @@
         <v>51</v>
       </c>
       <c r="C289" s="13" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D289" s="45"/>
       <c r="E289" s="45"/>
       <c r="F289" s="45"/>
-      <c r="G289" s="17"/>
+      <c r="G289" s="17">
+        <v>1</v>
+      </c>
       <c r="H289" s="17">
         <v>1</v>
       </c>
@@ -10245,47 +10242,25 @@
         <v>47</v>
       </c>
       <c r="B290" s="12" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C290" s="13" t="s">
-        <v>204</v>
+        <v>240</v>
       </c>
       <c r="D290" s="45"/>
       <c r="E290" s="45"/>
       <c r="F290" s="45"/>
-      <c r="G290" s="17">
-        <v>1</v>
-      </c>
-      <c r="H290" s="17">
-        <v>1</v>
-      </c>
-      <c r="I290" s="17">
-        <v>1</v>
-      </c>
-      <c r="J290" s="17">
-        <v>1</v>
-      </c>
-      <c r="K290" s="17">
-        <v>1</v>
-      </c>
-      <c r="L290" s="17">
-        <v>1</v>
-      </c>
-      <c r="M290" s="17">
-        <v>1</v>
-      </c>
-      <c r="N290" s="17">
-        <v>1</v>
-      </c>
-      <c r="O290" s="17">
-        <v>1</v>
-      </c>
-      <c r="P290" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q290" s="17">
-        <v>1</v>
-      </c>
+      <c r="G290" s="17"/>
+      <c r="H290" s="17"/>
+      <c r="I290" s="17"/>
+      <c r="J290" s="17"/>
+      <c r="K290" s="17"/>
+      <c r="L290" s="17"/>
+      <c r="M290" s="17"/>
+      <c r="N290" s="17"/>
+      <c r="O290" s="17"/>
+      <c r="P290" s="17"/>
+      <c r="Q290" s="17"/>
     </row>
     <row r="291" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A291" s="11" t="s">
@@ -10295,44 +10270,28 @@
         <v>51</v>
       </c>
       <c r="C291" s="13" t="s">
-        <v>264</v>
+        <v>143</v>
       </c>
       <c r="D291" s="45"/>
       <c r="E291" s="45"/>
       <c r="F291" s="45"/>
-      <c r="G291" s="17">
-        <v>1</v>
-      </c>
+      <c r="G291" s="17"/>
       <c r="H291" s="17">
         <v>1</v>
       </c>
-      <c r="I291" s="17">
-        <v>1</v>
-      </c>
+      <c r="I291" s="17"/>
       <c r="J291" s="17">
         <v>1</v>
       </c>
       <c r="K291" s="17">
         <v>1</v>
       </c>
-      <c r="L291" s="17">
-        <v>1</v>
-      </c>
-      <c r="M291" s="17">
-        <v>1</v>
-      </c>
-      <c r="N291" s="17">
-        <v>1</v>
-      </c>
-      <c r="O291" s="17">
-        <v>1</v>
-      </c>
-      <c r="P291" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q291" s="17">
-        <v>1</v>
-      </c>
+      <c r="L291" s="17"/>
+      <c r="M291" s="17"/>
+      <c r="N291" s="17"/>
+      <c r="O291" s="17"/>
+      <c r="P291" s="17"/>
+      <c r="Q291" s="17"/>
     </row>
     <row r="292" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A292" s="11" t="s">
@@ -10342,161 +10301,193 @@
         <v>51</v>
       </c>
       <c r="C292" s="13" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="D292" s="45"/>
       <c r="E292" s="45"/>
       <c r="F292" s="45"/>
-      <c r="G292" s="17">
-        <v>1</v>
-      </c>
+      <c r="G292" s="17"/>
       <c r="H292" s="17">
         <v>1</v>
       </c>
-      <c r="I292" s="17">
-        <v>1</v>
-      </c>
+      <c r="I292" s="17"/>
       <c r="J292" s="17">
         <v>1</v>
       </c>
       <c r="K292" s="17">
         <v>1</v>
       </c>
-      <c r="L292" s="17">
-        <v>1</v>
-      </c>
-      <c r="M292" s="17">
-        <v>1</v>
-      </c>
-      <c r="N292" s="17">
-        <v>1</v>
-      </c>
-      <c r="O292" s="17">
-        <v>1</v>
-      </c>
-      <c r="P292" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q292" s="17">
-        <v>1</v>
-      </c>
+      <c r="L292" s="17"/>
+      <c r="M292" s="17"/>
+      <c r="N292" s="17"/>
+      <c r="O292" s="17"/>
+      <c r="P292" s="17"/>
+      <c r="Q292" s="17"/>
     </row>
     <row r="293" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A293" s="11" t="s">
         <v>47</v>
       </c>
       <c r="B293" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C293" s="56" t="s">
-        <v>124</v>
-      </c>
-      <c r="D293" s="48"/>
-      <c r="E293" s="48"/>
-      <c r="F293" s="48"/>
-      <c r="G293" s="54">
-        <v>1</v>
-      </c>
-      <c r="H293" s="54">
-        <v>1</v>
-      </c>
-      <c r="I293" s="54"/>
-      <c r="J293" s="54">
-        <v>1</v>
-      </c>
-      <c r="K293" s="54">
-        <v>1</v>
-      </c>
-      <c r="L293" s="54"/>
-      <c r="M293" s="54"/>
-      <c r="N293" s="54">
-        <v>1</v>
-      </c>
-      <c r="O293" s="54"/>
-      <c r="P293" s="54"/>
-      <c r="Q293" s="54"/>
+        <v>51</v>
+      </c>
+      <c r="C293" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="D293" s="45"/>
+      <c r="E293" s="45"/>
+      <c r="F293" s="45"/>
+      <c r="G293" s="17">
+        <v>1</v>
+      </c>
+      <c r="H293" s="17">
+        <v>1</v>
+      </c>
+      <c r="I293" s="17">
+        <v>1</v>
+      </c>
+      <c r="J293" s="17">
+        <v>1</v>
+      </c>
+      <c r="K293" s="17">
+        <v>1</v>
+      </c>
+      <c r="L293" s="17">
+        <v>1</v>
+      </c>
+      <c r="M293" s="17">
+        <v>1</v>
+      </c>
+      <c r="N293" s="17">
+        <v>1</v>
+      </c>
+      <c r="O293" s="17">
+        <v>1</v>
+      </c>
+      <c r="P293" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q293" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="294" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A294" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B294" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="C294" s="57" t="s">
-        <v>315</v>
-      </c>
-      <c r="D294" s="48"/>
-      <c r="E294" s="48"/>
-      <c r="F294" s="48"/>
-      <c r="G294" s="54"/>
-      <c r="H294" s="54">
-        <v>1</v>
-      </c>
-      <c r="I294" s="54"/>
-      <c r="J294" s="54"/>
-      <c r="K294" s="54">
-        <v>1</v>
-      </c>
-      <c r="L294" s="54"/>
-      <c r="M294" s="54"/>
-      <c r="N294" s="54">
-        <v>1</v>
-      </c>
-      <c r="O294" s="54"/>
-      <c r="P294" s="54"/>
-      <c r="Q294" s="54"/>
+      <c r="B294" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C294" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="D294" s="45"/>
+      <c r="E294" s="45"/>
+      <c r="F294" s="45"/>
+      <c r="G294" s="17">
+        <v>1</v>
+      </c>
+      <c r="H294" s="17">
+        <v>1</v>
+      </c>
+      <c r="I294" s="17">
+        <v>1</v>
+      </c>
+      <c r="J294" s="17">
+        <v>1</v>
+      </c>
+      <c r="K294" s="17">
+        <v>1</v>
+      </c>
+      <c r="L294" s="17">
+        <v>1</v>
+      </c>
+      <c r="M294" s="17">
+        <v>1</v>
+      </c>
+      <c r="N294" s="17">
+        <v>1</v>
+      </c>
+      <c r="O294" s="17">
+        <v>1</v>
+      </c>
+      <c r="P294" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q294" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="295" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A295" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B295" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="C295" s="57" t="s">
-        <v>314</v>
-      </c>
-      <c r="D295" s="48"/>
-      <c r="E295" s="48"/>
-      <c r="F295" s="48"/>
-      <c r="G295" s="54"/>
-      <c r="H295" s="54">
-        <v>1</v>
-      </c>
-      <c r="I295" s="54"/>
-      <c r="J295" s="54"/>
-      <c r="K295" s="54">
-        <v>1</v>
-      </c>
-      <c r="L295" s="54"/>
-      <c r="M295" s="54"/>
-      <c r="N295" s="54">
-        <v>1</v>
-      </c>
-      <c r="O295" s="54"/>
-      <c r="P295" s="54"/>
-      <c r="Q295" s="54"/>
+      <c r="B295" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C295" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D295" s="45"/>
+      <c r="E295" s="45"/>
+      <c r="F295" s="45"/>
+      <c r="G295" s="17">
+        <v>1</v>
+      </c>
+      <c r="H295" s="17">
+        <v>1</v>
+      </c>
+      <c r="I295" s="17">
+        <v>1</v>
+      </c>
+      <c r="J295" s="17">
+        <v>1</v>
+      </c>
+      <c r="K295" s="17">
+        <v>1</v>
+      </c>
+      <c r="L295" s="17">
+        <v>1</v>
+      </c>
+      <c r="M295" s="17">
+        <v>1</v>
+      </c>
+      <c r="N295" s="17">
+        <v>1</v>
+      </c>
+      <c r="O295" s="17">
+        <v>1</v>
+      </c>
+      <c r="P295" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q295" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="296" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A296" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B296" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="C296" s="57" t="s">
-        <v>313</v>
+      <c r="B296" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C296" s="56" t="s">
+        <v>124</v>
       </c>
       <c r="D296" s="48"/>
       <c r="E296" s="48"/>
       <c r="F296" s="48"/>
-      <c r="G296" s="54"/>
+      <c r="G296" s="54">
+        <v>1</v>
+      </c>
       <c r="H296" s="54">
         <v>1</v>
       </c>
       <c r="I296" s="54"/>
-      <c r="J296" s="54"/>
+      <c r="J296" s="54">
+        <v>1</v>
+      </c>
       <c r="K296" s="54">
         <v>1</v>
       </c>
@@ -10517,7 +10508,7 @@
         <v>6</v>
       </c>
       <c r="C297" s="57" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D297" s="48"/>
       <c r="E297" s="48"/>
@@ -10548,7 +10539,7 @@
         <v>6</v>
       </c>
       <c r="C298" s="57" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D298" s="48"/>
       <c r="E298" s="48"/>
@@ -10571,32 +10562,125 @@
       <c r="P298" s="54"/>
       <c r="Q298" s="54"/>
     </row>
+    <row r="299" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A299" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B299" s="55" t="s">
+        <v>6</v>
+      </c>
+      <c r="C299" s="57" t="s">
+        <v>313</v>
+      </c>
+      <c r="D299" s="48"/>
+      <c r="E299" s="48"/>
+      <c r="F299" s="48"/>
+      <c r="G299" s="54"/>
+      <c r="H299" s="54">
+        <v>1</v>
+      </c>
+      <c r="I299" s="54"/>
+      <c r="J299" s="54"/>
+      <c r="K299" s="54">
+        <v>1</v>
+      </c>
+      <c r="L299" s="54"/>
+      <c r="M299" s="54"/>
+      <c r="N299" s="54">
+        <v>1</v>
+      </c>
+      <c r="O299" s="54"/>
+      <c r="P299" s="54"/>
+      <c r="Q299" s="54"/>
+    </row>
+    <row r="300" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A300" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B300" s="55" t="s">
+        <v>6</v>
+      </c>
+      <c r="C300" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D300" s="48"/>
+      <c r="E300" s="48"/>
+      <c r="F300" s="48"/>
+      <c r="G300" s="54"/>
+      <c r="H300" s="54">
+        <v>1</v>
+      </c>
+      <c r="I300" s="54"/>
+      <c r="J300" s="54"/>
+      <c r="K300" s="54">
+        <v>1</v>
+      </c>
+      <c r="L300" s="54"/>
+      <c r="M300" s="54"/>
+      <c r="N300" s="54">
+        <v>1</v>
+      </c>
+      <c r="O300" s="54"/>
+      <c r="P300" s="54"/>
+      <c r="Q300" s="54"/>
+    </row>
+    <row r="301" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A301" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B301" s="55" t="s">
+        <v>6</v>
+      </c>
+      <c r="C301" s="57" t="s">
+        <v>317</v>
+      </c>
+      <c r="D301" s="48"/>
+      <c r="E301" s="48"/>
+      <c r="F301" s="48"/>
+      <c r="G301" s="54"/>
+      <c r="H301" s="54">
+        <v>1</v>
+      </c>
+      <c r="I301" s="54"/>
+      <c r="J301" s="54"/>
+      <c r="K301" s="54">
+        <v>1</v>
+      </c>
+      <c r="L301" s="54"/>
+      <c r="M301" s="54"/>
+      <c r="N301" s="54">
+        <v>1</v>
+      </c>
+      <c r="O301" s="54"/>
+      <c r="P301" s="54"/>
+      <c r="Q301" s="54"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Q298" xr:uid="{A96C7FF1-A6C9-A643-BFCA-7D7FCDAF5533}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q298">
-      <sortCondition ref="A1:A298"/>
+  <autoFilter ref="A1:Q301" xr:uid="{A96C7FF1-A6C9-A643-BFCA-7D7FCDAF5533}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q301">
+      <sortCondition ref="A1:A301"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q292">
-    <sortCondition ref="A2:A292"/>
-    <sortCondition ref="C2:C292"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q295">
+    <sortCondition ref="A2:A295"/>
+    <sortCondition ref="C2:C295"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C92" r:id="rId1" display="https://aws.amazon.com/amplify/" xr:uid="{DD07C612-9881-1744-BD8F-2791C5BF0A5F}"/>
-    <hyperlink ref="C242" r:id="rId2" display="https://aws.amazon.com/app-mesh/" xr:uid="{F151395F-8E37-1049-9FCA-8474F2603F07}"/>
+    <hyperlink ref="C245" r:id="rId2" display="https://aws.amazon.com/app-mesh/" xr:uid="{F151395F-8E37-1049-9FCA-8474F2603F07}"/>
     <hyperlink ref="C28" r:id="rId3" display="https://aws.amazon.com/appsync/" xr:uid="{DB5645FD-41DF-9D4C-ADDB-CEEB9418B261}"/>
-    <hyperlink ref="C260" r:id="rId4" display="https://aws.amazon.com/artifact/" xr:uid="{0251BE44-6F83-3541-8CD4-81AEF00F1760}"/>
-    <hyperlink ref="C261" r:id="rId5" display="https://aws.amazon.com/audit-manager/" xr:uid="{FE0C678B-66B4-5041-87CB-7B1FF56DF53B}"/>
+    <hyperlink ref="C263" r:id="rId4" display="https://aws.amazon.com/artifact/" xr:uid="{0251BE44-6F83-3541-8CD4-81AEF00F1760}"/>
+    <hyperlink ref="C264" r:id="rId5" display="https://aws.amazon.com/audit-manager/" xr:uid="{FE0C678B-66B4-5041-87CB-7B1FF56DF53B}"/>
     <hyperlink ref="C166" r:id="rId6" display="https://aws.amazon.com/autoscaling/" xr:uid="{900D412E-B452-CD43-BEB1-C8C1CB7269C8}"/>
     <hyperlink ref="C167" r:id="rId7" display="https://aws.amazon.com/backup/" xr:uid="{E0DD5920-BDCE-E647-9AF3-74760943689B}"/>
     <hyperlink ref="C43" r:id="rId8" display="https://aws.amazon.com/batch/" xr:uid="{784C0A03-DDEC-BE4D-88F7-7005C1BB046B}"/>
     <hyperlink ref="C66" r:id="rId9" display="https://aws.amazon.com/aws-cost-management/aws-budgets/" xr:uid="{57F5A17A-4752-B94C-8FBB-FC20BBF1A0BE}"/>
-    <hyperlink ref="C262" r:id="rId10" display="https://aws.amazon.com/certificate-manager/" xr:uid="{1F5BBCA8-0D50-C44C-907B-68E23D8E605C}"/>
+    <hyperlink ref="C265" r:id="rId10" display="https://aws.amazon.com/certificate-manager/" xr:uid="{1F5BBCA8-0D50-C44C-907B-68E23D8E605C}"/>
     <hyperlink ref="C38" r:id="rId11" display="https://aws.amazon.com/chatbot/" xr:uid="{F29F6239-1ADB-7049-AAA7-6E39F247047B}"/>
-    <hyperlink ref="C244" r:id="rId12" display="https://aws.amazon.com/cloud-map/" xr:uid="{D482891E-9EB7-EA40-9A4B-6A8D3FEADBE3}"/>
+    <hyperlink ref="C247" r:id="rId12" display="https://aws.amazon.com/cloud-map/" xr:uid="{D482891E-9EB7-EA40-9A4B-6A8D3FEADBE3}"/>
     <hyperlink ref="C94" r:id="rId13" display="https://aws.amazon.com/cloud9/" xr:uid="{D565484B-E9EF-EA40-BDBE-0314AF229AE7}"/>
     <hyperlink ref="C168" r:id="rId14" display="https://aws.amazon.com/cloudformation/" xr:uid="{602EC08B-B845-E049-943E-890A120862C8}"/>
-    <hyperlink ref="C264" r:id="rId15" display="https://aws.amazon.com/cloudhsm/" xr:uid="{76B855B6-4A01-1642-8706-3316A1643BA7}"/>
+    <hyperlink ref="C267" r:id="rId15" display="https://aws.amazon.com/cloudhsm/" xr:uid="{76B855B6-4A01-1642-8706-3316A1643BA7}"/>
     <hyperlink ref="C169" r:id="rId16" display="https://aws.amazon.com/cloudtrail/" xr:uid="{F1C2A161-2AD0-B14D-B62A-2640A558856F}"/>
     <hyperlink ref="C96" r:id="rId17" display="https://aws.amazon.com/codeartifact" xr:uid="{A5B8559F-E4FA-BC42-AC7A-9D708C1D63A0}"/>
     <hyperlink ref="C97" r:id="rId18" display="https://aws.amazon.com/codebuild/" xr:uid="{E4144166-80F6-E741-B704-7C3864420913}"/>
@@ -10607,22 +10691,22 @@
     <hyperlink ref="C171" r:id="rId23" display="https://aws.amazon.com/compute-optimizer/" xr:uid="{099597B3-D96C-124F-8A6B-DB661823AC75}"/>
     <hyperlink ref="C172" r:id="rId24" display="https://aws.amazon.com/config/" xr:uid="{1DE61048-35C8-FB4C-A941-8996CBD19463}"/>
     <hyperlink ref="C173" r:id="rId25" display="https://aws.amazon.com/controltower" xr:uid="{5ACDD884-3684-1840-9A42-603B4BFD4DFA}"/>
-    <hyperlink ref="C229" r:id="rId26" display="https://aws.amazon.com/data-exchange/" xr:uid="{EF81BA84-5C8F-DD4B-A31A-47BF7D5C826C}"/>
-    <hyperlink ref="C232" r:id="rId27" display="https://aws.amazon.com/datasync" xr:uid="{7CED07B2-F329-1D46-A78D-E74BADEF8307}"/>
-    <hyperlink ref="C231" r:id="rId28" display="https://aws.amazon.com/dms/" xr:uid="{C9210BF6-9C8C-5E48-824D-711353B0A5C4}"/>
-    <hyperlink ref="C246" r:id="rId29" display="https://aws.amazon.com/directconnect/" xr:uid="{D4260538-1F28-C64D-999E-B57D8B4A110D}"/>
-    <hyperlink ref="C267" r:id="rId30" display="https://aws.amazon.com/directoryservice/" xr:uid="{71568105-08FB-3E48-ADDD-31FCAC00E550}"/>
+    <hyperlink ref="C230" r:id="rId26" display="https://aws.amazon.com/data-exchange/" xr:uid="{EF81BA84-5C8F-DD4B-A31A-47BF7D5C826C}"/>
+    <hyperlink ref="C233" r:id="rId27" display="https://aws.amazon.com/datasync" xr:uid="{7CED07B2-F329-1D46-A78D-E74BADEF8307}"/>
+    <hyperlink ref="C232" r:id="rId28" display="https://aws.amazon.com/dms/" xr:uid="{C9210BF6-9C8C-5E48-824D-711353B0A5C4}"/>
+    <hyperlink ref="C249" r:id="rId29" display="https://aws.amazon.com/directconnect/" xr:uid="{D4260538-1F28-C64D-999E-B57D8B4A110D}"/>
+    <hyperlink ref="C270" r:id="rId30" display="https://aws.amazon.com/directoryservice/" xr:uid="{71568105-08FB-3E48-ADDD-31FCAC00E550}"/>
     <hyperlink ref="C46" r:id="rId31" display="https://aws.amazon.com/elasticbeanstalk/" xr:uid="{503FA701-A8C3-BA4D-8F14-4F45B1936437}"/>
     <hyperlink ref="C211" r:id="rId32" display="https://aws.amazon.com/mediaconnect" xr:uid="{97EBEF96-B9F8-0444-803B-77B7686AD926}"/>
     <hyperlink ref="C212" r:id="rId33" display="https://aws.amazon.com/mediaconvert/" xr:uid="{A189CA26-8FE5-724E-AB4C-DA1684A9397C}"/>
     <hyperlink ref="C213" r:id="rId34" display="https://aws.amazon.com/medialive/" xr:uid="{8A1902D4-C3B2-6540-B6A2-D0939C092476}"/>
     <hyperlink ref="C61" r:id="rId35" display="https://aws.amazon.com/fargate/" xr:uid="{8AAC0488-BCAF-394A-B65D-1C8169C9015E}"/>
-    <hyperlink ref="C271" r:id="rId36" display="https://aws.amazon.com/firewall-manager/" xr:uid="{C1FC3FB2-6BB1-124F-AA39-0A32AEF1D03C}"/>
-    <hyperlink ref="C248" r:id="rId37" display="https://aws.amazon.com/global-accelerator" xr:uid="{94823B64-0747-B847-98EC-9C84C21B2DE2}"/>
+    <hyperlink ref="C274" r:id="rId36" display="https://aws.amazon.com/firewall-manager/" xr:uid="{C1FC3FB2-6BB1-124F-AA39-0A32AEF1D03C}"/>
+    <hyperlink ref="C251" r:id="rId37" display="https://aws.amazon.com/global-accelerator" xr:uid="{94823B64-0747-B847-98EC-9C84C21B2DE2}"/>
     <hyperlink ref="C6" r:id="rId38" display="https://aws.amazon.com/glue/" xr:uid="{A2984E2F-A64C-D74C-A499-872A26B2DE44}"/>
-    <hyperlink ref="C259" r:id="rId39" display="https://aws.amazon.com/ground-station/" xr:uid="{DB86E86A-EF5B-2541-9BD8-5CDA9965E40C}"/>
+    <hyperlink ref="C262" r:id="rId39" display="https://aws.amazon.com/ground-station/" xr:uid="{DB86E86A-EF5B-2541-9BD8-5CDA9965E40C}"/>
     <hyperlink ref="C72" r:id="rId40" display="https://aws.amazon.com/iq/" xr:uid="{66074B4A-E4D5-724E-AD29-24C171CEC0BA}"/>
-    <hyperlink ref="C274" r:id="rId41" display="https://aws.amazon.com/iam" xr:uid="{97081695-DB1E-424E-B0EE-79AAD8D6E1CE}"/>
+    <hyperlink ref="C277" r:id="rId41" display="https://aws.amazon.com/iam" xr:uid="{97081695-DB1E-424E-B0EE-79AAD8D6E1CE}"/>
     <hyperlink ref="C119" r:id="rId42" display="https://aws.amazon.com/iot-1-click/" xr:uid="{ADC027FD-055F-9343-AF7A-479D41533208}"/>
     <hyperlink ref="C120" r:id="rId43" display="https://aws.amazon.com/iot-analytics/" xr:uid="{6587843B-FF8F-E445-A148-97BAA80660A5}"/>
     <hyperlink ref="C121" r:id="rId44" display="https://aws.amazon.com/iot/" xr:uid="{72ADB53E-C5C8-6E45-9DE6-006357ADBB14}"/>
@@ -10630,77 +10714,77 @@
     <hyperlink ref="C123" r:id="rId46" display="https://aws.amazon.com/iot-device-management/" xr:uid="{47327A94-A7DA-D44B-8D5D-137A2C1DB78D}"/>
     <hyperlink ref="C125" r:id="rId47" display="https://aws.amazon.com/iot-events/" xr:uid="{09A17074-F045-D045-99F3-289DE651CC4B}"/>
     <hyperlink ref="C126" r:id="rId48" display="https://aws.amazon.com/greengrass/" xr:uid="{86C6B532-C282-AD49-84FC-E7151CC17562}"/>
-    <hyperlink ref="C276" r:id="rId49" display="https://aws.amazon.com/kms/" xr:uid="{C0A6E0DF-7D93-854D-AF8E-5B9C19B8AF02}"/>
+    <hyperlink ref="C279" r:id="rId49" display="https://aws.amazon.com/kms/" xr:uid="{C0A6E0DF-7D93-854D-AF8E-5B9C19B8AF02}"/>
     <hyperlink ref="C17" r:id="rId50" display="https://aws.amazon.com/lake-formation/" xr:uid="{8B1B5135-7A0D-7645-A701-475DDEBCFDA0}"/>
     <hyperlink ref="C48" r:id="rId51" display="https://aws.amazon.com/lambda/" xr:uid="{23B44498-C148-BD4C-86FE-EFAA00464E5B}"/>
     <hyperlink ref="C176" r:id="rId52" display="https://aws.amazon.com/license-manager/" xr:uid="{A80531A2-32DF-5E46-A8A2-AD514A9E876E}"/>
     <hyperlink ref="C74" r:id="rId53" display="https://aws.amazon.com/mp/" xr:uid="{83E81132-B5F9-A141-93D4-67826C5C6C2F}"/>
-    <hyperlink ref="C249" r:id="rId54" display="https://aws.amazon.com/network-firewall/" xr:uid="{380438F2-2136-CA48-8A93-614BD286828F}"/>
+    <hyperlink ref="C252" r:id="rId54" display="https://aws.amazon.com/network-firewall/" xr:uid="{380438F2-2136-CA48-8A93-614BD286828F}"/>
     <hyperlink ref="C181" r:id="rId55" display="https://aws.amazon.com/opsworks/stacks/" xr:uid="{C7B2C66E-7305-8A45-B44D-ED0E58D460E7}"/>
     <hyperlink ref="C179" r:id="rId56" display="https://aws.amazon.com/opsworks/chefautomate/" xr:uid="{44B83691-1D72-4540-A13B-BDA885E2E12D}"/>
     <hyperlink ref="C180" r:id="rId57" display="https://aws.amazon.com/opsworks/puppetenterprise/" xr:uid="{23F41EB8-3A55-A44E-BD0D-93039495EA49}"/>
     <hyperlink ref="C182" r:id="rId58" display="https://aws.amazon.com/organizations" xr:uid="{A3AB0BF0-AC79-A142-8708-144AD8A2BAF3}"/>
     <hyperlink ref="C50" r:id="rId59" display="https://aws.amazon.com/outposts/" xr:uid="{EC0218BA-7EA9-5F4D-8A2F-8D931B087AA0}"/>
     <hyperlink ref="C183" r:id="rId60" display="https://aws.amazon.com/premiumsupport/phd/" xr:uid="{BC843AAF-6516-F341-B87D-0984C181B4B5}"/>
-    <hyperlink ref="C250" r:id="rId61" display="https://aws.amazon.com/privatelink/" xr:uid="{908DA648-769A-FB47-86E4-3D66FA675B1C}"/>
+    <hyperlink ref="C253" r:id="rId61" display="https://aws.amazon.com/privatelink/" xr:uid="{908DA648-769A-FB47-86E4-3D66FA675B1C}"/>
     <hyperlink ref="C63" r:id="rId62" display="https://aws.amazon.com/proton/" xr:uid="{73BECBB6-D4BE-F445-97BF-0A1D62BCA194}"/>
     <hyperlink ref="C184" r:id="rId63" display="https://aws.amazon.com/ram/" xr:uid="{F8E211FB-42AB-6848-88B7-49CC2A833913}"/>
-    <hyperlink ref="C258" r:id="rId64" display="https://aws.amazon.com/robomaker/" xr:uid="{DBD68496-4CE8-804C-B893-9CFFB849F53A}"/>
-    <hyperlink ref="C278" r:id="rId65" display="https://aws.amazon.com/secrets-manager/" xr:uid="{632A5D67-D598-184C-AB9B-96F30896117D}"/>
-    <hyperlink ref="C279" r:id="rId66" display="https://aws.amazon.com/security-hub/" xr:uid="{342A4832-F3A0-DB4D-840C-8118FD830399}"/>
-    <hyperlink ref="C236" r:id="rId67" display="https://aws.amazon.com/server-migration-service/" xr:uid="{9446514E-0CE8-EC41-A9F1-0DC1FB7ADA55}"/>
+    <hyperlink ref="C261" r:id="rId64" display="https://aws.amazon.com/robomaker/" xr:uid="{DBD68496-4CE8-804C-B893-9CFFB849F53A}"/>
+    <hyperlink ref="C281" r:id="rId65" display="https://aws.amazon.com/secrets-manager/" xr:uid="{632A5D67-D598-184C-AB9B-96F30896117D}"/>
+    <hyperlink ref="C282" r:id="rId66" display="https://aws.amazon.com/security-hub/" xr:uid="{342A4832-F3A0-DB4D-840C-8118FD830399}"/>
+    <hyperlink ref="C239" r:id="rId67" display="https://aws.amazon.com/server-migration-service/" xr:uid="{9446514E-0CE8-EC41-A9F1-0DC1FB7ADA55}"/>
     <hyperlink ref="C51" r:id="rId68" display="https://aws.amazon.com/serverless/serverlessrepo/" xr:uid="{8F7AC4BC-9A37-EC4F-8183-7D7404D19E14}"/>
     <hyperlink ref="C185" r:id="rId69" display="https://aws.amazon.com/servicecatalog/" xr:uid="{2D2653B1-3D13-014A-9B9C-2386E2577635}"/>
-    <hyperlink ref="C280" r:id="rId70" display="https://aws.amazon.com/shield/" xr:uid="{76E091F3-F618-A648-879F-3F09BEBFABFD}"/>
-    <hyperlink ref="C281" r:id="rId71" display="https://aws.amazon.com/single-sign-on/" xr:uid="{A8360283-DE5C-1140-A85B-F33A2D6F72B8}"/>
-    <hyperlink ref="C237" r:id="rId72" display="https://aws.amazon.com/snowball/" xr:uid="{8A7E1B57-5F26-F64E-853D-BDD63390D5E6}"/>
-    <hyperlink ref="C239" r:id="rId73" display="https://aws.amazon.com/snowmobile/" xr:uid="{62B7D92F-3C96-DA44-9F02-BCC308391061}"/>
+    <hyperlink ref="C283" r:id="rId70" display="https://aws.amazon.com/shield/" xr:uid="{76E091F3-F618-A648-879F-3F09BEBFABFD}"/>
+    <hyperlink ref="C284" r:id="rId71" display="https://aws.amazon.com/single-sign-on/" xr:uid="{A8360283-DE5C-1140-A85B-F33A2D6F72B8}"/>
+    <hyperlink ref="C240" r:id="rId72" display="https://aws.amazon.com/snowball/" xr:uid="{8A7E1B57-5F26-F64E-853D-BDD63390D5E6}"/>
+    <hyperlink ref="C242" r:id="rId73" display="https://aws.amazon.com/snowmobile/" xr:uid="{62B7D92F-3C96-DA44-9F02-BCC308391061}"/>
     <hyperlink ref="C35" r:id="rId74" display="https://aws.amazon.com/step-functions/details/" xr:uid="{10824B81-0A5F-634D-84E6-9D2ADE3A6B39}"/>
-    <hyperlink ref="C293" r:id="rId75" display="https://aws.amazon.com/storagegateway/" xr:uid="{7BF17EFE-FF03-1D4A-BE9E-1FA982DA5C2A}"/>
+    <hyperlink ref="C296" r:id="rId75" display="https://aws.amazon.com/storagegateway/" xr:uid="{7BF17EFE-FF03-1D4A-BE9E-1FA982DA5C2A}"/>
     <hyperlink ref="C76" r:id="rId76" display="https://aws.amazon.com/premiumsupport/" xr:uid="{A5466C95-EFB7-3944-9E29-8D19BB6E169F}"/>
     <hyperlink ref="C203" r:id="rId77" display="https://aws.amazon.com/systems-manager/" xr:uid="{D6C17500-BE92-C444-BA4A-7116B75319D3}"/>
-    <hyperlink ref="C240" r:id="rId78" display="https://aws.amazon.com/aws-transfer-family/" xr:uid="{F0069BD4-8633-FB4B-8185-293CB3193797}"/>
-    <hyperlink ref="C253" r:id="rId79" display="https://aws.amazon.com/transit-gateway/" xr:uid="{2C10B2F7-EEE3-3444-A855-B387D48706EA}"/>
+    <hyperlink ref="C243" r:id="rId78" display="https://aws.amazon.com/aws-transfer-family/" xr:uid="{F0069BD4-8633-FB4B-8185-293CB3193797}"/>
+    <hyperlink ref="C256" r:id="rId79" display="https://aws.amazon.com/transit-gateway/" xr:uid="{2C10B2F7-EEE3-3444-A855-B387D48706EA}"/>
     <hyperlink ref="C204" r:id="rId80" display="https://aws.amazon.com/premiumsupport/trustedadvisor/" xr:uid="{436ECB3D-7EFE-764A-B2E3-3CF79C97B742}"/>
-    <hyperlink ref="C256" r:id="rId81" display="https://aws.amazon.com/vpn/" xr:uid="{5F2B553B-98BD-8D4B-849C-55A6F659C6B1}"/>
-    <hyperlink ref="C282" r:id="rId82" display="https://aws.amazon.com/waf/" xr:uid="{CF739D06-0B1B-6B46-91CF-6EE57FF09613}"/>
+    <hyperlink ref="C259" r:id="rId81" display="https://aws.amazon.com/vpn/" xr:uid="{5F2B553B-98BD-8D4B-849C-55A6F659C6B1}"/>
+    <hyperlink ref="C285" r:id="rId82" display="https://aws.amazon.com/waf/" xr:uid="{CF739D06-0B1B-6B46-91CF-6EE57FF09613}"/>
     <hyperlink ref="C205" r:id="rId83" display="https://aws.amazon.com/well-architected-tool" xr:uid="{81A34672-555C-B74A-9D7B-58590B7D3C75}"/>
     <hyperlink ref="C111" r:id="rId84" display="https://aws.amazon.com/xray/" xr:uid="{91A2B229-E348-8B4C-AF47-A5192DE45AEC}"/>
-    <hyperlink ref="C241" r:id="rId85" display="https://aws.amazon.com/api-gateway/" xr:uid="{81259B3E-1AB3-F64C-B232-9643470BBB0C}"/>
+    <hyperlink ref="C244" r:id="rId85" display="https://aws.amazon.com/api-gateway/" xr:uid="{81259B3E-1AB3-F64C-B232-9643470BBB0C}"/>
     <hyperlink ref="C27" r:id="rId86" display="https://aws.amazon.com/appflow/" xr:uid="{C427BFEE-537C-9B4C-B5FD-EF94DAB3195F}"/>
     <hyperlink ref="C2" r:id="rId87" display="https://aws.amazon.com/athena/" xr:uid="{8CA6E242-2CF4-E843-A8CA-4391EDA4CB08}"/>
     <hyperlink ref="C130" r:id="rId88" display="https://aws.amazon.com/augmented-ai/" xr:uid="{9B0A35B8-349D-874F-B406-0C378A70E4A7}"/>
     <hyperlink ref="C81" r:id="rId89" display="https://aws.amazon.com/rds/aurora/" xr:uid="{5BA37BE5-5EFA-D640-9340-68572A5C8B0A}"/>
     <hyperlink ref="C39" r:id="rId90" display="https://chime.aws/" xr:uid="{08A22D72-3716-8743-A4B8-3002293D3436}"/>
-    <hyperlink ref="C263" r:id="rId91" display="https://aws.amazon.com/cloud-directory/" xr:uid="{E41D133C-BA4E-4642-BA6F-656788DBC830}"/>
-    <hyperlink ref="C245" r:id="rId92" display="https://aws.amazon.com/cloudfront/" xr:uid="{8065D5C6-B564-A941-80CC-5D6C65B3D725}"/>
+    <hyperlink ref="C266" r:id="rId91" display="https://aws.amazon.com/cloud-directory/" xr:uid="{E41D133C-BA4E-4642-BA6F-656788DBC830}"/>
+    <hyperlink ref="C248" r:id="rId92" display="https://aws.amazon.com/cloudfront/" xr:uid="{8065D5C6-B564-A941-80CC-5D6C65B3D725}"/>
     <hyperlink ref="C170" r:id="rId93" display="https://aws.amazon.com/cloudwatch/" xr:uid="{52B01F49-5EAB-E540-BA38-BEED42EB43F4}"/>
     <hyperlink ref="C100" r:id="rId94" display="https://aws.amazon.com/codeguru/" xr:uid="{D5D1E2B5-ED1C-0D45-BCD8-07A6431E8C14}"/>
-    <hyperlink ref="C265" r:id="rId95" display="https://aws.amazon.com/cognito/" xr:uid="{5631285D-2790-B940-99E8-7A2AFBF2A4F8}"/>
+    <hyperlink ref="C268" r:id="rId95" display="https://aws.amazon.com/cognito/" xr:uid="{5631285D-2790-B940-99E8-7A2AFBF2A4F8}"/>
     <hyperlink ref="C131" r:id="rId96" display="https://aws.amazon.com/comprehend/" xr:uid="{EF9B7DCD-AAB7-C840-B56B-6901E4208F3C}"/>
     <hyperlink ref="C132" r:id="rId97" display="https://aws.amazon.com/comprehend/medical/" xr:uid="{E755C2E6-BB69-1547-AEEA-159FA230C6E0}"/>
-    <hyperlink ref="C266" r:id="rId98" display="https://aws.amazon.com/detective/" xr:uid="{4F6306C8-7E6E-B543-8987-505512DF8B38}"/>
+    <hyperlink ref="C269" r:id="rId98" display="https://aws.amazon.com/detective/" xr:uid="{4F6306C8-7E6E-B543-8987-505512DF8B38}"/>
     <hyperlink ref="C137" r:id="rId99" display="https://aws.amazon.com/devops-guru/" xr:uid="{0DE3687A-6EED-D846-93EF-2FF3EDCA2FE7}"/>
     <hyperlink ref="C82" r:id="rId100" display="https://aws.amazon.com/documentdb/" xr:uid="{E9BE873B-93B3-744C-82A3-AE676C942786}"/>
     <hyperlink ref="C83" r:id="rId101" display="https://aws.amazon.com/dynamodb/" xr:uid="{667C0B17-E586-7843-9ABA-2156F328D1C2}"/>
     <hyperlink ref="C84" r:id="rId102" display="https://aws.amazon.com/elasticache/" xr:uid="{0D3B6893-EB9F-F441-97F2-EAE3A531E741}"/>
-    <hyperlink ref="C285" r:id="rId103" display="https://aws.amazon.com/ebs/" xr:uid="{6475A1BA-F9EA-3643-A91C-960971815276}"/>
+    <hyperlink ref="C288" r:id="rId103" display="https://aws.amazon.com/ebs/" xr:uid="{6475A1BA-F9EA-3643-A91C-960971815276}"/>
     <hyperlink ref="C44" r:id="rId104" xr:uid="{F6BE2D25-6B4D-D545-BEF5-6353621F7D77}"/>
     <hyperlink ref="C58" r:id="rId105" display="https://aws.amazon.com/ecr/" xr:uid="{4DB8575D-FD4E-F24B-9A6D-4B237DEB4216}"/>
     <hyperlink ref="C59" r:id="rId106" display="https://aws.amazon.com/ecs/" xr:uid="{2A857716-DB7F-4D4C-9C3A-923E359FCE4B}"/>
-    <hyperlink ref="C286" r:id="rId107" display="https://aws.amazon.com/efs/" xr:uid="{17293663-847A-2945-BEEE-DB5C14186604}"/>
+    <hyperlink ref="C289" r:id="rId107" display="https://aws.amazon.com/efs/" xr:uid="{17293663-847A-2945-BEEE-DB5C14186604}"/>
     <hyperlink ref="C138" r:id="rId108" display="https://aws.amazon.com/elastic-inference/" xr:uid="{D7F32AC2-662A-044F-8D07-6056298BD732}"/>
     <hyperlink ref="C60" r:id="rId109" display="https://aws.amazon.com/eks" xr:uid="{8EA95DB8-FAF6-354A-8701-9BC26B99AF7A}"/>
     <hyperlink ref="C4" r:id="rId110" display="https://aws.amazon.com/emr/" xr:uid="{45F7CBE2-565C-A24D-A38F-B3A8800D8B65}"/>
     <hyperlink ref="C19" r:id="rId111" display="Elasticsearch Service (ES) / OpenSearch Service" xr:uid="{6AF99F4A-A394-8249-8B46-B05EDE624400}"/>
     <hyperlink ref="C29" r:id="rId112" display="https://aws.amazon.com/eventbridge/" xr:uid="{66CE333B-4CBB-9246-B3B7-51C615E2BFF5}"/>
-    <hyperlink ref="C288" r:id="rId113" display="https://aws.amazon.com/fsx/lustre/" xr:uid="{723E4B6B-4225-F149-A1D1-0C9ED96BB728}"/>
-    <hyperlink ref="C289" r:id="rId114" display="https://aws.amazon.com/fsx/windows/" xr:uid="{1B6B9E68-B13B-3B45-B1A5-A8F3F5BDE985}"/>
+    <hyperlink ref="C291" r:id="rId113" display="https://aws.amazon.com/fsx/lustre/" xr:uid="{723E4B6B-4225-F149-A1D1-0C9ED96BB728}"/>
+    <hyperlink ref="C292" r:id="rId114" display="https://aws.amazon.com/fsx/windows/" xr:uid="{1B6B9E68-B13B-3B45-B1A5-A8F3F5BDE985}"/>
     <hyperlink ref="C139" r:id="rId115" display="https://aws.amazon.com/forecast/" xr:uid="{1F07E3AD-D0E3-4442-9220-92E85E3DF861}"/>
     <hyperlink ref="C140" r:id="rId116" display="https://aws.amazon.com/fraud-detector/" xr:uid="{A16ABA87-0E9D-1749-BE3E-718E7599E24B}"/>
     <hyperlink ref="C115" r:id="rId117" display="https://aws.amazon.com/gamelift/" xr:uid="{ABE766D8-2E8B-B341-9103-F503839AC514}"/>
-    <hyperlink ref="C272" r:id="rId118" display="https://aws.amazon.com/guardduty/" xr:uid="{D1B6E14A-AD6C-E844-9AD0-215698F4E3BE}"/>
-    <hyperlink ref="C275" r:id="rId119" display="https://aws.amazon.com/inspector/" xr:uid="{176BE9A8-3FF5-874F-8EFA-6BB4665C2F33}"/>
+    <hyperlink ref="C275" r:id="rId118" display="https://aws.amazon.com/guardduty/" xr:uid="{D1B6E14A-AD6C-E844-9AD0-215698F4E3BE}"/>
+    <hyperlink ref="C278" r:id="rId119" display="https://aws.amazon.com/inspector/" xr:uid="{176BE9A8-3FF5-874F-8EFA-6BB4665C2F33}"/>
     <hyperlink ref="C85" r:id="rId120" display="https://aws.amazon.com/keyspaces/" xr:uid="{08537BC8-9E18-E341-B811-B357F4073FF5}"/>
     <hyperlink ref="C14" r:id="rId121" display="https://aws.amazon.com/kinesis/analytics/" xr:uid="{55091A39-96DB-9A41-B453-9AB88556B85B}"/>
     <hyperlink ref="C15" r:id="rId122" display="https://aws.amazon.com/kinesis/firehose/" xr:uid="{AB91BD64-7EBD-8A40-89D5-415AC999E5A7}"/>
@@ -10711,7 +10795,7 @@
     <hyperlink ref="C142" r:id="rId127" display="https://aws.amazon.com/lookout-for-vision/" xr:uid="{56891F15-488A-2D4F-957F-9C19DBC09E8C}"/>
     <hyperlink ref="C116" r:id="rId128" display="https://aws.amazon.com/lumberyard/" xr:uid="{0793FA7F-F861-E448-B351-2625AB793E29}"/>
     <hyperlink ref="C31" r:id="rId129" display="https://aws.amazon.com/amazon-mq/" xr:uid="{8F7E8190-F83B-7E45-9B55-465E1F7C79F3}"/>
-    <hyperlink ref="C277" r:id="rId130" display="https://aws.amazon.com/macie/" xr:uid="{0A9A9C7B-64FF-4944-8B73-82D7A54412E2}"/>
+    <hyperlink ref="C280" r:id="rId130" display="https://aws.amazon.com/macie/" xr:uid="{0A9A9C7B-64FF-4944-8B73-82D7A54412E2}"/>
     <hyperlink ref="C18" r:id="rId131" display="https://aws.amazon.com/msk/" xr:uid="{46024F01-6B35-0740-B92F-18BA0D596F3D}"/>
     <hyperlink ref="C30" r:id="rId132" display="https://aws.amazon.com/managed-workflows-for-apache-airflow/" xr:uid="{E7D50CE9-B395-AE40-B3BD-7B31072C139C}"/>
     <hyperlink ref="C87" r:id="rId133" display="https://aws.amazon.com/neptune/" xr:uid="{35EB7CA9-2F10-7E4E-9B05-D1C561AFFA79}"/>
@@ -10722,12 +10806,12 @@
     <hyperlink ref="C21" r:id="rId138" display="https://aws.amazon.com/redshift/" xr:uid="{BD068AB5-9542-BA4D-9D2D-3E01553833FF}"/>
     <hyperlink ref="C146" r:id="rId139" display="https://aws.amazon.com/rekognition/" xr:uid="{06B644B6-712E-EB4F-BDC1-2826A6E207A2}"/>
     <hyperlink ref="C90" r:id="rId140" display="https://aws.amazon.com/rds/" xr:uid="{52A384FE-5551-524F-8BE4-640C39EE59DB}"/>
-    <hyperlink ref="C251" r:id="rId141" display="https://aws.amazon.com/route53/" xr:uid="{2B9EF04D-DB6D-9948-8F0B-1F85D1FFA02C}"/>
+    <hyperlink ref="C254" r:id="rId141" display="https://aws.amazon.com/route53/" xr:uid="{2B9EF04D-DB6D-9948-8F0B-1F85D1FFA02C}"/>
     <hyperlink ref="C147" r:id="rId142" display="https://aws.amazon.com/sagemaker/" xr:uid="{FF819C8F-B472-6A4D-BF36-8803B10C8D16}"/>
     <hyperlink ref="C80" r:id="rId143" display="https://aws.amazon.com/ses/" xr:uid="{708BC6D8-3F72-374C-AB65-9002B2EB5C60}"/>
     <hyperlink ref="C32" r:id="rId144" display="https://aws.amazon.com/sns/" xr:uid="{2A7374BD-4C80-7C42-9E56-E3671DF3D17F}"/>
     <hyperlink ref="C33" r:id="rId145" display="https://aws.amazon.com/sqs/" xr:uid="{7EC87AB6-C5A3-0F4B-915C-BD9EF4201FD5}"/>
-    <hyperlink ref="C292" r:id="rId146" display="https://aws.amazon.com/s3/" xr:uid="{CD425C97-24D5-9747-8B23-DF9DD7A486F9}"/>
+    <hyperlink ref="C295" r:id="rId146" display="https://aws.amazon.com/s3/" xr:uid="{CD425C97-24D5-9747-8B23-DF9DD7A486F9}"/>
     <hyperlink ref="C34" r:id="rId147" display="https://aws.amazon.com/swf/" xr:uid="{631F304E-E46F-644E-8407-57836778A272}"/>
     <hyperlink ref="C117" r:id="rId148" display="https://aws.amazon.com/sumerian/" xr:uid="{1F8D41FC-B82F-8C44-A79F-AA91C3811E29}"/>
     <hyperlink ref="C161" r:id="rId149" display="https://aws.amazon.com/textract" xr:uid="{E50E8082-94C1-7947-963B-3A384A890F42}"/>
@@ -10735,18 +10819,18 @@
     <hyperlink ref="C162" r:id="rId151" display="https://aws.amazon.com/transcribe/" xr:uid="{7391FC88-BBA3-5846-9CA8-5612809D5D1E}"/>
     <hyperlink ref="C163" r:id="rId152" display="https://aws.amazon.com/transcribe/medical/" xr:uid="{5D3CF2D8-5264-E342-A8E8-E042131AE7AF}"/>
     <hyperlink ref="C164" r:id="rId153" display="https://aws.amazon.com/translate/" xr:uid="{D94B1850-F477-024B-8A15-72298FF44F81}"/>
-    <hyperlink ref="C254" r:id="rId154" display="https://aws.amazon.com/vpc/" xr:uid="{81704202-B35B-314F-9611-62D10520486C}"/>
+    <hyperlink ref="C257" r:id="rId154" display="https://aws.amazon.com/vpc/" xr:uid="{81704202-B35B-314F-9611-62D10520486C}"/>
     <hyperlink ref="C113" r:id="rId155" display="https://aws.amazon.com/worklink/" xr:uid="{A564F6A5-A25E-984E-AB0E-10859F299F79}"/>
-    <hyperlink ref="C284" r:id="rId156" display="https://aws.amazon.com/cloudendure-disaster-recovery/" xr:uid="{19E2670B-B70B-2246-875A-A798E313AD4C}"/>
+    <hyperlink ref="C287" r:id="rId156" display="https://aws.amazon.com/cloudendure-disaster-recovery/" xr:uid="{19E2670B-B70B-2246-875A-A798E313AD4C}"/>
     <hyperlink ref="C228" r:id="rId157" display="https://aws.amazon.com/cloudendure-migration/" xr:uid="{3011454A-BA14-2640-A5B0-1665DE5015EB}"/>
-    <hyperlink ref="C247" r:id="rId158" display="https://aws.amazon.com/elasticloadbalancing/" xr:uid="{48C41A56-7B49-954B-8607-BA52CE86305D}"/>
+    <hyperlink ref="C250" r:id="rId158" display="https://aws.amazon.com/elasticloadbalancing/" xr:uid="{48C41A56-7B49-954B-8607-BA52CE86305D}"/>
     <hyperlink ref="C118" r:id="rId159" display="https://aws.amazon.com/freertos/" xr:uid="{9A951967-4675-1546-8716-0568BF98D1CE}"/>
     <hyperlink ref="C52" r:id="rId160" display="https://aws.amazon.com/vmware/" xr:uid="{1D088AE8-27BE-C042-AB38-9D218A238493}"/>
     <hyperlink ref="C47" r:id="rId161" display="https://aws.amazon.com/ec2/" xr:uid="{A67A7092-80C0-9A4E-A55B-97FA160377E8}"/>
-    <hyperlink ref="C290" r:id="rId162" xr:uid="{9237F063-BA80-DC44-882A-D4F7F6FD5EE9}"/>
+    <hyperlink ref="C293" r:id="rId162" xr:uid="{9237F063-BA80-DC44-882A-D4F7F6FD5EE9}"/>
     <hyperlink ref="C105" r:id="rId163" xr:uid="{75CD952A-625F-DE4E-B2D6-41E51DC1F7E3}"/>
     <hyperlink ref="C36" r:id="rId164" xr:uid="{49E4FD14-55A4-2E46-8EFF-5EF1766DCF38}"/>
-    <hyperlink ref="C238" r:id="rId165" xr:uid="{7054BAB5-94B7-0C4D-A749-E850E72E4B65}"/>
+    <hyperlink ref="C241" r:id="rId165" xr:uid="{7054BAB5-94B7-0C4D-A749-E850E72E4B65}"/>
     <hyperlink ref="C79" r:id="rId166" xr:uid="{AD71ACB3-ABC2-514F-A36F-2373C95B6534}"/>
     <hyperlink ref="C78" r:id="rId167" xr:uid="{BD82E153-E205-2541-8061-196FC264C5B0}"/>
     <hyperlink ref="C5" r:id="rId168" xr:uid="{A6E6DBD8-12FD-894D-842E-E5DA02E3DBF4}"/>
@@ -10759,7 +10843,7 @@
     <hyperlink ref="C53" r:id="rId175" xr:uid="{005354BD-081E-9E46-8937-381CB8592473}"/>
     <hyperlink ref="C57" r:id="rId176" xr:uid="{1CFA07FC-268F-C84D-B8E8-D13B2E092826}"/>
     <hyperlink ref="C177" r:id="rId177" xr:uid="{667DCA05-C10B-394B-ADBD-C91C39C8EFA9}"/>
-    <hyperlink ref="C287" r:id="rId178" xr:uid="{19712BF9-B0E9-FC4A-855C-37C622207421}"/>
+    <hyperlink ref="C290" r:id="rId178" xr:uid="{19712BF9-B0E9-FC4A-855C-37C622207421}"/>
     <hyperlink ref="C95" r:id="rId179" xr:uid="{532F9FAB-7588-934A-BECA-94DB57B3EA86}"/>
     <hyperlink ref="C93" r:id="rId180" xr:uid="{03EA6A9E-9AED-E449-AEAE-E07C9D687ADF}"/>
     <hyperlink ref="C110" r:id="rId181" xr:uid="{1A9B8E63-391D-0446-8004-324356B6D2C7}"/>
@@ -10793,20 +10877,20 @@
     <hyperlink ref="C192" r:id="rId209" xr:uid="{D7F493BC-3996-E14D-8B4E-AF698AF15CF3}"/>
     <hyperlink ref="C197" r:id="rId210" xr:uid="{158C22B5-B282-0E45-819B-E1F6D3588EB5}"/>
     <hyperlink ref="C193" r:id="rId211" xr:uid="{060EF427-1526-CB41-B8B7-D967487671FE}"/>
-    <hyperlink ref="C291" r:id="rId212" display="S3 Glacier" xr:uid="{69E65928-2461-9D41-874A-E2DD597C93F4}"/>
+    <hyperlink ref="C294" r:id="rId212" display="S3 Glacier" xr:uid="{69E65928-2461-9D41-874A-E2DD597C93F4}"/>
     <hyperlink ref="C154" r:id="rId213" xr:uid="{985BD89A-8A6D-3646-8654-90328345A506}"/>
     <hyperlink ref="C133" r:id="rId214" xr:uid="{590CE714-967E-A245-B8FF-739BCA3B026A}"/>
     <hyperlink ref="C134" r:id="rId215" xr:uid="{1D9605EA-560D-C04A-9C84-34D242F7CD14}"/>
     <hyperlink ref="C135" r:id="rId216" xr:uid="{16002AA9-2EA1-E344-8204-E762411450D2}"/>
     <hyperlink ref="C136" r:id="rId217" xr:uid="{A4BCE370-7F9E-AD48-8C7A-1D6984474130}"/>
-    <hyperlink ref="C230" r:id="rId218" xr:uid="{8AB16A6A-B47A-404E-B8D0-B5341D99BBA0}"/>
+    <hyperlink ref="C231" r:id="rId218" xr:uid="{8AB16A6A-B47A-404E-B8D0-B5341D99BBA0}"/>
     <hyperlink ref="C37" r:id="rId219" xr:uid="{B76C300C-E4E2-7849-9BD6-6C37B6A3A3E9}"/>
     <hyperlink ref="C40" r:id="rId220" xr:uid="{94ED9A38-CC0B-6547-A3F8-0E1E5184307C}"/>
     <hyperlink ref="C41" r:id="rId221" xr:uid="{484C0088-17D4-5E46-9E7E-4B7D0CADC15E}"/>
     <hyperlink ref="C42" r:id="rId222" xr:uid="{AD3D4FE9-D4D4-D34A-8BFC-469E359937BD}"/>
-    <hyperlink ref="C257" r:id="rId223" xr:uid="{1A1FF780-D417-4E48-8B89-324891ACD5EB}"/>
-    <hyperlink ref="C234" r:id="rId224" xr:uid="{A55A32E4-E04D-3D4E-B771-FF5015CDE5FC}"/>
-    <hyperlink ref="C235" r:id="rId225" xr:uid="{470F8C84-D502-374E-8550-CF45C7EE93CD}"/>
+    <hyperlink ref="C260" r:id="rId223" xr:uid="{1A1FF780-D417-4E48-8B89-324891ACD5EB}"/>
+    <hyperlink ref="C235" r:id="rId224" xr:uid="{A55A32E4-E04D-3D4E-B771-FF5015CDE5FC}"/>
+    <hyperlink ref="C236" r:id="rId225" xr:uid="{470F8C84-D502-374E-8550-CF45C7EE93CD}"/>
     <hyperlink ref="C67" r:id="rId226" xr:uid="{14B6B46E-839F-BF4A-B271-B234D8C79A65}"/>
     <hyperlink ref="C68" r:id="rId227" xr:uid="{831473DF-5435-A34B-AD2F-B228DE3531C9}"/>
     <hyperlink ref="C69" r:id="rId228" location="/" xr:uid="{E971A21E-CC8D-5648-B51E-E10B69902AA4}"/>
@@ -10815,13 +10899,13 @@
     <hyperlink ref="C128" r:id="rId231" xr:uid="{40FD60AC-B589-0B4B-AB36-1989E529CD39}"/>
     <hyperlink ref="C129" r:id="rId232" xr:uid="{56F27AA2-5183-E94B-ACC4-73885A21F096}"/>
     <hyperlink ref="C62" r:id="rId233" display="Managed Service for Prometheus" xr:uid="{15FBF981-0EC3-6343-ACAF-575D9CF01C72}"/>
-    <hyperlink ref="C268" r:id="rId234" display="Directory Service AD Connector" xr:uid="{CE8FDA92-983D-F241-9A3C-214FB6ED4987}"/>
-    <hyperlink ref="C270" r:id="rId235" display="Directory Service Simple AD" xr:uid="{BDF803C1-C55F-7B4E-B548-FB056C33B7F8}"/>
-    <hyperlink ref="C269" r:id="rId236" display="Directory Service Managed Microsoft AD" xr:uid="{A2682350-698B-164E-854C-B72B425BF114}"/>
+    <hyperlink ref="C271" r:id="rId234" display="Directory Service AD Connector" xr:uid="{CE8FDA92-983D-F241-9A3C-214FB6ED4987}"/>
+    <hyperlink ref="C273" r:id="rId235" display="Directory Service Simple AD" xr:uid="{BDF803C1-C55F-7B4E-B548-FB056C33B7F8}"/>
+    <hyperlink ref="C272" r:id="rId236" display="Directory Service Managed Microsoft AD" xr:uid="{A2682350-698B-164E-854C-B72B425BF114}"/>
     <hyperlink ref="C178" r:id="rId237" xr:uid="{51AE8255-80F9-1246-AF04-CAD49D7BD8ED}"/>
     <hyperlink ref="C106" r:id="rId238" xr:uid="{F72E5D13-7F9C-A74A-B15B-60DA5CBC35BF}"/>
     <hyperlink ref="C141" r:id="rId239" xr:uid="{A021BA43-B246-CF41-8A4E-1E391CD06D94}"/>
-    <hyperlink ref="C233" r:id="rId240" xr:uid="{66C98670-091A-A841-9473-A308D3D03C92}"/>
+    <hyperlink ref="C234" r:id="rId240" xr:uid="{66C98670-091A-A841-9473-A308D3D03C92}"/>
     <hyperlink ref="C89" r:id="rId241" xr:uid="{A18DAD6F-3F0D-2F41-8ECF-C20C2E59C987}"/>
     <hyperlink ref="C73" r:id="rId242" xr:uid="{BB9AA509-E09D-604B-9392-FAF5D5E1155F}"/>
     <hyperlink ref="C75" r:id="rId243" xr:uid="{2260673B-2C63-EA41-A726-76787E04ADC6}"/>
@@ -10854,11 +10938,11 @@
     <hyperlink ref="C224" r:id="rId270" xr:uid="{3B6EA2BE-9E87-CD43-BD86-90EF411A17C9}"/>
     <hyperlink ref="C225" r:id="rId271" xr:uid="{BE5AE3F2-6AF4-FB45-A4C7-58EE1FA83493}"/>
     <hyperlink ref="C226" r:id="rId272" xr:uid="{9F9A6701-301A-8946-8181-9D1074CEB3F6}"/>
-    <hyperlink ref="C298" r:id="rId273" display="Storage Gateway - Volume Gateway" xr:uid="{D2EC8952-5BC9-2B49-B394-D7BE012603FF}"/>
-    <hyperlink ref="C296" r:id="rId274" xr:uid="{1B5D263F-5321-B54A-BF60-2932447DCE26}"/>
-    <hyperlink ref="C294" r:id="rId275" display="Storage Gateway - FSx File Gateway" xr:uid="{2125FCAA-C46E-224B-8BE0-19D32D161491}"/>
-    <hyperlink ref="C295" r:id="rId276" display="Storage Gateway - S3 File Gateway" xr:uid="{96B9D02E-E08D-3E44-9C8E-08A2BE24E99A}"/>
-    <hyperlink ref="C297" r:id="rId277" display="Storage Gateway - Volume Gateway" xr:uid="{FFBC4DD5-5D45-9B42-A545-70A2598E87B0}"/>
+    <hyperlink ref="C301" r:id="rId273" display="Storage Gateway - Volume Gateway" xr:uid="{D2EC8952-5BC9-2B49-B394-D7BE012603FF}"/>
+    <hyperlink ref="C299" r:id="rId274" xr:uid="{1B5D263F-5321-B54A-BF60-2932447DCE26}"/>
+    <hyperlink ref="C297" r:id="rId275" display="Storage Gateway - FSx File Gateway" xr:uid="{2125FCAA-C46E-224B-8BE0-19D32D161491}"/>
+    <hyperlink ref="C298" r:id="rId276" display="Storage Gateway - S3 File Gateway" xr:uid="{96B9D02E-E08D-3E44-9C8E-08A2BE24E99A}"/>
+    <hyperlink ref="C300" r:id="rId277" display="Storage Gateway - Volume Gateway" xr:uid="{FFBC4DD5-5D45-9B42-A545-70A2598E87B0}"/>
     <hyperlink ref="C23" r:id="rId278" xr:uid="{F8A9F9A7-CC98-EC42-8596-0253E0A2BB97}"/>
     <hyperlink ref="C22" r:id="rId279" xr:uid="{8B655CFD-0968-7140-84E8-2070B49F002B}"/>
     <hyperlink ref="C26" r:id="rId280" xr:uid="{FD22D76A-0562-0640-85D0-C48AA580C483}"/>
@@ -10868,16 +10952,19 @@
     <hyperlink ref="C112" r:id="rId284" xr:uid="{5961D4D9-3072-2149-961B-0C10629539E7}"/>
     <hyperlink ref="C86" r:id="rId285" xr:uid="{863934C0-971A-AF48-A43D-B4B914AECC39}"/>
     <hyperlink ref="C174" r:id="rId286" xr:uid="{3295CEB8-10D1-5A43-BEA9-DF5FD886C0AB}"/>
-    <hyperlink ref="C283" r:id="rId287" xr:uid="{4F9FE344-D5EC-AC40-97FF-2F5F45F27D96}"/>
+    <hyperlink ref="C286" r:id="rId287" xr:uid="{4F9FE344-D5EC-AC40-97FF-2F5F45F27D96}"/>
     <hyperlink ref="C189" r:id="rId288" xr:uid="{AEDB8326-231C-C744-8B10-AF02B678D9B4}"/>
     <hyperlink ref="C13" r:id="rId289" xr:uid="{2E249962-989F-944F-B761-2BAA0EC7CAEC}"/>
     <hyperlink ref="C165" r:id="rId290" xr:uid="{DCE5737A-9A5B-DC4D-850F-450E2D238525}"/>
     <hyperlink ref="C45" r:id="rId291" xr:uid="{FE31CE04-AE8C-B545-B85E-3E35079AA70A}"/>
-    <hyperlink ref="C243" r:id="rId292" xr:uid="{D321FD11-72A4-9F4D-857D-939FF8BB6E1B}"/>
-    <hyperlink ref="C252" r:id="rId293" xr:uid="{E997CB7A-902E-064D-B6FF-8470A806D5A0}"/>
-    <hyperlink ref="C255" r:id="rId294" xr:uid="{0A132D4A-E971-7246-889D-EB0D9E3ED74A}"/>
-    <hyperlink ref="C273" r:id="rId295" xr:uid="{5D89926F-F8DE-F748-ADBE-85B87EFE8273}"/>
+    <hyperlink ref="C246" r:id="rId292" xr:uid="{D321FD11-72A4-9F4D-857D-939FF8BB6E1B}"/>
+    <hyperlink ref="C255" r:id="rId293" xr:uid="{E997CB7A-902E-064D-B6FF-8470A806D5A0}"/>
+    <hyperlink ref="C258" r:id="rId294" xr:uid="{0A132D4A-E971-7246-889D-EB0D9E3ED74A}"/>
+    <hyperlink ref="C276" r:id="rId295" xr:uid="{5D89926F-F8DE-F748-ADBE-85B87EFE8273}"/>
     <hyperlink ref="C124" r:id="rId296" xr:uid="{2B14DC1E-31E9-E643-8322-E37BB77A61F2}"/>
+    <hyperlink ref="C237" r:id="rId297" xr:uid="{09886B01-263E-164A-BB8E-628947483324}"/>
+    <hyperlink ref="C238" r:id="rId298" xr:uid="{5F2F3CFC-7F4A-FD4D-941C-DED03BD1B5FC}"/>
+    <hyperlink ref="C229" r:id="rId299" xr:uid="{7C8F3176-C207-894A-B174-4BEF8A9DAF7C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
SApro official list, lex and elastic transcoder added
</commit_message>
<xml_diff>
--- a/aws-services-crib-sheet.xlsx
+++ b/aws-services-crib-sheet.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corbuno/WorkDocs/courses/aws-services-crib-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17916AF-F883-294D-BEE5-71FADAE5AAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2717418D-E3D1-9043-80B0-EA81C675FD9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="500" windowWidth="27800" windowHeight="17500" xr2:uid="{8DC9DE24-CECC-4748-B90E-52259685D84E}"/>
+    <workbookView xWindow="1020" yWindow="500" windowWidth="27780" windowHeight="17500" xr2:uid="{8DC9DE24-CECC-4748-B90E-52259685D84E}"/>
   </bookViews>
   <sheets>
     <sheet name="AWS Services" sheetId="1" r:id="rId1"/>
     <sheet name="source" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AWS Services'!$A$1:$Q$308</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AWS Services'!$A$1:$Q$310</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="353">
   <si>
     <t>CloudEndure Disaster Recovery</t>
   </si>
@@ -1082,6 +1082,12 @@
   </si>
   <si>
     <t>Genomics CLI</t>
+  </si>
+  <si>
+    <t>Lex</t>
+  </si>
+  <si>
+    <t>Elastic Transcoder</t>
   </si>
 </sst>
 </file>
@@ -1527,8 +1533,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFD15D16"/>
       <color rgb="FFB1094E"/>
-      <color rgb="FFD15D16"/>
       <color rgb="FF1F8901"/>
       <color rgb="FFC00A17"/>
       <color rgb="FF2F29AE"/>
@@ -1847,11 +1853,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00D01EA-5C3E-F64B-8B7F-2EE6141A689A}">
-  <dimension ref="A1:Q308"/>
+  <dimension ref="A1:Q310"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="E301" sqref="E301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2754,7 +2760,9 @@
       <c r="H29" s="17"/>
       <c r="I29" s="17"/>
       <c r="J29" s="17"/>
-      <c r="K29" s="17"/>
+      <c r="K29" s="17">
+        <v>1</v>
+      </c>
       <c r="L29" s="17"/>
       <c r="M29" s="17"/>
       <c r="N29" s="17"/>
@@ -2841,7 +2849,9 @@
       <c r="H32" s="17"/>
       <c r="I32" s="17"/>
       <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
+      <c r="K32" s="17">
+        <v>1</v>
+      </c>
       <c r="L32" s="17"/>
       <c r="M32" s="17"/>
       <c r="N32" s="17"/>
@@ -3022,7 +3032,9 @@
       <c r="H37" s="17"/>
       <c r="I37" s="17"/>
       <c r="J37" s="17"/>
-      <c r="K37" s="17"/>
+      <c r="K37" s="17">
+        <v>1</v>
+      </c>
       <c r="L37" s="17"/>
       <c r="M37" s="17"/>
       <c r="N37" s="17"/>
@@ -3045,7 +3057,9 @@
       <c r="H38" s="17"/>
       <c r="I38" s="17"/>
       <c r="J38" s="17"/>
-      <c r="K38" s="17"/>
+      <c r="K38" s="17">
+        <v>1</v>
+      </c>
       <c r="L38" s="17"/>
       <c r="M38" s="17"/>
       <c r="N38" s="17"/>
@@ -3431,7 +3445,9 @@
       <c r="H50" s="17"/>
       <c r="I50" s="17"/>
       <c r="J50" s="17"/>
-      <c r="K50" s="17"/>
+      <c r="K50" s="17">
+        <v>1</v>
+      </c>
       <c r="L50" s="17"/>
       <c r="M50" s="17"/>
       <c r="N50" s="17"/>
@@ -4018,9 +4034,7 @@
       <c r="J71" s="17">
         <v>1</v>
       </c>
-      <c r="K71" s="17">
-        <v>1</v>
-      </c>
+      <c r="K71" s="17"/>
       <c r="L71" s="17"/>
       <c r="M71" s="17"/>
       <c r="N71" s="17"/>
@@ -4278,7 +4292,9 @@
       <c r="H81" s="17"/>
       <c r="I81" s="17"/>
       <c r="J81" s="17"/>
-      <c r="K81" s="17"/>
+      <c r="K81" s="17">
+        <v>1</v>
+      </c>
       <c r="L81" s="17"/>
       <c r="M81" s="17"/>
       <c r="N81" s="17"/>
@@ -4416,7 +4432,9 @@
       <c r="D85" s="45"/>
       <c r="E85" s="45"/>
       <c r="F85" s="45"/>
-      <c r="G85" s="17"/>
+      <c r="G85" s="17">
+        <v>1</v>
+      </c>
       <c r="H85" s="17">
         <v>1</v>
       </c>
@@ -4567,7 +4585,9 @@
       <c r="H90" s="17"/>
       <c r="I90" s="17"/>
       <c r="J90" s="17"/>
-      <c r="K90" s="17"/>
+      <c r="K90" s="17">
+        <v>1</v>
+      </c>
       <c r="L90" s="17"/>
       <c r="M90" s="17"/>
       <c r="N90" s="17"/>
@@ -4843,7 +4863,9 @@
       <c r="H100" s="17"/>
       <c r="I100" s="17"/>
       <c r="J100" s="17"/>
-      <c r="K100" s="17"/>
+      <c r="K100" s="17">
+        <v>1</v>
+      </c>
       <c r="L100" s="17"/>
       <c r="M100" s="17"/>
       <c r="N100" s="17"/>
@@ -4924,7 +4946,9 @@
         <v>1</v>
       </c>
       <c r="J103" s="17"/>
-      <c r="K103" s="17"/>
+      <c r="K103" s="17">
+        <v>1</v>
+      </c>
       <c r="L103" s="17"/>
       <c r="M103" s="17"/>
       <c r="N103" s="17"/>
@@ -4953,7 +4977,9 @@
         <v>1</v>
       </c>
       <c r="J104" s="17"/>
-      <c r="K104" s="17"/>
+      <c r="K104" s="17">
+        <v>1</v>
+      </c>
       <c r="L104" s="17"/>
       <c r="M104" s="17"/>
       <c r="N104" s="17"/>
@@ -4982,7 +5008,9 @@
         <v>1</v>
       </c>
       <c r="J105" s="17"/>
-      <c r="K105" s="17"/>
+      <c r="K105" s="17">
+        <v>1</v>
+      </c>
       <c r="L105" s="17"/>
       <c r="M105" s="17"/>
       <c r="N105" s="17"/>
@@ -5038,7 +5066,9 @@
         <v>1</v>
       </c>
       <c r="J107" s="17"/>
-      <c r="K107" s="17"/>
+      <c r="K107" s="17">
+        <v>1</v>
+      </c>
       <c r="L107" s="17"/>
       <c r="M107" s="17"/>
       <c r="N107" s="17"/>
@@ -5327,7 +5357,9 @@
       <c r="H118" s="17"/>
       <c r="I118" s="17"/>
       <c r="J118" s="17"/>
-      <c r="K118" s="17"/>
+      <c r="K118" s="17">
+        <v>1</v>
+      </c>
       <c r="L118" s="17"/>
       <c r="M118" s="17"/>
       <c r="N118" s="17"/>
@@ -5379,7 +5411,9 @@
       <c r="H120" s="17"/>
       <c r="I120" s="17"/>
       <c r="J120" s="17"/>
-      <c r="K120" s="17"/>
+      <c r="K120" s="17">
+        <v>1</v>
+      </c>
       <c r="L120" s="17"/>
       <c r="M120" s="17"/>
       <c r="N120" s="17"/>
@@ -5804,7 +5838,9 @@
       <c r="H137" s="17"/>
       <c r="I137" s="17"/>
       <c r="J137" s="17"/>
-      <c r="K137" s="17"/>
+      <c r="K137" s="17">
+        <v>1</v>
+      </c>
       <c r="L137" s="17"/>
       <c r="M137" s="17"/>
       <c r="N137" s="17"/>
@@ -6014,7 +6050,9 @@
       <c r="H145" s="17"/>
       <c r="I145" s="17"/>
       <c r="J145" s="17"/>
-      <c r="K145" s="17"/>
+      <c r="K145" s="17">
+        <v>1</v>
+      </c>
       <c r="L145" s="17"/>
       <c r="M145" s="17"/>
       <c r="N145" s="17"/>
@@ -6084,7 +6122,7 @@
         <v>51</v>
       </c>
       <c r="C148" s="24" t="s">
-        <v>151</v>
+        <v>351</v>
       </c>
       <c r="D148" s="45"/>
       <c r="E148" s="45"/>
@@ -6093,7 +6131,9 @@
       <c r="H148" s="17"/>
       <c r="I148" s="17"/>
       <c r="J148" s="17"/>
-      <c r="K148" s="17"/>
+      <c r="K148" s="17">
+        <v>1</v>
+      </c>
       <c r="L148" s="17"/>
       <c r="M148" s="17"/>
       <c r="N148" s="17"/>
@@ -6106,10 +6146,10 @@
         <v>234</v>
       </c>
       <c r="B149" s="23" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C149" s="24" t="s">
-        <v>193</v>
+        <v>151</v>
       </c>
       <c r="D149" s="45"/>
       <c r="E149" s="45"/>
@@ -6131,10 +6171,10 @@
         <v>234</v>
       </c>
       <c r="B150" s="23" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C150" s="24" t="s">
-        <v>73</v>
+        <v>193</v>
       </c>
       <c r="D150" s="45"/>
       <c r="E150" s="45"/>
@@ -6147,9 +6187,7 @@
       <c r="L150" s="17"/>
       <c r="M150" s="17"/>
       <c r="N150" s="17"/>
-      <c r="O150" s="17">
-        <v>1</v>
-      </c>
+      <c r="O150" s="17"/>
       <c r="P150" s="17"/>
       <c r="Q150" s="17"/>
     </row>
@@ -6161,7 +6199,7 @@
         <v>51</v>
       </c>
       <c r="C151" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D151" s="45"/>
       <c r="E151" s="45"/>
@@ -6188,7 +6226,7 @@
         <v>51</v>
       </c>
       <c r="C152" s="24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D152" s="45"/>
       <c r="E152" s="45"/>
@@ -6215,7 +6253,7 @@
         <v>51</v>
       </c>
       <c r="C153" s="24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D153" s="45"/>
       <c r="E153" s="45"/>
@@ -6224,16 +6262,16 @@
       <c r="H153" s="17"/>
       <c r="I153" s="17"/>
       <c r="J153" s="17"/>
-      <c r="K153" s="17"/>
+      <c r="K153" s="17">
+        <v>1</v>
+      </c>
       <c r="L153" s="17"/>
       <c r="M153" s="17"/>
       <c r="N153" s="17"/>
       <c r="O153" s="17">
         <v>1</v>
       </c>
-      <c r="P153" s="17">
-        <v>1</v>
-      </c>
+      <c r="P153" s="17"/>
       <c r="Q153" s="17"/>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.2">
@@ -6244,7 +6282,7 @@
         <v>51</v>
       </c>
       <c r="C154" s="24" t="s">
-        <v>243</v>
+        <v>79</v>
       </c>
       <c r="D154" s="45"/>
       <c r="E154" s="45"/>
@@ -6253,14 +6291,18 @@
       <c r="H154" s="17"/>
       <c r="I154" s="17"/>
       <c r="J154" s="17"/>
-      <c r="K154" s="17"/>
+      <c r="K154" s="17">
+        <v>1</v>
+      </c>
       <c r="L154" s="17"/>
       <c r="M154" s="17"/>
       <c r="N154" s="17"/>
       <c r="O154" s="17">
         <v>1</v>
       </c>
-      <c r="P154" s="17"/>
+      <c r="P154" s="17">
+        <v>1</v>
+      </c>
       <c r="Q154" s="17"/>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.2">
@@ -6271,7 +6313,7 @@
         <v>51</v>
       </c>
       <c r="C155" s="24" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D155" s="45"/>
       <c r="E155" s="45"/>
@@ -6298,7 +6340,7 @@
         <v>51</v>
       </c>
       <c r="C156" s="24" t="s">
-        <v>191</v>
+        <v>241</v>
       </c>
       <c r="D156" s="45"/>
       <c r="E156" s="45"/>
@@ -6325,7 +6367,7 @@
         <v>51</v>
       </c>
       <c r="C157" s="24" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D157" s="45"/>
       <c r="E157" s="45"/>
@@ -6352,7 +6394,7 @@
         <v>51</v>
       </c>
       <c r="C158" s="24" t="s">
-        <v>244</v>
+        <v>196</v>
       </c>
       <c r="D158" s="45"/>
       <c r="E158" s="45"/>
@@ -6379,7 +6421,7 @@
         <v>51</v>
       </c>
       <c r="C159" s="24" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D159" s="45"/>
       <c r="E159" s="45"/>
@@ -6406,7 +6448,7 @@
         <v>51</v>
       </c>
       <c r="C160" s="24" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="D160" s="45"/>
       <c r="E160" s="45"/>
@@ -6433,7 +6475,7 @@
         <v>51</v>
       </c>
       <c r="C161" s="24" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D161" s="45"/>
       <c r="E161" s="45"/>
@@ -6460,7 +6502,7 @@
         <v>51</v>
       </c>
       <c r="C162" s="24" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D162" s="45"/>
       <c r="E162" s="45"/>
@@ -6487,7 +6529,7 @@
         <v>51</v>
       </c>
       <c r="C163" s="24" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="D163" s="45"/>
       <c r="E163" s="45"/>
@@ -6514,7 +6556,7 @@
         <v>51</v>
       </c>
       <c r="C164" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D164" s="45"/>
       <c r="E164" s="45"/>
@@ -6541,7 +6583,7 @@
         <v>51</v>
       </c>
       <c r="C165" s="24" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="D165" s="45"/>
       <c r="E165" s="45"/>
@@ -6568,7 +6610,7 @@
         <v>51</v>
       </c>
       <c r="C166" s="24" t="s">
-        <v>242</v>
+        <v>195</v>
       </c>
       <c r="D166" s="45"/>
       <c r="E166" s="45"/>
@@ -6595,7 +6637,7 @@
         <v>51</v>
       </c>
       <c r="C167" s="24" t="s">
-        <v>81</v>
+        <v>242</v>
       </c>
       <c r="D167" s="45"/>
       <c r="E167" s="45"/>
@@ -6622,7 +6664,7 @@
         <v>51</v>
       </c>
       <c r="C168" s="24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D168" s="45"/>
       <c r="E168" s="45"/>
@@ -6649,7 +6691,7 @@
         <v>51</v>
       </c>
       <c r="C169" s="24" t="s">
-        <v>160</v>
+        <v>83</v>
       </c>
       <c r="D169" s="45"/>
       <c r="E169" s="45"/>
@@ -6658,7 +6700,9 @@
       <c r="H169" s="17"/>
       <c r="I169" s="17"/>
       <c r="J169" s="17"/>
-      <c r="K169" s="17"/>
+      <c r="K169" s="17">
+        <v>1</v>
+      </c>
       <c r="L169" s="17"/>
       <c r="M169" s="17"/>
       <c r="N169" s="17"/>
@@ -6676,7 +6720,7 @@
         <v>51</v>
       </c>
       <c r="C170" s="24" t="s">
-        <v>84</v>
+        <v>160</v>
       </c>
       <c r="D170" s="45"/>
       <c r="E170" s="45"/>
@@ -6695,61 +6739,57 @@
       <c r="P170" s="17"/>
       <c r="Q170" s="17"/>
     </row>
-    <row r="171" spans="1:17" ht="19" x14ac:dyDescent="0.2">
-      <c r="A171" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B171" s="30"/>
-      <c r="C171" s="31" t="s">
-        <v>334</v>
+    <row r="171" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A171" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="B171" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C171" s="24" t="s">
+        <v>84</v>
       </c>
       <c r="D171" s="45"/>
-      <c r="E171" s="46"/>
+      <c r="E171" s="45"/>
       <c r="F171" s="45"/>
       <c r="G171" s="17"/>
       <c r="H171" s="17"/>
       <c r="I171" s="17"/>
-      <c r="J171" s="17">
-        <v>1</v>
-      </c>
-      <c r="K171" s="17"/>
+      <c r="J171" s="17"/>
+      <c r="K171" s="17">
+        <v>1</v>
+      </c>
       <c r="L171" s="17"/>
       <c r="M171" s="17"/>
       <c r="N171" s="17"/>
-      <c r="O171" s="17"/>
+      <c r="O171" s="17">
+        <v>1</v>
+      </c>
       <c r="P171" s="17"/>
       <c r="Q171" s="17"/>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:17" ht="19" x14ac:dyDescent="0.2">
       <c r="A172" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B172" s="30" t="s">
-        <v>6</v>
-      </c>
+      <c r="B172" s="30"/>
       <c r="C172" s="31" t="s">
-        <v>88</v>
+        <v>334</v>
       </c>
       <c r="D172" s="45"/>
-      <c r="E172" s="45"/>
+      <c r="E172" s="46"/>
       <c r="F172" s="45"/>
-      <c r="G172" s="17">
-        <v>1</v>
-      </c>
-      <c r="H172" s="17">
-        <v>1</v>
-      </c>
+      <c r="G172" s="17"/>
+      <c r="H172" s="17"/>
       <c r="I172" s="17"/>
-      <c r="J172" s="17"/>
-      <c r="K172" s="17">
-        <v>1</v>
-      </c>
+      <c r="J172" s="17">
+        <v>1</v>
+      </c>
+      <c r="K172" s="17"/>
       <c r="L172" s="17"/>
       <c r="M172" s="17"/>
       <c r="N172" s="17"/>
-      <c r="O172" s="17">
-        <v>1</v>
-      </c>
+      <c r="O172" s="17"/>
       <c r="P172" s="17"/>
       <c r="Q172" s="17"/>
     </row>
@@ -6761,7 +6801,7 @@
         <v>6</v>
       </c>
       <c r="C173" s="31" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
       <c r="D173" s="45"/>
       <c r="E173" s="45"/>
@@ -6773,16 +6813,16 @@
         <v>1</v>
       </c>
       <c r="I173" s="17"/>
-      <c r="J173" s="17">
-        <v>1</v>
-      </c>
+      <c r="J173" s="17"/>
       <c r="K173" s="17">
         <v>1</v>
       </c>
       <c r="L173" s="17"/>
       <c r="M173" s="17"/>
       <c r="N173" s="17"/>
-      <c r="O173" s="17"/>
+      <c r="O173" s="17">
+        <v>1</v>
+      </c>
       <c r="P173" s="17"/>
       <c r="Q173" s="17"/>
     </row>
@@ -6794,7 +6834,7 @@
         <v>6</v>
       </c>
       <c r="C174" s="31" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D174" s="45"/>
       <c r="E174" s="45"/>
@@ -6805,33 +6845,19 @@
       <c r="H174" s="17">
         <v>1</v>
       </c>
-      <c r="I174" s="17">
-        <v>1</v>
-      </c>
+      <c r="I174" s="17"/>
       <c r="J174" s="17">
         <v>1</v>
       </c>
       <c r="K174" s="17">
         <v>1</v>
       </c>
-      <c r="L174" s="17">
-        <v>1</v>
-      </c>
-      <c r="M174" s="17">
-        <v>1</v>
-      </c>
-      <c r="N174" s="17">
-        <v>1</v>
-      </c>
-      <c r="O174" s="17">
-        <v>1</v>
-      </c>
-      <c r="P174" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q174" s="17">
-        <v>1</v>
-      </c>
+      <c r="L174" s="17"/>
+      <c r="M174" s="17"/>
+      <c r="N174" s="17"/>
+      <c r="O174" s="17"/>
+      <c r="P174" s="17"/>
+      <c r="Q174" s="17"/>
     </row>
     <row r="175" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A175" s="29" t="s">
@@ -6841,7 +6867,7 @@
         <v>6</v>
       </c>
       <c r="C175" s="31" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D175" s="45"/>
       <c r="E175" s="45"/>
@@ -6861,26 +6887,34 @@
       <c r="K175" s="17">
         <v>1</v>
       </c>
-      <c r="L175" s="17"/>
+      <c r="L175" s="17">
+        <v>1</v>
+      </c>
       <c r="M175" s="17">
         <v>1</v>
       </c>
-      <c r="N175" s="17"/>
+      <c r="N175" s="17">
+        <v>1</v>
+      </c>
       <c r="O175" s="17">
         <v>1</v>
       </c>
-      <c r="P175" s="17"/>
-      <c r="Q175" s="17"/>
+      <c r="P175" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q175" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A176" s="29" t="s">
         <v>33</v>
       </c>
       <c r="B176" s="30" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C176" s="31" t="s">
-        <v>57</v>
+        <v>17</v>
       </c>
       <c r="D176" s="45"/>
       <c r="E176" s="45"/>
@@ -6900,51 +6934,63 @@
       <c r="K176" s="17">
         <v>1</v>
       </c>
-      <c r="L176" s="17">
-        <v>1</v>
-      </c>
+      <c r="L176" s="17"/>
       <c r="M176" s="17">
         <v>1</v>
       </c>
-      <c r="N176" s="17">
-        <v>1</v>
-      </c>
+      <c r="N176" s="17"/>
       <c r="O176" s="17">
         <v>1</v>
       </c>
-      <c r="P176" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q176" s="17">
-        <v>1</v>
-      </c>
+      <c r="P176" s="17"/>
+      <c r="Q176" s="17"/>
     </row>
     <row r="177" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A177" s="29" t="s">
         <v>33</v>
       </c>
       <c r="B177" s="30" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C177" s="31" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="D177" s="45"/>
       <c r="E177" s="45"/>
       <c r="F177" s="45"/>
-      <c r="G177" s="17"/>
-      <c r="H177" s="17"/>
-      <c r="I177" s="17"/>
+      <c r="G177" s="17">
+        <v>1</v>
+      </c>
+      <c r="H177" s="17">
+        <v>1</v>
+      </c>
+      <c r="I177" s="17">
+        <v>1</v>
+      </c>
       <c r="J177" s="17">
         <v>1</v>
       </c>
-      <c r="K177" s="17"/>
-      <c r="L177" s="17"/>
-      <c r="M177" s="17"/>
-      <c r="N177" s="17"/>
-      <c r="O177" s="17"/>
-      <c r="P177" s="17"/>
-      <c r="Q177" s="17"/>
+      <c r="K177" s="17">
+        <v>1</v>
+      </c>
+      <c r="L177" s="17">
+        <v>1</v>
+      </c>
+      <c r="M177" s="17">
+        <v>1</v>
+      </c>
+      <c r="N177" s="17">
+        <v>1</v>
+      </c>
+      <c r="O177" s="17">
+        <v>1</v>
+      </c>
+      <c r="P177" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q177" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="178" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A178" s="29" t="s">
@@ -6954,24 +7000,18 @@
         <v>6</v>
       </c>
       <c r="C178" s="31" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="D178" s="45"/>
       <c r="E178" s="45"/>
       <c r="F178" s="45"/>
-      <c r="G178" s="17">
-        <v>1</v>
-      </c>
-      <c r="H178" s="17">
-        <v>1</v>
-      </c>
+      <c r="G178" s="17"/>
+      <c r="H178" s="17"/>
       <c r="I178" s="17"/>
       <c r="J178" s="17">
         <v>1</v>
       </c>
-      <c r="K178" s="17">
-        <v>1</v>
-      </c>
+      <c r="K178" s="17"/>
       <c r="L178" s="17"/>
       <c r="M178" s="17"/>
       <c r="N178" s="17"/>
@@ -6987,16 +7027,24 @@
         <v>6</v>
       </c>
       <c r="C179" s="31" t="s">
-        <v>344</v>
+        <v>25</v>
       </c>
       <c r="D179" s="45"/>
       <c r="E179" s="45"/>
       <c r="F179" s="45"/>
-      <c r="G179" s="17"/>
-      <c r="H179" s="17"/>
+      <c r="G179" s="17">
+        <v>1</v>
+      </c>
+      <c r="H179" s="17">
+        <v>1</v>
+      </c>
       <c r="I179" s="17"/>
-      <c r="J179" s="17"/>
-      <c r="K179" s="17"/>
+      <c r="J179" s="17">
+        <v>1</v>
+      </c>
+      <c r="K179" s="17">
+        <v>1</v>
+      </c>
       <c r="L179" s="17"/>
       <c r="M179" s="17"/>
       <c r="N179" s="17"/>
@@ -7012,7 +7060,7 @@
         <v>6</v>
       </c>
       <c r="C180" s="31" t="s">
-        <v>91</v>
+        <v>344</v>
       </c>
       <c r="D180" s="45"/>
       <c r="E180" s="45"/>
@@ -7020,9 +7068,7 @@
       <c r="G180" s="17"/>
       <c r="H180" s="17"/>
       <c r="I180" s="17"/>
-      <c r="J180" s="17">
-        <v>1</v>
-      </c>
+      <c r="J180" s="17"/>
       <c r="K180" s="17"/>
       <c r="L180" s="17"/>
       <c r="M180" s="17"/>
@@ -7036,10 +7082,10 @@
         <v>33</v>
       </c>
       <c r="B181" s="30" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C181" s="31" t="s">
-        <v>329</v>
+        <v>91</v>
       </c>
       <c r="D181" s="45"/>
       <c r="E181" s="45"/>
@@ -7047,8 +7093,12 @@
       <c r="G181" s="17"/>
       <c r="H181" s="17"/>
       <c r="I181" s="17"/>
-      <c r="J181" s="17"/>
-      <c r="K181" s="17"/>
+      <c r="J181" s="17">
+        <v>1</v>
+      </c>
+      <c r="K181" s="17">
+        <v>1</v>
+      </c>
       <c r="L181" s="17"/>
       <c r="M181" s="17"/>
       <c r="N181" s="17"/>
@@ -7061,10 +7111,10 @@
         <v>33</v>
       </c>
       <c r="B182" s="30" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C182" s="31" t="s">
-        <v>302</v>
+        <v>329</v>
       </c>
       <c r="D182" s="45"/>
       <c r="E182" s="45"/>
@@ -7089,19 +7139,15 @@
         <v>6</v>
       </c>
       <c r="C183" s="31" t="s">
-        <v>111</v>
+        <v>302</v>
       </c>
       <c r="D183" s="45"/>
       <c r="E183" s="45"/>
       <c r="F183" s="45"/>
-      <c r="G183" s="17">
-        <v>1</v>
-      </c>
+      <c r="G183" s="17"/>
       <c r="H183" s="17"/>
       <c r="I183" s="17"/>
-      <c r="J183" s="17">
-        <v>1</v>
-      </c>
+      <c r="J183" s="17"/>
       <c r="K183" s="17"/>
       <c r="L183" s="17"/>
       <c r="M183" s="17"/>
@@ -7115,19 +7161,25 @@
         <v>33</v>
       </c>
       <c r="B184" s="30" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C184" s="31" t="s">
-        <v>220</v>
+        <v>111</v>
       </c>
       <c r="D184" s="45"/>
       <c r="E184" s="45"/>
       <c r="F184" s="45"/>
-      <c r="G184" s="17"/>
+      <c r="G184" s="17">
+        <v>1</v>
+      </c>
       <c r="H184" s="17"/>
       <c r="I184" s="17"/>
-      <c r="J184" s="17"/>
-      <c r="K184" s="17"/>
+      <c r="J184" s="17">
+        <v>1</v>
+      </c>
+      <c r="K184" s="17">
+        <v>1</v>
+      </c>
       <c r="L184" s="17"/>
       <c r="M184" s="17"/>
       <c r="N184" s="17"/>
@@ -7140,22 +7192,18 @@
         <v>33</v>
       </c>
       <c r="B185" s="30" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C185" s="31" t="s">
-        <v>273</v>
+        <v>220</v>
       </c>
       <c r="D185" s="45"/>
       <c r="E185" s="45"/>
       <c r="F185" s="45"/>
-      <c r="G185" s="17">
-        <v>1</v>
-      </c>
+      <c r="G185" s="17"/>
       <c r="H185" s="17"/>
       <c r="I185" s="17"/>
-      <c r="J185" s="17">
-        <v>1</v>
-      </c>
+      <c r="J185" s="17"/>
       <c r="K185" s="17"/>
       <c r="L185" s="17"/>
       <c r="M185" s="17"/>
@@ -7172,22 +7220,20 @@
         <v>6</v>
       </c>
       <c r="C186" s="31" t="s">
-        <v>114</v>
+        <v>273</v>
       </c>
       <c r="D186" s="45"/>
       <c r="E186" s="45"/>
       <c r="F186" s="45"/>
-      <c r="G186" s="17"/>
-      <c r="H186" s="17">
-        <v>1</v>
-      </c>
+      <c r="G186" s="17">
+        <v>1</v>
+      </c>
+      <c r="H186" s="17"/>
       <c r="I186" s="17"/>
       <c r="J186" s="17">
         <v>1</v>
       </c>
-      <c r="K186" s="17">
-        <v>1</v>
-      </c>
+      <c r="K186" s="17"/>
       <c r="L186" s="17"/>
       <c r="M186" s="17"/>
       <c r="N186" s="17"/>
@@ -7203,7 +7249,7 @@
         <v>6</v>
       </c>
       <c r="C187" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D187" s="45"/>
       <c r="E187" s="45"/>
@@ -7216,9 +7262,7 @@
       <c r="J187" s="17">
         <v>1</v>
       </c>
-      <c r="K187" s="17">
-        <v>1</v>
-      </c>
+      <c r="K187" s="17"/>
       <c r="L187" s="17"/>
       <c r="M187" s="17"/>
       <c r="N187" s="17"/>
@@ -7234,7 +7278,7 @@
         <v>6</v>
       </c>
       <c r="C188" s="31" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D188" s="45"/>
       <c r="E188" s="45"/>
@@ -7247,9 +7291,7 @@
       <c r="J188" s="17">
         <v>1</v>
       </c>
-      <c r="K188" s="17">
-        <v>1</v>
-      </c>
+      <c r="K188" s="17"/>
       <c r="L188" s="17"/>
       <c r="M188" s="17"/>
       <c r="N188" s="17"/>
@@ -7265,14 +7307,12 @@
         <v>6</v>
       </c>
       <c r="C189" s="31" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="D189" s="45"/>
       <c r="E189" s="45"/>
       <c r="F189" s="45"/>
-      <c r="G189" s="17">
-        <v>1</v>
-      </c>
+      <c r="G189" s="17"/>
       <c r="H189" s="17">
         <v>1</v>
       </c>
@@ -7280,9 +7320,7 @@
       <c r="J189" s="17">
         <v>1</v>
       </c>
-      <c r="K189" s="17">
-        <v>1</v>
-      </c>
+      <c r="K189" s="17"/>
       <c r="L189" s="17"/>
       <c r="M189" s="17"/>
       <c r="N189" s="17"/>
@@ -7298,7 +7336,7 @@
         <v>6</v>
       </c>
       <c r="C190" s="31" t="s">
-        <v>116</v>
+        <v>38</v>
       </c>
       <c r="D190" s="45"/>
       <c r="E190" s="45"/>
@@ -7306,12 +7344,16 @@
       <c r="G190" s="17">
         <v>1</v>
       </c>
-      <c r="H190" s="17"/>
+      <c r="H190" s="17">
+        <v>1</v>
+      </c>
       <c r="I190" s="17"/>
       <c r="J190" s="17">
         <v>1</v>
       </c>
-      <c r="K190" s="17"/>
+      <c r="K190" s="17">
+        <v>1</v>
+      </c>
       <c r="L190" s="17"/>
       <c r="M190" s="17"/>
       <c r="N190" s="17"/>
@@ -7327,20 +7369,20 @@
         <v>6</v>
       </c>
       <c r="C191" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D191" s="45"/>
       <c r="E191" s="45"/>
       <c r="F191" s="45"/>
-      <c r="G191" s="17"/>
-      <c r="H191" s="17">
-        <v>1</v>
-      </c>
+      <c r="G191" s="17">
+        <v>1</v>
+      </c>
+      <c r="H191" s="17"/>
       <c r="I191" s="17"/>
-      <c r="J191" s="17"/>
-      <c r="K191" s="17">
-        <v>1</v>
-      </c>
+      <c r="J191" s="17">
+        <v>1</v>
+      </c>
+      <c r="K191" s="17"/>
       <c r="L191" s="17"/>
       <c r="M191" s="17"/>
       <c r="N191" s="17"/>
@@ -7356,23 +7398,21 @@
         <v>6</v>
       </c>
       <c r="C192" s="31" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="D192" s="45"/>
       <c r="E192" s="45"/>
       <c r="F192" s="45"/>
       <c r="G192" s="17"/>
-      <c r="H192" s="17"/>
+      <c r="H192" s="17">
+        <v>1</v>
+      </c>
       <c r="I192" s="17"/>
-      <c r="J192" s="17">
-        <v>1</v>
-      </c>
+      <c r="J192" s="17"/>
       <c r="K192" s="17">
         <v>1</v>
       </c>
-      <c r="L192" s="17">
-        <v>1</v>
-      </c>
+      <c r="L192" s="17"/>
       <c r="M192" s="17"/>
       <c r="N192" s="17"/>
       <c r="O192" s="17"/>
@@ -7387,7 +7427,7 @@
         <v>6</v>
       </c>
       <c r="C193" s="31" t="s">
-        <v>247</v>
+        <v>122</v>
       </c>
       <c r="D193" s="45"/>
       <c r="E193" s="45"/>
@@ -7398,7 +7438,9 @@
       <c r="J193" s="17">
         <v>1</v>
       </c>
-      <c r="K193" s="17"/>
+      <c r="K193" s="17">
+        <v>1</v>
+      </c>
       <c r="L193" s="17">
         <v>1</v>
       </c>
@@ -7416,7 +7458,7 @@
         <v>6</v>
       </c>
       <c r="C194" s="31" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D194" s="45"/>
       <c r="E194" s="45"/>
@@ -7445,7 +7487,7 @@
         <v>6</v>
       </c>
       <c r="C195" s="31" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D195" s="45"/>
       <c r="E195" s="45"/>
@@ -7474,7 +7516,7 @@
         <v>6</v>
       </c>
       <c r="C196" s="31" t="s">
-        <v>331</v>
+        <v>254</v>
       </c>
       <c r="D196" s="45"/>
       <c r="E196" s="45"/>
@@ -7482,9 +7524,13 @@
       <c r="G196" s="17"/>
       <c r="H196" s="17"/>
       <c r="I196" s="17"/>
-      <c r="J196" s="17"/>
+      <c r="J196" s="17">
+        <v>1</v>
+      </c>
       <c r="K196" s="17"/>
-      <c r="L196" s="17"/>
+      <c r="L196" s="17">
+        <v>1</v>
+      </c>
       <c r="M196" s="17"/>
       <c r="N196" s="17"/>
       <c r="O196" s="17"/>
@@ -7499,7 +7545,7 @@
         <v>6</v>
       </c>
       <c r="C197" s="31" t="s">
-        <v>253</v>
+        <v>331</v>
       </c>
       <c r="D197" s="45"/>
       <c r="E197" s="45"/>
@@ -7509,9 +7555,7 @@
       <c r="I197" s="17"/>
       <c r="J197" s="17"/>
       <c r="K197" s="17"/>
-      <c r="L197" s="17">
-        <v>1</v>
-      </c>
+      <c r="L197" s="17"/>
       <c r="M197" s="17"/>
       <c r="N197" s="17"/>
       <c r="O197" s="17"/>
@@ -7526,7 +7570,7 @@
         <v>6</v>
       </c>
       <c r="C198" s="31" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D198" s="45"/>
       <c r="E198" s="45"/>
@@ -7553,7 +7597,7 @@
         <v>6</v>
       </c>
       <c r="C199" s="31" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D199" s="45"/>
       <c r="E199" s="45"/>
@@ -7580,7 +7624,7 @@
         <v>6</v>
       </c>
       <c r="C200" s="31" t="s">
-        <v>249</v>
+        <v>263</v>
       </c>
       <c r="D200" s="45"/>
       <c r="E200" s="45"/>
@@ -7607,7 +7651,7 @@
         <v>6</v>
       </c>
       <c r="C201" s="31" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D201" s="45"/>
       <c r="E201" s="45"/>
@@ -7634,7 +7678,7 @@
         <v>6</v>
       </c>
       <c r="C202" s="31" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D202" s="45"/>
       <c r="E202" s="45"/>
@@ -7661,7 +7705,7 @@
         <v>6</v>
       </c>
       <c r="C203" s="31" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="D203" s="45"/>
       <c r="E203" s="45"/>
@@ -7688,11 +7732,11 @@
         <v>6</v>
       </c>
       <c r="C204" s="31" t="s">
-        <v>250</v>
-      </c>
-      <c r="D204" s="47"/>
-      <c r="E204" s="47"/>
-      <c r="F204" s="47"/>
+        <v>255</v>
+      </c>
+      <c r="D204" s="45"/>
+      <c r="E204" s="45"/>
+      <c r="F204" s="45"/>
       <c r="G204" s="17"/>
       <c r="H204" s="17"/>
       <c r="I204" s="17"/>
@@ -7715,24 +7759,16 @@
         <v>6</v>
       </c>
       <c r="C205" s="31" t="s">
-        <v>252</v>
-      </c>
-      <c r="D205" s="45"/>
-      <c r="E205" s="45"/>
-      <c r="F205" s="45"/>
-      <c r="G205" s="17">
-        <v>1</v>
-      </c>
-      <c r="H205" s="17">
-        <v>1</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="D205" s="47"/>
+      <c r="E205" s="47"/>
+      <c r="F205" s="47"/>
+      <c r="G205" s="17"/>
+      <c r="H205" s="17"/>
       <c r="I205" s="17"/>
-      <c r="J205" s="17">
-        <v>1</v>
-      </c>
-      <c r="K205" s="17">
-        <v>1</v>
-      </c>
+      <c r="J205" s="17"/>
+      <c r="K205" s="17"/>
       <c r="L205" s="17">
         <v>1</v>
       </c>
@@ -7750,16 +7786,24 @@
         <v>6</v>
       </c>
       <c r="C206" s="31" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="D206" s="45"/>
       <c r="E206" s="45"/>
       <c r="F206" s="45"/>
-      <c r="G206" s="17"/>
-      <c r="H206" s="17"/>
+      <c r="G206" s="17">
+        <v>1</v>
+      </c>
+      <c r="H206" s="17">
+        <v>1</v>
+      </c>
       <c r="I206" s="17"/>
-      <c r="J206" s="17"/>
-      <c r="K206" s="17"/>
+      <c r="J206" s="17">
+        <v>1</v>
+      </c>
+      <c r="K206" s="17">
+        <v>1</v>
+      </c>
       <c r="L206" s="17">
         <v>1</v>
       </c>
@@ -7777,7 +7821,7 @@
         <v>6</v>
       </c>
       <c r="C207" s="31" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D207" s="45"/>
       <c r="E207" s="45"/>
@@ -7804,7 +7848,7 @@
         <v>6</v>
       </c>
       <c r="C208" s="31" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D208" s="45"/>
       <c r="E208" s="45"/>
@@ -7831,7 +7875,7 @@
         <v>6</v>
       </c>
       <c r="C209" s="31" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D209" s="45"/>
       <c r="E209" s="45"/>
@@ -7858,24 +7902,16 @@
         <v>6</v>
       </c>
       <c r="C210" s="31" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
       <c r="D210" s="45"/>
       <c r="E210" s="45"/>
       <c r="F210" s="45"/>
-      <c r="G210" s="17">
-        <v>1</v>
-      </c>
-      <c r="H210" s="17">
-        <v>1</v>
-      </c>
+      <c r="G210" s="17"/>
+      <c r="H210" s="17"/>
       <c r="I210" s="17"/>
-      <c r="J210" s="17">
-        <v>1</v>
-      </c>
-      <c r="K210" s="17">
-        <v>1</v>
-      </c>
+      <c r="J210" s="17"/>
+      <c r="K210" s="17"/>
       <c r="L210" s="17">
         <v>1</v>
       </c>
@@ -7893,7 +7929,7 @@
         <v>6</v>
       </c>
       <c r="C211" s="31" t="s">
-        <v>127</v>
+        <v>246</v>
       </c>
       <c r="D211" s="45"/>
       <c r="E211" s="45"/>
@@ -7911,13 +7947,13 @@
       <c r="K211" s="17">
         <v>1</v>
       </c>
-      <c r="L211" s="17"/>
+      <c r="L211" s="17">
+        <v>1</v>
+      </c>
       <c r="M211" s="17"/>
       <c r="N211" s="17"/>
       <c r="O211" s="17"/>
-      <c r="P211" s="17">
-        <v>1</v>
-      </c>
+      <c r="P211" s="17"/>
       <c r="Q211" s="17"/>
     </row>
     <row r="212" spans="1:17" x14ac:dyDescent="0.2">
@@ -7928,32 +7964,42 @@
         <v>6</v>
       </c>
       <c r="C212" s="31" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D212" s="45"/>
       <c r="E212" s="45"/>
       <c r="F212" s="45"/>
-      <c r="G212" s="17"/>
-      <c r="H212" s="17"/>
+      <c r="G212" s="17">
+        <v>1</v>
+      </c>
+      <c r="H212" s="17">
+        <v>1</v>
+      </c>
       <c r="I212" s="17"/>
-      <c r="J212" s="17"/>
-      <c r="K212" s="17"/>
+      <c r="J212" s="17">
+        <v>1</v>
+      </c>
+      <c r="K212" s="17">
+        <v>1</v>
+      </c>
       <c r="L212" s="17"/>
       <c r="M212" s="17"/>
       <c r="N212" s="17"/>
       <c r="O212" s="17"/>
-      <c r="P212" s="17"/>
+      <c r="P212" s="17">
+        <v>1</v>
+      </c>
       <c r="Q212" s="17"/>
     </row>
     <row r="213" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A213" s="14" t="s">
-        <v>290</v>
-      </c>
-      <c r="B213" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C213" s="16" t="s">
-        <v>298</v>
+      <c r="A213" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B213" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C213" s="31" t="s">
+        <v>128</v>
       </c>
       <c r="D213" s="45"/>
       <c r="E213" s="45"/>
@@ -7962,7 +8008,9 @@
       <c r="H213" s="17"/>
       <c r="I213" s="17"/>
       <c r="J213" s="17"/>
-      <c r="K213" s="17"/>
+      <c r="K213" s="17">
+        <v>1</v>
+      </c>
       <c r="L213" s="17"/>
       <c r="M213" s="17"/>
       <c r="N213" s="17"/>
@@ -7975,10 +8023,10 @@
         <v>290</v>
       </c>
       <c r="B214" s="15" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C214" s="16" t="s">
-        <v>294</v>
+        <v>352</v>
       </c>
       <c r="D214" s="45"/>
       <c r="E214" s="45"/>
@@ -7987,7 +8035,9 @@
       <c r="H214" s="17"/>
       <c r="I214" s="17"/>
       <c r="J214" s="17"/>
-      <c r="K214" s="17"/>
+      <c r="K214" s="17">
+        <v>1</v>
+      </c>
       <c r="L214" s="17"/>
       <c r="M214" s="17"/>
       <c r="N214" s="17"/>
@@ -8003,7 +8053,7 @@
         <v>6</v>
       </c>
       <c r="C215" s="16" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="D215" s="45"/>
       <c r="E215" s="45"/>
@@ -8028,7 +8078,7 @@
         <v>6</v>
       </c>
       <c r="C216" s="16" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D216" s="45"/>
       <c r="E216" s="45"/>
@@ -8053,7 +8103,7 @@
         <v>6</v>
       </c>
       <c r="C217" s="16" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D217" s="45"/>
       <c r="E217" s="45"/>
@@ -8078,7 +8128,7 @@
         <v>6</v>
       </c>
       <c r="C218" s="16" t="s">
-        <v>96</v>
+        <v>300</v>
       </c>
       <c r="D218" s="45"/>
       <c r="E218" s="45"/>
@@ -8103,7 +8153,7 @@
         <v>6</v>
       </c>
       <c r="C219" s="16" t="s">
-        <v>97</v>
+        <v>296</v>
       </c>
       <c r="D219" s="45"/>
       <c r="E219" s="45"/>
@@ -8128,7 +8178,7 @@
         <v>6</v>
       </c>
       <c r="C220" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D220" s="45"/>
       <c r="E220" s="45"/>
@@ -8153,7 +8203,7 @@
         <v>6</v>
       </c>
       <c r="C221" s="16" t="s">
-        <v>293</v>
+        <v>97</v>
       </c>
       <c r="D221" s="45"/>
       <c r="E221" s="45"/>
@@ -8178,7 +8228,7 @@
         <v>6</v>
       </c>
       <c r="C222" s="16" t="s">
-        <v>240</v>
+        <v>98</v>
       </c>
       <c r="D222" s="45"/>
       <c r="E222" s="45"/>
@@ -8203,7 +8253,7 @@
         <v>6</v>
       </c>
       <c r="C223" s="16" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="D223" s="45"/>
       <c r="E223" s="45"/>
@@ -8228,7 +8278,7 @@
         <v>6</v>
       </c>
       <c r="C224" s="16" t="s">
-        <v>297</v>
+        <v>240</v>
       </c>
       <c r="D224" s="45"/>
       <c r="E224" s="45"/>
@@ -8250,10 +8300,10 @@
         <v>290</v>
       </c>
       <c r="B225" s="15" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C225" s="16" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="D225" s="45"/>
       <c r="E225" s="45"/>
@@ -8275,10 +8325,10 @@
         <v>290</v>
       </c>
       <c r="B226" s="15" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C226" s="16" t="s">
-        <v>327</v>
+        <v>297</v>
       </c>
       <c r="D226" s="45"/>
       <c r="E226" s="45"/>
@@ -8303,7 +8353,7 @@
         <v>51</v>
       </c>
       <c r="C227" s="16" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="D227" s="45"/>
       <c r="E227" s="45"/>
@@ -8325,10 +8375,10 @@
         <v>290</v>
       </c>
       <c r="B228" s="15" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C228" s="16" t="s">
-        <v>306</v>
+        <v>327</v>
       </c>
       <c r="D228" s="45"/>
       <c r="E228" s="45"/>
@@ -8350,10 +8400,10 @@
         <v>290</v>
       </c>
       <c r="B229" s="15" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C229" s="16" t="s">
-        <v>308</v>
+        <v>291</v>
       </c>
       <c r="D229" s="45"/>
       <c r="E229" s="45"/>
@@ -8378,7 +8428,7 @@
         <v>6</v>
       </c>
       <c r="C230" s="16" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="D230" s="45"/>
       <c r="E230" s="45"/>
@@ -8403,7 +8453,7 @@
         <v>6</v>
       </c>
       <c r="C231" s="16" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D231" s="45"/>
       <c r="E231" s="45"/>
@@ -8428,7 +8478,7 @@
         <v>6</v>
       </c>
       <c r="C232" s="16" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D232" s="45"/>
       <c r="E232" s="45"/>
@@ -8453,7 +8503,7 @@
         <v>6</v>
       </c>
       <c r="C233" s="16" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="D233" s="45"/>
       <c r="E233" s="45"/>
@@ -8471,14 +8521,14 @@
       <c r="Q233" s="17"/>
     </row>
     <row r="234" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A234" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B234" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C234" s="24" t="s">
-        <v>304</v>
+      <c r="A234" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="B234" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C234" s="16" t="s">
+        <v>311</v>
       </c>
       <c r="D234" s="45"/>
       <c r="E234" s="45"/>
@@ -8496,12 +8546,14 @@
       <c r="Q234" s="17"/>
     </row>
     <row r="235" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A235" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B235" s="32"/>
-      <c r="C235" s="24" t="s">
-        <v>1</v>
+      <c r="A235" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="B235" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C235" s="16" t="s">
+        <v>307</v>
       </c>
       <c r="D235" s="45"/>
       <c r="E235" s="45"/>
@@ -8526,7 +8578,7 @@
         <v>6</v>
       </c>
       <c r="C236" s="24" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="D236" s="45"/>
       <c r="E236" s="45"/>
@@ -8551,7 +8603,7 @@
         <v>6</v>
       </c>
       <c r="C237" s="24" t="s">
-        <v>92</v>
+        <v>343</v>
       </c>
       <c r="D237" s="45"/>
       <c r="E237" s="45"/>
@@ -8572,29 +8624,23 @@
       <c r="A238" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B238" s="23" t="s">
-        <v>6</v>
-      </c>
+      <c r="B238" s="32"/>
       <c r="C238" s="24" t="s">
-        <v>265</v>
+        <v>1</v>
       </c>
       <c r="D238" s="45"/>
       <c r="E238" s="45"/>
       <c r="F238" s="45"/>
       <c r="G238" s="17"/>
       <c r="H238" s="17"/>
-      <c r="I238" s="17">
-        <v>1</v>
-      </c>
+      <c r="I238" s="17"/>
       <c r="J238" s="17"/>
       <c r="K238" s="17"/>
       <c r="L238" s="17"/>
       <c r="M238" s="17"/>
       <c r="N238" s="17"/>
       <c r="O238" s="17"/>
-      <c r="P238" s="17">
-        <v>1</v>
-      </c>
+      <c r="P238" s="17"/>
       <c r="Q238" s="17"/>
     </row>
     <row r="239" spans="1:17" x14ac:dyDescent="0.2">
@@ -8605,32 +8651,22 @@
         <v>6</v>
       </c>
       <c r="C239" s="24" t="s">
-        <v>276</v>
+        <v>92</v>
       </c>
       <c r="D239" s="45"/>
       <c r="E239" s="45"/>
       <c r="F239" s="45"/>
-      <c r="G239" s="17">
-        <v>1</v>
-      </c>
-      <c r="H239" s="17">
-        <v>1</v>
-      </c>
+      <c r="G239" s="17"/>
+      <c r="H239" s="17"/>
       <c r="I239" s="17"/>
       <c r="J239" s="17"/>
-      <c r="K239" s="17">
-        <v>1</v>
-      </c>
+      <c r="K239" s="17"/>
       <c r="L239" s="17"/>
       <c r="M239" s="17"/>
       <c r="N239" s="17"/>
       <c r="O239" s="17"/>
-      <c r="P239" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q239" s="17">
-        <v>1</v>
-      </c>
+      <c r="P239" s="17"/>
+      <c r="Q239" s="17"/>
     </row>
     <row r="240" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A240" s="22" t="s">
@@ -8640,22 +8676,18 @@
         <v>6</v>
       </c>
       <c r="C240" s="24" t="s">
-        <v>26</v>
+        <v>265</v>
       </c>
       <c r="D240" s="45"/>
       <c r="E240" s="45"/>
       <c r="F240" s="45"/>
       <c r="G240" s="17"/>
-      <c r="H240" s="17">
-        <v>1</v>
-      </c>
-      <c r="I240" s="17"/>
-      <c r="J240" s="17">
-        <v>1</v>
-      </c>
-      <c r="K240" s="17">
-        <v>1</v>
-      </c>
+      <c r="H240" s="17"/>
+      <c r="I240" s="17">
+        <v>1</v>
+      </c>
+      <c r="J240" s="17"/>
+      <c r="K240" s="17"/>
       <c r="L240" s="17"/>
       <c r="M240" s="17"/>
       <c r="N240" s="17"/>
@@ -8673,7 +8705,7 @@
         <v>6</v>
       </c>
       <c r="C241" s="24" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D241" s="45"/>
       <c r="E241" s="45"/>
@@ -8693,7 +8725,9 @@
       <c r="M241" s="17"/>
       <c r="N241" s="17"/>
       <c r="O241" s="17"/>
-      <c r="P241" s="17"/>
+      <c r="P241" s="17">
+        <v>1</v>
+      </c>
       <c r="Q241" s="17">
         <v>1</v>
       </c>
@@ -8702,23 +8736,33 @@
       <c r="A242" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B242" s="23"/>
+      <c r="B242" s="23" t="s">
+        <v>6</v>
+      </c>
       <c r="C242" s="24" t="s">
-        <v>222</v>
+        <v>26</v>
       </c>
       <c r="D242" s="45"/>
       <c r="E242" s="45"/>
       <c r="F242" s="45"/>
       <c r="G242" s="17"/>
-      <c r="H242" s="17"/>
+      <c r="H242" s="17">
+        <v>1</v>
+      </c>
       <c r="I242" s="17"/>
-      <c r="J242" s="17"/>
-      <c r="K242" s="17"/>
+      <c r="J242" s="17">
+        <v>1</v>
+      </c>
+      <c r="K242" s="17">
+        <v>1</v>
+      </c>
       <c r="L242" s="17"/>
       <c r="M242" s="17"/>
       <c r="N242" s="17"/>
       <c r="O242" s="17"/>
-      <c r="P242" s="17"/>
+      <c r="P242" s="17">
+        <v>1</v>
+      </c>
       <c r="Q242" s="17"/>
     </row>
     <row r="243" spans="1:17" x14ac:dyDescent="0.2">
@@ -8729,12 +8773,14 @@
         <v>6</v>
       </c>
       <c r="C243" s="24" t="s">
-        <v>221</v>
+        <v>277</v>
       </c>
       <c r="D243" s="45"/>
       <c r="E243" s="45"/>
       <c r="F243" s="45"/>
-      <c r="G243" s="17"/>
+      <c r="G243" s="17">
+        <v>1</v>
+      </c>
       <c r="H243" s="17">
         <v>1</v>
       </c>
@@ -8748,17 +8794,17 @@
       <c r="N243" s="17"/>
       <c r="O243" s="17"/>
       <c r="P243" s="17"/>
-      <c r="Q243" s="17"/>
+      <c r="Q243" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="244" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A244" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B244" s="23" t="s">
-        <v>6</v>
-      </c>
+      <c r="B244" s="23"/>
       <c r="C244" s="24" t="s">
-        <v>341</v>
+        <v>222</v>
       </c>
       <c r="D244" s="45"/>
       <c r="E244" s="45"/>
@@ -8783,16 +8829,20 @@
         <v>6</v>
       </c>
       <c r="C245" s="24" t="s">
-        <v>342</v>
+        <v>221</v>
       </c>
       <c r="D245" s="45"/>
       <c r="E245" s="45"/>
       <c r="F245" s="45"/>
       <c r="G245" s="17"/>
-      <c r="H245" s="17"/>
+      <c r="H245" s="17">
+        <v>1</v>
+      </c>
       <c r="I245" s="17"/>
       <c r="J245" s="17"/>
-      <c r="K245" s="17"/>
+      <c r="K245" s="17">
+        <v>1</v>
+      </c>
       <c r="L245" s="17"/>
       <c r="M245" s="17"/>
       <c r="N245" s="17"/>
@@ -8808,20 +8858,16 @@
         <v>6</v>
       </c>
       <c r="C246" s="24" t="s">
-        <v>120</v>
+        <v>341</v>
       </c>
       <c r="D246" s="45"/>
       <c r="E246" s="45"/>
       <c r="F246" s="45"/>
       <c r="G246" s="17"/>
-      <c r="H246" s="17">
-        <v>1</v>
-      </c>
+      <c r="H246" s="17"/>
       <c r="I246" s="17"/>
       <c r="J246" s="17"/>
-      <c r="K246" s="17">
-        <v>1</v>
-      </c>
+      <c r="K246" s="17"/>
       <c r="L246" s="17"/>
       <c r="M246" s="17"/>
       <c r="N246" s="17"/>
@@ -8837,29 +8883,21 @@
         <v>6</v>
       </c>
       <c r="C247" s="24" t="s">
-        <v>45</v>
+        <v>342</v>
       </c>
       <c r="D247" s="45"/>
       <c r="E247" s="45"/>
       <c r="F247" s="45"/>
-      <c r="G247" s="17">
-        <v>1</v>
-      </c>
-      <c r="H247" s="17">
-        <v>1</v>
-      </c>
+      <c r="G247" s="17"/>
+      <c r="H247" s="17"/>
       <c r="I247" s="17"/>
       <c r="J247" s="17"/>
-      <c r="K247" s="17">
-        <v>1</v>
-      </c>
+      <c r="K247" s="17"/>
       <c r="L247" s="17"/>
       <c r="M247" s="17"/>
       <c r="N247" s="17"/>
       <c r="O247" s="17"/>
-      <c r="P247" s="17">
-        <v>1</v>
-      </c>
+      <c r="P247" s="17"/>
       <c r="Q247" s="17"/>
     </row>
     <row r="248" spans="1:17" x14ac:dyDescent="0.2">
@@ -8870,18 +8908,20 @@
         <v>6</v>
       </c>
       <c r="C248" s="24" t="s">
-        <v>226</v>
+        <v>120</v>
       </c>
       <c r="D248" s="45"/>
       <c r="E248" s="45"/>
       <c r="F248" s="45"/>
-      <c r="G248" s="17">
-        <v>1</v>
-      </c>
-      <c r="H248" s="17"/>
+      <c r="G248" s="17"/>
+      <c r="H248" s="17">
+        <v>1</v>
+      </c>
       <c r="I248" s="17"/>
       <c r="J248" s="17"/>
-      <c r="K248" s="17"/>
+      <c r="K248" s="17">
+        <v>1</v>
+      </c>
       <c r="L248" s="17"/>
       <c r="M248" s="17"/>
       <c r="N248" s="17"/>
@@ -8897,7 +8937,7 @@
         <v>6</v>
       </c>
       <c r="C249" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D249" s="45"/>
       <c r="E249" s="45"/>
@@ -8917,7 +8957,9 @@
       <c r="M249" s="17"/>
       <c r="N249" s="17"/>
       <c r="O249" s="17"/>
-      <c r="P249" s="17"/>
+      <c r="P249" s="17">
+        <v>1</v>
+      </c>
       <c r="Q249" s="17"/>
     </row>
     <row r="250" spans="1:17" x14ac:dyDescent="0.2">
@@ -8928,40 +8970,34 @@
         <v>6</v>
       </c>
       <c r="C250" s="24" t="s">
-        <v>125</v>
+        <v>226</v>
       </c>
       <c r="D250" s="45"/>
       <c r="E250" s="45"/>
       <c r="F250" s="45"/>
-      <c r="G250" s="17"/>
-      <c r="H250" s="17">
-        <v>1</v>
-      </c>
+      <c r="G250" s="17">
+        <v>1</v>
+      </c>
+      <c r="H250" s="17"/>
       <c r="I250" s="17"/>
-      <c r="J250" s="17">
-        <v>1</v>
-      </c>
-      <c r="K250" s="17">
-        <v>1</v>
-      </c>
+      <c r="J250" s="17"/>
+      <c r="K250" s="17"/>
       <c r="L250" s="17"/>
       <c r="M250" s="17"/>
       <c r="N250" s="17"/>
       <c r="O250" s="17"/>
-      <c r="P250" s="17">
-        <v>1</v>
-      </c>
+      <c r="P250" s="17"/>
       <c r="Q250" s="17"/>
     </row>
     <row r="251" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A251" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="B251" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="C251" s="35" t="s">
-        <v>129</v>
+      <c r="A251" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B251" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C251" s="24" t="s">
+        <v>46</v>
       </c>
       <c r="D251" s="45"/>
       <c r="E251" s="45"/>
@@ -8972,53 +9008,47 @@
       <c r="H251" s="17">
         <v>1</v>
       </c>
-      <c r="I251" s="17">
-        <v>1</v>
-      </c>
+      <c r="I251" s="17"/>
       <c r="J251" s="17"/>
-      <c r="K251" s="17">
-        <v>1</v>
-      </c>
-      <c r="L251" s="17">
-        <v>1</v>
-      </c>
-      <c r="M251" s="17">
-        <v>1</v>
-      </c>
-      <c r="N251" s="17">
-        <v>1</v>
-      </c>
+      <c r="K251" s="17"/>
+      <c r="L251" s="17"/>
+      <c r="M251" s="17"/>
+      <c r="N251" s="17"/>
       <c r="O251" s="17"/>
-      <c r="P251" s="17">
-        <v>1</v>
-      </c>
+      <c r="P251" s="17"/>
       <c r="Q251" s="17"/>
     </row>
     <row r="252" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A252" s="33" t="s">
-        <v>169</v>
-      </c>
-      <c r="B252" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="C252" s="35" t="s">
-        <v>86</v>
+      <c r="A252" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="B252" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C252" s="24" t="s">
+        <v>125</v>
       </c>
       <c r="D252" s="45"/>
       <c r="E252" s="45"/>
       <c r="F252" s="45"/>
       <c r="G252" s="17"/>
-      <c r="H252" s="17"/>
+      <c r="H252" s="17">
+        <v>1</v>
+      </c>
       <c r="I252" s="17"/>
-      <c r="J252" s="17"/>
-      <c r="K252" s="17"/>
+      <c r="J252" s="17">
+        <v>1</v>
+      </c>
+      <c r="K252" s="17">
+        <v>1</v>
+      </c>
       <c r="L252" s="17"/>
       <c r="M252" s="17"/>
-      <c r="N252" s="17">
-        <v>1</v>
-      </c>
+      <c r="N252" s="17"/>
       <c r="O252" s="17"/>
-      <c r="P252" s="17"/>
+      <c r="P252" s="17">
+        <v>1</v>
+      </c>
       <c r="Q252" s="17"/>
     </row>
     <row r="253" spans="1:17" x14ac:dyDescent="0.2">
@@ -9026,26 +9056,40 @@
         <v>169</v>
       </c>
       <c r="B253" s="34" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C253" s="35" t="s">
-        <v>336</v>
+        <v>129</v>
       </c>
       <c r="D253" s="45"/>
       <c r="E253" s="45"/>
       <c r="F253" s="45"/>
-      <c r="G253" s="17"/>
-      <c r="H253" s="17"/>
-      <c r="I253" s="17"/>
-      <c r="J253" s="17">
-        <v>1</v>
-      </c>
-      <c r="K253" s="17"/>
-      <c r="L253" s="17"/>
-      <c r="M253" s="17"/>
-      <c r="N253" s="17"/>
+      <c r="G253" s="17">
+        <v>1</v>
+      </c>
+      <c r="H253" s="17">
+        <v>1</v>
+      </c>
+      <c r="I253" s="17">
+        <v>1</v>
+      </c>
+      <c r="J253" s="17"/>
+      <c r="K253" s="17">
+        <v>1</v>
+      </c>
+      <c r="L253" s="17">
+        <v>1</v>
+      </c>
+      <c r="M253" s="17">
+        <v>1</v>
+      </c>
+      <c r="N253" s="17">
+        <v>1</v>
+      </c>
       <c r="O253" s="17"/>
-      <c r="P253" s="17"/>
+      <c r="P253" s="17">
+        <v>1</v>
+      </c>
       <c r="Q253" s="17"/>
     </row>
     <row r="254" spans="1:17" x14ac:dyDescent="0.2">
@@ -9056,7 +9100,7 @@
         <v>6</v>
       </c>
       <c r="C254" s="35" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D254" s="45"/>
       <c r="E254" s="45"/>
@@ -9080,36 +9124,24 @@
         <v>169</v>
       </c>
       <c r="B255" s="34" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C255" s="35" t="s">
-        <v>56</v>
+        <v>336</v>
       </c>
       <c r="D255" s="45"/>
       <c r="E255" s="45"/>
       <c r="F255" s="45"/>
-      <c r="G255" s="17">
-        <v>1</v>
-      </c>
-      <c r="H255" s="17">
-        <v>1</v>
-      </c>
-      <c r="I255" s="17">
-        <v>1</v>
-      </c>
+      <c r="G255" s="17"/>
+      <c r="H255" s="17"/>
+      <c r="I255" s="17"/>
       <c r="J255" s="17">
         <v>1</v>
       </c>
-      <c r="K255" s="17">
-        <v>1</v>
-      </c>
+      <c r="K255" s="17"/>
       <c r="L255" s="17"/>
-      <c r="M255" s="17">
-        <v>1</v>
-      </c>
-      <c r="N255" s="17">
-        <v>1</v>
-      </c>
+      <c r="M255" s="17"/>
+      <c r="N255" s="17"/>
       <c r="O255" s="17"/>
       <c r="P255" s="17"/>
       <c r="Q255" s="17"/>
@@ -9122,40 +9154,34 @@
         <v>6</v>
       </c>
       <c r="C256" s="35" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D256" s="45"/>
       <c r="E256" s="45"/>
       <c r="F256" s="45"/>
-      <c r="G256" s="17">
-        <v>1</v>
-      </c>
-      <c r="H256" s="17">
-        <v>1</v>
-      </c>
+      <c r="G256" s="17"/>
+      <c r="H256" s="17"/>
       <c r="I256" s="17"/>
       <c r="J256" s="17"/>
-      <c r="K256" s="17">
-        <v>1</v>
-      </c>
+      <c r="K256" s="17"/>
       <c r="L256" s="17"/>
       <c r="M256" s="17"/>
       <c r="N256" s="17">
         <v>1</v>
       </c>
       <c r="O256" s="17"/>
-      <c r="P256" s="17">
-        <v>1</v>
-      </c>
+      <c r="P256" s="17"/>
       <c r="Q256" s="17"/>
     </row>
     <row r="257" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A257" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="B257" s="36"/>
+      <c r="B257" s="34" t="s">
+        <v>51</v>
+      </c>
       <c r="C257" s="35" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
       <c r="D257" s="45"/>
       <c r="E257" s="45"/>
@@ -9175,24 +9201,16 @@
       <c r="K257" s="17">
         <v>1</v>
       </c>
-      <c r="L257" s="17">
-        <v>1</v>
-      </c>
+      <c r="L257" s="17"/>
       <c r="M257" s="17">
         <v>1</v>
       </c>
       <c r="N257" s="17">
         <v>1</v>
       </c>
-      <c r="O257" s="17">
-        <v>1</v>
-      </c>
-      <c r="P257" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q257" s="17">
-        <v>1</v>
-      </c>
+      <c r="O257" s="17"/>
+      <c r="P257" s="17"/>
+      <c r="Q257" s="17"/>
     </row>
     <row r="258" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A258" s="33" t="s">
@@ -9202,19 +9220,19 @@
         <v>6</v>
       </c>
       <c r="C258" s="35" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="D258" s="45"/>
       <c r="E258" s="45"/>
       <c r="F258" s="45"/>
-      <c r="G258" s="17"/>
+      <c r="G258" s="17">
+        <v>1</v>
+      </c>
       <c r="H258" s="17">
         <v>1</v>
       </c>
       <c r="I258" s="17"/>
-      <c r="J258" s="17">
-        <v>1</v>
-      </c>
+      <c r="J258" s="17"/>
       <c r="K258" s="17">
         <v>1</v>
       </c>
@@ -9224,35 +9242,55 @@
         <v>1</v>
       </c>
       <c r="O258" s="17"/>
-      <c r="P258" s="17"/>
+      <c r="P258" s="17">
+        <v>1</v>
+      </c>
       <c r="Q258" s="17"/>
     </row>
     <row r="259" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A259" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="B259" s="34" t="s">
-        <v>6</v>
-      </c>
+      <c r="B259" s="36"/>
       <c r="C259" s="35" t="s">
-        <v>112</v>
+        <v>2</v>
       </c>
       <c r="D259" s="45"/>
       <c r="E259" s="45"/>
       <c r="F259" s="45"/>
-      <c r="G259" s="17"/>
-      <c r="H259" s="17"/>
-      <c r="I259" s="17"/>
-      <c r="J259" s="17"/>
-      <c r="K259" s="17"/>
-      <c r="L259" s="17"/>
-      <c r="M259" s="17"/>
+      <c r="G259" s="17">
+        <v>1</v>
+      </c>
+      <c r="H259" s="17">
+        <v>1</v>
+      </c>
+      <c r="I259" s="17">
+        <v>1</v>
+      </c>
+      <c r="J259" s="17">
+        <v>1</v>
+      </c>
+      <c r="K259" s="17">
+        <v>1</v>
+      </c>
+      <c r="L259" s="17">
+        <v>1</v>
+      </c>
+      <c r="M259" s="17">
+        <v>1</v>
+      </c>
       <c r="N259" s="17">
         <v>1</v>
       </c>
-      <c r="O259" s="17"/>
-      <c r="P259" s="17"/>
-      <c r="Q259" s="17"/>
+      <c r="O259" s="17">
+        <v>1</v>
+      </c>
+      <c r="P259" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q259" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="260" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A260" s="33" t="s">
@@ -9262,15 +9300,19 @@
         <v>6</v>
       </c>
       <c r="C260" s="35" t="s">
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="D260" s="45"/>
       <c r="E260" s="45"/>
       <c r="F260" s="45"/>
       <c r="G260" s="17"/>
-      <c r="H260" s="17"/>
+      <c r="H260" s="17">
+        <v>1</v>
+      </c>
       <c r="I260" s="17"/>
-      <c r="J260" s="17"/>
+      <c r="J260" s="17">
+        <v>1</v>
+      </c>
       <c r="K260" s="17">
         <v>1</v>
       </c>
@@ -9288,30 +9330,20 @@
         <v>169</v>
       </c>
       <c r="B261" s="34" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C261" s="35" t="s">
-        <v>154</v>
+        <v>112</v>
       </c>
       <c r="D261" s="45"/>
       <c r="E261" s="45"/>
       <c r="F261" s="45"/>
-      <c r="G261" s="17">
-        <v>1</v>
-      </c>
-      <c r="H261" s="17">
-        <v>1</v>
-      </c>
+      <c r="G261" s="17"/>
+      <c r="H261" s="17"/>
       <c r="I261" s="17"/>
-      <c r="J261" s="17">
-        <v>1</v>
-      </c>
-      <c r="K261" s="17">
-        <v>1</v>
-      </c>
-      <c r="L261" s="17">
-        <v>1</v>
-      </c>
+      <c r="J261" s="17"/>
+      <c r="K261" s="17"/>
+      <c r="L261" s="17"/>
       <c r="M261" s="17"/>
       <c r="N261" s="17">
         <v>1</v>
@@ -9328,7 +9360,7 @@
         <v>6</v>
       </c>
       <c r="C262" s="35" t="s">
-        <v>337</v>
+        <v>40</v>
       </c>
       <c r="D262" s="45"/>
       <c r="E262" s="45"/>
@@ -9337,10 +9369,14 @@
       <c r="H262" s="17"/>
       <c r="I262" s="17"/>
       <c r="J262" s="17"/>
-      <c r="K262" s="17"/>
+      <c r="K262" s="17">
+        <v>1</v>
+      </c>
       <c r="L262" s="17"/>
       <c r="M262" s="17"/>
-      <c r="N262" s="17"/>
+      <c r="N262" s="17">
+        <v>1</v>
+      </c>
       <c r="O262" s="17"/>
       <c r="P262" s="17"/>
       <c r="Q262" s="17"/>
@@ -9350,15 +9386,17 @@
         <v>169</v>
       </c>
       <c r="B263" s="34" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C263" s="35" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
       <c r="D263" s="45"/>
       <c r="E263" s="45"/>
       <c r="F263" s="45"/>
-      <c r="G263" s="17"/>
+      <c r="G263" s="17">
+        <v>1</v>
+      </c>
       <c r="H263" s="17">
         <v>1</v>
       </c>
@@ -9369,7 +9407,9 @@
       <c r="K263" s="17">
         <v>1</v>
       </c>
-      <c r="L263" s="17"/>
+      <c r="L263" s="17">
+        <v>1</v>
+      </c>
       <c r="M263" s="17"/>
       <c r="N263" s="17">
         <v>1</v>
@@ -9383,71 +9423,55 @@
         <v>169</v>
       </c>
       <c r="B264" s="34" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C264" s="35" t="s">
-        <v>161</v>
+        <v>337</v>
       </c>
       <c r="D264" s="45"/>
       <c r="E264" s="45"/>
       <c r="F264" s="45"/>
-      <c r="G264" s="17">
-        <v>1</v>
-      </c>
-      <c r="H264" s="17">
-        <v>1</v>
-      </c>
-      <c r="I264" s="17">
-        <v>1</v>
-      </c>
-      <c r="J264" s="17">
-        <v>1</v>
-      </c>
-      <c r="K264" s="17">
-        <v>1</v>
-      </c>
-      <c r="L264" s="17">
-        <v>1</v>
-      </c>
-      <c r="M264" s="17">
-        <v>1</v>
-      </c>
-      <c r="N264" s="17">
-        <v>1</v>
-      </c>
-      <c r="O264" s="17">
-        <v>1</v>
-      </c>
-      <c r="P264" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q264" s="17">
-        <v>1</v>
-      </c>
+      <c r="G264" s="17"/>
+      <c r="H264" s="17"/>
+      <c r="I264" s="17"/>
+      <c r="J264" s="17"/>
+      <c r="K264" s="17"/>
+      <c r="L264" s="17"/>
+      <c r="M264" s="17"/>
+      <c r="N264" s="17"/>
+      <c r="O264" s="17"/>
+      <c r="P264" s="17"/>
+      <c r="Q264" s="17"/>
     </row>
     <row r="265" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A265" s="33" t="s">
         <v>169</v>
       </c>
       <c r="B265" s="34" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C265" s="35" t="s">
-        <v>338</v>
+        <v>126</v>
       </c>
       <c r="D265" s="45"/>
       <c r="E265" s="45"/>
       <c r="F265" s="45"/>
       <c r="G265" s="17"/>
-      <c r="H265" s="17"/>
+      <c r="H265" s="17">
+        <v>1</v>
+      </c>
       <c r="I265" s="17"/>
       <c r="J265" s="17">
         <v>1</v>
       </c>
-      <c r="K265" s="17"/>
+      <c r="K265" s="17">
+        <v>1</v>
+      </c>
       <c r="L265" s="17"/>
       <c r="M265" s="17"/>
-      <c r="N265" s="17"/>
+      <c r="N265" s="17">
+        <v>1</v>
+      </c>
       <c r="O265" s="17"/>
       <c r="P265" s="17"/>
       <c r="Q265" s="17"/>
@@ -9457,10 +9481,10 @@
         <v>169</v>
       </c>
       <c r="B266" s="34" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C266" s="35" t="s">
-        <v>49</v>
+        <v>161</v>
       </c>
       <c r="D266" s="45"/>
       <c r="E266" s="45"/>
@@ -9471,29 +9495,43 @@
       <c r="H266" s="17">
         <v>1</v>
       </c>
-      <c r="I266" s="17"/>
-      <c r="J266" s="17"/>
+      <c r="I266" s="17">
+        <v>1</v>
+      </c>
+      <c r="J266" s="17">
+        <v>1</v>
+      </c>
       <c r="K266" s="17">
         <v>1</v>
       </c>
-      <c r="L266" s="17"/>
-      <c r="M266" s="17"/>
+      <c r="L266" s="17">
+        <v>1</v>
+      </c>
+      <c r="M266" s="17">
+        <v>1</v>
+      </c>
       <c r="N266" s="17">
         <v>1</v>
       </c>
-      <c r="O266" s="17"/>
-      <c r="P266" s="17"/>
-      <c r="Q266" s="17"/>
+      <c r="O266" s="17">
+        <v>1</v>
+      </c>
+      <c r="P266" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q266" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="267" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A267" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="B267" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C267" s="16" t="s">
-        <v>179</v>
+      <c r="A267" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="B267" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C267" s="35" t="s">
+        <v>338</v>
       </c>
       <c r="D267" s="45"/>
       <c r="E267" s="45"/>
@@ -9501,7 +9539,9 @@
       <c r="G267" s="17"/>
       <c r="H267" s="17"/>
       <c r="I267" s="17"/>
-      <c r="J267" s="17"/>
+      <c r="J267" s="17">
+        <v>1</v>
+      </c>
       <c r="K267" s="17"/>
       <c r="L267" s="17"/>
       <c r="M267" s="17"/>
@@ -9511,39 +9551,47 @@
       <c r="Q267" s="17"/>
     </row>
     <row r="268" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A268" s="37" t="s">
-        <v>223</v>
-      </c>
-      <c r="B268" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="C268" s="39" t="s">
-        <v>42</v>
+      <c r="A268" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="B268" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C268" s="35" t="s">
+        <v>49</v>
       </c>
       <c r="D268" s="45"/>
       <c r="E268" s="45"/>
       <c r="F268" s="45"/>
-      <c r="G268" s="17"/>
-      <c r="H268" s="17"/>
+      <c r="G268" s="17">
+        <v>1</v>
+      </c>
+      <c r="H268" s="17">
+        <v>1</v>
+      </c>
       <c r="I268" s="17"/>
       <c r="J268" s="17"/>
-      <c r="K268" s="17"/>
+      <c r="K268" s="17">
+        <v>1</v>
+      </c>
       <c r="L268" s="17"/>
       <c r="M268" s="17"/>
-      <c r="N268" s="17"/>
+      <c r="N268" s="17">
+        <v>1</v>
+      </c>
       <c r="O268" s="17"/>
       <c r="P268" s="17"/>
       <c r="Q268" s="17"/>
     </row>
     <row r="269" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A269" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="B269" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C269" s="21" t="s">
-        <v>101</v>
+      <c r="A269" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="B269" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C269" s="16" t="s">
+        <v>179</v>
       </c>
       <c r="D269" s="45"/>
       <c r="E269" s="45"/>
@@ -9562,44 +9610,38 @@
     </row>
     <row r="270" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A270" s="37" t="s">
-        <v>43</v>
+        <v>223</v>
       </c>
       <c r="B270" s="38" t="s">
         <v>6</v>
       </c>
       <c r="C270" s="39" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="D270" s="45"/>
       <c r="E270" s="45"/>
       <c r="F270" s="45"/>
-      <c r="G270" s="17">
-        <v>1</v>
-      </c>
+      <c r="G270" s="17"/>
       <c r="H270" s="17"/>
       <c r="I270" s="17"/>
       <c r="J270" s="17"/>
       <c r="K270" s="17"/>
       <c r="L270" s="17"/>
-      <c r="M270" s="17">
-        <v>1</v>
-      </c>
+      <c r="M270" s="17"/>
       <c r="N270" s="17"/>
       <c r="O270" s="17"/>
-      <c r="P270" s="17">
-        <v>1</v>
-      </c>
+      <c r="P270" s="17"/>
       <c r="Q270" s="17"/>
     </row>
     <row r="271" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A271" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B271" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="C271" s="39" t="s">
-        <v>87</v>
+      <c r="A271" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="B271" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C271" s="21" t="s">
+        <v>101</v>
       </c>
       <c r="D271" s="45"/>
       <c r="E271" s="45"/>
@@ -9610,9 +9652,7 @@
       <c r="J271" s="17"/>
       <c r="K271" s="17"/>
       <c r="L271" s="17"/>
-      <c r="M271" s="17">
-        <v>1</v>
-      </c>
+      <c r="M271" s="17"/>
       <c r="N271" s="17"/>
       <c r="O271" s="17"/>
       <c r="P271" s="17"/>
@@ -9626,7 +9666,7 @@
         <v>6</v>
       </c>
       <c r="C272" s="39" t="s">
-        <v>225</v>
+        <v>9</v>
       </c>
       <c r="D272" s="45"/>
       <c r="E272" s="45"/>
@@ -9634,13 +9674,9 @@
       <c r="G272" s="17">
         <v>1</v>
       </c>
-      <c r="H272" s="17">
-        <v>1</v>
-      </c>
+      <c r="H272" s="17"/>
       <c r="I272" s="17"/>
-      <c r="J272" s="17">
-        <v>1</v>
-      </c>
+      <c r="J272" s="17"/>
       <c r="K272" s="17">
         <v>1</v>
       </c>
@@ -9660,10 +9696,10 @@
         <v>43</v>
       </c>
       <c r="B273" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C273" s="39" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="D273" s="45"/>
       <c r="E273" s="45"/>
@@ -9690,7 +9726,7 @@
         <v>6</v>
       </c>
       <c r="C274" s="39" t="s">
-        <v>16</v>
+        <v>225</v>
       </c>
       <c r="D274" s="45"/>
       <c r="E274" s="45"/>
@@ -9702,7 +9738,9 @@
         <v>1</v>
       </c>
       <c r="I274" s="17"/>
-      <c r="J274" s="17"/>
+      <c r="J274" s="17">
+        <v>1</v>
+      </c>
       <c r="K274" s="17">
         <v>1</v>
       </c>
@@ -9725,33 +9763,23 @@
         <v>51</v>
       </c>
       <c r="C275" s="39" t="s">
-        <v>59</v>
+        <v>131</v>
       </c>
       <c r="D275" s="45"/>
       <c r="E275" s="45"/>
       <c r="F275" s="45"/>
-      <c r="G275" s="17">
-        <v>1</v>
-      </c>
-      <c r="H275" s="17">
-        <v>1</v>
-      </c>
-      <c r="I275" s="17">
-        <v>1</v>
-      </c>
+      <c r="G275" s="17"/>
+      <c r="H275" s="17"/>
+      <c r="I275" s="17"/>
       <c r="J275" s="17"/>
-      <c r="K275" s="17">
-        <v>1</v>
-      </c>
+      <c r="K275" s="17"/>
       <c r="L275" s="17"/>
       <c r="M275" s="17">
         <v>1</v>
       </c>
       <c r="N275" s="17"/>
       <c r="O275" s="17"/>
-      <c r="P275" s="17">
-        <v>1</v>
-      </c>
+      <c r="P275" s="17"/>
       <c r="Q275" s="17"/>
     </row>
     <row r="276" spans="1:17" x14ac:dyDescent="0.2">
@@ -9759,10 +9787,10 @@
         <v>43</v>
       </c>
       <c r="B276" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C276" s="39" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="D276" s="45"/>
       <c r="E276" s="45"/>
@@ -9770,11 +9798,11 @@
       <c r="G276" s="17">
         <v>1</v>
       </c>
-      <c r="H276" s="17"/>
+      <c r="H276" s="17">
+        <v>1</v>
+      </c>
       <c r="I276" s="17"/>
-      <c r="J276" s="17">
-        <v>1</v>
-      </c>
+      <c r="J276" s="17"/>
       <c r="K276" s="17"/>
       <c r="L276" s="17"/>
       <c r="M276" s="17">
@@ -9782,7 +9810,9 @@
       </c>
       <c r="N276" s="17"/>
       <c r="O276" s="17"/>
-      <c r="P276" s="17"/>
+      <c r="P276" s="17">
+        <v>1</v>
+      </c>
       <c r="Q276" s="17"/>
     </row>
     <row r="277" spans="1:17" x14ac:dyDescent="0.2">
@@ -9790,22 +9820,24 @@
         <v>43</v>
       </c>
       <c r="B277" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C277" s="39" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="D277" s="45"/>
       <c r="E277" s="45"/>
       <c r="F277" s="45"/>
-      <c r="G277" s="17"/>
+      <c r="G277" s="17">
+        <v>1</v>
+      </c>
       <c r="H277" s="17">
         <v>1</v>
       </c>
-      <c r="I277" s="17"/>
-      <c r="J277" s="17">
-        <v>1</v>
-      </c>
+      <c r="I277" s="17">
+        <v>1</v>
+      </c>
+      <c r="J277" s="17"/>
       <c r="K277" s="17">
         <v>1</v>
       </c>
@@ -9815,7 +9847,9 @@
       </c>
       <c r="N277" s="17"/>
       <c r="O277" s="17"/>
-      <c r="P277" s="17"/>
+      <c r="P277" s="17">
+        <v>1</v>
+      </c>
       <c r="Q277" s="17"/>
     </row>
     <row r="278" spans="1:17" x14ac:dyDescent="0.2">
@@ -9823,25 +9857,27 @@
         <v>43</v>
       </c>
       <c r="B278" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C278" s="39" t="s">
-        <v>271</v>
+        <v>61</v>
       </c>
       <c r="D278" s="45"/>
       <c r="E278" s="45"/>
       <c r="F278" s="45"/>
-      <c r="G278" s="17"/>
-      <c r="H278" s="17">
-        <v>1</v>
-      </c>
+      <c r="G278" s="17">
+        <v>1</v>
+      </c>
+      <c r="H278" s="17"/>
       <c r="I278" s="17"/>
-      <c r="J278" s="17"/>
-      <c r="K278" s="17">
-        <v>1</v>
-      </c>
+      <c r="J278" s="17">
+        <v>1</v>
+      </c>
+      <c r="K278" s="17"/>
       <c r="L278" s="17"/>
-      <c r="M278" s="17"/>
+      <c r="M278" s="17">
+        <v>1</v>
+      </c>
       <c r="N278" s="17"/>
       <c r="O278" s="17"/>
       <c r="P278" s="17"/>
@@ -9855,7 +9891,7 @@
         <v>6</v>
       </c>
       <c r="C279" s="39" t="s">
-        <v>270</v>
+        <v>94</v>
       </c>
       <c r="D279" s="45"/>
       <c r="E279" s="45"/>
@@ -9865,12 +9901,16 @@
         <v>1</v>
       </c>
       <c r="I279" s="17"/>
-      <c r="J279" s="17"/>
+      <c r="J279" s="17">
+        <v>1</v>
+      </c>
       <c r="K279" s="17">
         <v>1</v>
       </c>
       <c r="L279" s="17"/>
-      <c r="M279" s="17"/>
+      <c r="M279" s="17">
+        <v>1</v>
+      </c>
       <c r="N279" s="17"/>
       <c r="O279" s="17"/>
       <c r="P279" s="17"/>
@@ -9884,7 +9924,7 @@
         <v>6</v>
       </c>
       <c r="C280" s="39" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D280" s="45"/>
       <c r="E280" s="45"/>
@@ -9913,22 +9953,22 @@
         <v>6</v>
       </c>
       <c r="C281" s="39" t="s">
-        <v>99</v>
+        <v>270</v>
       </c>
       <c r="D281" s="45"/>
       <c r="E281" s="45"/>
       <c r="F281" s="45"/>
       <c r="G281" s="17"/>
-      <c r="H281" s="17"/>
+      <c r="H281" s="17">
+        <v>1</v>
+      </c>
       <c r="I281" s="17"/>
-      <c r="J281" s="17">
-        <v>1</v>
-      </c>
-      <c r="K281" s="17"/>
+      <c r="J281" s="17"/>
+      <c r="K281" s="17">
+        <v>1</v>
+      </c>
       <c r="L281" s="17"/>
-      <c r="M281" s="17">
-        <v>1</v>
-      </c>
+      <c r="M281" s="17"/>
       <c r="N281" s="17"/>
       <c r="O281" s="17"/>
       <c r="P281" s="17"/>
@@ -9939,31 +9979,25 @@
         <v>43</v>
       </c>
       <c r="B282" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C282" s="39" t="s">
-        <v>66</v>
+        <v>272</v>
       </c>
       <c r="D282" s="45"/>
       <c r="E282" s="45"/>
       <c r="F282" s="45"/>
-      <c r="G282" s="17">
-        <v>1</v>
-      </c>
+      <c r="G282" s="17"/>
       <c r="H282" s="17">
         <v>1</v>
       </c>
       <c r="I282" s="17"/>
-      <c r="J282" s="17">
-        <v>1</v>
-      </c>
+      <c r="J282" s="17"/>
       <c r="K282" s="17">
         <v>1</v>
       </c>
       <c r="L282" s="17"/>
-      <c r="M282" s="17">
-        <v>1</v>
-      </c>
+      <c r="M282" s="17"/>
       <c r="N282" s="17"/>
       <c r="O282" s="17"/>
       <c r="P282" s="17"/>
@@ -9977,7 +10011,7 @@
         <v>6</v>
       </c>
       <c r="C283" s="39" t="s">
-        <v>339</v>
+        <v>99</v>
       </c>
       <c r="D283" s="45"/>
       <c r="E283" s="45"/>
@@ -9990,7 +10024,9 @@
       </c>
       <c r="K283" s="17"/>
       <c r="L283" s="17"/>
-      <c r="M283" s="17"/>
+      <c r="M283" s="17">
+        <v>1</v>
+      </c>
       <c r="N283" s="17"/>
       <c r="O283" s="17"/>
       <c r="P283" s="17"/>
@@ -10001,10 +10037,10 @@
         <v>43</v>
       </c>
       <c r="B284" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C284" s="39" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="D284" s="45"/>
       <c r="E284" s="45"/>
@@ -10015,64 +10051,44 @@
       <c r="H284" s="17">
         <v>1</v>
       </c>
-      <c r="I284" s="17">
-        <v>1</v>
-      </c>
+      <c r="I284" s="17"/>
       <c r="J284" s="17">
         <v>1</v>
       </c>
       <c r="K284" s="17">
         <v>1</v>
       </c>
-      <c r="L284" s="17">
-        <v>1</v>
-      </c>
+      <c r="L284" s="17"/>
       <c r="M284" s="17">
         <v>1</v>
       </c>
-      <c r="N284" s="17">
-        <v>1</v>
-      </c>
-      <c r="O284" s="17">
-        <v>1</v>
-      </c>
-      <c r="P284" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q284" s="17">
-        <v>1</v>
-      </c>
+      <c r="N284" s="17"/>
+      <c r="O284" s="17"/>
+      <c r="P284" s="17"/>
+      <c r="Q284" s="17"/>
     </row>
     <row r="285" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A285" s="37" t="s">
         <v>43</v>
       </c>
       <c r="B285" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C285" s="39" t="s">
-        <v>67</v>
+        <v>339</v>
       </c>
       <c r="D285" s="45"/>
       <c r="E285" s="45"/>
       <c r="F285" s="45"/>
-      <c r="G285" s="17">
-        <v>1</v>
-      </c>
-      <c r="H285" s="17">
-        <v>1</v>
-      </c>
+      <c r="G285" s="17"/>
+      <c r="H285" s="17"/>
       <c r="I285" s="17"/>
       <c r="J285" s="17">
         <v>1</v>
       </c>
-      <c r="K285" s="17">
-        <v>1</v>
-      </c>
+      <c r="K285" s="17"/>
       <c r="L285" s="17"/>
-      <c r="M285" s="17">
-        <v>1</v>
-      </c>
+      <c r="M285" s="17"/>
       <c r="N285" s="17"/>
       <c r="O285" s="17"/>
       <c r="P285" s="17"/>
@@ -10086,7 +10102,7 @@
         <v>6</v>
       </c>
       <c r="C286" s="39" t="s">
-        <v>312</v>
+        <v>102</v>
       </c>
       <c r="D286" s="45"/>
       <c r="E286" s="45"/>
@@ -10112,12 +10128,18 @@
       <c r="M286" s="17">
         <v>1</v>
       </c>
-      <c r="N286" s="17"/>
-      <c r="O286" s="17"/>
+      <c r="N286" s="17">
+        <v>1</v>
+      </c>
+      <c r="O286" s="17">
+        <v>1</v>
+      </c>
       <c r="P286" s="17">
         <v>1</v>
       </c>
-      <c r="Q286" s="17"/>
+      <c r="Q286" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="287" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A287" s="37" t="s">
@@ -10127,7 +10149,7 @@
         <v>51</v>
       </c>
       <c r="C287" s="39" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D287" s="45"/>
       <c r="E287" s="45"/>
@@ -10139,7 +10161,9 @@
         <v>1</v>
       </c>
       <c r="I287" s="17"/>
-      <c r="J287" s="17"/>
+      <c r="J287" s="17">
+        <v>1</v>
+      </c>
       <c r="K287" s="17">
         <v>1</v>
       </c>
@@ -10149,9 +10173,7 @@
       </c>
       <c r="N287" s="17"/>
       <c r="O287" s="17"/>
-      <c r="P287" s="17">
-        <v>1</v>
-      </c>
+      <c r="P287" s="17"/>
       <c r="Q287" s="17"/>
     </row>
     <row r="288" spans="1:17" x14ac:dyDescent="0.2">
@@ -10162,7 +10184,7 @@
         <v>6</v>
       </c>
       <c r="C288" s="39" t="s">
-        <v>118</v>
+        <v>312</v>
       </c>
       <c r="D288" s="45"/>
       <c r="E288" s="45"/>
@@ -10173,14 +10195,18 @@
       <c r="H288" s="17">
         <v>1</v>
       </c>
-      <c r="I288" s="17"/>
+      <c r="I288" s="17">
+        <v>1</v>
+      </c>
       <c r="J288" s="17">
         <v>1</v>
       </c>
       <c r="K288" s="17">
         <v>1</v>
       </c>
-      <c r="L288" s="17"/>
+      <c r="L288" s="17">
+        <v>1</v>
+      </c>
       <c r="M288" s="17">
         <v>1</v>
       </c>
@@ -10196,28 +10222,34 @@
         <v>43</v>
       </c>
       <c r="B289" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C289" s="39" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="D289" s="45"/>
       <c r="E289" s="45"/>
       <c r="F289" s="45"/>
-      <c r="G289" s="17"/>
-      <c r="H289" s="17"/>
+      <c r="G289" s="17">
+        <v>1</v>
+      </c>
+      <c r="H289" s="17">
+        <v>1</v>
+      </c>
       <c r="I289" s="17"/>
-      <c r="J289" s="17">
-        <v>1</v>
-      </c>
-      <c r="K289" s="17"/>
+      <c r="J289" s="17"/>
+      <c r="K289" s="17">
+        <v>1</v>
+      </c>
       <c r="L289" s="17"/>
       <c r="M289" s="17">
         <v>1</v>
       </c>
       <c r="N289" s="17"/>
       <c r="O289" s="17"/>
-      <c r="P289" s="17"/>
+      <c r="P289" s="17">
+        <v>1</v>
+      </c>
       <c r="Q289" s="17"/>
     </row>
     <row r="290" spans="1:17" x14ac:dyDescent="0.2">
@@ -10228,7 +10260,7 @@
         <v>6</v>
       </c>
       <c r="C290" s="39" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="D290" s="45"/>
       <c r="E290" s="45"/>
@@ -10252,7 +10284,9 @@
       </c>
       <c r="N290" s="17"/>
       <c r="O290" s="17"/>
-      <c r="P290" s="17"/>
+      <c r="P290" s="17">
+        <v>1</v>
+      </c>
       <c r="Q290" s="17"/>
     </row>
     <row r="291" spans="1:17" x14ac:dyDescent="0.2">
@@ -10263,17 +10297,17 @@
         <v>6</v>
       </c>
       <c r="C291" s="39" t="s">
-        <v>269</v>
+        <v>119</v>
       </c>
       <c r="D291" s="45"/>
       <c r="E291" s="45"/>
       <c r="F291" s="45"/>
       <c r="G291" s="17"/>
-      <c r="H291" s="17">
-        <v>1</v>
-      </c>
+      <c r="H291" s="17"/>
       <c r="I291" s="17"/>
-      <c r="J291" s="17"/>
+      <c r="J291" s="17">
+        <v>1</v>
+      </c>
       <c r="K291" s="17">
         <v>1</v>
       </c>
@@ -10283,9 +10317,7 @@
       </c>
       <c r="N291" s="17"/>
       <c r="O291" s="17"/>
-      <c r="P291" s="17">
-        <v>1</v>
-      </c>
+      <c r="P291" s="17"/>
       <c r="Q291" s="17"/>
     </row>
     <row r="292" spans="1:17" x14ac:dyDescent="0.2">
@@ -10296,7 +10328,7 @@
         <v>6</v>
       </c>
       <c r="C292" s="39" t="s">
-        <v>324</v>
+        <v>44</v>
       </c>
       <c r="D292" s="45"/>
       <c r="E292" s="45"/>
@@ -10324,48 +10356,68 @@
       <c r="Q292" s="17"/>
     </row>
     <row r="293" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A293" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B293" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C293" s="13" t="s">
-        <v>330</v>
+      <c r="A293" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B293" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C293" s="39" t="s">
+        <v>269</v>
       </c>
       <c r="D293" s="45"/>
       <c r="E293" s="45"/>
       <c r="F293" s="45"/>
       <c r="G293" s="17"/>
-      <c r="H293" s="17"/>
+      <c r="H293" s="17">
+        <v>1</v>
+      </c>
       <c r="I293" s="17"/>
       <c r="J293" s="17"/>
-      <c r="K293" s="17"/>
+      <c r="K293" s="17">
+        <v>1</v>
+      </c>
       <c r="L293" s="17"/>
-      <c r="M293" s="17"/>
+      <c r="M293" s="17">
+        <v>1</v>
+      </c>
       <c r="N293" s="17"/>
       <c r="O293" s="17"/>
-      <c r="P293" s="17"/>
+      <c r="P293" s="17">
+        <v>1</v>
+      </c>
       <c r="Q293" s="17"/>
     </row>
     <row r="294" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A294" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B294" s="40"/>
-      <c r="C294" s="13" t="s">
-        <v>0</v>
+      <c r="A294" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B294" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C294" s="39" t="s">
+        <v>324</v>
       </c>
       <c r="D294" s="45"/>
       <c r="E294" s="45"/>
       <c r="F294" s="45"/>
-      <c r="G294" s="17"/>
-      <c r="H294" s="17"/>
+      <c r="G294" s="17">
+        <v>1</v>
+      </c>
+      <c r="H294" s="17">
+        <v>1</v>
+      </c>
       <c r="I294" s="17"/>
-      <c r="J294" s="17"/>
-      <c r="K294" s="17"/>
+      <c r="J294" s="17">
+        <v>1</v>
+      </c>
+      <c r="K294" s="17">
+        <v>1</v>
+      </c>
       <c r="L294" s="17"/>
-      <c r="M294" s="17"/>
+      <c r="M294" s="17">
+        <v>1</v>
+      </c>
       <c r="N294" s="17"/>
       <c r="O294" s="17"/>
       <c r="P294" s="17"/>
@@ -10379,24 +10431,16 @@
         <v>51</v>
       </c>
       <c r="C295" s="13" t="s">
-        <v>135</v>
+        <v>330</v>
       </c>
       <c r="D295" s="45"/>
       <c r="E295" s="45"/>
       <c r="F295" s="45"/>
-      <c r="G295" s="17">
-        <v>1</v>
-      </c>
-      <c r="H295" s="17">
-        <v>1</v>
-      </c>
+      <c r="G295" s="17"/>
+      <c r="H295" s="17"/>
       <c r="I295" s="17"/>
-      <c r="J295" s="17">
-        <v>1</v>
-      </c>
-      <c r="K295" s="17">
-        <v>1</v>
-      </c>
+      <c r="J295" s="17"/>
+      <c r="K295" s="17"/>
       <c r="L295" s="17"/>
       <c r="M295" s="17"/>
       <c r="N295" s="17"/>
@@ -10408,28 +10452,18 @@
       <c r="A296" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B296" s="12" t="s">
-        <v>51</v>
-      </c>
+      <c r="B296" s="40"/>
       <c r="C296" s="13" t="s">
-        <v>139</v>
+        <v>0</v>
       </c>
       <c r="D296" s="45"/>
       <c r="E296" s="45"/>
       <c r="F296" s="45"/>
-      <c r="G296" s="17">
-        <v>1</v>
-      </c>
-      <c r="H296" s="17">
-        <v>1</v>
-      </c>
+      <c r="G296" s="17"/>
+      <c r="H296" s="17"/>
       <c r="I296" s="17"/>
-      <c r="J296" s="17">
-        <v>1</v>
-      </c>
-      <c r="K296" s="17">
-        <v>1</v>
-      </c>
+      <c r="J296" s="17"/>
+      <c r="K296" s="17"/>
       <c r="L296" s="17"/>
       <c r="M296" s="17"/>
       <c r="N296" s="17"/>
@@ -10442,19 +10476,27 @@
         <v>47</v>
       </c>
       <c r="B297" s="12" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C297" s="13" t="s">
-        <v>240</v>
+        <v>135</v>
       </c>
       <c r="D297" s="45"/>
       <c r="E297" s="45"/>
       <c r="F297" s="45"/>
-      <c r="G297" s="17"/>
-      <c r="H297" s="17"/>
+      <c r="G297" s="17">
+        <v>1</v>
+      </c>
+      <c r="H297" s="17">
+        <v>1</v>
+      </c>
       <c r="I297" s="17"/>
-      <c r="J297" s="17"/>
-      <c r="K297" s="17"/>
+      <c r="J297" s="17">
+        <v>1</v>
+      </c>
+      <c r="K297" s="17">
+        <v>1</v>
+      </c>
       <c r="L297" s="17"/>
       <c r="M297" s="17"/>
       <c r="N297" s="17"/>
@@ -10470,12 +10512,14 @@
         <v>51</v>
       </c>
       <c r="C298" s="13" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D298" s="45"/>
       <c r="E298" s="45"/>
       <c r="F298" s="45"/>
-      <c r="G298" s="17"/>
+      <c r="G298" s="17">
+        <v>1</v>
+      </c>
       <c r="H298" s="17">
         <v>1</v>
       </c>
@@ -10498,25 +10542,19 @@
         <v>47</v>
       </c>
       <c r="B299" s="12" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C299" s="13" t="s">
-        <v>144</v>
+        <v>240</v>
       </c>
       <c r="D299" s="45"/>
       <c r="E299" s="45"/>
       <c r="F299" s="45"/>
       <c r="G299" s="17"/>
-      <c r="H299" s="17">
-        <v>1</v>
-      </c>
+      <c r="H299" s="17"/>
       <c r="I299" s="17"/>
-      <c r="J299" s="17">
-        <v>1</v>
-      </c>
-      <c r="K299" s="17">
-        <v>1</v>
-      </c>
+      <c r="J299" s="17"/>
+      <c r="K299" s="17"/>
       <c r="L299" s="17"/>
       <c r="M299" s="17"/>
       <c r="N299" s="17"/>
@@ -10532,44 +10570,28 @@
         <v>51</v>
       </c>
       <c r="C300" s="13" t="s">
-        <v>204</v>
+        <v>143</v>
       </c>
       <c r="D300" s="45"/>
       <c r="E300" s="45"/>
       <c r="F300" s="45"/>
-      <c r="G300" s="17">
-        <v>1</v>
-      </c>
+      <c r="G300" s="17"/>
       <c r="H300" s="17">
         <v>1</v>
       </c>
-      <c r="I300" s="17">
-        <v>1</v>
-      </c>
+      <c r="I300" s="17"/>
       <c r="J300" s="17">
         <v>1</v>
       </c>
       <c r="K300" s="17">
         <v>1</v>
       </c>
-      <c r="L300" s="17">
-        <v>1</v>
-      </c>
-      <c r="M300" s="17">
-        <v>1</v>
-      </c>
-      <c r="N300" s="17">
-        <v>1</v>
-      </c>
-      <c r="O300" s="17">
-        <v>1</v>
-      </c>
-      <c r="P300" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q300" s="17">
-        <v>1</v>
-      </c>
+      <c r="L300" s="17"/>
+      <c r="M300" s="17"/>
+      <c r="N300" s="17"/>
+      <c r="O300" s="17"/>
+      <c r="P300" s="17"/>
+      <c r="Q300" s="17"/>
     </row>
     <row r="301" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A301" s="11" t="s">
@@ -10579,44 +10601,28 @@
         <v>51</v>
       </c>
       <c r="C301" s="13" t="s">
-        <v>264</v>
+        <v>144</v>
       </c>
       <c r="D301" s="45"/>
       <c r="E301" s="45"/>
       <c r="F301" s="45"/>
-      <c r="G301" s="17">
-        <v>1</v>
-      </c>
+      <c r="G301" s="17"/>
       <c r="H301" s="17">
         <v>1</v>
       </c>
-      <c r="I301" s="17">
-        <v>1</v>
-      </c>
+      <c r="I301" s="17"/>
       <c r="J301" s="17">
         <v>1</v>
       </c>
       <c r="K301" s="17">
         <v>1</v>
       </c>
-      <c r="L301" s="17">
-        <v>1</v>
-      </c>
-      <c r="M301" s="17">
-        <v>1</v>
-      </c>
-      <c r="N301" s="17">
-        <v>1</v>
-      </c>
-      <c r="O301" s="17">
-        <v>1</v>
-      </c>
-      <c r="P301" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q301" s="17">
-        <v>1</v>
-      </c>
+      <c r="L301" s="17"/>
+      <c r="M301" s="17"/>
+      <c r="N301" s="17"/>
+      <c r="O301" s="17"/>
+      <c r="P301" s="17"/>
+      <c r="Q301" s="17"/>
     </row>
     <row r="302" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A302" s="11" t="s">
@@ -10626,7 +10632,7 @@
         <v>51</v>
       </c>
       <c r="C302" s="13" t="s">
-        <v>158</v>
+        <v>204</v>
       </c>
       <c r="D302" s="45"/>
       <c r="E302" s="45"/>
@@ -10670,86 +10676,118 @@
         <v>47</v>
       </c>
       <c r="B303" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C303" s="56" t="s">
-        <v>124</v>
-      </c>
-      <c r="D303" s="48"/>
-      <c r="E303" s="48"/>
-      <c r="F303" s="48"/>
-      <c r="G303" s="54">
-        <v>1</v>
-      </c>
-      <c r="H303" s="54">
-        <v>1</v>
-      </c>
-      <c r="I303" s="54"/>
-      <c r="J303" s="54">
-        <v>1</v>
-      </c>
-      <c r="K303" s="54">
-        <v>1</v>
-      </c>
-      <c r="L303" s="54"/>
-      <c r="M303" s="54"/>
-      <c r="N303" s="54">
-        <v>1</v>
-      </c>
-      <c r="O303" s="54"/>
-      <c r="P303" s="54"/>
-      <c r="Q303" s="54"/>
+        <v>51</v>
+      </c>
+      <c r="C303" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="D303" s="45"/>
+      <c r="E303" s="45"/>
+      <c r="F303" s="45"/>
+      <c r="G303" s="17">
+        <v>1</v>
+      </c>
+      <c r="H303" s="17">
+        <v>1</v>
+      </c>
+      <c r="I303" s="17">
+        <v>1</v>
+      </c>
+      <c r="J303" s="17">
+        <v>1</v>
+      </c>
+      <c r="K303" s="17">
+        <v>1</v>
+      </c>
+      <c r="L303" s="17">
+        <v>1</v>
+      </c>
+      <c r="M303" s="17">
+        <v>1</v>
+      </c>
+      <c r="N303" s="17">
+        <v>1</v>
+      </c>
+      <c r="O303" s="17">
+        <v>1</v>
+      </c>
+      <c r="P303" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q303" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="304" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A304" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B304" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="C304" s="57" t="s">
-        <v>315</v>
-      </c>
-      <c r="D304" s="48"/>
-      <c r="E304" s="48"/>
-      <c r="F304" s="48"/>
-      <c r="G304" s="54"/>
-      <c r="H304" s="54">
-        <v>1</v>
-      </c>
-      <c r="I304" s="54"/>
-      <c r="J304" s="54"/>
-      <c r="K304" s="54">
-        <v>1</v>
-      </c>
-      <c r="L304" s="54"/>
-      <c r="M304" s="54"/>
-      <c r="N304" s="54">
-        <v>1</v>
-      </c>
-      <c r="O304" s="54"/>
-      <c r="P304" s="54"/>
-      <c r="Q304" s="54"/>
+      <c r="B304" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C304" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="D304" s="45"/>
+      <c r="E304" s="45"/>
+      <c r="F304" s="45"/>
+      <c r="G304" s="17">
+        <v>1</v>
+      </c>
+      <c r="H304" s="17">
+        <v>1</v>
+      </c>
+      <c r="I304" s="17">
+        <v>1</v>
+      </c>
+      <c r="J304" s="17">
+        <v>1</v>
+      </c>
+      <c r="K304" s="17">
+        <v>1</v>
+      </c>
+      <c r="L304" s="17">
+        <v>1</v>
+      </c>
+      <c r="M304" s="17">
+        <v>1</v>
+      </c>
+      <c r="N304" s="17">
+        <v>1</v>
+      </c>
+      <c r="O304" s="17">
+        <v>1</v>
+      </c>
+      <c r="P304" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q304" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="305" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A305" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B305" s="55" t="s">
-        <v>6</v>
-      </c>
-      <c r="C305" s="57" t="s">
-        <v>314</v>
+      <c r="B305" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C305" s="56" t="s">
+        <v>124</v>
       </c>
       <c r="D305" s="48"/>
       <c r="E305" s="48"/>
       <c r="F305" s="48"/>
-      <c r="G305" s="54"/>
+      <c r="G305" s="54">
+        <v>1</v>
+      </c>
       <c r="H305" s="54">
         <v>1</v>
       </c>
       <c r="I305" s="54"/>
-      <c r="J305" s="54"/>
+      <c r="J305" s="54">
+        <v>1</v>
+      </c>
       <c r="K305" s="54">
         <v>1</v>
       </c>
@@ -10770,7 +10808,7 @@
         <v>6</v>
       </c>
       <c r="C306" s="57" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D306" s="48"/>
       <c r="E306" s="48"/>
@@ -10801,7 +10839,7 @@
         <v>6</v>
       </c>
       <c r="C307" s="57" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D307" s="48"/>
       <c r="E307" s="48"/>
@@ -10832,7 +10870,7 @@
         <v>6</v>
       </c>
       <c r="C308" s="57" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D308" s="48"/>
       <c r="E308" s="48"/>
@@ -10855,58 +10893,120 @@
       <c r="P308" s="54"/>
       <c r="Q308" s="54"/>
     </row>
+    <row r="309" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A309" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B309" s="55" t="s">
+        <v>6</v>
+      </c>
+      <c r="C309" s="57" t="s">
+        <v>316</v>
+      </c>
+      <c r="D309" s="48"/>
+      <c r="E309" s="48"/>
+      <c r="F309" s="48"/>
+      <c r="G309" s="54"/>
+      <c r="H309" s="54">
+        <v>1</v>
+      </c>
+      <c r="I309" s="54"/>
+      <c r="J309" s="54"/>
+      <c r="K309" s="54">
+        <v>1</v>
+      </c>
+      <c r="L309" s="54"/>
+      <c r="M309" s="54"/>
+      <c r="N309" s="54">
+        <v>1</v>
+      </c>
+      <c r="O309" s="54"/>
+      <c r="P309" s="54"/>
+      <c r="Q309" s="54"/>
+    </row>
+    <row r="310" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A310" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B310" s="55" t="s">
+        <v>6</v>
+      </c>
+      <c r="C310" s="57" t="s">
+        <v>317</v>
+      </c>
+      <c r="D310" s="48"/>
+      <c r="E310" s="48"/>
+      <c r="F310" s="48"/>
+      <c r="G310" s="54"/>
+      <c r="H310" s="54">
+        <v>1</v>
+      </c>
+      <c r="I310" s="54"/>
+      <c r="J310" s="54"/>
+      <c r="K310" s="54">
+        <v>1</v>
+      </c>
+      <c r="L310" s="54"/>
+      <c r="M310" s="54"/>
+      <c r="N310" s="54">
+        <v>1</v>
+      </c>
+      <c r="O310" s="54"/>
+      <c r="P310" s="54"/>
+      <c r="Q310" s="54"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Q308" xr:uid="{A96C7FF1-A6C9-A643-BFCA-7D7FCDAF5533}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q308">
-      <sortCondition ref="A1:A308"/>
+  <autoFilter ref="A1:Q310" xr:uid="{A96C7FF1-A6C9-A643-BFCA-7D7FCDAF5533}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q310">
+      <sortCondition ref="A1:A310"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q302">
-    <sortCondition ref="A2:A302"/>
-    <sortCondition ref="C2:C302"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q304">
+    <sortCondition ref="A2:A304"/>
+    <sortCondition ref="C2:C304"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C95" r:id="rId1" display="https://aws.amazon.com/amplify/" xr:uid="{DD07C612-9881-1744-BD8F-2791C5BF0A5F}"/>
-    <hyperlink ref="C252" r:id="rId2" display="https://aws.amazon.com/app-mesh/" xr:uid="{F151395F-8E37-1049-9FCA-8474F2603F07}"/>
+    <hyperlink ref="C254" r:id="rId2" display="https://aws.amazon.com/app-mesh/" xr:uid="{F151395F-8E37-1049-9FCA-8474F2603F07}"/>
     <hyperlink ref="C29" r:id="rId3" display="https://aws.amazon.com/appsync/" xr:uid="{DB5645FD-41DF-9D4C-ADDB-CEEB9418B261}"/>
-    <hyperlink ref="C270" r:id="rId4" display="https://aws.amazon.com/artifact/" xr:uid="{0251BE44-6F83-3541-8CD4-81AEF00F1760}"/>
-    <hyperlink ref="C271" r:id="rId5" display="https://aws.amazon.com/audit-manager/" xr:uid="{FE0C678B-66B4-5041-87CB-7B1FF56DF53B}"/>
-    <hyperlink ref="C172" r:id="rId6" display="https://aws.amazon.com/autoscaling/" xr:uid="{900D412E-B452-CD43-BEB1-C8C1CB7269C8}"/>
-    <hyperlink ref="C173" r:id="rId7" display="https://aws.amazon.com/backup/" xr:uid="{E0DD5920-BDCE-E647-9AF3-74760943689B}"/>
+    <hyperlink ref="C272" r:id="rId4" display="https://aws.amazon.com/artifact/" xr:uid="{0251BE44-6F83-3541-8CD4-81AEF00F1760}"/>
+    <hyperlink ref="C273" r:id="rId5" display="https://aws.amazon.com/audit-manager/" xr:uid="{FE0C678B-66B4-5041-87CB-7B1FF56DF53B}"/>
+    <hyperlink ref="C173" r:id="rId6" display="https://aws.amazon.com/autoscaling/" xr:uid="{900D412E-B452-CD43-BEB1-C8C1CB7269C8}"/>
+    <hyperlink ref="C174" r:id="rId7" display="https://aws.amazon.com/backup/" xr:uid="{E0DD5920-BDCE-E647-9AF3-74760943689B}"/>
     <hyperlink ref="C44" r:id="rId8" display="https://aws.amazon.com/batch/" xr:uid="{784C0A03-DDEC-BE4D-88F7-7005C1BB046B}"/>
     <hyperlink ref="C67" r:id="rId9" display="https://aws.amazon.com/aws-cost-management/aws-budgets/" xr:uid="{57F5A17A-4752-B94C-8FBB-FC20BBF1A0BE}"/>
-    <hyperlink ref="C272" r:id="rId10" display="https://aws.amazon.com/certificate-manager/" xr:uid="{1F5BBCA8-0D50-C44C-907B-68E23D8E605C}"/>
+    <hyperlink ref="C274" r:id="rId10" display="https://aws.amazon.com/certificate-manager/" xr:uid="{1F5BBCA8-0D50-C44C-907B-68E23D8E605C}"/>
     <hyperlink ref="C39" r:id="rId11" display="https://aws.amazon.com/chatbot/" xr:uid="{F29F6239-1ADB-7049-AAA7-6E39F247047B}"/>
-    <hyperlink ref="C254" r:id="rId12" display="https://aws.amazon.com/cloud-map/" xr:uid="{D482891E-9EB7-EA40-9A4B-6A8D3FEADBE3}"/>
+    <hyperlink ref="C256" r:id="rId12" display="https://aws.amazon.com/cloud-map/" xr:uid="{D482891E-9EB7-EA40-9A4B-6A8D3FEADBE3}"/>
     <hyperlink ref="C100" r:id="rId13" display="https://aws.amazon.com/cloud9/" xr:uid="{D565484B-E9EF-EA40-BDBE-0314AF229AE7}"/>
-    <hyperlink ref="C174" r:id="rId14" display="https://aws.amazon.com/cloudformation/" xr:uid="{602EC08B-B845-E049-943E-890A120862C8}"/>
-    <hyperlink ref="C274" r:id="rId15" display="https://aws.amazon.com/cloudhsm/" xr:uid="{76B855B6-4A01-1642-8706-3316A1643BA7}"/>
-    <hyperlink ref="C175" r:id="rId16" display="https://aws.amazon.com/cloudtrail/" xr:uid="{F1C2A161-2AD0-B14D-B62A-2640A558856F}"/>
+    <hyperlink ref="C175" r:id="rId14" display="https://aws.amazon.com/cloudformation/" xr:uid="{602EC08B-B845-E049-943E-890A120862C8}"/>
+    <hyperlink ref="C276" r:id="rId15" display="https://aws.amazon.com/cloudhsm/" xr:uid="{76B855B6-4A01-1642-8706-3316A1643BA7}"/>
+    <hyperlink ref="C176" r:id="rId16" display="https://aws.amazon.com/cloudtrail/" xr:uid="{F1C2A161-2AD0-B14D-B62A-2640A558856F}"/>
     <hyperlink ref="C102" r:id="rId17" display="https://aws.amazon.com/codeartifact" xr:uid="{A5B8559F-E4FA-BC42-AC7A-9D708C1D63A0}"/>
     <hyperlink ref="C103" r:id="rId18" display="https://aws.amazon.com/codebuild/" xr:uid="{E4144166-80F6-E741-B704-7C3864420913}"/>
     <hyperlink ref="C104" r:id="rId19" display="https://aws.amazon.com/codecommit/" xr:uid="{C9DB0F3B-CAEF-524C-A620-ACEA3E04FA66}"/>
     <hyperlink ref="C105" r:id="rId20" display="https://aws.amazon.com/codedeploy/" xr:uid="{D94C938E-B3D5-054D-AC63-39672D0C0DFC}"/>
     <hyperlink ref="C107" r:id="rId21" display="https://aws.amazon.com/codepipeline/" xr:uid="{DA2435A7-DA61-A54F-B02D-9BA62C072DF8}"/>
     <hyperlink ref="C108" r:id="rId22" display="https://aws.amazon.com/codestar/" xr:uid="{80EC7E07-A675-4540-8CC7-7CD9427476B0}"/>
-    <hyperlink ref="C177" r:id="rId23" display="https://aws.amazon.com/compute-optimizer/" xr:uid="{099597B3-D96C-124F-8A6B-DB661823AC75}"/>
-    <hyperlink ref="C178" r:id="rId24" display="https://aws.amazon.com/config/" xr:uid="{1DE61048-35C8-FB4C-A941-8996CBD19463}"/>
-    <hyperlink ref="C180" r:id="rId25" display="https://aws.amazon.com/controltower" xr:uid="{5ACDD884-3684-1840-9A42-603B4BFD4DFA}"/>
-    <hyperlink ref="C237" r:id="rId26" display="https://aws.amazon.com/data-exchange/" xr:uid="{EF81BA84-5C8F-DD4B-A31A-47BF7D5C826C}"/>
-    <hyperlink ref="C240" r:id="rId27" display="https://aws.amazon.com/datasync" xr:uid="{7CED07B2-F329-1D46-A78D-E74BADEF8307}"/>
-    <hyperlink ref="C239" r:id="rId28" display="https://aws.amazon.com/dms/" xr:uid="{C9210BF6-9C8C-5E48-824D-711353B0A5C4}"/>
-    <hyperlink ref="C256" r:id="rId29" display="https://aws.amazon.com/directconnect/" xr:uid="{D4260538-1F28-C64D-999E-B57D8B4A110D}"/>
-    <hyperlink ref="C277" r:id="rId30" display="https://aws.amazon.com/directoryservice/" xr:uid="{71568105-08FB-3E48-ADDD-31FCAC00E550}"/>
+    <hyperlink ref="C178" r:id="rId23" display="https://aws.amazon.com/compute-optimizer/" xr:uid="{099597B3-D96C-124F-8A6B-DB661823AC75}"/>
+    <hyperlink ref="C179" r:id="rId24" display="https://aws.amazon.com/config/" xr:uid="{1DE61048-35C8-FB4C-A941-8996CBD19463}"/>
+    <hyperlink ref="C181" r:id="rId25" display="https://aws.amazon.com/controltower" xr:uid="{5ACDD884-3684-1840-9A42-603B4BFD4DFA}"/>
+    <hyperlink ref="C239" r:id="rId26" display="https://aws.amazon.com/data-exchange/" xr:uid="{EF81BA84-5C8F-DD4B-A31A-47BF7D5C826C}"/>
+    <hyperlink ref="C242" r:id="rId27" display="https://aws.amazon.com/datasync" xr:uid="{7CED07B2-F329-1D46-A78D-E74BADEF8307}"/>
+    <hyperlink ref="C241" r:id="rId28" display="https://aws.amazon.com/dms/" xr:uid="{C9210BF6-9C8C-5E48-824D-711353B0A5C4}"/>
+    <hyperlink ref="C258" r:id="rId29" display="https://aws.amazon.com/directconnect/" xr:uid="{D4260538-1F28-C64D-999E-B57D8B4A110D}"/>
+    <hyperlink ref="C279" r:id="rId30" display="https://aws.amazon.com/directoryservice/" xr:uid="{71568105-08FB-3E48-ADDD-31FCAC00E550}"/>
     <hyperlink ref="C47" r:id="rId31" display="https://aws.amazon.com/elasticbeanstalk/" xr:uid="{503FA701-A8C3-BA4D-8F14-4F45B1936437}"/>
-    <hyperlink ref="C218" r:id="rId32" display="https://aws.amazon.com/mediaconnect" xr:uid="{97EBEF96-B9F8-0444-803B-77B7686AD926}"/>
-    <hyperlink ref="C219" r:id="rId33" display="https://aws.amazon.com/mediaconvert/" xr:uid="{A189CA26-8FE5-724E-AB4C-DA1684A9397C}"/>
-    <hyperlink ref="C220" r:id="rId34" display="https://aws.amazon.com/medialive/" xr:uid="{8A1902D4-C3B2-6540-B6A2-D0939C092476}"/>
+    <hyperlink ref="C220" r:id="rId32" display="https://aws.amazon.com/mediaconnect" xr:uid="{97EBEF96-B9F8-0444-803B-77B7686AD926}"/>
+    <hyperlink ref="C221" r:id="rId33" display="https://aws.amazon.com/mediaconvert/" xr:uid="{A189CA26-8FE5-724E-AB4C-DA1684A9397C}"/>
+    <hyperlink ref="C222" r:id="rId34" display="https://aws.amazon.com/medialive/" xr:uid="{8A1902D4-C3B2-6540-B6A2-D0939C092476}"/>
     <hyperlink ref="C62" r:id="rId35" display="https://aws.amazon.com/fargate/" xr:uid="{8AAC0488-BCAF-394A-B65D-1C8169C9015E}"/>
-    <hyperlink ref="C281" r:id="rId36" display="https://aws.amazon.com/firewall-manager/" xr:uid="{C1FC3FB2-6BB1-124F-AA39-0A32AEF1D03C}"/>
-    <hyperlink ref="C258" r:id="rId37" display="https://aws.amazon.com/global-accelerator" xr:uid="{94823B64-0747-B847-98EC-9C84C21B2DE2}"/>
+    <hyperlink ref="C283" r:id="rId36" display="https://aws.amazon.com/firewall-manager/" xr:uid="{C1FC3FB2-6BB1-124F-AA39-0A32AEF1D03C}"/>
+    <hyperlink ref="C260" r:id="rId37" display="https://aws.amazon.com/global-accelerator" xr:uid="{94823B64-0747-B847-98EC-9C84C21B2DE2}"/>
     <hyperlink ref="C7" r:id="rId38" display="https://aws.amazon.com/glue/" xr:uid="{A2984E2F-A64C-D74C-A499-872A26B2DE44}"/>
-    <hyperlink ref="C269" r:id="rId39" display="https://aws.amazon.com/ground-station/" xr:uid="{DB86E86A-EF5B-2541-9BD8-5CDA9965E40C}"/>
+    <hyperlink ref="C271" r:id="rId39" display="https://aws.amazon.com/ground-station/" xr:uid="{DB86E86A-EF5B-2541-9BD8-5CDA9965E40C}"/>
     <hyperlink ref="C73" r:id="rId40" display="https://aws.amazon.com/iq/" xr:uid="{66074B4A-E4D5-724E-AD29-24C171CEC0BA}"/>
-    <hyperlink ref="C284" r:id="rId41" display="https://aws.amazon.com/iam" xr:uid="{97081695-DB1E-424E-B0EE-79AAD8D6E1CE}"/>
+    <hyperlink ref="C286" r:id="rId41" display="https://aws.amazon.com/iam" xr:uid="{97081695-DB1E-424E-B0EE-79AAD8D6E1CE}"/>
     <hyperlink ref="C125" r:id="rId42" display="https://aws.amazon.com/iot-1-click/" xr:uid="{ADC027FD-055F-9343-AF7A-479D41533208}"/>
     <hyperlink ref="C126" r:id="rId43" display="https://aws.amazon.com/iot-analytics/" xr:uid="{6587843B-FF8F-E445-A148-97BAA80660A5}"/>
     <hyperlink ref="C127" r:id="rId44" display="https://aws.amazon.com/iot/" xr:uid="{72ADB53E-C5C8-6E45-9DE6-006357ADBB14}"/>
@@ -10914,123 +11014,123 @@
     <hyperlink ref="C129" r:id="rId46" display="https://aws.amazon.com/iot-device-management/" xr:uid="{47327A94-A7DA-D44B-8D5D-137A2C1DB78D}"/>
     <hyperlink ref="C131" r:id="rId47" display="https://aws.amazon.com/iot-events/" xr:uid="{09A17074-F045-D045-99F3-289DE651CC4B}"/>
     <hyperlink ref="C132" r:id="rId48" display="https://aws.amazon.com/greengrass/" xr:uid="{86C6B532-C282-AD49-84FC-E7151CC17562}"/>
-    <hyperlink ref="C286" r:id="rId49" display="https://aws.amazon.com/kms/" xr:uid="{C0A6E0DF-7D93-854D-AF8E-5B9C19B8AF02}"/>
+    <hyperlink ref="C288" r:id="rId49" display="https://aws.amazon.com/kms/" xr:uid="{C0A6E0DF-7D93-854D-AF8E-5B9C19B8AF02}"/>
     <hyperlink ref="C18" r:id="rId50" display="https://aws.amazon.com/lake-formation/" xr:uid="{8B1B5135-7A0D-7645-A701-475DDEBCFDA0}"/>
     <hyperlink ref="C49" r:id="rId51" display="https://aws.amazon.com/lambda/" xr:uid="{23B44498-C148-BD4C-86FE-EFAA00464E5B}"/>
-    <hyperlink ref="C183" r:id="rId52" display="https://aws.amazon.com/license-manager/" xr:uid="{A80531A2-32DF-5E46-A8A2-AD514A9E876E}"/>
+    <hyperlink ref="C184" r:id="rId52" display="https://aws.amazon.com/license-manager/" xr:uid="{A80531A2-32DF-5E46-A8A2-AD514A9E876E}"/>
     <hyperlink ref="C75" r:id="rId53" display="https://aws.amazon.com/mp/" xr:uid="{83E81132-B5F9-A141-93D4-67826C5C6C2F}"/>
-    <hyperlink ref="C259" r:id="rId54" display="https://aws.amazon.com/network-firewall/" xr:uid="{380438F2-2136-CA48-8A93-614BD286828F}"/>
-    <hyperlink ref="C188" r:id="rId55" display="https://aws.amazon.com/opsworks/stacks/" xr:uid="{C7B2C66E-7305-8A45-B44D-ED0E58D460E7}"/>
-    <hyperlink ref="C186" r:id="rId56" display="https://aws.amazon.com/opsworks/chefautomate/" xr:uid="{44B83691-1D72-4540-A13B-BDA885E2E12D}"/>
-    <hyperlink ref="C187" r:id="rId57" display="https://aws.amazon.com/opsworks/puppetenterprise/" xr:uid="{23F41EB8-3A55-A44E-BD0D-93039495EA49}"/>
-    <hyperlink ref="C189" r:id="rId58" display="https://aws.amazon.com/organizations" xr:uid="{A3AB0BF0-AC79-A142-8708-144AD8A2BAF3}"/>
+    <hyperlink ref="C261" r:id="rId54" display="https://aws.amazon.com/network-firewall/" xr:uid="{380438F2-2136-CA48-8A93-614BD286828F}"/>
+    <hyperlink ref="C189" r:id="rId55" display="https://aws.amazon.com/opsworks/stacks/" xr:uid="{C7B2C66E-7305-8A45-B44D-ED0E58D460E7}"/>
+    <hyperlink ref="C187" r:id="rId56" display="https://aws.amazon.com/opsworks/chefautomate/" xr:uid="{44B83691-1D72-4540-A13B-BDA885E2E12D}"/>
+    <hyperlink ref="C188" r:id="rId57" display="https://aws.amazon.com/opsworks/puppetenterprise/" xr:uid="{23F41EB8-3A55-A44E-BD0D-93039495EA49}"/>
+    <hyperlink ref="C190" r:id="rId58" display="https://aws.amazon.com/organizations" xr:uid="{A3AB0BF0-AC79-A142-8708-144AD8A2BAF3}"/>
     <hyperlink ref="C51" r:id="rId59" display="https://aws.amazon.com/outposts/" xr:uid="{EC0218BA-7EA9-5F4D-8A2F-8D931B087AA0}"/>
-    <hyperlink ref="C190" r:id="rId60" display="https://aws.amazon.com/premiumsupport/phd/" xr:uid="{BC843AAF-6516-F341-B87D-0984C181B4B5}"/>
-    <hyperlink ref="C260" r:id="rId61" display="https://aws.amazon.com/privatelink/" xr:uid="{908DA648-769A-FB47-86E4-3D66FA675B1C}"/>
+    <hyperlink ref="C191" r:id="rId60" display="https://aws.amazon.com/premiumsupport/phd/" xr:uid="{BC843AAF-6516-F341-B87D-0984C181B4B5}"/>
+    <hyperlink ref="C262" r:id="rId61" display="https://aws.amazon.com/privatelink/" xr:uid="{908DA648-769A-FB47-86E4-3D66FA675B1C}"/>
     <hyperlink ref="C64" r:id="rId62" display="https://aws.amazon.com/proton/" xr:uid="{73BECBB6-D4BE-F445-97BF-0A1D62BCA194}"/>
-    <hyperlink ref="C191" r:id="rId63" display="https://aws.amazon.com/ram/" xr:uid="{F8E211FB-42AB-6848-88B7-49CC2A833913}"/>
-    <hyperlink ref="C268" r:id="rId64" display="https://aws.amazon.com/robomaker/" xr:uid="{DBD68496-4CE8-804C-B893-9CFFB849F53A}"/>
-    <hyperlink ref="C288" r:id="rId65" display="https://aws.amazon.com/secrets-manager/" xr:uid="{632A5D67-D598-184C-AB9B-96F30896117D}"/>
-    <hyperlink ref="C289" r:id="rId66" display="https://aws.amazon.com/security-hub/" xr:uid="{342A4832-F3A0-DB4D-840C-8118FD830399}"/>
-    <hyperlink ref="C246" r:id="rId67" display="https://aws.amazon.com/server-migration-service/" xr:uid="{9446514E-0CE8-EC41-A9F1-0DC1FB7ADA55}"/>
+    <hyperlink ref="C192" r:id="rId63" display="https://aws.amazon.com/ram/" xr:uid="{F8E211FB-42AB-6848-88B7-49CC2A833913}"/>
+    <hyperlink ref="C270" r:id="rId64" display="https://aws.amazon.com/robomaker/" xr:uid="{DBD68496-4CE8-804C-B893-9CFFB849F53A}"/>
+    <hyperlink ref="C290" r:id="rId65" display="https://aws.amazon.com/secrets-manager/" xr:uid="{632A5D67-D598-184C-AB9B-96F30896117D}"/>
+    <hyperlink ref="C291" r:id="rId66" display="https://aws.amazon.com/security-hub/" xr:uid="{342A4832-F3A0-DB4D-840C-8118FD830399}"/>
+    <hyperlink ref="C248" r:id="rId67" display="https://aws.amazon.com/server-migration-service/" xr:uid="{9446514E-0CE8-EC41-A9F1-0DC1FB7ADA55}"/>
     <hyperlink ref="C52" r:id="rId68" display="https://aws.amazon.com/serverless/serverlessrepo/" xr:uid="{8F7AC4BC-9A37-EC4F-8183-7D7404D19E14}"/>
-    <hyperlink ref="C192" r:id="rId69" display="https://aws.amazon.com/servicecatalog/" xr:uid="{2D2653B1-3D13-014A-9B9C-2386E2577635}"/>
-    <hyperlink ref="C290" r:id="rId70" display="https://aws.amazon.com/shield/" xr:uid="{76E091F3-F618-A648-879F-3F09BEBFABFD}"/>
-    <hyperlink ref="C291" r:id="rId71" display="https://aws.amazon.com/single-sign-on/" xr:uid="{A8360283-DE5C-1140-A85B-F33A2D6F72B8}"/>
-    <hyperlink ref="C247" r:id="rId72" display="https://aws.amazon.com/snowball/" xr:uid="{8A7E1B57-5F26-F64E-853D-BDD63390D5E6}"/>
-    <hyperlink ref="C249" r:id="rId73" display="https://aws.amazon.com/snowmobile/" xr:uid="{62B7D92F-3C96-DA44-9F02-BCC308391061}"/>
+    <hyperlink ref="C193" r:id="rId69" display="https://aws.amazon.com/servicecatalog/" xr:uid="{2D2653B1-3D13-014A-9B9C-2386E2577635}"/>
+    <hyperlink ref="C292" r:id="rId70" display="https://aws.amazon.com/shield/" xr:uid="{76E091F3-F618-A648-879F-3F09BEBFABFD}"/>
+    <hyperlink ref="C293" r:id="rId71" display="https://aws.amazon.com/single-sign-on/" xr:uid="{A8360283-DE5C-1140-A85B-F33A2D6F72B8}"/>
+    <hyperlink ref="C249" r:id="rId72" display="https://aws.amazon.com/snowball/" xr:uid="{8A7E1B57-5F26-F64E-853D-BDD63390D5E6}"/>
+    <hyperlink ref="C251" r:id="rId73" display="https://aws.amazon.com/snowmobile/" xr:uid="{62B7D92F-3C96-DA44-9F02-BCC308391061}"/>
     <hyperlink ref="C36" r:id="rId74" display="https://aws.amazon.com/step-functions/details/" xr:uid="{10824B81-0A5F-634D-84E6-9D2ADE3A6B39}"/>
-    <hyperlink ref="C303" r:id="rId75" display="https://aws.amazon.com/storagegateway/" xr:uid="{7BF17EFE-FF03-1D4A-BE9E-1FA982DA5C2A}"/>
+    <hyperlink ref="C305" r:id="rId75" display="https://aws.amazon.com/storagegateway/" xr:uid="{7BF17EFE-FF03-1D4A-BE9E-1FA982DA5C2A}"/>
     <hyperlink ref="C77" r:id="rId76" display="https://aws.amazon.com/premiumsupport/" xr:uid="{A5466C95-EFB7-3944-9E29-8D19BB6E169F}"/>
-    <hyperlink ref="C210" r:id="rId77" display="https://aws.amazon.com/systems-manager/" xr:uid="{D6C17500-BE92-C444-BA4A-7116B75319D3}"/>
-    <hyperlink ref="C250" r:id="rId78" display="https://aws.amazon.com/aws-transfer-family/" xr:uid="{F0069BD4-8633-FB4B-8185-293CB3193797}"/>
-    <hyperlink ref="C263" r:id="rId79" display="https://aws.amazon.com/transit-gateway/" xr:uid="{2C10B2F7-EEE3-3444-A855-B387D48706EA}"/>
-    <hyperlink ref="C211" r:id="rId80" display="https://aws.amazon.com/premiumsupport/trustedadvisor/" xr:uid="{436ECB3D-7EFE-764A-B2E3-3CF79C97B742}"/>
-    <hyperlink ref="C266" r:id="rId81" display="https://aws.amazon.com/vpn/" xr:uid="{5F2B553B-98BD-8D4B-849C-55A6F659C6B1}"/>
-    <hyperlink ref="C292" r:id="rId82" display="https://aws.amazon.com/waf/" xr:uid="{CF739D06-0B1B-6B46-91CF-6EE57FF09613}"/>
-    <hyperlink ref="C212" r:id="rId83" display="https://aws.amazon.com/well-architected-tool" xr:uid="{81A34672-555C-B74A-9D7B-58590B7D3C75}"/>
+    <hyperlink ref="C211" r:id="rId77" display="https://aws.amazon.com/systems-manager/" xr:uid="{D6C17500-BE92-C444-BA4A-7116B75319D3}"/>
+    <hyperlink ref="C252" r:id="rId78" display="https://aws.amazon.com/aws-transfer-family/" xr:uid="{F0069BD4-8633-FB4B-8185-293CB3193797}"/>
+    <hyperlink ref="C265" r:id="rId79" display="https://aws.amazon.com/transit-gateway/" xr:uid="{2C10B2F7-EEE3-3444-A855-B387D48706EA}"/>
+    <hyperlink ref="C212" r:id="rId80" display="https://aws.amazon.com/premiumsupport/trustedadvisor/" xr:uid="{436ECB3D-7EFE-764A-B2E3-3CF79C97B742}"/>
+    <hyperlink ref="C268" r:id="rId81" display="https://aws.amazon.com/vpn/" xr:uid="{5F2B553B-98BD-8D4B-849C-55A6F659C6B1}"/>
+    <hyperlink ref="C294" r:id="rId82" display="https://aws.amazon.com/waf/" xr:uid="{CF739D06-0B1B-6B46-91CF-6EE57FF09613}"/>
+    <hyperlink ref="C213" r:id="rId83" display="https://aws.amazon.com/well-architected-tool" xr:uid="{81A34672-555C-B74A-9D7B-58590B7D3C75}"/>
     <hyperlink ref="C117" r:id="rId84" display="https://aws.amazon.com/xray/" xr:uid="{91A2B229-E348-8B4C-AF47-A5192DE45AEC}"/>
-    <hyperlink ref="C251" r:id="rId85" display="https://aws.amazon.com/api-gateway/" xr:uid="{81259B3E-1AB3-F64C-B232-9643470BBB0C}"/>
+    <hyperlink ref="C253" r:id="rId85" display="https://aws.amazon.com/api-gateway/" xr:uid="{81259B3E-1AB3-F64C-B232-9643470BBB0C}"/>
     <hyperlink ref="C28" r:id="rId86" display="https://aws.amazon.com/appflow/" xr:uid="{C427BFEE-537C-9B4C-B5FD-EF94DAB3195F}"/>
     <hyperlink ref="C2" r:id="rId87" display="https://aws.amazon.com/athena/" xr:uid="{8CA6E242-2CF4-E843-A8CA-4391EDA4CB08}"/>
     <hyperlink ref="C136" r:id="rId88" display="https://aws.amazon.com/augmented-ai/" xr:uid="{9B0A35B8-349D-874F-B406-0C378A70E4A7}"/>
     <hyperlink ref="C82" r:id="rId89" display="https://aws.amazon.com/rds/aurora/" xr:uid="{5BA37BE5-5EFA-D640-9340-68572A5C8B0A}"/>
     <hyperlink ref="C40" r:id="rId90" display="https://chime.aws/" xr:uid="{08A22D72-3716-8743-A4B8-3002293D3436}"/>
-    <hyperlink ref="C273" r:id="rId91" display="https://aws.amazon.com/cloud-directory/" xr:uid="{E41D133C-BA4E-4642-BA6F-656788DBC830}"/>
-    <hyperlink ref="C255" r:id="rId92" display="https://aws.amazon.com/cloudfront/" xr:uid="{8065D5C6-B564-A941-80CC-5D6C65B3D725}"/>
-    <hyperlink ref="C176" r:id="rId93" display="https://aws.amazon.com/cloudwatch/" xr:uid="{52B01F49-5EAB-E540-BA38-BEED42EB43F4}"/>
+    <hyperlink ref="C275" r:id="rId91" display="https://aws.amazon.com/cloud-directory/" xr:uid="{E41D133C-BA4E-4642-BA6F-656788DBC830}"/>
+    <hyperlink ref="C257" r:id="rId92" display="https://aws.amazon.com/cloudfront/" xr:uid="{8065D5C6-B564-A941-80CC-5D6C65B3D725}"/>
+    <hyperlink ref="C177" r:id="rId93" display="https://aws.amazon.com/cloudwatch/" xr:uid="{52B01F49-5EAB-E540-BA38-BEED42EB43F4}"/>
     <hyperlink ref="C106" r:id="rId94" display="https://aws.amazon.com/codeguru/" xr:uid="{D5D1E2B5-ED1C-0D45-BCD8-07A6431E8C14}"/>
-    <hyperlink ref="C275" r:id="rId95" display="https://aws.amazon.com/cognito/" xr:uid="{5631285D-2790-B940-99E8-7A2AFBF2A4F8}"/>
+    <hyperlink ref="C277" r:id="rId95" display="https://aws.amazon.com/cognito/" xr:uid="{5631285D-2790-B940-99E8-7A2AFBF2A4F8}"/>
     <hyperlink ref="C137" r:id="rId96" display="https://aws.amazon.com/comprehend/" xr:uid="{EF9B7DCD-AAB7-C840-B56B-6901E4208F3C}"/>
     <hyperlink ref="C138" r:id="rId97" display="https://aws.amazon.com/comprehend/medical/" xr:uid="{E755C2E6-BB69-1547-AEEA-159FA230C6E0}"/>
-    <hyperlink ref="C276" r:id="rId98" display="https://aws.amazon.com/detective/" xr:uid="{4F6306C8-7E6E-B543-8987-505512DF8B38}"/>
+    <hyperlink ref="C278" r:id="rId98" display="https://aws.amazon.com/detective/" xr:uid="{4F6306C8-7E6E-B543-8987-505512DF8B38}"/>
     <hyperlink ref="C143" r:id="rId99" display="https://aws.amazon.com/devops-guru/" xr:uid="{0DE3687A-6EED-D846-93EF-2FF3EDCA2FE7}"/>
     <hyperlink ref="C83" r:id="rId100" display="https://aws.amazon.com/documentdb/" xr:uid="{E9BE873B-93B3-744C-82A3-AE676C942786}"/>
     <hyperlink ref="C84" r:id="rId101" display="https://aws.amazon.com/dynamodb/" xr:uid="{667C0B17-E586-7843-9ABA-2156F328D1C2}"/>
     <hyperlink ref="C87" r:id="rId102" display="https://aws.amazon.com/elasticache/" xr:uid="{0D3B6893-EB9F-F441-97F2-EAE3A531E741}"/>
-    <hyperlink ref="C295" r:id="rId103" display="https://aws.amazon.com/ebs/" xr:uid="{6475A1BA-F9EA-3643-A91C-960971815276}"/>
+    <hyperlink ref="C297" r:id="rId103" display="https://aws.amazon.com/ebs/" xr:uid="{6475A1BA-F9EA-3643-A91C-960971815276}"/>
     <hyperlink ref="C45" r:id="rId104" xr:uid="{F6BE2D25-6B4D-D545-BEF5-6353621F7D77}"/>
     <hyperlink ref="C59" r:id="rId105" display="https://aws.amazon.com/ecr/" xr:uid="{4DB8575D-FD4E-F24B-9A6D-4B237DEB4216}"/>
     <hyperlink ref="C60" r:id="rId106" display="https://aws.amazon.com/ecs/" xr:uid="{2A857716-DB7F-4D4C-9C3A-923E359FCE4B}"/>
-    <hyperlink ref="C296" r:id="rId107" display="https://aws.amazon.com/efs/" xr:uid="{17293663-847A-2945-BEEE-DB5C14186604}"/>
+    <hyperlink ref="C298" r:id="rId107" display="https://aws.amazon.com/efs/" xr:uid="{17293663-847A-2945-BEEE-DB5C14186604}"/>
     <hyperlink ref="C144" r:id="rId108" display="https://aws.amazon.com/elastic-inference/" xr:uid="{D7F32AC2-662A-044F-8D07-6056298BD732}"/>
     <hyperlink ref="C61" r:id="rId109" display="https://aws.amazon.com/eks" xr:uid="{8EA95DB8-FAF6-354A-8701-9BC26B99AF7A}"/>
     <hyperlink ref="C4" r:id="rId110" display="https://aws.amazon.com/emr/" xr:uid="{45F7CBE2-565C-A24D-A38F-B3A8800D8B65}"/>
     <hyperlink ref="C20" r:id="rId111" display="Elasticsearch Service (ES) / OpenSearch Service" xr:uid="{6AF99F4A-A394-8249-8B46-B05EDE624400}"/>
     <hyperlink ref="C30" r:id="rId112" display="https://aws.amazon.com/eventbridge/" xr:uid="{66CE333B-4CBB-9246-B3B7-51C615E2BFF5}"/>
-    <hyperlink ref="C298" r:id="rId113" display="https://aws.amazon.com/fsx/lustre/" xr:uid="{723E4B6B-4225-F149-A1D1-0C9ED96BB728}"/>
-    <hyperlink ref="C299" r:id="rId114" display="https://aws.amazon.com/fsx/windows/" xr:uid="{1B6B9E68-B13B-3B45-B1A5-A8F3F5BDE985}"/>
+    <hyperlink ref="C300" r:id="rId113" display="https://aws.amazon.com/fsx/lustre/" xr:uid="{723E4B6B-4225-F149-A1D1-0C9ED96BB728}"/>
+    <hyperlink ref="C301" r:id="rId114" display="https://aws.amazon.com/fsx/windows/" xr:uid="{1B6B9E68-B13B-3B45-B1A5-A8F3F5BDE985}"/>
     <hyperlink ref="C145" r:id="rId115" display="https://aws.amazon.com/forecast/" xr:uid="{1F07E3AD-D0E3-4442-9220-92E85E3DF861}"/>
     <hyperlink ref="C146" r:id="rId116" display="https://aws.amazon.com/fraud-detector/" xr:uid="{A16ABA87-0E9D-1749-BE3E-718E7599E24B}"/>
     <hyperlink ref="C121" r:id="rId117" display="https://aws.amazon.com/gamelift/" xr:uid="{ABE766D8-2E8B-B341-9103-F503839AC514}"/>
-    <hyperlink ref="C282" r:id="rId118" display="https://aws.amazon.com/guardduty/" xr:uid="{D1B6E14A-AD6C-E844-9AD0-215698F4E3BE}"/>
-    <hyperlink ref="C285" r:id="rId119" display="https://aws.amazon.com/inspector/" xr:uid="{176BE9A8-3FF5-874F-8EFA-6BB4665C2F33}"/>
+    <hyperlink ref="C284" r:id="rId118" display="https://aws.amazon.com/guardduty/" xr:uid="{D1B6E14A-AD6C-E844-9AD0-215698F4E3BE}"/>
+    <hyperlink ref="C287" r:id="rId119" display="https://aws.amazon.com/inspector/" xr:uid="{176BE9A8-3FF5-874F-8EFA-6BB4665C2F33}"/>
     <hyperlink ref="C88" r:id="rId120" display="https://aws.amazon.com/keyspaces/" xr:uid="{08537BC8-9E18-E341-B811-B357F4073FF5}"/>
     <hyperlink ref="C15" r:id="rId121" display="https://aws.amazon.com/kinesis/analytics/" xr:uid="{55091A39-96DB-9A41-B453-9AB88556B85B}"/>
     <hyperlink ref="C16" r:id="rId122" display="https://aws.amazon.com/kinesis/firehose/" xr:uid="{AB91BD64-7EBD-8A40-89D5-415AC999E5A7}"/>
     <hyperlink ref="C17" r:id="rId123" display="https://aws.amazon.com/kinesis/streams/" xr:uid="{683B50F9-C9B3-9046-A380-EAD32C0551EC}"/>
-    <hyperlink ref="C226" r:id="rId124" display="https://aws.amazon.com/kinesis/video-streams/" xr:uid="{92727233-FF93-4048-90C3-EB7CFF6B76A0}"/>
+    <hyperlink ref="C228" r:id="rId124" display="https://aws.amazon.com/kinesis/video-streams/" xr:uid="{92727233-FF93-4048-90C3-EB7CFF6B76A0}"/>
     <hyperlink ref="C50" r:id="rId125" display="https://amazonlightsail.com/" xr:uid="{5C26023E-C913-634E-BBA9-96985AD232E5}"/>
     <hyperlink ref="C114" r:id="rId126" display="https://aws.amazon.com/location" xr:uid="{3A5DA1F4-704B-4A4F-B42A-0132FA3F769F}"/>
-    <hyperlink ref="C148" r:id="rId127" display="https://aws.amazon.com/lookout-for-vision/" xr:uid="{56891F15-488A-2D4F-957F-9C19DBC09E8C}"/>
+    <hyperlink ref="C149" r:id="rId127" display="https://aws.amazon.com/lookout-for-vision/" xr:uid="{56891F15-488A-2D4F-957F-9C19DBC09E8C}"/>
     <hyperlink ref="C122" r:id="rId128" display="https://aws.amazon.com/lumberyard/" xr:uid="{0793FA7F-F861-E448-B351-2625AB793E29}"/>
     <hyperlink ref="C32" r:id="rId129" display="https://aws.amazon.com/amazon-mq/" xr:uid="{8F7E8190-F83B-7E45-9B55-465E1F7C79F3}"/>
-    <hyperlink ref="C287" r:id="rId130" display="https://aws.amazon.com/macie/" xr:uid="{0A9A9C7B-64FF-4944-8B73-82D7A54412E2}"/>
+    <hyperlink ref="C289" r:id="rId130" display="https://aws.amazon.com/macie/" xr:uid="{0A9A9C7B-64FF-4944-8B73-82D7A54412E2}"/>
     <hyperlink ref="C19" r:id="rId131" display="https://aws.amazon.com/msk/" xr:uid="{46024F01-6B35-0740-B92F-18BA0D596F3D}"/>
     <hyperlink ref="C31" r:id="rId132" display="https://aws.amazon.com/managed-workflows-for-apache-airflow/" xr:uid="{E7D50CE9-B395-AE40-B3BD-7B31072C139C}"/>
     <hyperlink ref="C90" r:id="rId133" display="https://aws.amazon.com/neptune/" xr:uid="{35EB7CA9-2F10-7E4E-9B05-D1C561AFFA79}"/>
-    <hyperlink ref="C150" r:id="rId134" display="https://aws.amazon.com/personalize/" xr:uid="{F1130D50-7EEE-8441-87AC-E48D5971C615}"/>
-    <hyperlink ref="C151" r:id="rId135" display="https://aws.amazon.com/polly/" xr:uid="{8F307293-7304-3046-AD9B-0CD5031F0E44}"/>
+    <hyperlink ref="C151" r:id="rId134" display="https://aws.amazon.com/personalize/" xr:uid="{F1130D50-7EEE-8441-87AC-E48D5971C615}"/>
+    <hyperlink ref="C152" r:id="rId135" display="https://aws.amazon.com/polly/" xr:uid="{8F307293-7304-3046-AD9B-0CD5031F0E44}"/>
     <hyperlink ref="C91" r:id="rId136" display="https://aws.amazon.com/qldb/" xr:uid="{2B8E2EAE-162D-EC46-B1CB-A6147249DD22}"/>
     <hyperlink ref="C21" r:id="rId137" display="https://aws.amazon.com/quicksight/" xr:uid="{F27D6948-59C0-D243-94F0-696D4BC6ED9E}"/>
     <hyperlink ref="C22" r:id="rId138" display="https://aws.amazon.com/redshift/" xr:uid="{BD068AB5-9542-BA4D-9D2D-3E01553833FF}"/>
-    <hyperlink ref="C152" r:id="rId139" display="https://aws.amazon.com/rekognition/" xr:uid="{06B644B6-712E-EB4F-BDC1-2826A6E207A2}"/>
+    <hyperlink ref="C153" r:id="rId139" display="https://aws.amazon.com/rekognition/" xr:uid="{06B644B6-712E-EB4F-BDC1-2826A6E207A2}"/>
     <hyperlink ref="C93" r:id="rId140" display="https://aws.amazon.com/rds/" xr:uid="{52A384FE-5551-524F-8BE4-640C39EE59DB}"/>
-    <hyperlink ref="C261" r:id="rId141" display="https://aws.amazon.com/route53/" xr:uid="{2B9EF04D-DB6D-9948-8F0B-1F85D1FFA02C}"/>
-    <hyperlink ref="C153" r:id="rId142" display="https://aws.amazon.com/sagemaker/" xr:uid="{FF819C8F-B472-6A4D-BF36-8803B10C8D16}"/>
+    <hyperlink ref="C263" r:id="rId141" display="https://aws.amazon.com/route53/" xr:uid="{2B9EF04D-DB6D-9948-8F0B-1F85D1FFA02C}"/>
+    <hyperlink ref="C154" r:id="rId142" display="https://aws.amazon.com/sagemaker/" xr:uid="{FF819C8F-B472-6A4D-BF36-8803B10C8D16}"/>
     <hyperlink ref="C81" r:id="rId143" display="https://aws.amazon.com/ses/" xr:uid="{708BC6D8-3F72-374C-AB65-9002B2EB5C60}"/>
     <hyperlink ref="C33" r:id="rId144" display="https://aws.amazon.com/sns/" xr:uid="{2A7374BD-4C80-7C42-9E56-E3671DF3D17F}"/>
     <hyperlink ref="C34" r:id="rId145" display="https://aws.amazon.com/sqs/" xr:uid="{7EC87AB6-C5A3-0F4B-915C-BD9EF4201FD5}"/>
-    <hyperlink ref="C302" r:id="rId146" display="https://aws.amazon.com/s3/" xr:uid="{CD425C97-24D5-9747-8B23-DF9DD7A486F9}"/>
+    <hyperlink ref="C304" r:id="rId146" display="https://aws.amazon.com/s3/" xr:uid="{CD425C97-24D5-9747-8B23-DF9DD7A486F9}"/>
     <hyperlink ref="C35" r:id="rId147" display="https://aws.amazon.com/swf/" xr:uid="{631F304E-E46F-644E-8407-57836778A272}"/>
     <hyperlink ref="C123" r:id="rId148" display="https://aws.amazon.com/sumerian/" xr:uid="{1F8D41FC-B82F-8C44-A79F-AA91C3811E29}"/>
-    <hyperlink ref="C167" r:id="rId149" display="https://aws.amazon.com/textract" xr:uid="{E50E8082-94C1-7947-963B-3A384A890F42}"/>
+    <hyperlink ref="C168" r:id="rId149" display="https://aws.amazon.com/textract" xr:uid="{E50E8082-94C1-7947-963B-3A384A890F42}"/>
     <hyperlink ref="C94" r:id="rId150" display="https://aws.amazon.com/timestream" xr:uid="{9C058FBD-47D6-324E-B7AC-2A5C552E471E}"/>
-    <hyperlink ref="C168" r:id="rId151" display="https://aws.amazon.com/transcribe/" xr:uid="{7391FC88-BBA3-5846-9CA8-5612809D5D1E}"/>
-    <hyperlink ref="C169" r:id="rId152" display="https://aws.amazon.com/transcribe/medical/" xr:uid="{5D3CF2D8-5264-E342-A8E8-E042131AE7AF}"/>
-    <hyperlink ref="C170" r:id="rId153" display="https://aws.amazon.com/translate/" xr:uid="{D94B1850-F477-024B-8A15-72298FF44F81}"/>
-    <hyperlink ref="C264" r:id="rId154" display="https://aws.amazon.com/vpc/" xr:uid="{81704202-B35B-314F-9611-62D10520486C}"/>
+    <hyperlink ref="C169" r:id="rId151" display="https://aws.amazon.com/transcribe/" xr:uid="{7391FC88-BBA3-5846-9CA8-5612809D5D1E}"/>
+    <hyperlink ref="C170" r:id="rId152" display="https://aws.amazon.com/transcribe/medical/" xr:uid="{5D3CF2D8-5264-E342-A8E8-E042131AE7AF}"/>
+    <hyperlink ref="C171" r:id="rId153" display="https://aws.amazon.com/translate/" xr:uid="{D94B1850-F477-024B-8A15-72298FF44F81}"/>
+    <hyperlink ref="C266" r:id="rId154" display="https://aws.amazon.com/vpc/" xr:uid="{81704202-B35B-314F-9611-62D10520486C}"/>
     <hyperlink ref="C119" r:id="rId155" display="https://aws.amazon.com/worklink/" xr:uid="{A564F6A5-A25E-984E-AB0E-10859F299F79}"/>
-    <hyperlink ref="C294" r:id="rId156" display="https://aws.amazon.com/cloudendure-disaster-recovery/" xr:uid="{19E2670B-B70B-2246-875A-A798E313AD4C}"/>
-    <hyperlink ref="C235" r:id="rId157" display="https://aws.amazon.com/cloudendure-migration/" xr:uid="{3011454A-BA14-2640-A5B0-1665DE5015EB}"/>
-    <hyperlink ref="C257" r:id="rId158" display="https://aws.amazon.com/elasticloadbalancing/" xr:uid="{48C41A56-7B49-954B-8607-BA52CE86305D}"/>
+    <hyperlink ref="C296" r:id="rId156" display="https://aws.amazon.com/cloudendure-disaster-recovery/" xr:uid="{19E2670B-B70B-2246-875A-A798E313AD4C}"/>
+    <hyperlink ref="C238" r:id="rId157" display="https://aws.amazon.com/cloudendure-migration/" xr:uid="{3011454A-BA14-2640-A5B0-1665DE5015EB}"/>
+    <hyperlink ref="C259" r:id="rId158" display="https://aws.amazon.com/elasticloadbalancing/" xr:uid="{48C41A56-7B49-954B-8607-BA52CE86305D}"/>
     <hyperlink ref="C124" r:id="rId159" display="https://aws.amazon.com/freertos/" xr:uid="{9A951967-4675-1546-8716-0568BF98D1CE}"/>
     <hyperlink ref="C53" r:id="rId160" display="https://aws.amazon.com/vmware/" xr:uid="{1D088AE8-27BE-C042-AB38-9D218A238493}"/>
     <hyperlink ref="C48" r:id="rId161" display="https://aws.amazon.com/ec2/" xr:uid="{A67A7092-80C0-9A4E-A55B-97FA160377E8}"/>
-    <hyperlink ref="C300" r:id="rId162" xr:uid="{9237F063-BA80-DC44-882A-D4F7F6FD5EE9}"/>
+    <hyperlink ref="C302" r:id="rId162" xr:uid="{9237F063-BA80-DC44-882A-D4F7F6FD5EE9}"/>
     <hyperlink ref="C111" r:id="rId163" xr:uid="{75CD952A-625F-DE4E-B2D6-41E51DC1F7E3}"/>
     <hyperlink ref="C37" r:id="rId164" xr:uid="{49E4FD14-55A4-2E46-8EFF-5EF1766DCF38}"/>
-    <hyperlink ref="C248" r:id="rId165" xr:uid="{7054BAB5-94B7-0C4D-A749-E850E72E4B65}"/>
+    <hyperlink ref="C250" r:id="rId165" xr:uid="{7054BAB5-94B7-0C4D-A749-E850E72E4B65}"/>
     <hyperlink ref="C80" r:id="rId166" xr:uid="{AD71ACB3-ABC2-514F-A36F-2373C95B6534}"/>
     <hyperlink ref="C79" r:id="rId167" xr:uid="{BD82E153-E205-2541-8061-196FC264C5B0}"/>
     <hyperlink ref="C5" r:id="rId168" xr:uid="{A6E6DBD8-12FD-894D-842E-E5DA02E3DBF4}"/>
@@ -11042,55 +11142,55 @@
     <hyperlink ref="C56" r:id="rId174" xr:uid="{161791FF-9796-5D41-9399-C5CC0A52B777}"/>
     <hyperlink ref="C54" r:id="rId175" xr:uid="{005354BD-081E-9E46-8937-381CB8592473}"/>
     <hyperlink ref="C58" r:id="rId176" xr:uid="{1CFA07FC-268F-C84D-B8E8-D13B2E092826}"/>
-    <hyperlink ref="C184" r:id="rId177" xr:uid="{667DCA05-C10B-394B-ADBD-C91C39C8EFA9}"/>
-    <hyperlink ref="C297" r:id="rId178" xr:uid="{19712BF9-B0E9-FC4A-855C-37C622207421}"/>
+    <hyperlink ref="C185" r:id="rId177" xr:uid="{667DCA05-C10B-394B-ADBD-C91C39C8EFA9}"/>
+    <hyperlink ref="C299" r:id="rId178" xr:uid="{19712BF9-B0E9-FC4A-855C-37C622207421}"/>
     <hyperlink ref="C101" r:id="rId179" xr:uid="{532F9FAB-7588-934A-BECA-94DB57B3EA86}"/>
     <hyperlink ref="C97" r:id="rId180" xr:uid="{03EA6A9E-9AED-E449-AEAE-E07C9D687ADF}"/>
     <hyperlink ref="C116" r:id="rId181" xr:uid="{1A9B8E63-391D-0446-8004-324356B6D2C7}"/>
     <hyperlink ref="C109" r:id="rId182" xr:uid="{D75707AD-F5F7-3548-84AF-E5C1BF57FF52}"/>
-    <hyperlink ref="C156" r:id="rId183" xr:uid="{90119A2D-8816-4C42-9A55-374991BC4E87}"/>
-    <hyperlink ref="C157" r:id="rId184" xr:uid="{CEABA1E7-2899-F04D-BD6D-ED96CD9046F5}"/>
-    <hyperlink ref="C161" r:id="rId185" xr:uid="{749E98B1-AEE6-7941-980C-8181E99A3D90}"/>
-    <hyperlink ref="C162" r:id="rId186" xr:uid="{A17C9372-FDAE-394E-9459-9D94976C283F}"/>
-    <hyperlink ref="C163" r:id="rId187" xr:uid="{29ADB2F7-F1BD-EA44-B4ED-EA881E48115D}"/>
-    <hyperlink ref="C164" r:id="rId188" xr:uid="{23D88EB1-54FB-5241-B58D-8DF71DA770BD}"/>
-    <hyperlink ref="C165" r:id="rId189" xr:uid="{FCEB0F17-6CED-E248-80B6-327E6AB92FA6}"/>
-    <hyperlink ref="C155" r:id="rId190" xr:uid="{0DF5FC7F-490C-7441-A762-E8B3E49758A0}"/>
-    <hyperlink ref="C166" r:id="rId191" xr:uid="{659782CC-853B-8944-B7EA-9CF7FC65A9C9}"/>
-    <hyperlink ref="C154" r:id="rId192" xr:uid="{9E1D2DC2-5A45-7D44-95AF-765ACB09C728}"/>
-    <hyperlink ref="C158" r:id="rId193" xr:uid="{534A3538-6476-C049-B1F4-C7F42A4A0CE2}"/>
-    <hyperlink ref="C159" r:id="rId194" xr:uid="{AD37C4EC-6AA6-7445-886F-F12B10EC4962}"/>
-    <hyperlink ref="C149" r:id="rId195" xr:uid="{32D673E8-4729-054A-941B-0538347DFE6B}"/>
-    <hyperlink ref="C193" r:id="rId196" display="AppConfig" xr:uid="{D7D5BCB4-B018-9449-8DE4-7BAC0B834A94}"/>
-    <hyperlink ref="C205" r:id="rId197" xr:uid="{6C997D60-3DAC-C54C-A365-6925F32D808B}"/>
-    <hyperlink ref="C194" r:id="rId198" xr:uid="{704C5761-85F7-8840-90D5-B9C68A5711E5}"/>
-    <hyperlink ref="C197" r:id="rId199" xr:uid="{0AE4E9A5-C51C-054C-8C1C-DFC93B7DE436}"/>
-    <hyperlink ref="C195" r:id="rId200" xr:uid="{D396B2A5-863A-0A4F-886E-AC0425111A74}"/>
-    <hyperlink ref="C203" r:id="rId201" xr:uid="{154E52D7-25A2-7B48-861E-130AEFF52429}"/>
-    <hyperlink ref="C201" r:id="rId202" xr:uid="{B55B16FC-FF18-784A-A974-098400EB5613}"/>
-    <hyperlink ref="C198" r:id="rId203" xr:uid="{2E1084D5-EB92-104E-9B36-C1C783851CEE}"/>
-    <hyperlink ref="C202" r:id="rId204" xr:uid="{CE1FE151-6237-2B48-BAA5-A0485476B07E}"/>
-    <hyperlink ref="C207" r:id="rId205" xr:uid="{8B651CA8-4121-954F-A1FD-E2ABDAE2711A}"/>
-    <hyperlink ref="C208" r:id="rId206" xr:uid="{73E53697-EA4F-5D44-BABF-E4DDE08A2949}"/>
-    <hyperlink ref="C209" r:id="rId207" xr:uid="{1F5BA02E-7700-F84C-896F-C3320A138F8C}"/>
-    <hyperlink ref="C206" r:id="rId208" xr:uid="{965DAB0C-1533-9C43-9931-A81FDFEE4801}"/>
-    <hyperlink ref="C199" r:id="rId209" xr:uid="{D7F493BC-3996-E14D-8B4E-AF698AF15CF3}"/>
-    <hyperlink ref="C204" r:id="rId210" xr:uid="{158C22B5-B282-0E45-819B-E1F6D3588EB5}"/>
-    <hyperlink ref="C200" r:id="rId211" xr:uid="{060EF427-1526-CB41-B8B7-D967487671FE}"/>
-    <hyperlink ref="C301" r:id="rId212" display="S3 Glacier" xr:uid="{69E65928-2461-9D41-874A-E2DD597C93F4}"/>
-    <hyperlink ref="C160" r:id="rId213" xr:uid="{985BD89A-8A6D-3646-8654-90328345A506}"/>
+    <hyperlink ref="C157" r:id="rId183" xr:uid="{90119A2D-8816-4C42-9A55-374991BC4E87}"/>
+    <hyperlink ref="C158" r:id="rId184" xr:uid="{CEABA1E7-2899-F04D-BD6D-ED96CD9046F5}"/>
+    <hyperlink ref="C162" r:id="rId185" xr:uid="{749E98B1-AEE6-7941-980C-8181E99A3D90}"/>
+    <hyperlink ref="C163" r:id="rId186" xr:uid="{A17C9372-FDAE-394E-9459-9D94976C283F}"/>
+    <hyperlink ref="C164" r:id="rId187" xr:uid="{29ADB2F7-F1BD-EA44-B4ED-EA881E48115D}"/>
+    <hyperlink ref="C165" r:id="rId188" xr:uid="{23D88EB1-54FB-5241-B58D-8DF71DA770BD}"/>
+    <hyperlink ref="C166" r:id="rId189" xr:uid="{FCEB0F17-6CED-E248-80B6-327E6AB92FA6}"/>
+    <hyperlink ref="C156" r:id="rId190" xr:uid="{0DF5FC7F-490C-7441-A762-E8B3E49758A0}"/>
+    <hyperlink ref="C167" r:id="rId191" xr:uid="{659782CC-853B-8944-B7EA-9CF7FC65A9C9}"/>
+    <hyperlink ref="C155" r:id="rId192" xr:uid="{9E1D2DC2-5A45-7D44-95AF-765ACB09C728}"/>
+    <hyperlink ref="C159" r:id="rId193" xr:uid="{534A3538-6476-C049-B1F4-C7F42A4A0CE2}"/>
+    <hyperlink ref="C160" r:id="rId194" xr:uid="{AD37C4EC-6AA6-7445-886F-F12B10EC4962}"/>
+    <hyperlink ref="C150" r:id="rId195" xr:uid="{32D673E8-4729-054A-941B-0538347DFE6B}"/>
+    <hyperlink ref="C194" r:id="rId196" display="AppConfig" xr:uid="{D7D5BCB4-B018-9449-8DE4-7BAC0B834A94}"/>
+    <hyperlink ref="C206" r:id="rId197" xr:uid="{6C997D60-3DAC-C54C-A365-6925F32D808B}"/>
+    <hyperlink ref="C195" r:id="rId198" xr:uid="{704C5761-85F7-8840-90D5-B9C68A5711E5}"/>
+    <hyperlink ref="C198" r:id="rId199" xr:uid="{0AE4E9A5-C51C-054C-8C1C-DFC93B7DE436}"/>
+    <hyperlink ref="C196" r:id="rId200" xr:uid="{D396B2A5-863A-0A4F-886E-AC0425111A74}"/>
+    <hyperlink ref="C204" r:id="rId201" xr:uid="{154E52D7-25A2-7B48-861E-130AEFF52429}"/>
+    <hyperlink ref="C202" r:id="rId202" xr:uid="{B55B16FC-FF18-784A-A974-098400EB5613}"/>
+    <hyperlink ref="C199" r:id="rId203" xr:uid="{2E1084D5-EB92-104E-9B36-C1C783851CEE}"/>
+    <hyperlink ref="C203" r:id="rId204" xr:uid="{CE1FE151-6237-2B48-BAA5-A0485476B07E}"/>
+    <hyperlink ref="C208" r:id="rId205" xr:uid="{8B651CA8-4121-954F-A1FD-E2ABDAE2711A}"/>
+    <hyperlink ref="C209" r:id="rId206" xr:uid="{73E53697-EA4F-5D44-BABF-E4DDE08A2949}"/>
+    <hyperlink ref="C210" r:id="rId207" xr:uid="{1F5BA02E-7700-F84C-896F-C3320A138F8C}"/>
+    <hyperlink ref="C207" r:id="rId208" xr:uid="{965DAB0C-1533-9C43-9931-A81FDFEE4801}"/>
+    <hyperlink ref="C200" r:id="rId209" xr:uid="{D7F493BC-3996-E14D-8B4E-AF698AF15CF3}"/>
+    <hyperlink ref="C205" r:id="rId210" xr:uid="{158C22B5-B282-0E45-819B-E1F6D3588EB5}"/>
+    <hyperlink ref="C201" r:id="rId211" xr:uid="{060EF427-1526-CB41-B8B7-D967487671FE}"/>
+    <hyperlink ref="C303" r:id="rId212" display="S3 Glacier" xr:uid="{69E65928-2461-9D41-874A-E2DD597C93F4}"/>
+    <hyperlink ref="C161" r:id="rId213" xr:uid="{985BD89A-8A6D-3646-8654-90328345A506}"/>
     <hyperlink ref="C139" r:id="rId214" xr:uid="{590CE714-967E-A245-B8FF-739BCA3B026A}"/>
     <hyperlink ref="C140" r:id="rId215" xr:uid="{1D9605EA-560D-C04A-9C84-34D242F7CD14}"/>
     <hyperlink ref="C141" r:id="rId216" xr:uid="{16002AA9-2EA1-E344-8204-E762411450D2}"/>
     <hyperlink ref="C142" r:id="rId217" xr:uid="{A4BCE370-7F9E-AD48-8C7A-1D6984474130}"/>
-    <hyperlink ref="C238" r:id="rId218" xr:uid="{8AB16A6A-B47A-404E-B8D0-B5341D99BBA0}"/>
+    <hyperlink ref="C240" r:id="rId218" xr:uid="{8AB16A6A-B47A-404E-B8D0-B5341D99BBA0}"/>
     <hyperlink ref="C38" r:id="rId219" xr:uid="{B76C300C-E4E2-7849-9BD6-6C37B6A3A3E9}"/>
     <hyperlink ref="C41" r:id="rId220" xr:uid="{94ED9A38-CC0B-6547-A3F8-0E1E5184307C}"/>
     <hyperlink ref="C42" r:id="rId221" xr:uid="{484C0088-17D4-5E46-9E7E-4B7D0CADC15E}"/>
     <hyperlink ref="C43" r:id="rId222" xr:uid="{AD3D4FE9-D4D4-D34A-8BFC-469E359937BD}"/>
-    <hyperlink ref="C267" r:id="rId223" xr:uid="{1A1FF780-D417-4E48-8B89-324891ACD5EB}"/>
-    <hyperlink ref="C242" r:id="rId224" xr:uid="{A55A32E4-E04D-3D4E-B771-FF5015CDE5FC}"/>
-    <hyperlink ref="C243" r:id="rId225" xr:uid="{470F8C84-D502-374E-8550-CF45C7EE93CD}"/>
+    <hyperlink ref="C269" r:id="rId223" xr:uid="{1A1FF780-D417-4E48-8B89-324891ACD5EB}"/>
+    <hyperlink ref="C244" r:id="rId224" xr:uid="{A55A32E4-E04D-3D4E-B771-FF5015CDE5FC}"/>
+    <hyperlink ref="C245" r:id="rId225" xr:uid="{470F8C84-D502-374E-8550-CF45C7EE93CD}"/>
     <hyperlink ref="C68" r:id="rId226" xr:uid="{14B6B46E-839F-BF4A-B271-B234D8C79A65}"/>
     <hyperlink ref="C69" r:id="rId227" xr:uid="{831473DF-5435-A34B-AD2F-B228DE3531C9}"/>
     <hyperlink ref="C70" r:id="rId228" location="/" xr:uid="{E971A21E-CC8D-5648-B51E-E10B69902AA4}"/>
@@ -11099,13 +11199,13 @@
     <hyperlink ref="C134" r:id="rId231" xr:uid="{40FD60AC-B589-0B4B-AB36-1989E529CD39}"/>
     <hyperlink ref="C135" r:id="rId232" xr:uid="{56F27AA2-5183-E94B-ACC4-73885A21F096}"/>
     <hyperlink ref="C63" r:id="rId233" display="Managed Service for Prometheus" xr:uid="{15FBF981-0EC3-6343-ACAF-575D9CF01C72}"/>
-    <hyperlink ref="C278" r:id="rId234" display="Directory Service AD Connector" xr:uid="{CE8FDA92-983D-F241-9A3C-214FB6ED4987}"/>
-    <hyperlink ref="C280" r:id="rId235" display="Directory Service Simple AD" xr:uid="{BDF803C1-C55F-7B4E-B548-FB056C33B7F8}"/>
-    <hyperlink ref="C279" r:id="rId236" display="Directory Service Managed Microsoft AD" xr:uid="{A2682350-698B-164E-854C-B72B425BF114}"/>
-    <hyperlink ref="C185" r:id="rId237" xr:uid="{51AE8255-80F9-1246-AF04-CAD49D7BD8ED}"/>
+    <hyperlink ref="C280" r:id="rId234" display="Directory Service AD Connector" xr:uid="{CE8FDA92-983D-F241-9A3C-214FB6ED4987}"/>
+    <hyperlink ref="C282" r:id="rId235" display="Directory Service Simple AD" xr:uid="{BDF803C1-C55F-7B4E-B548-FB056C33B7F8}"/>
+    <hyperlink ref="C281" r:id="rId236" display="Directory Service Managed Microsoft AD" xr:uid="{A2682350-698B-164E-854C-B72B425BF114}"/>
+    <hyperlink ref="C186" r:id="rId237" xr:uid="{51AE8255-80F9-1246-AF04-CAD49D7BD8ED}"/>
     <hyperlink ref="C112" r:id="rId238" xr:uid="{F72E5D13-7F9C-A74A-B15B-60DA5CBC35BF}"/>
     <hyperlink ref="C147" r:id="rId239" xr:uid="{A021BA43-B246-CF41-8A4E-1E391CD06D94}"/>
-    <hyperlink ref="C241" r:id="rId240" xr:uid="{66C98670-091A-A841-9473-A308D3D03C92}"/>
+    <hyperlink ref="C243" r:id="rId240" xr:uid="{66C98670-091A-A841-9473-A308D3D03C92}"/>
     <hyperlink ref="C92" r:id="rId241" xr:uid="{A18DAD6F-3F0D-2F41-8ECF-C20C2E59C987}"/>
     <hyperlink ref="C74" r:id="rId242" xr:uid="{BB9AA509-E09D-604B-9392-FAF5D5E1155F}"/>
     <hyperlink ref="C76" r:id="rId243" xr:uid="{2260673B-2C63-EA41-A726-76787E04ADC6}"/>
@@ -11116,33 +11216,33 @@
     <hyperlink ref="C8" r:id="rId248" xr:uid="{F4DFDDD1-B34C-4B4D-BCC8-3F72037E5C85}"/>
     <hyperlink ref="C13" r:id="rId249" xr:uid="{83DFEBC3-E8B1-A840-9964-33EB0A44BF40}"/>
     <hyperlink ref="C11" r:id="rId250" xr:uid="{27A3B616-FD7B-514A-B8BE-D948ED83FC6A}"/>
-    <hyperlink ref="C227" r:id="rId251" xr:uid="{134B5D93-8F9E-1A42-8A9E-4E0085135FD2}"/>
-    <hyperlink ref="C222" r:id="rId252" xr:uid="{705303B4-CB6D-D341-99C3-B418AED6111E}"/>
-    <hyperlink ref="C223" r:id="rId253" xr:uid="{929D3CEF-2347-054E-AAB9-97BA63678E88}"/>
-    <hyperlink ref="C221" r:id="rId254" xr:uid="{18DFC23B-D8CF-664F-A27D-285F1D736B19}"/>
-    <hyperlink ref="C214" r:id="rId255" xr:uid="{51486E41-53D6-7944-B9CA-AE136AD869CF}"/>
-    <hyperlink ref="C215" r:id="rId256" xr:uid="{54539032-2AD1-AF48-A0D7-EA1CBAAE68E7}"/>
-    <hyperlink ref="C217" r:id="rId257" xr:uid="{D9B0B2CA-86A7-954B-B0BE-2A10B768C199}"/>
-    <hyperlink ref="C224" r:id="rId258" xr:uid="{D3E6FCB5-DDCB-CC4A-8B97-DAF02EFEBAC2}"/>
-    <hyperlink ref="C213" r:id="rId259" xr:uid="{4C08CBB6-3E9B-524D-A92A-28DF7EBE8F6E}"/>
-    <hyperlink ref="C225" r:id="rId260" xr:uid="{46CEB576-1991-6A4C-9819-8C32AAD5A3F1}"/>
-    <hyperlink ref="C216" r:id="rId261" xr:uid="{98567FEC-ACF3-D64E-8831-23F0AF44FDF4}"/>
+    <hyperlink ref="C229" r:id="rId251" xr:uid="{134B5D93-8F9E-1A42-8A9E-4E0085135FD2}"/>
+    <hyperlink ref="C224" r:id="rId252" xr:uid="{705303B4-CB6D-D341-99C3-B418AED6111E}"/>
+    <hyperlink ref="C225" r:id="rId253" xr:uid="{929D3CEF-2347-054E-AAB9-97BA63678E88}"/>
+    <hyperlink ref="C223" r:id="rId254" xr:uid="{18DFC23B-D8CF-664F-A27D-285F1D736B19}"/>
+    <hyperlink ref="C216" r:id="rId255" xr:uid="{51486E41-53D6-7944-B9CA-AE136AD869CF}"/>
+    <hyperlink ref="C217" r:id="rId256" xr:uid="{54539032-2AD1-AF48-A0D7-EA1CBAAE68E7}"/>
+    <hyperlink ref="C219" r:id="rId257" xr:uid="{D9B0B2CA-86A7-954B-B0BE-2A10B768C199}"/>
+    <hyperlink ref="C226" r:id="rId258" xr:uid="{D3E6FCB5-DDCB-CC4A-8B97-DAF02EFEBAC2}"/>
+    <hyperlink ref="C215" r:id="rId259" xr:uid="{4C08CBB6-3E9B-524D-A92A-28DF7EBE8F6E}"/>
+    <hyperlink ref="C227" r:id="rId260" xr:uid="{46CEB576-1991-6A4C-9819-8C32AAD5A3F1}"/>
+    <hyperlink ref="C218" r:id="rId261" xr:uid="{98567FEC-ACF3-D64E-8831-23F0AF44FDF4}"/>
     <hyperlink ref="C115" r:id="rId262" xr:uid="{CBE97B7F-03A3-3B47-A836-0FDA32E32458}"/>
-    <hyperlink ref="C182" r:id="rId263" xr:uid="{98ADDE2A-ABDD-EB4A-8EBE-C43795A8F20B}"/>
+    <hyperlink ref="C183" r:id="rId263" xr:uid="{98ADDE2A-ABDD-EB4A-8EBE-C43795A8F20B}"/>
     <hyperlink ref="C55" r:id="rId264" xr:uid="{FE878825-B0CA-394C-95F4-6879C16270CC}"/>
-    <hyperlink ref="C234" r:id="rId265" xr:uid="{8AF37CA7-BEF8-0E46-AFB3-906542482AD8}"/>
+    <hyperlink ref="C236" r:id="rId265" xr:uid="{8AF37CA7-BEF8-0E46-AFB3-906542482AD8}"/>
     <hyperlink ref="C57" r:id="rId266" xr:uid="{E1C253C0-789F-454D-B650-AD9042907E63}"/>
-    <hyperlink ref="C228" r:id="rId267" xr:uid="{9D564718-2FE7-3448-AD3C-AAF79FF31E5C}"/>
-    <hyperlink ref="C230" r:id="rId268" xr:uid="{A196A362-95A2-B841-8B36-8DB86E6BB01F}"/>
-    <hyperlink ref="C229" r:id="rId269" xr:uid="{7D48E632-B0D9-FA4A-87EB-84A674C74042}"/>
-    <hyperlink ref="C231" r:id="rId270" xr:uid="{3B6EA2BE-9E87-CD43-BD86-90EF411A17C9}"/>
-    <hyperlink ref="C232" r:id="rId271" xr:uid="{BE5AE3F2-6AF4-FB45-A4C7-58EE1FA83493}"/>
-    <hyperlink ref="C233" r:id="rId272" xr:uid="{9F9A6701-301A-8946-8181-9D1074CEB3F6}"/>
-    <hyperlink ref="C308" r:id="rId273" display="Storage Gateway - Volume Gateway" xr:uid="{D2EC8952-5BC9-2B49-B394-D7BE012603FF}"/>
-    <hyperlink ref="C306" r:id="rId274" xr:uid="{1B5D263F-5321-B54A-BF60-2932447DCE26}"/>
-    <hyperlink ref="C304" r:id="rId275" display="Storage Gateway - FSx File Gateway" xr:uid="{2125FCAA-C46E-224B-8BE0-19D32D161491}"/>
-    <hyperlink ref="C305" r:id="rId276" display="Storage Gateway - S3 File Gateway" xr:uid="{96B9D02E-E08D-3E44-9C8E-08A2BE24E99A}"/>
-    <hyperlink ref="C307" r:id="rId277" display="Storage Gateway - Volume Gateway" xr:uid="{FFBC4DD5-5D45-9B42-A545-70A2598E87B0}"/>
+    <hyperlink ref="C230" r:id="rId267" xr:uid="{9D564718-2FE7-3448-AD3C-AAF79FF31E5C}"/>
+    <hyperlink ref="C232" r:id="rId268" xr:uid="{A196A362-95A2-B841-8B36-8DB86E6BB01F}"/>
+    <hyperlink ref="C231" r:id="rId269" xr:uid="{7D48E632-B0D9-FA4A-87EB-84A674C74042}"/>
+    <hyperlink ref="C233" r:id="rId270" xr:uid="{3B6EA2BE-9E87-CD43-BD86-90EF411A17C9}"/>
+    <hyperlink ref="C234" r:id="rId271" xr:uid="{BE5AE3F2-6AF4-FB45-A4C7-58EE1FA83493}"/>
+    <hyperlink ref="C235" r:id="rId272" xr:uid="{9F9A6701-301A-8946-8181-9D1074CEB3F6}"/>
+    <hyperlink ref="C310" r:id="rId273" display="Storage Gateway - Volume Gateway" xr:uid="{D2EC8952-5BC9-2B49-B394-D7BE012603FF}"/>
+    <hyperlink ref="C308" r:id="rId274" xr:uid="{1B5D263F-5321-B54A-BF60-2932447DCE26}"/>
+    <hyperlink ref="C306" r:id="rId275" display="Storage Gateway - FSx File Gateway" xr:uid="{2125FCAA-C46E-224B-8BE0-19D32D161491}"/>
+    <hyperlink ref="C307" r:id="rId276" display="Storage Gateway - S3 File Gateway" xr:uid="{96B9D02E-E08D-3E44-9C8E-08A2BE24E99A}"/>
+    <hyperlink ref="C309" r:id="rId277" display="Storage Gateway - Volume Gateway" xr:uid="{FFBC4DD5-5D45-9B42-A545-70A2598E87B0}"/>
     <hyperlink ref="C24" r:id="rId278" xr:uid="{F8A9F9A7-CC98-EC42-8596-0253E0A2BB97}"/>
     <hyperlink ref="C23" r:id="rId279" xr:uid="{8B655CFD-0968-7140-84E8-2070B49F002B}"/>
     <hyperlink ref="C27" r:id="rId280" xr:uid="{FD22D76A-0562-0640-85D0-C48AA580C483}"/>
@@ -11151,21 +11251,21 @@
     <hyperlink ref="C66" r:id="rId283" xr:uid="{1CA75B5D-40F7-EE46-91F1-45EA22AB9C53}"/>
     <hyperlink ref="C118" r:id="rId284" xr:uid="{5961D4D9-3072-2149-961B-0C10629539E7}"/>
     <hyperlink ref="C89" r:id="rId285" xr:uid="{863934C0-971A-AF48-A43D-B4B914AECC39}"/>
-    <hyperlink ref="C181" r:id="rId286" xr:uid="{3295CEB8-10D1-5A43-BEA9-DF5FD886C0AB}"/>
-    <hyperlink ref="C293" r:id="rId287" xr:uid="{4F9FE344-D5EC-AC40-97FF-2F5F45F27D96}"/>
-    <hyperlink ref="C196" r:id="rId288" xr:uid="{AEDB8326-231C-C744-8B10-AF02B678D9B4}"/>
+    <hyperlink ref="C182" r:id="rId286" xr:uid="{3295CEB8-10D1-5A43-BEA9-DF5FD886C0AB}"/>
+    <hyperlink ref="C295" r:id="rId287" xr:uid="{4F9FE344-D5EC-AC40-97FF-2F5F45F27D96}"/>
+    <hyperlink ref="C197" r:id="rId288" xr:uid="{AEDB8326-231C-C744-8B10-AF02B678D9B4}"/>
     <hyperlink ref="C14" r:id="rId289" xr:uid="{2E249962-989F-944F-B761-2BAA0EC7CAEC}"/>
-    <hyperlink ref="C171" r:id="rId290" xr:uid="{DCE5737A-9A5B-DC4D-850F-450E2D238525}"/>
+    <hyperlink ref="C172" r:id="rId290" xr:uid="{DCE5737A-9A5B-DC4D-850F-450E2D238525}"/>
     <hyperlink ref="C46" r:id="rId291" xr:uid="{FE31CE04-AE8C-B545-B85E-3E35079AA70A}"/>
-    <hyperlink ref="C253" r:id="rId292" xr:uid="{D321FD11-72A4-9F4D-857D-939FF8BB6E1B}"/>
-    <hyperlink ref="C262" r:id="rId293" xr:uid="{E997CB7A-902E-064D-B6FF-8470A806D5A0}"/>
-    <hyperlink ref="C265" r:id="rId294" xr:uid="{0A132D4A-E971-7246-889D-EB0D9E3ED74A}"/>
-    <hyperlink ref="C283" r:id="rId295" xr:uid="{5D89926F-F8DE-F748-ADBE-85B87EFE8273}"/>
+    <hyperlink ref="C255" r:id="rId292" xr:uid="{D321FD11-72A4-9F4D-857D-939FF8BB6E1B}"/>
+    <hyperlink ref="C264" r:id="rId293" xr:uid="{E997CB7A-902E-064D-B6FF-8470A806D5A0}"/>
+    <hyperlink ref="C267" r:id="rId294" xr:uid="{0A132D4A-E971-7246-889D-EB0D9E3ED74A}"/>
+    <hyperlink ref="C285" r:id="rId295" xr:uid="{5D89926F-F8DE-F748-ADBE-85B87EFE8273}"/>
     <hyperlink ref="C130" r:id="rId296" xr:uid="{2B14DC1E-31E9-E643-8322-E37BB77A61F2}"/>
-    <hyperlink ref="C244" r:id="rId297" xr:uid="{09886B01-263E-164A-BB8E-628947483324}"/>
-    <hyperlink ref="C245" r:id="rId298" xr:uid="{5F2F3CFC-7F4A-FD4D-941C-DED03BD1B5FC}"/>
-    <hyperlink ref="C236" r:id="rId299" xr:uid="{7C8F3176-C207-894A-B174-4BEF8A9DAF7C}"/>
-    <hyperlink ref="C179" r:id="rId300" xr:uid="{E43F582E-778D-E840-BF2A-38A6E4E85D0B}"/>
+    <hyperlink ref="C246" r:id="rId297" xr:uid="{09886B01-263E-164A-BB8E-628947483324}"/>
+    <hyperlink ref="C247" r:id="rId298" xr:uid="{5F2F3CFC-7F4A-FD4D-941C-DED03BD1B5FC}"/>
+    <hyperlink ref="C237" r:id="rId299" xr:uid="{7C8F3176-C207-894A-B174-4BEF8A9DAF7C}"/>
+    <hyperlink ref="C180" r:id="rId300" xr:uid="{E43F582E-778D-E840-BF2A-38A6E4E85D0B}"/>
     <hyperlink ref="C98:C99" r:id="rId301" display="Cloud Development Kit (CDK)" xr:uid="{74EF9526-5AAF-4446-8604-03C2DD1F15BF}"/>
     <hyperlink ref="C98" r:id="rId302" xr:uid="{C3C5B093-C1E6-354A-B80D-C83A330D70CE}"/>
     <hyperlink ref="C99" r:id="rId303" xr:uid="{3EF40231-9DF0-E848-9274-0E658AE48B9A}"/>
@@ -11173,6 +11273,8 @@
     <hyperlink ref="C85" r:id="rId305" xr:uid="{A7DADC96-9A99-1546-BEF8-93711E890D49}"/>
     <hyperlink ref="C96" r:id="rId306" xr:uid="{C4F45C7A-5C31-D248-96FB-33A8F7D021E1}"/>
     <hyperlink ref="C6" r:id="rId307" xr:uid="{2E031E8F-871D-C04B-954C-80D85FE644BE}"/>
+    <hyperlink ref="C148" r:id="rId308" xr:uid="{24692CE4-8A78-3C4D-8C8A-5B3D1B6F36AA}"/>
+    <hyperlink ref="C214" r:id="rId309" xr:uid="{B6E1487F-81B1-384D-A9E3-DFD2ED50BF4B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11183,7 +11285,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
sec specialty official list
</commit_message>
<xml_diff>
--- a/aws-services-crib-sheet.xlsx
+++ b/aws-services-crib-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corbuno/WorkDocs/courses/aws-services-crib-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDD1C6CA-F63A-D645-8B07-0ADD752AE860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EEEC7A-58AF-2B43-BD66-05B521199103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="500" windowWidth="27780" windowHeight="17500" xr2:uid="{8DC9DE24-CECC-4748-B90E-52259685D84E}"/>
   </bookViews>
@@ -1855,9 +1855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00D01EA-5C3E-F64B-8B7F-2EE6141A689A}">
   <dimension ref="A1:Q310"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="M96" sqref="M96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2906,9 +2906,7 @@
       <c r="L33" s="17">
         <v>1</v>
       </c>
-      <c r="M33" s="17">
-        <v>1</v>
-      </c>
+      <c r="M33" s="17"/>
       <c r="N33" s="17">
         <v>1</v>
       </c>
@@ -2953,9 +2951,7 @@
       <c r="L34" s="17">
         <v>1</v>
       </c>
-      <c r="M34" s="17">
-        <v>1</v>
-      </c>
+      <c r="M34" s="17"/>
       <c r="N34" s="17">
         <v>1</v>
       </c>
@@ -3213,10 +3209,10 @@
         <v>24</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>11</v>
+        <v>136</v>
       </c>
       <c r="D44" s="45"/>
       <c r="E44" s="45"/>
@@ -3227,29 +3223,43 @@
       <c r="H44" s="17">
         <v>1</v>
       </c>
-      <c r="I44" s="17"/>
-      <c r="J44" s="17"/>
+      <c r="I44" s="17">
+        <v>1</v>
+      </c>
+      <c r="J44" s="17">
+        <v>1</v>
+      </c>
       <c r="K44" s="17">
         <v>1</v>
       </c>
-      <c r="L44" s="17"/>
-      <c r="M44" s="17"/>
-      <c r="N44" s="17"/>
+      <c r="L44" s="17">
+        <v>1</v>
+      </c>
+      <c r="M44" s="17">
+        <v>1</v>
+      </c>
+      <c r="N44" s="17">
+        <v>1</v>
+      </c>
       <c r="O44" s="17">
         <v>1</v>
       </c>
-      <c r="P44" s="17"/>
-      <c r="Q44" s="17"/>
+      <c r="P44" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>176</v>
+        <v>11</v>
       </c>
       <c r="D45" s="45"/>
       <c r="E45" s="45"/>
@@ -3260,33 +3270,19 @@
       <c r="H45" s="17">
         <v>1</v>
       </c>
-      <c r="I45" s="17">
-        <v>1</v>
-      </c>
-      <c r="J45" s="17">
-        <v>1</v>
-      </c>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
       <c r="K45" s="17">
         <v>1</v>
       </c>
-      <c r="L45" s="17">
-        <v>1</v>
-      </c>
-      <c r="M45" s="17">
-        <v>1</v>
-      </c>
-      <c r="N45" s="17">
-        <v>1</v>
-      </c>
+      <c r="L45" s="17"/>
+      <c r="M45" s="17"/>
+      <c r="N45" s="17"/>
       <c r="O45" s="17">
         <v>1</v>
       </c>
-      <c r="P45" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q45" s="17">
-        <v>1</v>
-      </c>
+      <c r="P45" s="17"/>
+      <c r="Q45" s="17"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="14" t="s">
@@ -3296,51 +3292,63 @@
         <v>51</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>335</v>
+        <v>176</v>
       </c>
       <c r="D46" s="45"/>
       <c r="E46" s="45"/>
       <c r="F46" s="45"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
+      <c r="G46" s="17">
+        <v>1</v>
+      </c>
+      <c r="H46" s="17">
+        <v>1</v>
+      </c>
+      <c r="I46" s="17">
+        <v>1</v>
+      </c>
       <c r="J46" s="17">
         <v>1</v>
       </c>
-      <c r="K46" s="17"/>
-      <c r="L46" s="17"/>
+      <c r="K46" s="17">
+        <v>1</v>
+      </c>
+      <c r="L46" s="17">
+        <v>1</v>
+      </c>
       <c r="M46" s="17"/>
-      <c r="N46" s="17"/>
-      <c r="O46" s="17"/>
-      <c r="P46" s="17"/>
-      <c r="Q46" s="17"/>
+      <c r="N46" s="17">
+        <v>1</v>
+      </c>
+      <c r="O46" s="17">
+        <v>1</v>
+      </c>
+      <c r="P46" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>95</v>
+        <v>335</v>
       </c>
       <c r="D47" s="45"/>
       <c r="E47" s="45"/>
       <c r="F47" s="45"/>
-      <c r="G47" s="17">
-        <v>1</v>
-      </c>
-      <c r="H47" s="17">
-        <v>1</v>
-      </c>
-      <c r="I47" s="17">
-        <v>1</v>
-      </c>
-      <c r="J47" s="17"/>
-      <c r="K47" s="17">
-        <v>1</v>
-      </c>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17">
+        <v>1</v>
+      </c>
+      <c r="K47" s="17"/>
       <c r="L47" s="17"/>
       <c r="M47" s="17"/>
       <c r="N47" s="17"/>
@@ -3353,10 +3361,10 @@
         <v>24</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>136</v>
+        <v>95</v>
       </c>
       <c r="D48" s="45"/>
       <c r="E48" s="45"/>
@@ -3370,30 +3378,16 @@
       <c r="I48" s="17">
         <v>1</v>
       </c>
-      <c r="J48" s="17">
-        <v>1</v>
-      </c>
+      <c r="J48" s="17"/>
       <c r="K48" s="17">
         <v>1</v>
       </c>
-      <c r="L48" s="17">
-        <v>1</v>
-      </c>
-      <c r="M48" s="17">
-        <v>1</v>
-      </c>
-      <c r="N48" s="17">
-        <v>1</v>
-      </c>
-      <c r="O48" s="17">
-        <v>1</v>
-      </c>
-      <c r="P48" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q48" s="17">
-        <v>1</v>
-      </c>
+      <c r="L48" s="17"/>
+      <c r="M48" s="17"/>
+      <c r="N48" s="17"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="17"/>
+      <c r="Q48" s="17"/>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
@@ -3426,9 +3420,7 @@
       <c r="L49" s="17">
         <v>1</v>
       </c>
-      <c r="M49" s="17">
-        <v>1</v>
-      </c>
+      <c r="M49" s="17"/>
       <c r="N49" s="17">
         <v>1</v>
       </c>
@@ -4419,9 +4411,7 @@
       <c r="L84" s="17">
         <v>1</v>
       </c>
-      <c r="M84" s="17">
-        <v>1</v>
-      </c>
+      <c r="M84" s="17"/>
       <c r="N84" s="17">
         <v>1</v>
       </c>
@@ -6909,7 +6899,7 @@
         <v>6</v>
       </c>
       <c r="C175" s="31" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D175" s="45"/>
       <c r="E175" s="45"/>
@@ -6935,18 +6925,12 @@
       <c r="M175" s="17">
         <v>1</v>
       </c>
-      <c r="N175" s="17">
-        <v>1</v>
-      </c>
+      <c r="N175" s="17"/>
       <c r="O175" s="17">
         <v>1</v>
       </c>
-      <c r="P175" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q175" s="17">
-        <v>1</v>
-      </c>
+      <c r="P175" s="17"/>
+      <c r="Q175" s="17"/>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A176" s="29" t="s">
@@ -6956,7 +6940,7 @@
         <v>6</v>
       </c>
       <c r="C176" s="31" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D176" s="45"/>
       <c r="E176" s="45"/>
@@ -6979,15 +6963,19 @@
       <c r="L176" s="17">
         <v>1</v>
       </c>
-      <c r="M176" s="17">
-        <v>1</v>
-      </c>
-      <c r="N176" s="17"/>
+      <c r="M176" s="17"/>
+      <c r="N176" s="17">
+        <v>1</v>
+      </c>
       <c r="O176" s="17">
         <v>1</v>
       </c>
-      <c r="P176" s="17"/>
-      <c r="Q176" s="17"/>
+      <c r="P176" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q176" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="177" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A177" s="29" t="s">
@@ -7044,20 +7032,30 @@
         <v>6</v>
       </c>
       <c r="C178" s="31" t="s">
-        <v>90</v>
+        <v>25</v>
       </c>
       <c r="D178" s="45"/>
       <c r="E178" s="45"/>
       <c r="F178" s="45"/>
-      <c r="G178" s="17"/>
-      <c r="H178" s="17"/>
+      <c r="G178" s="17">
+        <v>1</v>
+      </c>
+      <c r="H178" s="17">
+        <v>1</v>
+      </c>
       <c r="I178" s="17"/>
       <c r="J178" s="17">
         <v>1</v>
       </c>
-      <c r="K178" s="17"/>
-      <c r="L178" s="17"/>
-      <c r="M178" s="17"/>
+      <c r="K178" s="17">
+        <v>1</v>
+      </c>
+      <c r="L178" s="17">
+        <v>1</v>
+      </c>
+      <c r="M178" s="17">
+        <v>1</v>
+      </c>
       <c r="N178" s="17"/>
       <c r="O178" s="17"/>
       <c r="P178" s="17"/>
@@ -7071,7 +7069,7 @@
         <v>6</v>
       </c>
       <c r="C179" s="31" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="D179" s="45"/>
       <c r="E179" s="45"/>
@@ -7092,7 +7090,9 @@
       <c r="L179" s="17">
         <v>1</v>
       </c>
-      <c r="M179" s="17"/>
+      <c r="M179" s="17">
+        <v>1</v>
+      </c>
       <c r="N179" s="17"/>
       <c r="O179" s="17"/>
       <c r="P179" s="17"/>
@@ -7106,7 +7106,7 @@
         <v>6</v>
       </c>
       <c r="C180" s="31" t="s">
-        <v>344</v>
+        <v>90</v>
       </c>
       <c r="D180" s="45"/>
       <c r="E180" s="45"/>
@@ -7114,7 +7114,9 @@
       <c r="G180" s="17"/>
       <c r="H180" s="17"/>
       <c r="I180" s="17"/>
-      <c r="J180" s="17"/>
+      <c r="J180" s="17">
+        <v>1</v>
+      </c>
       <c r="K180" s="17"/>
       <c r="L180" s="17"/>
       <c r="M180" s="17"/>
@@ -7131,13 +7133,17 @@
         <v>6</v>
       </c>
       <c r="C181" s="31" t="s">
-        <v>91</v>
+        <v>252</v>
       </c>
       <c r="D181" s="45"/>
       <c r="E181" s="45"/>
       <c r="F181" s="45"/>
-      <c r="G181" s="17"/>
-      <c r="H181" s="17"/>
+      <c r="G181" s="17">
+        <v>1</v>
+      </c>
+      <c r="H181" s="17">
+        <v>1</v>
+      </c>
       <c r="I181" s="17"/>
       <c r="J181" s="17">
         <v>1</v>
@@ -7145,8 +7151,12 @@
       <c r="K181" s="17">
         <v>1</v>
       </c>
-      <c r="L181" s="17"/>
-      <c r="M181" s="17"/>
+      <c r="L181" s="17">
+        <v>1</v>
+      </c>
+      <c r="M181" s="17">
+        <v>1</v>
+      </c>
       <c r="N181" s="17"/>
       <c r="O181" s="17"/>
       <c r="P181" s="17"/>
@@ -7157,10 +7167,10 @@
         <v>33</v>
       </c>
       <c r="B182" s="30" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C182" s="31" t="s">
-        <v>329</v>
+        <v>344</v>
       </c>
       <c r="D182" s="45"/>
       <c r="E182" s="45"/>
@@ -7185,7 +7195,7 @@
         <v>6</v>
       </c>
       <c r="C183" s="31" t="s">
-        <v>302</v>
+        <v>91</v>
       </c>
       <c r="D183" s="45"/>
       <c r="E183" s="45"/>
@@ -7193,8 +7203,12 @@
       <c r="G183" s="17"/>
       <c r="H183" s="17"/>
       <c r="I183" s="17"/>
-      <c r="J183" s="17"/>
-      <c r="K183" s="17"/>
+      <c r="J183" s="17">
+        <v>1</v>
+      </c>
+      <c r="K183" s="17">
+        <v>1</v>
+      </c>
       <c r="L183" s="17"/>
       <c r="M183" s="17"/>
       <c r="N183" s="17"/>
@@ -7207,25 +7221,19 @@
         <v>33</v>
       </c>
       <c r="B184" s="30" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C184" s="31" t="s">
-        <v>111</v>
+        <v>329</v>
       </c>
       <c r="D184" s="45"/>
       <c r="E184" s="45"/>
       <c r="F184" s="45"/>
-      <c r="G184" s="17">
-        <v>1</v>
-      </c>
+      <c r="G184" s="17"/>
       <c r="H184" s="17"/>
       <c r="I184" s="17"/>
-      <c r="J184" s="17">
-        <v>1</v>
-      </c>
-      <c r="K184" s="17">
-        <v>1</v>
-      </c>
+      <c r="J184" s="17"/>
+      <c r="K184" s="17"/>
       <c r="L184" s="17"/>
       <c r="M184" s="17"/>
       <c r="N184" s="17"/>
@@ -7238,10 +7246,10 @@
         <v>33</v>
       </c>
       <c r="B185" s="30" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C185" s="31" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="D185" s="45"/>
       <c r="E185" s="45"/>
@@ -7251,8 +7259,12 @@
       <c r="I185" s="17"/>
       <c r="J185" s="17"/>
       <c r="K185" s="17"/>
-      <c r="L185" s="17"/>
-      <c r="M185" s="17"/>
+      <c r="L185" s="17">
+        <v>1</v>
+      </c>
+      <c r="M185" s="17">
+        <v>1</v>
+      </c>
       <c r="N185" s="17"/>
       <c r="O185" s="17"/>
       <c r="P185" s="17"/>
@@ -7266,7 +7278,7 @@
         <v>6</v>
       </c>
       <c r="C186" s="31" t="s">
-        <v>273</v>
+        <v>246</v>
       </c>
       <c r="D186" s="45"/>
       <c r="E186" s="45"/>
@@ -7274,14 +7286,22 @@
       <c r="G186" s="17">
         <v>1</v>
       </c>
-      <c r="H186" s="17"/>
+      <c r="H186" s="17">
+        <v>1</v>
+      </c>
       <c r="I186" s="17"/>
       <c r="J186" s="17">
         <v>1</v>
       </c>
-      <c r="K186" s="17"/>
-      <c r="L186" s="17"/>
-      <c r="M186" s="17"/>
+      <c r="K186" s="17">
+        <v>1</v>
+      </c>
+      <c r="L186" s="17">
+        <v>1</v>
+      </c>
+      <c r="M186" s="17">
+        <v>1</v>
+      </c>
       <c r="N186" s="17"/>
       <c r="O186" s="17"/>
       <c r="P186" s="17"/>
@@ -7295,12 +7315,14 @@
         <v>6</v>
       </c>
       <c r="C187" s="31" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="D187" s="45"/>
       <c r="E187" s="45"/>
       <c r="F187" s="45"/>
-      <c r="G187" s="17"/>
+      <c r="G187" s="17">
+        <v>1</v>
+      </c>
       <c r="H187" s="17">
         <v>1</v>
       </c>
@@ -7308,14 +7330,20 @@
       <c r="J187" s="17">
         <v>1</v>
       </c>
-      <c r="K187" s="17"/>
+      <c r="K187" s="17">
+        <v>1</v>
+      </c>
       <c r="L187" s="17">
         <v>1</v>
       </c>
-      <c r="M187" s="17"/>
+      <c r="M187" s="17">
+        <v>1</v>
+      </c>
       <c r="N187" s="17"/>
       <c r="O187" s="17"/>
-      <c r="P187" s="17"/>
+      <c r="P187" s="17">
+        <v>1</v>
+      </c>
       <c r="Q187" s="17"/>
     </row>
     <row r="188" spans="1:17" x14ac:dyDescent="0.2">
@@ -7326,23 +7354,17 @@
         <v>6</v>
       </c>
       <c r="C188" s="31" t="s">
-        <v>115</v>
+        <v>302</v>
       </c>
       <c r="D188" s="45"/>
       <c r="E188" s="45"/>
       <c r="F188" s="45"/>
       <c r="G188" s="17"/>
-      <c r="H188" s="17">
-        <v>1</v>
-      </c>
+      <c r="H188" s="17"/>
       <c r="I188" s="17"/>
-      <c r="J188" s="17">
-        <v>1</v>
-      </c>
+      <c r="J188" s="17"/>
       <c r="K188" s="17"/>
-      <c r="L188" s="17">
-        <v>1</v>
-      </c>
+      <c r="L188" s="17"/>
       <c r="M188" s="17"/>
       <c r="N188" s="17"/>
       <c r="O188" s="17"/>
@@ -7357,23 +7379,23 @@
         <v>6</v>
       </c>
       <c r="C189" s="31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D189" s="45"/>
       <c r="E189" s="45"/>
       <c r="F189" s="45"/>
-      <c r="G189" s="17"/>
-      <c r="H189" s="17">
-        <v>1</v>
-      </c>
+      <c r="G189" s="17">
+        <v>1</v>
+      </c>
+      <c r="H189" s="17"/>
       <c r="I189" s="17"/>
       <c r="J189" s="17">
         <v>1</v>
       </c>
-      <c r="K189" s="17"/>
-      <c r="L189" s="17">
-        <v>1</v>
-      </c>
+      <c r="K189" s="17">
+        <v>1</v>
+      </c>
+      <c r="L189" s="17"/>
       <c r="M189" s="17"/>
       <c r="N189" s="17"/>
       <c r="O189" s="17"/>
@@ -7385,30 +7407,20 @@
         <v>33</v>
       </c>
       <c r="B190" s="30" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C190" s="31" t="s">
-        <v>38</v>
+        <v>220</v>
       </c>
       <c r="D190" s="45"/>
       <c r="E190" s="45"/>
       <c r="F190" s="45"/>
-      <c r="G190" s="17">
-        <v>1</v>
-      </c>
-      <c r="H190" s="17">
-        <v>1</v>
-      </c>
+      <c r="G190" s="17"/>
+      <c r="H190" s="17"/>
       <c r="I190" s="17"/>
-      <c r="J190" s="17">
-        <v>1</v>
-      </c>
-      <c r="K190" s="17">
-        <v>1</v>
-      </c>
-      <c r="L190" s="17">
-        <v>1</v>
-      </c>
+      <c r="J190" s="17"/>
+      <c r="K190" s="17"/>
+      <c r="L190" s="17"/>
       <c r="M190" s="17"/>
       <c r="N190" s="17"/>
       <c r="O190" s="17"/>
@@ -7423,7 +7435,7 @@
         <v>6</v>
       </c>
       <c r="C191" s="31" t="s">
-        <v>116</v>
+        <v>273</v>
       </c>
       <c r="D191" s="45"/>
       <c r="E191" s="45"/>
@@ -7452,7 +7464,7 @@
         <v>6</v>
       </c>
       <c r="C192" s="31" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D192" s="45"/>
       <c r="E192" s="45"/>
@@ -7462,11 +7474,13 @@
         <v>1</v>
       </c>
       <c r="I192" s="17"/>
-      <c r="J192" s="17"/>
-      <c r="K192" s="17">
-        <v>1</v>
-      </c>
-      <c r="L192" s="17"/>
+      <c r="J192" s="17">
+        <v>1</v>
+      </c>
+      <c r="K192" s="17"/>
+      <c r="L192" s="17">
+        <v>1</v>
+      </c>
       <c r="M192" s="17"/>
       <c r="N192" s="17"/>
       <c r="O192" s="17"/>
@@ -7481,21 +7495,23 @@
         <v>6</v>
       </c>
       <c r="C193" s="31" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D193" s="45"/>
       <c r="E193" s="45"/>
       <c r="F193" s="45"/>
       <c r="G193" s="17"/>
-      <c r="H193" s="17"/>
+      <c r="H193" s="17">
+        <v>1</v>
+      </c>
       <c r="I193" s="17"/>
       <c r="J193" s="17">
         <v>1</v>
       </c>
-      <c r="K193" s="17">
-        <v>1</v>
-      </c>
-      <c r="L193" s="17"/>
+      <c r="K193" s="17"/>
+      <c r="L193" s="17">
+        <v>1</v>
+      </c>
       <c r="M193" s="17"/>
       <c r="N193" s="17"/>
       <c r="O193" s="17"/>
@@ -7510,13 +7526,15 @@
         <v>6</v>
       </c>
       <c r="C194" s="31" t="s">
-        <v>247</v>
+        <v>113</v>
       </c>
       <c r="D194" s="45"/>
       <c r="E194" s="45"/>
       <c r="F194" s="45"/>
       <c r="G194" s="17"/>
-      <c r="H194" s="17"/>
+      <c r="H194" s="17">
+        <v>1</v>
+      </c>
       <c r="I194" s="17"/>
       <c r="J194" s="17">
         <v>1</v>
@@ -7539,21 +7557,21 @@
         <v>6</v>
       </c>
       <c r="C195" s="31" t="s">
-        <v>251</v>
+        <v>116</v>
       </c>
       <c r="D195" s="45"/>
       <c r="E195" s="45"/>
       <c r="F195" s="45"/>
-      <c r="G195" s="17"/>
+      <c r="G195" s="17">
+        <v>1</v>
+      </c>
       <c r="H195" s="17"/>
       <c r="I195" s="17"/>
       <c r="J195" s="17">
         <v>1</v>
       </c>
       <c r="K195" s="17"/>
-      <c r="L195" s="17">
-        <v>1</v>
-      </c>
+      <c r="L195" s="17"/>
       <c r="M195" s="17"/>
       <c r="N195" s="17"/>
       <c r="O195" s="17"/>
@@ -7568,21 +7586,21 @@
         <v>6</v>
       </c>
       <c r="C196" s="31" t="s">
-        <v>254</v>
+        <v>117</v>
       </c>
       <c r="D196" s="45"/>
       <c r="E196" s="45"/>
       <c r="F196" s="45"/>
       <c r="G196" s="17"/>
-      <c r="H196" s="17"/>
+      <c r="H196" s="17">
+        <v>1</v>
+      </c>
       <c r="I196" s="17"/>
-      <c r="J196" s="17">
-        <v>1</v>
-      </c>
-      <c r="K196" s="17"/>
-      <c r="L196" s="17">
-        <v>1</v>
-      </c>
+      <c r="J196" s="17"/>
+      <c r="K196" s="17">
+        <v>1</v>
+      </c>
+      <c r="L196" s="17"/>
       <c r="M196" s="17"/>
       <c r="N196" s="17"/>
       <c r="O196" s="17"/>
@@ -7597,7 +7615,7 @@
         <v>6</v>
       </c>
       <c r="C197" s="31" t="s">
-        <v>331</v>
+        <v>122</v>
       </c>
       <c r="D197" s="45"/>
       <c r="E197" s="45"/>
@@ -7605,8 +7623,12 @@
       <c r="G197" s="17"/>
       <c r="H197" s="17"/>
       <c r="I197" s="17"/>
-      <c r="J197" s="17"/>
-      <c r="K197" s="17"/>
+      <c r="J197" s="17">
+        <v>1</v>
+      </c>
+      <c r="K197" s="17">
+        <v>1</v>
+      </c>
       <c r="L197" s="17"/>
       <c r="M197" s="17"/>
       <c r="N197" s="17"/>
@@ -7622,7 +7644,7 @@
         <v>6</v>
       </c>
       <c r="C198" s="31" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D198" s="45"/>
       <c r="E198" s="45"/>
@@ -7630,7 +7652,9 @@
       <c r="G198" s="17"/>
       <c r="H198" s="17"/>
       <c r="I198" s="17"/>
-      <c r="J198" s="17"/>
+      <c r="J198" s="17">
+        <v>1</v>
+      </c>
       <c r="K198" s="17"/>
       <c r="L198" s="17">
         <v>1</v>
@@ -7649,7 +7673,7 @@
         <v>6</v>
       </c>
       <c r="C199" s="31" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D199" s="45"/>
       <c r="E199" s="45"/>
@@ -7657,7 +7681,9 @@
       <c r="G199" s="17"/>
       <c r="H199" s="17"/>
       <c r="I199" s="17"/>
-      <c r="J199" s="17"/>
+      <c r="J199" s="17">
+        <v>1</v>
+      </c>
       <c r="K199" s="17"/>
       <c r="L199" s="17">
         <v>1</v>
@@ -7676,7 +7702,7 @@
         <v>6</v>
       </c>
       <c r="C200" s="31" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="D200" s="45"/>
       <c r="E200" s="45"/>
@@ -7684,7 +7710,9 @@
       <c r="G200" s="17"/>
       <c r="H200" s="17"/>
       <c r="I200" s="17"/>
-      <c r="J200" s="17"/>
+      <c r="J200" s="17">
+        <v>1</v>
+      </c>
       <c r="K200" s="17"/>
       <c r="L200" s="17">
         <v>1</v>
@@ -7703,7 +7731,7 @@
         <v>6</v>
       </c>
       <c r="C201" s="31" t="s">
-        <v>249</v>
+        <v>331</v>
       </c>
       <c r="D201" s="45"/>
       <c r="E201" s="45"/>
@@ -7713,9 +7741,7 @@
       <c r="I201" s="17"/>
       <c r="J201" s="17"/>
       <c r="K201" s="17"/>
-      <c r="L201" s="17">
-        <v>1</v>
-      </c>
+      <c r="L201" s="17"/>
       <c r="M201" s="17"/>
       <c r="N201" s="17"/>
       <c r="O201" s="17"/>
@@ -7730,7 +7756,7 @@
         <v>6</v>
       </c>
       <c r="C202" s="31" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D202" s="45"/>
       <c r="E202" s="45"/>
@@ -7757,7 +7783,7 @@
         <v>6</v>
       </c>
       <c r="C203" s="31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D203" s="45"/>
       <c r="E203" s="45"/>
@@ -7784,7 +7810,7 @@
         <v>6</v>
       </c>
       <c r="C204" s="31" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="D204" s="45"/>
       <c r="E204" s="45"/>
@@ -7811,11 +7837,11 @@
         <v>6</v>
       </c>
       <c r="C205" s="31" t="s">
-        <v>250</v>
-      </c>
-      <c r="D205" s="47"/>
-      <c r="E205" s="47"/>
-      <c r="F205" s="47"/>
+        <v>249</v>
+      </c>
+      <c r="D205" s="45"/>
+      <c r="E205" s="45"/>
+      <c r="F205" s="45"/>
       <c r="G205" s="17"/>
       <c r="H205" s="17"/>
       <c r="I205" s="17"/>
@@ -7838,24 +7864,16 @@
         <v>6</v>
       </c>
       <c r="C206" s="31" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="D206" s="45"/>
       <c r="E206" s="45"/>
       <c r="F206" s="45"/>
-      <c r="G206" s="17">
-        <v>1</v>
-      </c>
-      <c r="H206" s="17">
-        <v>1</v>
-      </c>
+      <c r="G206" s="17"/>
+      <c r="H206" s="17"/>
       <c r="I206" s="17"/>
-      <c r="J206" s="17">
-        <v>1</v>
-      </c>
-      <c r="K206" s="17">
-        <v>1</v>
-      </c>
+      <c r="J206" s="17"/>
+      <c r="K206" s="17"/>
       <c r="L206" s="17">
         <v>1</v>
       </c>
@@ -7873,7 +7891,7 @@
         <v>6</v>
       </c>
       <c r="C207" s="31" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D207" s="45"/>
       <c r="E207" s="45"/>
@@ -7900,7 +7918,7 @@
         <v>6</v>
       </c>
       <c r="C208" s="31" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D208" s="45"/>
       <c r="E208" s="45"/>
@@ -7927,11 +7945,11 @@
         <v>6</v>
       </c>
       <c r="C209" s="31" t="s">
-        <v>259</v>
-      </c>
-      <c r="D209" s="45"/>
-      <c r="E209" s="45"/>
-      <c r="F209" s="45"/>
+        <v>250</v>
+      </c>
+      <c r="D209" s="47"/>
+      <c r="E209" s="47"/>
+      <c r="F209" s="47"/>
       <c r="G209" s="17"/>
       <c r="H209" s="17"/>
       <c r="I209" s="17"/>
@@ -7954,7 +7972,7 @@
         <v>6</v>
       </c>
       <c r="C210" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D210" s="45"/>
       <c r="E210" s="45"/>
@@ -7981,24 +7999,16 @@
         <v>6</v>
       </c>
       <c r="C211" s="31" t="s">
-        <v>246</v>
+        <v>259</v>
       </c>
       <c r="D211" s="45"/>
       <c r="E211" s="45"/>
       <c r="F211" s="45"/>
-      <c r="G211" s="17">
-        <v>1</v>
-      </c>
-      <c r="H211" s="17">
-        <v>1</v>
-      </c>
+      <c r="G211" s="17"/>
+      <c r="H211" s="17"/>
       <c r="I211" s="17"/>
-      <c r="J211" s="17">
-        <v>1</v>
-      </c>
-      <c r="K211" s="17">
-        <v>1</v>
-      </c>
+      <c r="J211" s="17"/>
+      <c r="K211" s="17"/>
       <c r="L211" s="17">
         <v>1</v>
       </c>
@@ -8016,33 +8026,23 @@
         <v>6</v>
       </c>
       <c r="C212" s="31" t="s">
-        <v>127</v>
+        <v>261</v>
       </c>
       <c r="D212" s="45"/>
       <c r="E212" s="45"/>
       <c r="F212" s="45"/>
-      <c r="G212" s="17">
-        <v>1</v>
-      </c>
-      <c r="H212" s="17">
-        <v>1</v>
-      </c>
+      <c r="G212" s="17"/>
+      <c r="H212" s="17"/>
       <c r="I212" s="17"/>
-      <c r="J212" s="17">
-        <v>1</v>
-      </c>
-      <c r="K212" s="17">
-        <v>1</v>
-      </c>
+      <c r="J212" s="17"/>
+      <c r="K212" s="17"/>
       <c r="L212" s="17">
         <v>1</v>
       </c>
       <c r="M212" s="17"/>
       <c r="N212" s="17"/>
       <c r="O212" s="17"/>
-      <c r="P212" s="17">
-        <v>1</v>
-      </c>
+      <c r="P212" s="17"/>
       <c r="Q212" s="17"/>
     </row>
     <row r="213" spans="1:17" x14ac:dyDescent="0.2">
@@ -9134,9 +9134,7 @@
       <c r="L253" s="17">
         <v>1</v>
       </c>
-      <c r="M253" s="17">
-        <v>1</v>
-      </c>
+      <c r="M253" s="17"/>
       <c r="N253" s="17">
         <v>1</v>
       </c>
@@ -9260,9 +9258,7 @@
       <c r="L257" s="17">
         <v>1</v>
       </c>
-      <c r="M257" s="17">
-        <v>1</v>
-      </c>
+      <c r="M257" s="17"/>
       <c r="N257" s="17">
         <v>1</v>
       </c>
@@ -9334,9 +9330,7 @@
       <c r="L259" s="17">
         <v>1</v>
       </c>
-      <c r="M259" s="17">
-        <v>1</v>
-      </c>
+      <c r="M259" s="17"/>
       <c r="N259" s="17">
         <v>1</v>
       </c>
@@ -9358,24 +9352,20 @@
         <v>6</v>
       </c>
       <c r="C260" s="35" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="D260" s="45"/>
       <c r="E260" s="45"/>
       <c r="F260" s="45"/>
       <c r="G260" s="17"/>
-      <c r="H260" s="17">
-        <v>1</v>
-      </c>
+      <c r="H260" s="17"/>
       <c r="I260" s="17"/>
-      <c r="J260" s="17">
-        <v>1</v>
-      </c>
-      <c r="K260" s="17">
-        <v>1</v>
-      </c>
+      <c r="J260" s="17"/>
+      <c r="K260" s="17"/>
       <c r="L260" s="17"/>
-      <c r="M260" s="17"/>
+      <c r="M260" s="17">
+        <v>1</v>
+      </c>
       <c r="N260" s="17">
         <v>1</v>
       </c>
@@ -9391,16 +9381,22 @@
         <v>6</v>
       </c>
       <c r="C261" s="35" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D261" s="45"/>
       <c r="E261" s="45"/>
       <c r="F261" s="45"/>
       <c r="G261" s="17"/>
-      <c r="H261" s="17"/>
+      <c r="H261" s="17">
+        <v>1</v>
+      </c>
       <c r="I261" s="17"/>
-      <c r="J261" s="17"/>
-      <c r="K261" s="17"/>
+      <c r="J261" s="17">
+        <v>1</v>
+      </c>
+      <c r="K261" s="17">
+        <v>1</v>
+      </c>
       <c r="L261" s="17"/>
       <c r="M261" s="17"/>
       <c r="N261" s="17">
@@ -9415,59 +9411,69 @@
         <v>169</v>
       </c>
       <c r="B262" s="34" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C262" s="35" t="s">
-        <v>40</v>
+        <v>161</v>
       </c>
       <c r="D262" s="45"/>
       <c r="E262" s="45"/>
       <c r="F262" s="45"/>
-      <c r="G262" s="17"/>
-      <c r="H262" s="17"/>
-      <c r="I262" s="17"/>
-      <c r="J262" s="17"/>
+      <c r="G262" s="17">
+        <v>1</v>
+      </c>
+      <c r="H262" s="17">
+        <v>1</v>
+      </c>
+      <c r="I262" s="17">
+        <v>1</v>
+      </c>
+      <c r="J262" s="17">
+        <v>1</v>
+      </c>
       <c r="K262" s="17">
         <v>1</v>
       </c>
-      <c r="L262" s="17"/>
-      <c r="M262" s="17"/>
+      <c r="L262" s="17">
+        <v>1</v>
+      </c>
+      <c r="M262" s="17">
+        <v>1</v>
+      </c>
       <c r="N262" s="17">
         <v>1</v>
       </c>
-      <c r="O262" s="17"/>
-      <c r="P262" s="17"/>
-      <c r="Q262" s="17"/>
+      <c r="O262" s="17">
+        <v>1</v>
+      </c>
+      <c r="P262" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q262" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="263" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A263" s="33" t="s">
         <v>169</v>
       </c>
       <c r="B263" s="34" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C263" s="35" t="s">
-        <v>154</v>
+        <v>40</v>
       </c>
       <c r="D263" s="45"/>
       <c r="E263" s="45"/>
       <c r="F263" s="45"/>
-      <c r="G263" s="17">
-        <v>1</v>
-      </c>
-      <c r="H263" s="17">
-        <v>1</v>
-      </c>
+      <c r="G263" s="17"/>
+      <c r="H263" s="17"/>
       <c r="I263" s="17"/>
-      <c r="J263" s="17">
-        <v>1</v>
-      </c>
+      <c r="J263" s="17"/>
       <c r="K263" s="17">
         <v>1</v>
       </c>
-      <c r="L263" s="17">
-        <v>1</v>
-      </c>
+      <c r="L263" s="17"/>
       <c r="M263" s="17"/>
       <c r="N263" s="17">
         <v>1</v>
@@ -9481,24 +9487,34 @@
         <v>169</v>
       </c>
       <c r="B264" s="34" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C264" s="35" t="s">
-        <v>337</v>
+        <v>154</v>
       </c>
       <c r="D264" s="45"/>
       <c r="E264" s="45"/>
       <c r="F264" s="45"/>
-      <c r="G264" s="17"/>
-      <c r="H264" s="17"/>
+      <c r="G264" s="17">
+        <v>1</v>
+      </c>
+      <c r="H264" s="17">
+        <v>1</v>
+      </c>
       <c r="I264" s="17"/>
-      <c r="J264" s="17"/>
-      <c r="K264" s="17"/>
+      <c r="J264" s="17">
+        <v>1</v>
+      </c>
+      <c r="K264" s="17">
+        <v>1</v>
+      </c>
       <c r="L264" s="17">
         <v>1</v>
       </c>
       <c r="M264" s="17"/>
-      <c r="N264" s="17"/>
+      <c r="N264" s="17">
+        <v>1</v>
+      </c>
       <c r="O264" s="17"/>
       <c r="P264" s="17"/>
       <c r="Q264" s="17"/>
@@ -9511,29 +9527,21 @@
         <v>6</v>
       </c>
       <c r="C265" s="35" t="s">
-        <v>126</v>
+        <v>337</v>
       </c>
       <c r="D265" s="45"/>
       <c r="E265" s="45"/>
       <c r="F265" s="45"/>
       <c r="G265" s="17"/>
-      <c r="H265" s="17">
-        <v>1</v>
-      </c>
+      <c r="H265" s="17"/>
       <c r="I265" s="17"/>
-      <c r="J265" s="17">
-        <v>1</v>
-      </c>
-      <c r="K265" s="17">
-        <v>1</v>
-      </c>
+      <c r="J265" s="17"/>
+      <c r="K265" s="17"/>
       <c r="L265" s="17">
         <v>1</v>
       </c>
       <c r="M265" s="17"/>
-      <c r="N265" s="17">
-        <v>1</v>
-      </c>
+      <c r="N265" s="17"/>
       <c r="O265" s="17"/>
       <c r="P265" s="17"/>
       <c r="Q265" s="17"/>
@@ -9543,23 +9551,19 @@
         <v>169</v>
       </c>
       <c r="B266" s="34" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C266" s="35" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="D266" s="45"/>
       <c r="E266" s="45"/>
       <c r="F266" s="45"/>
-      <c r="G266" s="17">
-        <v>1</v>
-      </c>
+      <c r="G266" s="17"/>
       <c r="H266" s="17">
         <v>1</v>
       </c>
-      <c r="I266" s="17">
-        <v>1</v>
-      </c>
+      <c r="I266" s="17"/>
       <c r="J266" s="17">
         <v>1</v>
       </c>
@@ -9569,21 +9573,13 @@
       <c r="L266" s="17">
         <v>1</v>
       </c>
-      <c r="M266" s="17">
-        <v>1</v>
-      </c>
+      <c r="M266" s="17"/>
       <c r="N266" s="17">
         <v>1</v>
       </c>
-      <c r="O266" s="17">
-        <v>1</v>
-      </c>
-      <c r="P266" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q266" s="17">
-        <v>1</v>
-      </c>
+      <c r="O266" s="17"/>
+      <c r="P266" s="17"/>
+      <c r="Q266" s="17"/>
     </row>
     <row r="267" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A267" s="33" t="s">
@@ -9743,9 +9739,7 @@
         <v>1</v>
       </c>
       <c r="L272" s="17"/>
-      <c r="M272" s="17">
-        <v>1</v>
-      </c>
+      <c r="M272" s="17"/>
       <c r="N272" s="17"/>
       <c r="O272" s="17"/>
       <c r="P272" s="17">
@@ -9758,10 +9752,10 @@
         <v>43</v>
       </c>
       <c r="B273" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C273" s="39" t="s">
-        <v>87</v>
+        <v>131</v>
       </c>
       <c r="D273" s="45"/>
       <c r="E273" s="45"/>
@@ -9772,9 +9766,7 @@
       <c r="J273" s="17"/>
       <c r="K273" s="17"/>
       <c r="L273" s="17"/>
-      <c r="M273" s="17">
-        <v>1</v>
-      </c>
+      <c r="M273" s="17"/>
       <c r="N273" s="17"/>
       <c r="O273" s="17"/>
       <c r="P273" s="17"/>
@@ -9785,10 +9777,10 @@
         <v>43</v>
       </c>
       <c r="B274" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C274" s="39" t="s">
-        <v>225</v>
+        <v>59</v>
       </c>
       <c r="D274" s="45"/>
       <c r="E274" s="45"/>
@@ -9799,17 +9791,15 @@
       <c r="H274" s="17">
         <v>1</v>
       </c>
-      <c r="I274" s="17"/>
-      <c r="J274" s="17">
-        <v>1</v>
-      </c>
+      <c r="I274" s="17">
+        <v>1</v>
+      </c>
+      <c r="J274" s="17"/>
       <c r="K274" s="17">
         <v>1</v>
       </c>
       <c r="L274" s="17"/>
-      <c r="M274" s="17">
-        <v>1</v>
-      </c>
+      <c r="M274" s="17"/>
       <c r="N274" s="17"/>
       <c r="O274" s="17"/>
       <c r="P274" s="17">
@@ -9822,23 +9812,25 @@
         <v>43</v>
       </c>
       <c r="B275" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C275" s="39" t="s">
-        <v>131</v>
+        <v>271</v>
       </c>
       <c r="D275" s="45"/>
       <c r="E275" s="45"/>
       <c r="F275" s="45"/>
       <c r="G275" s="17"/>
-      <c r="H275" s="17"/>
+      <c r="H275" s="17">
+        <v>1</v>
+      </c>
       <c r="I275" s="17"/>
       <c r="J275" s="17"/>
-      <c r="K275" s="17"/>
+      <c r="K275" s="17">
+        <v>1</v>
+      </c>
       <c r="L275" s="17"/>
-      <c r="M275" s="17">
-        <v>1</v>
-      </c>
+      <c r="M275" s="17"/>
       <c r="N275" s="17"/>
       <c r="O275" s="17"/>
       <c r="P275" s="17"/>
@@ -9852,29 +9844,25 @@
         <v>6</v>
       </c>
       <c r="C276" s="39" t="s">
-        <v>16</v>
+        <v>270</v>
       </c>
       <c r="D276" s="45"/>
       <c r="E276" s="45"/>
       <c r="F276" s="45"/>
-      <c r="G276" s="17">
-        <v>1</v>
-      </c>
+      <c r="G276" s="17"/>
       <c r="H276" s="17">
         <v>1</v>
       </c>
       <c r="I276" s="17"/>
       <c r="J276" s="17"/>
-      <c r="K276" s="17"/>
+      <c r="K276" s="17">
+        <v>1</v>
+      </c>
       <c r="L276" s="17"/>
-      <c r="M276" s="17">
-        <v>1</v>
-      </c>
+      <c r="M276" s="17"/>
       <c r="N276" s="17"/>
       <c r="O276" s="17"/>
-      <c r="P276" s="17">
-        <v>1</v>
-      </c>
+      <c r="P276" s="17"/>
       <c r="Q276" s="17"/>
     </row>
     <row r="277" spans="1:17" x14ac:dyDescent="0.2">
@@ -9882,36 +9870,28 @@
         <v>43</v>
       </c>
       <c r="B277" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C277" s="39" t="s">
-        <v>59</v>
+        <v>272</v>
       </c>
       <c r="D277" s="45"/>
       <c r="E277" s="45"/>
       <c r="F277" s="45"/>
-      <c r="G277" s="17">
-        <v>1</v>
-      </c>
+      <c r="G277" s="17"/>
       <c r="H277" s="17">
         <v>1</v>
       </c>
-      <c r="I277" s="17">
-        <v>1</v>
-      </c>
+      <c r="I277" s="17"/>
       <c r="J277" s="17"/>
       <c r="K277" s="17">
         <v>1</v>
       </c>
       <c r="L277" s="17"/>
-      <c r="M277" s="17">
-        <v>1</v>
-      </c>
+      <c r="M277" s="17"/>
       <c r="N277" s="17"/>
       <c r="O277" s="17"/>
-      <c r="P277" s="17">
-        <v>1</v>
-      </c>
+      <c r="P277" s="17"/>
       <c r="Q277" s="17"/>
     </row>
     <row r="278" spans="1:17" x14ac:dyDescent="0.2">
@@ -9919,17 +9899,15 @@
         <v>43</v>
       </c>
       <c r="B278" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C278" s="39" t="s">
-        <v>61</v>
+        <v>339</v>
       </c>
       <c r="D278" s="45"/>
       <c r="E278" s="45"/>
       <c r="F278" s="45"/>
-      <c r="G278" s="17">
-        <v>1</v>
-      </c>
+      <c r="G278" s="17"/>
       <c r="H278" s="17"/>
       <c r="I278" s="17"/>
       <c r="J278" s="17">
@@ -9937,9 +9915,7 @@
       </c>
       <c r="K278" s="17"/>
       <c r="L278" s="17"/>
-      <c r="M278" s="17">
-        <v>1</v>
-      </c>
+      <c r="M278" s="17"/>
       <c r="N278" s="17"/>
       <c r="O278" s="17"/>
       <c r="P278" s="17"/>
@@ -9953,22 +9929,16 @@
         <v>6</v>
       </c>
       <c r="C279" s="39" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D279" s="45"/>
       <c r="E279" s="45"/>
       <c r="F279" s="45"/>
       <c r="G279" s="17"/>
-      <c r="H279" s="17">
-        <v>1</v>
-      </c>
+      <c r="H279" s="17"/>
       <c r="I279" s="17"/>
-      <c r="J279" s="17">
-        <v>1</v>
-      </c>
-      <c r="K279" s="17">
-        <v>1</v>
-      </c>
+      <c r="J279" s="17"/>
+      <c r="K279" s="17"/>
       <c r="L279" s="17"/>
       <c r="M279" s="17">
         <v>1</v>
@@ -9986,25 +9956,33 @@
         <v>6</v>
       </c>
       <c r="C280" s="39" t="s">
-        <v>271</v>
+        <v>225</v>
       </c>
       <c r="D280" s="45"/>
       <c r="E280" s="45"/>
       <c r="F280" s="45"/>
-      <c r="G280" s="17"/>
+      <c r="G280" s="17">
+        <v>1</v>
+      </c>
       <c r="H280" s="17">
         <v>1</v>
       </c>
       <c r="I280" s="17"/>
-      <c r="J280" s="17"/>
+      <c r="J280" s="17">
+        <v>1</v>
+      </c>
       <c r="K280" s="17">
         <v>1</v>
       </c>
       <c r="L280" s="17"/>
-      <c r="M280" s="17"/>
+      <c r="M280" s="17">
+        <v>1</v>
+      </c>
       <c r="N280" s="17"/>
       <c r="O280" s="17"/>
-      <c r="P280" s="17"/>
+      <c r="P280" s="17">
+        <v>1</v>
+      </c>
       <c r="Q280" s="17"/>
     </row>
     <row r="281" spans="1:17" x14ac:dyDescent="0.2">
@@ -10015,25 +9993,29 @@
         <v>6</v>
       </c>
       <c r="C281" s="39" t="s">
-        <v>270</v>
+        <v>16</v>
       </c>
       <c r="D281" s="45"/>
       <c r="E281" s="45"/>
       <c r="F281" s="45"/>
-      <c r="G281" s="17"/>
+      <c r="G281" s="17">
+        <v>1</v>
+      </c>
       <c r="H281" s="17">
         <v>1</v>
       </c>
       <c r="I281" s="17"/>
       <c r="J281" s="17"/>
-      <c r="K281" s="17">
-        <v>1</v>
-      </c>
+      <c r="K281" s="17"/>
       <c r="L281" s="17"/>
-      <c r="M281" s="17"/>
+      <c r="M281" s="17">
+        <v>1</v>
+      </c>
       <c r="N281" s="17"/>
       <c r="O281" s="17"/>
-      <c r="P281" s="17"/>
+      <c r="P281" s="17">
+        <v>1</v>
+      </c>
       <c r="Q281" s="17"/>
     </row>
     <row r="282" spans="1:17" x14ac:dyDescent="0.2">
@@ -10041,25 +10023,27 @@
         <v>43</v>
       </c>
       <c r="B282" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C282" s="39" t="s">
-        <v>272</v>
+        <v>61</v>
       </c>
       <c r="D282" s="45"/>
       <c r="E282" s="45"/>
       <c r="F282" s="45"/>
-      <c r="G282" s="17"/>
-      <c r="H282" s="17">
-        <v>1</v>
-      </c>
+      <c r="G282" s="17">
+        <v>1</v>
+      </c>
+      <c r="H282" s="17"/>
       <c r="I282" s="17"/>
-      <c r="J282" s="17"/>
-      <c r="K282" s="17">
-        <v>1</v>
-      </c>
+      <c r="J282" s="17">
+        <v>1</v>
+      </c>
+      <c r="K282" s="17"/>
       <c r="L282" s="17"/>
-      <c r="M282" s="17"/>
+      <c r="M282" s="17">
+        <v>1</v>
+      </c>
       <c r="N282" s="17"/>
       <c r="O282" s="17"/>
       <c r="P282" s="17"/>
@@ -10073,18 +10057,22 @@
         <v>6</v>
       </c>
       <c r="C283" s="39" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D283" s="45"/>
       <c r="E283" s="45"/>
       <c r="F283" s="45"/>
       <c r="G283" s="17"/>
-      <c r="H283" s="17"/>
+      <c r="H283" s="17">
+        <v>1</v>
+      </c>
       <c r="I283" s="17"/>
       <c r="J283" s="17">
         <v>1</v>
       </c>
-      <c r="K283" s="17"/>
+      <c r="K283" s="17">
+        <v>1</v>
+      </c>
       <c r="L283" s="17"/>
       <c r="M283" s="17">
         <v>1</v>
@@ -10099,30 +10087,22 @@
         <v>43</v>
       </c>
       <c r="B284" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C284" s="39" t="s">
-        <v>66</v>
+        <v>99</v>
       </c>
       <c r="D284" s="45"/>
       <c r="E284" s="45"/>
       <c r="F284" s="45"/>
-      <c r="G284" s="17">
-        <v>1</v>
-      </c>
-      <c r="H284" s="17">
-        <v>1</v>
-      </c>
+      <c r="G284" s="17"/>
+      <c r="H284" s="17"/>
       <c r="I284" s="17"/>
       <c r="J284" s="17">
         <v>1</v>
       </c>
-      <c r="K284" s="17">
-        <v>1</v>
-      </c>
-      <c r="L284" s="17">
-        <v>1</v>
-      </c>
+      <c r="K284" s="17"/>
+      <c r="L284" s="17"/>
       <c r="M284" s="17">
         <v>1</v>
       </c>
@@ -10139,23 +10119,33 @@
         <v>6</v>
       </c>
       <c r="C285" s="39" t="s">
-        <v>339</v>
+        <v>118</v>
       </c>
       <c r="D285" s="45"/>
       <c r="E285" s="45"/>
       <c r="F285" s="45"/>
-      <c r="G285" s="17"/>
-      <c r="H285" s="17"/>
+      <c r="G285" s="17">
+        <v>1</v>
+      </c>
+      <c r="H285" s="17">
+        <v>1</v>
+      </c>
       <c r="I285" s="17"/>
       <c r="J285" s="17">
         <v>1</v>
       </c>
-      <c r="K285" s="17"/>
-      <c r="L285" s="17"/>
+      <c r="K285" s="17">
+        <v>1</v>
+      </c>
+      <c r="L285" s="17">
+        <v>1</v>
+      </c>
       <c r="M285" s="17"/>
       <c r="N285" s="17"/>
       <c r="O285" s="17"/>
-      <c r="P285" s="17"/>
+      <c r="P285" s="17">
+        <v>1</v>
+      </c>
       <c r="Q285" s="17"/>
     </row>
     <row r="286" spans="1:17" x14ac:dyDescent="0.2">
@@ -10163,10 +10153,10 @@
         <v>43</v>
       </c>
       <c r="B286" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C286" s="39" t="s">
-        <v>102</v>
+        <v>66</v>
       </c>
       <c r="D286" s="45"/>
       <c r="E286" s="45"/>
@@ -10177,9 +10167,7 @@
       <c r="H286" s="17">
         <v>1</v>
       </c>
-      <c r="I286" s="17">
-        <v>1</v>
-      </c>
+      <c r="I286" s="17"/>
       <c r="J286" s="17">
         <v>1</v>
       </c>
@@ -10192,28 +10180,20 @@
       <c r="M286" s="17">
         <v>1</v>
       </c>
-      <c r="N286" s="17">
-        <v>1</v>
-      </c>
-      <c r="O286" s="17">
-        <v>1</v>
-      </c>
-      <c r="P286" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q286" s="17">
-        <v>1</v>
-      </c>
+      <c r="N286" s="17"/>
+      <c r="O286" s="17"/>
+      <c r="P286" s="17"/>
+      <c r="Q286" s="17"/>
     </row>
     <row r="287" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A287" s="37" t="s">
         <v>43</v>
       </c>
       <c r="B287" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C287" s="39" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
       <c r="D287" s="45"/>
       <c r="E287" s="45"/>
@@ -10224,7 +10204,9 @@
       <c r="H287" s="17">
         <v>1</v>
       </c>
-      <c r="I287" s="17"/>
+      <c r="I287" s="17">
+        <v>1</v>
+      </c>
       <c r="J287" s="17">
         <v>1</v>
       </c>
@@ -10237,20 +10219,28 @@
       <c r="M287" s="17">
         <v>1</v>
       </c>
-      <c r="N287" s="17"/>
-      <c r="O287" s="17"/>
-      <c r="P287" s="17"/>
-      <c r="Q287" s="17"/>
+      <c r="N287" s="17">
+        <v>1</v>
+      </c>
+      <c r="O287" s="17">
+        <v>1</v>
+      </c>
+      <c r="P287" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q287" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="288" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A288" s="37" t="s">
         <v>43</v>
       </c>
       <c r="B288" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C288" s="39" t="s">
-        <v>312</v>
+        <v>67</v>
       </c>
       <c r="D288" s="45"/>
       <c r="E288" s="45"/>
@@ -10261,9 +10251,7 @@
       <c r="H288" s="17">
         <v>1</v>
       </c>
-      <c r="I288" s="17">
-        <v>1</v>
-      </c>
+      <c r="I288" s="17"/>
       <c r="J288" s="17">
         <v>1</v>
       </c>
@@ -10278,9 +10266,7 @@
       </c>
       <c r="N288" s="17"/>
       <c r="O288" s="17"/>
-      <c r="P288" s="17">
-        <v>1</v>
-      </c>
+      <c r="P288" s="17"/>
       <c r="Q288" s="17"/>
     </row>
     <row r="289" spans="1:17" x14ac:dyDescent="0.2">
@@ -10288,10 +10274,10 @@
         <v>43</v>
       </c>
       <c r="B289" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C289" s="39" t="s">
-        <v>71</v>
+        <v>312</v>
       </c>
       <c r="D289" s="45"/>
       <c r="E289" s="45"/>
@@ -10302,12 +10288,18 @@
       <c r="H289" s="17">
         <v>1</v>
       </c>
-      <c r="I289" s="17"/>
-      <c r="J289" s="17"/>
+      <c r="I289" s="17">
+        <v>1</v>
+      </c>
+      <c r="J289" s="17">
+        <v>1</v>
+      </c>
       <c r="K289" s="17">
         <v>1</v>
       </c>
-      <c r="L289" s="17"/>
+      <c r="L289" s="17">
+        <v>1</v>
+      </c>
       <c r="M289" s="17">
         <v>1</v>
       </c>
@@ -10323,10 +10315,10 @@
         <v>43</v>
       </c>
       <c r="B290" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C290" s="39" t="s">
-        <v>118</v>
+        <v>71</v>
       </c>
       <c r="D290" s="45"/>
       <c r="E290" s="45"/>
@@ -10338,15 +10330,11 @@
         <v>1</v>
       </c>
       <c r="I290" s="17"/>
-      <c r="J290" s="17">
-        <v>1</v>
-      </c>
+      <c r="J290" s="17"/>
       <c r="K290" s="17">
         <v>1</v>
       </c>
-      <c r="L290" s="17">
-        <v>1</v>
-      </c>
+      <c r="L290" s="17"/>
       <c r="M290" s="17">
         <v>1</v>
       </c>
@@ -10729,9 +10717,7 @@
         <v>1</v>
       </c>
       <c r="L302" s="17"/>
-      <c r="M302" s="17">
-        <v>1</v>
-      </c>
+      <c r="M302" s="17"/>
       <c r="N302" s="17">
         <v>1</v>
       </c>
@@ -10774,9 +10760,7 @@
         <v>1</v>
       </c>
       <c r="L303" s="17"/>
-      <c r="M303" s="17">
-        <v>1</v>
-      </c>
+      <c r="M303" s="17"/>
       <c r="N303" s="17">
         <v>1</v>
       </c>
@@ -10795,10 +10779,10 @@
         <v>47</v>
       </c>
       <c r="B304" s="12" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C304" s="13" t="s">
-        <v>158</v>
+        <v>124</v>
       </c>
       <c r="D304" s="45"/>
       <c r="E304" s="45"/>
@@ -10809,9 +10793,7 @@
       <c r="H304" s="17">
         <v>1</v>
       </c>
-      <c r="I304" s="17">
-        <v>1</v>
-      </c>
+      <c r="I304" s="17"/>
       <c r="J304" s="17">
         <v>1</v>
       </c>
@@ -10821,21 +10803,13 @@
       <c r="L304" s="17">
         <v>1</v>
       </c>
-      <c r="M304" s="17">
-        <v>1</v>
-      </c>
+      <c r="M304" s="17"/>
       <c r="N304" s="17">
         <v>1</v>
       </c>
-      <c r="O304" s="17">
-        <v>1</v>
-      </c>
-      <c r="P304" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q304" s="17">
-        <v>1</v>
-      </c>
+      <c r="O304" s="17"/>
+      <c r="P304" s="17"/>
+      <c r="Q304" s="17"/>
     </row>
     <row r="305" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A305" s="11" t="s">
@@ -10845,21 +10819,17 @@
         <v>6</v>
       </c>
       <c r="C305" s="56" t="s">
-        <v>124</v>
+        <v>315</v>
       </c>
       <c r="D305" s="48"/>
       <c r="E305" s="48"/>
       <c r="F305" s="48"/>
-      <c r="G305" s="54">
-        <v>1</v>
-      </c>
+      <c r="G305" s="54"/>
       <c r="H305" s="54">
         <v>1</v>
       </c>
       <c r="I305" s="54"/>
-      <c r="J305" s="54">
-        <v>1</v>
-      </c>
+      <c r="J305" s="54"/>
       <c r="K305" s="54">
         <v>1</v>
       </c>
@@ -10882,7 +10852,7 @@
         <v>6</v>
       </c>
       <c r="C306" s="57" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D306" s="48"/>
       <c r="E306" s="48"/>
@@ -10915,7 +10885,7 @@
         <v>6</v>
       </c>
       <c r="C307" s="57" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D307" s="48"/>
       <c r="E307" s="48"/>
@@ -10948,7 +10918,7 @@
         <v>6</v>
       </c>
       <c r="C308" s="57" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="D308" s="48"/>
       <c r="E308" s="48"/>
@@ -10981,7 +10951,7 @@
         <v>6</v>
       </c>
       <c r="C309" s="57" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D309" s="48"/>
       <c r="E309" s="48"/>
@@ -11011,33 +10981,47 @@
         <v>47</v>
       </c>
       <c r="B310" s="55" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C310" s="57" t="s">
-        <v>317</v>
+        <v>158</v>
       </c>
       <c r="D310" s="48"/>
       <c r="E310" s="48"/>
       <c r="F310" s="48"/>
-      <c r="G310" s="54"/>
+      <c r="G310" s="54">
+        <v>1</v>
+      </c>
       <c r="H310" s="54">
         <v>1</v>
       </c>
-      <c r="I310" s="54"/>
-      <c r="J310" s="54"/>
+      <c r="I310" s="54">
+        <v>1</v>
+      </c>
+      <c r="J310" s="54">
+        <v>1</v>
+      </c>
       <c r="K310" s="54">
         <v>1</v>
       </c>
       <c r="L310" s="54">
         <v>1</v>
       </c>
-      <c r="M310" s="54"/>
+      <c r="M310" s="54">
+        <v>1</v>
+      </c>
       <c r="N310" s="54">
         <v>1</v>
       </c>
-      <c r="O310" s="54"/>
-      <c r="P310" s="54"/>
-      <c r="Q310" s="54"/>
+      <c r="O310" s="54">
+        <v>1</v>
+      </c>
+      <c r="P310" s="54">
+        <v>1</v>
+      </c>
+      <c r="Q310" s="54">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q310" xr:uid="{A96C7FF1-A6C9-A643-BFCA-7D7FCDAF5533}">
@@ -11054,43 +11038,43 @@
     <hyperlink ref="C254" r:id="rId2" display="https://aws.amazon.com/app-mesh/" xr:uid="{F151395F-8E37-1049-9FCA-8474F2603F07}"/>
     <hyperlink ref="C29" r:id="rId3" display="https://aws.amazon.com/appsync/" xr:uid="{DB5645FD-41DF-9D4C-ADDB-CEEB9418B261}"/>
     <hyperlink ref="C272" r:id="rId4" display="https://aws.amazon.com/artifact/" xr:uid="{0251BE44-6F83-3541-8CD4-81AEF00F1760}"/>
-    <hyperlink ref="C273" r:id="rId5" display="https://aws.amazon.com/audit-manager/" xr:uid="{FE0C678B-66B4-5041-87CB-7B1FF56DF53B}"/>
+    <hyperlink ref="C279" r:id="rId5" display="https://aws.amazon.com/audit-manager/" xr:uid="{FE0C678B-66B4-5041-87CB-7B1FF56DF53B}"/>
     <hyperlink ref="C173" r:id="rId6" display="https://aws.amazon.com/autoscaling/" xr:uid="{900D412E-B452-CD43-BEB1-C8C1CB7269C8}"/>
     <hyperlink ref="C174" r:id="rId7" display="https://aws.amazon.com/backup/" xr:uid="{E0DD5920-BDCE-E647-9AF3-74760943689B}"/>
-    <hyperlink ref="C44" r:id="rId8" display="https://aws.amazon.com/batch/" xr:uid="{784C0A03-DDEC-BE4D-88F7-7005C1BB046B}"/>
+    <hyperlink ref="C45" r:id="rId8" display="https://aws.amazon.com/batch/" xr:uid="{784C0A03-DDEC-BE4D-88F7-7005C1BB046B}"/>
     <hyperlink ref="C67" r:id="rId9" display="https://aws.amazon.com/aws-cost-management/aws-budgets/" xr:uid="{57F5A17A-4752-B94C-8FBB-FC20BBF1A0BE}"/>
-    <hyperlink ref="C274" r:id="rId10" display="https://aws.amazon.com/certificate-manager/" xr:uid="{1F5BBCA8-0D50-C44C-907B-68E23D8E605C}"/>
+    <hyperlink ref="C280" r:id="rId10" display="https://aws.amazon.com/certificate-manager/" xr:uid="{1F5BBCA8-0D50-C44C-907B-68E23D8E605C}"/>
     <hyperlink ref="C39" r:id="rId11" display="https://aws.amazon.com/chatbot/" xr:uid="{F29F6239-1ADB-7049-AAA7-6E39F247047B}"/>
     <hyperlink ref="C256" r:id="rId12" display="https://aws.amazon.com/cloud-map/" xr:uid="{D482891E-9EB7-EA40-9A4B-6A8D3FEADBE3}"/>
     <hyperlink ref="C100" r:id="rId13" display="https://aws.amazon.com/cloud9/" xr:uid="{D565484B-E9EF-EA40-BDBE-0314AF229AE7}"/>
-    <hyperlink ref="C175" r:id="rId14" display="https://aws.amazon.com/cloudformation/" xr:uid="{602EC08B-B845-E049-943E-890A120862C8}"/>
-    <hyperlink ref="C276" r:id="rId15" display="https://aws.amazon.com/cloudhsm/" xr:uid="{76B855B6-4A01-1642-8706-3316A1643BA7}"/>
-    <hyperlink ref="C176" r:id="rId16" display="https://aws.amazon.com/cloudtrail/" xr:uid="{F1C2A161-2AD0-B14D-B62A-2640A558856F}"/>
+    <hyperlink ref="C176" r:id="rId14" display="https://aws.amazon.com/cloudformation/" xr:uid="{602EC08B-B845-E049-943E-890A120862C8}"/>
+    <hyperlink ref="C281" r:id="rId15" display="https://aws.amazon.com/cloudhsm/" xr:uid="{76B855B6-4A01-1642-8706-3316A1643BA7}"/>
+    <hyperlink ref="C175" r:id="rId16" display="https://aws.amazon.com/cloudtrail/" xr:uid="{F1C2A161-2AD0-B14D-B62A-2640A558856F}"/>
     <hyperlink ref="C102" r:id="rId17" display="https://aws.amazon.com/codeartifact" xr:uid="{A5B8559F-E4FA-BC42-AC7A-9D708C1D63A0}"/>
     <hyperlink ref="C103" r:id="rId18" display="https://aws.amazon.com/codebuild/" xr:uid="{E4144166-80F6-E741-B704-7C3864420913}"/>
     <hyperlink ref="C104" r:id="rId19" display="https://aws.amazon.com/codecommit/" xr:uid="{C9DB0F3B-CAEF-524C-A620-ACEA3E04FA66}"/>
     <hyperlink ref="C105" r:id="rId20" display="https://aws.amazon.com/codedeploy/" xr:uid="{D94C938E-B3D5-054D-AC63-39672D0C0DFC}"/>
     <hyperlink ref="C107" r:id="rId21" display="https://aws.amazon.com/codepipeline/" xr:uid="{DA2435A7-DA61-A54F-B02D-9BA62C072DF8}"/>
     <hyperlink ref="C108" r:id="rId22" display="https://aws.amazon.com/codestar/" xr:uid="{80EC7E07-A675-4540-8CC7-7CD9427476B0}"/>
-    <hyperlink ref="C178" r:id="rId23" display="https://aws.amazon.com/compute-optimizer/" xr:uid="{099597B3-D96C-124F-8A6B-DB661823AC75}"/>
-    <hyperlink ref="C179" r:id="rId24" display="https://aws.amazon.com/config/" xr:uid="{1DE61048-35C8-FB4C-A941-8996CBD19463}"/>
-    <hyperlink ref="C181" r:id="rId25" display="https://aws.amazon.com/controltower" xr:uid="{5ACDD884-3684-1840-9A42-603B4BFD4DFA}"/>
+    <hyperlink ref="C180" r:id="rId23" display="https://aws.amazon.com/compute-optimizer/" xr:uid="{099597B3-D96C-124F-8A6B-DB661823AC75}"/>
+    <hyperlink ref="C178" r:id="rId24" display="https://aws.amazon.com/config/" xr:uid="{1DE61048-35C8-FB4C-A941-8996CBD19463}"/>
+    <hyperlink ref="C183" r:id="rId25" display="https://aws.amazon.com/controltower" xr:uid="{5ACDD884-3684-1840-9A42-603B4BFD4DFA}"/>
     <hyperlink ref="C239" r:id="rId26" display="https://aws.amazon.com/data-exchange/" xr:uid="{EF81BA84-5C8F-DD4B-A31A-47BF7D5C826C}"/>
     <hyperlink ref="C242" r:id="rId27" display="https://aws.amazon.com/datasync" xr:uid="{7CED07B2-F329-1D46-A78D-E74BADEF8307}"/>
     <hyperlink ref="C241" r:id="rId28" display="https://aws.amazon.com/dms/" xr:uid="{C9210BF6-9C8C-5E48-824D-711353B0A5C4}"/>
     <hyperlink ref="C258" r:id="rId29" display="https://aws.amazon.com/directconnect/" xr:uid="{D4260538-1F28-C64D-999E-B57D8B4A110D}"/>
-    <hyperlink ref="C279" r:id="rId30" display="https://aws.amazon.com/directoryservice/" xr:uid="{71568105-08FB-3E48-ADDD-31FCAC00E550}"/>
-    <hyperlink ref="C47" r:id="rId31" display="https://aws.amazon.com/elasticbeanstalk/" xr:uid="{503FA701-A8C3-BA4D-8F14-4F45B1936437}"/>
+    <hyperlink ref="C283" r:id="rId30" display="https://aws.amazon.com/directoryservice/" xr:uid="{71568105-08FB-3E48-ADDD-31FCAC00E550}"/>
+    <hyperlink ref="C48" r:id="rId31" display="https://aws.amazon.com/elasticbeanstalk/" xr:uid="{503FA701-A8C3-BA4D-8F14-4F45B1936437}"/>
     <hyperlink ref="C220" r:id="rId32" display="https://aws.amazon.com/mediaconnect" xr:uid="{97EBEF96-B9F8-0444-803B-77B7686AD926}"/>
     <hyperlink ref="C221" r:id="rId33" display="https://aws.amazon.com/mediaconvert/" xr:uid="{A189CA26-8FE5-724E-AB4C-DA1684A9397C}"/>
     <hyperlink ref="C222" r:id="rId34" display="https://aws.amazon.com/medialive/" xr:uid="{8A1902D4-C3B2-6540-B6A2-D0939C092476}"/>
     <hyperlink ref="C62" r:id="rId35" display="https://aws.amazon.com/fargate/" xr:uid="{8AAC0488-BCAF-394A-B65D-1C8169C9015E}"/>
-    <hyperlink ref="C283" r:id="rId36" display="https://aws.amazon.com/firewall-manager/" xr:uid="{C1FC3FB2-6BB1-124F-AA39-0A32AEF1D03C}"/>
-    <hyperlink ref="C260" r:id="rId37" display="https://aws.amazon.com/global-accelerator" xr:uid="{94823B64-0747-B847-98EC-9C84C21B2DE2}"/>
+    <hyperlink ref="C284" r:id="rId36" display="https://aws.amazon.com/firewall-manager/" xr:uid="{C1FC3FB2-6BB1-124F-AA39-0A32AEF1D03C}"/>
+    <hyperlink ref="C261" r:id="rId37" display="https://aws.amazon.com/global-accelerator" xr:uid="{94823B64-0747-B847-98EC-9C84C21B2DE2}"/>
     <hyperlink ref="C7" r:id="rId38" display="https://aws.amazon.com/glue/" xr:uid="{A2984E2F-A64C-D74C-A499-872A26B2DE44}"/>
     <hyperlink ref="C271" r:id="rId39" display="https://aws.amazon.com/ground-station/" xr:uid="{DB86E86A-EF5B-2541-9BD8-5CDA9965E40C}"/>
     <hyperlink ref="C73" r:id="rId40" display="https://aws.amazon.com/iq/" xr:uid="{66074B4A-E4D5-724E-AD29-24C171CEC0BA}"/>
-    <hyperlink ref="C286" r:id="rId41" display="https://aws.amazon.com/iam" xr:uid="{97081695-DB1E-424E-B0EE-79AAD8D6E1CE}"/>
+    <hyperlink ref="C287" r:id="rId41" display="https://aws.amazon.com/iam" xr:uid="{97081695-DB1E-424E-B0EE-79AAD8D6E1CE}"/>
     <hyperlink ref="C125" r:id="rId42" display="https://aws.amazon.com/iot-1-click/" xr:uid="{ADC027FD-055F-9343-AF7A-479D41533208}"/>
     <hyperlink ref="C126" r:id="rId43" display="https://aws.amazon.com/iot-analytics/" xr:uid="{6587843B-FF8F-E445-A148-97BAA80660A5}"/>
     <hyperlink ref="C127" r:id="rId44" display="https://aws.amazon.com/iot/" xr:uid="{72ADB53E-C5C8-6E45-9DE6-006357ADBB14}"/>
@@ -11098,38 +11082,38 @@
     <hyperlink ref="C129" r:id="rId46" display="https://aws.amazon.com/iot-device-management/" xr:uid="{47327A94-A7DA-D44B-8D5D-137A2C1DB78D}"/>
     <hyperlink ref="C131" r:id="rId47" display="https://aws.amazon.com/iot-events/" xr:uid="{09A17074-F045-D045-99F3-289DE651CC4B}"/>
     <hyperlink ref="C132" r:id="rId48" display="https://aws.amazon.com/greengrass/" xr:uid="{86C6B532-C282-AD49-84FC-E7151CC17562}"/>
-    <hyperlink ref="C288" r:id="rId49" display="https://aws.amazon.com/kms/" xr:uid="{C0A6E0DF-7D93-854D-AF8E-5B9C19B8AF02}"/>
+    <hyperlink ref="C289" r:id="rId49" display="https://aws.amazon.com/kms/" xr:uid="{C0A6E0DF-7D93-854D-AF8E-5B9C19B8AF02}"/>
     <hyperlink ref="C18" r:id="rId50" display="https://aws.amazon.com/lake-formation/" xr:uid="{8B1B5135-7A0D-7645-A701-475DDEBCFDA0}"/>
     <hyperlink ref="C49" r:id="rId51" display="https://aws.amazon.com/lambda/" xr:uid="{23B44498-C148-BD4C-86FE-EFAA00464E5B}"/>
-    <hyperlink ref="C184" r:id="rId52" display="https://aws.amazon.com/license-manager/" xr:uid="{A80531A2-32DF-5E46-A8A2-AD514A9E876E}"/>
+    <hyperlink ref="C189" r:id="rId52" display="https://aws.amazon.com/license-manager/" xr:uid="{A80531A2-32DF-5E46-A8A2-AD514A9E876E}"/>
     <hyperlink ref="C75" r:id="rId53" display="https://aws.amazon.com/mp/" xr:uid="{83E81132-B5F9-A141-93D4-67826C5C6C2F}"/>
-    <hyperlink ref="C261" r:id="rId54" display="https://aws.amazon.com/network-firewall/" xr:uid="{380438F2-2136-CA48-8A93-614BD286828F}"/>
-    <hyperlink ref="C189" r:id="rId55" display="https://aws.amazon.com/opsworks/stacks/" xr:uid="{C7B2C66E-7305-8A45-B44D-ED0E58D460E7}"/>
-    <hyperlink ref="C187" r:id="rId56" display="https://aws.amazon.com/opsworks/chefautomate/" xr:uid="{44B83691-1D72-4540-A13B-BDA885E2E12D}"/>
-    <hyperlink ref="C188" r:id="rId57" display="https://aws.amazon.com/opsworks/puppetenterprise/" xr:uid="{23F41EB8-3A55-A44E-BD0D-93039495EA49}"/>
-    <hyperlink ref="C190" r:id="rId58" display="https://aws.amazon.com/organizations" xr:uid="{A3AB0BF0-AC79-A142-8708-144AD8A2BAF3}"/>
+    <hyperlink ref="C260" r:id="rId54" display="https://aws.amazon.com/network-firewall/" xr:uid="{380438F2-2136-CA48-8A93-614BD286828F}"/>
+    <hyperlink ref="C194" r:id="rId55" display="https://aws.amazon.com/opsworks/stacks/" xr:uid="{C7B2C66E-7305-8A45-B44D-ED0E58D460E7}"/>
+    <hyperlink ref="C192" r:id="rId56" display="https://aws.amazon.com/opsworks/chefautomate/" xr:uid="{44B83691-1D72-4540-A13B-BDA885E2E12D}"/>
+    <hyperlink ref="C193" r:id="rId57" display="https://aws.amazon.com/opsworks/puppetenterprise/" xr:uid="{23F41EB8-3A55-A44E-BD0D-93039495EA49}"/>
+    <hyperlink ref="C179" r:id="rId58" display="https://aws.amazon.com/organizations" xr:uid="{A3AB0BF0-AC79-A142-8708-144AD8A2BAF3}"/>
     <hyperlink ref="C51" r:id="rId59" display="https://aws.amazon.com/outposts/" xr:uid="{EC0218BA-7EA9-5F4D-8A2F-8D931B087AA0}"/>
-    <hyperlink ref="C191" r:id="rId60" display="https://aws.amazon.com/premiumsupport/phd/" xr:uid="{BC843AAF-6516-F341-B87D-0984C181B4B5}"/>
-    <hyperlink ref="C262" r:id="rId61" display="https://aws.amazon.com/privatelink/" xr:uid="{908DA648-769A-FB47-86E4-3D66FA675B1C}"/>
+    <hyperlink ref="C195" r:id="rId60" display="https://aws.amazon.com/premiumsupport/phd/" xr:uid="{BC843AAF-6516-F341-B87D-0984C181B4B5}"/>
+    <hyperlink ref="C263" r:id="rId61" display="https://aws.amazon.com/privatelink/" xr:uid="{908DA648-769A-FB47-86E4-3D66FA675B1C}"/>
     <hyperlink ref="C64" r:id="rId62" display="https://aws.amazon.com/proton/" xr:uid="{73BECBB6-D4BE-F445-97BF-0A1D62BCA194}"/>
-    <hyperlink ref="C192" r:id="rId63" display="https://aws.amazon.com/ram/" xr:uid="{F8E211FB-42AB-6848-88B7-49CC2A833913}"/>
+    <hyperlink ref="C196" r:id="rId63" display="https://aws.amazon.com/ram/" xr:uid="{F8E211FB-42AB-6848-88B7-49CC2A833913}"/>
     <hyperlink ref="C270" r:id="rId64" display="https://aws.amazon.com/robomaker/" xr:uid="{DBD68496-4CE8-804C-B893-9CFFB849F53A}"/>
-    <hyperlink ref="C290" r:id="rId65" display="https://aws.amazon.com/secrets-manager/" xr:uid="{632A5D67-D598-184C-AB9B-96F30896117D}"/>
+    <hyperlink ref="C285" r:id="rId65" display="https://aws.amazon.com/secrets-manager/" xr:uid="{632A5D67-D598-184C-AB9B-96F30896117D}"/>
     <hyperlink ref="C291" r:id="rId66" display="https://aws.amazon.com/security-hub/" xr:uid="{342A4832-F3A0-DB4D-840C-8118FD830399}"/>
     <hyperlink ref="C248" r:id="rId67" display="https://aws.amazon.com/server-migration-service/" xr:uid="{9446514E-0CE8-EC41-A9F1-0DC1FB7ADA55}"/>
     <hyperlink ref="C52" r:id="rId68" display="https://aws.amazon.com/serverless/serverlessrepo/" xr:uid="{8F7AC4BC-9A37-EC4F-8183-7D7404D19E14}"/>
-    <hyperlink ref="C193" r:id="rId69" display="https://aws.amazon.com/servicecatalog/" xr:uid="{2D2653B1-3D13-014A-9B9C-2386E2577635}"/>
+    <hyperlink ref="C197" r:id="rId69" display="https://aws.amazon.com/servicecatalog/" xr:uid="{2D2653B1-3D13-014A-9B9C-2386E2577635}"/>
     <hyperlink ref="C292" r:id="rId70" display="https://aws.amazon.com/shield/" xr:uid="{76E091F3-F618-A648-879F-3F09BEBFABFD}"/>
     <hyperlink ref="C293" r:id="rId71" display="https://aws.amazon.com/single-sign-on/" xr:uid="{A8360283-DE5C-1140-A85B-F33A2D6F72B8}"/>
     <hyperlink ref="C249" r:id="rId72" display="https://aws.amazon.com/snowball/" xr:uid="{8A7E1B57-5F26-F64E-853D-BDD63390D5E6}"/>
     <hyperlink ref="C251" r:id="rId73" display="https://aws.amazon.com/snowmobile/" xr:uid="{62B7D92F-3C96-DA44-9F02-BCC308391061}"/>
     <hyperlink ref="C36" r:id="rId74" display="https://aws.amazon.com/step-functions/details/" xr:uid="{10824B81-0A5F-634D-84E6-9D2ADE3A6B39}"/>
-    <hyperlink ref="C305" r:id="rId75" display="https://aws.amazon.com/storagegateway/" xr:uid="{7BF17EFE-FF03-1D4A-BE9E-1FA982DA5C2A}"/>
+    <hyperlink ref="C304" r:id="rId75" display="https://aws.amazon.com/storagegateway/" xr:uid="{7BF17EFE-FF03-1D4A-BE9E-1FA982DA5C2A}"/>
     <hyperlink ref="C77" r:id="rId76" display="https://aws.amazon.com/premiumsupport/" xr:uid="{A5466C95-EFB7-3944-9E29-8D19BB6E169F}"/>
-    <hyperlink ref="C211" r:id="rId77" display="https://aws.amazon.com/systems-manager/" xr:uid="{D6C17500-BE92-C444-BA4A-7116B75319D3}"/>
+    <hyperlink ref="C186" r:id="rId77" display="https://aws.amazon.com/systems-manager/" xr:uid="{D6C17500-BE92-C444-BA4A-7116B75319D3}"/>
     <hyperlink ref="C252" r:id="rId78" display="https://aws.amazon.com/aws-transfer-family/" xr:uid="{F0069BD4-8633-FB4B-8185-293CB3193797}"/>
-    <hyperlink ref="C265" r:id="rId79" display="https://aws.amazon.com/transit-gateway/" xr:uid="{2C10B2F7-EEE3-3444-A855-B387D48706EA}"/>
-    <hyperlink ref="C212" r:id="rId80" display="https://aws.amazon.com/premiumsupport/trustedadvisor/" xr:uid="{436ECB3D-7EFE-764A-B2E3-3CF79C97B742}"/>
+    <hyperlink ref="C266" r:id="rId79" display="https://aws.amazon.com/transit-gateway/" xr:uid="{2C10B2F7-EEE3-3444-A855-B387D48706EA}"/>
+    <hyperlink ref="C187" r:id="rId80" display="https://aws.amazon.com/premiumsupport/trustedadvisor/" xr:uid="{436ECB3D-7EFE-764A-B2E3-3CF79C97B742}"/>
     <hyperlink ref="C268" r:id="rId81" display="https://aws.amazon.com/vpn/" xr:uid="{5F2B553B-98BD-8D4B-849C-55A6F659C6B1}"/>
     <hyperlink ref="C294" r:id="rId82" display="https://aws.amazon.com/waf/" xr:uid="{CF739D06-0B1B-6B46-91CF-6EE57FF09613}"/>
     <hyperlink ref="C213" r:id="rId83" display="https://aws.amazon.com/well-architected-tool" xr:uid="{81A34672-555C-B74A-9D7B-58590B7D3C75}"/>
@@ -11140,20 +11124,20 @@
     <hyperlink ref="C136" r:id="rId88" display="https://aws.amazon.com/augmented-ai/" xr:uid="{9B0A35B8-349D-874F-B406-0C378A70E4A7}"/>
     <hyperlink ref="C82" r:id="rId89" display="https://aws.amazon.com/rds/aurora/" xr:uid="{5BA37BE5-5EFA-D640-9340-68572A5C8B0A}"/>
     <hyperlink ref="C40" r:id="rId90" display="https://chime.aws/" xr:uid="{08A22D72-3716-8743-A4B8-3002293D3436}"/>
-    <hyperlink ref="C275" r:id="rId91" display="https://aws.amazon.com/cloud-directory/" xr:uid="{E41D133C-BA4E-4642-BA6F-656788DBC830}"/>
+    <hyperlink ref="C273" r:id="rId91" display="https://aws.amazon.com/cloud-directory/" xr:uid="{E41D133C-BA4E-4642-BA6F-656788DBC830}"/>
     <hyperlink ref="C257" r:id="rId92" display="https://aws.amazon.com/cloudfront/" xr:uid="{8065D5C6-B564-A941-80CC-5D6C65B3D725}"/>
     <hyperlink ref="C177" r:id="rId93" display="https://aws.amazon.com/cloudwatch/" xr:uid="{52B01F49-5EAB-E540-BA38-BEED42EB43F4}"/>
     <hyperlink ref="C106" r:id="rId94" display="https://aws.amazon.com/codeguru/" xr:uid="{D5D1E2B5-ED1C-0D45-BCD8-07A6431E8C14}"/>
-    <hyperlink ref="C277" r:id="rId95" display="https://aws.amazon.com/cognito/" xr:uid="{5631285D-2790-B940-99E8-7A2AFBF2A4F8}"/>
+    <hyperlink ref="C274" r:id="rId95" display="https://aws.amazon.com/cognito/" xr:uid="{5631285D-2790-B940-99E8-7A2AFBF2A4F8}"/>
     <hyperlink ref="C137" r:id="rId96" display="https://aws.amazon.com/comprehend/" xr:uid="{EF9B7DCD-AAB7-C840-B56B-6901E4208F3C}"/>
     <hyperlink ref="C138" r:id="rId97" display="https://aws.amazon.com/comprehend/medical/" xr:uid="{E755C2E6-BB69-1547-AEEA-159FA230C6E0}"/>
-    <hyperlink ref="C278" r:id="rId98" display="https://aws.amazon.com/detective/" xr:uid="{4F6306C8-7E6E-B543-8987-505512DF8B38}"/>
+    <hyperlink ref="C282" r:id="rId98" display="https://aws.amazon.com/detective/" xr:uid="{4F6306C8-7E6E-B543-8987-505512DF8B38}"/>
     <hyperlink ref="C143" r:id="rId99" display="https://aws.amazon.com/devops-guru/" xr:uid="{0DE3687A-6EED-D846-93EF-2FF3EDCA2FE7}"/>
     <hyperlink ref="C83" r:id="rId100" display="https://aws.amazon.com/documentdb/" xr:uid="{E9BE873B-93B3-744C-82A3-AE676C942786}"/>
     <hyperlink ref="C84" r:id="rId101" display="https://aws.amazon.com/dynamodb/" xr:uid="{667C0B17-E586-7843-9ABA-2156F328D1C2}"/>
     <hyperlink ref="C87" r:id="rId102" display="https://aws.amazon.com/elasticache/" xr:uid="{0D3B6893-EB9F-F441-97F2-EAE3A531E741}"/>
     <hyperlink ref="C297" r:id="rId103" display="https://aws.amazon.com/ebs/" xr:uid="{6475A1BA-F9EA-3643-A91C-960971815276}"/>
-    <hyperlink ref="C45" r:id="rId104" xr:uid="{F6BE2D25-6B4D-D545-BEF5-6353621F7D77}"/>
+    <hyperlink ref="C46" r:id="rId104" xr:uid="{F6BE2D25-6B4D-D545-BEF5-6353621F7D77}"/>
     <hyperlink ref="C59" r:id="rId105" display="https://aws.amazon.com/ecr/" xr:uid="{4DB8575D-FD4E-F24B-9A6D-4B237DEB4216}"/>
     <hyperlink ref="C60" r:id="rId106" display="https://aws.amazon.com/ecs/" xr:uid="{2A857716-DB7F-4D4C-9C3A-923E359FCE4B}"/>
     <hyperlink ref="C298" r:id="rId107" display="https://aws.amazon.com/efs/" xr:uid="{17293663-847A-2945-BEEE-DB5C14186604}"/>
@@ -11167,8 +11151,8 @@
     <hyperlink ref="C145" r:id="rId115" display="https://aws.amazon.com/forecast/" xr:uid="{1F07E3AD-D0E3-4442-9220-92E85E3DF861}"/>
     <hyperlink ref="C146" r:id="rId116" display="https://aws.amazon.com/fraud-detector/" xr:uid="{A16ABA87-0E9D-1749-BE3E-718E7599E24B}"/>
     <hyperlink ref="C121" r:id="rId117" display="https://aws.amazon.com/gamelift/" xr:uid="{ABE766D8-2E8B-B341-9103-F503839AC514}"/>
-    <hyperlink ref="C284" r:id="rId118" display="https://aws.amazon.com/guardduty/" xr:uid="{D1B6E14A-AD6C-E844-9AD0-215698F4E3BE}"/>
-    <hyperlink ref="C287" r:id="rId119" display="https://aws.amazon.com/inspector/" xr:uid="{176BE9A8-3FF5-874F-8EFA-6BB4665C2F33}"/>
+    <hyperlink ref="C286" r:id="rId118" display="https://aws.amazon.com/guardduty/" xr:uid="{D1B6E14A-AD6C-E844-9AD0-215698F4E3BE}"/>
+    <hyperlink ref="C288" r:id="rId119" display="https://aws.amazon.com/inspector/" xr:uid="{176BE9A8-3FF5-874F-8EFA-6BB4665C2F33}"/>
     <hyperlink ref="C88" r:id="rId120" display="https://aws.amazon.com/keyspaces/" xr:uid="{08537BC8-9E18-E341-B811-B357F4073FF5}"/>
     <hyperlink ref="C15" r:id="rId121" display="https://aws.amazon.com/kinesis/analytics/" xr:uid="{55091A39-96DB-9A41-B453-9AB88556B85B}"/>
     <hyperlink ref="C16" r:id="rId122" display="https://aws.amazon.com/kinesis/firehose/" xr:uid="{AB91BD64-7EBD-8A40-89D5-415AC999E5A7}"/>
@@ -11179,7 +11163,7 @@
     <hyperlink ref="C149" r:id="rId127" display="https://aws.amazon.com/lookout-for-vision/" xr:uid="{56891F15-488A-2D4F-957F-9C19DBC09E8C}"/>
     <hyperlink ref="C122" r:id="rId128" display="https://aws.amazon.com/lumberyard/" xr:uid="{0793FA7F-F861-E448-B351-2625AB793E29}"/>
     <hyperlink ref="C32" r:id="rId129" display="https://aws.amazon.com/amazon-mq/" xr:uid="{8F7E8190-F83B-7E45-9B55-465E1F7C79F3}"/>
-    <hyperlink ref="C289" r:id="rId130" display="https://aws.amazon.com/macie/" xr:uid="{0A9A9C7B-64FF-4944-8B73-82D7A54412E2}"/>
+    <hyperlink ref="C290" r:id="rId130" display="https://aws.amazon.com/macie/" xr:uid="{0A9A9C7B-64FF-4944-8B73-82D7A54412E2}"/>
     <hyperlink ref="C19" r:id="rId131" display="https://aws.amazon.com/msk/" xr:uid="{46024F01-6B35-0740-B92F-18BA0D596F3D}"/>
     <hyperlink ref="C31" r:id="rId132" display="https://aws.amazon.com/managed-workflows-for-apache-airflow/" xr:uid="{E7D50CE9-B395-AE40-B3BD-7B31072C139C}"/>
     <hyperlink ref="C90" r:id="rId133" display="https://aws.amazon.com/neptune/" xr:uid="{35EB7CA9-2F10-7E4E-9B05-D1C561AFFA79}"/>
@@ -11190,12 +11174,12 @@
     <hyperlink ref="C22" r:id="rId138" display="https://aws.amazon.com/redshift/" xr:uid="{BD068AB5-9542-BA4D-9D2D-3E01553833FF}"/>
     <hyperlink ref="C153" r:id="rId139" display="https://aws.amazon.com/rekognition/" xr:uid="{06B644B6-712E-EB4F-BDC1-2826A6E207A2}"/>
     <hyperlink ref="C93" r:id="rId140" display="https://aws.amazon.com/rds/" xr:uid="{52A384FE-5551-524F-8BE4-640C39EE59DB}"/>
-    <hyperlink ref="C263" r:id="rId141" display="https://aws.amazon.com/route53/" xr:uid="{2B9EF04D-DB6D-9948-8F0B-1F85D1FFA02C}"/>
+    <hyperlink ref="C264" r:id="rId141" display="https://aws.amazon.com/route53/" xr:uid="{2B9EF04D-DB6D-9948-8F0B-1F85D1FFA02C}"/>
     <hyperlink ref="C154" r:id="rId142" display="https://aws.amazon.com/sagemaker/" xr:uid="{FF819C8F-B472-6A4D-BF36-8803B10C8D16}"/>
     <hyperlink ref="C81" r:id="rId143" display="https://aws.amazon.com/ses/" xr:uid="{708BC6D8-3F72-374C-AB65-9002B2EB5C60}"/>
     <hyperlink ref="C33" r:id="rId144" display="https://aws.amazon.com/sns/" xr:uid="{2A7374BD-4C80-7C42-9E56-E3671DF3D17F}"/>
     <hyperlink ref="C34" r:id="rId145" display="https://aws.amazon.com/sqs/" xr:uid="{7EC87AB6-C5A3-0F4B-915C-BD9EF4201FD5}"/>
-    <hyperlink ref="C304" r:id="rId146" display="https://aws.amazon.com/s3/" xr:uid="{CD425C97-24D5-9747-8B23-DF9DD7A486F9}"/>
+    <hyperlink ref="C310" r:id="rId146" display="https://aws.amazon.com/s3/" xr:uid="{CD425C97-24D5-9747-8B23-DF9DD7A486F9}"/>
     <hyperlink ref="C35" r:id="rId147" display="https://aws.amazon.com/swf/" xr:uid="{631F304E-E46F-644E-8407-57836778A272}"/>
     <hyperlink ref="C123" r:id="rId148" display="https://aws.amazon.com/sumerian/" xr:uid="{1F8D41FC-B82F-8C44-A79F-AA91C3811E29}"/>
     <hyperlink ref="C168" r:id="rId149" display="https://aws.amazon.com/textract" xr:uid="{E50E8082-94C1-7947-963B-3A384A890F42}"/>
@@ -11203,14 +11187,14 @@
     <hyperlink ref="C169" r:id="rId151" display="https://aws.amazon.com/transcribe/" xr:uid="{7391FC88-BBA3-5846-9CA8-5612809D5D1E}"/>
     <hyperlink ref="C170" r:id="rId152" display="https://aws.amazon.com/transcribe/medical/" xr:uid="{5D3CF2D8-5264-E342-A8E8-E042131AE7AF}"/>
     <hyperlink ref="C171" r:id="rId153" display="https://aws.amazon.com/translate/" xr:uid="{D94B1850-F477-024B-8A15-72298FF44F81}"/>
-    <hyperlink ref="C266" r:id="rId154" display="https://aws.amazon.com/vpc/" xr:uid="{81704202-B35B-314F-9611-62D10520486C}"/>
+    <hyperlink ref="C262" r:id="rId154" display="https://aws.amazon.com/vpc/" xr:uid="{81704202-B35B-314F-9611-62D10520486C}"/>
     <hyperlink ref="C119" r:id="rId155" display="https://aws.amazon.com/worklink/" xr:uid="{A564F6A5-A25E-984E-AB0E-10859F299F79}"/>
     <hyperlink ref="C296" r:id="rId156" display="https://aws.amazon.com/cloudendure-disaster-recovery/" xr:uid="{19E2670B-B70B-2246-875A-A798E313AD4C}"/>
     <hyperlink ref="C238" r:id="rId157" display="https://aws.amazon.com/cloudendure-migration/" xr:uid="{3011454A-BA14-2640-A5B0-1665DE5015EB}"/>
     <hyperlink ref="C259" r:id="rId158" display="https://aws.amazon.com/elasticloadbalancing/" xr:uid="{48C41A56-7B49-954B-8607-BA52CE86305D}"/>
     <hyperlink ref="C124" r:id="rId159" display="https://aws.amazon.com/freertos/" xr:uid="{9A951967-4675-1546-8716-0568BF98D1CE}"/>
     <hyperlink ref="C53" r:id="rId160" display="https://aws.amazon.com/vmware/" xr:uid="{1D088AE8-27BE-C042-AB38-9D218A238493}"/>
-    <hyperlink ref="C48" r:id="rId161" display="https://aws.amazon.com/ec2/" xr:uid="{A67A7092-80C0-9A4E-A55B-97FA160377E8}"/>
+    <hyperlink ref="C44" r:id="rId161" display="https://aws.amazon.com/ec2/" xr:uid="{A67A7092-80C0-9A4E-A55B-97FA160377E8}"/>
     <hyperlink ref="C302" r:id="rId162" xr:uid="{9237F063-BA80-DC44-882A-D4F7F6FD5EE9}"/>
     <hyperlink ref="C111" r:id="rId163" xr:uid="{75CD952A-625F-DE4E-B2D6-41E51DC1F7E3}"/>
     <hyperlink ref="C37" r:id="rId164" xr:uid="{49E4FD14-55A4-2E46-8EFF-5EF1766DCF38}"/>
@@ -11226,7 +11210,7 @@
     <hyperlink ref="C56" r:id="rId174" xr:uid="{161791FF-9796-5D41-9399-C5CC0A52B777}"/>
     <hyperlink ref="C54" r:id="rId175" xr:uid="{005354BD-081E-9E46-8937-381CB8592473}"/>
     <hyperlink ref="C58" r:id="rId176" xr:uid="{1CFA07FC-268F-C84D-B8E8-D13B2E092826}"/>
-    <hyperlink ref="C185" r:id="rId177" xr:uid="{667DCA05-C10B-394B-ADBD-C91C39C8EFA9}"/>
+    <hyperlink ref="C190" r:id="rId177" xr:uid="{667DCA05-C10B-394B-ADBD-C91C39C8EFA9}"/>
     <hyperlink ref="C299" r:id="rId178" xr:uid="{19712BF9-B0E9-FC4A-855C-37C622207421}"/>
     <hyperlink ref="C101" r:id="rId179" xr:uid="{532F9FAB-7588-934A-BECA-94DB57B3EA86}"/>
     <hyperlink ref="C97" r:id="rId180" xr:uid="{03EA6A9E-9AED-E449-AEAE-E07C9D687ADF}"/>
@@ -11245,22 +11229,22 @@
     <hyperlink ref="C159" r:id="rId193" xr:uid="{534A3538-6476-C049-B1F4-C7F42A4A0CE2}"/>
     <hyperlink ref="C160" r:id="rId194" xr:uid="{AD37C4EC-6AA6-7445-886F-F12B10EC4962}"/>
     <hyperlink ref="C150" r:id="rId195" xr:uid="{32D673E8-4729-054A-941B-0538347DFE6B}"/>
-    <hyperlink ref="C194" r:id="rId196" display="AppConfig" xr:uid="{D7D5BCB4-B018-9449-8DE4-7BAC0B834A94}"/>
-    <hyperlink ref="C206" r:id="rId197" xr:uid="{6C997D60-3DAC-C54C-A365-6925F32D808B}"/>
-    <hyperlink ref="C195" r:id="rId198" xr:uid="{704C5761-85F7-8840-90D5-B9C68A5711E5}"/>
-    <hyperlink ref="C198" r:id="rId199" xr:uid="{0AE4E9A5-C51C-054C-8C1C-DFC93B7DE436}"/>
-    <hyperlink ref="C196" r:id="rId200" xr:uid="{D396B2A5-863A-0A4F-886E-AC0425111A74}"/>
-    <hyperlink ref="C204" r:id="rId201" xr:uid="{154E52D7-25A2-7B48-861E-130AEFF52429}"/>
-    <hyperlink ref="C202" r:id="rId202" xr:uid="{B55B16FC-FF18-784A-A974-098400EB5613}"/>
-    <hyperlink ref="C199" r:id="rId203" xr:uid="{2E1084D5-EB92-104E-9B36-C1C783851CEE}"/>
-    <hyperlink ref="C203" r:id="rId204" xr:uid="{CE1FE151-6237-2B48-BAA5-A0485476B07E}"/>
-    <hyperlink ref="C208" r:id="rId205" xr:uid="{8B651CA8-4121-954F-A1FD-E2ABDAE2711A}"/>
-    <hyperlink ref="C209" r:id="rId206" xr:uid="{73E53697-EA4F-5D44-BABF-E4DDE08A2949}"/>
-    <hyperlink ref="C210" r:id="rId207" xr:uid="{1F5BA02E-7700-F84C-896F-C3320A138F8C}"/>
-    <hyperlink ref="C207" r:id="rId208" xr:uid="{965DAB0C-1533-9C43-9931-A81FDFEE4801}"/>
-    <hyperlink ref="C200" r:id="rId209" xr:uid="{D7F493BC-3996-E14D-8B4E-AF698AF15CF3}"/>
-    <hyperlink ref="C205" r:id="rId210" xr:uid="{158C22B5-B282-0E45-819B-E1F6D3588EB5}"/>
-    <hyperlink ref="C201" r:id="rId211" xr:uid="{060EF427-1526-CB41-B8B7-D967487671FE}"/>
+    <hyperlink ref="C198" r:id="rId196" display="AppConfig" xr:uid="{D7D5BCB4-B018-9449-8DE4-7BAC0B834A94}"/>
+    <hyperlink ref="C181" r:id="rId197" xr:uid="{6C997D60-3DAC-C54C-A365-6925F32D808B}"/>
+    <hyperlink ref="C199" r:id="rId198" xr:uid="{704C5761-85F7-8840-90D5-B9C68A5711E5}"/>
+    <hyperlink ref="C202" r:id="rId199" xr:uid="{0AE4E9A5-C51C-054C-8C1C-DFC93B7DE436}"/>
+    <hyperlink ref="C200" r:id="rId200" xr:uid="{D396B2A5-863A-0A4F-886E-AC0425111A74}"/>
+    <hyperlink ref="C208" r:id="rId201" xr:uid="{154E52D7-25A2-7B48-861E-130AEFF52429}"/>
+    <hyperlink ref="C206" r:id="rId202" xr:uid="{B55B16FC-FF18-784A-A974-098400EB5613}"/>
+    <hyperlink ref="C203" r:id="rId203" xr:uid="{2E1084D5-EB92-104E-9B36-C1C783851CEE}"/>
+    <hyperlink ref="C207" r:id="rId204" xr:uid="{CE1FE151-6237-2B48-BAA5-A0485476B07E}"/>
+    <hyperlink ref="C210" r:id="rId205" xr:uid="{8B651CA8-4121-954F-A1FD-E2ABDAE2711A}"/>
+    <hyperlink ref="C211" r:id="rId206" xr:uid="{73E53697-EA4F-5D44-BABF-E4DDE08A2949}"/>
+    <hyperlink ref="C212" r:id="rId207" xr:uid="{1F5BA02E-7700-F84C-896F-C3320A138F8C}"/>
+    <hyperlink ref="C185" r:id="rId208" xr:uid="{965DAB0C-1533-9C43-9931-A81FDFEE4801}"/>
+    <hyperlink ref="C204" r:id="rId209" xr:uid="{D7F493BC-3996-E14D-8B4E-AF698AF15CF3}"/>
+    <hyperlink ref="C209" r:id="rId210" xr:uid="{158C22B5-B282-0E45-819B-E1F6D3588EB5}"/>
+    <hyperlink ref="C205" r:id="rId211" xr:uid="{060EF427-1526-CB41-B8B7-D967487671FE}"/>
     <hyperlink ref="C303" r:id="rId212" display="S3 Glacier" xr:uid="{69E65928-2461-9D41-874A-E2DD597C93F4}"/>
     <hyperlink ref="C161" r:id="rId213" xr:uid="{985BD89A-8A6D-3646-8654-90328345A506}"/>
     <hyperlink ref="C139" r:id="rId214" xr:uid="{590CE714-967E-A245-B8FF-739BCA3B026A}"/>
@@ -11283,10 +11267,10 @@
     <hyperlink ref="C134" r:id="rId231" xr:uid="{40FD60AC-B589-0B4B-AB36-1989E529CD39}"/>
     <hyperlink ref="C135" r:id="rId232" xr:uid="{56F27AA2-5183-E94B-ACC4-73885A21F096}"/>
     <hyperlink ref="C63" r:id="rId233" display="Managed Service for Prometheus" xr:uid="{15FBF981-0EC3-6343-ACAF-575D9CF01C72}"/>
-    <hyperlink ref="C280" r:id="rId234" display="Directory Service AD Connector" xr:uid="{CE8FDA92-983D-F241-9A3C-214FB6ED4987}"/>
-    <hyperlink ref="C282" r:id="rId235" display="Directory Service Simple AD" xr:uid="{BDF803C1-C55F-7B4E-B548-FB056C33B7F8}"/>
-    <hyperlink ref="C281" r:id="rId236" display="Directory Service Managed Microsoft AD" xr:uid="{A2682350-698B-164E-854C-B72B425BF114}"/>
-    <hyperlink ref="C186" r:id="rId237" xr:uid="{51AE8255-80F9-1246-AF04-CAD49D7BD8ED}"/>
+    <hyperlink ref="C275" r:id="rId234" display="Directory Service AD Connector" xr:uid="{CE8FDA92-983D-F241-9A3C-214FB6ED4987}"/>
+    <hyperlink ref="C277" r:id="rId235" display="Directory Service Simple AD" xr:uid="{BDF803C1-C55F-7B4E-B548-FB056C33B7F8}"/>
+    <hyperlink ref="C276" r:id="rId236" display="Directory Service Managed Microsoft AD" xr:uid="{A2682350-698B-164E-854C-B72B425BF114}"/>
+    <hyperlink ref="C191" r:id="rId237" xr:uid="{51AE8255-80F9-1246-AF04-CAD49D7BD8ED}"/>
     <hyperlink ref="C112" r:id="rId238" xr:uid="{F72E5D13-7F9C-A74A-B15B-60DA5CBC35BF}"/>
     <hyperlink ref="C147" r:id="rId239" xr:uid="{A021BA43-B246-CF41-8A4E-1E391CD06D94}"/>
     <hyperlink ref="C243" r:id="rId240" xr:uid="{66C98670-091A-A841-9473-A308D3D03C92}"/>
@@ -11312,7 +11296,7 @@
     <hyperlink ref="C227" r:id="rId260" xr:uid="{46CEB576-1991-6A4C-9819-8C32AAD5A3F1}"/>
     <hyperlink ref="C218" r:id="rId261" xr:uid="{98567FEC-ACF3-D64E-8831-23F0AF44FDF4}"/>
     <hyperlink ref="C115" r:id="rId262" xr:uid="{CBE97B7F-03A3-3B47-A836-0FDA32E32458}"/>
-    <hyperlink ref="C183" r:id="rId263" xr:uid="{98ADDE2A-ABDD-EB4A-8EBE-C43795A8F20B}"/>
+    <hyperlink ref="C188" r:id="rId263" xr:uid="{98ADDE2A-ABDD-EB4A-8EBE-C43795A8F20B}"/>
     <hyperlink ref="C55" r:id="rId264" xr:uid="{FE878825-B0CA-394C-95F4-6879C16270CC}"/>
     <hyperlink ref="C236" r:id="rId265" xr:uid="{8AF37CA7-BEF8-0E46-AFB3-906542482AD8}"/>
     <hyperlink ref="C57" r:id="rId266" xr:uid="{E1C253C0-789F-454D-B650-AD9042907E63}"/>
@@ -11322,11 +11306,11 @@
     <hyperlink ref="C233" r:id="rId270" xr:uid="{3B6EA2BE-9E87-CD43-BD86-90EF411A17C9}"/>
     <hyperlink ref="C234" r:id="rId271" xr:uid="{BE5AE3F2-6AF4-FB45-A4C7-58EE1FA83493}"/>
     <hyperlink ref="C235" r:id="rId272" xr:uid="{9F9A6701-301A-8946-8181-9D1074CEB3F6}"/>
-    <hyperlink ref="C310" r:id="rId273" display="Storage Gateway - Volume Gateway" xr:uid="{D2EC8952-5BC9-2B49-B394-D7BE012603FF}"/>
-    <hyperlink ref="C308" r:id="rId274" xr:uid="{1B5D263F-5321-B54A-BF60-2932447DCE26}"/>
-    <hyperlink ref="C306" r:id="rId275" display="Storage Gateway - FSx File Gateway" xr:uid="{2125FCAA-C46E-224B-8BE0-19D32D161491}"/>
-    <hyperlink ref="C307" r:id="rId276" display="Storage Gateway - S3 File Gateway" xr:uid="{96B9D02E-E08D-3E44-9C8E-08A2BE24E99A}"/>
-    <hyperlink ref="C309" r:id="rId277" display="Storage Gateway - Volume Gateway" xr:uid="{FFBC4DD5-5D45-9B42-A545-70A2598E87B0}"/>
+    <hyperlink ref="C309" r:id="rId273" display="Storage Gateway - Volume Gateway" xr:uid="{D2EC8952-5BC9-2B49-B394-D7BE012603FF}"/>
+    <hyperlink ref="C307" r:id="rId274" xr:uid="{1B5D263F-5321-B54A-BF60-2932447DCE26}"/>
+    <hyperlink ref="C305" r:id="rId275" display="Storage Gateway - FSx File Gateway" xr:uid="{2125FCAA-C46E-224B-8BE0-19D32D161491}"/>
+    <hyperlink ref="C306" r:id="rId276" display="Storage Gateway - S3 File Gateway" xr:uid="{96B9D02E-E08D-3E44-9C8E-08A2BE24E99A}"/>
+    <hyperlink ref="C308" r:id="rId277" display="Storage Gateway - Volume Gateway" xr:uid="{FFBC4DD5-5D45-9B42-A545-70A2598E87B0}"/>
     <hyperlink ref="C24" r:id="rId278" xr:uid="{F8A9F9A7-CC98-EC42-8596-0253E0A2BB97}"/>
     <hyperlink ref="C23" r:id="rId279" xr:uid="{8B655CFD-0968-7140-84E8-2070B49F002B}"/>
     <hyperlink ref="C27" r:id="rId280" xr:uid="{FD22D76A-0562-0640-85D0-C48AA580C483}"/>
@@ -11335,21 +11319,21 @@
     <hyperlink ref="C66" r:id="rId283" xr:uid="{1CA75B5D-40F7-EE46-91F1-45EA22AB9C53}"/>
     <hyperlink ref="C118" r:id="rId284" xr:uid="{5961D4D9-3072-2149-961B-0C10629539E7}"/>
     <hyperlink ref="C89" r:id="rId285" xr:uid="{863934C0-971A-AF48-A43D-B4B914AECC39}"/>
-    <hyperlink ref="C182" r:id="rId286" xr:uid="{3295CEB8-10D1-5A43-BEA9-DF5FD886C0AB}"/>
+    <hyperlink ref="C184" r:id="rId286" xr:uid="{3295CEB8-10D1-5A43-BEA9-DF5FD886C0AB}"/>
     <hyperlink ref="C295" r:id="rId287" xr:uid="{4F9FE344-D5EC-AC40-97FF-2F5F45F27D96}"/>
-    <hyperlink ref="C197" r:id="rId288" xr:uid="{AEDB8326-231C-C744-8B10-AF02B678D9B4}"/>
+    <hyperlink ref="C201" r:id="rId288" xr:uid="{AEDB8326-231C-C744-8B10-AF02B678D9B4}"/>
     <hyperlink ref="C14" r:id="rId289" xr:uid="{2E249962-989F-944F-B761-2BAA0EC7CAEC}"/>
     <hyperlink ref="C172" r:id="rId290" xr:uid="{DCE5737A-9A5B-DC4D-850F-450E2D238525}"/>
-    <hyperlink ref="C46" r:id="rId291" xr:uid="{FE31CE04-AE8C-B545-B85E-3E35079AA70A}"/>
+    <hyperlink ref="C47" r:id="rId291" xr:uid="{FE31CE04-AE8C-B545-B85E-3E35079AA70A}"/>
     <hyperlink ref="C255" r:id="rId292" xr:uid="{D321FD11-72A4-9F4D-857D-939FF8BB6E1B}"/>
-    <hyperlink ref="C264" r:id="rId293" xr:uid="{E997CB7A-902E-064D-B6FF-8470A806D5A0}"/>
+    <hyperlink ref="C265" r:id="rId293" xr:uid="{E997CB7A-902E-064D-B6FF-8470A806D5A0}"/>
     <hyperlink ref="C267" r:id="rId294" xr:uid="{0A132D4A-E971-7246-889D-EB0D9E3ED74A}"/>
-    <hyperlink ref="C285" r:id="rId295" xr:uid="{5D89926F-F8DE-F748-ADBE-85B87EFE8273}"/>
+    <hyperlink ref="C278" r:id="rId295" xr:uid="{5D89926F-F8DE-F748-ADBE-85B87EFE8273}"/>
     <hyperlink ref="C130" r:id="rId296" xr:uid="{2B14DC1E-31E9-E643-8322-E37BB77A61F2}"/>
     <hyperlink ref="C246" r:id="rId297" xr:uid="{09886B01-263E-164A-BB8E-628947483324}"/>
     <hyperlink ref="C247" r:id="rId298" xr:uid="{5F2F3CFC-7F4A-FD4D-941C-DED03BD1B5FC}"/>
     <hyperlink ref="C237" r:id="rId299" xr:uid="{7C8F3176-C207-894A-B174-4BEF8A9DAF7C}"/>
-    <hyperlink ref="C180" r:id="rId300" xr:uid="{E43F582E-778D-E840-BF2A-38A6E4E85D0B}"/>
+    <hyperlink ref="C182" r:id="rId300" xr:uid="{E43F582E-778D-E840-BF2A-38A6E4E85D0B}"/>
     <hyperlink ref="C98:C99" r:id="rId301" display="Cloud Development Kit (CDK)" xr:uid="{74EF9526-5AAF-4446-8604-03C2DD1F15BF}"/>
     <hyperlink ref="C98" r:id="rId302" xr:uid="{C3C5B093-C1E6-354A-B80D-C83A330D70CE}"/>
     <hyperlink ref="C99" r:id="rId303" xr:uid="{3EF40231-9DF0-E848-9274-0E658AE48B9A}"/>

</xml_diff>

<commit_message>
ml specialty official list
</commit_message>
<xml_diff>
--- a/aws-services-crib-sheet.xlsx
+++ b/aws-services-crib-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corbuno/WorkDocs/courses/aws-services-crib-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96EEEC7A-58AF-2B43-BD66-05B521199103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11426E8-07A2-E148-9AB8-CB8B63F56784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="500" windowWidth="27780" windowHeight="17500" xr2:uid="{8DC9DE24-CECC-4748-B90E-52259685D84E}"/>
   </bookViews>
@@ -1857,7 +1857,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M96" sqref="M96"/>
+      <selection pane="bottomLeft" activeCell="O303" sqref="O303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1961,7 +1961,9 @@
       </c>
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
+      <c r="O2" s="17">
+        <v>1</v>
+      </c>
       <c r="P2" s="17">
         <v>1</v>
       </c>
@@ -2021,7 +2023,9 @@
       </c>
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
+      <c r="O4" s="17">
+        <v>1</v>
+      </c>
       <c r="P4" s="17">
         <v>1</v>
       </c>
@@ -2102,7 +2106,9 @@
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
+      <c r="O7" s="17">
+        <v>1</v>
+      </c>
       <c r="P7" s="17">
         <v>1</v>
       </c>
@@ -2289,7 +2295,9 @@
       <c r="L14" s="17"/>
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
+      <c r="O14" s="17">
+        <v>1</v>
+      </c>
       <c r="P14" s="17">
         <v>1</v>
       </c>
@@ -2324,7 +2332,9 @@
       <c r="L15" s="17"/>
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
+      <c r="O15" s="17">
+        <v>1</v>
+      </c>
       <c r="P15" s="17">
         <v>1</v>
       </c>
@@ -2361,7 +2371,9 @@
       </c>
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
+      <c r="O16" s="17">
+        <v>1</v>
+      </c>
       <c r="P16" s="17">
         <v>1</v>
       </c>
@@ -2398,7 +2410,9 @@
       </c>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
+      <c r="O17" s="17">
+        <v>1</v>
+      </c>
       <c r="P17" s="17">
         <v>1</v>
       </c>
@@ -2557,7 +2571,9 @@
       </c>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
+      <c r="O22" s="17">
+        <v>1</v>
+      </c>
       <c r="P22" s="17">
         <v>1</v>
       </c>
@@ -2910,9 +2926,7 @@
       <c r="N33" s="17">
         <v>1</v>
       </c>
-      <c r="O33" s="17">
-        <v>1</v>
-      </c>
+      <c r="O33" s="17"/>
       <c r="P33" s="17">
         <v>1</v>
       </c>
@@ -2955,9 +2969,7 @@
       <c r="N34" s="17">
         <v>1</v>
       </c>
-      <c r="O34" s="17">
-        <v>1</v>
-      </c>
+      <c r="O34" s="17"/>
       <c r="P34" s="17">
         <v>1</v>
       </c>
@@ -3316,12 +3328,8 @@
         <v>1</v>
       </c>
       <c r="M46" s="17"/>
-      <c r="N46" s="17">
-        <v>1</v>
-      </c>
-      <c r="O46" s="17">
-        <v>1</v>
-      </c>
+      <c r="N46" s="17"/>
+      <c r="O46" s="17"/>
       <c r="P46" s="17">
         <v>1</v>
       </c>
@@ -3696,7 +3704,9 @@
       </c>
       <c r="M59" s="17"/>
       <c r="N59" s="17"/>
-      <c r="O59" s="17"/>
+      <c r="O59" s="17">
+        <v>1</v>
+      </c>
       <c r="P59" s="17"/>
       <c r="Q59" s="17"/>
     </row>
@@ -3731,7 +3741,9 @@
       </c>
       <c r="M60" s="17"/>
       <c r="N60" s="17"/>
-      <c r="O60" s="17"/>
+      <c r="O60" s="17">
+        <v>1</v>
+      </c>
       <c r="P60" s="17"/>
       <c r="Q60" s="17"/>
     </row>
@@ -3766,7 +3778,9 @@
       </c>
       <c r="M61" s="17"/>
       <c r="N61" s="17"/>
-      <c r="O61" s="17"/>
+      <c r="O61" s="17">
+        <v>1</v>
+      </c>
       <c r="P61" s="17"/>
       <c r="Q61" s="17"/>
     </row>
@@ -3801,7 +3815,9 @@
       </c>
       <c r="M62" s="17"/>
       <c r="N62" s="17"/>
-      <c r="O62" s="17"/>
+      <c r="O62" s="17">
+        <v>1</v>
+      </c>
       <c r="P62" s="17"/>
       <c r="Q62" s="17"/>
     </row>
@@ -4415,9 +4431,7 @@
       <c r="N84" s="17">
         <v>1</v>
       </c>
-      <c r="O84" s="17">
-        <v>1</v>
-      </c>
+      <c r="O84" s="17"/>
       <c r="P84" s="17">
         <v>1</v>
       </c>
@@ -5747,7 +5761,9 @@
       <c r="L132" s="17"/>
       <c r="M132" s="17"/>
       <c r="N132" s="17"/>
-      <c r="O132" s="17"/>
+      <c r="O132" s="17">
+        <v>1</v>
+      </c>
       <c r="P132" s="17"/>
       <c r="Q132" s="17"/>
     </row>
@@ -5847,9 +5863,7 @@
       <c r="L136" s="17"/>
       <c r="M136" s="17"/>
       <c r="N136" s="17"/>
-      <c r="O136" s="17">
-        <v>1</v>
-      </c>
+      <c r="O136" s="17"/>
       <c r="P136" s="17"/>
       <c r="Q136" s="17"/>
     </row>
@@ -5903,9 +5917,7 @@
       <c r="L138" s="17"/>
       <c r="M138" s="17"/>
       <c r="N138" s="17"/>
-      <c r="O138" s="17">
-        <v>1</v>
-      </c>
+      <c r="O138" s="17"/>
       <c r="P138" s="17"/>
       <c r="Q138" s="17"/>
     </row>
@@ -5982,7 +5994,9 @@
       <c r="L141" s="17"/>
       <c r="M141" s="17"/>
       <c r="N141" s="17"/>
-      <c r="O141" s="17"/>
+      <c r="O141" s="17">
+        <v>1</v>
+      </c>
       <c r="P141" s="17"/>
       <c r="Q141" s="17"/>
     </row>
@@ -6032,9 +6046,7 @@
       <c r="L143" s="17"/>
       <c r="M143" s="17"/>
       <c r="N143" s="17"/>
-      <c r="O143" s="17">
-        <v>1</v>
-      </c>
+      <c r="O143" s="17"/>
       <c r="P143" s="17"/>
       <c r="Q143" s="17"/>
     </row>
@@ -6059,9 +6071,7 @@
       <c r="L144" s="17"/>
       <c r="M144" s="17"/>
       <c r="N144" s="17"/>
-      <c r="O144" s="17">
-        <v>1</v>
-      </c>
+      <c r="O144" s="17"/>
       <c r="P144" s="17"/>
       <c r="Q144" s="17"/>
     </row>
@@ -6169,7 +6179,9 @@
       <c r="L148" s="17"/>
       <c r="M148" s="17"/>
       <c r="N148" s="17"/>
-      <c r="O148" s="17"/>
+      <c r="O148" s="17">
+        <v>1</v>
+      </c>
       <c r="P148" s="17"/>
       <c r="Q148" s="17"/>
     </row>
@@ -6244,9 +6256,7 @@
       <c r="L151" s="17"/>
       <c r="M151" s="17"/>
       <c r="N151" s="17"/>
-      <c r="O151" s="17">
-        <v>1</v>
-      </c>
+      <c r="O151" s="17"/>
       <c r="P151" s="17"/>
       <c r="Q151" s="17"/>
     </row>
@@ -6765,9 +6775,7 @@
       <c r="L170" s="17"/>
       <c r="M170" s="17"/>
       <c r="N170" s="17"/>
-      <c r="O170" s="17">
-        <v>1</v>
-      </c>
+      <c r="O170" s="17"/>
       <c r="P170" s="17"/>
       <c r="Q170" s="17"/>
     </row>
@@ -6852,9 +6860,7 @@
       <c r="L173" s="17"/>
       <c r="M173" s="17"/>
       <c r="N173" s="17"/>
-      <c r="O173" s="17">
-        <v>1</v>
-      </c>
+      <c r="O173" s="17"/>
       <c r="P173" s="17"/>
       <c r="Q173" s="17"/>
     </row>
@@ -6967,9 +6973,7 @@
       <c r="N176" s="17">
         <v>1</v>
       </c>
-      <c r="O176" s="17">
-        <v>1</v>
-      </c>
+      <c r="O176" s="17"/>
       <c r="P176" s="17">
         <v>1</v>
       </c>
@@ -9334,9 +9338,7 @@
       <c r="N259" s="17">
         <v>1</v>
       </c>
-      <c r="O259" s="17">
-        <v>1</v>
-      </c>
+      <c r="O259" s="17"/>
       <c r="P259" s="17">
         <v>1</v>
       </c>
@@ -10597,7 +10599,9 @@
       </c>
       <c r="M298" s="17"/>
       <c r="N298" s="17"/>
-      <c r="O298" s="17"/>
+      <c r="O298" s="17">
+        <v>1</v>
+      </c>
       <c r="P298" s="17"/>
       <c r="Q298" s="17"/>
     </row>
@@ -10653,7 +10657,9 @@
       <c r="L300" s="17"/>
       <c r="M300" s="17"/>
       <c r="N300" s="17"/>
-      <c r="O300" s="17"/>
+      <c r="O300" s="17">
+        <v>1</v>
+      </c>
       <c r="P300" s="17"/>
       <c r="Q300" s="17"/>
     </row>
@@ -10684,7 +10690,9 @@
       <c r="L301" s="17"/>
       <c r="M301" s="17"/>
       <c r="N301" s="17"/>
-      <c r="O301" s="17"/>
+      <c r="O301" s="17">
+        <v>1</v>
+      </c>
       <c r="P301" s="17"/>
       <c r="Q301" s="17"/>
     </row>
@@ -10721,9 +10729,7 @@
       <c r="N302" s="17">
         <v>1</v>
       </c>
-      <c r="O302" s="17">
-        <v>1</v>
-      </c>
+      <c r="O302" s="17"/>
       <c r="P302" s="17">
         <v>1</v>
       </c>
@@ -10764,9 +10770,7 @@
       <c r="N303" s="17">
         <v>1</v>
       </c>
-      <c r="O303" s="17">
-        <v>1</v>
-      </c>
+      <c r="O303" s="17"/>
       <c r="P303" s="17">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
DA specialty official list
</commit_message>
<xml_diff>
--- a/aws-services-crib-sheet.xlsx
+++ b/aws-services-crib-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corbuno/WorkDocs/courses/aws-services-crib-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11426E8-07A2-E148-9AB8-CB8B63F56784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57FEB2A-7349-B041-8AC6-DAC984BC8423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="500" windowWidth="27780" windowHeight="17500" xr2:uid="{8DC9DE24-CECC-4748-B90E-52259685D84E}"/>
   </bookViews>
@@ -1855,9 +1855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00D01EA-5C3E-F64B-8B7F-2EE6141A689A}">
   <dimension ref="A1:Q310"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O303" sqref="O303"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -6861,7 +6861,9 @@
       <c r="M173" s="17"/>
       <c r="N173" s="17"/>
       <c r="O173" s="17"/>
-      <c r="P173" s="17"/>
+      <c r="P173" s="17">
+        <v>1</v>
+      </c>
       <c r="Q173" s="17"/>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.2">
@@ -6935,7 +6937,9 @@
       <c r="O175" s="17">
         <v>1</v>
       </c>
-      <c r="P175" s="17"/>
+      <c r="P175" s="17">
+        <v>1</v>
+      </c>
       <c r="Q175" s="17"/>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.2">
@@ -8750,9 +8754,7 @@
       <c r="M240" s="17"/>
       <c r="N240" s="17"/>
       <c r="O240" s="17"/>
-      <c r="P240" s="17">
-        <v>1</v>
-      </c>
+      <c r="P240" s="17"/>
       <c r="Q240" s="17"/>
     </row>
     <row r="241" spans="1:17" x14ac:dyDescent="0.2">
@@ -10565,7 +10567,9 @@
       <c r="M297" s="17"/>
       <c r="N297" s="17"/>
       <c r="O297" s="17"/>
-      <c r="P297" s="17"/>
+      <c r="P297" s="17">
+        <v>1</v>
+      </c>
       <c r="Q297" s="17"/>
     </row>
     <row r="298" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
DB specialty official list
</commit_message>
<xml_diff>
--- a/aws-services-crib-sheet.xlsx
+++ b/aws-services-crib-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corbuno/WorkDocs/courses/aws-services-crib-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57FEB2A-7349-B041-8AC6-DAC984BC8423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72163789-390B-F749-8049-F540D9D83253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="500" windowWidth="27780" windowHeight="17500" xr2:uid="{8DC9DE24-CECC-4748-B90E-52259685D84E}"/>
   </bookViews>
@@ -1857,7 +1857,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -3221,10 +3221,10 @@
         <v>24</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>136</v>
+        <v>11</v>
       </c>
       <c r="D44" s="45"/>
       <c r="E44" s="45"/>
@@ -3235,43 +3235,29 @@
       <c r="H44" s="17">
         <v>1</v>
       </c>
-      <c r="I44" s="17">
-        <v>1</v>
-      </c>
-      <c r="J44" s="17">
-        <v>1</v>
-      </c>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
       <c r="K44" s="17">
         <v>1</v>
       </c>
-      <c r="L44" s="17">
-        <v>1</v>
-      </c>
-      <c r="M44" s="17">
-        <v>1</v>
-      </c>
-      <c r="N44" s="17">
-        <v>1</v>
-      </c>
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
       <c r="O44" s="17">
         <v>1</v>
       </c>
-      <c r="P44" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q44" s="17">
-        <v>1</v>
-      </c>
+      <c r="P44" s="17"/>
+      <c r="Q44" s="17"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>11</v>
+        <v>176</v>
       </c>
       <c r="D45" s="45"/>
       <c r="E45" s="45"/>
@@ -3282,18 +3268,24 @@
       <c r="H45" s="17">
         <v>1</v>
       </c>
-      <c r="I45" s="17"/>
-      <c r="J45" s="17"/>
+      <c r="I45" s="17">
+        <v>1</v>
+      </c>
+      <c r="J45" s="17">
+        <v>1</v>
+      </c>
       <c r="K45" s="17">
         <v>1</v>
       </c>
-      <c r="L45" s="17"/>
+      <c r="L45" s="17">
+        <v>1</v>
+      </c>
       <c r="M45" s="17"/>
       <c r="N45" s="17"/>
-      <c r="O45" s="17">
-        <v>1</v>
-      </c>
-      <c r="P45" s="17"/>
+      <c r="O45" s="17"/>
+      <c r="P45" s="17">
+        <v>1</v>
+      </c>
       <c r="Q45" s="17"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
@@ -3304,59 +3296,51 @@
         <v>51</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>176</v>
+        <v>335</v>
       </c>
       <c r="D46" s="45"/>
       <c r="E46" s="45"/>
       <c r="F46" s="45"/>
-      <c r="G46" s="17">
-        <v>1</v>
-      </c>
-      <c r="H46" s="17">
-        <v>1</v>
-      </c>
-      <c r="I46" s="17">
-        <v>1</v>
-      </c>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
       <c r="J46" s="17">
         <v>1</v>
       </c>
-      <c r="K46" s="17">
-        <v>1</v>
-      </c>
-      <c r="L46" s="17">
-        <v>1</v>
-      </c>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
       <c r="O46" s="17"/>
-      <c r="P46" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q46" s="17">
-        <v>1</v>
-      </c>
+      <c r="P46" s="17"/>
+      <c r="Q46" s="17"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>335</v>
+        <v>95</v>
       </c>
       <c r="D47" s="45"/>
       <c r="E47" s="45"/>
       <c r="F47" s="45"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
-      <c r="J47" s="17">
-        <v>1</v>
-      </c>
-      <c r="K47" s="17"/>
+      <c r="G47" s="17">
+        <v>1</v>
+      </c>
+      <c r="H47" s="17">
+        <v>1</v>
+      </c>
+      <c r="I47" s="17">
+        <v>1</v>
+      </c>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17">
+        <v>1</v>
+      </c>
       <c r="L47" s="17"/>
       <c r="M47" s="17"/>
       <c r="N47" s="17"/>
@@ -3369,10 +3353,10 @@
         <v>24</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>95</v>
+        <v>136</v>
       </c>
       <c r="D48" s="45"/>
       <c r="E48" s="45"/>
@@ -3386,16 +3370,30 @@
       <c r="I48" s="17">
         <v>1</v>
       </c>
-      <c r="J48" s="17"/>
+      <c r="J48" s="17">
+        <v>1</v>
+      </c>
       <c r="K48" s="17">
         <v>1</v>
       </c>
-      <c r="L48" s="17"/>
-      <c r="M48" s="17"/>
-      <c r="N48" s="17"/>
-      <c r="O48" s="17"/>
-      <c r="P48" s="17"/>
-      <c r="Q48" s="17"/>
+      <c r="L48" s="17">
+        <v>1</v>
+      </c>
+      <c r="M48" s="17">
+        <v>1</v>
+      </c>
+      <c r="N48" s="17">
+        <v>1</v>
+      </c>
+      <c r="O48" s="17">
+        <v>1</v>
+      </c>
+      <c r="P48" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q48" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
@@ -3745,7 +3743,9 @@
         <v>1</v>
       </c>
       <c r="P60" s="17"/>
-      <c r="Q60" s="17"/>
+      <c r="Q60" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
@@ -3782,7 +3782,9 @@
         <v>1</v>
       </c>
       <c r="P61" s="17"/>
-      <c r="Q61" s="17"/>
+      <c r="Q61" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="14" t="s">
@@ -3948,7 +3950,9 @@
       <c r="N67" s="17"/>
       <c r="O67" s="17"/>
       <c r="P67" s="17"/>
-      <c r="Q67" s="17"/>
+      <c r="Q67" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" s="11" t="s">
@@ -4010,7 +4014,9 @@
       <c r="N69" s="17"/>
       <c r="O69" s="17"/>
       <c r="P69" s="17"/>
-      <c r="Q69" s="17"/>
+      <c r="Q69" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" s="11" t="s">
@@ -4468,7 +4474,9 @@
       <c r="N85" s="17"/>
       <c r="O85" s="17"/>
       <c r="P85" s="17"/>
-      <c r="Q85" s="17"/>
+      <c r="Q85" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="86" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A86" s="19" t="s">
@@ -4557,9 +4565,7 @@
       <c r="N88" s="17"/>
       <c r="O88" s="17"/>
       <c r="P88" s="17"/>
-      <c r="Q88" s="17">
-        <v>1</v>
-      </c>
+      <c r="Q88" s="17"/>
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A89" s="19" t="s">
@@ -5174,7 +5180,9 @@
       <c r="N109" s="17"/>
       <c r="O109" s="17"/>
       <c r="P109" s="17"/>
-      <c r="Q109" s="17"/>
+      <c r="Q109" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="110" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A110" s="19" t="s">
@@ -6864,7 +6872,9 @@
       <c r="P173" s="17">
         <v>1</v>
       </c>
-      <c r="Q173" s="17"/>
+      <c r="Q173" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A174" s="29" t="s">
@@ -6907,7 +6917,7 @@
         <v>6</v>
       </c>
       <c r="C175" s="31" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D175" s="45"/>
       <c r="E175" s="45"/>
@@ -6930,17 +6940,17 @@
       <c r="L175" s="17">
         <v>1</v>
       </c>
-      <c r="M175" s="17">
-        <v>1</v>
-      </c>
-      <c r="N175" s="17"/>
-      <c r="O175" s="17">
-        <v>1</v>
-      </c>
+      <c r="M175" s="17"/>
+      <c r="N175" s="17">
+        <v>1</v>
+      </c>
+      <c r="O175" s="17"/>
       <c r="P175" s="17">
         <v>1</v>
       </c>
-      <c r="Q175" s="17"/>
+      <c r="Q175" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="176" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A176" s="29" t="s">
@@ -6950,7 +6960,7 @@
         <v>6</v>
       </c>
       <c r="C176" s="31" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D176" s="45"/>
       <c r="E176" s="45"/>
@@ -6973,11 +6983,13 @@
       <c r="L176" s="17">
         <v>1</v>
       </c>
-      <c r="M176" s="17"/>
-      <c r="N176" s="17">
-        <v>1</v>
-      </c>
-      <c r="O176" s="17"/>
+      <c r="M176" s="17">
+        <v>1</v>
+      </c>
+      <c r="N176" s="17"/>
+      <c r="O176" s="17">
+        <v>1</v>
+      </c>
       <c r="P176" s="17">
         <v>1</v>
       </c>
@@ -7040,30 +7052,20 @@
         <v>6</v>
       </c>
       <c r="C178" s="31" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="D178" s="45"/>
       <c r="E178" s="45"/>
       <c r="F178" s="45"/>
-      <c r="G178" s="17">
-        <v>1</v>
-      </c>
-      <c r="H178" s="17">
-        <v>1</v>
-      </c>
+      <c r="G178" s="17"/>
+      <c r="H178" s="17"/>
       <c r="I178" s="17"/>
       <c r="J178" s="17">
         <v>1</v>
       </c>
-      <c r="K178" s="17">
-        <v>1</v>
-      </c>
-      <c r="L178" s="17">
-        <v>1</v>
-      </c>
-      <c r="M178" s="17">
-        <v>1</v>
-      </c>
+      <c r="K178" s="17"/>
+      <c r="L178" s="17"/>
+      <c r="M178" s="17"/>
       <c r="N178" s="17"/>
       <c r="O178" s="17"/>
       <c r="P178" s="17"/>
@@ -7077,7 +7079,7 @@
         <v>6</v>
       </c>
       <c r="C179" s="31" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D179" s="45"/>
       <c r="E179" s="45"/>
@@ -7104,7 +7106,9 @@
       <c r="N179" s="17"/>
       <c r="O179" s="17"/>
       <c r="P179" s="17"/>
-      <c r="Q179" s="17"/>
+      <c r="Q179" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="180" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A180" s="29" t="s">
@@ -7114,7 +7118,7 @@
         <v>6</v>
       </c>
       <c r="C180" s="31" t="s">
-        <v>90</v>
+        <v>344</v>
       </c>
       <c r="D180" s="45"/>
       <c r="E180" s="45"/>
@@ -7122,9 +7126,7 @@
       <c r="G180" s="17"/>
       <c r="H180" s="17"/>
       <c r="I180" s="17"/>
-      <c r="J180" s="17">
-        <v>1</v>
-      </c>
+      <c r="J180" s="17"/>
       <c r="K180" s="17"/>
       <c r="L180" s="17"/>
       <c r="M180" s="17"/>
@@ -7141,17 +7143,13 @@
         <v>6</v>
       </c>
       <c r="C181" s="31" t="s">
-        <v>252</v>
+        <v>91</v>
       </c>
       <c r="D181" s="45"/>
       <c r="E181" s="45"/>
       <c r="F181" s="45"/>
-      <c r="G181" s="17">
-        <v>1</v>
-      </c>
-      <c r="H181" s="17">
-        <v>1</v>
-      </c>
+      <c r="G181" s="17"/>
+      <c r="H181" s="17"/>
       <c r="I181" s="17"/>
       <c r="J181" s="17">
         <v>1</v>
@@ -7159,12 +7157,8 @@
       <c r="K181" s="17">
         <v>1</v>
       </c>
-      <c r="L181" s="17">
-        <v>1</v>
-      </c>
-      <c r="M181" s="17">
-        <v>1</v>
-      </c>
+      <c r="L181" s="17"/>
+      <c r="M181" s="17"/>
       <c r="N181" s="17"/>
       <c r="O181" s="17"/>
       <c r="P181" s="17"/>
@@ -7175,10 +7169,10 @@
         <v>33</v>
       </c>
       <c r="B182" s="30" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C182" s="31" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="D182" s="45"/>
       <c r="E182" s="45"/>
@@ -7203,7 +7197,7 @@
         <v>6</v>
       </c>
       <c r="C183" s="31" t="s">
-        <v>91</v>
+        <v>302</v>
       </c>
       <c r="D183" s="45"/>
       <c r="E183" s="45"/>
@@ -7211,12 +7205,8 @@
       <c r="G183" s="17"/>
       <c r="H183" s="17"/>
       <c r="I183" s="17"/>
-      <c r="J183" s="17">
-        <v>1</v>
-      </c>
-      <c r="K183" s="17">
-        <v>1</v>
-      </c>
+      <c r="J183" s="17"/>
+      <c r="K183" s="17"/>
       <c r="L183" s="17"/>
       <c r="M183" s="17"/>
       <c r="N183" s="17"/>
@@ -7229,19 +7219,25 @@
         <v>33</v>
       </c>
       <c r="B184" s="30" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C184" s="31" t="s">
-        <v>329</v>
+        <v>111</v>
       </c>
       <c r="D184" s="45"/>
       <c r="E184" s="45"/>
       <c r="F184" s="45"/>
-      <c r="G184" s="17"/>
+      <c r="G184" s="17">
+        <v>1</v>
+      </c>
       <c r="H184" s="17"/>
       <c r="I184" s="17"/>
-      <c r="J184" s="17"/>
-      <c r="K184" s="17"/>
+      <c r="J184" s="17">
+        <v>1</v>
+      </c>
+      <c r="K184" s="17">
+        <v>1</v>
+      </c>
       <c r="L184" s="17"/>
       <c r="M184" s="17"/>
       <c r="N184" s="17"/>
@@ -7254,10 +7250,10 @@
         <v>33</v>
       </c>
       <c r="B185" s="30" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C185" s="31" t="s">
-        <v>262</v>
+        <v>220</v>
       </c>
       <c r="D185" s="45"/>
       <c r="E185" s="45"/>
@@ -7267,12 +7263,8 @@
       <c r="I185" s="17"/>
       <c r="J185" s="17"/>
       <c r="K185" s="17"/>
-      <c r="L185" s="17">
-        <v>1</v>
-      </c>
-      <c r="M185" s="17">
-        <v>1</v>
-      </c>
+      <c r="L185" s="17"/>
+      <c r="M185" s="17"/>
       <c r="N185" s="17"/>
       <c r="O185" s="17"/>
       <c r="P185" s="17"/>
@@ -7286,7 +7278,7 @@
         <v>6</v>
       </c>
       <c r="C186" s="31" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="D186" s="45"/>
       <c r="E186" s="45"/>
@@ -7294,22 +7286,14 @@
       <c r="G186" s="17">
         <v>1</v>
       </c>
-      <c r="H186" s="17">
-        <v>1</v>
-      </c>
+      <c r="H186" s="17"/>
       <c r="I186" s="17"/>
       <c r="J186" s="17">
         <v>1</v>
       </c>
-      <c r="K186" s="17">
-        <v>1</v>
-      </c>
-      <c r="L186" s="17">
-        <v>1</v>
-      </c>
-      <c r="M186" s="17">
-        <v>1</v>
-      </c>
+      <c r="K186" s="17"/>
+      <c r="L186" s="17"/>
+      <c r="M186" s="17"/>
       <c r="N186" s="17"/>
       <c r="O186" s="17"/>
       <c r="P186" s="17"/>
@@ -7323,14 +7307,12 @@
         <v>6</v>
       </c>
       <c r="C187" s="31" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D187" s="45"/>
       <c r="E187" s="45"/>
       <c r="F187" s="45"/>
-      <c r="G187" s="17">
-        <v>1</v>
-      </c>
+      <c r="G187" s="17"/>
       <c r="H187" s="17">
         <v>1</v>
       </c>
@@ -7338,20 +7320,14 @@
       <c r="J187" s="17">
         <v>1</v>
       </c>
-      <c r="K187" s="17">
-        <v>1</v>
-      </c>
+      <c r="K187" s="17"/>
       <c r="L187" s="17">
         <v>1</v>
       </c>
-      <c r="M187" s="17">
-        <v>1</v>
-      </c>
+      <c r="M187" s="17"/>
       <c r="N187" s="17"/>
       <c r="O187" s="17"/>
-      <c r="P187" s="17">
-        <v>1</v>
-      </c>
+      <c r="P187" s="17"/>
       <c r="Q187" s="17"/>
     </row>
     <row r="188" spans="1:17" x14ac:dyDescent="0.2">
@@ -7362,17 +7338,23 @@
         <v>6</v>
       </c>
       <c r="C188" s="31" t="s">
-        <v>302</v>
+        <v>115</v>
       </c>
       <c r="D188" s="45"/>
       <c r="E188" s="45"/>
       <c r="F188" s="45"/>
       <c r="G188" s="17"/>
-      <c r="H188" s="17"/>
+      <c r="H188" s="17">
+        <v>1</v>
+      </c>
       <c r="I188" s="17"/>
-      <c r="J188" s="17"/>
+      <c r="J188" s="17">
+        <v>1</v>
+      </c>
       <c r="K188" s="17"/>
-      <c r="L188" s="17"/>
+      <c r="L188" s="17">
+        <v>1</v>
+      </c>
       <c r="M188" s="17"/>
       <c r="N188" s="17"/>
       <c r="O188" s="17"/>
@@ -7387,23 +7369,23 @@
         <v>6</v>
       </c>
       <c r="C189" s="31" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D189" s="45"/>
       <c r="E189" s="45"/>
       <c r="F189" s="45"/>
-      <c r="G189" s="17">
-        <v>1</v>
-      </c>
-      <c r="H189" s="17"/>
+      <c r="G189" s="17"/>
+      <c r="H189" s="17">
+        <v>1</v>
+      </c>
       <c r="I189" s="17"/>
       <c r="J189" s="17">
         <v>1</v>
       </c>
-      <c r="K189" s="17">
-        <v>1</v>
-      </c>
-      <c r="L189" s="17"/>
+      <c r="K189" s="17"/>
+      <c r="L189" s="17">
+        <v>1</v>
+      </c>
       <c r="M189" s="17"/>
       <c r="N189" s="17"/>
       <c r="O189" s="17"/>
@@ -7415,21 +7397,33 @@
         <v>33</v>
       </c>
       <c r="B190" s="30" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C190" s="31" t="s">
-        <v>220</v>
+        <v>38</v>
       </c>
       <c r="D190" s="45"/>
       <c r="E190" s="45"/>
       <c r="F190" s="45"/>
-      <c r="G190" s="17"/>
-      <c r="H190" s="17"/>
+      <c r="G190" s="17">
+        <v>1</v>
+      </c>
+      <c r="H190" s="17">
+        <v>1</v>
+      </c>
       <c r="I190" s="17"/>
-      <c r="J190" s="17"/>
-      <c r="K190" s="17"/>
-      <c r="L190" s="17"/>
-      <c r="M190" s="17"/>
+      <c r="J190" s="17">
+        <v>1</v>
+      </c>
+      <c r="K190" s="17">
+        <v>1</v>
+      </c>
+      <c r="L190" s="17">
+        <v>1</v>
+      </c>
+      <c r="M190" s="17">
+        <v>1</v>
+      </c>
       <c r="N190" s="17"/>
       <c r="O190" s="17"/>
       <c r="P190" s="17"/>
@@ -7443,7 +7437,7 @@
         <v>6</v>
       </c>
       <c r="C191" s="31" t="s">
-        <v>273</v>
+        <v>116</v>
       </c>
       <c r="D191" s="45"/>
       <c r="E191" s="45"/>
@@ -7472,7 +7466,7 @@
         <v>6</v>
       </c>
       <c r="C192" s="31" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D192" s="45"/>
       <c r="E192" s="45"/>
@@ -7482,13 +7476,11 @@
         <v>1</v>
       </c>
       <c r="I192" s="17"/>
-      <c r="J192" s="17">
-        <v>1</v>
-      </c>
-      <c r="K192" s="17"/>
-      <c r="L192" s="17">
-        <v>1</v>
-      </c>
+      <c r="J192" s="17"/>
+      <c r="K192" s="17">
+        <v>1</v>
+      </c>
+      <c r="L192" s="17"/>
       <c r="M192" s="17"/>
       <c r="N192" s="17"/>
       <c r="O192" s="17"/>
@@ -7503,23 +7495,21 @@
         <v>6</v>
       </c>
       <c r="C193" s="31" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="D193" s="45"/>
       <c r="E193" s="45"/>
       <c r="F193" s="45"/>
       <c r="G193" s="17"/>
-      <c r="H193" s="17">
-        <v>1</v>
-      </c>
+      <c r="H193" s="17"/>
       <c r="I193" s="17"/>
       <c r="J193" s="17">
         <v>1</v>
       </c>
-      <c r="K193" s="17"/>
-      <c r="L193" s="17">
-        <v>1</v>
-      </c>
+      <c r="K193" s="17">
+        <v>1</v>
+      </c>
+      <c r="L193" s="17"/>
       <c r="M193" s="17"/>
       <c r="N193" s="17"/>
       <c r="O193" s="17"/>
@@ -7534,15 +7524,13 @@
         <v>6</v>
       </c>
       <c r="C194" s="31" t="s">
-        <v>113</v>
+        <v>247</v>
       </c>
       <c r="D194" s="45"/>
       <c r="E194" s="45"/>
       <c r="F194" s="45"/>
       <c r="G194" s="17"/>
-      <c r="H194" s="17">
-        <v>1</v>
-      </c>
+      <c r="H194" s="17"/>
       <c r="I194" s="17"/>
       <c r="J194" s="17">
         <v>1</v>
@@ -7565,21 +7553,21 @@
         <v>6</v>
       </c>
       <c r="C195" s="31" t="s">
-        <v>116</v>
+        <v>251</v>
       </c>
       <c r="D195" s="45"/>
       <c r="E195" s="45"/>
       <c r="F195" s="45"/>
-      <c r="G195" s="17">
-        <v>1</v>
-      </c>
+      <c r="G195" s="17"/>
       <c r="H195" s="17"/>
       <c r="I195" s="17"/>
       <c r="J195" s="17">
         <v>1</v>
       </c>
       <c r="K195" s="17"/>
-      <c r="L195" s="17"/>
+      <c r="L195" s="17">
+        <v>1</v>
+      </c>
       <c r="M195" s="17"/>
       <c r="N195" s="17"/>
       <c r="O195" s="17"/>
@@ -7594,21 +7582,21 @@
         <v>6</v>
       </c>
       <c r="C196" s="31" t="s">
-        <v>117</v>
+        <v>254</v>
       </c>
       <c r="D196" s="45"/>
       <c r="E196" s="45"/>
       <c r="F196" s="45"/>
       <c r="G196" s="17"/>
-      <c r="H196" s="17">
-        <v>1</v>
-      </c>
+      <c r="H196" s="17"/>
       <c r="I196" s="17"/>
-      <c r="J196" s="17"/>
-      <c r="K196" s="17">
-        <v>1</v>
-      </c>
-      <c r="L196" s="17"/>
+      <c r="J196" s="17">
+        <v>1</v>
+      </c>
+      <c r="K196" s="17"/>
+      <c r="L196" s="17">
+        <v>1</v>
+      </c>
       <c r="M196" s="17"/>
       <c r="N196" s="17"/>
       <c r="O196" s="17"/>
@@ -7623,7 +7611,7 @@
         <v>6</v>
       </c>
       <c r="C197" s="31" t="s">
-        <v>122</v>
+        <v>331</v>
       </c>
       <c r="D197" s="45"/>
       <c r="E197" s="45"/>
@@ -7631,12 +7619,8 @@
       <c r="G197" s="17"/>
       <c r="H197" s="17"/>
       <c r="I197" s="17"/>
-      <c r="J197" s="17">
-        <v>1</v>
-      </c>
-      <c r="K197" s="17">
-        <v>1</v>
-      </c>
+      <c r="J197" s="17"/>
+      <c r="K197" s="17"/>
       <c r="L197" s="17"/>
       <c r="M197" s="17"/>
       <c r="N197" s="17"/>
@@ -7652,7 +7636,7 @@
         <v>6</v>
       </c>
       <c r="C198" s="31" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="D198" s="45"/>
       <c r="E198" s="45"/>
@@ -7660,9 +7644,7 @@
       <c r="G198" s="17"/>
       <c r="H198" s="17"/>
       <c r="I198" s="17"/>
-      <c r="J198" s="17">
-        <v>1</v>
-      </c>
+      <c r="J198" s="17"/>
       <c r="K198" s="17"/>
       <c r="L198" s="17">
         <v>1</v>
@@ -7681,7 +7663,7 @@
         <v>6</v>
       </c>
       <c r="C199" s="31" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="D199" s="45"/>
       <c r="E199" s="45"/>
@@ -7689,9 +7671,7 @@
       <c r="G199" s="17"/>
       <c r="H199" s="17"/>
       <c r="I199" s="17"/>
-      <c r="J199" s="17">
-        <v>1</v>
-      </c>
+      <c r="J199" s="17"/>
       <c r="K199" s="17"/>
       <c r="L199" s="17">
         <v>1</v>
@@ -7710,7 +7690,7 @@
         <v>6</v>
       </c>
       <c r="C200" s="31" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="D200" s="45"/>
       <c r="E200" s="45"/>
@@ -7718,9 +7698,7 @@
       <c r="G200" s="17"/>
       <c r="H200" s="17"/>
       <c r="I200" s="17"/>
-      <c r="J200" s="17">
-        <v>1</v>
-      </c>
+      <c r="J200" s="17"/>
       <c r="K200" s="17"/>
       <c r="L200" s="17">
         <v>1</v>
@@ -7739,7 +7717,7 @@
         <v>6</v>
       </c>
       <c r="C201" s="31" t="s">
-        <v>331</v>
+        <v>249</v>
       </c>
       <c r="D201" s="45"/>
       <c r="E201" s="45"/>
@@ -7749,7 +7727,9 @@
       <c r="I201" s="17"/>
       <c r="J201" s="17"/>
       <c r="K201" s="17"/>
-      <c r="L201" s="17"/>
+      <c r="L201" s="17">
+        <v>1</v>
+      </c>
       <c r="M201" s="17"/>
       <c r="N201" s="17"/>
       <c r="O201" s="17"/>
@@ -7764,7 +7744,7 @@
         <v>6</v>
       </c>
       <c r="C202" s="31" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="D202" s="45"/>
       <c r="E202" s="45"/>
@@ -7791,7 +7771,7 @@
         <v>6</v>
       </c>
       <c r="C203" s="31" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D203" s="45"/>
       <c r="E203" s="45"/>
@@ -7818,7 +7798,7 @@
         <v>6</v>
       </c>
       <c r="C204" s="31" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="D204" s="45"/>
       <c r="E204" s="45"/>
@@ -7845,11 +7825,11 @@
         <v>6</v>
       </c>
       <c r="C205" s="31" t="s">
-        <v>249</v>
-      </c>
-      <c r="D205" s="45"/>
-      <c r="E205" s="45"/>
-      <c r="F205" s="45"/>
+        <v>250</v>
+      </c>
+      <c r="D205" s="47"/>
+      <c r="E205" s="47"/>
+      <c r="F205" s="47"/>
       <c r="G205" s="17"/>
       <c r="H205" s="17"/>
       <c r="I205" s="17"/>
@@ -7872,20 +7852,30 @@
         <v>6</v>
       </c>
       <c r="C206" s="31" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D206" s="45"/>
       <c r="E206" s="45"/>
       <c r="F206" s="45"/>
-      <c r="G206" s="17"/>
-      <c r="H206" s="17"/>
+      <c r="G206" s="17">
+        <v>1</v>
+      </c>
+      <c r="H206" s="17">
+        <v>1</v>
+      </c>
       <c r="I206" s="17"/>
-      <c r="J206" s="17"/>
-      <c r="K206" s="17"/>
+      <c r="J206" s="17">
+        <v>1</v>
+      </c>
+      <c r="K206" s="17">
+        <v>1</v>
+      </c>
       <c r="L206" s="17">
         <v>1</v>
       </c>
-      <c r="M206" s="17"/>
+      <c r="M206" s="17">
+        <v>1</v>
+      </c>
       <c r="N206" s="17"/>
       <c r="O206" s="17"/>
       <c r="P206" s="17"/>
@@ -7899,7 +7889,7 @@
         <v>6</v>
       </c>
       <c r="C207" s="31" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="D207" s="45"/>
       <c r="E207" s="45"/>
@@ -7912,7 +7902,9 @@
       <c r="L207" s="17">
         <v>1</v>
       </c>
-      <c r="M207" s="17"/>
+      <c r="M207" s="17">
+        <v>1</v>
+      </c>
       <c r="N207" s="17"/>
       <c r="O207" s="17"/>
       <c r="P207" s="17"/>
@@ -7926,7 +7918,7 @@
         <v>6</v>
       </c>
       <c r="C208" s="31" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="D208" s="45"/>
       <c r="E208" s="45"/>
@@ -7953,11 +7945,11 @@
         <v>6</v>
       </c>
       <c r="C209" s="31" t="s">
-        <v>250</v>
-      </c>
-      <c r="D209" s="47"/>
-      <c r="E209" s="47"/>
-      <c r="F209" s="47"/>
+        <v>259</v>
+      </c>
+      <c r="D209" s="45"/>
+      <c r="E209" s="45"/>
+      <c r="F209" s="45"/>
       <c r="G209" s="17"/>
       <c r="H209" s="17"/>
       <c r="I209" s="17"/>
@@ -7980,7 +7972,7 @@
         <v>6</v>
       </c>
       <c r="C210" s="31" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D210" s="45"/>
       <c r="E210" s="45"/>
@@ -8007,20 +7999,30 @@
         <v>6</v>
       </c>
       <c r="C211" s="31" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="D211" s="45"/>
       <c r="E211" s="45"/>
       <c r="F211" s="45"/>
-      <c r="G211" s="17"/>
-      <c r="H211" s="17"/>
+      <c r="G211" s="17">
+        <v>1</v>
+      </c>
+      <c r="H211" s="17">
+        <v>1</v>
+      </c>
       <c r="I211" s="17"/>
-      <c r="J211" s="17"/>
-      <c r="K211" s="17"/>
+      <c r="J211" s="17">
+        <v>1</v>
+      </c>
+      <c r="K211" s="17">
+        <v>1</v>
+      </c>
       <c r="L211" s="17">
         <v>1</v>
       </c>
-      <c r="M211" s="17"/>
+      <c r="M211" s="17">
+        <v>1</v>
+      </c>
       <c r="N211" s="17"/>
       <c r="O211" s="17"/>
       <c r="P211" s="17"/>
@@ -8034,24 +8036,38 @@
         <v>6</v>
       </c>
       <c r="C212" s="31" t="s">
-        <v>261</v>
+        <v>127</v>
       </c>
       <c r="D212" s="45"/>
       <c r="E212" s="45"/>
       <c r="F212" s="45"/>
-      <c r="G212" s="17"/>
-      <c r="H212" s="17"/>
+      <c r="G212" s="17">
+        <v>1</v>
+      </c>
+      <c r="H212" s="17">
+        <v>1</v>
+      </c>
       <c r="I212" s="17"/>
-      <c r="J212" s="17"/>
-      <c r="K212" s="17"/>
+      <c r="J212" s="17">
+        <v>1</v>
+      </c>
+      <c r="K212" s="17">
+        <v>1</v>
+      </c>
       <c r="L212" s="17">
         <v>1</v>
       </c>
-      <c r="M212" s="17"/>
+      <c r="M212" s="17">
+        <v>1</v>
+      </c>
       <c r="N212" s="17"/>
       <c r="O212" s="17"/>
-      <c r="P212" s="17"/>
-      <c r="Q212" s="17"/>
+      <c r="P212" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q212" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="213" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A213" s="29" t="s">
@@ -8823,7 +8839,9 @@
       <c r="P242" s="17">
         <v>1</v>
       </c>
-      <c r="Q242" s="17"/>
+      <c r="Q242" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="243" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A243" s="22" t="s">
@@ -9020,7 +9038,9 @@
       <c r="P249" s="17">
         <v>1</v>
       </c>
-      <c r="Q249" s="17"/>
+      <c r="Q249" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="250" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A250" s="22" t="s">
@@ -9047,7 +9067,9 @@
       <c r="N250" s="17"/>
       <c r="O250" s="17"/>
       <c r="P250" s="17"/>
-      <c r="Q250" s="17"/>
+      <c r="Q250" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="251" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A251" s="22" t="s">
@@ -9076,7 +9098,9 @@
       <c r="N251" s="17"/>
       <c r="O251" s="17"/>
       <c r="P251" s="17"/>
-      <c r="Q251" s="17"/>
+      <c r="Q251" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="252" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A252" s="22" t="s">
@@ -9305,7 +9329,9 @@
       <c r="P258" s="17">
         <v>1</v>
       </c>
-      <c r="Q258" s="17"/>
+      <c r="Q258" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="259" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A259" s="33" t="s">
@@ -9356,20 +9382,24 @@
         <v>6</v>
       </c>
       <c r="C260" s="35" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D260" s="45"/>
       <c r="E260" s="45"/>
       <c r="F260" s="45"/>
       <c r="G260" s="17"/>
-      <c r="H260" s="17"/>
+      <c r="H260" s="17">
+        <v>1</v>
+      </c>
       <c r="I260" s="17"/>
-      <c r="J260" s="17"/>
-      <c r="K260" s="17"/>
+      <c r="J260" s="17">
+        <v>1</v>
+      </c>
+      <c r="K260" s="17">
+        <v>1</v>
+      </c>
       <c r="L260" s="17"/>
-      <c r="M260" s="17">
-        <v>1</v>
-      </c>
+      <c r="M260" s="17"/>
       <c r="N260" s="17">
         <v>1</v>
       </c>
@@ -9385,24 +9415,20 @@
         <v>6</v>
       </c>
       <c r="C261" s="35" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="D261" s="45"/>
       <c r="E261" s="45"/>
       <c r="F261" s="45"/>
       <c r="G261" s="17"/>
-      <c r="H261" s="17">
-        <v>1</v>
-      </c>
+      <c r="H261" s="17"/>
       <c r="I261" s="17"/>
-      <c r="J261" s="17">
-        <v>1</v>
-      </c>
-      <c r="K261" s="17">
-        <v>1</v>
-      </c>
+      <c r="J261" s="17"/>
+      <c r="K261" s="17"/>
       <c r="L261" s="17"/>
-      <c r="M261" s="17"/>
+      <c r="M261" s="17">
+        <v>1</v>
+      </c>
       <c r="N261" s="17">
         <v>1</v>
       </c>
@@ -9415,110 +9441,92 @@
         <v>169</v>
       </c>
       <c r="B262" s="34" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C262" s="35" t="s">
-        <v>161</v>
+        <v>40</v>
       </c>
       <c r="D262" s="45"/>
       <c r="E262" s="45"/>
       <c r="F262" s="45"/>
-      <c r="G262" s="17">
-        <v>1</v>
-      </c>
-      <c r="H262" s="17">
-        <v>1</v>
-      </c>
-      <c r="I262" s="17">
-        <v>1</v>
-      </c>
-      <c r="J262" s="17">
-        <v>1</v>
-      </c>
+      <c r="G262" s="17"/>
+      <c r="H262" s="17"/>
+      <c r="I262" s="17"/>
+      <c r="J262" s="17"/>
       <c r="K262" s="17">
         <v>1</v>
       </c>
-      <c r="L262" s="17">
-        <v>1</v>
-      </c>
-      <c r="M262" s="17">
-        <v>1</v>
-      </c>
+      <c r="L262" s="17"/>
+      <c r="M262" s="17"/>
       <c r="N262" s="17">
         <v>1</v>
       </c>
-      <c r="O262" s="17">
-        <v>1</v>
-      </c>
-      <c r="P262" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q262" s="17">
-        <v>1</v>
-      </c>
+      <c r="O262" s="17"/>
+      <c r="P262" s="17"/>
+      <c r="Q262" s="17"/>
     </row>
     <row r="263" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A263" s="33" t="s">
         <v>169</v>
       </c>
       <c r="B263" s="34" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C263" s="35" t="s">
-        <v>40</v>
+        <v>154</v>
       </c>
       <c r="D263" s="45"/>
       <c r="E263" s="45"/>
       <c r="F263" s="45"/>
-      <c r="G263" s="17"/>
-      <c r="H263" s="17"/>
+      <c r="G263" s="17">
+        <v>1</v>
+      </c>
+      <c r="H263" s="17">
+        <v>1</v>
+      </c>
       <c r="I263" s="17"/>
-      <c r="J263" s="17"/>
+      <c r="J263" s="17">
+        <v>1</v>
+      </c>
       <c r="K263" s="17">
         <v>1</v>
       </c>
-      <c r="L263" s="17"/>
+      <c r="L263" s="17">
+        <v>1</v>
+      </c>
       <c r="M263" s="17"/>
       <c r="N263" s="17">
         <v>1</v>
       </c>
       <c r="O263" s="17"/>
       <c r="P263" s="17"/>
-      <c r="Q263" s="17"/>
+      <c r="Q263" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="264" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A264" s="33" t="s">
         <v>169</v>
       </c>
       <c r="B264" s="34" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C264" s="35" t="s">
-        <v>154</v>
+        <v>337</v>
       </c>
       <c r="D264" s="45"/>
       <c r="E264" s="45"/>
       <c r="F264" s="45"/>
-      <c r="G264" s="17">
-        <v>1</v>
-      </c>
-      <c r="H264" s="17">
-        <v>1</v>
-      </c>
+      <c r="G264" s="17"/>
+      <c r="H264" s="17"/>
       <c r="I264" s="17"/>
-      <c r="J264" s="17">
-        <v>1</v>
-      </c>
-      <c r="K264" s="17">
-        <v>1</v>
-      </c>
+      <c r="J264" s="17"/>
+      <c r="K264" s="17"/>
       <c r="L264" s="17">
         <v>1</v>
       </c>
       <c r="M264" s="17"/>
-      <c r="N264" s="17">
-        <v>1</v>
-      </c>
+      <c r="N264" s="17"/>
       <c r="O264" s="17"/>
       <c r="P264" s="17"/>
       <c r="Q264" s="17"/>
@@ -9531,21 +9539,29 @@
         <v>6</v>
       </c>
       <c r="C265" s="35" t="s">
-        <v>337</v>
+        <v>126</v>
       </c>
       <c r="D265" s="45"/>
       <c r="E265" s="45"/>
       <c r="F265" s="45"/>
       <c r="G265" s="17"/>
-      <c r="H265" s="17"/>
+      <c r="H265" s="17">
+        <v>1</v>
+      </c>
       <c r="I265" s="17"/>
-      <c r="J265" s="17"/>
-      <c r="K265" s="17"/>
+      <c r="J265" s="17">
+        <v>1</v>
+      </c>
+      <c r="K265" s="17">
+        <v>1</v>
+      </c>
       <c r="L265" s="17">
         <v>1</v>
       </c>
       <c r="M265" s="17"/>
-      <c r="N265" s="17"/>
+      <c r="N265" s="17">
+        <v>1</v>
+      </c>
       <c r="O265" s="17"/>
       <c r="P265" s="17"/>
       <c r="Q265" s="17"/>
@@ -9555,19 +9571,23 @@
         <v>169</v>
       </c>
       <c r="B266" s="34" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C266" s="35" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="D266" s="45"/>
       <c r="E266" s="45"/>
       <c r="F266" s="45"/>
-      <c r="G266" s="17"/>
+      <c r="G266" s="17">
+        <v>1</v>
+      </c>
       <c r="H266" s="17">
         <v>1</v>
       </c>
-      <c r="I266" s="17"/>
+      <c r="I266" s="17">
+        <v>1</v>
+      </c>
       <c r="J266" s="17">
         <v>1</v>
       </c>
@@ -9577,13 +9597,21 @@
       <c r="L266" s="17">
         <v>1</v>
       </c>
-      <c r="M266" s="17"/>
+      <c r="M266" s="17">
+        <v>1</v>
+      </c>
       <c r="N266" s="17">
         <v>1</v>
       </c>
-      <c r="O266" s="17"/>
-      <c r="P266" s="17"/>
-      <c r="Q266" s="17"/>
+      <c r="O266" s="17">
+        <v>1</v>
+      </c>
+      <c r="P266" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q266" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="267" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A267" s="33" t="s">
@@ -9756,10 +9784,10 @@
         <v>43</v>
       </c>
       <c r="B273" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C273" s="39" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="D273" s="45"/>
       <c r="E273" s="45"/>
@@ -9770,7 +9798,9 @@
       <c r="J273" s="17"/>
       <c r="K273" s="17"/>
       <c r="L273" s="17"/>
-      <c r="M273" s="17"/>
+      <c r="M273" s="17">
+        <v>1</v>
+      </c>
       <c r="N273" s="17"/>
       <c r="O273" s="17"/>
       <c r="P273" s="17"/>
@@ -9781,10 +9811,10 @@
         <v>43</v>
       </c>
       <c r="B274" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C274" s="39" t="s">
-        <v>59</v>
+        <v>225</v>
       </c>
       <c r="D274" s="45"/>
       <c r="E274" s="45"/>
@@ -9795,15 +9825,17 @@
       <c r="H274" s="17">
         <v>1</v>
       </c>
-      <c r="I274" s="17">
-        <v>1</v>
-      </c>
-      <c r="J274" s="17"/>
+      <c r="I274" s="17"/>
+      <c r="J274" s="17">
+        <v>1</v>
+      </c>
       <c r="K274" s="17">
         <v>1</v>
       </c>
       <c r="L274" s="17"/>
-      <c r="M274" s="17"/>
+      <c r="M274" s="17">
+        <v>1</v>
+      </c>
       <c r="N274" s="17"/>
       <c r="O274" s="17"/>
       <c r="P274" s="17">
@@ -9816,23 +9848,19 @@
         <v>43</v>
       </c>
       <c r="B275" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C275" s="39" t="s">
-        <v>271</v>
+        <v>131</v>
       </c>
       <c r="D275" s="45"/>
       <c r="E275" s="45"/>
       <c r="F275" s="45"/>
       <c r="G275" s="17"/>
-      <c r="H275" s="17">
-        <v>1</v>
-      </c>
+      <c r="H275" s="17"/>
       <c r="I275" s="17"/>
       <c r="J275" s="17"/>
-      <c r="K275" s="17">
-        <v>1</v>
-      </c>
+      <c r="K275" s="17"/>
       <c r="L275" s="17"/>
       <c r="M275" s="17"/>
       <c r="N275" s="17"/>
@@ -9848,45 +9876,55 @@
         <v>6</v>
       </c>
       <c r="C276" s="39" t="s">
-        <v>270</v>
+        <v>16</v>
       </c>
       <c r="D276" s="45"/>
       <c r="E276" s="45"/>
       <c r="F276" s="45"/>
-      <c r="G276" s="17"/>
+      <c r="G276" s="17">
+        <v>1</v>
+      </c>
       <c r="H276" s="17">
         <v>1</v>
       </c>
       <c r="I276" s="17"/>
       <c r="J276" s="17"/>
-      <c r="K276" s="17">
-        <v>1</v>
-      </c>
+      <c r="K276" s="17"/>
       <c r="L276" s="17"/>
-      <c r="M276" s="17"/>
+      <c r="M276" s="17">
+        <v>1</v>
+      </c>
       <c r="N276" s="17"/>
       <c r="O276" s="17"/>
-      <c r="P276" s="17"/>
-      <c r="Q276" s="17"/>
+      <c r="P276" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q276" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="277" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A277" s="37" t="s">
         <v>43</v>
       </c>
       <c r="B277" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C277" s="39" t="s">
-        <v>272</v>
+        <v>59</v>
       </c>
       <c r="D277" s="45"/>
       <c r="E277" s="45"/>
       <c r="F277" s="45"/>
-      <c r="G277" s="17"/>
+      <c r="G277" s="17">
+        <v>1</v>
+      </c>
       <c r="H277" s="17">
         <v>1</v>
       </c>
-      <c r="I277" s="17"/>
+      <c r="I277" s="17">
+        <v>1</v>
+      </c>
       <c r="J277" s="17"/>
       <c r="K277" s="17">
         <v>1</v>
@@ -9895,7 +9933,9 @@
       <c r="M277" s="17"/>
       <c r="N277" s="17"/>
       <c r="O277" s="17"/>
-      <c r="P277" s="17"/>
+      <c r="P277" s="17">
+        <v>1</v>
+      </c>
       <c r="Q277" s="17"/>
     </row>
     <row r="278" spans="1:17" x14ac:dyDescent="0.2">
@@ -9903,15 +9943,17 @@
         <v>43</v>
       </c>
       <c r="B278" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C278" s="39" t="s">
-        <v>339</v>
+        <v>61</v>
       </c>
       <c r="D278" s="45"/>
       <c r="E278" s="45"/>
       <c r="F278" s="45"/>
-      <c r="G278" s="17"/>
+      <c r="G278" s="17">
+        <v>1</v>
+      </c>
       <c r="H278" s="17"/>
       <c r="I278" s="17"/>
       <c r="J278" s="17">
@@ -9919,7 +9961,9 @@
       </c>
       <c r="K278" s="17"/>
       <c r="L278" s="17"/>
-      <c r="M278" s="17"/>
+      <c r="M278" s="17">
+        <v>1</v>
+      </c>
       <c r="N278" s="17"/>
       <c r="O278" s="17"/>
       <c r="P278" s="17"/>
@@ -9933,16 +9977,22 @@
         <v>6</v>
       </c>
       <c r="C279" s="39" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="D279" s="45"/>
       <c r="E279" s="45"/>
       <c r="F279" s="45"/>
       <c r="G279" s="17"/>
-      <c r="H279" s="17"/>
+      <c r="H279" s="17">
+        <v>1</v>
+      </c>
       <c r="I279" s="17"/>
-      <c r="J279" s="17"/>
-      <c r="K279" s="17"/>
+      <c r="J279" s="17">
+        <v>1</v>
+      </c>
+      <c r="K279" s="17">
+        <v>1</v>
+      </c>
       <c r="L279" s="17"/>
       <c r="M279" s="17">
         <v>1</v>
@@ -9950,7 +10000,9 @@
       <c r="N279" s="17"/>
       <c r="O279" s="17"/>
       <c r="P279" s="17"/>
-      <c r="Q279" s="17"/>
+      <c r="Q279" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="280" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A280" s="37" t="s">
@@ -9960,33 +10012,25 @@
         <v>6</v>
       </c>
       <c r="C280" s="39" t="s">
-        <v>225</v>
+        <v>271</v>
       </c>
       <c r="D280" s="45"/>
       <c r="E280" s="45"/>
       <c r="F280" s="45"/>
-      <c r="G280" s="17">
-        <v>1</v>
-      </c>
+      <c r="G280" s="17"/>
       <c r="H280" s="17">
         <v>1</v>
       </c>
       <c r="I280" s="17"/>
-      <c r="J280" s="17">
-        <v>1</v>
-      </c>
+      <c r="J280" s="17"/>
       <c r="K280" s="17">
         <v>1</v>
       </c>
       <c r="L280" s="17"/>
-      <c r="M280" s="17">
-        <v>1</v>
-      </c>
+      <c r="M280" s="17"/>
       <c r="N280" s="17"/>
       <c r="O280" s="17"/>
-      <c r="P280" s="17">
-        <v>1</v>
-      </c>
+      <c r="P280" s="17"/>
       <c r="Q280" s="17"/>
     </row>
     <row r="281" spans="1:17" x14ac:dyDescent="0.2">
@@ -9997,29 +10041,25 @@
         <v>6</v>
       </c>
       <c r="C281" s="39" t="s">
-        <v>16</v>
+        <v>270</v>
       </c>
       <c r="D281" s="45"/>
       <c r="E281" s="45"/>
       <c r="F281" s="45"/>
-      <c r="G281" s="17">
-        <v>1</v>
-      </c>
+      <c r="G281" s="17"/>
       <c r="H281" s="17">
         <v>1</v>
       </c>
       <c r="I281" s="17"/>
       <c r="J281" s="17"/>
-      <c r="K281" s="17"/>
+      <c r="K281" s="17">
+        <v>1</v>
+      </c>
       <c r="L281" s="17"/>
-      <c r="M281" s="17">
-        <v>1</v>
-      </c>
+      <c r="M281" s="17"/>
       <c r="N281" s="17"/>
       <c r="O281" s="17"/>
-      <c r="P281" s="17">
-        <v>1</v>
-      </c>
+      <c r="P281" s="17"/>
       <c r="Q281" s="17"/>
     </row>
     <row r="282" spans="1:17" x14ac:dyDescent="0.2">
@@ -10027,27 +10067,25 @@
         <v>43</v>
       </c>
       <c r="B282" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C282" s="39" t="s">
-        <v>61</v>
+        <v>272</v>
       </c>
       <c r="D282" s="45"/>
       <c r="E282" s="45"/>
       <c r="F282" s="45"/>
-      <c r="G282" s="17">
-        <v>1</v>
-      </c>
-      <c r="H282" s="17"/>
+      <c r="G282" s="17"/>
+      <c r="H282" s="17">
+        <v>1</v>
+      </c>
       <c r="I282" s="17"/>
-      <c r="J282" s="17">
-        <v>1</v>
-      </c>
-      <c r="K282" s="17"/>
+      <c r="J282" s="17"/>
+      <c r="K282" s="17">
+        <v>1</v>
+      </c>
       <c r="L282" s="17"/>
-      <c r="M282" s="17">
-        <v>1</v>
-      </c>
+      <c r="M282" s="17"/>
       <c r="N282" s="17"/>
       <c r="O282" s="17"/>
       <c r="P282" s="17"/>
@@ -10061,22 +10099,18 @@
         <v>6</v>
       </c>
       <c r="C283" s="39" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D283" s="45"/>
       <c r="E283" s="45"/>
       <c r="F283" s="45"/>
       <c r="G283" s="17"/>
-      <c r="H283" s="17">
-        <v>1</v>
-      </c>
+      <c r="H283" s="17"/>
       <c r="I283" s="17"/>
       <c r="J283" s="17">
         <v>1</v>
       </c>
-      <c r="K283" s="17">
-        <v>1</v>
-      </c>
+      <c r="K283" s="17"/>
       <c r="L283" s="17"/>
       <c r="M283" s="17">
         <v>1</v>
@@ -10091,22 +10125,30 @@
         <v>43</v>
       </c>
       <c r="B284" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C284" s="39" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="D284" s="45"/>
       <c r="E284" s="45"/>
       <c r="F284" s="45"/>
-      <c r="G284" s="17"/>
-      <c r="H284" s="17"/>
+      <c r="G284" s="17">
+        <v>1</v>
+      </c>
+      <c r="H284" s="17">
+        <v>1</v>
+      </c>
       <c r="I284" s="17"/>
       <c r="J284" s="17">
         <v>1</v>
       </c>
-      <c r="K284" s="17"/>
-      <c r="L284" s="17"/>
+      <c r="K284" s="17">
+        <v>1</v>
+      </c>
+      <c r="L284" s="17">
+        <v>1</v>
+      </c>
       <c r="M284" s="17">
         <v>1</v>
       </c>
@@ -10123,33 +10165,23 @@
         <v>6</v>
       </c>
       <c r="C285" s="39" t="s">
-        <v>118</v>
+        <v>339</v>
       </c>
       <c r="D285" s="45"/>
       <c r="E285" s="45"/>
       <c r="F285" s="45"/>
-      <c r="G285" s="17">
-        <v>1</v>
-      </c>
-      <c r="H285" s="17">
-        <v>1</v>
-      </c>
+      <c r="G285" s="17"/>
+      <c r="H285" s="17"/>
       <c r="I285" s="17"/>
       <c r="J285" s="17">
         <v>1</v>
       </c>
-      <c r="K285" s="17">
-        <v>1</v>
-      </c>
-      <c r="L285" s="17">
-        <v>1</v>
-      </c>
+      <c r="K285" s="17"/>
+      <c r="L285" s="17"/>
       <c r="M285" s="17"/>
       <c r="N285" s="17"/>
       <c r="O285" s="17"/>
-      <c r="P285" s="17">
-        <v>1</v>
-      </c>
+      <c r="P285" s="17"/>
       <c r="Q285" s="17"/>
     </row>
     <row r="286" spans="1:17" x14ac:dyDescent="0.2">
@@ -10157,10 +10189,10 @@
         <v>43</v>
       </c>
       <c r="B286" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C286" s="39" t="s">
-        <v>66</v>
+        <v>102</v>
       </c>
       <c r="D286" s="45"/>
       <c r="E286" s="45"/>
@@ -10171,7 +10203,9 @@
       <c r="H286" s="17">
         <v>1</v>
       </c>
-      <c r="I286" s="17"/>
+      <c r="I286" s="17">
+        <v>1</v>
+      </c>
       <c r="J286" s="17">
         <v>1</v>
       </c>
@@ -10184,20 +10218,28 @@
       <c r="M286" s="17">
         <v>1</v>
       </c>
-      <c r="N286" s="17"/>
-      <c r="O286" s="17"/>
-      <c r="P286" s="17"/>
-      <c r="Q286" s="17"/>
+      <c r="N286" s="17">
+        <v>1</v>
+      </c>
+      <c r="O286" s="17">
+        <v>1</v>
+      </c>
+      <c r="P286" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q286" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="287" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A287" s="37" t="s">
         <v>43</v>
       </c>
       <c r="B287" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C287" s="39" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="D287" s="45"/>
       <c r="E287" s="45"/>
@@ -10208,9 +10250,7 @@
       <c r="H287" s="17">
         <v>1</v>
       </c>
-      <c r="I287" s="17">
-        <v>1</v>
-      </c>
+      <c r="I287" s="17"/>
       <c r="J287" s="17">
         <v>1</v>
       </c>
@@ -10223,28 +10263,20 @@
       <c r="M287" s="17">
         <v>1</v>
       </c>
-      <c r="N287" s="17">
-        <v>1</v>
-      </c>
-      <c r="O287" s="17">
-        <v>1</v>
-      </c>
-      <c r="P287" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q287" s="17">
-        <v>1</v>
-      </c>
+      <c r="N287" s="17"/>
+      <c r="O287" s="17"/>
+      <c r="P287" s="17"/>
+      <c r="Q287" s="17"/>
     </row>
     <row r="288" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A288" s="37" t="s">
         <v>43</v>
       </c>
       <c r="B288" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C288" s="39" t="s">
-        <v>67</v>
+        <v>312</v>
       </c>
       <c r="D288" s="45"/>
       <c r="E288" s="45"/>
@@ -10255,7 +10287,9 @@
       <c r="H288" s="17">
         <v>1</v>
       </c>
-      <c r="I288" s="17"/>
+      <c r="I288" s="17">
+        <v>1</v>
+      </c>
       <c r="J288" s="17">
         <v>1</v>
       </c>
@@ -10270,18 +10304,22 @@
       </c>
       <c r="N288" s="17"/>
       <c r="O288" s="17"/>
-      <c r="P288" s="17"/>
-      <c r="Q288" s="17"/>
+      <c r="P288" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q288" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="289" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A289" s="37" t="s">
         <v>43</v>
       </c>
       <c r="B289" s="38" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C289" s="39" t="s">
-        <v>312</v>
+        <v>71</v>
       </c>
       <c r="D289" s="45"/>
       <c r="E289" s="45"/>
@@ -10292,18 +10330,12 @@
       <c r="H289" s="17">
         <v>1</v>
       </c>
-      <c r="I289" s="17">
-        <v>1</v>
-      </c>
-      <c r="J289" s="17">
-        <v>1</v>
-      </c>
+      <c r="I289" s="17"/>
+      <c r="J289" s="17"/>
       <c r="K289" s="17">
         <v>1</v>
       </c>
-      <c r="L289" s="17">
-        <v>1</v>
-      </c>
+      <c r="L289" s="17"/>
       <c r="M289" s="17">
         <v>1</v>
       </c>
@@ -10319,10 +10351,10 @@
         <v>43</v>
       </c>
       <c r="B290" s="38" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C290" s="39" t="s">
-        <v>71</v>
+        <v>118</v>
       </c>
       <c r="D290" s="45"/>
       <c r="E290" s="45"/>
@@ -10334,20 +10366,24 @@
         <v>1</v>
       </c>
       <c r="I290" s="17"/>
-      <c r="J290" s="17"/>
+      <c r="J290" s="17">
+        <v>1</v>
+      </c>
       <c r="K290" s="17">
         <v>1</v>
       </c>
-      <c r="L290" s="17"/>
-      <c r="M290" s="17">
-        <v>1</v>
-      </c>
+      <c r="L290" s="17">
+        <v>1</v>
+      </c>
+      <c r="M290" s="17"/>
       <c r="N290" s="17"/>
       <c r="O290" s="17"/>
       <c r="P290" s="17">
         <v>1</v>
       </c>
-      <c r="Q290" s="17"/>
+      <c r="Q290" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="291" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A291" s="37" t="s">
@@ -10570,7 +10606,9 @@
       <c r="P297" s="17">
         <v>1</v>
       </c>
-      <c r="Q297" s="17"/>
+      <c r="Q297" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="298" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A298" s="11" t="s">
@@ -10787,10 +10825,10 @@
         <v>47</v>
       </c>
       <c r="B304" s="12" t="s">
-        <v>6</v>
+        <v>51</v>
       </c>
       <c r="C304" s="13" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="D304" s="45"/>
       <c r="E304" s="45"/>
@@ -10801,7 +10839,9 @@
       <c r="H304" s="17">
         <v>1</v>
       </c>
-      <c r="I304" s="17"/>
+      <c r="I304" s="17">
+        <v>1</v>
+      </c>
       <c r="J304" s="17">
         <v>1</v>
       </c>
@@ -10811,13 +10851,21 @@
       <c r="L304" s="17">
         <v>1</v>
       </c>
-      <c r="M304" s="17"/>
+      <c r="M304" s="17">
+        <v>1</v>
+      </c>
       <c r="N304" s="17">
         <v>1</v>
       </c>
-      <c r="O304" s="17"/>
-      <c r="P304" s="17"/>
-      <c r="Q304" s="17"/>
+      <c r="O304" s="17">
+        <v>1</v>
+      </c>
+      <c r="P304" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q304" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="305" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A305" s="11" t="s">
@@ -10827,17 +10875,21 @@
         <v>6</v>
       </c>
       <c r="C305" s="56" t="s">
-        <v>315</v>
+        <v>124</v>
       </c>
       <c r="D305" s="48"/>
       <c r="E305" s="48"/>
       <c r="F305" s="48"/>
-      <c r="G305" s="54"/>
+      <c r="G305" s="54">
+        <v>1</v>
+      </c>
       <c r="H305" s="54">
         <v>1</v>
       </c>
       <c r="I305" s="54"/>
-      <c r="J305" s="54"/>
+      <c r="J305" s="54">
+        <v>1</v>
+      </c>
       <c r="K305" s="54">
         <v>1</v>
       </c>
@@ -10860,7 +10912,7 @@
         <v>6</v>
       </c>
       <c r="C306" s="57" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="D306" s="48"/>
       <c r="E306" s="48"/>
@@ -10893,7 +10945,7 @@
         <v>6</v>
       </c>
       <c r="C307" s="57" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D307" s="48"/>
       <c r="E307" s="48"/>
@@ -10926,7 +10978,7 @@
         <v>6</v>
       </c>
       <c r="C308" s="57" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D308" s="48"/>
       <c r="E308" s="48"/>
@@ -10959,7 +11011,7 @@
         <v>6</v>
       </c>
       <c r="C309" s="57" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D309" s="48"/>
       <c r="E309" s="48"/>
@@ -10989,47 +11041,33 @@
         <v>47</v>
       </c>
       <c r="B310" s="55" t="s">
-        <v>51</v>
+        <v>6</v>
       </c>
       <c r="C310" s="57" t="s">
-        <v>158</v>
+        <v>317</v>
       </c>
       <c r="D310" s="48"/>
       <c r="E310" s="48"/>
       <c r="F310" s="48"/>
-      <c r="G310" s="54">
-        <v>1</v>
-      </c>
+      <c r="G310" s="54"/>
       <c r="H310" s="54">
         <v>1</v>
       </c>
-      <c r="I310" s="54">
-        <v>1</v>
-      </c>
-      <c r="J310" s="54">
-        <v>1</v>
-      </c>
+      <c r="I310" s="54"/>
+      <c r="J310" s="54"/>
       <c r="K310" s="54">
         <v>1</v>
       </c>
       <c r="L310" s="54">
         <v>1</v>
       </c>
-      <c r="M310" s="54">
-        <v>1</v>
-      </c>
+      <c r="M310" s="54"/>
       <c r="N310" s="54">
         <v>1</v>
       </c>
-      <c r="O310" s="54">
-        <v>1</v>
-      </c>
-      <c r="P310" s="54">
-        <v>1</v>
-      </c>
-      <c r="Q310" s="54">
-        <v>1</v>
-      </c>
+      <c r="O310" s="54"/>
+      <c r="P310" s="54"/>
+      <c r="Q310" s="54"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Q310" xr:uid="{A96C7FF1-A6C9-A643-BFCA-7D7FCDAF5533}">
@@ -11046,43 +11084,43 @@
     <hyperlink ref="C254" r:id="rId2" display="https://aws.amazon.com/app-mesh/" xr:uid="{F151395F-8E37-1049-9FCA-8474F2603F07}"/>
     <hyperlink ref="C29" r:id="rId3" display="https://aws.amazon.com/appsync/" xr:uid="{DB5645FD-41DF-9D4C-ADDB-CEEB9418B261}"/>
     <hyperlink ref="C272" r:id="rId4" display="https://aws.amazon.com/artifact/" xr:uid="{0251BE44-6F83-3541-8CD4-81AEF00F1760}"/>
-    <hyperlink ref="C279" r:id="rId5" display="https://aws.amazon.com/audit-manager/" xr:uid="{FE0C678B-66B4-5041-87CB-7B1FF56DF53B}"/>
+    <hyperlink ref="C273" r:id="rId5" display="https://aws.amazon.com/audit-manager/" xr:uid="{FE0C678B-66B4-5041-87CB-7B1FF56DF53B}"/>
     <hyperlink ref="C173" r:id="rId6" display="https://aws.amazon.com/autoscaling/" xr:uid="{900D412E-B452-CD43-BEB1-C8C1CB7269C8}"/>
     <hyperlink ref="C174" r:id="rId7" display="https://aws.amazon.com/backup/" xr:uid="{E0DD5920-BDCE-E647-9AF3-74760943689B}"/>
-    <hyperlink ref="C45" r:id="rId8" display="https://aws.amazon.com/batch/" xr:uid="{784C0A03-DDEC-BE4D-88F7-7005C1BB046B}"/>
+    <hyperlink ref="C44" r:id="rId8" display="https://aws.amazon.com/batch/" xr:uid="{784C0A03-DDEC-BE4D-88F7-7005C1BB046B}"/>
     <hyperlink ref="C67" r:id="rId9" display="https://aws.amazon.com/aws-cost-management/aws-budgets/" xr:uid="{57F5A17A-4752-B94C-8FBB-FC20BBF1A0BE}"/>
-    <hyperlink ref="C280" r:id="rId10" display="https://aws.amazon.com/certificate-manager/" xr:uid="{1F5BBCA8-0D50-C44C-907B-68E23D8E605C}"/>
+    <hyperlink ref="C274" r:id="rId10" display="https://aws.amazon.com/certificate-manager/" xr:uid="{1F5BBCA8-0D50-C44C-907B-68E23D8E605C}"/>
     <hyperlink ref="C39" r:id="rId11" display="https://aws.amazon.com/chatbot/" xr:uid="{F29F6239-1ADB-7049-AAA7-6E39F247047B}"/>
     <hyperlink ref="C256" r:id="rId12" display="https://aws.amazon.com/cloud-map/" xr:uid="{D482891E-9EB7-EA40-9A4B-6A8D3FEADBE3}"/>
     <hyperlink ref="C100" r:id="rId13" display="https://aws.amazon.com/cloud9/" xr:uid="{D565484B-E9EF-EA40-BDBE-0314AF229AE7}"/>
-    <hyperlink ref="C176" r:id="rId14" display="https://aws.amazon.com/cloudformation/" xr:uid="{602EC08B-B845-E049-943E-890A120862C8}"/>
-    <hyperlink ref="C281" r:id="rId15" display="https://aws.amazon.com/cloudhsm/" xr:uid="{76B855B6-4A01-1642-8706-3316A1643BA7}"/>
-    <hyperlink ref="C175" r:id="rId16" display="https://aws.amazon.com/cloudtrail/" xr:uid="{F1C2A161-2AD0-B14D-B62A-2640A558856F}"/>
+    <hyperlink ref="C175" r:id="rId14" display="https://aws.amazon.com/cloudformation/" xr:uid="{602EC08B-B845-E049-943E-890A120862C8}"/>
+    <hyperlink ref="C276" r:id="rId15" display="https://aws.amazon.com/cloudhsm/" xr:uid="{76B855B6-4A01-1642-8706-3316A1643BA7}"/>
+    <hyperlink ref="C176" r:id="rId16" display="https://aws.amazon.com/cloudtrail/" xr:uid="{F1C2A161-2AD0-B14D-B62A-2640A558856F}"/>
     <hyperlink ref="C102" r:id="rId17" display="https://aws.amazon.com/codeartifact" xr:uid="{A5B8559F-E4FA-BC42-AC7A-9D708C1D63A0}"/>
     <hyperlink ref="C103" r:id="rId18" display="https://aws.amazon.com/codebuild/" xr:uid="{E4144166-80F6-E741-B704-7C3864420913}"/>
     <hyperlink ref="C104" r:id="rId19" display="https://aws.amazon.com/codecommit/" xr:uid="{C9DB0F3B-CAEF-524C-A620-ACEA3E04FA66}"/>
     <hyperlink ref="C105" r:id="rId20" display="https://aws.amazon.com/codedeploy/" xr:uid="{D94C938E-B3D5-054D-AC63-39672D0C0DFC}"/>
     <hyperlink ref="C107" r:id="rId21" display="https://aws.amazon.com/codepipeline/" xr:uid="{DA2435A7-DA61-A54F-B02D-9BA62C072DF8}"/>
     <hyperlink ref="C108" r:id="rId22" display="https://aws.amazon.com/codestar/" xr:uid="{80EC7E07-A675-4540-8CC7-7CD9427476B0}"/>
-    <hyperlink ref="C180" r:id="rId23" display="https://aws.amazon.com/compute-optimizer/" xr:uid="{099597B3-D96C-124F-8A6B-DB661823AC75}"/>
-    <hyperlink ref="C178" r:id="rId24" display="https://aws.amazon.com/config/" xr:uid="{1DE61048-35C8-FB4C-A941-8996CBD19463}"/>
-    <hyperlink ref="C183" r:id="rId25" display="https://aws.amazon.com/controltower" xr:uid="{5ACDD884-3684-1840-9A42-603B4BFD4DFA}"/>
+    <hyperlink ref="C178" r:id="rId23" display="https://aws.amazon.com/compute-optimizer/" xr:uid="{099597B3-D96C-124F-8A6B-DB661823AC75}"/>
+    <hyperlink ref="C179" r:id="rId24" display="https://aws.amazon.com/config/" xr:uid="{1DE61048-35C8-FB4C-A941-8996CBD19463}"/>
+    <hyperlink ref="C181" r:id="rId25" display="https://aws.amazon.com/controltower" xr:uid="{5ACDD884-3684-1840-9A42-603B4BFD4DFA}"/>
     <hyperlink ref="C239" r:id="rId26" display="https://aws.amazon.com/data-exchange/" xr:uid="{EF81BA84-5C8F-DD4B-A31A-47BF7D5C826C}"/>
     <hyperlink ref="C242" r:id="rId27" display="https://aws.amazon.com/datasync" xr:uid="{7CED07B2-F329-1D46-A78D-E74BADEF8307}"/>
     <hyperlink ref="C241" r:id="rId28" display="https://aws.amazon.com/dms/" xr:uid="{C9210BF6-9C8C-5E48-824D-711353B0A5C4}"/>
     <hyperlink ref="C258" r:id="rId29" display="https://aws.amazon.com/directconnect/" xr:uid="{D4260538-1F28-C64D-999E-B57D8B4A110D}"/>
-    <hyperlink ref="C283" r:id="rId30" display="https://aws.amazon.com/directoryservice/" xr:uid="{71568105-08FB-3E48-ADDD-31FCAC00E550}"/>
-    <hyperlink ref="C48" r:id="rId31" display="https://aws.amazon.com/elasticbeanstalk/" xr:uid="{503FA701-A8C3-BA4D-8F14-4F45B1936437}"/>
+    <hyperlink ref="C279" r:id="rId30" display="https://aws.amazon.com/directoryservice/" xr:uid="{71568105-08FB-3E48-ADDD-31FCAC00E550}"/>
+    <hyperlink ref="C47" r:id="rId31" display="https://aws.amazon.com/elasticbeanstalk/" xr:uid="{503FA701-A8C3-BA4D-8F14-4F45B1936437}"/>
     <hyperlink ref="C220" r:id="rId32" display="https://aws.amazon.com/mediaconnect" xr:uid="{97EBEF96-B9F8-0444-803B-77B7686AD926}"/>
     <hyperlink ref="C221" r:id="rId33" display="https://aws.amazon.com/mediaconvert/" xr:uid="{A189CA26-8FE5-724E-AB4C-DA1684A9397C}"/>
     <hyperlink ref="C222" r:id="rId34" display="https://aws.amazon.com/medialive/" xr:uid="{8A1902D4-C3B2-6540-B6A2-D0939C092476}"/>
     <hyperlink ref="C62" r:id="rId35" display="https://aws.amazon.com/fargate/" xr:uid="{8AAC0488-BCAF-394A-B65D-1C8169C9015E}"/>
-    <hyperlink ref="C284" r:id="rId36" display="https://aws.amazon.com/firewall-manager/" xr:uid="{C1FC3FB2-6BB1-124F-AA39-0A32AEF1D03C}"/>
-    <hyperlink ref="C261" r:id="rId37" display="https://aws.amazon.com/global-accelerator" xr:uid="{94823B64-0747-B847-98EC-9C84C21B2DE2}"/>
+    <hyperlink ref="C283" r:id="rId36" display="https://aws.amazon.com/firewall-manager/" xr:uid="{C1FC3FB2-6BB1-124F-AA39-0A32AEF1D03C}"/>
+    <hyperlink ref="C260" r:id="rId37" display="https://aws.amazon.com/global-accelerator" xr:uid="{94823B64-0747-B847-98EC-9C84C21B2DE2}"/>
     <hyperlink ref="C7" r:id="rId38" display="https://aws.amazon.com/glue/" xr:uid="{A2984E2F-A64C-D74C-A499-872A26B2DE44}"/>
     <hyperlink ref="C271" r:id="rId39" display="https://aws.amazon.com/ground-station/" xr:uid="{DB86E86A-EF5B-2541-9BD8-5CDA9965E40C}"/>
     <hyperlink ref="C73" r:id="rId40" display="https://aws.amazon.com/iq/" xr:uid="{66074B4A-E4D5-724E-AD29-24C171CEC0BA}"/>
-    <hyperlink ref="C287" r:id="rId41" display="https://aws.amazon.com/iam" xr:uid="{97081695-DB1E-424E-B0EE-79AAD8D6E1CE}"/>
+    <hyperlink ref="C286" r:id="rId41" display="https://aws.amazon.com/iam" xr:uid="{97081695-DB1E-424E-B0EE-79AAD8D6E1CE}"/>
     <hyperlink ref="C125" r:id="rId42" display="https://aws.amazon.com/iot-1-click/" xr:uid="{ADC027FD-055F-9343-AF7A-479D41533208}"/>
     <hyperlink ref="C126" r:id="rId43" display="https://aws.amazon.com/iot-analytics/" xr:uid="{6587843B-FF8F-E445-A148-97BAA80660A5}"/>
     <hyperlink ref="C127" r:id="rId44" display="https://aws.amazon.com/iot/" xr:uid="{72ADB53E-C5C8-6E45-9DE6-006357ADBB14}"/>
@@ -11090,38 +11128,38 @@
     <hyperlink ref="C129" r:id="rId46" display="https://aws.amazon.com/iot-device-management/" xr:uid="{47327A94-A7DA-D44B-8D5D-137A2C1DB78D}"/>
     <hyperlink ref="C131" r:id="rId47" display="https://aws.amazon.com/iot-events/" xr:uid="{09A17074-F045-D045-99F3-289DE651CC4B}"/>
     <hyperlink ref="C132" r:id="rId48" display="https://aws.amazon.com/greengrass/" xr:uid="{86C6B532-C282-AD49-84FC-E7151CC17562}"/>
-    <hyperlink ref="C289" r:id="rId49" display="https://aws.amazon.com/kms/" xr:uid="{C0A6E0DF-7D93-854D-AF8E-5B9C19B8AF02}"/>
+    <hyperlink ref="C288" r:id="rId49" display="https://aws.amazon.com/kms/" xr:uid="{C0A6E0DF-7D93-854D-AF8E-5B9C19B8AF02}"/>
     <hyperlink ref="C18" r:id="rId50" display="https://aws.amazon.com/lake-formation/" xr:uid="{8B1B5135-7A0D-7645-A701-475DDEBCFDA0}"/>
     <hyperlink ref="C49" r:id="rId51" display="https://aws.amazon.com/lambda/" xr:uid="{23B44498-C148-BD4C-86FE-EFAA00464E5B}"/>
-    <hyperlink ref="C189" r:id="rId52" display="https://aws.amazon.com/license-manager/" xr:uid="{A80531A2-32DF-5E46-A8A2-AD514A9E876E}"/>
+    <hyperlink ref="C184" r:id="rId52" display="https://aws.amazon.com/license-manager/" xr:uid="{A80531A2-32DF-5E46-A8A2-AD514A9E876E}"/>
     <hyperlink ref="C75" r:id="rId53" display="https://aws.amazon.com/mp/" xr:uid="{83E81132-B5F9-A141-93D4-67826C5C6C2F}"/>
-    <hyperlink ref="C260" r:id="rId54" display="https://aws.amazon.com/network-firewall/" xr:uid="{380438F2-2136-CA48-8A93-614BD286828F}"/>
-    <hyperlink ref="C194" r:id="rId55" display="https://aws.amazon.com/opsworks/stacks/" xr:uid="{C7B2C66E-7305-8A45-B44D-ED0E58D460E7}"/>
-    <hyperlink ref="C192" r:id="rId56" display="https://aws.amazon.com/opsworks/chefautomate/" xr:uid="{44B83691-1D72-4540-A13B-BDA885E2E12D}"/>
-    <hyperlink ref="C193" r:id="rId57" display="https://aws.amazon.com/opsworks/puppetenterprise/" xr:uid="{23F41EB8-3A55-A44E-BD0D-93039495EA49}"/>
-    <hyperlink ref="C179" r:id="rId58" display="https://aws.amazon.com/organizations" xr:uid="{A3AB0BF0-AC79-A142-8708-144AD8A2BAF3}"/>
+    <hyperlink ref="C261" r:id="rId54" display="https://aws.amazon.com/network-firewall/" xr:uid="{380438F2-2136-CA48-8A93-614BD286828F}"/>
+    <hyperlink ref="C189" r:id="rId55" display="https://aws.amazon.com/opsworks/stacks/" xr:uid="{C7B2C66E-7305-8A45-B44D-ED0E58D460E7}"/>
+    <hyperlink ref="C187" r:id="rId56" display="https://aws.amazon.com/opsworks/chefautomate/" xr:uid="{44B83691-1D72-4540-A13B-BDA885E2E12D}"/>
+    <hyperlink ref="C188" r:id="rId57" display="https://aws.amazon.com/opsworks/puppetenterprise/" xr:uid="{23F41EB8-3A55-A44E-BD0D-93039495EA49}"/>
+    <hyperlink ref="C190" r:id="rId58" display="https://aws.amazon.com/organizations" xr:uid="{A3AB0BF0-AC79-A142-8708-144AD8A2BAF3}"/>
     <hyperlink ref="C51" r:id="rId59" display="https://aws.amazon.com/outposts/" xr:uid="{EC0218BA-7EA9-5F4D-8A2F-8D931B087AA0}"/>
-    <hyperlink ref="C195" r:id="rId60" display="https://aws.amazon.com/premiumsupport/phd/" xr:uid="{BC843AAF-6516-F341-B87D-0984C181B4B5}"/>
-    <hyperlink ref="C263" r:id="rId61" display="https://aws.amazon.com/privatelink/" xr:uid="{908DA648-769A-FB47-86E4-3D66FA675B1C}"/>
+    <hyperlink ref="C191" r:id="rId60" display="https://aws.amazon.com/premiumsupport/phd/" xr:uid="{BC843AAF-6516-F341-B87D-0984C181B4B5}"/>
+    <hyperlink ref="C262" r:id="rId61" display="https://aws.amazon.com/privatelink/" xr:uid="{908DA648-769A-FB47-86E4-3D66FA675B1C}"/>
     <hyperlink ref="C64" r:id="rId62" display="https://aws.amazon.com/proton/" xr:uid="{73BECBB6-D4BE-F445-97BF-0A1D62BCA194}"/>
-    <hyperlink ref="C196" r:id="rId63" display="https://aws.amazon.com/ram/" xr:uid="{F8E211FB-42AB-6848-88B7-49CC2A833913}"/>
+    <hyperlink ref="C192" r:id="rId63" display="https://aws.amazon.com/ram/" xr:uid="{F8E211FB-42AB-6848-88B7-49CC2A833913}"/>
     <hyperlink ref="C270" r:id="rId64" display="https://aws.amazon.com/robomaker/" xr:uid="{DBD68496-4CE8-804C-B893-9CFFB849F53A}"/>
-    <hyperlink ref="C285" r:id="rId65" display="https://aws.amazon.com/secrets-manager/" xr:uid="{632A5D67-D598-184C-AB9B-96F30896117D}"/>
+    <hyperlink ref="C290" r:id="rId65" display="https://aws.amazon.com/secrets-manager/" xr:uid="{632A5D67-D598-184C-AB9B-96F30896117D}"/>
     <hyperlink ref="C291" r:id="rId66" display="https://aws.amazon.com/security-hub/" xr:uid="{342A4832-F3A0-DB4D-840C-8118FD830399}"/>
     <hyperlink ref="C248" r:id="rId67" display="https://aws.amazon.com/server-migration-service/" xr:uid="{9446514E-0CE8-EC41-A9F1-0DC1FB7ADA55}"/>
     <hyperlink ref="C52" r:id="rId68" display="https://aws.amazon.com/serverless/serverlessrepo/" xr:uid="{8F7AC4BC-9A37-EC4F-8183-7D7404D19E14}"/>
-    <hyperlink ref="C197" r:id="rId69" display="https://aws.amazon.com/servicecatalog/" xr:uid="{2D2653B1-3D13-014A-9B9C-2386E2577635}"/>
+    <hyperlink ref="C193" r:id="rId69" display="https://aws.amazon.com/servicecatalog/" xr:uid="{2D2653B1-3D13-014A-9B9C-2386E2577635}"/>
     <hyperlink ref="C292" r:id="rId70" display="https://aws.amazon.com/shield/" xr:uid="{76E091F3-F618-A648-879F-3F09BEBFABFD}"/>
     <hyperlink ref="C293" r:id="rId71" display="https://aws.amazon.com/single-sign-on/" xr:uid="{A8360283-DE5C-1140-A85B-F33A2D6F72B8}"/>
     <hyperlink ref="C249" r:id="rId72" display="https://aws.amazon.com/snowball/" xr:uid="{8A7E1B57-5F26-F64E-853D-BDD63390D5E6}"/>
     <hyperlink ref="C251" r:id="rId73" display="https://aws.amazon.com/snowmobile/" xr:uid="{62B7D92F-3C96-DA44-9F02-BCC308391061}"/>
     <hyperlink ref="C36" r:id="rId74" display="https://aws.amazon.com/step-functions/details/" xr:uid="{10824B81-0A5F-634D-84E6-9D2ADE3A6B39}"/>
-    <hyperlink ref="C304" r:id="rId75" display="https://aws.amazon.com/storagegateway/" xr:uid="{7BF17EFE-FF03-1D4A-BE9E-1FA982DA5C2A}"/>
+    <hyperlink ref="C305" r:id="rId75" display="https://aws.amazon.com/storagegateway/" xr:uid="{7BF17EFE-FF03-1D4A-BE9E-1FA982DA5C2A}"/>
     <hyperlink ref="C77" r:id="rId76" display="https://aws.amazon.com/premiumsupport/" xr:uid="{A5466C95-EFB7-3944-9E29-8D19BB6E169F}"/>
-    <hyperlink ref="C186" r:id="rId77" display="https://aws.amazon.com/systems-manager/" xr:uid="{D6C17500-BE92-C444-BA4A-7116B75319D3}"/>
+    <hyperlink ref="C211" r:id="rId77" display="https://aws.amazon.com/systems-manager/" xr:uid="{D6C17500-BE92-C444-BA4A-7116B75319D3}"/>
     <hyperlink ref="C252" r:id="rId78" display="https://aws.amazon.com/aws-transfer-family/" xr:uid="{F0069BD4-8633-FB4B-8185-293CB3193797}"/>
-    <hyperlink ref="C266" r:id="rId79" display="https://aws.amazon.com/transit-gateway/" xr:uid="{2C10B2F7-EEE3-3444-A855-B387D48706EA}"/>
-    <hyperlink ref="C187" r:id="rId80" display="https://aws.amazon.com/premiumsupport/trustedadvisor/" xr:uid="{436ECB3D-7EFE-764A-B2E3-3CF79C97B742}"/>
+    <hyperlink ref="C265" r:id="rId79" display="https://aws.amazon.com/transit-gateway/" xr:uid="{2C10B2F7-EEE3-3444-A855-B387D48706EA}"/>
+    <hyperlink ref="C212" r:id="rId80" display="https://aws.amazon.com/premiumsupport/trustedadvisor/" xr:uid="{436ECB3D-7EFE-764A-B2E3-3CF79C97B742}"/>
     <hyperlink ref="C268" r:id="rId81" display="https://aws.amazon.com/vpn/" xr:uid="{5F2B553B-98BD-8D4B-849C-55A6F659C6B1}"/>
     <hyperlink ref="C294" r:id="rId82" display="https://aws.amazon.com/waf/" xr:uid="{CF739D06-0B1B-6B46-91CF-6EE57FF09613}"/>
     <hyperlink ref="C213" r:id="rId83" display="https://aws.amazon.com/well-architected-tool" xr:uid="{81A34672-555C-B74A-9D7B-58590B7D3C75}"/>
@@ -11132,20 +11170,20 @@
     <hyperlink ref="C136" r:id="rId88" display="https://aws.amazon.com/augmented-ai/" xr:uid="{9B0A35B8-349D-874F-B406-0C378A70E4A7}"/>
     <hyperlink ref="C82" r:id="rId89" display="https://aws.amazon.com/rds/aurora/" xr:uid="{5BA37BE5-5EFA-D640-9340-68572A5C8B0A}"/>
     <hyperlink ref="C40" r:id="rId90" display="https://chime.aws/" xr:uid="{08A22D72-3716-8743-A4B8-3002293D3436}"/>
-    <hyperlink ref="C273" r:id="rId91" display="https://aws.amazon.com/cloud-directory/" xr:uid="{E41D133C-BA4E-4642-BA6F-656788DBC830}"/>
+    <hyperlink ref="C275" r:id="rId91" display="https://aws.amazon.com/cloud-directory/" xr:uid="{E41D133C-BA4E-4642-BA6F-656788DBC830}"/>
     <hyperlink ref="C257" r:id="rId92" display="https://aws.amazon.com/cloudfront/" xr:uid="{8065D5C6-B564-A941-80CC-5D6C65B3D725}"/>
     <hyperlink ref="C177" r:id="rId93" display="https://aws.amazon.com/cloudwatch/" xr:uid="{52B01F49-5EAB-E540-BA38-BEED42EB43F4}"/>
     <hyperlink ref="C106" r:id="rId94" display="https://aws.amazon.com/codeguru/" xr:uid="{D5D1E2B5-ED1C-0D45-BCD8-07A6431E8C14}"/>
-    <hyperlink ref="C274" r:id="rId95" display="https://aws.amazon.com/cognito/" xr:uid="{5631285D-2790-B940-99E8-7A2AFBF2A4F8}"/>
+    <hyperlink ref="C277" r:id="rId95" display="https://aws.amazon.com/cognito/" xr:uid="{5631285D-2790-B940-99E8-7A2AFBF2A4F8}"/>
     <hyperlink ref="C137" r:id="rId96" display="https://aws.amazon.com/comprehend/" xr:uid="{EF9B7DCD-AAB7-C840-B56B-6901E4208F3C}"/>
     <hyperlink ref="C138" r:id="rId97" display="https://aws.amazon.com/comprehend/medical/" xr:uid="{E755C2E6-BB69-1547-AEEA-159FA230C6E0}"/>
-    <hyperlink ref="C282" r:id="rId98" display="https://aws.amazon.com/detective/" xr:uid="{4F6306C8-7E6E-B543-8987-505512DF8B38}"/>
+    <hyperlink ref="C278" r:id="rId98" display="https://aws.amazon.com/detective/" xr:uid="{4F6306C8-7E6E-B543-8987-505512DF8B38}"/>
     <hyperlink ref="C143" r:id="rId99" display="https://aws.amazon.com/devops-guru/" xr:uid="{0DE3687A-6EED-D846-93EF-2FF3EDCA2FE7}"/>
     <hyperlink ref="C83" r:id="rId100" display="https://aws.amazon.com/documentdb/" xr:uid="{E9BE873B-93B3-744C-82A3-AE676C942786}"/>
     <hyperlink ref="C84" r:id="rId101" display="https://aws.amazon.com/dynamodb/" xr:uid="{667C0B17-E586-7843-9ABA-2156F328D1C2}"/>
     <hyperlink ref="C87" r:id="rId102" display="https://aws.amazon.com/elasticache/" xr:uid="{0D3B6893-EB9F-F441-97F2-EAE3A531E741}"/>
     <hyperlink ref="C297" r:id="rId103" display="https://aws.amazon.com/ebs/" xr:uid="{6475A1BA-F9EA-3643-A91C-960971815276}"/>
-    <hyperlink ref="C46" r:id="rId104" xr:uid="{F6BE2D25-6B4D-D545-BEF5-6353621F7D77}"/>
+    <hyperlink ref="C45" r:id="rId104" xr:uid="{F6BE2D25-6B4D-D545-BEF5-6353621F7D77}"/>
     <hyperlink ref="C59" r:id="rId105" display="https://aws.amazon.com/ecr/" xr:uid="{4DB8575D-FD4E-F24B-9A6D-4B237DEB4216}"/>
     <hyperlink ref="C60" r:id="rId106" display="https://aws.amazon.com/ecs/" xr:uid="{2A857716-DB7F-4D4C-9C3A-923E359FCE4B}"/>
     <hyperlink ref="C298" r:id="rId107" display="https://aws.amazon.com/efs/" xr:uid="{17293663-847A-2945-BEEE-DB5C14186604}"/>
@@ -11159,8 +11197,8 @@
     <hyperlink ref="C145" r:id="rId115" display="https://aws.amazon.com/forecast/" xr:uid="{1F07E3AD-D0E3-4442-9220-92E85E3DF861}"/>
     <hyperlink ref="C146" r:id="rId116" display="https://aws.amazon.com/fraud-detector/" xr:uid="{A16ABA87-0E9D-1749-BE3E-718E7599E24B}"/>
     <hyperlink ref="C121" r:id="rId117" display="https://aws.amazon.com/gamelift/" xr:uid="{ABE766D8-2E8B-B341-9103-F503839AC514}"/>
-    <hyperlink ref="C286" r:id="rId118" display="https://aws.amazon.com/guardduty/" xr:uid="{D1B6E14A-AD6C-E844-9AD0-215698F4E3BE}"/>
-    <hyperlink ref="C288" r:id="rId119" display="https://aws.amazon.com/inspector/" xr:uid="{176BE9A8-3FF5-874F-8EFA-6BB4665C2F33}"/>
+    <hyperlink ref="C284" r:id="rId118" display="https://aws.amazon.com/guardduty/" xr:uid="{D1B6E14A-AD6C-E844-9AD0-215698F4E3BE}"/>
+    <hyperlink ref="C287" r:id="rId119" display="https://aws.amazon.com/inspector/" xr:uid="{176BE9A8-3FF5-874F-8EFA-6BB4665C2F33}"/>
     <hyperlink ref="C88" r:id="rId120" display="https://aws.amazon.com/keyspaces/" xr:uid="{08537BC8-9E18-E341-B811-B357F4073FF5}"/>
     <hyperlink ref="C15" r:id="rId121" display="https://aws.amazon.com/kinesis/analytics/" xr:uid="{55091A39-96DB-9A41-B453-9AB88556B85B}"/>
     <hyperlink ref="C16" r:id="rId122" display="https://aws.amazon.com/kinesis/firehose/" xr:uid="{AB91BD64-7EBD-8A40-89D5-415AC999E5A7}"/>
@@ -11171,7 +11209,7 @@
     <hyperlink ref="C149" r:id="rId127" display="https://aws.amazon.com/lookout-for-vision/" xr:uid="{56891F15-488A-2D4F-957F-9C19DBC09E8C}"/>
     <hyperlink ref="C122" r:id="rId128" display="https://aws.amazon.com/lumberyard/" xr:uid="{0793FA7F-F861-E448-B351-2625AB793E29}"/>
     <hyperlink ref="C32" r:id="rId129" display="https://aws.amazon.com/amazon-mq/" xr:uid="{8F7E8190-F83B-7E45-9B55-465E1F7C79F3}"/>
-    <hyperlink ref="C290" r:id="rId130" display="https://aws.amazon.com/macie/" xr:uid="{0A9A9C7B-64FF-4944-8B73-82D7A54412E2}"/>
+    <hyperlink ref="C289" r:id="rId130" display="https://aws.amazon.com/macie/" xr:uid="{0A9A9C7B-64FF-4944-8B73-82D7A54412E2}"/>
     <hyperlink ref="C19" r:id="rId131" display="https://aws.amazon.com/msk/" xr:uid="{46024F01-6B35-0740-B92F-18BA0D596F3D}"/>
     <hyperlink ref="C31" r:id="rId132" display="https://aws.amazon.com/managed-workflows-for-apache-airflow/" xr:uid="{E7D50CE9-B395-AE40-B3BD-7B31072C139C}"/>
     <hyperlink ref="C90" r:id="rId133" display="https://aws.amazon.com/neptune/" xr:uid="{35EB7CA9-2F10-7E4E-9B05-D1C561AFFA79}"/>
@@ -11182,12 +11220,12 @@
     <hyperlink ref="C22" r:id="rId138" display="https://aws.amazon.com/redshift/" xr:uid="{BD068AB5-9542-BA4D-9D2D-3E01553833FF}"/>
     <hyperlink ref="C153" r:id="rId139" display="https://aws.amazon.com/rekognition/" xr:uid="{06B644B6-712E-EB4F-BDC1-2826A6E207A2}"/>
     <hyperlink ref="C93" r:id="rId140" display="https://aws.amazon.com/rds/" xr:uid="{52A384FE-5551-524F-8BE4-640C39EE59DB}"/>
-    <hyperlink ref="C264" r:id="rId141" display="https://aws.amazon.com/route53/" xr:uid="{2B9EF04D-DB6D-9948-8F0B-1F85D1FFA02C}"/>
+    <hyperlink ref="C263" r:id="rId141" display="https://aws.amazon.com/route53/" xr:uid="{2B9EF04D-DB6D-9948-8F0B-1F85D1FFA02C}"/>
     <hyperlink ref="C154" r:id="rId142" display="https://aws.amazon.com/sagemaker/" xr:uid="{FF819C8F-B472-6A4D-BF36-8803B10C8D16}"/>
     <hyperlink ref="C81" r:id="rId143" display="https://aws.amazon.com/ses/" xr:uid="{708BC6D8-3F72-374C-AB65-9002B2EB5C60}"/>
     <hyperlink ref="C33" r:id="rId144" display="https://aws.amazon.com/sns/" xr:uid="{2A7374BD-4C80-7C42-9E56-E3671DF3D17F}"/>
     <hyperlink ref="C34" r:id="rId145" display="https://aws.amazon.com/sqs/" xr:uid="{7EC87AB6-C5A3-0F4B-915C-BD9EF4201FD5}"/>
-    <hyperlink ref="C310" r:id="rId146" display="https://aws.amazon.com/s3/" xr:uid="{CD425C97-24D5-9747-8B23-DF9DD7A486F9}"/>
+    <hyperlink ref="C304" r:id="rId146" display="https://aws.amazon.com/s3/" xr:uid="{CD425C97-24D5-9747-8B23-DF9DD7A486F9}"/>
     <hyperlink ref="C35" r:id="rId147" display="https://aws.amazon.com/swf/" xr:uid="{631F304E-E46F-644E-8407-57836778A272}"/>
     <hyperlink ref="C123" r:id="rId148" display="https://aws.amazon.com/sumerian/" xr:uid="{1F8D41FC-B82F-8C44-A79F-AA91C3811E29}"/>
     <hyperlink ref="C168" r:id="rId149" display="https://aws.amazon.com/textract" xr:uid="{E50E8082-94C1-7947-963B-3A384A890F42}"/>
@@ -11195,14 +11233,14 @@
     <hyperlink ref="C169" r:id="rId151" display="https://aws.amazon.com/transcribe/" xr:uid="{7391FC88-BBA3-5846-9CA8-5612809D5D1E}"/>
     <hyperlink ref="C170" r:id="rId152" display="https://aws.amazon.com/transcribe/medical/" xr:uid="{5D3CF2D8-5264-E342-A8E8-E042131AE7AF}"/>
     <hyperlink ref="C171" r:id="rId153" display="https://aws.amazon.com/translate/" xr:uid="{D94B1850-F477-024B-8A15-72298FF44F81}"/>
-    <hyperlink ref="C262" r:id="rId154" display="https://aws.amazon.com/vpc/" xr:uid="{81704202-B35B-314F-9611-62D10520486C}"/>
+    <hyperlink ref="C266" r:id="rId154" display="https://aws.amazon.com/vpc/" xr:uid="{81704202-B35B-314F-9611-62D10520486C}"/>
     <hyperlink ref="C119" r:id="rId155" display="https://aws.amazon.com/worklink/" xr:uid="{A564F6A5-A25E-984E-AB0E-10859F299F79}"/>
     <hyperlink ref="C296" r:id="rId156" display="https://aws.amazon.com/cloudendure-disaster-recovery/" xr:uid="{19E2670B-B70B-2246-875A-A798E313AD4C}"/>
     <hyperlink ref="C238" r:id="rId157" display="https://aws.amazon.com/cloudendure-migration/" xr:uid="{3011454A-BA14-2640-A5B0-1665DE5015EB}"/>
     <hyperlink ref="C259" r:id="rId158" display="https://aws.amazon.com/elasticloadbalancing/" xr:uid="{48C41A56-7B49-954B-8607-BA52CE86305D}"/>
     <hyperlink ref="C124" r:id="rId159" display="https://aws.amazon.com/freertos/" xr:uid="{9A951967-4675-1546-8716-0568BF98D1CE}"/>
     <hyperlink ref="C53" r:id="rId160" display="https://aws.amazon.com/vmware/" xr:uid="{1D088AE8-27BE-C042-AB38-9D218A238493}"/>
-    <hyperlink ref="C44" r:id="rId161" display="https://aws.amazon.com/ec2/" xr:uid="{A67A7092-80C0-9A4E-A55B-97FA160377E8}"/>
+    <hyperlink ref="C48" r:id="rId161" display="https://aws.amazon.com/ec2/" xr:uid="{A67A7092-80C0-9A4E-A55B-97FA160377E8}"/>
     <hyperlink ref="C302" r:id="rId162" xr:uid="{9237F063-BA80-DC44-882A-D4F7F6FD5EE9}"/>
     <hyperlink ref="C111" r:id="rId163" xr:uid="{75CD952A-625F-DE4E-B2D6-41E51DC1F7E3}"/>
     <hyperlink ref="C37" r:id="rId164" xr:uid="{49E4FD14-55A4-2E46-8EFF-5EF1766DCF38}"/>
@@ -11218,7 +11256,7 @@
     <hyperlink ref="C56" r:id="rId174" xr:uid="{161791FF-9796-5D41-9399-C5CC0A52B777}"/>
     <hyperlink ref="C54" r:id="rId175" xr:uid="{005354BD-081E-9E46-8937-381CB8592473}"/>
     <hyperlink ref="C58" r:id="rId176" xr:uid="{1CFA07FC-268F-C84D-B8E8-D13B2E092826}"/>
-    <hyperlink ref="C190" r:id="rId177" xr:uid="{667DCA05-C10B-394B-ADBD-C91C39C8EFA9}"/>
+    <hyperlink ref="C185" r:id="rId177" xr:uid="{667DCA05-C10B-394B-ADBD-C91C39C8EFA9}"/>
     <hyperlink ref="C299" r:id="rId178" xr:uid="{19712BF9-B0E9-FC4A-855C-37C622207421}"/>
     <hyperlink ref="C101" r:id="rId179" xr:uid="{532F9FAB-7588-934A-BECA-94DB57B3EA86}"/>
     <hyperlink ref="C97" r:id="rId180" xr:uid="{03EA6A9E-9AED-E449-AEAE-E07C9D687ADF}"/>
@@ -11237,22 +11275,22 @@
     <hyperlink ref="C159" r:id="rId193" xr:uid="{534A3538-6476-C049-B1F4-C7F42A4A0CE2}"/>
     <hyperlink ref="C160" r:id="rId194" xr:uid="{AD37C4EC-6AA6-7445-886F-F12B10EC4962}"/>
     <hyperlink ref="C150" r:id="rId195" xr:uid="{32D673E8-4729-054A-941B-0538347DFE6B}"/>
-    <hyperlink ref="C198" r:id="rId196" display="AppConfig" xr:uid="{D7D5BCB4-B018-9449-8DE4-7BAC0B834A94}"/>
-    <hyperlink ref="C181" r:id="rId197" xr:uid="{6C997D60-3DAC-C54C-A365-6925F32D808B}"/>
-    <hyperlink ref="C199" r:id="rId198" xr:uid="{704C5761-85F7-8840-90D5-B9C68A5711E5}"/>
-    <hyperlink ref="C202" r:id="rId199" xr:uid="{0AE4E9A5-C51C-054C-8C1C-DFC93B7DE436}"/>
-    <hyperlink ref="C200" r:id="rId200" xr:uid="{D396B2A5-863A-0A4F-886E-AC0425111A74}"/>
-    <hyperlink ref="C208" r:id="rId201" xr:uid="{154E52D7-25A2-7B48-861E-130AEFF52429}"/>
-    <hyperlink ref="C206" r:id="rId202" xr:uid="{B55B16FC-FF18-784A-A974-098400EB5613}"/>
-    <hyperlink ref="C203" r:id="rId203" xr:uid="{2E1084D5-EB92-104E-9B36-C1C783851CEE}"/>
-    <hyperlink ref="C207" r:id="rId204" xr:uid="{CE1FE151-6237-2B48-BAA5-A0485476B07E}"/>
-    <hyperlink ref="C210" r:id="rId205" xr:uid="{8B651CA8-4121-954F-A1FD-E2ABDAE2711A}"/>
-    <hyperlink ref="C211" r:id="rId206" xr:uid="{73E53697-EA4F-5D44-BABF-E4DDE08A2949}"/>
-    <hyperlink ref="C212" r:id="rId207" xr:uid="{1F5BA02E-7700-F84C-896F-C3320A138F8C}"/>
-    <hyperlink ref="C185" r:id="rId208" xr:uid="{965DAB0C-1533-9C43-9931-A81FDFEE4801}"/>
-    <hyperlink ref="C204" r:id="rId209" xr:uid="{D7F493BC-3996-E14D-8B4E-AF698AF15CF3}"/>
-    <hyperlink ref="C209" r:id="rId210" xr:uid="{158C22B5-B282-0E45-819B-E1F6D3588EB5}"/>
-    <hyperlink ref="C205" r:id="rId211" xr:uid="{060EF427-1526-CB41-B8B7-D967487671FE}"/>
+    <hyperlink ref="C194" r:id="rId196" display="AppConfig" xr:uid="{D7D5BCB4-B018-9449-8DE4-7BAC0B834A94}"/>
+    <hyperlink ref="C206" r:id="rId197" xr:uid="{6C997D60-3DAC-C54C-A365-6925F32D808B}"/>
+    <hyperlink ref="C195" r:id="rId198" xr:uid="{704C5761-85F7-8840-90D5-B9C68A5711E5}"/>
+    <hyperlink ref="C198" r:id="rId199" xr:uid="{0AE4E9A5-C51C-054C-8C1C-DFC93B7DE436}"/>
+    <hyperlink ref="C196" r:id="rId200" xr:uid="{D396B2A5-863A-0A4F-886E-AC0425111A74}"/>
+    <hyperlink ref="C204" r:id="rId201" xr:uid="{154E52D7-25A2-7B48-861E-130AEFF52429}"/>
+    <hyperlink ref="C202" r:id="rId202" xr:uid="{B55B16FC-FF18-784A-A974-098400EB5613}"/>
+    <hyperlink ref="C199" r:id="rId203" xr:uid="{2E1084D5-EB92-104E-9B36-C1C783851CEE}"/>
+    <hyperlink ref="C203" r:id="rId204" xr:uid="{CE1FE151-6237-2B48-BAA5-A0485476B07E}"/>
+    <hyperlink ref="C208" r:id="rId205" xr:uid="{8B651CA8-4121-954F-A1FD-E2ABDAE2711A}"/>
+    <hyperlink ref="C209" r:id="rId206" xr:uid="{73E53697-EA4F-5D44-BABF-E4DDE08A2949}"/>
+    <hyperlink ref="C210" r:id="rId207" xr:uid="{1F5BA02E-7700-F84C-896F-C3320A138F8C}"/>
+    <hyperlink ref="C207" r:id="rId208" xr:uid="{965DAB0C-1533-9C43-9931-A81FDFEE4801}"/>
+    <hyperlink ref="C200" r:id="rId209" xr:uid="{D7F493BC-3996-E14D-8B4E-AF698AF15CF3}"/>
+    <hyperlink ref="C205" r:id="rId210" xr:uid="{158C22B5-B282-0E45-819B-E1F6D3588EB5}"/>
+    <hyperlink ref="C201" r:id="rId211" xr:uid="{060EF427-1526-CB41-B8B7-D967487671FE}"/>
     <hyperlink ref="C303" r:id="rId212" display="S3 Glacier" xr:uid="{69E65928-2461-9D41-874A-E2DD597C93F4}"/>
     <hyperlink ref="C161" r:id="rId213" xr:uid="{985BD89A-8A6D-3646-8654-90328345A506}"/>
     <hyperlink ref="C139" r:id="rId214" xr:uid="{590CE714-967E-A245-B8FF-739BCA3B026A}"/>
@@ -11275,10 +11313,10 @@
     <hyperlink ref="C134" r:id="rId231" xr:uid="{40FD60AC-B589-0B4B-AB36-1989E529CD39}"/>
     <hyperlink ref="C135" r:id="rId232" xr:uid="{56F27AA2-5183-E94B-ACC4-73885A21F096}"/>
     <hyperlink ref="C63" r:id="rId233" display="Managed Service for Prometheus" xr:uid="{15FBF981-0EC3-6343-ACAF-575D9CF01C72}"/>
-    <hyperlink ref="C275" r:id="rId234" display="Directory Service AD Connector" xr:uid="{CE8FDA92-983D-F241-9A3C-214FB6ED4987}"/>
-    <hyperlink ref="C277" r:id="rId235" display="Directory Service Simple AD" xr:uid="{BDF803C1-C55F-7B4E-B548-FB056C33B7F8}"/>
-    <hyperlink ref="C276" r:id="rId236" display="Directory Service Managed Microsoft AD" xr:uid="{A2682350-698B-164E-854C-B72B425BF114}"/>
-    <hyperlink ref="C191" r:id="rId237" xr:uid="{51AE8255-80F9-1246-AF04-CAD49D7BD8ED}"/>
+    <hyperlink ref="C280" r:id="rId234" display="Directory Service AD Connector" xr:uid="{CE8FDA92-983D-F241-9A3C-214FB6ED4987}"/>
+    <hyperlink ref="C282" r:id="rId235" display="Directory Service Simple AD" xr:uid="{BDF803C1-C55F-7B4E-B548-FB056C33B7F8}"/>
+    <hyperlink ref="C281" r:id="rId236" display="Directory Service Managed Microsoft AD" xr:uid="{A2682350-698B-164E-854C-B72B425BF114}"/>
+    <hyperlink ref="C186" r:id="rId237" xr:uid="{51AE8255-80F9-1246-AF04-CAD49D7BD8ED}"/>
     <hyperlink ref="C112" r:id="rId238" xr:uid="{F72E5D13-7F9C-A74A-B15B-60DA5CBC35BF}"/>
     <hyperlink ref="C147" r:id="rId239" xr:uid="{A021BA43-B246-CF41-8A4E-1E391CD06D94}"/>
     <hyperlink ref="C243" r:id="rId240" xr:uid="{66C98670-091A-A841-9473-A308D3D03C92}"/>
@@ -11304,7 +11342,7 @@
     <hyperlink ref="C227" r:id="rId260" xr:uid="{46CEB576-1991-6A4C-9819-8C32AAD5A3F1}"/>
     <hyperlink ref="C218" r:id="rId261" xr:uid="{98567FEC-ACF3-D64E-8831-23F0AF44FDF4}"/>
     <hyperlink ref="C115" r:id="rId262" xr:uid="{CBE97B7F-03A3-3B47-A836-0FDA32E32458}"/>
-    <hyperlink ref="C188" r:id="rId263" xr:uid="{98ADDE2A-ABDD-EB4A-8EBE-C43795A8F20B}"/>
+    <hyperlink ref="C183" r:id="rId263" xr:uid="{98ADDE2A-ABDD-EB4A-8EBE-C43795A8F20B}"/>
     <hyperlink ref="C55" r:id="rId264" xr:uid="{FE878825-B0CA-394C-95F4-6879C16270CC}"/>
     <hyperlink ref="C236" r:id="rId265" xr:uid="{8AF37CA7-BEF8-0E46-AFB3-906542482AD8}"/>
     <hyperlink ref="C57" r:id="rId266" xr:uid="{E1C253C0-789F-454D-B650-AD9042907E63}"/>
@@ -11314,11 +11352,11 @@
     <hyperlink ref="C233" r:id="rId270" xr:uid="{3B6EA2BE-9E87-CD43-BD86-90EF411A17C9}"/>
     <hyperlink ref="C234" r:id="rId271" xr:uid="{BE5AE3F2-6AF4-FB45-A4C7-58EE1FA83493}"/>
     <hyperlink ref="C235" r:id="rId272" xr:uid="{9F9A6701-301A-8946-8181-9D1074CEB3F6}"/>
-    <hyperlink ref="C309" r:id="rId273" display="Storage Gateway - Volume Gateway" xr:uid="{D2EC8952-5BC9-2B49-B394-D7BE012603FF}"/>
-    <hyperlink ref="C307" r:id="rId274" xr:uid="{1B5D263F-5321-B54A-BF60-2932447DCE26}"/>
-    <hyperlink ref="C305" r:id="rId275" display="Storage Gateway - FSx File Gateway" xr:uid="{2125FCAA-C46E-224B-8BE0-19D32D161491}"/>
-    <hyperlink ref="C306" r:id="rId276" display="Storage Gateway - S3 File Gateway" xr:uid="{96B9D02E-E08D-3E44-9C8E-08A2BE24E99A}"/>
-    <hyperlink ref="C308" r:id="rId277" display="Storage Gateway - Volume Gateway" xr:uid="{FFBC4DD5-5D45-9B42-A545-70A2598E87B0}"/>
+    <hyperlink ref="C310" r:id="rId273" display="Storage Gateway - Volume Gateway" xr:uid="{D2EC8952-5BC9-2B49-B394-D7BE012603FF}"/>
+    <hyperlink ref="C308" r:id="rId274" xr:uid="{1B5D263F-5321-B54A-BF60-2932447DCE26}"/>
+    <hyperlink ref="C306" r:id="rId275" display="Storage Gateway - FSx File Gateway" xr:uid="{2125FCAA-C46E-224B-8BE0-19D32D161491}"/>
+    <hyperlink ref="C307" r:id="rId276" display="Storage Gateway - S3 File Gateway" xr:uid="{96B9D02E-E08D-3E44-9C8E-08A2BE24E99A}"/>
+    <hyperlink ref="C309" r:id="rId277" display="Storage Gateway - Volume Gateway" xr:uid="{FFBC4DD5-5D45-9B42-A545-70A2598E87B0}"/>
     <hyperlink ref="C24" r:id="rId278" xr:uid="{F8A9F9A7-CC98-EC42-8596-0253E0A2BB97}"/>
     <hyperlink ref="C23" r:id="rId279" xr:uid="{8B655CFD-0968-7140-84E8-2070B49F002B}"/>
     <hyperlink ref="C27" r:id="rId280" xr:uid="{FD22D76A-0562-0640-85D0-C48AA580C483}"/>
@@ -11327,21 +11365,21 @@
     <hyperlink ref="C66" r:id="rId283" xr:uid="{1CA75B5D-40F7-EE46-91F1-45EA22AB9C53}"/>
     <hyperlink ref="C118" r:id="rId284" xr:uid="{5961D4D9-3072-2149-961B-0C10629539E7}"/>
     <hyperlink ref="C89" r:id="rId285" xr:uid="{863934C0-971A-AF48-A43D-B4B914AECC39}"/>
-    <hyperlink ref="C184" r:id="rId286" xr:uid="{3295CEB8-10D1-5A43-BEA9-DF5FD886C0AB}"/>
+    <hyperlink ref="C182" r:id="rId286" xr:uid="{3295CEB8-10D1-5A43-BEA9-DF5FD886C0AB}"/>
     <hyperlink ref="C295" r:id="rId287" xr:uid="{4F9FE344-D5EC-AC40-97FF-2F5F45F27D96}"/>
-    <hyperlink ref="C201" r:id="rId288" xr:uid="{AEDB8326-231C-C744-8B10-AF02B678D9B4}"/>
+    <hyperlink ref="C197" r:id="rId288" xr:uid="{AEDB8326-231C-C744-8B10-AF02B678D9B4}"/>
     <hyperlink ref="C14" r:id="rId289" xr:uid="{2E249962-989F-944F-B761-2BAA0EC7CAEC}"/>
     <hyperlink ref="C172" r:id="rId290" xr:uid="{DCE5737A-9A5B-DC4D-850F-450E2D238525}"/>
-    <hyperlink ref="C47" r:id="rId291" xr:uid="{FE31CE04-AE8C-B545-B85E-3E35079AA70A}"/>
+    <hyperlink ref="C46" r:id="rId291" xr:uid="{FE31CE04-AE8C-B545-B85E-3E35079AA70A}"/>
     <hyperlink ref="C255" r:id="rId292" xr:uid="{D321FD11-72A4-9F4D-857D-939FF8BB6E1B}"/>
-    <hyperlink ref="C265" r:id="rId293" xr:uid="{E997CB7A-902E-064D-B6FF-8470A806D5A0}"/>
+    <hyperlink ref="C264" r:id="rId293" xr:uid="{E997CB7A-902E-064D-B6FF-8470A806D5A0}"/>
     <hyperlink ref="C267" r:id="rId294" xr:uid="{0A132D4A-E971-7246-889D-EB0D9E3ED74A}"/>
-    <hyperlink ref="C278" r:id="rId295" xr:uid="{5D89926F-F8DE-F748-ADBE-85B87EFE8273}"/>
+    <hyperlink ref="C285" r:id="rId295" xr:uid="{5D89926F-F8DE-F748-ADBE-85B87EFE8273}"/>
     <hyperlink ref="C130" r:id="rId296" xr:uid="{2B14DC1E-31E9-E643-8322-E37BB77A61F2}"/>
     <hyperlink ref="C246" r:id="rId297" xr:uid="{09886B01-263E-164A-BB8E-628947483324}"/>
     <hyperlink ref="C247" r:id="rId298" xr:uid="{5F2F3CFC-7F4A-FD4D-941C-DED03BD1B5FC}"/>
     <hyperlink ref="C237" r:id="rId299" xr:uid="{7C8F3176-C207-894A-B174-4BEF8A9DAF7C}"/>
-    <hyperlink ref="C182" r:id="rId300" xr:uid="{E43F582E-778D-E840-BF2A-38A6E4E85D0B}"/>
+    <hyperlink ref="C180" r:id="rId300" xr:uid="{E43F582E-778D-E840-BF2A-38A6E4E85D0B}"/>
     <hyperlink ref="C98:C99" r:id="rId301" display="Cloud Development Kit (CDK)" xr:uid="{74EF9526-5AAF-4446-8604-03C2DD1F15BF}"/>
     <hyperlink ref="C98" r:id="rId302" xr:uid="{C3C5B093-C1E6-354A-B80D-C83A330D70CE}"/>
     <hyperlink ref="C99" r:id="rId303" xr:uid="{3EF40231-9DF0-E848-9274-0E658AE48B9A}"/>

</xml_diff>

<commit_message>
XKS, verified access, verified permissions
</commit_message>
<xml_diff>
--- a/aws-services-crib-sheet.xlsx
+++ b/aws-services-crib-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corbuno/courses/aws-services-crib-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34E99F5-6012-8B40-B33E-4B92A6994E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DFBD5A-4A8D-FB4B-8EA0-1EDE2AEB7858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8DC9DE24-CECC-4748-B90E-52259685D84E}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="source" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AWS Services'!$A$1:$R$369</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AWS Services'!$A$1:$R$372</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1106" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="420">
   <si>
     <t>Elastic Load Balancing</t>
   </si>
@@ -1280,6 +1280,15 @@
   </si>
   <si>
     <t>EMR Serverless</t>
+  </si>
+  <si>
+    <t>Verified Permissions</t>
+  </si>
+  <si>
+    <t>Verified Access</t>
+  </si>
+  <si>
+    <t>KMS External Key Store (XKS)</t>
   </si>
 </sst>
 </file>
@@ -2068,11 +2077,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00D01EA-5C3E-F64B-8B7F-2EE6141A689A}">
-  <dimension ref="A1:R369"/>
+  <dimension ref="A1:R372"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -12008,34 +12017,24 @@
         <v>41</v>
       </c>
       <c r="B341" s="37" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C341" s="38" t="s">
-        <v>68</v>
+        <v>419</v>
       </c>
       <c r="D341" s="43"/>
       <c r="E341" s="43"/>
       <c r="F341" s="43"/>
-      <c r="G341" s="16">
-        <v>1</v>
-      </c>
-      <c r="H341" s="16">
-        <v>1</v>
-      </c>
+      <c r="G341" s="16"/>
+      <c r="H341" s="16"/>
       <c r="I341" s="16"/>
       <c r="J341" s="16"/>
-      <c r="K341" s="16">
-        <v>1</v>
-      </c>
+      <c r="K341" s="16"/>
       <c r="L341" s="16"/>
-      <c r="M341" s="16">
-        <v>1</v>
-      </c>
+      <c r="M341" s="16"/>
       <c r="N341" s="16"/>
       <c r="O341" s="16"/>
-      <c r="P341" s="16">
-        <v>1</v>
-      </c>
+      <c r="P341" s="16"/>
       <c r="Q341" s="16"/>
     </row>
     <row r="342" spans="1:18" x14ac:dyDescent="0.2">
@@ -12043,24 +12042,34 @@
         <v>41</v>
       </c>
       <c r="B342" s="37" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C342" s="38" t="s">
-        <v>398</v>
+        <v>68</v>
       </c>
       <c r="D342" s="43"/>
       <c r="E342" s="43"/>
       <c r="F342" s="43"/>
-      <c r="G342" s="16"/>
-      <c r="H342" s="16"/>
+      <c r="G342" s="16">
+        <v>1</v>
+      </c>
+      <c r="H342" s="16">
+        <v>1</v>
+      </c>
       <c r="I342" s="16"/>
       <c r="J342" s="16"/>
-      <c r="K342" s="16"/>
+      <c r="K342" s="16">
+        <v>1</v>
+      </c>
       <c r="L342" s="16"/>
-      <c r="M342" s="16"/>
+      <c r="M342" s="16">
+        <v>1</v>
+      </c>
       <c r="N342" s="16"/>
       <c r="O342" s="16"/>
-      <c r="P342" s="16"/>
+      <c r="P342" s="16">
+        <v>1</v>
+      </c>
       <c r="Q342" s="16"/>
     </row>
     <row r="343" spans="1:18" x14ac:dyDescent="0.2">
@@ -12071,38 +12080,22 @@
         <v>4</v>
       </c>
       <c r="C343" s="38" t="s">
-        <v>113</v>
+        <v>398</v>
       </c>
       <c r="D343" s="43"/>
       <c r="E343" s="43"/>
       <c r="F343" s="43"/>
-      <c r="G343" s="16">
-        <v>1</v>
-      </c>
-      <c r="H343" s="16">
-        <v>1</v>
-      </c>
-      <c r="I343" s="16">
-        <v>1</v>
-      </c>
-      <c r="J343" s="16">
-        <v>1</v>
-      </c>
-      <c r="K343" s="16">
-        <v>1</v>
-      </c>
-      <c r="L343" s="16">
-        <v>1</v>
-      </c>
+      <c r="G343" s="16"/>
+      <c r="H343" s="16"/>
+      <c r="I343" s="16"/>
+      <c r="J343" s="16"/>
+      <c r="K343" s="16"/>
+      <c r="L343" s="16"/>
       <c r="M343" s="16"/>
       <c r="N343" s="16"/>
       <c r="O343" s="16"/>
-      <c r="P343" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q343" s="16">
-        <v>1</v>
-      </c>
+      <c r="P343" s="16"/>
+      <c r="Q343" s="16"/>
     </row>
     <row r="344" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A344" s="36" t="s">
@@ -12112,89 +12105,95 @@
         <v>4</v>
       </c>
       <c r="C344" s="38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D344" s="43"/>
       <c r="E344" s="43"/>
       <c r="F344" s="43"/>
-      <c r="G344" s="16"/>
-      <c r="H344" s="16"/>
-      <c r="I344" s="16"/>
+      <c r="G344" s="16">
+        <v>1</v>
+      </c>
+      <c r="H344" s="16">
+        <v>1</v>
+      </c>
+      <c r="I344" s="16">
+        <v>1</v>
+      </c>
       <c r="J344" s="16">
         <v>1</v>
       </c>
       <c r="K344" s="16">
         <v>1</v>
       </c>
-      <c r="L344" s="16"/>
-      <c r="M344" s="16">
-        <v>1</v>
-      </c>
+      <c r="L344" s="16">
+        <v>1</v>
+      </c>
+      <c r="M344" s="16"/>
       <c r="N344" s="16"/>
       <c r="O344" s="16"/>
-      <c r="P344" s="16"/>
-      <c r="Q344" s="16"/>
-    </row>
-    <row r="345" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P344" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q344" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A345" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B345" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C345" s="59" t="s">
-        <v>412</v>
-      </c>
-      <c r="H345" s="43">
-        <v>1</v>
-      </c>
-      <c r="I345" s="43">
-        <v>1</v>
-      </c>
-      <c r="J345" s="43">
-        <v>1</v>
-      </c>
-      <c r="K345" s="43">
-        <v>1</v>
-      </c>
-      <c r="M345" s="43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="346" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C345" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="D345" s="43"/>
+      <c r="E345" s="43"/>
+      <c r="F345" s="43"/>
+      <c r="G345" s="16"/>
+      <c r="H345" s="16"/>
+      <c r="I345" s="16"/>
+      <c r="J345" s="16">
+        <v>1</v>
+      </c>
+      <c r="K345" s="16">
+        <v>1</v>
+      </c>
+      <c r="L345" s="16"/>
+      <c r="M345" s="16">
+        <v>1</v>
+      </c>
+      <c r="N345" s="16"/>
+      <c r="O345" s="16"/>
+      <c r="P345" s="16"/>
+      <c r="Q345" s="16"/>
+    </row>
+    <row r="346" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A346" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B346" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C346" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D346" s="43"/>
-      <c r="E346" s="43"/>
-      <c r="F346" s="43"/>
-      <c r="G346" s="16">
-        <v>1</v>
-      </c>
-      <c r="H346" s="16">
-        <v>1</v>
-      </c>
-      <c r="I346" s="16"/>
-      <c r="J346" s="16">
-        <v>1</v>
-      </c>
-      <c r="K346" s="16">
-        <v>1</v>
-      </c>
-      <c r="L346" s="16"/>
-      <c r="M346" s="16">
-        <v>1</v>
-      </c>
-      <c r="N346" s="16"/>
-      <c r="O346" s="16"/>
-      <c r="P346" s="16"/>
-      <c r="Q346" s="16"/>
+      <c r="C346" s="59" t="s">
+        <v>412</v>
+      </c>
+      <c r="H346" s="43">
+        <v>1</v>
+      </c>
+      <c r="I346" s="43">
+        <v>1</v>
+      </c>
+      <c r="J346" s="43">
+        <v>1</v>
+      </c>
+      <c r="K346" s="43">
+        <v>1</v>
+      </c>
+      <c r="M346" s="43">
+        <v>1</v>
+      </c>
     </row>
     <row r="347" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A347" s="36" t="s">
@@ -12204,7 +12203,7 @@
         <v>4</v>
       </c>
       <c r="C347" s="38" t="s">
-        <v>311</v>
+        <v>42</v>
       </c>
       <c r="D347" s="43"/>
       <c r="E347" s="43"/>
@@ -12215,18 +12214,14 @@
       <c r="H347" s="16">
         <v>1</v>
       </c>
-      <c r="I347" s="16">
-        <v>1</v>
-      </c>
+      <c r="I347" s="16"/>
       <c r="J347" s="16">
         <v>1</v>
       </c>
       <c r="K347" s="16">
         <v>1</v>
       </c>
-      <c r="L347" s="16">
-        <v>1</v>
-      </c>
+      <c r="L347" s="16"/>
       <c r="M347" s="16">
         <v>1</v>
       </c>
@@ -12236,14 +12231,14 @@
       <c r="Q347" s="16"/>
     </row>
     <row r="348" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A348" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B348" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C348" s="12" t="s">
-        <v>385</v>
+      <c r="A348" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B348" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C348" s="38" t="s">
+        <v>418</v>
       </c>
       <c r="D348" s="43"/>
       <c r="E348" s="43"/>
@@ -12259,17 +12254,16 @@
       <c r="O348" s="16"/>
       <c r="P348" s="16"/>
       <c r="Q348" s="16"/>
-      <c r="R348" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="349" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A349" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B349" s="39"/>
-      <c r="C349" s="12" t="s">
-        <v>365</v>
+      <c r="A349" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B349" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C349" s="38" t="s">
+        <v>417</v>
       </c>
       <c r="D349" s="43"/>
       <c r="E349" s="43"/>
@@ -12285,30 +12279,41 @@
       <c r="O349" s="16"/>
       <c r="P349" s="16"/>
       <c r="Q349" s="16"/>
-      <c r="R349" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="350" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A350" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B350" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C350" s="12" t="s">
-        <v>350</v>
+      <c r="A350" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B350" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C350" s="38" t="s">
+        <v>311</v>
       </c>
       <c r="D350" s="43"/>
       <c r="E350" s="43"/>
       <c r="F350" s="43"/>
-      <c r="G350" s="16"/>
-      <c r="H350" s="16"/>
-      <c r="I350" s="16"/>
-      <c r="J350" s="16"/>
-      <c r="K350" s="16"/>
-      <c r="L350" s="16"/>
-      <c r="M350" s="16"/>
+      <c r="G350" s="16">
+        <v>1</v>
+      </c>
+      <c r="H350" s="16">
+        <v>1</v>
+      </c>
+      <c r="I350" s="16">
+        <v>1</v>
+      </c>
+      <c r="J350" s="16">
+        <v>1</v>
+      </c>
+      <c r="K350" s="16">
+        <v>1</v>
+      </c>
+      <c r="L350" s="16">
+        <v>1</v>
+      </c>
+      <c r="M350" s="16">
+        <v>1</v>
+      </c>
       <c r="N350" s="16"/>
       <c r="O350" s="16"/>
       <c r="P350" s="16"/>
@@ -12319,41 +12324,25 @@
         <v>45</v>
       </c>
       <c r="B351" s="11" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C351" s="12" t="s">
-        <v>130</v>
+        <v>385</v>
       </c>
       <c r="D351" s="43"/>
       <c r="E351" s="43"/>
       <c r="F351" s="43"/>
-      <c r="G351" s="16">
-        <v>1</v>
-      </c>
-      <c r="H351" s="16">
-        <v>1</v>
-      </c>
-      <c r="I351" s="16">
-        <v>1</v>
-      </c>
-      <c r="J351" s="16">
-        <v>1</v>
-      </c>
-      <c r="K351" s="16">
-        <v>1</v>
-      </c>
-      <c r="L351" s="16">
-        <v>1</v>
-      </c>
+      <c r="G351" s="16"/>
+      <c r="H351" s="16"/>
+      <c r="I351" s="16"/>
+      <c r="J351" s="16"/>
+      <c r="K351" s="16"/>
+      <c r="L351" s="16"/>
       <c r="M351" s="16"/>
       <c r="N351" s="16"/>
       <c r="O351" s="16"/>
-      <c r="P351" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q351" s="16">
-        <v>1</v>
-      </c>
+      <c r="P351" s="16"/>
+      <c r="Q351" s="16"/>
       <c r="R351" s="2">
         <v>1</v>
       </c>
@@ -12362,11 +12351,9 @@
       <c r="A352" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B352" s="11" t="s">
-        <v>4</v>
-      </c>
+      <c r="B352" s="39"/>
       <c r="C352" s="12" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="D352" s="43"/>
       <c r="E352" s="43"/>
@@ -12394,74 +12381,76 @@
         <v>49</v>
       </c>
       <c r="C353" s="12" t="s">
-        <v>134</v>
+        <v>350</v>
       </c>
       <c r="D353" s="43"/>
       <c r="E353" s="43"/>
       <c r="F353" s="43"/>
-      <c r="G353" s="16">
-        <v>1</v>
-      </c>
-      <c r="H353" s="16">
-        <v>1</v>
-      </c>
-      <c r="I353" s="16">
-        <v>1</v>
-      </c>
-      <c r="J353" s="16">
-        <v>1</v>
-      </c>
-      <c r="K353" s="16">
-        <v>1</v>
-      </c>
-      <c r="L353" s="16">
-        <v>1</v>
-      </c>
+      <c r="G353" s="16"/>
+      <c r="H353" s="16"/>
+      <c r="I353" s="16"/>
+      <c r="J353" s="16"/>
+      <c r="K353" s="16"/>
+      <c r="L353" s="16"/>
       <c r="M353" s="16"/>
       <c r="N353" s="16"/>
-      <c r="O353" s="16">
-        <v>1</v>
-      </c>
+      <c r="O353" s="16"/>
       <c r="P353" s="16"/>
       <c r="Q353" s="16"/>
-      <c r="R353" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="354" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A354" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B354" s="11" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C354" s="12" t="s">
-        <v>228</v>
+        <v>130</v>
       </c>
       <c r="D354" s="43"/>
       <c r="E354" s="43"/>
       <c r="F354" s="43"/>
-      <c r="G354" s="16"/>
-      <c r="H354" s="16"/>
-      <c r="I354" s="16"/>
-      <c r="J354" s="16"/>
-      <c r="K354" s="16"/>
-      <c r="L354" s="16"/>
+      <c r="G354" s="16">
+        <v>1</v>
+      </c>
+      <c r="H354" s="16">
+        <v>1</v>
+      </c>
+      <c r="I354" s="16">
+        <v>1</v>
+      </c>
+      <c r="J354" s="16">
+        <v>1</v>
+      </c>
+      <c r="K354" s="16">
+        <v>1</v>
+      </c>
+      <c r="L354" s="16">
+        <v>1</v>
+      </c>
       <c r="M354" s="16"/>
       <c r="N354" s="16"/>
       <c r="O354" s="16"/>
-      <c r="P354" s="16"/>
-      <c r="Q354" s="16"/>
+      <c r="P354" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q354" s="16">
+        <v>1</v>
+      </c>
+      <c r="R354" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="355" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A355" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B355" s="11" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C355" s="12" t="s">
-        <v>399</v>
+        <v>364</v>
       </c>
       <c r="D355" s="43"/>
       <c r="E355" s="43"/>
@@ -12477,6 +12466,9 @@
       <c r="O355" s="16"/>
       <c r="P355" s="16"/>
       <c r="Q355" s="16"/>
+      <c r="R355" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="356" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A356" s="10" t="s">
@@ -12486,23 +12478,29 @@
         <v>49</v>
       </c>
       <c r="C356" s="12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D356" s="43"/>
       <c r="E356" s="43"/>
       <c r="F356" s="43"/>
-      <c r="G356" s="16"/>
+      <c r="G356" s="16">
+        <v>1</v>
+      </c>
       <c r="H356" s="16">
         <v>1</v>
       </c>
-      <c r="I356" s="16"/>
+      <c r="I356" s="16">
+        <v>1</v>
+      </c>
       <c r="J356" s="16">
         <v>1</v>
       </c>
       <c r="K356" s="16">
         <v>1</v>
       </c>
-      <c r="L356" s="16"/>
+      <c r="L356" s="16">
+        <v>1</v>
+      </c>
       <c r="M356" s="16"/>
       <c r="N356" s="16"/>
       <c r="O356" s="16">
@@ -12510,16 +12508,19 @@
       </c>
       <c r="P356" s="16"/>
       <c r="Q356" s="16"/>
+      <c r="R356" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="357" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A357" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B357" s="11" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C357" s="12" t="s">
-        <v>352</v>
+        <v>228</v>
       </c>
       <c r="D357" s="43"/>
       <c r="E357" s="43"/>
@@ -12544,7 +12545,7 @@
         <v>49</v>
       </c>
       <c r="C358" s="12" t="s">
-        <v>353</v>
+        <v>399</v>
       </c>
       <c r="D358" s="43"/>
       <c r="E358" s="43"/>
@@ -12569,7 +12570,7 @@
         <v>49</v>
       </c>
       <c r="C359" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D359" s="43"/>
       <c r="E359" s="43"/>
@@ -12593,9 +12594,6 @@
       </c>
       <c r="P359" s="16"/>
       <c r="Q359" s="16"/>
-      <c r="R359" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="360" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A360" s="10" t="s">
@@ -12605,41 +12603,22 @@
         <v>49</v>
       </c>
       <c r="C360" s="12" t="s">
-        <v>252</v>
+        <v>352</v>
       </c>
       <c r="D360" s="43"/>
       <c r="E360" s="43"/>
       <c r="F360" s="43"/>
-      <c r="G360" s="16">
-        <v>1</v>
-      </c>
-      <c r="H360" s="16">
-        <v>1</v>
-      </c>
-      <c r="I360" s="16">
-        <v>1</v>
-      </c>
-      <c r="J360" s="16">
-        <v>1</v>
-      </c>
-      <c r="K360" s="16">
-        <v>1</v>
-      </c>
+      <c r="G360" s="16"/>
+      <c r="H360" s="16"/>
+      <c r="I360" s="16"/>
+      <c r="J360" s="16"/>
+      <c r="K360" s="16"/>
       <c r="L360" s="16"/>
       <c r="M360" s="16"/>
-      <c r="N360" s="16">
-        <v>1</v>
-      </c>
+      <c r="N360" s="16"/>
       <c r="O360" s="16"/>
-      <c r="P360" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q360" s="16">
-        <v>1</v>
-      </c>
-      <c r="R360" s="2">
-        <v>1</v>
-      </c>
+      <c r="P360" s="16"/>
+      <c r="Q360" s="16"/>
     </row>
     <row r="361" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A361" s="10" t="s">
@@ -12649,41 +12628,22 @@
         <v>49</v>
       </c>
       <c r="C361" s="12" t="s">
-        <v>401</v>
+        <v>353</v>
       </c>
       <c r="D361" s="43"/>
       <c r="E361" s="43"/>
       <c r="F361" s="43"/>
-      <c r="G361" s="16">
-        <v>1</v>
-      </c>
-      <c r="H361" s="16">
-        <v>1</v>
-      </c>
-      <c r="I361" s="16">
-        <v>1</v>
-      </c>
-      <c r="J361" s="16">
-        <v>1</v>
-      </c>
-      <c r="K361" s="16">
-        <v>1</v>
-      </c>
+      <c r="G361" s="16"/>
+      <c r="H361" s="16"/>
+      <c r="I361" s="16"/>
+      <c r="J361" s="16"/>
+      <c r="K361" s="16"/>
       <c r="L361" s="16"/>
       <c r="M361" s="16"/>
-      <c r="N361" s="16">
-        <v>1</v>
-      </c>
+      <c r="N361" s="16"/>
       <c r="O361" s="16"/>
-      <c r="P361" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q361" s="16">
-        <v>1</v>
-      </c>
-      <c r="R361" s="2">
-        <v>1</v>
-      </c>
+      <c r="P361" s="16"/>
+      <c r="Q361" s="16"/>
     </row>
     <row r="362" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A362" s="10" t="s">
@@ -12693,20 +12653,16 @@
         <v>49</v>
       </c>
       <c r="C362" s="12" t="s">
-        <v>400</v>
+        <v>139</v>
       </c>
       <c r="D362" s="43"/>
       <c r="E362" s="43"/>
       <c r="F362" s="43"/>
-      <c r="G362" s="16">
-        <v>1</v>
-      </c>
+      <c r="G362" s="16"/>
       <c r="H362" s="16">
         <v>1</v>
       </c>
-      <c r="I362" s="16">
-        <v>1</v>
-      </c>
+      <c r="I362" s="16"/>
       <c r="J362" s="16">
         <v>1</v>
       </c>
@@ -12715,16 +12671,12 @@
       </c>
       <c r="L362" s="16"/>
       <c r="M362" s="16"/>
-      <c r="N362" s="16">
-        <v>1</v>
-      </c>
-      <c r="O362" s="16"/>
-      <c r="P362" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q362" s="16">
-        <v>1</v>
-      </c>
+      <c r="N362" s="16"/>
+      <c r="O362" s="16">
+        <v>1</v>
+      </c>
+      <c r="P362" s="16"/>
+      <c r="Q362" s="16"/>
       <c r="R362" s="2">
         <v>1</v>
       </c>
@@ -12737,7 +12689,7 @@
         <v>49</v>
       </c>
       <c r="C363" s="12" t="s">
-        <v>153</v>
+        <v>252</v>
       </c>
       <c r="D363" s="43"/>
       <c r="E363" s="43"/>
@@ -12757,18 +12709,12 @@
       <c r="K363" s="16">
         <v>1</v>
       </c>
-      <c r="L363" s="16">
-        <v>1</v>
-      </c>
-      <c r="M363" s="16">
-        <v>1</v>
-      </c>
+      <c r="L363" s="16"/>
+      <c r="M363" s="16"/>
       <c r="N363" s="16">
         <v>1</v>
       </c>
-      <c r="O363" s="16">
-        <v>1</v>
-      </c>
+      <c r="O363" s="16"/>
       <c r="P363" s="16">
         <v>1</v>
       </c>
@@ -12784,27 +12730,39 @@
         <v>45</v>
       </c>
       <c r="B364" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C364" s="52" t="s">
-        <v>119</v>
-      </c>
-      <c r="G364" s="40">
-        <v>1</v>
-      </c>
-      <c r="H364" s="40">
-        <v>1</v>
-      </c>
-      <c r="J364" s="40">
-        <v>1</v>
-      </c>
-      <c r="K364" s="40">
-        <v>1</v>
-      </c>
-      <c r="L364" s="40">
-        <v>1</v>
-      </c>
-      <c r="N364" s="40">
+        <v>49</v>
+      </c>
+      <c r="C364" s="12" t="s">
+        <v>401</v>
+      </c>
+      <c r="D364" s="43"/>
+      <c r="E364" s="43"/>
+      <c r="F364" s="43"/>
+      <c r="G364" s="16">
+        <v>1</v>
+      </c>
+      <c r="H364" s="16">
+        <v>1</v>
+      </c>
+      <c r="I364" s="16">
+        <v>1</v>
+      </c>
+      <c r="J364" s="16">
+        <v>1</v>
+      </c>
+      <c r="K364" s="16">
+        <v>1</v>
+      </c>
+      <c r="L364" s="16"/>
+      <c r="M364" s="16"/>
+      <c r="N364" s="16">
+        <v>1</v>
+      </c>
+      <c r="O364" s="16"/>
+      <c r="P364" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q364" s="16">
         <v>1</v>
       </c>
       <c r="R364" s="2">
@@ -12815,22 +12773,40 @@
       <c r="A365" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B365" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C365" s="53" t="s">
-        <v>302</v>
-      </c>
-      <c r="H365" s="40">
-        <v>1</v>
-      </c>
-      <c r="K365" s="40">
-        <v>1</v>
-      </c>
-      <c r="L365" s="40">
-        <v>1</v>
-      </c>
-      <c r="N365" s="40">
+      <c r="B365" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C365" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="D365" s="43"/>
+      <c r="E365" s="43"/>
+      <c r="F365" s="43"/>
+      <c r="G365" s="16">
+        <v>1</v>
+      </c>
+      <c r="H365" s="16">
+        <v>1</v>
+      </c>
+      <c r="I365" s="16">
+        <v>1</v>
+      </c>
+      <c r="J365" s="16">
+        <v>1</v>
+      </c>
+      <c r="K365" s="16">
+        <v>1</v>
+      </c>
+      <c r="L365" s="16"/>
+      <c r="M365" s="16"/>
+      <c r="N365" s="16">
+        <v>1</v>
+      </c>
+      <c r="O365" s="16"/>
+      <c r="P365" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q365" s="16">
         <v>1</v>
       </c>
       <c r="R365" s="2">
@@ -12841,22 +12817,46 @@
       <c r="A366" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B366" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C366" s="53" t="s">
-        <v>301</v>
-      </c>
-      <c r="H366" s="40">
-        <v>1</v>
-      </c>
-      <c r="K366" s="40">
-        <v>1</v>
-      </c>
-      <c r="L366" s="40">
-        <v>1</v>
-      </c>
-      <c r="N366" s="40">
+      <c r="B366" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C366" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D366" s="43"/>
+      <c r="E366" s="43"/>
+      <c r="F366" s="43"/>
+      <c r="G366" s="16">
+        <v>1</v>
+      </c>
+      <c r="H366" s="16">
+        <v>1</v>
+      </c>
+      <c r="I366" s="16">
+        <v>1</v>
+      </c>
+      <c r="J366" s="16">
+        <v>1</v>
+      </c>
+      <c r="K366" s="16">
+        <v>1</v>
+      </c>
+      <c r="L366" s="16">
+        <v>1</v>
+      </c>
+      <c r="M366" s="16">
+        <v>1</v>
+      </c>
+      <c r="N366" s="16">
+        <v>1</v>
+      </c>
+      <c r="O366" s="16">
+        <v>1</v>
+      </c>
+      <c r="P366" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q366" s="16">
         <v>1</v>
       </c>
       <c r="R366" s="2">
@@ -12867,13 +12867,19 @@
       <c r="A367" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B367" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C367" s="53" t="s">
-        <v>300</v>
+      <c r="B367" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C367" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="G367" s="40">
+        <v>1</v>
       </c>
       <c r="H367" s="40">
+        <v>1</v>
+      </c>
+      <c r="J367" s="40">
         <v>1</v>
       </c>
       <c r="K367" s="40">
@@ -12897,7 +12903,7 @@
         <v>4</v>
       </c>
       <c r="C368" s="53" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H368" s="40">
         <v>1</v>
@@ -12923,33 +12929,111 @@
         <v>4</v>
       </c>
       <c r="C369" s="53" t="s">
+        <v>301</v>
+      </c>
+      <c r="H369" s="40">
+        <v>1</v>
+      </c>
+      <c r="K369" s="40">
+        <v>1</v>
+      </c>
+      <c r="L369" s="40">
+        <v>1</v>
+      </c>
+      <c r="N369" s="40">
+        <v>1</v>
+      </c>
+      <c r="R369" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A370" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B370" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C370" s="53" t="s">
+        <v>300</v>
+      </c>
+      <c r="H370" s="40">
+        <v>1</v>
+      </c>
+      <c r="K370" s="40">
+        <v>1</v>
+      </c>
+      <c r="L370" s="40">
+        <v>1</v>
+      </c>
+      <c r="N370" s="40">
+        <v>1</v>
+      </c>
+      <c r="R370" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="371" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A371" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B371" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C371" s="53" t="s">
+        <v>303</v>
+      </c>
+      <c r="H371" s="40">
+        <v>1</v>
+      </c>
+      <c r="K371" s="40">
+        <v>1</v>
+      </c>
+      <c r="L371" s="40">
+        <v>1</v>
+      </c>
+      <c r="N371" s="40">
+        <v>1</v>
+      </c>
+      <c r="R371" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="372" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A372" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B372" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C372" s="53" t="s">
         <v>304</v>
       </c>
-      <c r="H369" s="40">
-        <v>1</v>
-      </c>
-      <c r="K369" s="40">
-        <v>1</v>
-      </c>
-      <c r="L369" s="40">
-        <v>1</v>
-      </c>
-      <c r="N369" s="40">
-        <v>1</v>
-      </c>
-      <c r="R369" s="2">
+      <c r="H372" s="40">
+        <v>1</v>
+      </c>
+      <c r="K372" s="40">
+        <v>1</v>
+      </c>
+      <c r="L372" s="40">
+        <v>1</v>
+      </c>
+      <c r="N372" s="40">
+        <v>1</v>
+      </c>
+      <c r="R372" s="2">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R369" xr:uid="{F00D01EA-5C3E-F64B-8B7F-2EE6141A689A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R369">
-      <sortCondition ref="A1:A369"/>
+  <autoFilter ref="A1:R372" xr:uid="{F00D01EA-5C3E-F64B-8B7F-2EE6141A689A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R372">
+      <sortCondition ref="A1:A372"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q363">
-    <sortCondition ref="A2:A363"/>
-    <sortCondition ref="C2:C363"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q366">
+    <sortCondition ref="A2:A366"/>
+    <sortCondition ref="C2:C366"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C112" r:id="rId1" display="https://aws.amazon.com/amplify/" xr:uid="{DD07C612-9881-1744-BD8F-2791C5BF0A5F}"/>
@@ -13016,24 +13100,24 @@
     <hyperlink ref="C230" r:id="rId62" display="https://aws.amazon.com/proton/" xr:uid="{73BECBB6-D4BE-F445-97BF-0A1D62BCA194}"/>
     <hyperlink ref="C232" r:id="rId63" display="https://aws.amazon.com/ram/" xr:uid="{F8E211FB-42AB-6848-88B7-49CC2A833913}"/>
     <hyperlink ref="C320" r:id="rId64" display="https://aws.amazon.com/robomaker/" xr:uid="{DBD68496-4CE8-804C-B893-9CFFB849F53A}"/>
-    <hyperlink ref="C343" r:id="rId65" display="https://aws.amazon.com/secrets-manager/" xr:uid="{632A5D67-D598-184C-AB9B-96F30896117D}"/>
-    <hyperlink ref="C344" r:id="rId66" display="https://aws.amazon.com/security-hub/" xr:uid="{342A4832-F3A0-DB4D-840C-8118FD830399}"/>
+    <hyperlink ref="C344" r:id="rId65" display="https://aws.amazon.com/secrets-manager/" xr:uid="{632A5D67-D598-184C-AB9B-96F30896117D}"/>
+    <hyperlink ref="C345" r:id="rId66" display="https://aws.amazon.com/security-hub/" xr:uid="{342A4832-F3A0-DB4D-840C-8118FD830399}"/>
     <hyperlink ref="C294" r:id="rId67" display="https://aws.amazon.com/server-migration-service/" xr:uid="{9446514E-0CE8-EC41-A9F1-0DC1FB7ADA55}"/>
     <hyperlink ref="C62" r:id="rId68" display="https://aws.amazon.com/serverless/serverlessrepo/" xr:uid="{8F7AC4BC-9A37-EC4F-8183-7D7404D19E14}"/>
     <hyperlink ref="C234" r:id="rId69" display="https://aws.amazon.com/servicecatalog/" xr:uid="{2D2653B1-3D13-014A-9B9C-2386E2577635}"/>
-    <hyperlink ref="C346" r:id="rId70" display="https://aws.amazon.com/shield/" xr:uid="{76E091F3-F618-A648-879F-3F09BEBFABFD}"/>
+    <hyperlink ref="C347" r:id="rId70" display="https://aws.amazon.com/shield/" xr:uid="{76E091F3-F618-A648-879F-3F09BEBFABFD}"/>
     <hyperlink ref="C337" r:id="rId71" display="IAM Identity Center (SSO)" xr:uid="{A8360283-DE5C-1140-A85B-F33A2D6F72B8}"/>
     <hyperlink ref="C295" r:id="rId72" display="https://aws.amazon.com/snowball/" xr:uid="{8A7E1B57-5F26-F64E-853D-BDD63390D5E6}"/>
     <hyperlink ref="C297" r:id="rId73" display="https://aws.amazon.com/snowmobile/" xr:uid="{62B7D92F-3C96-DA44-9F02-BCC308391061}"/>
     <hyperlink ref="C44" r:id="rId74" display="https://aws.amazon.com/step-functions/details/" xr:uid="{10824B81-0A5F-634D-84E6-9D2ADE3A6B39}"/>
-    <hyperlink ref="C364" r:id="rId75" display="https://aws.amazon.com/storagegateway/" xr:uid="{7BF17EFE-FF03-1D4A-BE9E-1FA982DA5C2A}"/>
+    <hyperlink ref="C367" r:id="rId75" display="https://aws.amazon.com/storagegateway/" xr:uid="{7BF17EFE-FF03-1D4A-BE9E-1FA982DA5C2A}"/>
     <hyperlink ref="C94" r:id="rId76" display="https://aws.amazon.com/premiumsupport/" xr:uid="{A5466C95-EFB7-3944-9E29-8D19BB6E169F}"/>
     <hyperlink ref="C256" r:id="rId77" display="https://aws.amazon.com/systems-manager/" xr:uid="{D6C17500-BE92-C444-BA4A-7116B75319D3}"/>
     <hyperlink ref="C298" r:id="rId78" display="https://aws.amazon.com/aws-transfer-family/" xr:uid="{F0069BD4-8633-FB4B-8185-293CB3193797}"/>
     <hyperlink ref="C315" r:id="rId79" display="https://aws.amazon.com/transit-gateway/" xr:uid="{2C10B2F7-EEE3-3444-A855-B387D48706EA}"/>
     <hyperlink ref="C257" r:id="rId80" display="https://aws.amazon.com/premiumsupport/trustedadvisor/" xr:uid="{436ECB3D-7EFE-764A-B2E3-3CF79C97B742}"/>
     <hyperlink ref="C318" r:id="rId81" display="https://aws.amazon.com/vpn/" xr:uid="{5F2B553B-98BD-8D4B-849C-55A6F659C6B1}"/>
-    <hyperlink ref="C347" r:id="rId82" display="https://aws.amazon.com/waf/" xr:uid="{CF739D06-0B1B-6B46-91CF-6EE57FF09613}"/>
+    <hyperlink ref="C350" r:id="rId82" display="https://aws.amazon.com/waf/" xr:uid="{CF739D06-0B1B-6B46-91CF-6EE57FF09613}"/>
     <hyperlink ref="C258" r:id="rId83" display="https://aws.amazon.com/well-architected-tool" xr:uid="{81A34672-555C-B74A-9D7B-58590B7D3C75}"/>
     <hyperlink ref="C142" r:id="rId84" display="https://aws.amazon.com/xray/" xr:uid="{91A2B229-E348-8B4C-AF47-A5192DE45AEC}"/>
     <hyperlink ref="C300" r:id="rId85" display="https://aws.amazon.com/api-gateway/" xr:uid="{81259B3E-1AB3-F64C-B232-9643470BBB0C}"/>
@@ -13054,18 +13138,18 @@
     <hyperlink ref="C100" r:id="rId100" display="https://aws.amazon.com/documentdb/" xr:uid="{E9BE873B-93B3-744C-82A3-AE676C942786}"/>
     <hyperlink ref="C101" r:id="rId101" display="https://aws.amazon.com/dynamodb/" xr:uid="{667C0B17-E586-7843-9ABA-2156F328D1C2}"/>
     <hyperlink ref="C104" r:id="rId102" display="https://aws.amazon.com/elasticache/" xr:uid="{0D3B6893-EB9F-F441-97F2-EAE3A531E741}"/>
-    <hyperlink ref="C351" r:id="rId103" display="https://aws.amazon.com/ebs/" xr:uid="{6475A1BA-F9EA-3643-A91C-960971815276}"/>
+    <hyperlink ref="C354" r:id="rId103" display="https://aws.amazon.com/ebs/" xr:uid="{6475A1BA-F9EA-3643-A91C-960971815276}"/>
     <hyperlink ref="C55" r:id="rId104" xr:uid="{F6BE2D25-6B4D-D545-BEF5-6353621F7D77}"/>
     <hyperlink ref="C71" r:id="rId105" display="https://aws.amazon.com/ecr/" xr:uid="{4DB8575D-FD4E-F24B-9A6D-4B237DEB4216}"/>
     <hyperlink ref="C72" r:id="rId106" display="https://aws.amazon.com/ecs/" xr:uid="{2A857716-DB7F-4D4C-9C3A-923E359FCE4B}"/>
-    <hyperlink ref="C353" r:id="rId107" display="https://aws.amazon.com/efs/" xr:uid="{17293663-847A-2945-BEEE-DB5C14186604}"/>
+    <hyperlink ref="C356" r:id="rId107" display="https://aws.amazon.com/efs/" xr:uid="{17293663-847A-2945-BEEE-DB5C14186604}"/>
     <hyperlink ref="C177" r:id="rId108" display="https://aws.amazon.com/elastic-inference/" xr:uid="{D7F32AC2-662A-044F-8D07-6056298BD732}"/>
     <hyperlink ref="C73" r:id="rId109" display="https://aws.amazon.com/eks" xr:uid="{8EA95DB8-FAF6-354A-8701-9BC26B99AF7A}"/>
     <hyperlink ref="C6" r:id="rId110" display="https://aws.amazon.com/emr/" xr:uid="{45F7CBE2-565C-A24D-A38F-B3A8800D8B65}"/>
     <hyperlink ref="C28" r:id="rId111" display="Elasticsearch Service (ES) / OpenSearch Service" xr:uid="{6AF99F4A-A394-8249-8B46-B05EDE624400}"/>
     <hyperlink ref="C38" r:id="rId112" display="https://aws.amazon.com/eventbridge/" xr:uid="{66CE333B-4CBB-9246-B3B7-51C615E2BFF5}"/>
-    <hyperlink ref="C356" r:id="rId113" display="https://aws.amazon.com/fsx/lustre/" xr:uid="{723E4B6B-4225-F149-A1D1-0C9ED96BB728}"/>
-    <hyperlink ref="C359" r:id="rId114" display="https://aws.amazon.com/fsx/windows/" xr:uid="{1B6B9E68-B13B-3B45-B1A5-A8F3F5BDE985}"/>
+    <hyperlink ref="C359" r:id="rId113" display="https://aws.amazon.com/fsx/lustre/" xr:uid="{723E4B6B-4225-F149-A1D1-0C9ED96BB728}"/>
+    <hyperlink ref="C362" r:id="rId114" display="https://aws.amazon.com/fsx/windows/" xr:uid="{1B6B9E68-B13B-3B45-B1A5-A8F3F5BDE985}"/>
     <hyperlink ref="C178" r:id="rId115" display="https://aws.amazon.com/forecast/" xr:uid="{1F07E3AD-D0E3-4442-9220-92E85E3DF861}"/>
     <hyperlink ref="C179" r:id="rId116" display="https://aws.amazon.com/fraud-detector/" xr:uid="{A16ABA87-0E9D-1749-BE3E-718E7599E24B}"/>
     <hyperlink ref="C148" r:id="rId117" display="https://aws.amazon.com/gamelift/" xr:uid="{ABE766D8-2E8B-B341-9103-F503839AC514}"/>
@@ -13081,7 +13165,7 @@
     <hyperlink ref="C182" r:id="rId127" display="https://aws.amazon.com/lookout-for-vision/" xr:uid="{56891F15-488A-2D4F-957F-9C19DBC09E8C}"/>
     <hyperlink ref="C150" r:id="rId128" display="https://aws.amazon.com/lumberyard/" xr:uid="{0793FA7F-F861-E448-B351-2625AB793E29}"/>
     <hyperlink ref="C40" r:id="rId129" display="https://aws.amazon.com/amazon-mq/" xr:uid="{8F7E8190-F83B-7E45-9B55-465E1F7C79F3}"/>
-    <hyperlink ref="C341" r:id="rId130" display="https://aws.amazon.com/macie/" xr:uid="{0A9A9C7B-64FF-4944-8B73-82D7A54412E2}"/>
+    <hyperlink ref="C342" r:id="rId130" display="https://aws.amazon.com/macie/" xr:uid="{0A9A9C7B-64FF-4944-8B73-82D7A54412E2}"/>
     <hyperlink ref="C26" r:id="rId131" display="https://aws.amazon.com/msk/" xr:uid="{46024F01-6B35-0740-B92F-18BA0D596F3D}"/>
     <hyperlink ref="C39" r:id="rId132" display="https://aws.amazon.com/managed-workflows-for-apache-airflow/" xr:uid="{E7D50CE9-B395-AE40-B3BD-7B31072C139C}"/>
     <hyperlink ref="C107" r:id="rId133" display="https://aws.amazon.com/neptune/" xr:uid="{35EB7CA9-2F10-7E4E-9B05-D1C561AFFA79}"/>
@@ -13097,7 +13181,7 @@
     <hyperlink ref="C98" r:id="rId143" display="https://aws.amazon.com/ses/" xr:uid="{708BC6D8-3F72-374C-AB65-9002B2EB5C60}"/>
     <hyperlink ref="C41" r:id="rId144" display="https://aws.amazon.com/sns/" xr:uid="{2A7374BD-4C80-7C42-9E56-E3671DF3D17F}"/>
     <hyperlink ref="C42" r:id="rId145" display="https://aws.amazon.com/sqs/" xr:uid="{7EC87AB6-C5A3-0F4B-915C-BD9EF4201FD5}"/>
-    <hyperlink ref="C363" r:id="rId146" display="https://aws.amazon.com/s3/" xr:uid="{CD425C97-24D5-9747-8B23-DF9DD7A486F9}"/>
+    <hyperlink ref="C366" r:id="rId146" display="https://aws.amazon.com/s3/" xr:uid="{CD425C97-24D5-9747-8B23-DF9DD7A486F9}"/>
     <hyperlink ref="C43" r:id="rId147" display="https://aws.amazon.com/swf/" xr:uid="{631F304E-E46F-644E-8407-57836778A272}"/>
     <hyperlink ref="C152" r:id="rId148" display="https://aws.amazon.com/sumerian/" xr:uid="{1F8D41FC-B82F-8C44-A79F-AA91C3811E29}"/>
     <hyperlink ref="C206" r:id="rId149" display="https://aws.amazon.com/textract" xr:uid="{E50E8082-94C1-7947-963B-3A384A890F42}"/>
@@ -13107,13 +13191,13 @@
     <hyperlink ref="C209" r:id="rId153" display="https://aws.amazon.com/translate/" xr:uid="{D94B1850-F477-024B-8A15-72298FF44F81}"/>
     <hyperlink ref="C316" r:id="rId154" display="https://aws.amazon.com/vpc/" xr:uid="{81704202-B35B-314F-9611-62D10520486C}"/>
     <hyperlink ref="C145" r:id="rId155" display="https://aws.amazon.com/worklink/" xr:uid="{A564F6A5-A25E-984E-AB0E-10859F299F79}"/>
-    <hyperlink ref="C349" r:id="rId156" display="https://aws.amazon.com/cloudendure-disaster-recovery/" xr:uid="{19E2670B-B70B-2246-875A-A798E313AD4C}"/>
+    <hyperlink ref="C352" r:id="rId156" display="https://aws.amazon.com/cloudendure-disaster-recovery/" xr:uid="{19E2670B-B70B-2246-875A-A798E313AD4C}"/>
     <hyperlink ref="C283" r:id="rId157" display="https://aws.amazon.com/cloudendure-migration/" xr:uid="{3011454A-BA14-2640-A5B0-1665DE5015EB}"/>
     <hyperlink ref="C307" r:id="rId158" display="https://aws.amazon.com/elasticloadbalancing/" xr:uid="{48C41A56-7B49-954B-8607-BA52CE86305D}"/>
     <hyperlink ref="C153" r:id="rId159" display="https://aws.amazon.com/freertos/" xr:uid="{9A951967-4675-1546-8716-0568BF98D1CE}"/>
     <hyperlink ref="C64" r:id="rId160" display="https://aws.amazon.com/vmware/" xr:uid="{1D088AE8-27BE-C042-AB38-9D218A238493}"/>
     <hyperlink ref="C58" r:id="rId161" display="https://aws.amazon.com/ec2/" xr:uid="{A67A7092-80C0-9A4E-A55B-97FA160377E8}"/>
-    <hyperlink ref="C361" r:id="rId162" display="S3 Glacier" xr:uid="{9237F063-BA80-DC44-882A-D4F7F6FD5EE9}"/>
+    <hyperlink ref="C364" r:id="rId162" display="S3 Glacier" xr:uid="{9237F063-BA80-DC44-882A-D4F7F6FD5EE9}"/>
     <hyperlink ref="C132" r:id="rId163" xr:uid="{75CD952A-625F-DE4E-B2D6-41E51DC1F7E3}"/>
     <hyperlink ref="C45" r:id="rId164" display="Managed Blockchain" xr:uid="{49E4FD14-55A4-2E46-8EFF-5EF1766DCF38}"/>
     <hyperlink ref="C296" r:id="rId165" xr:uid="{7054BAB5-94B7-0C4D-A749-E850E72E4B65}"/>
@@ -13129,7 +13213,7 @@
     <hyperlink ref="C65" r:id="rId175" xr:uid="{005354BD-081E-9E46-8937-381CB8592473}"/>
     <hyperlink ref="C70" r:id="rId176" xr:uid="{1CFA07FC-268F-C84D-B8E8-D13B2E092826}"/>
     <hyperlink ref="C224" r:id="rId177" xr:uid="{667DCA05-C10B-394B-ADBD-C91C39C8EFA9}"/>
-    <hyperlink ref="C354" r:id="rId178" xr:uid="{19712BF9-B0E9-FC4A-855C-37C622207421}"/>
+    <hyperlink ref="C357" r:id="rId178" xr:uid="{19712BF9-B0E9-FC4A-855C-37C622207421}"/>
     <hyperlink ref="C120" r:id="rId179" xr:uid="{532F9FAB-7588-934A-BECA-94DB57B3EA86}"/>
     <hyperlink ref="C115" r:id="rId180" xr:uid="{03EA6A9E-9AED-E449-AEAE-E07C9D687ADF}"/>
     <hyperlink ref="C141" r:id="rId181" xr:uid="{1A9B8E63-391D-0446-8004-324356B6D2C7}"/>
@@ -13163,7 +13247,7 @@
     <hyperlink ref="C243" r:id="rId209" xr:uid="{D7F493BC-3996-E14D-8B4E-AF698AF15CF3}"/>
     <hyperlink ref="C249" r:id="rId210" xr:uid="{158C22B5-B282-0E45-819B-E1F6D3588EB5}"/>
     <hyperlink ref="C244" r:id="rId211" xr:uid="{060EF427-1526-CB41-B8B7-D967487671FE}"/>
-    <hyperlink ref="C360" r:id="rId212" display="S3 Glacier" xr:uid="{69E65928-2461-9D41-874A-E2DD597C93F4}"/>
+    <hyperlink ref="C363" r:id="rId212" display="S3 Glacier" xr:uid="{69E65928-2461-9D41-874A-E2DD597C93F4}"/>
     <hyperlink ref="C195" r:id="rId213" xr:uid="{985BD89A-8A6D-3646-8654-90328345A506}"/>
     <hyperlink ref="C172" r:id="rId214" xr:uid="{590CE714-967E-A245-B8FF-739BCA3B026A}"/>
     <hyperlink ref="C173" r:id="rId215" xr:uid="{1D9605EA-560D-C04A-9C84-34D242F7CD14}"/>
@@ -13224,11 +13308,11 @@
     <hyperlink ref="C278" r:id="rId270" xr:uid="{3B6EA2BE-9E87-CD43-BD86-90EF411A17C9}"/>
     <hyperlink ref="C279" r:id="rId271" xr:uid="{BE5AE3F2-6AF4-FB45-A4C7-58EE1FA83493}"/>
     <hyperlink ref="C280" r:id="rId272" xr:uid="{9F9A6701-301A-8946-8181-9D1074CEB3F6}"/>
-    <hyperlink ref="C369" r:id="rId273" display="Storage Gateway - Volume Gateway" xr:uid="{D2EC8952-5BC9-2B49-B394-D7BE012603FF}"/>
-    <hyperlink ref="C367" r:id="rId274" xr:uid="{1B5D263F-5321-B54A-BF60-2932447DCE26}"/>
-    <hyperlink ref="C365" r:id="rId275" display="Storage Gateway - FSx File Gateway" xr:uid="{2125FCAA-C46E-224B-8BE0-19D32D161491}"/>
-    <hyperlink ref="C366" r:id="rId276" display="Storage Gateway - S3 File Gateway" xr:uid="{96B9D02E-E08D-3E44-9C8E-08A2BE24E99A}"/>
-    <hyperlink ref="C368" r:id="rId277" display="Storage Gateway - Volume Gateway" xr:uid="{FFBC4DD5-5D45-9B42-A545-70A2598E87B0}"/>
+    <hyperlink ref="C372" r:id="rId273" display="Storage Gateway - Volume Gateway" xr:uid="{D2EC8952-5BC9-2B49-B394-D7BE012603FF}"/>
+    <hyperlink ref="C370" r:id="rId274" xr:uid="{1B5D263F-5321-B54A-BF60-2932447DCE26}"/>
+    <hyperlink ref="C368" r:id="rId275" display="Storage Gateway - FSx File Gateway" xr:uid="{2125FCAA-C46E-224B-8BE0-19D32D161491}"/>
+    <hyperlink ref="C369" r:id="rId276" display="Storage Gateway - S3 File Gateway" xr:uid="{96B9D02E-E08D-3E44-9C8E-08A2BE24E99A}"/>
+    <hyperlink ref="C371" r:id="rId277" display="Storage Gateway - Volume Gateway" xr:uid="{FFBC4DD5-5D45-9B42-A545-70A2598E87B0}"/>
     <hyperlink ref="C32" r:id="rId278" xr:uid="{F8A9F9A7-CC98-EC42-8596-0253E0A2BB97}"/>
     <hyperlink ref="C31" r:id="rId279" xr:uid="{8B655CFD-0968-7140-84E8-2070B49F002B}"/>
     <hyperlink ref="C35" r:id="rId280" xr:uid="{FD22D76A-0562-0640-85D0-C48AA580C483}"/>
@@ -13238,7 +13322,7 @@
     <hyperlink ref="C143" r:id="rId284" xr:uid="{5961D4D9-3072-2149-961B-0C10629539E7}"/>
     <hyperlink ref="C106" r:id="rId285" xr:uid="{863934C0-971A-AF48-A43D-B4B914AECC39}"/>
     <hyperlink ref="C220" r:id="rId286" xr:uid="{3295CEB8-10D1-5A43-BEA9-DF5FD886C0AB}"/>
-    <hyperlink ref="C357" r:id="rId287" display="Amazon FSx for NetApp ONTAP" xr:uid="{4F9FE344-D5EC-AC40-97FF-2F5F45F27D96}"/>
+    <hyperlink ref="C360" r:id="rId287" display="Amazon FSx for NetApp ONTAP" xr:uid="{4F9FE344-D5EC-AC40-97FF-2F5F45F27D96}"/>
     <hyperlink ref="C240" r:id="rId288" xr:uid="{AEDB8326-231C-C744-8B10-AF02B678D9B4}"/>
     <hyperlink ref="C21" r:id="rId289" xr:uid="{2E249962-989F-944F-B761-2BAA0EC7CAEC}"/>
     <hyperlink ref="C210" r:id="rId290" xr:uid="{DCE5737A-9A5B-DC4D-850F-450E2D238525}"/>
@@ -13268,9 +13352,9 @@
     <hyperlink ref="C166" r:id="rId314" xr:uid="{31C0844F-7C3B-2D40-BFE8-59E8221E3954}"/>
     <hyperlink ref="C162" r:id="rId315" xr:uid="{54A2747E-43BA-F045-9C52-0FB8E93DA59A}"/>
     <hyperlink ref="C75" r:id="rId316" xr:uid="{1EB66100-17E6-1342-A186-2BA2C2F63D22}"/>
-    <hyperlink ref="C350" r:id="rId317" xr:uid="{DB538155-C3BB-2A40-8FD1-CA65D903A17D}"/>
+    <hyperlink ref="C353" r:id="rId317" xr:uid="{DB538155-C3BB-2A40-8FD1-CA65D903A17D}"/>
     <hyperlink ref="C161" r:id="rId318" xr:uid="{C3A4EFBA-B189-BD45-BFF4-A1CD0FD8C94F}"/>
-    <hyperlink ref="C358" r:id="rId319" xr:uid="{88BA82AB-CEFC-3744-A41B-1FD7D1E7136C}"/>
+    <hyperlink ref="C361" r:id="rId319" xr:uid="{88BA82AB-CEFC-3744-A41B-1FD7D1E7136C}"/>
     <hyperlink ref="C136" r:id="rId320" xr:uid="{8DA90EA8-849B-1B49-A28C-2A2F266777EE}"/>
     <hyperlink ref="C198" r:id="rId321" xr:uid="{FE15D563-8EB3-6F43-BE1A-57E5433E3D5C}"/>
     <hyperlink ref="C202" r:id="rId322" xr:uid="{6C62A9C8-F029-FD4F-9476-C123AA75F8CA}"/>
@@ -13282,7 +13366,7 @@
     <hyperlink ref="C151" r:id="rId328" xr:uid="{DA0855F0-F663-864F-A06E-E87C9E061AF4}"/>
     <hyperlink ref="C236" r:id="rId329" xr:uid="{CB383B55-0E52-B947-A592-980271C8692F}"/>
     <hyperlink ref="C235" r:id="rId330" xr:uid="{4F9CF5F4-FC6C-9541-8599-DC150894B479}"/>
-    <hyperlink ref="C352" r:id="rId331" xr:uid="{CA40C680-0DBD-4343-8DE5-E090CB8817CA}"/>
+    <hyperlink ref="C355" r:id="rId331" xr:uid="{CA40C680-0DBD-4343-8DE5-E090CB8817CA}"/>
     <hyperlink ref="C246" r:id="rId332" xr:uid="{D586CA6E-E909-E844-A264-3987E2724DC4}"/>
     <hyperlink ref="C146" r:id="rId333" xr:uid="{C8735485-A0EF-E24F-8279-22CB0E8428F6}"/>
     <hyperlink ref="C144" r:id="rId334" xr:uid="{5AC9EBB0-8920-8744-A148-D68938ACC8E8}"/>
@@ -13295,7 +13379,7 @@
     <hyperlink ref="C149" r:id="rId341" xr:uid="{0D933DDA-AB72-1640-BEBC-718751BE3F53}"/>
     <hyperlink ref="C85" r:id="rId342" xr:uid="{07BF52D4-5452-B34A-A03C-22767C637C7A}"/>
     <hyperlink ref="C333" r:id="rId343" display="AWS Encryption SDK" xr:uid="{33F5E068-1939-6946-A05C-520BF7F5E73D}"/>
-    <hyperlink ref="C348" r:id="rId344" xr:uid="{17414EBC-16B7-5042-9A20-53B1F60B49D6}"/>
+    <hyperlink ref="C351" r:id="rId344" xr:uid="{17414EBC-16B7-5042-9A20-53B1F60B49D6}"/>
     <hyperlink ref="C87" r:id="rId345" xr:uid="{49BDB63D-5793-7B41-8772-615181B6C834}"/>
     <hyperlink ref="C231" r:id="rId346" xr:uid="{4D966601-2D59-F04E-9495-8AA46ED9EE78}"/>
     <hyperlink ref="C252" r:id="rId347" xr:uid="{C10A4ED2-003D-7E4D-BE98-CECF30AF4344}"/>
@@ -13304,9 +13388,9 @@
     <hyperlink ref="C83" r:id="rId350" xr:uid="{D3C65AFD-BAD4-AA4E-BE9E-F8F69A6E7034}"/>
     <hyperlink ref="C140" r:id="rId351" xr:uid="{C34DE960-4123-5B4C-8754-CF42F1139B71}"/>
     <hyperlink ref="C119" r:id="rId352" xr:uid="{4D37DCA5-E332-7D43-ADF7-343653A50F60}"/>
-    <hyperlink ref="C342" r:id="rId353" xr:uid="{D96F285C-B638-7E41-B6F5-6FC9047BE3EF}"/>
-    <hyperlink ref="C355" r:id="rId354" xr:uid="{23EAC66D-29B2-0B4A-B439-4EE056114072}"/>
-    <hyperlink ref="C362" r:id="rId355" display="S3 Glacier" xr:uid="{85EA50A7-14B2-D149-A253-41B939F41318}"/>
+    <hyperlink ref="C343" r:id="rId353" xr:uid="{D96F285C-B638-7E41-B6F5-6FC9047BE3EF}"/>
+    <hyperlink ref="C358" r:id="rId354" xr:uid="{23EAC66D-29B2-0B4A-B439-4EE056114072}"/>
+    <hyperlink ref="C365" r:id="rId355" display="S3 Glacier" xr:uid="{85EA50A7-14B2-D149-A253-41B939F41318}"/>
     <hyperlink ref="C299" r:id="rId356" xr:uid="{5924D0B4-C3ED-7141-9DB4-F738AAAED8FD}"/>
     <hyperlink ref="C128" r:id="rId357" xr:uid="{0E05A36D-6E61-794C-94C0-8D1445341816}"/>
     <hyperlink ref="C79" r:id="rId358" xr:uid="{7477CB6A-F100-A34F-9008-B1BFB9967DA7}"/>
@@ -13316,11 +13400,14 @@
     <hyperlink ref="C50" r:id="rId362" xr:uid="{07941932-04CA-D14D-B516-833FCD650A67}"/>
     <hyperlink ref="C63" r:id="rId363" xr:uid="{438F4E0F-2656-3B4B-A75B-4361FF393940}"/>
     <hyperlink ref="C5" r:id="rId364" xr:uid="{3E5A0494-CA0B-014F-A243-AE4E024917C7}"/>
-    <hyperlink ref="C345" r:id="rId365" xr:uid="{EF3501C3-6722-B042-98D5-211CBE91441E}"/>
+    <hyperlink ref="C346" r:id="rId365" xr:uid="{EF3501C3-6722-B042-98D5-211CBE91441E}"/>
     <hyperlink ref="C3" r:id="rId366" xr:uid="{E80DDE27-8B15-7D4E-B079-859E8B3D4840}"/>
     <hyperlink ref="C7" r:id="rId367" xr:uid="{2BD4EAC1-9B52-F549-A5EF-09125D392FAD}"/>
     <hyperlink ref="C8" r:id="rId368" xr:uid="{D7671988-78D2-5D42-A661-9F1327506CFF}"/>
     <hyperlink ref="C9" r:id="rId369" xr:uid="{9B9AC072-01A0-A844-847C-B109A617D904}"/>
+    <hyperlink ref="C349" r:id="rId370" xr:uid="{B12E0A4B-2756-BC42-8B8D-F13EBD0781FC}"/>
+    <hyperlink ref="C348" r:id="rId371" xr:uid="{A42E2080-0217-3F47-AE51-390098505C99}"/>
+    <hyperlink ref="C341" r:id="rId372" xr:uid="{C755366D-FC78-4743-98C2-D8F2CF3EC22B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
DMS SC vs SCT
</commit_message>
<xml_diff>
--- a/aws-services-crib-sheet.xlsx
+++ b/aws-services-crib-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corbuno/courses/aws-services-crib-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DFBD5A-4A8D-FB4B-8EA0-1EDE2AEB7858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4234AEA-475E-1E49-A983-FF3E8A1617A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{8DC9DE24-CECC-4748-B90E-52259685D84E}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="source" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AWS Services'!$A$1:$R$372</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'AWS Services'!$A$1:$R$373</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="421">
   <si>
     <t>Elastic Load Balancing</t>
   </si>
@@ -823,9 +823,6 @@
     <t>Database Migration Service (DMS)</t>
   </si>
   <si>
-    <t>DMS Schema Convertion Tool (SCT)</t>
-  </si>
-  <si>
     <t>RDS Performance Insights</t>
   </si>
   <si>
@@ -1289,6 +1286,12 @@
   </si>
   <si>
     <t>KMS External Key Store (XKS)</t>
+  </si>
+  <si>
+    <t>DMS Schema Conversion (DMS SC)</t>
+  </si>
+  <si>
+    <t>Schema Conversion Tool (SCT)</t>
   </si>
 </sst>
 </file>
@@ -1570,7 +1573,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1738,7 +1741,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1748,6 +1750,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1757,12 +1768,12 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF1D7C6A"/>
+      <color rgb="FF1F8901"/>
       <color rgb="FFB1094E"/>
       <color rgb="FFD15D16"/>
-      <color rgb="FF1F8901"/>
       <color rgb="FFC00A17"/>
       <color rgb="FF2F29AE"/>
-      <color rgb="FF1D7C6A"/>
       <color rgb="FF4F28AC"/>
       <color rgb="FF208A01"/>
       <color rgb="FF5B31B6"/>
@@ -2077,11 +2088,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00D01EA-5C3E-F64B-8B7F-2EE6141A689A}">
-  <dimension ref="A1:R372"/>
+  <dimension ref="A1:R373"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="1" topLeftCell="A274" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D282" sqref="D282"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2112,7 +2123,7 @@
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D1" s="42" t="s">
         <v>3</v>
@@ -2127,19 +2138,19 @@
         <v>158</v>
       </c>
       <c r="H1" s="48" t="s">
+        <v>382</v>
+      </c>
+      <c r="I1" s="48" t="s">
+        <v>381</v>
+      </c>
+      <c r="J1" s="48" t="s">
+        <v>380</v>
+      </c>
+      <c r="K1" s="49" t="s">
+        <v>379</v>
+      </c>
+      <c r="L1" s="49" t="s">
         <v>383</v>
-      </c>
-      <c r="I1" s="48" t="s">
-        <v>382</v>
-      </c>
-      <c r="J1" s="48" t="s">
-        <v>381</v>
-      </c>
-      <c r="K1" s="49" t="s">
-        <v>380</v>
-      </c>
-      <c r="L1" s="49" t="s">
-        <v>384</v>
       </c>
       <c r="M1" s="50" t="s">
         <v>162</v>
@@ -2207,7 +2218,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D3" s="43"/>
       <c r="E3" s="43"/>
@@ -2259,7 +2270,7 @@
         <v>49</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D5" s="43"/>
       <c r="E5" s="43"/>
@@ -2319,7 +2330,7 @@
         <v>49</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D7" s="43"/>
       <c r="E7" s="43"/>
@@ -2354,7 +2365,7 @@
         <v>49</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D8" s="43"/>
       <c r="E8" s="43"/>
@@ -2379,7 +2390,7 @@
         <v>49</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D9" s="43"/>
       <c r="E9" s="43"/>
@@ -2429,7 +2440,7 @@
         <v>49</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D11" s="43"/>
       <c r="E11" s="43"/>
@@ -2487,7 +2498,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D13" s="43"/>
       <c r="E13" s="43"/>
@@ -2514,7 +2525,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>223</v>
+        <v>406</v>
       </c>
       <c r="D14" s="43"/>
       <c r="E14" s="43"/>
@@ -2539,7 +2550,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>407</v>
+        <v>223</v>
       </c>
       <c r="D15" s="43"/>
       <c r="E15" s="43"/>
@@ -2564,7 +2575,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D16" s="43"/>
       <c r="E16" s="43"/>
@@ -2589,7 +2600,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D17" s="43"/>
       <c r="E17" s="43"/>
@@ -2616,7 +2627,7 @@
         <v>4</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D18" s="43"/>
       <c r="E18" s="43"/>
@@ -2641,7 +2652,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D19" s="43"/>
       <c r="E19" s="43"/>
@@ -2666,7 +2677,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D20" s="43"/>
       <c r="E20" s="43"/>
@@ -2691,7 +2702,7 @@
         <v>49</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D21" s="43"/>
       <c r="E21" s="43"/>
@@ -2868,7 +2879,7 @@
         <v>49</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D26" s="43"/>
       <c r="E26" s="43"/>
@@ -2895,7 +2906,7 @@
         <v>49</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D27" s="43"/>
       <c r="E27" s="43"/>
@@ -2920,7 +2931,7 @@
         <v>49</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D28" s="43"/>
       <c r="E28" s="43"/>
@@ -3029,7 +3040,7 @@
         <v>49</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D31" s="43"/>
       <c r="E31" s="43"/>
@@ -3062,7 +3073,7 @@
         <v>49</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D32" s="43"/>
       <c r="E32" s="43"/>
@@ -3095,7 +3106,7 @@
         <v>49</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D33" s="43"/>
       <c r="E33" s="43"/>
@@ -3128,7 +3139,7 @@
         <v>49</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D34" s="43"/>
       <c r="E34" s="43"/>
@@ -3161,7 +3172,7 @@
         <v>49</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D35" s="43"/>
       <c r="E35" s="43"/>
@@ -3250,7 +3261,7 @@
         <v>49</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D38" s="43"/>
       <c r="E38" s="43"/>
@@ -3493,7 +3504,7 @@
         <v>49</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D45" s="43"/>
       <c r="E45" s="43"/>
@@ -3622,7 +3633,7 @@
         <v>49</v>
       </c>
       <c r="C50" s="38" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D50" s="43"/>
       <c r="E50" s="43"/>
@@ -3647,7 +3658,7 @@
         <v>49</v>
       </c>
       <c r="C51" s="38" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D51" s="43"/>
       <c r="E51" s="43"/>
@@ -3797,7 +3808,7 @@
         <v>49</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D56" s="43"/>
       <c r="E56" s="43"/>
@@ -4040,7 +4051,7 @@
         <v>4</v>
       </c>
       <c r="C63" s="15" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D63" s="43"/>
       <c r="E63" s="43"/>
@@ -4113,7 +4124,7 @@
         <v>4</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D66" s="43"/>
       <c r="E66" s="43"/>
@@ -4163,7 +4174,7 @@
       </c>
       <c r="B68" s="14"/>
       <c r="C68" s="15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D68" s="43"/>
       <c r="E68" s="43"/>
@@ -4188,7 +4199,7 @@
         <v>165</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D69" s="43"/>
       <c r="E69" s="43"/>
@@ -4392,7 +4403,7 @@
       </c>
       <c r="B75" s="14"/>
       <c r="C75" s="15" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D75" s="43"/>
       <c r="E75" s="43"/>
@@ -4459,13 +4470,13 @@
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B78" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C78" s="12" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D78" s="43"/>
       <c r="E78" s="43"/>
@@ -4484,13 +4495,13 @@
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B79" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C79" s="12" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D79" s="43"/>
       <c r="E79" s="43"/>
@@ -4509,7 +4520,7 @@
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B80" s="11" t="s">
         <v>4</v>
@@ -4545,13 +4556,13 @@
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B81" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C81" s="12" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D81" s="43"/>
       <c r="E81" s="43"/>
@@ -4577,13 +4588,13 @@
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B82" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C82" s="12" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D82" s="43"/>
       <c r="E82" s="43"/>
@@ -4602,13 +4613,13 @@
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B83" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C83" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D83" s="43"/>
       <c r="E83" s="43"/>
@@ -4627,7 +4638,7 @@
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B84" s="11" t="s">
         <v>4</v>
@@ -4665,11 +4676,11 @@
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B85" s="11"/>
       <c r="C85" s="12" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D85" s="43"/>
       <c r="E85" s="43"/>
@@ -4688,7 +4699,7 @@
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A86" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B86" s="11" t="s">
         <v>4</v>
@@ -4715,11 +4726,11 @@
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B87" s="11"/>
       <c r="C87" s="12" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D87" s="43"/>
       <c r="E87" s="43"/>
@@ -4741,7 +4752,7 @@
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A88" s="10" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B88" s="11"/>
       <c r="C88" s="12" t="s">
@@ -4779,7 +4790,7 @@
         <v>4</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D89" s="43"/>
       <c r="E89" s="43"/>
@@ -4829,7 +4840,7 @@
         <v>4</v>
       </c>
       <c r="C91" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D91" s="43"/>
       <c r="E91" s="43"/>
@@ -4883,7 +4894,7 @@
         <v>4</v>
       </c>
       <c r="C93" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D93" s="43"/>
       <c r="E93" s="43"/>
@@ -4935,7 +4946,7 @@
         <v>4</v>
       </c>
       <c r="C95" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D95" s="43"/>
       <c r="E95" s="43"/>
@@ -5150,7 +5161,7 @@
         <v>49</v>
       </c>
       <c r="C102" s="20" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D102" s="43"/>
       <c r="E102" s="43"/>
@@ -5183,7 +5194,7 @@
         <v>49</v>
       </c>
       <c r="C103" s="20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D103" s="43"/>
       <c r="E103" s="43"/>
@@ -5272,7 +5283,7 @@
         <v>49</v>
       </c>
       <c r="C106" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D106" s="43"/>
       <c r="E106" s="43"/>
@@ -5361,7 +5372,7 @@
         <v>49</v>
       </c>
       <c r="C109" s="20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D109" s="43"/>
       <c r="E109" s="43"/>
@@ -5486,7 +5497,7 @@
         <v>4</v>
       </c>
       <c r="C113" s="20" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D113" s="43"/>
       <c r="E113" s="43"/>
@@ -5513,7 +5524,7 @@
         <v>4</v>
       </c>
       <c r="C114" s="20" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D114" s="43"/>
       <c r="E114" s="43"/>
@@ -5570,7 +5581,7 @@
         <v>4</v>
       </c>
       <c r="C116" s="20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D116" s="43"/>
       <c r="E116" s="43"/>
@@ -5595,7 +5606,7 @@
         <v>4</v>
       </c>
       <c r="C117" s="20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D117" s="43"/>
       <c r="E117" s="43"/>
@@ -5647,7 +5658,7 @@
       </c>
       <c r="B119" s="19"/>
       <c r="C119" s="20" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D119" s="43"/>
       <c r="E119" s="43"/>
@@ -5922,7 +5933,7 @@
         <v>49</v>
       </c>
       <c r="C128" s="20" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D128" s="43"/>
       <c r="E128" s="43"/>
@@ -5983,7 +5994,7 @@
       </c>
       <c r="B130" s="19"/>
       <c r="C130" s="20" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D130" s="43"/>
       <c r="E130" s="43"/>
@@ -6135,7 +6146,7 @@
         <v>4</v>
       </c>
       <c r="C136" s="20" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D136" s="43"/>
       <c r="E136" s="43"/>
@@ -6158,7 +6169,7 @@
       </c>
       <c r="B137" s="19"/>
       <c r="C137" s="20" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D137" s="43"/>
       <c r="E137" s="43"/>
@@ -6181,7 +6192,7 @@
       </c>
       <c r="B138" s="19"/>
       <c r="C138" s="20" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D138" s="43"/>
       <c r="E138" s="43"/>
@@ -6206,7 +6217,7 @@
         <v>4</v>
       </c>
       <c r="C139" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D139" s="43"/>
       <c r="E139" s="43"/>
@@ -6233,7 +6244,7 @@
       </c>
       <c r="B140" s="19"/>
       <c r="C140" s="20" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D140" s="43"/>
       <c r="E140" s="43"/>
@@ -6349,7 +6360,7 @@
         <v>4</v>
       </c>
       <c r="C144" s="23" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D144" s="43"/>
       <c r="E144" s="43"/>
@@ -6431,7 +6442,7 @@
         <v>4</v>
       </c>
       <c r="C147" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D147" s="43"/>
       <c r="E147" s="43"/>
@@ -6481,7 +6492,7 @@
         <v>49</v>
       </c>
       <c r="C149" s="9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D149" s="43"/>
       <c r="E149" s="43"/>
@@ -6506,7 +6517,7 @@
         <v>49</v>
       </c>
       <c r="C150" s="9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D150" s="43"/>
       <c r="E150" s="43"/>
@@ -6529,7 +6540,7 @@
       </c>
       <c r="B151" s="8"/>
       <c r="C151" s="9" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D151" s="43"/>
       <c r="E151" s="43"/>
@@ -6727,7 +6738,7 @@
         <v>4</v>
       </c>
       <c r="C159" s="26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D159" s="43"/>
       <c r="E159" s="43"/>
@@ -6777,7 +6788,7 @@
         <v>4</v>
       </c>
       <c r="C161" s="26" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D161" s="43"/>
       <c r="E161" s="43"/>
@@ -6802,7 +6813,7 @@
         <v>4</v>
       </c>
       <c r="C162" s="26" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D162" s="43"/>
       <c r="E162" s="43"/>
@@ -6904,7 +6915,7 @@
         <v>4</v>
       </c>
       <c r="C166" s="26" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D166" s="43"/>
       <c r="E166" s="43"/>
@@ -6954,7 +6965,7 @@
         <v>4</v>
       </c>
       <c r="C168" s="26" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D168" s="43"/>
       <c r="E168" s="43"/>
@@ -7293,7 +7304,7 @@
         <v>49</v>
       </c>
       <c r="C181" s="23" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D181" s="43"/>
       <c r="E181" s="43"/>
@@ -7511,7 +7522,7 @@
         <v>49</v>
       </c>
       <c r="C189" s="23" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D189" s="43"/>
       <c r="E189" s="43"/>
@@ -7752,7 +7763,7 @@
         <v>49</v>
       </c>
       <c r="C198" s="23" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D198" s="43"/>
       <c r="E198" s="43"/>
@@ -7858,7 +7869,7 @@
         <v>49</v>
       </c>
       <c r="C202" s="23" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D202" s="43"/>
       <c r="E202" s="43"/>
@@ -7910,7 +7921,7 @@
         <v>49</v>
       </c>
       <c r="C204" s="23" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D204" s="43"/>
       <c r="E204" s="43"/>
@@ -7935,7 +7946,7 @@
         <v>49</v>
       </c>
       <c r="C205" s="23" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D205" s="43"/>
       <c r="E205" s="43"/>
@@ -8068,7 +8079,7 @@
       </c>
       <c r="B210" s="29"/>
       <c r="C210" s="30" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D210" s="43"/>
       <c r="E210" s="44"/>
@@ -8379,7 +8390,7 @@
         <v>4</v>
       </c>
       <c r="C218" s="30" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D218" s="43"/>
       <c r="E218" s="43"/>
@@ -8433,7 +8444,7 @@
         <v>49</v>
       </c>
       <c r="C220" s="30" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D220" s="43"/>
       <c r="E220" s="43"/>
@@ -8458,7 +8469,7 @@
         <v>4</v>
       </c>
       <c r="C221" s="30" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D221" s="43"/>
       <c r="E221" s="43"/>
@@ -8490,7 +8501,7 @@
         <v>4</v>
       </c>
       <c r="C222" s="30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D222" s="43"/>
       <c r="E222" s="43"/>
@@ -8764,7 +8775,7 @@
         <v>4</v>
       </c>
       <c r="C231" s="30" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D231" s="43"/>
       <c r="E231" s="43"/>
@@ -8818,7 +8829,7 @@
         <v>4</v>
       </c>
       <c r="C233" s="30" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D233" s="43"/>
       <c r="E233" s="43"/>
@@ -8872,7 +8883,7 @@
         <v>4</v>
       </c>
       <c r="C235" s="30" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="D235" s="43"/>
       <c r="E235" s="43"/>
@@ -8897,7 +8908,7 @@
         <v>4</v>
       </c>
       <c r="C236" s="30" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="D236" s="43"/>
       <c r="E236" s="43"/>
@@ -9011,7 +9022,7 @@
         <v>4</v>
       </c>
       <c r="C240" s="30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D240" s="43"/>
       <c r="E240" s="43"/>
@@ -9171,7 +9182,7 @@
         <v>4</v>
       </c>
       <c r="C246" s="30" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D246" s="43"/>
       <c r="E246" s="43"/>
@@ -9347,7 +9358,7 @@
         <v>4</v>
       </c>
       <c r="C252" s="30" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D252" s="43"/>
       <c r="E252" s="43"/>
@@ -9560,13 +9571,13 @@
     </row>
     <row r="259" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A259" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B259" s="14" t="s">
         <v>49</v>
       </c>
       <c r="C259" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D259" s="43"/>
       <c r="E259" s="43"/>
@@ -9587,13 +9598,13 @@
     </row>
     <row r="260" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A260" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B260" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C260" s="15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D260" s="43"/>
       <c r="E260" s="43"/>
@@ -9612,13 +9623,13 @@
     </row>
     <row r="261" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A261" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B261" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C261" s="15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D261" s="43"/>
       <c r="E261" s="43"/>
@@ -9637,13 +9648,13 @@
     </row>
     <row r="262" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A262" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B262" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C262" s="15" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D262" s="43"/>
       <c r="E262" s="43"/>
@@ -9662,13 +9673,13 @@
     </row>
     <row r="263" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A263" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B263" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C263" s="15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D263" s="43"/>
       <c r="E263" s="43"/>
@@ -9687,13 +9698,13 @@
     </row>
     <row r="264" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A264" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B264" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C264" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D264" s="43"/>
       <c r="E264" s="43"/>
@@ -9712,7 +9723,7 @@
     </row>
     <row r="265" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A265" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B265" s="14" t="s">
         <v>4</v>
@@ -9737,7 +9748,7 @@
     </row>
     <row r="266" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A266" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B266" s="14" t="s">
         <v>4</v>
@@ -9762,7 +9773,7 @@
     </row>
     <row r="267" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A267" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B267" s="14" t="s">
         <v>4</v>
@@ -9787,13 +9798,13 @@
     </row>
     <row r="268" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A268" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B268" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C268" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D268" s="43"/>
       <c r="E268" s="43"/>
@@ -9812,7 +9823,7 @@
     </row>
     <row r="269" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A269" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B269" s="14" t="s">
         <v>4</v>
@@ -9837,13 +9848,13 @@
     </row>
     <row r="270" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A270" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B270" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C270" s="15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D270" s="43"/>
       <c r="E270" s="43"/>
@@ -9862,13 +9873,13 @@
     </row>
     <row r="271" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A271" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B271" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C271" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D271" s="43"/>
       <c r="E271" s="43"/>
@@ -9887,13 +9898,13 @@
     </row>
     <row r="272" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A272" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B272" s="14" t="s">
         <v>49</v>
       </c>
       <c r="C272" s="15" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D272" s="43"/>
       <c r="E272" s="43"/>
@@ -9912,13 +9923,13 @@
     </row>
     <row r="273" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A273" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B273" s="14" t="s">
         <v>49</v>
       </c>
       <c r="C273" s="15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D273" s="43"/>
       <c r="E273" s="43"/>
@@ -9937,13 +9948,13 @@
     </row>
     <row r="274" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A274" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="B274" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C274" s="15" t="s">
         <v>277</v>
-      </c>
-      <c r="B274" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C274" s="15" t="s">
-        <v>278</v>
       </c>
       <c r="D274" s="43"/>
       <c r="E274" s="43"/>
@@ -9962,13 +9973,13 @@
     </row>
     <row r="275" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A275" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B275" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C275" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D275" s="43"/>
       <c r="E275" s="43"/>
@@ -9987,13 +9998,13 @@
     </row>
     <row r="276" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A276" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B276" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C276" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D276" s="43"/>
       <c r="E276" s="43"/>
@@ -10012,13 +10023,13 @@
     </row>
     <row r="277" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A277" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B277" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C277" s="15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D277" s="43"/>
       <c r="E277" s="43"/>
@@ -10037,13 +10048,13 @@
     </row>
     <row r="278" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A278" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B278" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C278" s="15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D278" s="43"/>
       <c r="E278" s="43"/>
@@ -10062,13 +10073,13 @@
     </row>
     <row r="279" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A279" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B279" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C279" s="15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D279" s="43"/>
       <c r="E279" s="43"/>
@@ -10087,13 +10098,13 @@
     </row>
     <row r="280" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A280" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B280" s="14" t="s">
         <v>4</v>
       </c>
       <c r="C280" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D280" s="43"/>
       <c r="E280" s="43"/>
@@ -10109,6 +10120,7 @@
       <c r="O280" s="16"/>
       <c r="P280" s="16"/>
       <c r="Q280" s="16"/>
+      <c r="R280" s="66"/>
     </row>
     <row r="281" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A281" s="21" t="s">
@@ -10118,7 +10130,7 @@
         <v>4</v>
       </c>
       <c r="C281" s="23" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D281" s="43"/>
       <c r="E281" s="43"/>
@@ -10146,7 +10158,7 @@
         <v>4</v>
       </c>
       <c r="C282" s="23" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D282" s="43"/>
       <c r="E282" s="43"/>
@@ -10169,7 +10181,7 @@
       </c>
       <c r="B283" s="31"/>
       <c r="C283" s="23" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D283" s="43"/>
       <c r="E283" s="43"/>
@@ -10194,7 +10206,7 @@
         <v>4</v>
       </c>
       <c r="C284" s="23" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D284" s="43"/>
       <c r="E284" s="43"/>
@@ -10316,31 +10328,23 @@
       <c r="B288" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C288" s="23" t="s">
-        <v>264</v>
+      <c r="C288" s="64" t="s">
+        <v>419</v>
       </c>
       <c r="D288" s="43"/>
       <c r="E288" s="43"/>
       <c r="F288" s="43"/>
-      <c r="G288" s="16">
-        <v>1</v>
-      </c>
-      <c r="H288" s="16">
-        <v>1</v>
-      </c>
+      <c r="G288" s="16"/>
+      <c r="H288" s="16"/>
       <c r="I288" s="16"/>
       <c r="J288" s="16"/>
-      <c r="K288" s="16">
-        <v>1</v>
-      </c>
+      <c r="K288" s="16"/>
       <c r="L288" s="16"/>
       <c r="M288" s="16"/>
       <c r="N288" s="16"/>
       <c r="O288" s="16"/>
       <c r="P288" s="16"/>
-      <c r="Q288" s="16">
-        <v>1</v>
-      </c>
+      <c r="Q288" s="16"/>
     </row>
     <row r="289" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A289" s="21" t="s">
@@ -10350,7 +10354,7 @@
         <v>4</v>
       </c>
       <c r="C289" s="23" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D289" s="43"/>
       <c r="E289" s="43"/>
@@ -10430,7 +10434,7 @@
         <v>4</v>
       </c>
       <c r="C292" s="23" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D292" s="43"/>
       <c r="E292" s="43"/>
@@ -10455,7 +10459,7 @@
         <v>4</v>
       </c>
       <c r="C293" s="23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D293" s="43"/>
       <c r="E293" s="43"/>
@@ -10480,12 +10484,14 @@
         <v>4</v>
       </c>
       <c r="C294" s="23" t="s">
-        <v>115</v>
+        <v>420</v>
       </c>
       <c r="D294" s="43"/>
       <c r="E294" s="43"/>
       <c r="F294" s="43"/>
-      <c r="G294" s="16"/>
+      <c r="G294" s="16">
+        <v>1</v>
+      </c>
       <c r="H294" s="16">
         <v>1</v>
       </c>
@@ -10499,8 +10505,7 @@
       <c r="N294" s="16"/>
       <c r="O294" s="16"/>
       <c r="P294" s="16"/>
-      <c r="Q294" s="16"/>
-      <c r="R294" s="2">
+      <c r="Q294" s="16">
         <v>1</v>
       </c>
     </row>
@@ -10512,14 +10517,12 @@
         <v>4</v>
       </c>
       <c r="C295" s="23" t="s">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="D295" s="43"/>
       <c r="E295" s="43"/>
       <c r="F295" s="43"/>
-      <c r="G295" s="16">
-        <v>1</v>
-      </c>
+      <c r="G295" s="16"/>
       <c r="H295" s="16">
         <v>1</v>
       </c>
@@ -10532,12 +10535,8 @@
       <c r="M295" s="16"/>
       <c r="N295" s="16"/>
       <c r="O295" s="16"/>
-      <c r="P295" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q295" s="16">
-        <v>1</v>
-      </c>
+      <c r="P295" s="16"/>
+      <c r="Q295" s="16"/>
       <c r="R295" s="2">
         <v>1</v>
       </c>
@@ -10550,7 +10549,7 @@
         <v>4</v>
       </c>
       <c r="C296" s="23" t="s">
-        <v>217</v>
+        <v>43</v>
       </c>
       <c r="D296" s="43"/>
       <c r="E296" s="43"/>
@@ -10558,15 +10557,21 @@
       <c r="G296" s="16">
         <v>1</v>
       </c>
-      <c r="H296" s="16"/>
+      <c r="H296" s="16">
+        <v>1</v>
+      </c>
       <c r="I296" s="16"/>
       <c r="J296" s="16"/>
-      <c r="K296" s="16"/>
+      <c r="K296" s="16">
+        <v>1</v>
+      </c>
       <c r="L296" s="16"/>
       <c r="M296" s="16"/>
       <c r="N296" s="16"/>
       <c r="O296" s="16"/>
-      <c r="P296" s="16"/>
+      <c r="P296" s="16">
+        <v>1</v>
+      </c>
       <c r="Q296" s="16">
         <v>1</v>
       </c>
@@ -10582,7 +10587,7 @@
         <v>4</v>
       </c>
       <c r="C297" s="23" t="s">
-        <v>44</v>
+        <v>217</v>
       </c>
       <c r="D297" s="43"/>
       <c r="E297" s="43"/>
@@ -10590,9 +10595,7 @@
       <c r="G297" s="16">
         <v>1</v>
       </c>
-      <c r="H297" s="16">
-        <v>1</v>
-      </c>
+      <c r="H297" s="16"/>
       <c r="I297" s="16"/>
       <c r="J297" s="16"/>
       <c r="K297" s="16"/>
@@ -10616,30 +10619,28 @@
         <v>4</v>
       </c>
       <c r="C298" s="23" t="s">
-        <v>120</v>
+        <v>44</v>
       </c>
       <c r="D298" s="43"/>
       <c r="E298" s="43"/>
       <c r="F298" s="43"/>
-      <c r="G298" s="16"/>
+      <c r="G298" s="16">
+        <v>1</v>
+      </c>
       <c r="H298" s="16">
         <v>1</v>
       </c>
       <c r="I298" s="16"/>
-      <c r="J298" s="16">
-        <v>1</v>
-      </c>
-      <c r="K298" s="16">
-        <v>1</v>
-      </c>
+      <c r="J298" s="16"/>
+      <c r="K298" s="16"/>
       <c r="L298" s="16"/>
       <c r="M298" s="16"/>
       <c r="N298" s="16"/>
       <c r="O298" s="16"/>
-      <c r="P298" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q298" s="16"/>
+      <c r="P298" s="16"/>
+      <c r="Q298" s="16">
+        <v>1</v>
+      </c>
       <c r="R298" s="2">
         <v>1</v>
       </c>
@@ -10648,93 +10649,102 @@
       <c r="A299" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B299" s="22"/>
+      <c r="B299" s="22" t="s">
+        <v>4</v>
+      </c>
       <c r="C299" s="23" t="s">
-        <v>402</v>
+        <v>120</v>
       </c>
       <c r="D299" s="43"/>
       <c r="E299" s="43"/>
       <c r="F299" s="43"/>
       <c r="G299" s="16"/>
-      <c r="H299" s="16"/>
+      <c r="H299" s="16">
+        <v>1</v>
+      </c>
       <c r="I299" s="16"/>
-      <c r="J299" s="16"/>
-      <c r="K299" s="16"/>
+      <c r="J299" s="16">
+        <v>1</v>
+      </c>
+      <c r="K299" s="16">
+        <v>1</v>
+      </c>
       <c r="L299" s="16"/>
       <c r="M299" s="16"/>
       <c r="N299" s="16"/>
       <c r="O299" s="16"/>
-      <c r="P299" s="16"/>
+      <c r="P299" s="16">
+        <v>1</v>
+      </c>
       <c r="Q299" s="16"/>
+      <c r="R299" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="300" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A300" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="B300" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="C300" s="34" t="s">
-        <v>124</v>
+      <c r="A300" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B300" s="22"/>
+      <c r="C300" s="23" t="s">
+        <v>401</v>
       </c>
       <c r="D300" s="43"/>
       <c r="E300" s="43"/>
       <c r="F300" s="43"/>
-      <c r="G300" s="16">
-        <v>1</v>
-      </c>
-      <c r="H300" s="16">
-        <v>1</v>
-      </c>
-      <c r="I300" s="16">
-        <v>1</v>
-      </c>
+      <c r="G300" s="16"/>
+      <c r="H300" s="16"/>
+      <c r="I300" s="16"/>
       <c r="J300" s="16"/>
-      <c r="K300" s="16">
-        <v>1</v>
-      </c>
-      <c r="L300" s="16">
-        <v>1</v>
-      </c>
+      <c r="K300" s="16"/>
+      <c r="L300" s="16"/>
       <c r="M300" s="16"/>
-      <c r="N300" s="16">
-        <v>1</v>
-      </c>
+      <c r="N300" s="16"/>
       <c r="O300" s="16"/>
-      <c r="P300" s="16">
-        <v>1</v>
-      </c>
+      <c r="P300" s="16"/>
       <c r="Q300" s="16"/>
-      <c r="R300" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="301" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A301" s="32" t="s">
         <v>163</v>
       </c>
       <c r="B301" s="33" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C301" s="34" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
       <c r="D301" s="43"/>
       <c r="E301" s="43"/>
       <c r="F301" s="43"/>
-      <c r="G301" s="16"/>
-      <c r="H301" s="16"/>
-      <c r="I301" s="16"/>
+      <c r="G301" s="16">
+        <v>1</v>
+      </c>
+      <c r="H301" s="16">
+        <v>1</v>
+      </c>
+      <c r="I301" s="16">
+        <v>1</v>
+      </c>
       <c r="J301" s="16"/>
-      <c r="K301" s="16"/>
-      <c r="L301" s="16"/>
+      <c r="K301" s="16">
+        <v>1</v>
+      </c>
+      <c r="L301" s="16">
+        <v>1</v>
+      </c>
       <c r="M301" s="16"/>
       <c r="N301" s="16">
         <v>1</v>
       </c>
       <c r="O301" s="16"/>
-      <c r="P301" s="16"/>
+      <c r="P301" s="16">
+        <v>1</v>
+      </c>
       <c r="Q301" s="16"/>
+      <c r="R301" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="302" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A302" s="32" t="s">
@@ -10744,7 +10754,7 @@
         <v>4</v>
       </c>
       <c r="C302" s="34" t="s">
-        <v>322</v>
+        <v>83</v>
       </c>
       <c r="D302" s="43"/>
       <c r="E302" s="43"/>
@@ -10752,15 +10762,13 @@
       <c r="G302" s="16"/>
       <c r="H302" s="16"/>
       <c r="I302" s="16"/>
-      <c r="J302" s="16">
-        <v>1</v>
-      </c>
+      <c r="J302" s="16"/>
       <c r="K302" s="16"/>
-      <c r="L302" s="16">
-        <v>1</v>
-      </c>
+      <c r="L302" s="16"/>
       <c r="M302" s="16"/>
-      <c r="N302" s="16"/>
+      <c r="N302" s="16">
+        <v>1</v>
+      </c>
       <c r="O302" s="16"/>
       <c r="P302" s="16"/>
       <c r="Q302" s="16"/>
@@ -10773,7 +10781,7 @@
         <v>4</v>
       </c>
       <c r="C303" s="34" t="s">
-        <v>86</v>
+        <v>321</v>
       </c>
       <c r="D303" s="43"/>
       <c r="E303" s="43"/>
@@ -10781,13 +10789,15 @@
       <c r="G303" s="16"/>
       <c r="H303" s="16"/>
       <c r="I303" s="16"/>
-      <c r="J303" s="16"/>
+      <c r="J303" s="16">
+        <v>1</v>
+      </c>
       <c r="K303" s="16"/>
-      <c r="L303" s="16"/>
+      <c r="L303" s="16">
+        <v>1</v>
+      </c>
       <c r="M303" s="16"/>
-      <c r="N303" s="16">
-        <v>1</v>
-      </c>
+      <c r="N303" s="16"/>
       <c r="O303" s="16"/>
       <c r="P303" s="16"/>
       <c r="Q303" s="16"/>
@@ -10800,7 +10810,7 @@
         <v>4</v>
       </c>
       <c r="C304" s="34" t="s">
-        <v>359</v>
+        <v>86</v>
       </c>
       <c r="D304" s="43"/>
       <c r="E304" s="43"/>
@@ -10812,7 +10822,9 @@
       <c r="K304" s="16"/>
       <c r="L304" s="16"/>
       <c r="M304" s="16"/>
-      <c r="N304" s="16"/>
+      <c r="N304" s="16">
+        <v>1</v>
+      </c>
       <c r="O304" s="16"/>
       <c r="P304" s="16"/>
       <c r="Q304" s="16"/>
@@ -10822,52 +10834,35 @@
         <v>163</v>
       </c>
       <c r="B305" s="33" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C305" s="34" t="s">
-        <v>54</v>
+        <v>358</v>
       </c>
       <c r="D305" s="43"/>
       <c r="E305" s="43"/>
       <c r="F305" s="43"/>
-      <c r="G305" s="16">
-        <v>1</v>
-      </c>
-      <c r="H305" s="16">
-        <v>1</v>
-      </c>
-      <c r="I305" s="16">
-        <v>1</v>
-      </c>
-      <c r="J305" s="16">
-        <v>1</v>
-      </c>
-      <c r="K305" s="16">
-        <v>1</v>
-      </c>
-      <c r="L305" s="16">
-        <v>1</v>
-      </c>
+      <c r="G305" s="16"/>
+      <c r="H305" s="16"/>
+      <c r="I305" s="16"/>
+      <c r="J305" s="16"/>
+      <c r="K305" s="16"/>
+      <c r="L305" s="16"/>
       <c r="M305" s="16"/>
-      <c r="N305" s="16">
-        <v>1</v>
-      </c>
+      <c r="N305" s="16"/>
       <c r="O305" s="16"/>
       <c r="P305" s="16"/>
       <c r="Q305" s="16"/>
-      <c r="R305" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="306" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A306" s="32" t="s">
         <v>163</v>
       </c>
       <c r="B306" s="33" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C306" s="34" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="D306" s="43"/>
       <c r="E306" s="43"/>
@@ -10878,23 +10873,25 @@
       <c r="H306" s="16">
         <v>1</v>
       </c>
-      <c r="I306" s="16"/>
-      <c r="J306" s="16"/>
+      <c r="I306" s="16">
+        <v>1</v>
+      </c>
+      <c r="J306" s="16">
+        <v>1</v>
+      </c>
       <c r="K306" s="16">
         <v>1</v>
       </c>
-      <c r="L306" s="16"/>
+      <c r="L306" s="16">
+        <v>1</v>
+      </c>
       <c r="M306" s="16"/>
       <c r="N306" s="16">
         <v>1</v>
       </c>
       <c r="O306" s="16"/>
-      <c r="P306" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q306" s="16">
-        <v>1</v>
-      </c>
+      <c r="P306" s="16"/>
+      <c r="Q306" s="16"/>
       <c r="R306" s="2">
         <v>1</v>
       </c>
@@ -10903,9 +10900,11 @@
       <c r="A307" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="B307" s="35"/>
+      <c r="B307" s="33" t="s">
+        <v>4</v>
+      </c>
       <c r="C307" s="34" t="s">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="D307" s="43"/>
       <c r="E307" s="43"/>
@@ -10916,18 +10915,12 @@
       <c r="H307" s="16">
         <v>1</v>
       </c>
-      <c r="I307" s="16">
-        <v>1</v>
-      </c>
-      <c r="J307" s="16">
-        <v>1</v>
-      </c>
+      <c r="I307" s="16"/>
+      <c r="J307" s="16"/>
       <c r="K307" s="16">
         <v>1</v>
       </c>
-      <c r="L307" s="16">
-        <v>1</v>
-      </c>
+      <c r="L307" s="16"/>
       <c r="M307" s="16"/>
       <c r="N307" s="16">
         <v>1</v>
@@ -10947,34 +10940,42 @@
       <c r="A308" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="B308" s="33" t="s">
-        <v>4</v>
-      </c>
+      <c r="B308" s="35"/>
       <c r="C308" s="34" t="s">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="D308" s="43"/>
       <c r="E308" s="43"/>
       <c r="F308" s="43"/>
-      <c r="G308" s="16"/>
+      <c r="G308" s="16">
+        <v>1</v>
+      </c>
       <c r="H308" s="16">
         <v>1</v>
       </c>
-      <c r="I308" s="16"/>
+      <c r="I308" s="16">
+        <v>1</v>
+      </c>
       <c r="J308" s="16">
         <v>1</v>
       </c>
       <c r="K308" s="16">
         <v>1</v>
       </c>
-      <c r="L308" s="16"/>
+      <c r="L308" s="16">
+        <v>1</v>
+      </c>
       <c r="M308" s="16"/>
       <c r="N308" s="16">
         <v>1</v>
       </c>
       <c r="O308" s="16"/>
-      <c r="P308" s="16"/>
-      <c r="Q308" s="16"/>
+      <c r="P308" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q308" s="16">
+        <v>1</v>
+      </c>
       <c r="R308" s="2">
         <v>1</v>
       </c>
@@ -10987,26 +10988,33 @@
         <v>4</v>
       </c>
       <c r="C309" s="34" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="D309" s="43"/>
       <c r="E309" s="43"/>
       <c r="F309" s="43"/>
       <c r="G309" s="16"/>
-      <c r="H309" s="16"/>
+      <c r="H309" s="16">
+        <v>1</v>
+      </c>
       <c r="I309" s="16"/>
-      <c r="J309" s="16"/>
-      <c r="K309" s="16"/>
+      <c r="J309" s="16">
+        <v>1</v>
+      </c>
+      <c r="K309" s="16">
+        <v>1</v>
+      </c>
       <c r="L309" s="16"/>
-      <c r="M309" s="16">
-        <v>1</v>
-      </c>
+      <c r="M309" s="16"/>
       <c r="N309" s="16">
         <v>1</v>
       </c>
       <c r="O309" s="16"/>
       <c r="P309" s="16"/>
       <c r="Q309" s="16"/>
+      <c r="R309" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="310" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A310" s="32" t="s">
@@ -11016,7 +11024,7 @@
         <v>4</v>
       </c>
       <c r="C310" s="34" t="s">
-        <v>345</v>
+        <v>108</v>
       </c>
       <c r="D310" s="43"/>
       <c r="E310" s="43"/>
@@ -11027,8 +11035,12 @@
       <c r="J310" s="16"/>
       <c r="K310" s="16"/>
       <c r="L310" s="16"/>
-      <c r="M310" s="16"/>
-      <c r="N310" s="16"/>
+      <c r="M310" s="16">
+        <v>1</v>
+      </c>
+      <c r="N310" s="16">
+        <v>1</v>
+      </c>
       <c r="O310" s="16"/>
       <c r="P310" s="16"/>
       <c r="Q310" s="16"/>
@@ -11041,7 +11053,7 @@
         <v>4</v>
       </c>
       <c r="C311" s="34" t="s">
-        <v>38</v>
+        <v>344</v>
       </c>
       <c r="D311" s="43"/>
       <c r="E311" s="43"/>
@@ -11050,61 +11062,42 @@
       <c r="H311" s="16"/>
       <c r="I311" s="16"/>
       <c r="J311" s="16"/>
-      <c r="K311" s="16">
-        <v>1</v>
-      </c>
+      <c r="K311" s="16"/>
       <c r="L311" s="16"/>
       <c r="M311" s="16"/>
-      <c r="N311" s="16">
-        <v>1</v>
-      </c>
+      <c r="N311" s="16"/>
       <c r="O311" s="16"/>
       <c r="P311" s="16"/>
       <c r="Q311" s="16"/>
-      <c r="R311" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="312" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A312" s="32" t="s">
         <v>163</v>
       </c>
       <c r="B312" s="33" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C312" s="34" t="s">
-        <v>149</v>
+        <v>38</v>
       </c>
       <c r="D312" s="43"/>
       <c r="E312" s="43"/>
       <c r="F312" s="43"/>
-      <c r="G312" s="16">
-        <v>1</v>
-      </c>
-      <c r="H312" s="16">
-        <v>1</v>
-      </c>
-      <c r="I312" s="16">
-        <v>1</v>
-      </c>
-      <c r="J312" s="16">
-        <v>1</v>
-      </c>
+      <c r="G312" s="16"/>
+      <c r="H312" s="16"/>
+      <c r="I312" s="16"/>
+      <c r="J312" s="16"/>
       <c r="K312" s="16">
         <v>1</v>
       </c>
-      <c r="L312" s="16">
-        <v>1</v>
-      </c>
+      <c r="L312" s="16"/>
       <c r="M312" s="16"/>
       <c r="N312" s="16">
         <v>1</v>
       </c>
       <c r="O312" s="16"/>
       <c r="P312" s="16"/>
-      <c r="Q312" s="16">
-        <v>1</v>
-      </c>
+      <c r="Q312" s="16"/>
       <c r="R312" s="2">
         <v>1</v>
       </c>
@@ -11114,37 +11107,54 @@
         <v>163</v>
       </c>
       <c r="B313" s="33" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C313" s="34" t="s">
-        <v>323</v>
+        <v>149</v>
       </c>
       <c r="D313" s="43"/>
       <c r="E313" s="43"/>
       <c r="F313" s="43"/>
-      <c r="G313" s="16"/>
-      <c r="H313" s="16"/>
-      <c r="I313" s="16"/>
-      <c r="J313" s="16"/>
-      <c r="K313" s="16"/>
+      <c r="G313" s="16">
+        <v>1</v>
+      </c>
+      <c r="H313" s="16">
+        <v>1</v>
+      </c>
+      <c r="I313" s="16">
+        <v>1</v>
+      </c>
+      <c r="J313" s="16">
+        <v>1</v>
+      </c>
+      <c r="K313" s="16">
+        <v>1</v>
+      </c>
       <c r="L313" s="16">
         <v>1</v>
       </c>
       <c r="M313" s="16"/>
-      <c r="N313" s="16"/>
+      <c r="N313" s="16">
+        <v>1</v>
+      </c>
       <c r="O313" s="16"/>
       <c r="P313" s="16"/>
-      <c r="Q313" s="16"/>
+      <c r="Q313" s="16">
+        <v>1</v>
+      </c>
+      <c r="R313" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="314" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A314" s="32" t="s">
         <v>163</v>
       </c>
       <c r="B314" s="33" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C314" s="34" t="s">
-        <v>406</v>
+        <v>322</v>
       </c>
       <c r="D314" s="43"/>
       <c r="E314" s="43"/>
@@ -11154,7 +11164,9 @@
       <c r="I314" s="16"/>
       <c r="J314" s="16"/>
       <c r="K314" s="16"/>
-      <c r="L314" s="16"/>
+      <c r="L314" s="16">
+        <v>1</v>
+      </c>
       <c r="M314" s="16"/>
       <c r="N314" s="16"/>
       <c r="O314" s="16"/>
@@ -11166,61 +11178,44 @@
         <v>163</v>
       </c>
       <c r="B315" s="33" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C315" s="34" t="s">
-        <v>121</v>
+        <v>405</v>
       </c>
       <c r="D315" s="43"/>
       <c r="E315" s="43"/>
       <c r="F315" s="43"/>
       <c r="G315" s="16"/>
-      <c r="H315" s="16">
-        <v>1</v>
-      </c>
+      <c r="H315" s="16"/>
       <c r="I315" s="16"/>
-      <c r="J315" s="16">
-        <v>1</v>
-      </c>
-      <c r="K315" s="16">
-        <v>1</v>
-      </c>
-      <c r="L315" s="16">
-        <v>1</v>
-      </c>
+      <c r="J315" s="16"/>
+      <c r="K315" s="16"/>
+      <c r="L315" s="16"/>
       <c r="M315" s="16"/>
-      <c r="N315" s="16">
-        <v>1</v>
-      </c>
+      <c r="N315" s="16"/>
       <c r="O315" s="16"/>
       <c r="P315" s="16"/>
       <c r="Q315" s="16"/>
-      <c r="R315" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="316" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A316" s="32" t="s">
         <v>163</v>
       </c>
       <c r="B316" s="33" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C316" s="34" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="D316" s="43"/>
       <c r="E316" s="43"/>
       <c r="F316" s="43"/>
-      <c r="G316" s="16">
-        <v>1</v>
-      </c>
+      <c r="G316" s="16"/>
       <c r="H316" s="16">
         <v>1</v>
       </c>
-      <c r="I316" s="16">
-        <v>1</v>
-      </c>
+      <c r="I316" s="16"/>
       <c r="J316" s="16">
         <v>1</v>
       </c>
@@ -11230,21 +11225,13 @@
       <c r="L316" s="16">
         <v>1</v>
       </c>
-      <c r="M316" s="16">
-        <v>1</v>
-      </c>
+      <c r="M316" s="16"/>
       <c r="N316" s="16">
         <v>1</v>
       </c>
-      <c r="O316" s="16">
-        <v>1</v>
-      </c>
-      <c r="P316" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q316" s="16">
-        <v>1</v>
-      </c>
+      <c r="O316" s="16"/>
+      <c r="P316" s="16"/>
+      <c r="Q316" s="16"/>
       <c r="R316" s="2">
         <v>1</v>
       </c>
@@ -11257,92 +11244,117 @@
         <v>49</v>
       </c>
       <c r="C317" s="34" t="s">
-        <v>324</v>
+        <v>156</v>
       </c>
       <c r="D317" s="43"/>
       <c r="E317" s="43"/>
       <c r="F317" s="43"/>
-      <c r="G317" s="16"/>
-      <c r="H317" s="16"/>
-      <c r="I317" s="16"/>
+      <c r="G317" s="16">
+        <v>1</v>
+      </c>
+      <c r="H317" s="16">
+        <v>1</v>
+      </c>
+      <c r="I317" s="16">
+        <v>1</v>
+      </c>
       <c r="J317" s="16">
         <v>1</v>
       </c>
-      <c r="K317" s="16"/>
-      <c r="L317" s="16"/>
-      <c r="M317" s="16"/>
-      <c r="N317" s="16"/>
-      <c r="O317" s="16"/>
-      <c r="P317" s="16"/>
-      <c r="Q317" s="16"/>
+      <c r="K317" s="16">
+        <v>1</v>
+      </c>
+      <c r="L317" s="16">
+        <v>1</v>
+      </c>
+      <c r="M317" s="16">
+        <v>1</v>
+      </c>
+      <c r="N317" s="16">
+        <v>1</v>
+      </c>
+      <c r="O317" s="16">
+        <v>1</v>
+      </c>
+      <c r="P317" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q317" s="16">
+        <v>1</v>
+      </c>
+      <c r="R317" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="318" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A318" s="32" t="s">
         <v>163</v>
       </c>
       <c r="B318" s="33" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C318" s="34" t="s">
-        <v>47</v>
+        <v>323</v>
       </c>
       <c r="D318" s="43"/>
       <c r="E318" s="43"/>
       <c r="F318" s="43"/>
-      <c r="G318" s="16">
-        <v>1</v>
-      </c>
-      <c r="H318" s="16">
-        <v>1</v>
-      </c>
+      <c r="G318" s="16"/>
+      <c r="H318" s="16"/>
       <c r="I318" s="16"/>
-      <c r="J318" s="16"/>
-      <c r="K318" s="16">
-        <v>1</v>
-      </c>
+      <c r="J318" s="16">
+        <v>1</v>
+      </c>
+      <c r="K318" s="16"/>
       <c r="L318" s="16"/>
       <c r="M318" s="16"/>
-      <c r="N318" s="16">
-        <v>1</v>
-      </c>
+      <c r="N318" s="16"/>
       <c r="O318" s="16"/>
       <c r="P318" s="16"/>
       <c r="Q318" s="16"/>
     </row>
     <row r="319" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A319" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B319" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C319" s="15" t="s">
-        <v>173</v>
+      <c r="A319" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="B319" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C319" s="34" t="s">
+        <v>47</v>
       </c>
       <c r="D319" s="43"/>
       <c r="E319" s="43"/>
       <c r="F319" s="43"/>
-      <c r="G319" s="16"/>
-      <c r="H319" s="16"/>
+      <c r="G319" s="16">
+        <v>1</v>
+      </c>
+      <c r="H319" s="16">
+        <v>1</v>
+      </c>
       <c r="I319" s="16"/>
       <c r="J319" s="16"/>
-      <c r="K319" s="16"/>
+      <c r="K319" s="16">
+        <v>1</v>
+      </c>
       <c r="L319" s="16"/>
       <c r="M319" s="16"/>
-      <c r="N319" s="16"/>
+      <c r="N319" s="16">
+        <v>1</v>
+      </c>
       <c r="O319" s="16"/>
       <c r="P319" s="16"/>
       <c r="Q319" s="16"/>
     </row>
     <row r="320" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A320" s="36" t="s">
-        <v>214</v>
-      </c>
-      <c r="B320" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C320" s="38" t="s">
-        <v>40</v>
+      <c r="A320" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B320" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C320" s="15" t="s">
+        <v>173</v>
       </c>
       <c r="D320" s="43"/>
       <c r="E320" s="43"/>
@@ -11360,14 +11372,14 @@
       <c r="Q320" s="16"/>
     </row>
     <row r="321" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A321" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="B321" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C321" s="20" t="s">
-        <v>97</v>
+      <c r="A321" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="B321" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C321" s="38" t="s">
+        <v>40</v>
       </c>
       <c r="D321" s="43"/>
       <c r="E321" s="43"/>
@@ -11385,34 +11397,28 @@
       <c r="Q321" s="16"/>
     </row>
     <row r="322" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A322" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B322" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="C322" s="38" t="s">
-        <v>7</v>
+      <c r="A322" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="B322" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C322" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="D322" s="43"/>
       <c r="E322" s="43"/>
       <c r="F322" s="43"/>
-      <c r="G322" s="16">
-        <v>1</v>
-      </c>
+      <c r="G322" s="16"/>
       <c r="H322" s="16"/>
       <c r="I322" s="16"/>
       <c r="J322" s="16"/>
-      <c r="K322" s="16">
-        <v>1</v>
-      </c>
+      <c r="K322" s="16"/>
       <c r="L322" s="16"/>
       <c r="M322" s="16"/>
       <c r="N322" s="16"/>
       <c r="O322" s="16"/>
-      <c r="P322" s="16">
-        <v>1</v>
-      </c>
+      <c r="P322" s="16"/>
       <c r="Q322" s="16"/>
     </row>
     <row r="323" spans="1:18" x14ac:dyDescent="0.2">
@@ -11423,23 +11429,27 @@
         <v>4</v>
       </c>
       <c r="C323" s="38" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="D323" s="43"/>
       <c r="E323" s="43"/>
       <c r="F323" s="43"/>
-      <c r="G323" s="16"/>
+      <c r="G323" s="16">
+        <v>1</v>
+      </c>
       <c r="H323" s="16"/>
       <c r="I323" s="16"/>
       <c r="J323" s="16"/>
-      <c r="K323" s="16"/>
+      <c r="K323" s="16">
+        <v>1</v>
+      </c>
       <c r="L323" s="16"/>
-      <c r="M323" s="16">
-        <v>1</v>
-      </c>
+      <c r="M323" s="16"/>
       <c r="N323" s="16"/>
       <c r="O323" s="16"/>
-      <c r="P323" s="16"/>
+      <c r="P323" s="16">
+        <v>1</v>
+      </c>
       <c r="Q323" s="16"/>
     </row>
     <row r="324" spans="1:18" x14ac:dyDescent="0.2">
@@ -11450,35 +11460,23 @@
         <v>4</v>
       </c>
       <c r="C324" s="38" t="s">
-        <v>216</v>
+        <v>84</v>
       </c>
       <c r="D324" s="43"/>
       <c r="E324" s="43"/>
       <c r="F324" s="43"/>
-      <c r="G324" s="16">
-        <v>1</v>
-      </c>
-      <c r="H324" s="16">
-        <v>1</v>
-      </c>
-      <c r="I324" s="16">
-        <v>1</v>
-      </c>
-      <c r="J324" s="16">
-        <v>1</v>
-      </c>
-      <c r="K324" s="16">
-        <v>1</v>
-      </c>
+      <c r="G324" s="16"/>
+      <c r="H324" s="16"/>
+      <c r="I324" s="16"/>
+      <c r="J324" s="16"/>
+      <c r="K324" s="16"/>
       <c r="L324" s="16"/>
       <c r="M324" s="16">
         <v>1</v>
       </c>
       <c r="N324" s="16"/>
       <c r="O324" s="16"/>
-      <c r="P324" s="16">
-        <v>1</v>
-      </c>
+      <c r="P324" s="16"/>
       <c r="Q324" s="16"/>
     </row>
     <row r="325" spans="1:18" x14ac:dyDescent="0.2">
@@ -11486,24 +11484,38 @@
         <v>41</v>
       </c>
       <c r="B325" s="37" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C325" s="38" t="s">
-        <v>126</v>
+        <v>216</v>
       </c>
       <c r="D325" s="43"/>
       <c r="E325" s="43"/>
       <c r="F325" s="43"/>
-      <c r="G325" s="16"/>
-      <c r="H325" s="16"/>
-      <c r="I325" s="16"/>
-      <c r="J325" s="16"/>
-      <c r="K325" s="16"/>
+      <c r="G325" s="16">
+        <v>1</v>
+      </c>
+      <c r="H325" s="16">
+        <v>1</v>
+      </c>
+      <c r="I325" s="16">
+        <v>1</v>
+      </c>
+      <c r="J325" s="16">
+        <v>1</v>
+      </c>
+      <c r="K325" s="16">
+        <v>1</v>
+      </c>
       <c r="L325" s="16"/>
-      <c r="M325" s="16"/>
+      <c r="M325" s="16">
+        <v>1</v>
+      </c>
       <c r="N325" s="16"/>
       <c r="O325" s="16"/>
-      <c r="P325" s="16"/>
+      <c r="P325" s="16">
+        <v>1</v>
+      </c>
       <c r="Q325" s="16"/>
     </row>
     <row r="326" spans="1:18" x14ac:dyDescent="0.2">
@@ -11511,45 +11523,35 @@
         <v>41</v>
       </c>
       <c r="B326" s="37" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C326" s="38" t="s">
-        <v>14</v>
+        <v>126</v>
       </c>
       <c r="D326" s="43"/>
       <c r="E326" s="43"/>
       <c r="F326" s="43"/>
-      <c r="G326" s="16">
-        <v>1</v>
-      </c>
-      <c r="H326" s="16">
-        <v>1</v>
-      </c>
+      <c r="G326" s="16"/>
+      <c r="H326" s="16"/>
       <c r="I326" s="16"/>
       <c r="J326" s="16"/>
       <c r="K326" s="16"/>
       <c r="L326" s="16"/>
-      <c r="M326" s="16">
-        <v>1</v>
-      </c>
+      <c r="M326" s="16"/>
       <c r="N326" s="16"/>
       <c r="O326" s="16"/>
-      <c r="P326" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q326" s="16">
-        <v>1</v>
-      </c>
+      <c r="P326" s="16"/>
+      <c r="Q326" s="16"/>
     </row>
     <row r="327" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A327" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B327" s="37" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C327" s="38" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="D327" s="43"/>
       <c r="E327" s="43"/>
@@ -11560,21 +11562,21 @@
       <c r="H327" s="16">
         <v>1</v>
       </c>
-      <c r="I327" s="16">
-        <v>1</v>
-      </c>
+      <c r="I327" s="16"/>
       <c r="J327" s="16"/>
-      <c r="K327" s="16">
-        <v>1</v>
-      </c>
+      <c r="K327" s="16"/>
       <c r="L327" s="16"/>
-      <c r="M327" s="16"/>
+      <c r="M327" s="16">
+        <v>1</v>
+      </c>
       <c r="N327" s="16"/>
       <c r="O327" s="16"/>
       <c r="P327" s="16">
         <v>1</v>
       </c>
-      <c r="Q327" s="16"/>
+      <c r="Q327" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="328" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A328" s="36" t="s">
@@ -11584,7 +11586,7 @@
         <v>49</v>
       </c>
       <c r="C328" s="38" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D328" s="43"/>
       <c r="E328" s="43"/>
@@ -11592,19 +11594,23 @@
       <c r="G328" s="16">
         <v>1</v>
       </c>
-      <c r="H328" s="16"/>
-      <c r="I328" s="16"/>
-      <c r="J328" s="16">
-        <v>1</v>
-      </c>
-      <c r="K328" s="16"/>
+      <c r="H328" s="16">
+        <v>1</v>
+      </c>
+      <c r="I328" s="16">
+        <v>1</v>
+      </c>
+      <c r="J328" s="16"/>
+      <c r="K328" s="16">
+        <v>1</v>
+      </c>
       <c r="L328" s="16"/>
-      <c r="M328" s="16">
-        <v>1</v>
-      </c>
+      <c r="M328" s="16"/>
       <c r="N328" s="16"/>
       <c r="O328" s="16"/>
-      <c r="P328" s="16"/>
+      <c r="P328" s="16">
+        <v>1</v>
+      </c>
       <c r="Q328" s="16"/>
     </row>
     <row r="329" spans="1:18" x14ac:dyDescent="0.2">
@@ -11612,25 +11618,23 @@
         <v>41</v>
       </c>
       <c r="B329" s="37" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C329" s="38" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="D329" s="43"/>
       <c r="E329" s="43"/>
       <c r="F329" s="43"/>
-      <c r="G329" s="16"/>
-      <c r="H329" s="16">
-        <v>1</v>
-      </c>
+      <c r="G329" s="16">
+        <v>1</v>
+      </c>
+      <c r="H329" s="16"/>
       <c r="I329" s="16"/>
       <c r="J329" s="16">
         <v>1</v>
       </c>
-      <c r="K329" s="16">
-        <v>1</v>
-      </c>
+      <c r="K329" s="16"/>
       <c r="L329" s="16"/>
       <c r="M329" s="16">
         <v>1</v>
@@ -11638,9 +11642,7 @@
       <c r="N329" s="16"/>
       <c r="O329" s="16"/>
       <c r="P329" s="16"/>
-      <c r="Q329" s="16">
-        <v>1</v>
-      </c>
+      <c r="Q329" s="16"/>
     </row>
     <row r="330" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A330" s="36" t="s">
@@ -11650,7 +11652,7 @@
         <v>4</v>
       </c>
       <c r="C330" s="38" t="s">
-        <v>258</v>
+        <v>90</v>
       </c>
       <c r="D330" s="43"/>
       <c r="E330" s="43"/>
@@ -11660,16 +11662,22 @@
         <v>1</v>
       </c>
       <c r="I330" s="16"/>
-      <c r="J330" s="16"/>
+      <c r="J330" s="16">
+        <v>1</v>
+      </c>
       <c r="K330" s="16">
         <v>1</v>
       </c>
       <c r="L330" s="16"/>
-      <c r="M330" s="16"/>
+      <c r="M330" s="16">
+        <v>1</v>
+      </c>
       <c r="N330" s="16"/>
       <c r="O330" s="16"/>
       <c r="P330" s="16"/>
-      <c r="Q330" s="16"/>
+      <c r="Q330" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="331" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A331" s="36" t="s">
@@ -11679,7 +11687,7 @@
         <v>4</v>
       </c>
       <c r="C331" s="38" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="D331" s="43"/>
       <c r="E331" s="43"/>
@@ -11708,7 +11716,7 @@
         <v>4</v>
       </c>
       <c r="C332" s="38" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D332" s="43"/>
       <c r="E332" s="43"/>
@@ -11737,16 +11745,20 @@
         <v>4</v>
       </c>
       <c r="C333" s="38" t="s">
-        <v>379</v>
+        <v>259</v>
       </c>
       <c r="D333" s="43"/>
       <c r="E333" s="43"/>
       <c r="F333" s="43"/>
       <c r="G333" s="16"/>
-      <c r="H333" s="16"/>
+      <c r="H333" s="16">
+        <v>1</v>
+      </c>
       <c r="I333" s="16"/>
       <c r="J333" s="16"/>
-      <c r="K333" s="16"/>
+      <c r="K333" s="16">
+        <v>1</v>
+      </c>
       <c r="L333" s="16"/>
       <c r="M333" s="16"/>
       <c r="N333" s="16"/>
@@ -11762,7 +11774,7 @@
         <v>4</v>
       </c>
       <c r="C334" s="38" t="s">
-        <v>95</v>
+        <v>378</v>
       </c>
       <c r="D334" s="43"/>
       <c r="E334" s="43"/>
@@ -11770,14 +11782,10 @@
       <c r="G334" s="16"/>
       <c r="H334" s="16"/>
       <c r="I334" s="16"/>
-      <c r="J334" s="16">
-        <v>1</v>
-      </c>
+      <c r="J334" s="16"/>
       <c r="K334" s="16"/>
       <c r="L334" s="16"/>
-      <c r="M334" s="16">
-        <v>1</v>
-      </c>
+      <c r="M334" s="16"/>
       <c r="N334" s="16"/>
       <c r="O334" s="16"/>
       <c r="P334" s="16"/>
@@ -11788,30 +11796,22 @@
         <v>41</v>
       </c>
       <c r="B335" s="37" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C335" s="38" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="D335" s="43"/>
       <c r="E335" s="43"/>
       <c r="F335" s="43"/>
-      <c r="G335" s="16">
-        <v>1</v>
-      </c>
-      <c r="H335" s="16">
-        <v>1</v>
-      </c>
+      <c r="G335" s="16"/>
+      <c r="H335" s="16"/>
       <c r="I335" s="16"/>
       <c r="J335" s="16">
         <v>1</v>
       </c>
-      <c r="K335" s="16">
-        <v>1</v>
-      </c>
-      <c r="L335" s="16">
-        <v>1</v>
-      </c>
+      <c r="K335" s="16"/>
+      <c r="L335" s="16"/>
       <c r="M335" s="16">
         <v>1</v>
       </c>
@@ -11819,36 +11819,46 @@
       <c r="O335" s="16"/>
       <c r="P335" s="16"/>
       <c r="Q335" s="16"/>
-      <c r="R335" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="336" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A336" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B336" s="37" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C336" s="38" t="s">
-        <v>325</v>
+        <v>64</v>
       </c>
       <c r="D336" s="43"/>
       <c r="E336" s="43"/>
       <c r="F336" s="43"/>
-      <c r="G336" s="16"/>
-      <c r="H336" s="16"/>
+      <c r="G336" s="16">
+        <v>1</v>
+      </c>
+      <c r="H336" s="16">
+        <v>1</v>
+      </c>
       <c r="I336" s="16"/>
       <c r="J336" s="16">
         <v>1</v>
       </c>
-      <c r="K336" s="16"/>
-      <c r="L336" s="16"/>
-      <c r="M336" s="16"/>
+      <c r="K336" s="16">
+        <v>1</v>
+      </c>
+      <c r="L336" s="16">
+        <v>1</v>
+      </c>
+      <c r="M336" s="16">
+        <v>1</v>
+      </c>
       <c r="N336" s="16"/>
       <c r="O336" s="16"/>
       <c r="P336" s="16"/>
       <c r="Q336" s="16"/>
+      <c r="R336" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="337" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A337" s="36" t="s">
@@ -11858,31 +11868,23 @@
         <v>4</v>
       </c>
       <c r="C337" s="38" t="s">
-        <v>393</v>
+        <v>324</v>
       </c>
       <c r="D337" s="43"/>
       <c r="E337" s="43"/>
       <c r="F337" s="43"/>
       <c r="G337" s="16"/>
-      <c r="H337" s="16">
-        <v>1</v>
-      </c>
+      <c r="H337" s="16"/>
       <c r="I337" s="16"/>
-      <c r="J337" s="16"/>
-      <c r="K337" s="16">
-        <v>1</v>
-      </c>
-      <c r="L337" s="16">
-        <v>1</v>
-      </c>
-      <c r="M337" s="16">
-        <v>1</v>
-      </c>
+      <c r="J337" s="16">
+        <v>1</v>
+      </c>
+      <c r="K337" s="16"/>
+      <c r="L337" s="16"/>
+      <c r="M337" s="16"/>
       <c r="N337" s="16"/>
       <c r="O337" s="16"/>
-      <c r="P337" s="16">
-        <v>1</v>
-      </c>
+      <c r="P337" s="16"/>
       <c r="Q337" s="16"/>
     </row>
     <row r="338" spans="1:18" x14ac:dyDescent="0.2">
@@ -11893,23 +11895,17 @@
         <v>4</v>
       </c>
       <c r="C338" s="38" t="s">
-        <v>98</v>
+        <v>392</v>
       </c>
       <c r="D338" s="43"/>
       <c r="E338" s="43"/>
       <c r="F338" s="43"/>
-      <c r="G338" s="16">
-        <v>1</v>
-      </c>
+      <c r="G338" s="16"/>
       <c r="H338" s="16">
         <v>1</v>
       </c>
-      <c r="I338" s="16">
-        <v>1</v>
-      </c>
-      <c r="J338" s="16">
-        <v>1</v>
-      </c>
+      <c r="I338" s="16"/>
+      <c r="J338" s="16"/>
       <c r="K338" s="16">
         <v>1</v>
       </c>
@@ -11919,28 +11915,22 @@
       <c r="M338" s="16">
         <v>1</v>
       </c>
-      <c r="N338" s="16">
-        <v>1</v>
-      </c>
-      <c r="O338" s="16">
-        <v>1</v>
-      </c>
+      <c r="N338" s="16"/>
+      <c r="O338" s="16"/>
       <c r="P338" s="16">
         <v>1</v>
       </c>
-      <c r="Q338" s="16">
-        <v>1</v>
-      </c>
+      <c r="Q338" s="16"/>
     </row>
     <row r="339" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A339" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B339" s="37" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C339" s="38" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="D339" s="43"/>
       <c r="E339" s="43"/>
@@ -11951,7 +11941,9 @@
       <c r="H339" s="16">
         <v>1</v>
       </c>
-      <c r="I339" s="16"/>
+      <c r="I339" s="16">
+        <v>1</v>
+      </c>
       <c r="J339" s="16">
         <v>1</v>
       </c>
@@ -11964,20 +11956,28 @@
       <c r="M339" s="16">
         <v>1</v>
       </c>
-      <c r="N339" s="16"/>
-      <c r="O339" s="16"/>
-      <c r="P339" s="16"/>
-      <c r="Q339" s="16"/>
+      <c r="N339" s="16">
+        <v>1</v>
+      </c>
+      <c r="O339" s="16">
+        <v>1</v>
+      </c>
+      <c r="P339" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q339" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="340" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A340" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B340" s="37" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C340" s="38" t="s">
-        <v>299</v>
+        <v>65</v>
       </c>
       <c r="D340" s="43"/>
       <c r="E340" s="43"/>
@@ -11988,9 +11988,7 @@
       <c r="H340" s="16">
         <v>1</v>
       </c>
-      <c r="I340" s="16">
-        <v>1</v>
-      </c>
+      <c r="I340" s="16"/>
       <c r="J340" s="16">
         <v>1</v>
       </c>
@@ -12005,12 +12003,8 @@
       </c>
       <c r="N340" s="16"/>
       <c r="O340" s="16"/>
-      <c r="P340" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q340" s="16">
-        <v>1</v>
-      </c>
+      <c r="P340" s="16"/>
+      <c r="Q340" s="16"/>
     </row>
     <row r="341" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A341" s="36" t="s">
@@ -12020,56 +12014,64 @@
         <v>4</v>
       </c>
       <c r="C341" s="38" t="s">
-        <v>419</v>
+        <v>298</v>
       </c>
       <c r="D341" s="43"/>
       <c r="E341" s="43"/>
       <c r="F341" s="43"/>
-      <c r="G341" s="16"/>
-      <c r="H341" s="16"/>
-      <c r="I341" s="16"/>
-      <c r="J341" s="16"/>
-      <c r="K341" s="16"/>
-      <c r="L341" s="16"/>
-      <c r="M341" s="16"/>
+      <c r="G341" s="16">
+        <v>1</v>
+      </c>
+      <c r="H341" s="16">
+        <v>1</v>
+      </c>
+      <c r="I341" s="16">
+        <v>1</v>
+      </c>
+      <c r="J341" s="16">
+        <v>1</v>
+      </c>
+      <c r="K341" s="16">
+        <v>1</v>
+      </c>
+      <c r="L341" s="16">
+        <v>1</v>
+      </c>
+      <c r="M341" s="16">
+        <v>1</v>
+      </c>
       <c r="N341" s="16"/>
       <c r="O341" s="16"/>
-      <c r="P341" s="16"/>
-      <c r="Q341" s="16"/>
+      <c r="P341" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q341" s="16">
+        <v>1</v>
+      </c>
     </row>
     <row r="342" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A342" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B342" s="37" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C342" s="38" t="s">
-        <v>68</v>
+        <v>418</v>
       </c>
       <c r="D342" s="43"/>
       <c r="E342" s="43"/>
       <c r="F342" s="43"/>
-      <c r="G342" s="16">
-        <v>1</v>
-      </c>
-      <c r="H342" s="16">
-        <v>1</v>
-      </c>
+      <c r="G342" s="16"/>
+      <c r="H342" s="16"/>
       <c r="I342" s="16"/>
       <c r="J342" s="16"/>
-      <c r="K342" s="16">
-        <v>1</v>
-      </c>
+      <c r="K342" s="16"/>
       <c r="L342" s="16"/>
-      <c r="M342" s="16">
-        <v>1</v>
-      </c>
+      <c r="M342" s="16"/>
       <c r="N342" s="16"/>
       <c r="O342" s="16"/>
-      <c r="P342" s="16">
-        <v>1</v>
-      </c>
+      <c r="P342" s="16"/>
       <c r="Q342" s="16"/>
     </row>
     <row r="343" spans="1:18" x14ac:dyDescent="0.2">
@@ -12077,24 +12079,34 @@
         <v>41</v>
       </c>
       <c r="B343" s="37" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C343" s="38" t="s">
-        <v>398</v>
+        <v>68</v>
       </c>
       <c r="D343" s="43"/>
       <c r="E343" s="43"/>
       <c r="F343" s="43"/>
-      <c r="G343" s="16"/>
-      <c r="H343" s="16"/>
+      <c r="G343" s="16">
+        <v>1</v>
+      </c>
+      <c r="H343" s="16">
+        <v>1</v>
+      </c>
       <c r="I343" s="16"/>
       <c r="J343" s="16"/>
-      <c r="K343" s="16"/>
+      <c r="K343" s="16">
+        <v>1</v>
+      </c>
       <c r="L343" s="16"/>
-      <c r="M343" s="16"/>
+      <c r="M343" s="16">
+        <v>1</v>
+      </c>
       <c r="N343" s="16"/>
       <c r="O343" s="16"/>
-      <c r="P343" s="16"/>
+      <c r="P343" s="16">
+        <v>1</v>
+      </c>
       <c r="Q343" s="16"/>
     </row>
     <row r="344" spans="1:18" x14ac:dyDescent="0.2">
@@ -12105,38 +12117,22 @@
         <v>4</v>
       </c>
       <c r="C344" s="38" t="s">
-        <v>113</v>
+        <v>397</v>
       </c>
       <c r="D344" s="43"/>
       <c r="E344" s="43"/>
       <c r="F344" s="43"/>
-      <c r="G344" s="16">
-        <v>1</v>
-      </c>
-      <c r="H344" s="16">
-        <v>1</v>
-      </c>
-      <c r="I344" s="16">
-        <v>1</v>
-      </c>
-      <c r="J344" s="16">
-        <v>1</v>
-      </c>
-      <c r="K344" s="16">
-        <v>1</v>
-      </c>
-      <c r="L344" s="16">
-        <v>1</v>
-      </c>
+      <c r="G344" s="16"/>
+      <c r="H344" s="16"/>
+      <c r="I344" s="16"/>
+      <c r="J344" s="16"/>
+      <c r="K344" s="16"/>
+      <c r="L344" s="16"/>
       <c r="M344" s="16"/>
       <c r="N344" s="16"/>
       <c r="O344" s="16"/>
-      <c r="P344" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q344" s="16">
-        <v>1</v>
-      </c>
+      <c r="P344" s="16"/>
+      <c r="Q344" s="16"/>
     </row>
     <row r="345" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A345" s="36" t="s">
@@ -12146,89 +12142,95 @@
         <v>4</v>
       </c>
       <c r="C345" s="38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D345" s="43"/>
       <c r="E345" s="43"/>
       <c r="F345" s="43"/>
-      <c r="G345" s="16"/>
-      <c r="H345" s="16"/>
-      <c r="I345" s="16"/>
+      <c r="G345" s="16">
+        <v>1</v>
+      </c>
+      <c r="H345" s="16">
+        <v>1</v>
+      </c>
+      <c r="I345" s="16">
+        <v>1</v>
+      </c>
       <c r="J345" s="16">
         <v>1</v>
       </c>
       <c r="K345" s="16">
         <v>1</v>
       </c>
-      <c r="L345" s="16"/>
-      <c r="M345" s="16">
-        <v>1</v>
-      </c>
+      <c r="L345" s="16">
+        <v>1</v>
+      </c>
+      <c r="M345" s="16"/>
       <c r="N345" s="16"/>
       <c r="O345" s="16"/>
-      <c r="P345" s="16"/>
-      <c r="Q345" s="16"/>
-    </row>
-    <row r="346" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P345" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q345" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="346" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A346" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B346" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C346" s="59" t="s">
-        <v>412</v>
-      </c>
-      <c r="H346" s="43">
-        <v>1</v>
-      </c>
-      <c r="I346" s="43">
-        <v>1</v>
-      </c>
-      <c r="J346" s="43">
-        <v>1</v>
-      </c>
-      <c r="K346" s="43">
-        <v>1</v>
-      </c>
-      <c r="M346" s="43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="347" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C346" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="D346" s="43"/>
+      <c r="E346" s="43"/>
+      <c r="F346" s="43"/>
+      <c r="G346" s="16"/>
+      <c r="H346" s="16"/>
+      <c r="I346" s="16"/>
+      <c r="J346" s="16">
+        <v>1</v>
+      </c>
+      <c r="K346" s="16">
+        <v>1</v>
+      </c>
+      <c r="L346" s="16"/>
+      <c r="M346" s="16">
+        <v>1</v>
+      </c>
+      <c r="N346" s="16"/>
+      <c r="O346" s="16"/>
+      <c r="P346" s="16"/>
+      <c r="Q346" s="16"/>
+    </row>
+    <row r="347" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A347" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B347" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C347" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D347" s="43"/>
-      <c r="E347" s="43"/>
-      <c r="F347" s="43"/>
-      <c r="G347" s="16">
-        <v>1</v>
-      </c>
-      <c r="H347" s="16">
-        <v>1</v>
-      </c>
-      <c r="I347" s="16"/>
-      <c r="J347" s="16">
-        <v>1</v>
-      </c>
-      <c r="K347" s="16">
-        <v>1</v>
-      </c>
-      <c r="L347" s="16"/>
-      <c r="M347" s="16">
-        <v>1</v>
-      </c>
-      <c r="N347" s="16"/>
-      <c r="O347" s="16"/>
-      <c r="P347" s="16"/>
-      <c r="Q347" s="16"/>
+      <c r="C347" s="65" t="s">
+        <v>411</v>
+      </c>
+      <c r="H347" s="43">
+        <v>1</v>
+      </c>
+      <c r="I347" s="43">
+        <v>1</v>
+      </c>
+      <c r="J347" s="43">
+        <v>1</v>
+      </c>
+      <c r="K347" s="43">
+        <v>1</v>
+      </c>
+      <c r="M347" s="43">
+        <v>1</v>
+      </c>
     </row>
     <row r="348" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A348" s="36" t="s">
@@ -12238,18 +12240,28 @@
         <v>4</v>
       </c>
       <c r="C348" s="38" t="s">
-        <v>418</v>
+        <v>42</v>
       </c>
       <c r="D348" s="43"/>
       <c r="E348" s="43"/>
       <c r="F348" s="43"/>
-      <c r="G348" s="16"/>
-      <c r="H348" s="16"/>
+      <c r="G348" s="16">
+        <v>1</v>
+      </c>
+      <c r="H348" s="16">
+        <v>1</v>
+      </c>
       <c r="I348" s="16"/>
-      <c r="J348" s="16"/>
-      <c r="K348" s="16"/>
+      <c r="J348" s="16">
+        <v>1</v>
+      </c>
+      <c r="K348" s="16">
+        <v>1</v>
+      </c>
       <c r="L348" s="16"/>
-      <c r="M348" s="16"/>
+      <c r="M348" s="16">
+        <v>1</v>
+      </c>
       <c r="N348" s="16"/>
       <c r="O348" s="16"/>
       <c r="P348" s="16"/>
@@ -12260,7 +12272,7 @@
         <v>41</v>
       </c>
       <c r="B349" s="37" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C349" s="38" t="s">
         <v>417</v>
@@ -12285,75 +12297,74 @@
         <v>41</v>
       </c>
       <c r="B350" s="37" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C350" s="38" t="s">
-        <v>311</v>
+        <v>416</v>
       </c>
       <c r="D350" s="43"/>
       <c r="E350" s="43"/>
       <c r="F350" s="43"/>
-      <c r="G350" s="16">
-        <v>1</v>
-      </c>
-      <c r="H350" s="16">
-        <v>1</v>
-      </c>
-      <c r="I350" s="16">
-        <v>1</v>
-      </c>
-      <c r="J350" s="16">
-        <v>1</v>
-      </c>
-      <c r="K350" s="16">
-        <v>1</v>
-      </c>
-      <c r="L350" s="16">
-        <v>1</v>
-      </c>
-      <c r="M350" s="16">
-        <v>1</v>
-      </c>
+      <c r="G350" s="16"/>
+      <c r="H350" s="16"/>
+      <c r="I350" s="16"/>
+      <c r="J350" s="16"/>
+      <c r="K350" s="16"/>
+      <c r="L350" s="16"/>
+      <c r="M350" s="16"/>
       <c r="N350" s="16"/>
       <c r="O350" s="16"/>
       <c r="P350" s="16"/>
       <c r="Q350" s="16"/>
     </row>
     <row r="351" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A351" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B351" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C351" s="12" t="s">
-        <v>385</v>
+      <c r="A351" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B351" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C351" s="38" t="s">
+        <v>310</v>
       </c>
       <c r="D351" s="43"/>
       <c r="E351" s="43"/>
       <c r="F351" s="43"/>
-      <c r="G351" s="16"/>
-      <c r="H351" s="16"/>
-      <c r="I351" s="16"/>
-      <c r="J351" s="16"/>
-      <c r="K351" s="16"/>
-      <c r="L351" s="16"/>
-      <c r="M351" s="16"/>
+      <c r="G351" s="16">
+        <v>1</v>
+      </c>
+      <c r="H351" s="16">
+        <v>1</v>
+      </c>
+      <c r="I351" s="16">
+        <v>1</v>
+      </c>
+      <c r="J351" s="16">
+        <v>1</v>
+      </c>
+      <c r="K351" s="16">
+        <v>1</v>
+      </c>
+      <c r="L351" s="16">
+        <v>1</v>
+      </c>
+      <c r="M351" s="16">
+        <v>1</v>
+      </c>
       <c r="N351" s="16"/>
       <c r="O351" s="16"/>
       <c r="P351" s="16"/>
       <c r="Q351" s="16"/>
-      <c r="R351" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="352" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A352" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B352" s="39"/>
+      <c r="B352" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="C352" s="12" t="s">
-        <v>365</v>
+        <v>384</v>
       </c>
       <c r="D352" s="43"/>
       <c r="E352" s="43"/>
@@ -12377,11 +12388,9 @@
       <c r="A353" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B353" s="11" t="s">
-        <v>49</v>
-      </c>
+      <c r="B353" s="39"/>
       <c r="C353" s="12" t="s">
-        <v>350</v>
+        <v>364</v>
       </c>
       <c r="D353" s="43"/>
       <c r="E353" s="43"/>
@@ -12397,6 +12406,9 @@
       <c r="O353" s="16"/>
       <c r="P353" s="16"/>
       <c r="Q353" s="16"/>
+      <c r="R353" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="354" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A354" s="10" t="s">
@@ -12406,66 +12418,63 @@
         <v>49</v>
       </c>
       <c r="C354" s="12" t="s">
-        <v>130</v>
+        <v>349</v>
       </c>
       <c r="D354" s="43"/>
       <c r="E354" s="43"/>
       <c r="F354" s="43"/>
-      <c r="G354" s="16">
-        <v>1</v>
-      </c>
-      <c r="H354" s="16">
-        <v>1</v>
-      </c>
-      <c r="I354" s="16">
-        <v>1</v>
-      </c>
-      <c r="J354" s="16">
-        <v>1</v>
-      </c>
-      <c r="K354" s="16">
-        <v>1</v>
-      </c>
-      <c r="L354" s="16">
-        <v>1</v>
-      </c>
+      <c r="G354" s="16"/>
+      <c r="H354" s="16"/>
+      <c r="I354" s="16"/>
+      <c r="J354" s="16"/>
+      <c r="K354" s="16"/>
+      <c r="L354" s="16"/>
       <c r="M354" s="16"/>
       <c r="N354" s="16"/>
       <c r="O354" s="16"/>
-      <c r="P354" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q354" s="16">
-        <v>1</v>
-      </c>
-      <c r="R354" s="2">
-        <v>1</v>
-      </c>
+      <c r="P354" s="16"/>
+      <c r="Q354" s="16"/>
     </row>
     <row r="355" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A355" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B355" s="11" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C355" s="12" t="s">
-        <v>364</v>
+        <v>130</v>
       </c>
       <c r="D355" s="43"/>
       <c r="E355" s="43"/>
       <c r="F355" s="43"/>
-      <c r="G355" s="16"/>
-      <c r="H355" s="16"/>
-      <c r="I355" s="16"/>
-      <c r="J355" s="16"/>
-      <c r="K355" s="16"/>
-      <c r="L355" s="16"/>
+      <c r="G355" s="16">
+        <v>1</v>
+      </c>
+      <c r="H355" s="16">
+        <v>1</v>
+      </c>
+      <c r="I355" s="16">
+        <v>1</v>
+      </c>
+      <c r="J355" s="16">
+        <v>1</v>
+      </c>
+      <c r="K355" s="16">
+        <v>1</v>
+      </c>
+      <c r="L355" s="16">
+        <v>1</v>
+      </c>
       <c r="M355" s="16"/>
       <c r="N355" s="16"/>
       <c r="O355" s="16"/>
-      <c r="P355" s="16"/>
-      <c r="Q355" s="16"/>
+      <c r="P355" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q355" s="16">
+        <v>1</v>
+      </c>
       <c r="R355" s="2">
         <v>1</v>
       </c>
@@ -12475,37 +12484,23 @@
         <v>45</v>
       </c>
       <c r="B356" s="11" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C356" s="12" t="s">
-        <v>134</v>
+        <v>363</v>
       </c>
       <c r="D356" s="43"/>
       <c r="E356" s="43"/>
       <c r="F356" s="43"/>
-      <c r="G356" s="16">
-        <v>1</v>
-      </c>
-      <c r="H356" s="16">
-        <v>1</v>
-      </c>
-      <c r="I356" s="16">
-        <v>1</v>
-      </c>
-      <c r="J356" s="16">
-        <v>1</v>
-      </c>
-      <c r="K356" s="16">
-        <v>1</v>
-      </c>
-      <c r="L356" s="16">
-        <v>1</v>
-      </c>
+      <c r="G356" s="16"/>
+      <c r="H356" s="16"/>
+      <c r="I356" s="16"/>
+      <c r="J356" s="16"/>
+      <c r="K356" s="16"/>
+      <c r="L356" s="16"/>
       <c r="M356" s="16"/>
       <c r="N356" s="16"/>
-      <c r="O356" s="16">
-        <v>1</v>
-      </c>
+      <c r="O356" s="16"/>
       <c r="P356" s="16"/>
       <c r="Q356" s="16"/>
       <c r="R356" s="2">
@@ -12517,35 +12512,52 @@
         <v>45</v>
       </c>
       <c r="B357" s="11" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C357" s="12" t="s">
-        <v>228</v>
+        <v>134</v>
       </c>
       <c r="D357" s="43"/>
       <c r="E357" s="43"/>
       <c r="F357" s="43"/>
-      <c r="G357" s="16"/>
-      <c r="H357" s="16"/>
-      <c r="I357" s="16"/>
-      <c r="J357" s="16"/>
-      <c r="K357" s="16"/>
-      <c r="L357" s="16"/>
+      <c r="G357" s="16">
+        <v>1</v>
+      </c>
+      <c r="H357" s="16">
+        <v>1</v>
+      </c>
+      <c r="I357" s="16">
+        <v>1</v>
+      </c>
+      <c r="J357" s="16">
+        <v>1</v>
+      </c>
+      <c r="K357" s="16">
+        <v>1</v>
+      </c>
+      <c r="L357" s="16">
+        <v>1</v>
+      </c>
       <c r="M357" s="16"/>
       <c r="N357" s="16"/>
-      <c r="O357" s="16"/>
+      <c r="O357" s="16">
+        <v>1</v>
+      </c>
       <c r="P357" s="16"/>
       <c r="Q357" s="16"/>
+      <c r="R357" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="358" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A358" s="10" t="s">
         <v>45</v>
       </c>
       <c r="B358" s="11" t="s">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="C358" s="12" t="s">
-        <v>399</v>
+        <v>228</v>
       </c>
       <c r="D358" s="43"/>
       <c r="E358" s="43"/>
@@ -12570,28 +12582,20 @@
         <v>49</v>
       </c>
       <c r="C359" s="12" t="s">
-        <v>138</v>
+        <v>398</v>
       </c>
       <c r="D359" s="43"/>
       <c r="E359" s="43"/>
       <c r="F359" s="43"/>
       <c r="G359" s="16"/>
-      <c r="H359" s="16">
-        <v>1</v>
-      </c>
+      <c r="H359" s="16"/>
       <c r="I359" s="16"/>
-      <c r="J359" s="16">
-        <v>1</v>
-      </c>
-      <c r="K359" s="16">
-        <v>1</v>
-      </c>
+      <c r="J359" s="16"/>
+      <c r="K359" s="16"/>
       <c r="L359" s="16"/>
       <c r="M359" s="16"/>
       <c r="N359" s="16"/>
-      <c r="O359" s="16">
-        <v>1</v>
-      </c>
+      <c r="O359" s="16"/>
       <c r="P359" s="16"/>
       <c r="Q359" s="16"/>
     </row>
@@ -12603,20 +12607,28 @@
         <v>49</v>
       </c>
       <c r="C360" s="12" t="s">
-        <v>352</v>
+        <v>138</v>
       </c>
       <c r="D360" s="43"/>
       <c r="E360" s="43"/>
       <c r="F360" s="43"/>
       <c r="G360" s="16"/>
-      <c r="H360" s="16"/>
+      <c r="H360" s="16">
+        <v>1</v>
+      </c>
       <c r="I360" s="16"/>
-      <c r="J360" s="16"/>
-      <c r="K360" s="16"/>
+      <c r="J360" s="16">
+        <v>1</v>
+      </c>
+      <c r="K360" s="16">
+        <v>1</v>
+      </c>
       <c r="L360" s="16"/>
       <c r="M360" s="16"/>
       <c r="N360" s="16"/>
-      <c r="O360" s="16"/>
+      <c r="O360" s="16">
+        <v>1</v>
+      </c>
       <c r="P360" s="16"/>
       <c r="Q360" s="16"/>
     </row>
@@ -12628,7 +12640,7 @@
         <v>49</v>
       </c>
       <c r="C361" s="12" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D361" s="43"/>
       <c r="E361" s="43"/>
@@ -12653,33 +12665,22 @@
         <v>49</v>
       </c>
       <c r="C362" s="12" t="s">
-        <v>139</v>
+        <v>352</v>
       </c>
       <c r="D362" s="43"/>
       <c r="E362" s="43"/>
       <c r="F362" s="43"/>
       <c r="G362" s="16"/>
-      <c r="H362" s="16">
-        <v>1</v>
-      </c>
+      <c r="H362" s="16"/>
       <c r="I362" s="16"/>
-      <c r="J362" s="16">
-        <v>1</v>
-      </c>
-      <c r="K362" s="16">
-        <v>1</v>
-      </c>
+      <c r="J362" s="16"/>
+      <c r="K362" s="16"/>
       <c r="L362" s="16"/>
       <c r="M362" s="16"/>
       <c r="N362" s="16"/>
-      <c r="O362" s="16">
-        <v>1</v>
-      </c>
+      <c r="O362" s="16"/>
       <c r="P362" s="16"/>
       <c r="Q362" s="16"/>
-      <c r="R362" s="2">
-        <v>1</v>
-      </c>
     </row>
     <row r="363" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A363" s="10" t="s">
@@ -12689,20 +12690,16 @@
         <v>49</v>
       </c>
       <c r="C363" s="12" t="s">
-        <v>252</v>
+        <v>139</v>
       </c>
       <c r="D363" s="43"/>
       <c r="E363" s="43"/>
       <c r="F363" s="43"/>
-      <c r="G363" s="16">
-        <v>1</v>
-      </c>
+      <c r="G363" s="16"/>
       <c r="H363" s="16">
         <v>1</v>
       </c>
-      <c r="I363" s="16">
-        <v>1</v>
-      </c>
+      <c r="I363" s="16"/>
       <c r="J363" s="16">
         <v>1</v>
       </c>
@@ -12711,16 +12708,12 @@
       </c>
       <c r="L363" s="16"/>
       <c r="M363" s="16"/>
-      <c r="N363" s="16">
-        <v>1</v>
-      </c>
-      <c r="O363" s="16"/>
-      <c r="P363" s="16">
-        <v>1</v>
-      </c>
-      <c r="Q363" s="16">
-        <v>1</v>
-      </c>
+      <c r="N363" s="16"/>
+      <c r="O363" s="16">
+        <v>1</v>
+      </c>
+      <c r="P363" s="16"/>
+      <c r="Q363" s="16"/>
       <c r="R363" s="2">
         <v>1</v>
       </c>
@@ -12733,7 +12726,7 @@
         <v>49</v>
       </c>
       <c r="C364" s="12" t="s">
-        <v>401</v>
+        <v>252</v>
       </c>
       <c r="D364" s="43"/>
       <c r="E364" s="43"/>
@@ -12821,7 +12814,7 @@
         <v>49</v>
       </c>
       <c r="C366" s="12" t="s">
-        <v>153</v>
+        <v>399</v>
       </c>
       <c r="D366" s="43"/>
       <c r="E366" s="43"/>
@@ -12841,18 +12834,12 @@
       <c r="K366" s="16">
         <v>1</v>
       </c>
-      <c r="L366" s="16">
-        <v>1</v>
-      </c>
-      <c r="M366" s="16">
-        <v>1</v>
-      </c>
+      <c r="L366" s="16"/>
+      <c r="M366" s="16"/>
       <c r="N366" s="16">
         <v>1</v>
       </c>
-      <c r="O366" s="16">
-        <v>1</v>
-      </c>
+      <c r="O366" s="16"/>
       <c r="P366" s="16">
         <v>1</v>
       </c>
@@ -12868,27 +12855,45 @@
         <v>45</v>
       </c>
       <c r="B367" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C367" s="52" t="s">
-        <v>119</v>
-      </c>
-      <c r="G367" s="40">
-        <v>1</v>
-      </c>
-      <c r="H367" s="40">
-        <v>1</v>
-      </c>
-      <c r="J367" s="40">
-        <v>1</v>
-      </c>
-      <c r="K367" s="40">
-        <v>1</v>
-      </c>
-      <c r="L367" s="40">
-        <v>1</v>
-      </c>
-      <c r="N367" s="40">
+        <v>49</v>
+      </c>
+      <c r="C367" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D367" s="43"/>
+      <c r="E367" s="43"/>
+      <c r="F367" s="43"/>
+      <c r="G367" s="16">
+        <v>1</v>
+      </c>
+      <c r="H367" s="16">
+        <v>1</v>
+      </c>
+      <c r="I367" s="16">
+        <v>1</v>
+      </c>
+      <c r="J367" s="16">
+        <v>1</v>
+      </c>
+      <c r="K367" s="16">
+        <v>1</v>
+      </c>
+      <c r="L367" s="16">
+        <v>1</v>
+      </c>
+      <c r="M367" s="16">
+        <v>1</v>
+      </c>
+      <c r="N367" s="16">
+        <v>1</v>
+      </c>
+      <c r="O367" s="16">
+        <v>1</v>
+      </c>
+      <c r="P367" s="16">
+        <v>1</v>
+      </c>
+      <c r="Q367" s="16">
         <v>1</v>
       </c>
       <c r="R367" s="2">
@@ -12899,24 +12904,38 @@
       <c r="A368" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B368" s="51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C368" s="53" t="s">
-        <v>302</v>
-      </c>
-      <c r="H368" s="40">
-        <v>1</v>
-      </c>
-      <c r="K368" s="40">
-        <v>1</v>
-      </c>
-      <c r="L368" s="40">
-        <v>1</v>
-      </c>
-      <c r="N368" s="40">
-        <v>1</v>
-      </c>
+      <c r="B368" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C368" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="D368" s="62"/>
+      <c r="E368" s="62"/>
+      <c r="F368" s="62"/>
+      <c r="G368" s="63">
+        <v>1</v>
+      </c>
+      <c r="H368" s="63">
+        <v>1</v>
+      </c>
+      <c r="I368" s="63"/>
+      <c r="J368" s="63">
+        <v>1</v>
+      </c>
+      <c r="K368" s="63">
+        <v>1</v>
+      </c>
+      <c r="L368" s="63">
+        <v>1</v>
+      </c>
+      <c r="M368" s="63"/>
+      <c r="N368" s="63">
+        <v>1</v>
+      </c>
+      <c r="O368" s="63"/>
+      <c r="P368" s="63"/>
+      <c r="Q368" s="63"/>
       <c r="R368" s="2">
         <v>1</v>
       </c>
@@ -12931,18 +12950,28 @@
       <c r="C369" s="53" t="s">
         <v>301</v>
       </c>
-      <c r="H369" s="40">
-        <v>1</v>
-      </c>
-      <c r="K369" s="40">
-        <v>1</v>
-      </c>
-      <c r="L369" s="40">
-        <v>1</v>
-      </c>
-      <c r="N369" s="40">
-        <v>1</v>
-      </c>
+      <c r="D369" s="62"/>
+      <c r="E369" s="62"/>
+      <c r="F369" s="62"/>
+      <c r="G369" s="63"/>
+      <c r="H369" s="63">
+        <v>1</v>
+      </c>
+      <c r="I369" s="63"/>
+      <c r="J369" s="63"/>
+      <c r="K369" s="63">
+        <v>1</v>
+      </c>
+      <c r="L369" s="63">
+        <v>1</v>
+      </c>
+      <c r="M369" s="63"/>
+      <c r="N369" s="63">
+        <v>1</v>
+      </c>
+      <c r="O369" s="63"/>
+      <c r="P369" s="63"/>
+      <c r="Q369" s="63"/>
       <c r="R369" s="2">
         <v>1</v>
       </c>
@@ -12957,18 +12986,28 @@
       <c r="C370" s="53" t="s">
         <v>300</v>
       </c>
-      <c r="H370" s="40">
-        <v>1</v>
-      </c>
-      <c r="K370" s="40">
-        <v>1</v>
-      </c>
-      <c r="L370" s="40">
-        <v>1</v>
-      </c>
-      <c r="N370" s="40">
-        <v>1</v>
-      </c>
+      <c r="D370" s="62"/>
+      <c r="E370" s="62"/>
+      <c r="F370" s="62"/>
+      <c r="G370" s="63"/>
+      <c r="H370" s="63">
+        <v>1</v>
+      </c>
+      <c r="I370" s="63"/>
+      <c r="J370" s="63"/>
+      <c r="K370" s="63">
+        <v>1</v>
+      </c>
+      <c r="L370" s="63">
+        <v>1</v>
+      </c>
+      <c r="M370" s="63"/>
+      <c r="N370" s="63">
+        <v>1</v>
+      </c>
+      <c r="O370" s="63"/>
+      <c r="P370" s="63"/>
+      <c r="Q370" s="63"/>
       <c r="R370" s="2">
         <v>1</v>
       </c>
@@ -12981,20 +13020,30 @@
         <v>4</v>
       </c>
       <c r="C371" s="53" t="s">
-        <v>303</v>
-      </c>
-      <c r="H371" s="40">
-        <v>1</v>
-      </c>
-      <c r="K371" s="40">
-        <v>1</v>
-      </c>
-      <c r="L371" s="40">
-        <v>1</v>
-      </c>
-      <c r="N371" s="40">
-        <v>1</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="D371" s="62"/>
+      <c r="E371" s="62"/>
+      <c r="F371" s="62"/>
+      <c r="G371" s="63"/>
+      <c r="H371" s="63">
+        <v>1</v>
+      </c>
+      <c r="I371" s="63"/>
+      <c r="J371" s="63"/>
+      <c r="K371" s="63">
+        <v>1</v>
+      </c>
+      <c r="L371" s="63">
+        <v>1</v>
+      </c>
+      <c r="M371" s="63"/>
+      <c r="N371" s="63">
+        <v>1</v>
+      </c>
+      <c r="O371" s="63"/>
+      <c r="P371" s="63"/>
+      <c r="Q371" s="63"/>
       <c r="R371" s="2">
         <v>1</v>
       </c>
@@ -13007,50 +13056,96 @@
         <v>4</v>
       </c>
       <c r="C372" s="53" t="s">
-        <v>304</v>
-      </c>
-      <c r="H372" s="40">
-        <v>1</v>
-      </c>
-      <c r="K372" s="40">
-        <v>1</v>
-      </c>
-      <c r="L372" s="40">
-        <v>1</v>
-      </c>
-      <c r="N372" s="40">
-        <v>1</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="D372" s="62"/>
+      <c r="E372" s="62"/>
+      <c r="F372" s="62"/>
+      <c r="G372" s="63"/>
+      <c r="H372" s="63">
+        <v>1</v>
+      </c>
+      <c r="I372" s="63"/>
+      <c r="J372" s="63"/>
+      <c r="K372" s="63">
+        <v>1</v>
+      </c>
+      <c r="L372" s="63">
+        <v>1</v>
+      </c>
+      <c r="M372" s="63"/>
+      <c r="N372" s="63">
+        <v>1</v>
+      </c>
+      <c r="O372" s="63"/>
+      <c r="P372" s="63"/>
+      <c r="Q372" s="63"/>
       <c r="R372" s="2">
         <v>1</v>
       </c>
     </row>
+    <row r="373" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A373" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B373" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C373" s="53" t="s">
+        <v>303</v>
+      </c>
+      <c r="D373" s="62"/>
+      <c r="E373" s="62"/>
+      <c r="F373" s="62"/>
+      <c r="G373" s="63"/>
+      <c r="H373" s="63">
+        <v>1</v>
+      </c>
+      <c r="I373" s="63"/>
+      <c r="J373" s="63"/>
+      <c r="K373" s="63">
+        <v>1</v>
+      </c>
+      <c r="L373" s="63">
+        <v>1</v>
+      </c>
+      <c r="M373" s="63"/>
+      <c r="N373" s="63">
+        <v>1</v>
+      </c>
+      <c r="O373" s="63"/>
+      <c r="P373" s="63"/>
+      <c r="Q373" s="63"/>
+      <c r="R373" s="2">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:R372" xr:uid="{F00D01EA-5C3E-F64B-8B7F-2EE6141A689A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R372">
-      <sortCondition ref="A1:A372"/>
+  <autoFilter ref="A1:R373" xr:uid="{F00D01EA-5C3E-F64B-8B7F-2EE6141A689A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R373">
+      <sortCondition ref="A1:A373"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q366">
-    <sortCondition ref="A2:A366"/>
-    <sortCondition ref="C2:C366"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q367">
+    <sortCondition ref="A2:A367"/>
+    <sortCondition ref="C2:C367"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="C112" r:id="rId1" display="https://aws.amazon.com/amplify/" xr:uid="{DD07C612-9881-1744-BD8F-2791C5BF0A5F}"/>
-    <hyperlink ref="C301" r:id="rId2" display="https://aws.amazon.com/app-mesh/" xr:uid="{F151395F-8E37-1049-9FCA-8474F2603F07}"/>
+    <hyperlink ref="C302" r:id="rId2" display="https://aws.amazon.com/app-mesh/" xr:uid="{F151395F-8E37-1049-9FCA-8474F2603F07}"/>
     <hyperlink ref="C37" r:id="rId3" display="https://aws.amazon.com/appsync/" xr:uid="{DB5645FD-41DF-9D4C-ADDB-CEEB9418B261}"/>
-    <hyperlink ref="C322" r:id="rId4" display="https://aws.amazon.com/artifact/" xr:uid="{0251BE44-6F83-3541-8CD4-81AEF00F1760}"/>
-    <hyperlink ref="C323" r:id="rId5" display="https://aws.amazon.com/audit-manager/" xr:uid="{FE0C678B-66B4-5041-87CB-7B1FF56DF53B}"/>
+    <hyperlink ref="C323" r:id="rId4" display="https://aws.amazon.com/artifact/" xr:uid="{0251BE44-6F83-3541-8CD4-81AEF00F1760}"/>
+    <hyperlink ref="C324" r:id="rId5" display="https://aws.amazon.com/audit-manager/" xr:uid="{FE0C678B-66B4-5041-87CB-7B1FF56DF53B}"/>
     <hyperlink ref="C211" r:id="rId6" display="https://aws.amazon.com/autoscaling/" xr:uid="{900D412E-B452-CD43-BEB1-C8C1CB7269C8}"/>
     <hyperlink ref="C212" r:id="rId7" display="https://aws.amazon.com/backup/" xr:uid="{E0DD5920-BDCE-E647-9AF3-74760943689B}"/>
     <hyperlink ref="C54" r:id="rId8" display="https://aws.amazon.com/batch/" xr:uid="{784C0A03-DDEC-BE4D-88F7-7005C1BB046B}"/>
     <hyperlink ref="C80" r:id="rId9" display="https://aws.amazon.com/aws-cost-management/aws-budgets/" xr:uid="{57F5A17A-4752-B94C-8FBB-FC20BBF1A0BE}"/>
-    <hyperlink ref="C324" r:id="rId10" display="https://aws.amazon.com/certificate-manager/" xr:uid="{1F5BBCA8-0D50-C44C-907B-68E23D8E605C}"/>
+    <hyperlink ref="C325" r:id="rId10" display="https://aws.amazon.com/certificate-manager/" xr:uid="{1F5BBCA8-0D50-C44C-907B-68E23D8E605C}"/>
     <hyperlink ref="C47" r:id="rId11" display="https://aws.amazon.com/chatbot/" xr:uid="{F29F6239-1ADB-7049-AAA7-6E39F247047B}"/>
-    <hyperlink ref="C303" r:id="rId12" display="https://aws.amazon.com/cloud-map/" xr:uid="{D482891E-9EB7-EA40-9A4B-6A8D3FEADBE3}"/>
+    <hyperlink ref="C304" r:id="rId12" display="https://aws.amazon.com/cloud-map/" xr:uid="{D482891E-9EB7-EA40-9A4B-6A8D3FEADBE3}"/>
     <hyperlink ref="C118" r:id="rId13" display="https://aws.amazon.com/cloud9/" xr:uid="{D565484B-E9EF-EA40-BDBE-0314AF229AE7}"/>
     <hyperlink ref="C213" r:id="rId14" display="https://aws.amazon.com/cloudformation/" xr:uid="{602EC08B-B845-E049-943E-890A120862C8}"/>
-    <hyperlink ref="C326" r:id="rId15" display="https://aws.amazon.com/cloudhsm/" xr:uid="{76B855B6-4A01-1642-8706-3316A1643BA7}"/>
+    <hyperlink ref="C327" r:id="rId15" display="https://aws.amazon.com/cloudhsm/" xr:uid="{76B855B6-4A01-1642-8706-3316A1643BA7}"/>
     <hyperlink ref="C214" r:id="rId16" display="https://aws.amazon.com/cloudtrail/" xr:uid="{F1C2A161-2AD0-B14D-B62A-2640A558856F}"/>
     <hyperlink ref="C121" r:id="rId17" display="https://aws.amazon.com/codeartifact" xr:uid="{A5B8559F-E4FA-BC42-AC7A-9D708C1D63A0}"/>
     <hyperlink ref="C122" r:id="rId18" display="https://aws.amazon.com/codebuild/" xr:uid="{E4144166-80F6-E741-B704-7C3864420913}"/>
@@ -13064,19 +13159,19 @@
     <hyperlink ref="C284" r:id="rId26" display="https://aws.amazon.com/data-exchange/" xr:uid="{EF81BA84-5C8F-DD4B-A31A-47BF7D5C826C}"/>
     <hyperlink ref="C287" r:id="rId27" display="https://aws.amazon.com/datasync" xr:uid="{7CED07B2-F329-1D46-A78D-E74BADEF8307}"/>
     <hyperlink ref="C286" r:id="rId28" display="https://aws.amazon.com/dms/" xr:uid="{C9210BF6-9C8C-5E48-824D-711353B0A5C4}"/>
-    <hyperlink ref="C306" r:id="rId29" display="https://aws.amazon.com/directconnect/" xr:uid="{D4260538-1F28-C64D-999E-B57D8B4A110D}"/>
-    <hyperlink ref="C329" r:id="rId30" display="https://aws.amazon.com/directoryservice/" xr:uid="{71568105-08FB-3E48-ADDD-31FCAC00E550}"/>
+    <hyperlink ref="C307" r:id="rId29" display="https://aws.amazon.com/directconnect/" xr:uid="{D4260538-1F28-C64D-999E-B57D8B4A110D}"/>
+    <hyperlink ref="C330" r:id="rId30" display="https://aws.amazon.com/directoryservice/" xr:uid="{71568105-08FB-3E48-ADDD-31FCAC00E550}"/>
     <hyperlink ref="C57" r:id="rId31" display="https://aws.amazon.com/elasticbeanstalk/" xr:uid="{503FA701-A8C3-BA4D-8F14-4F45B1936437}"/>
     <hyperlink ref="C265" r:id="rId32" display="https://aws.amazon.com/mediaconnect" xr:uid="{97EBEF96-B9F8-0444-803B-77B7686AD926}"/>
     <hyperlink ref="C266" r:id="rId33" display="https://aws.amazon.com/mediaconvert/" xr:uid="{A189CA26-8FE5-724E-AB4C-DA1684A9397C}"/>
     <hyperlink ref="C267" r:id="rId34" display="https://aws.amazon.com/medialive/" xr:uid="{8A1902D4-C3B2-6540-B6A2-D0939C092476}"/>
     <hyperlink ref="C74" r:id="rId35" display="https://aws.amazon.com/fargate/" xr:uid="{8AAC0488-BCAF-394A-B65D-1C8169C9015E}"/>
-    <hyperlink ref="C334" r:id="rId36" display="https://aws.amazon.com/firewall-manager/" xr:uid="{C1FC3FB2-6BB1-124F-AA39-0A32AEF1D03C}"/>
-    <hyperlink ref="C308" r:id="rId37" display="https://aws.amazon.com/global-accelerator" xr:uid="{94823B64-0747-B847-98EC-9C84C21B2DE2}"/>
+    <hyperlink ref="C335" r:id="rId36" display="https://aws.amazon.com/firewall-manager/" xr:uid="{C1FC3FB2-6BB1-124F-AA39-0A32AEF1D03C}"/>
+    <hyperlink ref="C309" r:id="rId37" display="https://aws.amazon.com/global-accelerator" xr:uid="{94823B64-0747-B847-98EC-9C84C21B2DE2}"/>
     <hyperlink ref="C12" r:id="rId38" display="https://aws.amazon.com/glue/" xr:uid="{A2984E2F-A64C-D74C-A499-872A26B2DE44}"/>
-    <hyperlink ref="C321" r:id="rId39" display="https://aws.amazon.com/ground-station/" xr:uid="{DB86E86A-EF5B-2541-9BD8-5CDA9965E40C}"/>
+    <hyperlink ref="C322" r:id="rId39" display="https://aws.amazon.com/ground-station/" xr:uid="{DB86E86A-EF5B-2541-9BD8-5CDA9965E40C}"/>
     <hyperlink ref="C90" r:id="rId40" display="https://aws.amazon.com/iq/" xr:uid="{66074B4A-E4D5-724E-AD29-24C171CEC0BA}"/>
-    <hyperlink ref="C338" r:id="rId41" display="https://aws.amazon.com/iam" xr:uid="{97081695-DB1E-424E-B0EE-79AAD8D6E1CE}"/>
+    <hyperlink ref="C339" r:id="rId41" display="https://aws.amazon.com/iam" xr:uid="{97081695-DB1E-424E-B0EE-79AAD8D6E1CE}"/>
     <hyperlink ref="C154" r:id="rId42" display="https://aws.amazon.com/iot-1-click/" xr:uid="{ADC027FD-055F-9343-AF7A-479D41533208}"/>
     <hyperlink ref="C155" r:id="rId43" display="https://aws.amazon.com/iot-analytics/" xr:uid="{6587843B-FF8F-E445-A148-97BAA80660A5}"/>
     <hyperlink ref="C156" r:id="rId44" display="https://aws.amazon.com/iot/" xr:uid="{72ADB53E-C5C8-6E45-9DE6-006357ADBB14}"/>
@@ -13084,77 +13179,77 @@
     <hyperlink ref="C158" r:id="rId46" display="https://aws.amazon.com/iot-device-management/" xr:uid="{47327A94-A7DA-D44B-8D5D-137A2C1DB78D}"/>
     <hyperlink ref="C160" r:id="rId47" display="https://aws.amazon.com/iot-events/" xr:uid="{09A17074-F045-D045-99F3-289DE651CC4B}"/>
     <hyperlink ref="C163" r:id="rId48" display="https://aws.amazon.com/greengrass/" xr:uid="{86C6B532-C282-AD49-84FC-E7151CC17562}"/>
-    <hyperlink ref="C340" r:id="rId49" display="https://aws.amazon.com/kms/" xr:uid="{C0A6E0DF-7D93-854D-AF8E-5B9C19B8AF02}"/>
+    <hyperlink ref="C341" r:id="rId49" display="https://aws.amazon.com/kms/" xr:uid="{C0A6E0DF-7D93-854D-AF8E-5B9C19B8AF02}"/>
     <hyperlink ref="C25" r:id="rId50" display="https://aws.amazon.com/lake-formation/" xr:uid="{8B1B5135-7A0D-7645-A701-475DDEBCFDA0}"/>
     <hyperlink ref="C59" r:id="rId51" display="https://aws.amazon.com/lambda/" xr:uid="{23B44498-C148-BD4C-86FE-EFAA00464E5B}"/>
     <hyperlink ref="C223" r:id="rId52" display="https://aws.amazon.com/license-manager/" xr:uid="{A80531A2-32DF-5E46-A8A2-AD514A9E876E}"/>
     <hyperlink ref="C92" r:id="rId53" display="https://aws.amazon.com/mp/" xr:uid="{83E81132-B5F9-A141-93D4-67826C5C6C2F}"/>
-    <hyperlink ref="C309" r:id="rId54" display="https://aws.amazon.com/network-firewall/" xr:uid="{380438F2-2136-CA48-8A93-614BD286828F}"/>
+    <hyperlink ref="C310" r:id="rId54" display="https://aws.amazon.com/network-firewall/" xr:uid="{380438F2-2136-CA48-8A93-614BD286828F}"/>
     <hyperlink ref="C228" r:id="rId55" display="https://aws.amazon.com/opsworks/stacks/" xr:uid="{C7B2C66E-7305-8A45-B44D-ED0E58D460E7}"/>
     <hyperlink ref="C226" r:id="rId56" display="https://aws.amazon.com/opsworks/chefautomate/" xr:uid="{44B83691-1D72-4540-A13B-BDA885E2E12D}"/>
     <hyperlink ref="C227" r:id="rId57" display="https://aws.amazon.com/opsworks/puppetenterprise/" xr:uid="{23F41EB8-3A55-A44E-BD0D-93039495EA49}"/>
     <hyperlink ref="C229" r:id="rId58" display="https://aws.amazon.com/organizations" xr:uid="{A3AB0BF0-AC79-A142-8708-144AD8A2BAF3}"/>
     <hyperlink ref="C61" r:id="rId59" display="https://aws.amazon.com/outposts/" xr:uid="{EC0218BA-7EA9-5F4D-8A2F-8D931B087AA0}"/>
     <hyperlink ref="C221" r:id="rId60" display="Personal Health Dashboard" xr:uid="{BC843AAF-6516-F341-B87D-0984C181B4B5}"/>
-    <hyperlink ref="C311" r:id="rId61" display="https://aws.amazon.com/privatelink/" xr:uid="{908DA648-769A-FB47-86E4-3D66FA675B1C}"/>
+    <hyperlink ref="C312" r:id="rId61" display="https://aws.amazon.com/privatelink/" xr:uid="{908DA648-769A-FB47-86E4-3D66FA675B1C}"/>
     <hyperlink ref="C230" r:id="rId62" display="https://aws.amazon.com/proton/" xr:uid="{73BECBB6-D4BE-F445-97BF-0A1D62BCA194}"/>
     <hyperlink ref="C232" r:id="rId63" display="https://aws.amazon.com/ram/" xr:uid="{F8E211FB-42AB-6848-88B7-49CC2A833913}"/>
-    <hyperlink ref="C320" r:id="rId64" display="https://aws.amazon.com/robomaker/" xr:uid="{DBD68496-4CE8-804C-B893-9CFFB849F53A}"/>
-    <hyperlink ref="C344" r:id="rId65" display="https://aws.amazon.com/secrets-manager/" xr:uid="{632A5D67-D598-184C-AB9B-96F30896117D}"/>
-    <hyperlink ref="C345" r:id="rId66" display="https://aws.amazon.com/security-hub/" xr:uid="{342A4832-F3A0-DB4D-840C-8118FD830399}"/>
-    <hyperlink ref="C294" r:id="rId67" display="https://aws.amazon.com/server-migration-service/" xr:uid="{9446514E-0CE8-EC41-A9F1-0DC1FB7ADA55}"/>
+    <hyperlink ref="C321" r:id="rId64" display="https://aws.amazon.com/robomaker/" xr:uid="{DBD68496-4CE8-804C-B893-9CFFB849F53A}"/>
+    <hyperlink ref="C345" r:id="rId65" display="https://aws.amazon.com/secrets-manager/" xr:uid="{632A5D67-D598-184C-AB9B-96F30896117D}"/>
+    <hyperlink ref="C346" r:id="rId66" display="https://aws.amazon.com/security-hub/" xr:uid="{342A4832-F3A0-DB4D-840C-8118FD830399}"/>
+    <hyperlink ref="C295" r:id="rId67" display="https://aws.amazon.com/server-migration-service/" xr:uid="{9446514E-0CE8-EC41-A9F1-0DC1FB7ADA55}"/>
     <hyperlink ref="C62" r:id="rId68" display="https://aws.amazon.com/serverless/serverlessrepo/" xr:uid="{8F7AC4BC-9A37-EC4F-8183-7D7404D19E14}"/>
     <hyperlink ref="C234" r:id="rId69" display="https://aws.amazon.com/servicecatalog/" xr:uid="{2D2653B1-3D13-014A-9B9C-2386E2577635}"/>
-    <hyperlink ref="C347" r:id="rId70" display="https://aws.amazon.com/shield/" xr:uid="{76E091F3-F618-A648-879F-3F09BEBFABFD}"/>
-    <hyperlink ref="C337" r:id="rId71" display="IAM Identity Center (SSO)" xr:uid="{A8360283-DE5C-1140-A85B-F33A2D6F72B8}"/>
-    <hyperlink ref="C295" r:id="rId72" display="https://aws.amazon.com/snowball/" xr:uid="{8A7E1B57-5F26-F64E-853D-BDD63390D5E6}"/>
-    <hyperlink ref="C297" r:id="rId73" display="https://aws.amazon.com/snowmobile/" xr:uid="{62B7D92F-3C96-DA44-9F02-BCC308391061}"/>
+    <hyperlink ref="C348" r:id="rId70" display="https://aws.amazon.com/shield/" xr:uid="{76E091F3-F618-A648-879F-3F09BEBFABFD}"/>
+    <hyperlink ref="C338" r:id="rId71" display="IAM Identity Center (SSO)" xr:uid="{A8360283-DE5C-1140-A85B-F33A2D6F72B8}"/>
+    <hyperlink ref="C296" r:id="rId72" display="https://aws.amazon.com/snowball/" xr:uid="{8A7E1B57-5F26-F64E-853D-BDD63390D5E6}"/>
+    <hyperlink ref="C298" r:id="rId73" display="https://aws.amazon.com/snowmobile/" xr:uid="{62B7D92F-3C96-DA44-9F02-BCC308391061}"/>
     <hyperlink ref="C44" r:id="rId74" display="https://aws.amazon.com/step-functions/details/" xr:uid="{10824B81-0A5F-634D-84E6-9D2ADE3A6B39}"/>
-    <hyperlink ref="C367" r:id="rId75" display="https://aws.amazon.com/storagegateway/" xr:uid="{7BF17EFE-FF03-1D4A-BE9E-1FA982DA5C2A}"/>
+    <hyperlink ref="C368" r:id="rId75" display="https://aws.amazon.com/storagegateway/" xr:uid="{7BF17EFE-FF03-1D4A-BE9E-1FA982DA5C2A}"/>
     <hyperlink ref="C94" r:id="rId76" display="https://aws.amazon.com/premiumsupport/" xr:uid="{A5466C95-EFB7-3944-9E29-8D19BB6E169F}"/>
     <hyperlink ref="C256" r:id="rId77" display="https://aws.amazon.com/systems-manager/" xr:uid="{D6C17500-BE92-C444-BA4A-7116B75319D3}"/>
-    <hyperlink ref="C298" r:id="rId78" display="https://aws.amazon.com/aws-transfer-family/" xr:uid="{F0069BD4-8633-FB4B-8185-293CB3193797}"/>
-    <hyperlink ref="C315" r:id="rId79" display="https://aws.amazon.com/transit-gateway/" xr:uid="{2C10B2F7-EEE3-3444-A855-B387D48706EA}"/>
+    <hyperlink ref="C299" r:id="rId78" display="https://aws.amazon.com/aws-transfer-family/" xr:uid="{F0069BD4-8633-FB4B-8185-293CB3193797}"/>
+    <hyperlink ref="C316" r:id="rId79" display="https://aws.amazon.com/transit-gateway/" xr:uid="{2C10B2F7-EEE3-3444-A855-B387D48706EA}"/>
     <hyperlink ref="C257" r:id="rId80" display="https://aws.amazon.com/premiumsupport/trustedadvisor/" xr:uid="{436ECB3D-7EFE-764A-B2E3-3CF79C97B742}"/>
-    <hyperlink ref="C318" r:id="rId81" display="https://aws.amazon.com/vpn/" xr:uid="{5F2B553B-98BD-8D4B-849C-55A6F659C6B1}"/>
-    <hyperlink ref="C350" r:id="rId82" display="https://aws.amazon.com/waf/" xr:uid="{CF739D06-0B1B-6B46-91CF-6EE57FF09613}"/>
+    <hyperlink ref="C319" r:id="rId81" display="https://aws.amazon.com/vpn/" xr:uid="{5F2B553B-98BD-8D4B-849C-55A6F659C6B1}"/>
+    <hyperlink ref="C351" r:id="rId82" display="https://aws.amazon.com/waf/" xr:uid="{CF739D06-0B1B-6B46-91CF-6EE57FF09613}"/>
     <hyperlink ref="C258" r:id="rId83" display="https://aws.amazon.com/well-architected-tool" xr:uid="{81A34672-555C-B74A-9D7B-58590B7D3C75}"/>
     <hyperlink ref="C142" r:id="rId84" display="https://aws.amazon.com/xray/" xr:uid="{91A2B229-E348-8B4C-AF47-A5192DE45AEC}"/>
-    <hyperlink ref="C300" r:id="rId85" display="https://aws.amazon.com/api-gateway/" xr:uid="{81259B3E-1AB3-F64C-B232-9643470BBB0C}"/>
+    <hyperlink ref="C301" r:id="rId85" display="https://aws.amazon.com/api-gateway/" xr:uid="{81259B3E-1AB3-F64C-B232-9643470BBB0C}"/>
     <hyperlink ref="C36" r:id="rId86" display="https://aws.amazon.com/appflow/" xr:uid="{C427BFEE-537C-9B4C-B5FD-EF94DAB3195F}"/>
     <hyperlink ref="C2" r:id="rId87" display="https://aws.amazon.com/athena/" xr:uid="{8CA6E242-2CF4-E843-A8CA-4391EDA4CB08}"/>
     <hyperlink ref="C169" r:id="rId88" display="https://aws.amazon.com/augmented-ai/" xr:uid="{9B0A35B8-349D-874F-B406-0C378A70E4A7}"/>
     <hyperlink ref="C99" r:id="rId89" display="https://aws.amazon.com/rds/aurora/" xr:uid="{5BA37BE5-5EFA-D640-9340-68572A5C8B0A}"/>
     <hyperlink ref="C48" r:id="rId90" display="https://chime.aws/" xr:uid="{08A22D72-3716-8743-A4B8-3002293D3436}"/>
-    <hyperlink ref="C325" r:id="rId91" display="https://aws.amazon.com/cloud-directory/" xr:uid="{E41D133C-BA4E-4642-BA6F-656788DBC830}"/>
-    <hyperlink ref="C305" r:id="rId92" display="https://aws.amazon.com/cloudfront/" xr:uid="{8065D5C6-B564-A941-80CC-5D6C65B3D725}"/>
+    <hyperlink ref="C326" r:id="rId91" display="https://aws.amazon.com/cloud-directory/" xr:uid="{E41D133C-BA4E-4642-BA6F-656788DBC830}"/>
+    <hyperlink ref="C306" r:id="rId92" display="https://aws.amazon.com/cloudfront/" xr:uid="{8065D5C6-B564-A941-80CC-5D6C65B3D725}"/>
     <hyperlink ref="C215" r:id="rId93" display="https://aws.amazon.com/cloudwatch/" xr:uid="{52B01F49-5EAB-E540-BA38-BEED42EB43F4}"/>
     <hyperlink ref="C125" r:id="rId94" display="https://aws.amazon.com/codeguru/" xr:uid="{D5D1E2B5-ED1C-0D45-BCD8-07A6431E8C14}"/>
-    <hyperlink ref="C327" r:id="rId95" display="https://aws.amazon.com/cognito/" xr:uid="{5631285D-2790-B940-99E8-7A2AFBF2A4F8}"/>
+    <hyperlink ref="C328" r:id="rId95" display="https://aws.amazon.com/cognito/" xr:uid="{5631285D-2790-B940-99E8-7A2AFBF2A4F8}"/>
     <hyperlink ref="C170" r:id="rId96" display="https://aws.amazon.com/comprehend/" xr:uid="{EF9B7DCD-AAB7-C840-B56B-6901E4208F3C}"/>
     <hyperlink ref="C171" r:id="rId97" display="https://aws.amazon.com/comprehend/medical/" xr:uid="{E755C2E6-BB69-1547-AEEA-159FA230C6E0}"/>
-    <hyperlink ref="C328" r:id="rId98" display="https://aws.amazon.com/detective/" xr:uid="{4F6306C8-7E6E-B543-8987-505512DF8B38}"/>
+    <hyperlink ref="C329" r:id="rId98" display="https://aws.amazon.com/detective/" xr:uid="{4F6306C8-7E6E-B543-8987-505512DF8B38}"/>
     <hyperlink ref="C176" r:id="rId99" display="https://aws.amazon.com/devops-guru/" xr:uid="{0DE3687A-6EED-D846-93EF-2FF3EDCA2FE7}"/>
     <hyperlink ref="C100" r:id="rId100" display="https://aws.amazon.com/documentdb/" xr:uid="{E9BE873B-93B3-744C-82A3-AE676C942786}"/>
     <hyperlink ref="C101" r:id="rId101" display="https://aws.amazon.com/dynamodb/" xr:uid="{667C0B17-E586-7843-9ABA-2156F328D1C2}"/>
     <hyperlink ref="C104" r:id="rId102" display="https://aws.amazon.com/elasticache/" xr:uid="{0D3B6893-EB9F-F441-97F2-EAE3A531E741}"/>
-    <hyperlink ref="C354" r:id="rId103" display="https://aws.amazon.com/ebs/" xr:uid="{6475A1BA-F9EA-3643-A91C-960971815276}"/>
+    <hyperlink ref="C355" r:id="rId103" display="https://aws.amazon.com/ebs/" xr:uid="{6475A1BA-F9EA-3643-A91C-960971815276}"/>
     <hyperlink ref="C55" r:id="rId104" xr:uid="{F6BE2D25-6B4D-D545-BEF5-6353621F7D77}"/>
     <hyperlink ref="C71" r:id="rId105" display="https://aws.amazon.com/ecr/" xr:uid="{4DB8575D-FD4E-F24B-9A6D-4B237DEB4216}"/>
     <hyperlink ref="C72" r:id="rId106" display="https://aws.amazon.com/ecs/" xr:uid="{2A857716-DB7F-4D4C-9C3A-923E359FCE4B}"/>
-    <hyperlink ref="C356" r:id="rId107" display="https://aws.amazon.com/efs/" xr:uid="{17293663-847A-2945-BEEE-DB5C14186604}"/>
+    <hyperlink ref="C357" r:id="rId107" display="https://aws.amazon.com/efs/" xr:uid="{17293663-847A-2945-BEEE-DB5C14186604}"/>
     <hyperlink ref="C177" r:id="rId108" display="https://aws.amazon.com/elastic-inference/" xr:uid="{D7F32AC2-662A-044F-8D07-6056298BD732}"/>
     <hyperlink ref="C73" r:id="rId109" display="https://aws.amazon.com/eks" xr:uid="{8EA95DB8-FAF6-354A-8701-9BC26B99AF7A}"/>
     <hyperlink ref="C6" r:id="rId110" display="https://aws.amazon.com/emr/" xr:uid="{45F7CBE2-565C-A24D-A38F-B3A8800D8B65}"/>
     <hyperlink ref="C28" r:id="rId111" display="Elasticsearch Service (ES) / OpenSearch Service" xr:uid="{6AF99F4A-A394-8249-8B46-B05EDE624400}"/>
     <hyperlink ref="C38" r:id="rId112" display="https://aws.amazon.com/eventbridge/" xr:uid="{66CE333B-4CBB-9246-B3B7-51C615E2BFF5}"/>
-    <hyperlink ref="C359" r:id="rId113" display="https://aws.amazon.com/fsx/lustre/" xr:uid="{723E4B6B-4225-F149-A1D1-0C9ED96BB728}"/>
-    <hyperlink ref="C362" r:id="rId114" display="https://aws.amazon.com/fsx/windows/" xr:uid="{1B6B9E68-B13B-3B45-B1A5-A8F3F5BDE985}"/>
+    <hyperlink ref="C360" r:id="rId113" display="https://aws.amazon.com/fsx/lustre/" xr:uid="{723E4B6B-4225-F149-A1D1-0C9ED96BB728}"/>
+    <hyperlink ref="C363" r:id="rId114" display="https://aws.amazon.com/fsx/windows/" xr:uid="{1B6B9E68-B13B-3B45-B1A5-A8F3F5BDE985}"/>
     <hyperlink ref="C178" r:id="rId115" display="https://aws.amazon.com/forecast/" xr:uid="{1F07E3AD-D0E3-4442-9220-92E85E3DF861}"/>
     <hyperlink ref="C179" r:id="rId116" display="https://aws.amazon.com/fraud-detector/" xr:uid="{A16ABA87-0E9D-1749-BE3E-718E7599E24B}"/>
     <hyperlink ref="C148" r:id="rId117" display="https://aws.amazon.com/gamelift/" xr:uid="{ABE766D8-2E8B-B341-9103-F503839AC514}"/>
-    <hyperlink ref="C335" r:id="rId118" display="https://aws.amazon.com/guardduty/" xr:uid="{D1B6E14A-AD6C-E844-9AD0-215698F4E3BE}"/>
-    <hyperlink ref="C339" r:id="rId119" display="https://aws.amazon.com/inspector/" xr:uid="{176BE9A8-3FF5-874F-8EFA-6BB4665C2F33}"/>
+    <hyperlink ref="C336" r:id="rId118" display="https://aws.amazon.com/guardduty/" xr:uid="{D1B6E14A-AD6C-E844-9AD0-215698F4E3BE}"/>
+    <hyperlink ref="C340" r:id="rId119" display="https://aws.amazon.com/inspector/" xr:uid="{176BE9A8-3FF5-874F-8EFA-6BB4665C2F33}"/>
     <hyperlink ref="C105" r:id="rId120" display="https://aws.amazon.com/keyspaces/" xr:uid="{08537BC8-9E18-E341-B811-B357F4073FF5}"/>
     <hyperlink ref="C22" r:id="rId121" display="https://aws.amazon.com/kinesis/analytics/" xr:uid="{55091A39-96DB-9A41-B453-9AB88556B85B}"/>
     <hyperlink ref="C23" r:id="rId122" display="https://aws.amazon.com/kinesis/firehose/" xr:uid="{AB91BD64-7EBD-8A40-89D5-415AC999E5A7}"/>
@@ -13165,7 +13260,7 @@
     <hyperlink ref="C182" r:id="rId127" display="https://aws.amazon.com/lookout-for-vision/" xr:uid="{56891F15-488A-2D4F-957F-9C19DBC09E8C}"/>
     <hyperlink ref="C150" r:id="rId128" display="https://aws.amazon.com/lumberyard/" xr:uid="{0793FA7F-F861-E448-B351-2625AB793E29}"/>
     <hyperlink ref="C40" r:id="rId129" display="https://aws.amazon.com/amazon-mq/" xr:uid="{8F7E8190-F83B-7E45-9B55-465E1F7C79F3}"/>
-    <hyperlink ref="C342" r:id="rId130" display="https://aws.amazon.com/macie/" xr:uid="{0A9A9C7B-64FF-4944-8B73-82D7A54412E2}"/>
+    <hyperlink ref="C343" r:id="rId130" display="https://aws.amazon.com/macie/" xr:uid="{0A9A9C7B-64FF-4944-8B73-82D7A54412E2}"/>
     <hyperlink ref="C26" r:id="rId131" display="https://aws.amazon.com/msk/" xr:uid="{46024F01-6B35-0740-B92F-18BA0D596F3D}"/>
     <hyperlink ref="C39" r:id="rId132" display="https://aws.amazon.com/managed-workflows-for-apache-airflow/" xr:uid="{E7D50CE9-B395-AE40-B3BD-7B31072C139C}"/>
     <hyperlink ref="C107" r:id="rId133" display="https://aws.amazon.com/neptune/" xr:uid="{35EB7CA9-2F10-7E4E-9B05-D1C561AFFA79}"/>
@@ -13176,12 +13271,12 @@
     <hyperlink ref="C30" r:id="rId138" display="https://aws.amazon.com/redshift/" xr:uid="{BD068AB5-9542-BA4D-9D2D-3E01553833FF}"/>
     <hyperlink ref="C186" r:id="rId139" display="https://aws.amazon.com/rekognition/" xr:uid="{06B644B6-712E-EB4F-BDC1-2826A6E207A2}"/>
     <hyperlink ref="C110" r:id="rId140" display="https://aws.amazon.com/rds/" xr:uid="{52A384FE-5551-524F-8BE4-640C39EE59DB}"/>
-    <hyperlink ref="C312" r:id="rId141" display="https://aws.amazon.com/route53/" xr:uid="{2B9EF04D-DB6D-9948-8F0B-1F85D1FFA02C}"/>
+    <hyperlink ref="C313" r:id="rId141" display="https://aws.amazon.com/route53/" xr:uid="{2B9EF04D-DB6D-9948-8F0B-1F85D1FFA02C}"/>
     <hyperlink ref="C187" r:id="rId142" display="https://aws.amazon.com/sagemaker/" xr:uid="{FF819C8F-B472-6A4D-BF36-8803B10C8D16}"/>
     <hyperlink ref="C98" r:id="rId143" display="https://aws.amazon.com/ses/" xr:uid="{708BC6D8-3F72-374C-AB65-9002B2EB5C60}"/>
     <hyperlink ref="C41" r:id="rId144" display="https://aws.amazon.com/sns/" xr:uid="{2A7374BD-4C80-7C42-9E56-E3671DF3D17F}"/>
     <hyperlink ref="C42" r:id="rId145" display="https://aws.amazon.com/sqs/" xr:uid="{7EC87AB6-C5A3-0F4B-915C-BD9EF4201FD5}"/>
-    <hyperlink ref="C366" r:id="rId146" display="https://aws.amazon.com/s3/" xr:uid="{CD425C97-24D5-9747-8B23-DF9DD7A486F9}"/>
+    <hyperlink ref="C367" r:id="rId146" display="https://aws.amazon.com/s3/" xr:uid="{CD425C97-24D5-9747-8B23-DF9DD7A486F9}"/>
     <hyperlink ref="C43" r:id="rId147" display="https://aws.amazon.com/swf/" xr:uid="{631F304E-E46F-644E-8407-57836778A272}"/>
     <hyperlink ref="C152" r:id="rId148" display="https://aws.amazon.com/sumerian/" xr:uid="{1F8D41FC-B82F-8C44-A79F-AA91C3811E29}"/>
     <hyperlink ref="C206" r:id="rId149" display="https://aws.amazon.com/textract" xr:uid="{E50E8082-94C1-7947-963B-3A384A890F42}"/>
@@ -13189,22 +13284,22 @@
     <hyperlink ref="C207" r:id="rId151" display="https://aws.amazon.com/transcribe/" xr:uid="{7391FC88-BBA3-5846-9CA8-5612809D5D1E}"/>
     <hyperlink ref="C208" r:id="rId152" display="https://aws.amazon.com/transcribe/medical/" xr:uid="{5D3CF2D8-5264-E342-A8E8-E042131AE7AF}"/>
     <hyperlink ref="C209" r:id="rId153" display="https://aws.amazon.com/translate/" xr:uid="{D94B1850-F477-024B-8A15-72298FF44F81}"/>
-    <hyperlink ref="C316" r:id="rId154" display="https://aws.amazon.com/vpc/" xr:uid="{81704202-B35B-314F-9611-62D10520486C}"/>
+    <hyperlink ref="C317" r:id="rId154" display="https://aws.amazon.com/vpc/" xr:uid="{81704202-B35B-314F-9611-62D10520486C}"/>
     <hyperlink ref="C145" r:id="rId155" display="https://aws.amazon.com/worklink/" xr:uid="{A564F6A5-A25E-984E-AB0E-10859F299F79}"/>
-    <hyperlink ref="C352" r:id="rId156" display="https://aws.amazon.com/cloudendure-disaster-recovery/" xr:uid="{19E2670B-B70B-2246-875A-A798E313AD4C}"/>
+    <hyperlink ref="C353" r:id="rId156" display="https://aws.amazon.com/cloudendure-disaster-recovery/" xr:uid="{19E2670B-B70B-2246-875A-A798E313AD4C}"/>
     <hyperlink ref="C283" r:id="rId157" display="https://aws.amazon.com/cloudendure-migration/" xr:uid="{3011454A-BA14-2640-A5B0-1665DE5015EB}"/>
-    <hyperlink ref="C307" r:id="rId158" display="https://aws.amazon.com/elasticloadbalancing/" xr:uid="{48C41A56-7B49-954B-8607-BA52CE86305D}"/>
+    <hyperlink ref="C308" r:id="rId158" display="https://aws.amazon.com/elasticloadbalancing/" xr:uid="{48C41A56-7B49-954B-8607-BA52CE86305D}"/>
     <hyperlink ref="C153" r:id="rId159" display="https://aws.amazon.com/freertos/" xr:uid="{9A951967-4675-1546-8716-0568BF98D1CE}"/>
     <hyperlink ref="C64" r:id="rId160" display="https://aws.amazon.com/vmware/" xr:uid="{1D088AE8-27BE-C042-AB38-9D218A238493}"/>
     <hyperlink ref="C58" r:id="rId161" display="https://aws.amazon.com/ec2/" xr:uid="{A67A7092-80C0-9A4E-A55B-97FA160377E8}"/>
-    <hyperlink ref="C364" r:id="rId162" display="S3 Glacier" xr:uid="{9237F063-BA80-DC44-882A-D4F7F6FD5EE9}"/>
+    <hyperlink ref="C365" r:id="rId162" display="S3 Glacier" xr:uid="{9237F063-BA80-DC44-882A-D4F7F6FD5EE9}"/>
     <hyperlink ref="C132" r:id="rId163" xr:uid="{75CD952A-625F-DE4E-B2D6-41E51DC1F7E3}"/>
     <hyperlink ref="C45" r:id="rId164" display="Managed Blockchain" xr:uid="{49E4FD14-55A4-2E46-8EFF-5EF1766DCF38}"/>
-    <hyperlink ref="C296" r:id="rId165" xr:uid="{7054BAB5-94B7-0C4D-A749-E850E72E4B65}"/>
+    <hyperlink ref="C297" r:id="rId165" xr:uid="{7054BAB5-94B7-0C4D-A749-E850E72E4B65}"/>
     <hyperlink ref="C97" r:id="rId166" xr:uid="{AD71ACB3-ABC2-514F-A36F-2373C95B6534}"/>
     <hyperlink ref="C96" r:id="rId167" xr:uid="{BD82E153-E205-2541-8061-196FC264C5B0}"/>
     <hyperlink ref="C10" r:id="rId168" xr:uid="{A6E6DBD8-12FD-894D-842E-E5DA02E3DBF4}"/>
-    <hyperlink ref="C14" r:id="rId169" xr:uid="{3BA957C8-CD3E-8248-A27A-F3A9F071F7E4}"/>
+    <hyperlink ref="C15" r:id="rId169" xr:uid="{3BA957C8-CD3E-8248-A27A-F3A9F071F7E4}"/>
     <hyperlink ref="C4" r:id="rId170" xr:uid="{1AF55A29-37E6-4C43-AA7B-0619293C9418}"/>
     <hyperlink ref="C134" r:id="rId171" xr:uid="{65854783-F9AA-2D48-AD7A-DAC4D0360562}"/>
     <hyperlink ref="C131" r:id="rId172" xr:uid="{284D93AA-4E06-6040-8A42-498B60D37169}"/>
@@ -13213,7 +13308,7 @@
     <hyperlink ref="C65" r:id="rId175" xr:uid="{005354BD-081E-9E46-8937-381CB8592473}"/>
     <hyperlink ref="C70" r:id="rId176" xr:uid="{1CFA07FC-268F-C84D-B8E8-D13B2E092826}"/>
     <hyperlink ref="C224" r:id="rId177" xr:uid="{667DCA05-C10B-394B-ADBD-C91C39C8EFA9}"/>
-    <hyperlink ref="C357" r:id="rId178" xr:uid="{19712BF9-B0E9-FC4A-855C-37C622207421}"/>
+    <hyperlink ref="C358" r:id="rId178" xr:uid="{19712BF9-B0E9-FC4A-855C-37C622207421}"/>
     <hyperlink ref="C120" r:id="rId179" xr:uid="{532F9FAB-7588-934A-BECA-94DB57B3EA86}"/>
     <hyperlink ref="C115" r:id="rId180" xr:uid="{03EA6A9E-9AED-E449-AEAE-E07C9D687ADF}"/>
     <hyperlink ref="C141" r:id="rId181" xr:uid="{1A9B8E63-391D-0446-8004-324356B6D2C7}"/>
@@ -13247,7 +13342,7 @@
     <hyperlink ref="C243" r:id="rId209" xr:uid="{D7F493BC-3996-E14D-8B4E-AF698AF15CF3}"/>
     <hyperlink ref="C249" r:id="rId210" xr:uid="{158C22B5-B282-0E45-819B-E1F6D3588EB5}"/>
     <hyperlink ref="C244" r:id="rId211" xr:uid="{060EF427-1526-CB41-B8B7-D967487671FE}"/>
-    <hyperlink ref="C363" r:id="rId212" display="S3 Glacier" xr:uid="{69E65928-2461-9D41-874A-E2DD597C93F4}"/>
+    <hyperlink ref="C364" r:id="rId212" display="S3 Glacier" xr:uid="{69E65928-2461-9D41-874A-E2DD597C93F4}"/>
     <hyperlink ref="C195" r:id="rId213" xr:uid="{985BD89A-8A6D-3646-8654-90328345A506}"/>
     <hyperlink ref="C172" r:id="rId214" xr:uid="{590CE714-967E-A245-B8FF-739BCA3B026A}"/>
     <hyperlink ref="C173" r:id="rId215" xr:uid="{1D9605EA-560D-C04A-9C84-34D242F7CD14}"/>
@@ -13258,7 +13353,7 @@
     <hyperlink ref="C49" r:id="rId220" xr:uid="{94ED9A38-CC0B-6547-A3F8-0E1E5184307C}"/>
     <hyperlink ref="C52" r:id="rId221" xr:uid="{484C0088-17D4-5E46-9E7E-4B7D0CADC15E}"/>
     <hyperlink ref="C53" r:id="rId222" xr:uid="{AD3D4FE9-D4D4-D34A-8BFC-469E359937BD}"/>
-    <hyperlink ref="C319" r:id="rId223" xr:uid="{1A1FF780-D417-4E48-8B89-324891ACD5EB}"/>
+    <hyperlink ref="C320" r:id="rId223" xr:uid="{1A1FF780-D417-4E48-8B89-324891ACD5EB}"/>
     <hyperlink ref="C290" r:id="rId224" xr:uid="{A55A32E4-E04D-3D4E-B771-FF5015CDE5FC}"/>
     <hyperlink ref="C291" r:id="rId225" xr:uid="{470F8C84-D502-374E-8550-CF45C7EE93CD}"/>
     <hyperlink ref="C81" r:id="rId226" display="Cost and Usage Report" xr:uid="{14B6B46E-839F-BF4A-B271-B234D8C79A65}"/>
@@ -13269,13 +13364,13 @@
     <hyperlink ref="C165" r:id="rId231" xr:uid="{40FD60AC-B589-0B4B-AB36-1989E529CD39}"/>
     <hyperlink ref="C167" r:id="rId232" xr:uid="{56F27AA2-5183-E94B-ACC4-73885A21F096}"/>
     <hyperlink ref="C76" r:id="rId233" display="Managed Service for Prometheus" xr:uid="{15FBF981-0EC3-6343-ACAF-575D9CF01C72}"/>
-    <hyperlink ref="C330" r:id="rId234" display="Directory Service AD Connector" xr:uid="{CE8FDA92-983D-F241-9A3C-214FB6ED4987}"/>
-    <hyperlink ref="C332" r:id="rId235" display="Directory Service Simple AD" xr:uid="{BDF803C1-C55F-7B4E-B548-FB056C33B7F8}"/>
-    <hyperlink ref="C331" r:id="rId236" display="Directory Service Managed Microsoft AD" xr:uid="{A2682350-698B-164E-854C-B72B425BF114}"/>
+    <hyperlink ref="C331" r:id="rId234" display="Directory Service AD Connector" xr:uid="{CE8FDA92-983D-F241-9A3C-214FB6ED4987}"/>
+    <hyperlink ref="C333" r:id="rId235" display="Directory Service Simple AD" xr:uid="{BDF803C1-C55F-7B4E-B548-FB056C33B7F8}"/>
+    <hyperlink ref="C332" r:id="rId236" display="Directory Service Managed Microsoft AD" xr:uid="{A2682350-698B-164E-854C-B72B425BF114}"/>
     <hyperlink ref="C225" r:id="rId237" xr:uid="{51AE8255-80F9-1246-AF04-CAD49D7BD8ED}"/>
     <hyperlink ref="C133" r:id="rId238" xr:uid="{F72E5D13-7F9C-A74A-B15B-60DA5CBC35BF}"/>
     <hyperlink ref="C180" r:id="rId239" xr:uid="{A021BA43-B246-CF41-8A4E-1E391CD06D94}"/>
-    <hyperlink ref="C288" r:id="rId240" xr:uid="{66C98670-091A-A841-9473-A308D3D03C92}"/>
+    <hyperlink ref="C294" r:id="rId240" display="DMS Schema Convertion Tool (SCT)" xr:uid="{66C98670-091A-A841-9473-A308D3D03C92}"/>
     <hyperlink ref="C109" r:id="rId241" xr:uid="{A18DAD6F-3F0D-2F41-8ECF-C20C2E59C987}"/>
     <hyperlink ref="C91" r:id="rId242" xr:uid="{BB9AA509-E09D-604B-9392-FAF5D5E1155F}"/>
     <hyperlink ref="C93" r:id="rId243" xr:uid="{2260673B-2C63-EA41-A726-76787E04ADC6}"/>
@@ -13308,11 +13403,11 @@
     <hyperlink ref="C278" r:id="rId270" xr:uid="{3B6EA2BE-9E87-CD43-BD86-90EF411A17C9}"/>
     <hyperlink ref="C279" r:id="rId271" xr:uid="{BE5AE3F2-6AF4-FB45-A4C7-58EE1FA83493}"/>
     <hyperlink ref="C280" r:id="rId272" xr:uid="{9F9A6701-301A-8946-8181-9D1074CEB3F6}"/>
-    <hyperlink ref="C372" r:id="rId273" display="Storage Gateway - Volume Gateway" xr:uid="{D2EC8952-5BC9-2B49-B394-D7BE012603FF}"/>
-    <hyperlink ref="C370" r:id="rId274" xr:uid="{1B5D263F-5321-B54A-BF60-2932447DCE26}"/>
-    <hyperlink ref="C368" r:id="rId275" display="Storage Gateway - FSx File Gateway" xr:uid="{2125FCAA-C46E-224B-8BE0-19D32D161491}"/>
-    <hyperlink ref="C369" r:id="rId276" display="Storage Gateway - S3 File Gateway" xr:uid="{96B9D02E-E08D-3E44-9C8E-08A2BE24E99A}"/>
-    <hyperlink ref="C371" r:id="rId277" display="Storage Gateway - Volume Gateway" xr:uid="{FFBC4DD5-5D45-9B42-A545-70A2598E87B0}"/>
+    <hyperlink ref="C373" r:id="rId273" display="Storage Gateway - Volume Gateway" xr:uid="{D2EC8952-5BC9-2B49-B394-D7BE012603FF}"/>
+    <hyperlink ref="C371" r:id="rId274" xr:uid="{1B5D263F-5321-B54A-BF60-2932447DCE26}"/>
+    <hyperlink ref="C369" r:id="rId275" display="Storage Gateway - FSx File Gateway" xr:uid="{2125FCAA-C46E-224B-8BE0-19D32D161491}"/>
+    <hyperlink ref="C370" r:id="rId276" display="Storage Gateway - S3 File Gateway" xr:uid="{96B9D02E-E08D-3E44-9C8E-08A2BE24E99A}"/>
+    <hyperlink ref="C372" r:id="rId277" display="Storage Gateway - Volume Gateway" xr:uid="{FFBC4DD5-5D45-9B42-A545-70A2598E87B0}"/>
     <hyperlink ref="C32" r:id="rId278" xr:uid="{F8A9F9A7-CC98-EC42-8596-0253E0A2BB97}"/>
     <hyperlink ref="C31" r:id="rId279" xr:uid="{8B655CFD-0968-7140-84E8-2070B49F002B}"/>
     <hyperlink ref="C35" r:id="rId280" xr:uid="{FD22D76A-0562-0640-85D0-C48AA580C483}"/>
@@ -13322,15 +13417,15 @@
     <hyperlink ref="C143" r:id="rId284" xr:uid="{5961D4D9-3072-2149-961B-0C10629539E7}"/>
     <hyperlink ref="C106" r:id="rId285" xr:uid="{863934C0-971A-AF48-A43D-B4B914AECC39}"/>
     <hyperlink ref="C220" r:id="rId286" xr:uid="{3295CEB8-10D1-5A43-BEA9-DF5FD886C0AB}"/>
-    <hyperlink ref="C360" r:id="rId287" display="Amazon FSx for NetApp ONTAP" xr:uid="{4F9FE344-D5EC-AC40-97FF-2F5F45F27D96}"/>
+    <hyperlink ref="C361" r:id="rId287" display="Amazon FSx for NetApp ONTAP" xr:uid="{4F9FE344-D5EC-AC40-97FF-2F5F45F27D96}"/>
     <hyperlink ref="C240" r:id="rId288" xr:uid="{AEDB8326-231C-C744-8B10-AF02B678D9B4}"/>
     <hyperlink ref="C21" r:id="rId289" xr:uid="{2E249962-989F-944F-B761-2BAA0EC7CAEC}"/>
     <hyperlink ref="C210" r:id="rId290" xr:uid="{DCE5737A-9A5B-DC4D-850F-450E2D238525}"/>
     <hyperlink ref="C56" r:id="rId291" xr:uid="{FE31CE04-AE8C-B545-B85E-3E35079AA70A}"/>
-    <hyperlink ref="C302" r:id="rId292" xr:uid="{D321FD11-72A4-9F4D-857D-939FF8BB6E1B}"/>
-    <hyperlink ref="C313" r:id="rId293" xr:uid="{E997CB7A-902E-064D-B6FF-8470A806D5A0}"/>
-    <hyperlink ref="C317" r:id="rId294" xr:uid="{0A132D4A-E971-7246-889D-EB0D9E3ED74A}"/>
-    <hyperlink ref="C336" r:id="rId295" xr:uid="{5D89926F-F8DE-F748-ADBE-85B87EFE8273}"/>
+    <hyperlink ref="C303" r:id="rId292" xr:uid="{D321FD11-72A4-9F4D-857D-939FF8BB6E1B}"/>
+    <hyperlink ref="C314" r:id="rId293" xr:uid="{E997CB7A-902E-064D-B6FF-8470A806D5A0}"/>
+    <hyperlink ref="C318" r:id="rId294" xr:uid="{0A132D4A-E971-7246-889D-EB0D9E3ED74A}"/>
+    <hyperlink ref="C337" r:id="rId295" xr:uid="{5D89926F-F8DE-F748-ADBE-85B87EFE8273}"/>
     <hyperlink ref="C159" r:id="rId296" xr:uid="{2B14DC1E-31E9-E643-8322-E37BB77A61F2}"/>
     <hyperlink ref="C292" r:id="rId297" xr:uid="{09886B01-263E-164A-BB8E-628947483324}"/>
     <hyperlink ref="C293" r:id="rId298" xr:uid="{5F2F3CFC-7F4A-FD4D-941C-DED03BD1B5FC}"/>
@@ -13347,26 +13442,26 @@
     <hyperlink ref="C259" r:id="rId309" xr:uid="{B6E1487F-81B1-384D-A9E3-DFD2ED50BF4B}"/>
     <hyperlink ref="C168" r:id="rId310" xr:uid="{AABC9A1F-7500-A844-B34D-0F19697B9A7A}"/>
     <hyperlink ref="C289" r:id="rId311" xr:uid="{4CB123AC-879F-9640-AC36-E72ADF139A0B}"/>
-    <hyperlink ref="C310" r:id="rId312" xr:uid="{66E15034-4647-CC49-90EC-3F56811C1769}"/>
+    <hyperlink ref="C311" r:id="rId312" xr:uid="{66E15034-4647-CC49-90EC-3F56811C1769}"/>
     <hyperlink ref="C189" r:id="rId313" xr:uid="{84E59E87-0965-C841-99D9-BFFDDC987D42}"/>
     <hyperlink ref="C166" r:id="rId314" xr:uid="{31C0844F-7C3B-2D40-BFE8-59E8221E3954}"/>
     <hyperlink ref="C162" r:id="rId315" xr:uid="{54A2747E-43BA-F045-9C52-0FB8E93DA59A}"/>
     <hyperlink ref="C75" r:id="rId316" xr:uid="{1EB66100-17E6-1342-A186-2BA2C2F63D22}"/>
-    <hyperlink ref="C353" r:id="rId317" xr:uid="{DB538155-C3BB-2A40-8FD1-CA65D903A17D}"/>
+    <hyperlink ref="C354" r:id="rId317" xr:uid="{DB538155-C3BB-2A40-8FD1-CA65D903A17D}"/>
     <hyperlink ref="C161" r:id="rId318" xr:uid="{C3A4EFBA-B189-BD45-BFF4-A1CD0FD8C94F}"/>
-    <hyperlink ref="C361" r:id="rId319" xr:uid="{88BA82AB-CEFC-3744-A41B-1FD7D1E7136C}"/>
+    <hyperlink ref="C362" r:id="rId319" xr:uid="{88BA82AB-CEFC-3744-A41B-1FD7D1E7136C}"/>
     <hyperlink ref="C136" r:id="rId320" xr:uid="{8DA90EA8-849B-1B49-A28C-2A2F266777EE}"/>
     <hyperlink ref="C198" r:id="rId321" xr:uid="{FE15D563-8EB3-6F43-BE1A-57E5433E3D5C}"/>
     <hyperlink ref="C202" r:id="rId322" xr:uid="{6C62A9C8-F029-FD4F-9476-C123AA75F8CA}"/>
     <hyperlink ref="C205" r:id="rId323" xr:uid="{DDCE13ED-0142-5945-A2C6-130062ABEE93}"/>
     <hyperlink ref="C204" r:id="rId324" xr:uid="{415C97AE-1F89-544C-8B1E-74D49B61D9CB}"/>
-    <hyperlink ref="C304" r:id="rId325" xr:uid="{0A929205-34D3-2E4E-8A75-0F460592E6C2}"/>
+    <hyperlink ref="C305" r:id="rId325" xr:uid="{0A929205-34D3-2E4E-8A75-0F460592E6C2}"/>
     <hyperlink ref="C113" r:id="rId326" xr:uid="{252D9266-A9E4-114B-BB96-706914B83BD1}"/>
     <hyperlink ref="C130" r:id="rId327" display="Construct Hub" xr:uid="{D5570897-0906-F349-9A5A-0C3635E773E7}"/>
     <hyperlink ref="C151" r:id="rId328" xr:uid="{DA0855F0-F663-864F-A06E-E87C9E061AF4}"/>
     <hyperlink ref="C236" r:id="rId329" xr:uid="{CB383B55-0E52-B947-A592-980271C8692F}"/>
     <hyperlink ref="C235" r:id="rId330" xr:uid="{4F9CF5F4-FC6C-9541-8599-DC150894B479}"/>
-    <hyperlink ref="C355" r:id="rId331" xr:uid="{CA40C680-0DBD-4343-8DE5-E090CB8817CA}"/>
+    <hyperlink ref="C356" r:id="rId331" xr:uid="{CA40C680-0DBD-4343-8DE5-E090CB8817CA}"/>
     <hyperlink ref="C246" r:id="rId332" xr:uid="{D586CA6E-E909-E844-A264-3987E2724DC4}"/>
     <hyperlink ref="C146" r:id="rId333" xr:uid="{C8735485-A0EF-E24F-8279-22CB0E8428F6}"/>
     <hyperlink ref="C144" r:id="rId334" xr:uid="{5AC9EBB0-8920-8744-A148-D68938ACC8E8}"/>
@@ -13378,8 +13473,8 @@
     <hyperlink ref="C147" r:id="rId340" xr:uid="{3FB21270-2F59-4B49-AC05-62DEE66C37B9}"/>
     <hyperlink ref="C149" r:id="rId341" xr:uid="{0D933DDA-AB72-1640-BEBC-718751BE3F53}"/>
     <hyperlink ref="C85" r:id="rId342" xr:uid="{07BF52D4-5452-B34A-A03C-22767C637C7A}"/>
-    <hyperlink ref="C333" r:id="rId343" display="AWS Encryption SDK" xr:uid="{33F5E068-1939-6946-A05C-520BF7F5E73D}"/>
-    <hyperlink ref="C351" r:id="rId344" xr:uid="{17414EBC-16B7-5042-9A20-53B1F60B49D6}"/>
+    <hyperlink ref="C334" r:id="rId343" display="AWS Encryption SDK" xr:uid="{33F5E068-1939-6946-A05C-520BF7F5E73D}"/>
+    <hyperlink ref="C352" r:id="rId344" xr:uid="{17414EBC-16B7-5042-9A20-53B1F60B49D6}"/>
     <hyperlink ref="C87" r:id="rId345" xr:uid="{49BDB63D-5793-7B41-8772-615181B6C834}"/>
     <hyperlink ref="C231" r:id="rId346" xr:uid="{4D966601-2D59-F04E-9495-8AA46ED9EE78}"/>
     <hyperlink ref="C252" r:id="rId347" xr:uid="{C10A4ED2-003D-7E4D-BE98-CECF30AF4344}"/>
@@ -13388,26 +13483,27 @@
     <hyperlink ref="C83" r:id="rId350" xr:uid="{D3C65AFD-BAD4-AA4E-BE9E-F8F69A6E7034}"/>
     <hyperlink ref="C140" r:id="rId351" xr:uid="{C34DE960-4123-5B4C-8754-CF42F1139B71}"/>
     <hyperlink ref="C119" r:id="rId352" xr:uid="{4D37DCA5-E332-7D43-ADF7-343653A50F60}"/>
-    <hyperlink ref="C343" r:id="rId353" xr:uid="{D96F285C-B638-7E41-B6F5-6FC9047BE3EF}"/>
-    <hyperlink ref="C358" r:id="rId354" xr:uid="{23EAC66D-29B2-0B4A-B439-4EE056114072}"/>
-    <hyperlink ref="C365" r:id="rId355" display="S3 Glacier" xr:uid="{85EA50A7-14B2-D149-A253-41B939F41318}"/>
-    <hyperlink ref="C299" r:id="rId356" xr:uid="{5924D0B4-C3ED-7141-9DB4-F738AAAED8FD}"/>
+    <hyperlink ref="C344" r:id="rId353" xr:uid="{D96F285C-B638-7E41-B6F5-6FC9047BE3EF}"/>
+    <hyperlink ref="C359" r:id="rId354" xr:uid="{23EAC66D-29B2-0B4A-B439-4EE056114072}"/>
+    <hyperlink ref="C366" r:id="rId355" display="S3 Glacier" xr:uid="{85EA50A7-14B2-D149-A253-41B939F41318}"/>
+    <hyperlink ref="C300" r:id="rId356" xr:uid="{5924D0B4-C3ED-7141-9DB4-F738AAAED8FD}"/>
     <hyperlink ref="C128" r:id="rId357" xr:uid="{0E05A36D-6E61-794C-94C0-8D1445341816}"/>
     <hyperlink ref="C79" r:id="rId358" xr:uid="{7477CB6A-F100-A34F-9008-B1BFB9967DA7}"/>
-    <hyperlink ref="C314" r:id="rId359" xr:uid="{6AD92B4E-E0EB-1848-9442-69AFE2F3AE78}"/>
-    <hyperlink ref="C15" r:id="rId360" xr:uid="{DF438ACC-C4F5-974D-96FC-A4F4FBD4D563}"/>
+    <hyperlink ref="C315" r:id="rId359" xr:uid="{6AD92B4E-E0EB-1848-9442-69AFE2F3AE78}"/>
+    <hyperlink ref="C14" r:id="rId360" xr:uid="{DF438ACC-C4F5-974D-96FC-A4F4FBD4D563}"/>
     <hyperlink ref="C27" r:id="rId361" xr:uid="{567A6139-66F6-6E46-9546-8DDB94DE141F}"/>
     <hyperlink ref="C50" r:id="rId362" xr:uid="{07941932-04CA-D14D-B516-833FCD650A67}"/>
     <hyperlink ref="C63" r:id="rId363" xr:uid="{438F4E0F-2656-3B4B-A75B-4361FF393940}"/>
     <hyperlink ref="C5" r:id="rId364" xr:uid="{3E5A0494-CA0B-014F-A243-AE4E024917C7}"/>
-    <hyperlink ref="C346" r:id="rId365" xr:uid="{EF3501C3-6722-B042-98D5-211CBE91441E}"/>
+    <hyperlink ref="C347" r:id="rId365" xr:uid="{EF3501C3-6722-B042-98D5-211CBE91441E}"/>
     <hyperlink ref="C3" r:id="rId366" xr:uid="{E80DDE27-8B15-7D4E-B079-859E8B3D4840}"/>
     <hyperlink ref="C7" r:id="rId367" xr:uid="{2BD4EAC1-9B52-F549-A5EF-09125D392FAD}"/>
     <hyperlink ref="C8" r:id="rId368" xr:uid="{D7671988-78D2-5D42-A661-9F1327506CFF}"/>
     <hyperlink ref="C9" r:id="rId369" xr:uid="{9B9AC072-01A0-A844-847C-B109A617D904}"/>
-    <hyperlink ref="C349" r:id="rId370" xr:uid="{B12E0A4B-2756-BC42-8B8D-F13EBD0781FC}"/>
-    <hyperlink ref="C348" r:id="rId371" xr:uid="{A42E2080-0217-3F47-AE51-390098505C99}"/>
-    <hyperlink ref="C341" r:id="rId372" xr:uid="{C755366D-FC78-4743-98C2-D8F2CF3EC22B}"/>
+    <hyperlink ref="C350" r:id="rId370" xr:uid="{B12E0A4B-2756-BC42-8B8D-F13EBD0781FC}"/>
+    <hyperlink ref="C349" r:id="rId371" xr:uid="{A42E2080-0217-3F47-AE51-390098505C99}"/>
+    <hyperlink ref="C342" r:id="rId372" xr:uid="{C755366D-FC78-4743-98C2-D8F2CF3EC22B}"/>
+    <hyperlink ref="C288" r:id="rId373" display="DMS Schema Convertion (DMS SC)" xr:uid="{48AE58DC-9BE4-F74C-8FEA-9594B5F4424F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13436,28 +13532,28 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="60" t="s">
-        <v>342</v>
-      </c>
-      <c r="B4" s="60"/>
+      <c r="A4" s="59" t="s">
+        <v>341</v>
+      </c>
+      <c r="B4" s="59"/>
     </row>
     <row r="5" spans="1:2" s="55" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="61" t="s">
-        <v>341</v>
-      </c>
-      <c r="B5" s="61"/>
+      <c r="A5" s="60" t="s">
+        <v>340</v>
+      </c>
+      <c r="B5" s="60"/>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="62" t="s">
-        <v>340</v>
-      </c>
-      <c r="B6" s="62"/>
+      <c r="A6" s="61" t="s">
+        <v>339</v>
+      </c>
+      <c r="B6" s="61"/>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="62" t="s">
-        <v>339</v>
-      </c>
-      <c r="B7" s="62"/>
+      <c r="A7" s="61" t="s">
+        <v>338</v>
+      </c>
+      <c r="B7" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Omics renamed and deprecations
</commit_message>
<xml_diff>
--- a/aws-services-crib-sheet.xlsx
+++ b/aws-services-crib-sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corbuno/courses/aws-services-crib-sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126AE263-BDC1-AA44-8C4D-D322E4A9E65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF5BA22-B050-8C46-BA12-49636842221D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27880" windowHeight="17500" xr2:uid="{8DC9DE24-CECC-4748-B90E-52259685D84E}"/>
+    <workbookView xWindow="39760" yWindow="-12800" windowWidth="21900" windowHeight="17320" xr2:uid="{8DC9DE24-CECC-4748-B90E-52259685D84E}"/>
   </bookViews>
   <sheets>
     <sheet name="AWS Services" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="474">
   <si>
     <t>Elastic Load Balancing</t>
   </si>
@@ -1180,9 +1180,6 @@
     <t>Glue Data Quality</t>
   </si>
   <si>
-    <t>Omics</t>
-  </si>
-  <si>
     <t>Supply Chain</t>
   </si>
   <si>
@@ -1451,19 +1448,28 @@
   </si>
   <si>
     <t>Q in AWS Supply Chain</t>
+  </si>
+  <si>
+    <t>HealthOmics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -1757,242 +1763,263 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2327,10 +2354,10 @@
   <dimension ref="A1:S421"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2365,10 +2392,10 @@
         <v>259</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>452</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>453</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>221</v>
@@ -2377,7 +2404,7 @@
         <v>153</v>
       </c>
       <c r="H1" s="63" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I1" s="66" t="s">
         <v>359</v>
@@ -2386,13 +2413,13 @@
         <v>358</v>
       </c>
       <c r="K1" s="66" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="L1" s="66" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="M1" s="66" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="N1" s="64" t="s">
         <v>357</v>
@@ -2401,16 +2428,16 @@
         <v>360</v>
       </c>
       <c r="P1" s="65" t="s">
+        <v>456</v>
+      </c>
+      <c r="Q1" s="65" t="s">
         <v>457</v>
       </c>
-      <c r="Q1" s="65" t="s">
+      <c r="R1" s="65" t="s">
         <v>458</v>
       </c>
-      <c r="R1" s="65" t="s">
-        <v>459</v>
-      </c>
       <c r="S1" s="48" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -2436,6 +2463,7 @@
       <c r="J2" s="62">
         <v>1</v>
       </c>
+      <c r="K2" s="85"/>
       <c r="L2" s="62">
         <v>1</v>
       </c>
@@ -2462,7 +2490,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D3" s="59"/>
       <c r="E3" s="59"/>
@@ -2471,6 +2499,7 @@
       <c r="H3" s="62"/>
       <c r="I3" s="62"/>
       <c r="J3" s="62"/>
+      <c r="K3" s="85"/>
       <c r="L3" s="62"/>
       <c r="N3" s="62"/>
       <c r="O3" s="62"/>
@@ -2495,7 +2524,7 @@
       <c r="H4" s="60"/>
       <c r="I4" s="60"/>
       <c r="J4" s="60"/>
-      <c r="K4" s="61"/>
+      <c r="K4" s="86"/>
       <c r="L4" s="60"/>
       <c r="M4" s="61"/>
       <c r="N4" s="60"/>
@@ -2504,7 +2533,7 @@
       <c r="Q4" s="60"/>
       <c r="R4" s="60"/>
       <c r="S4" s="73" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -2530,6 +2559,7 @@
         <v>1</v>
       </c>
       <c r="J5" s="62"/>
+      <c r="K5" s="85"/>
       <c r="L5" s="62"/>
       <c r="N5" s="62">
         <v>1</v>
@@ -2547,7 +2577,7 @@
         <v>48</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D6" s="59"/>
       <c r="E6" s="59"/>
@@ -2562,6 +2592,7 @@
       <c r="J6" s="62">
         <v>1</v>
       </c>
+      <c r="K6" s="85"/>
       <c r="L6" s="62">
         <v>1</v>
       </c>
@@ -2599,7 +2630,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="60"/>
-      <c r="K7" s="61"/>
+      <c r="K7" s="86"/>
       <c r="L7" s="60"/>
       <c r="M7" s="61"/>
       <c r="N7" s="60"/>
@@ -2608,7 +2639,7 @@
       <c r="Q7" s="60"/>
       <c r="R7" s="60"/>
       <c r="S7" s="73" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
@@ -2619,7 +2650,7 @@
         <v>48</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D8" s="59"/>
       <c r="E8" s="59"/>
@@ -2628,6 +2659,7 @@
       <c r="H8" s="62"/>
       <c r="I8" s="62"/>
       <c r="J8" s="62"/>
+      <c r="K8" s="85"/>
       <c r="L8" s="62"/>
       <c r="N8" s="62"/>
       <c r="O8" s="62"/>
@@ -2658,6 +2690,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="62"/>
+      <c r="K9" s="85"/>
       <c r="L9" s="62">
         <v>1</v>
       </c>
@@ -2684,7 +2717,7 @@
         <v>48</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D10" s="59"/>
       <c r="E10" s="59"/>
@@ -2693,6 +2726,7 @@
       <c r="H10" s="62"/>
       <c r="I10" s="62"/>
       <c r="J10" s="62"/>
+      <c r="K10" s="85"/>
       <c r="L10" s="62"/>
       <c r="N10" s="62">
         <v>1</v>
@@ -2714,7 +2748,7 @@
         <v>48</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D11" s="59"/>
       <c r="E11" s="59"/>
@@ -2723,6 +2757,7 @@
       <c r="H11" s="62"/>
       <c r="I11" s="62"/>
       <c r="J11" s="62"/>
+      <c r="K11" s="85"/>
       <c r="L11" s="62"/>
       <c r="N11" s="62"/>
       <c r="O11" s="62"/>
@@ -2738,7 +2773,7 @@
         <v>48</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D12" s="59"/>
       <c r="E12" s="59"/>
@@ -2747,6 +2782,7 @@
       <c r="H12" s="62"/>
       <c r="I12" s="62"/>
       <c r="J12" s="62"/>
+      <c r="K12" s="85"/>
       <c r="L12" s="62"/>
       <c r="N12" s="62"/>
       <c r="O12" s="62"/>
@@ -2771,6 +2807,7 @@
       <c r="H13" s="62"/>
       <c r="I13" s="62"/>
       <c r="J13" s="62"/>
+      <c r="K13" s="85"/>
       <c r="L13" s="62"/>
       <c r="N13" s="62"/>
       <c r="O13" s="62"/>
@@ -2795,6 +2832,7 @@
       <c r="H14" s="62"/>
       <c r="I14" s="62"/>
       <c r="J14" s="62"/>
+      <c r="K14" s="85"/>
       <c r="L14" s="62"/>
       <c r="N14" s="62"/>
       <c r="O14" s="62"/>
@@ -2825,6 +2863,7 @@
         <v>1</v>
       </c>
       <c r="J15" s="62"/>
+      <c r="K15" s="85"/>
       <c r="L15" s="62">
         <v>1</v>
       </c>
@@ -2858,6 +2897,7 @@
       <c r="H16" s="62"/>
       <c r="I16" s="62"/>
       <c r="J16" s="62"/>
+      <c r="K16" s="85"/>
       <c r="L16" s="62"/>
       <c r="N16" s="62"/>
       <c r="O16" s="62"/>
@@ -2913,6 +2953,7 @@
       <c r="I18" s="62"/>
       <c r="J18" s="62"/>
       <c r="K18" s="62"/>
+      <c r="L18" s="85"/>
       <c r="M18" s="68">
         <v>1</v>
       </c>
@@ -3055,104 +3096,91 @@
         <v>48</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>429</v>
+        <v>473</v>
       </c>
       <c r="D24" s="59"/>
       <c r="E24" s="59"/>
       <c r="F24" s="59"/>
-      <c r="G24" s="62">
-        <v>1</v>
-      </c>
+      <c r="G24" s="62"/>
       <c r="H24" s="62"/>
-      <c r="I24" s="62">
-        <v>1</v>
-      </c>
-      <c r="J24" s="62">
-        <v>1</v>
-      </c>
+      <c r="I24" s="62"/>
+      <c r="J24" s="62"/>
       <c r="K24" s="62"/>
-      <c r="L24" s="62">
-        <v>1</v>
-      </c>
-      <c r="M24" s="68">
-        <v>1</v>
-      </c>
-      <c r="N24" s="62">
-        <v>1</v>
-      </c>
-      <c r="O24" s="62">
-        <v>1</v>
-      </c>
+      <c r="L24" s="62"/>
+      <c r="N24" s="62"/>
+      <c r="O24" s="62"/>
       <c r="P24" s="62"/>
       <c r="Q24" s="62"/>
-      <c r="R24" s="62">
-        <v>1</v>
-      </c>
+      <c r="R24" s="62"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
         <v>32</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>104</v>
+        <v>428</v>
       </c>
       <c r="D25" s="59"/>
       <c r="E25" s="59"/>
       <c r="F25" s="59"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62">
-        <v>1</v>
-      </c>
+      <c r="G25" s="62">
+        <v>1</v>
+      </c>
+      <c r="H25" s="62"/>
       <c r="I25" s="62">
         <v>1</v>
       </c>
-      <c r="J25" s="62"/>
+      <c r="J25" s="62">
+        <v>1</v>
+      </c>
       <c r="K25" s="62"/>
       <c r="L25" s="62">
         <v>1</v>
       </c>
-      <c r="M25" s="68">
+      <c r="M25" s="85">
         <v>1</v>
       </c>
       <c r="N25" s="62">
         <v>1</v>
       </c>
-      <c r="O25" s="62"/>
+      <c r="O25" s="62">
+        <v>1</v>
+      </c>
       <c r="P25" s="62"/>
       <c r="Q25" s="62"/>
-      <c r="R25" s="62"/>
+      <c r="R25" s="62">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>450</v>
+        <v>104</v>
       </c>
       <c r="D26" s="59"/>
       <c r="E26" s="59"/>
       <c r="F26" s="59"/>
-      <c r="G26" s="62">
-        <v>1</v>
-      </c>
-      <c r="H26" s="62"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="62">
+        <v>1</v>
+      </c>
       <c r="I26" s="62">
         <v>1</v>
       </c>
-      <c r="J26" s="62">
-        <v>1</v>
-      </c>
+      <c r="J26" s="62"/>
       <c r="K26" s="62"/>
       <c r="L26" s="62">
         <v>1</v>
       </c>
-      <c r="M26" s="68">
+      <c r="M26" s="85">
         <v>1</v>
       </c>
       <c r="N26" s="62">
@@ -3161,9 +3189,7 @@
       <c r="O26" s="62"/>
       <c r="P26" s="62"/>
       <c r="Q26" s="62"/>
-      <c r="R26" s="62">
-        <v>1</v>
-      </c>
+      <c r="R26" s="62"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
@@ -3173,7 +3199,7 @@
         <v>48</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>258</v>
+        <v>449</v>
       </c>
       <c r="D27" s="59"/>
       <c r="E27" s="59"/>
@@ -3185,9 +3211,14 @@
       <c r="I27" s="62">
         <v>1</v>
       </c>
-      <c r="J27" s="62"/>
+      <c r="J27" s="62">
+        <v>1</v>
+      </c>
       <c r="K27" s="62"/>
       <c r="L27" s="62">
+        <v>1</v>
+      </c>
+      <c r="M27" s="85">
         <v>1</v>
       </c>
       <c r="N27" s="62">
@@ -3196,7 +3227,9 @@
       <c r="O27" s="62"/>
       <c r="P27" s="62"/>
       <c r="Q27" s="62"/>
-      <c r="R27" s="62"/>
+      <c r="R27" s="62">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
@@ -3206,18 +3239,27 @@
         <v>48</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>383</v>
+        <v>258</v>
       </c>
       <c r="D28" s="59"/>
       <c r="E28" s="59"/>
       <c r="F28" s="59"/>
-      <c r="G28" s="62"/>
+      <c r="G28" s="62">
+        <v>1</v>
+      </c>
       <c r="H28" s="62"/>
-      <c r="I28" s="62"/>
+      <c r="I28" s="62">
+        <v>1</v>
+      </c>
       <c r="J28" s="62"/>
       <c r="K28" s="62"/>
-      <c r="L28" s="62"/>
-      <c r="N28" s="62"/>
+      <c r="L28" s="62">
+        <v>1</v>
+      </c>
+      <c r="M28" s="85"/>
+      <c r="N28" s="62">
+        <v>1</v>
+      </c>
       <c r="O28" s="62"/>
       <c r="P28" s="62"/>
       <c r="Q28" s="62"/>
@@ -3561,7 +3603,7 @@
         <v>48</v>
       </c>
       <c r="C39" s="25" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D39" s="59"/>
       <c r="E39" s="59"/>
@@ -3603,7 +3645,7 @@
         <v>48</v>
       </c>
       <c r="C40" s="25" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D40" s="59"/>
       <c r="E40" s="59"/>
@@ -3628,7 +3670,7 @@
         <v>48</v>
       </c>
       <c r="C41" s="25" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D41" s="59"/>
       <c r="E41" s="59"/>
@@ -3653,7 +3695,7 @@
         <v>48</v>
       </c>
       <c r="C42" s="25" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D42" s="59"/>
       <c r="E42" s="59"/>
@@ -3691,7 +3733,7 @@
       <c r="L43" s="62">
         <v>1</v>
       </c>
-      <c r="M43" s="68">
+      <c r="M43" s="85">
         <v>1</v>
       </c>
       <c r="N43" s="62"/>
@@ -3721,6 +3763,7 @@
       <c r="J44" s="62"/>
       <c r="K44" s="62"/>
       <c r="L44" s="62"/>
+      <c r="M44" s="85"/>
       <c r="N44" s="62">
         <v>1</v>
       </c>
@@ -3882,7 +3925,7 @@
       <c r="Q48" s="62"/>
       <c r="R48" s="62"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A49" s="23" t="s">
         <v>165</v>
       </c>
@@ -3890,7 +3933,7 @@
         <v>3</v>
       </c>
       <c r="C49" s="25" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D49" s="59"/>
       <c r="E49" s="59"/>
@@ -3907,7 +3950,7 @@
       <c r="Q49" s="62"/>
       <c r="R49" s="62"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A50" s="26" t="s">
         <v>168</v>
       </c>
@@ -3928,6 +3971,7 @@
       <c r="J50" s="62"/>
       <c r="K50" s="62"/>
       <c r="L50" s="62"/>
+      <c r="M50" s="85"/>
       <c r="N50" s="62">
         <v>1</v>
       </c>
@@ -3936,7 +3980,7 @@
       <c r="Q50" s="62"/>
       <c r="R50" s="62"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A51" s="30" t="s">
         <v>188</v>
       </c>
@@ -3961,7 +4005,7 @@
       <c r="Q51" s="62"/>
       <c r="R51" s="62"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A52" s="30" t="s">
         <v>188</v>
       </c>
@@ -3969,7 +4013,7 @@
         <v>3</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D52" s="59"/>
       <c r="E52" s="59"/>
@@ -3986,7 +4030,7 @@
       <c r="Q52" s="62"/>
       <c r="R52" s="62"/>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A53" s="30" t="s">
         <v>188</v>
       </c>
@@ -4014,7 +4058,7 @@
       <c r="Q53" s="62"/>
       <c r="R53" s="62"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A54" s="30" t="s">
         <v>188</v>
       </c>
@@ -4039,32 +4083,36 @@
       <c r="Q54" s="62"/>
       <c r="R54" s="62"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A55" s="30" t="s">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A55" s="89" t="s">
         <v>188</v>
       </c>
-      <c r="B55" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="C55" s="32" t="s">
+      <c r="B55" s="90" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" s="91" t="s">
         <v>191</v>
       </c>
-      <c r="D55" s="59"/>
-      <c r="E55" s="59"/>
-      <c r="F55" s="59"/>
-      <c r="G55" s="62"/>
-      <c r="H55" s="62"/>
-      <c r="I55" s="62"/>
-      <c r="J55" s="62"/>
-      <c r="K55" s="62"/>
-      <c r="L55" s="62"/>
-      <c r="N55" s="62"/>
-      <c r="O55" s="62"/>
-      <c r="P55" s="62"/>
-      <c r="Q55" s="62"/>
-      <c r="R55" s="62"/>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="D55" s="44"/>
+      <c r="E55" s="44"/>
+      <c r="F55" s="44"/>
+      <c r="G55" s="60"/>
+      <c r="H55" s="60"/>
+      <c r="I55" s="60"/>
+      <c r="J55" s="60"/>
+      <c r="K55" s="60"/>
+      <c r="L55" s="60"/>
+      <c r="M55" s="61"/>
+      <c r="N55" s="60"/>
+      <c r="O55" s="60"/>
+      <c r="P55" s="60"/>
+      <c r="Q55" s="60"/>
+      <c r="R55" s="60"/>
+      <c r="S55" s="88" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A56" s="30" t="s">
         <v>188</v>
       </c>
@@ -4072,7 +4120,7 @@
         <v>48</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D56" s="59"/>
       <c r="E56" s="59"/>
@@ -4089,7 +4137,7 @@
       <c r="Q56" s="62"/>
       <c r="R56" s="62"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A57" s="30" t="s">
         <v>188</v>
       </c>
@@ -4097,7 +4145,7 @@
         <v>48</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D57" s="59"/>
       <c r="E57" s="59"/>
@@ -4114,7 +4162,7 @@
       <c r="Q57" s="62"/>
       <c r="R57" s="62"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A58" s="30" t="s">
         <v>188</v>
       </c>
@@ -4139,7 +4187,7 @@
       <c r="Q58" s="62"/>
       <c r="R58" s="62"/>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A59" s="30" t="s">
         <v>188</v>
       </c>
@@ -4164,7 +4212,7 @@
       <c r="Q59" s="62"/>
       <c r="R59" s="62"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A60" s="30" t="s">
         <v>188</v>
       </c>
@@ -4189,7 +4237,7 @@
       <c r="Q60" s="62"/>
       <c r="R60" s="62"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A61" s="26" t="s">
         <v>21</v>
       </c>
@@ -4227,7 +4275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A62" s="26" t="s">
         <v>21</v>
       </c>
@@ -4264,7 +4312,7 @@
       <c r="Q62" s="62"/>
       <c r="R62" s="62"/>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A63" s="26" t="s">
         <v>21</v>
       </c>
@@ -4291,7 +4339,7 @@
       <c r="Q63" s="62"/>
       <c r="R63" s="62"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A64" s="26" t="s">
         <v>21</v>
       </c>
@@ -4380,7 +4428,7 @@
       </c>
       <c r="B66" s="27"/>
       <c r="C66" s="28" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D66" s="59"/>
       <c r="E66" s="59"/>
@@ -4426,7 +4474,7 @@
       <c r="L67" s="62">
         <v>1</v>
       </c>
-      <c r="M67" s="68">
+      <c r="M67" s="85">
         <v>1</v>
       </c>
       <c r="N67" s="62">
@@ -4464,6 +4512,7 @@
       <c r="J68" s="62"/>
       <c r="K68" s="62"/>
       <c r="L68" s="62"/>
+      <c r="M68" s="85"/>
       <c r="N68" s="62">
         <v>1</v>
       </c>
@@ -4480,7 +4529,7 @@
         <v>48</v>
       </c>
       <c r="C69" s="28" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D69" s="59"/>
       <c r="E69" s="59"/>
@@ -4491,6 +4540,7 @@
       <c r="J69" s="62"/>
       <c r="K69" s="62"/>
       <c r="L69" s="62"/>
+      <c r="M69" s="85"/>
       <c r="N69" s="62"/>
       <c r="O69" s="62"/>
       <c r="P69" s="62"/>
@@ -4505,7 +4555,7 @@
         <v>3</v>
       </c>
       <c r="C70" s="28" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D70" s="59"/>
       <c r="E70" s="59"/>
@@ -4561,7 +4611,7 @@
         <v>3</v>
       </c>
       <c r="C72" s="28" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D72" s="59"/>
       <c r="E72" s="59"/>
@@ -4584,7 +4634,7 @@
       </c>
       <c r="B73" s="27"/>
       <c r="C73" s="28" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D73" s="59"/>
       <c r="E73" s="59"/>
@@ -4639,7 +4689,7 @@
         <v>3</v>
       </c>
       <c r="C75" s="28" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D75" s="59"/>
       <c r="E75" s="59"/>
@@ -4684,7 +4734,7 @@
       <c r="Q76" s="60"/>
       <c r="R76" s="60"/>
       <c r="S76" s="68" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="77" spans="1:19" x14ac:dyDescent="0.2">
@@ -4737,6 +4787,7 @@
       <c r="J78" s="62"/>
       <c r="K78" s="62"/>
       <c r="L78" s="62"/>
+      <c r="N78" s="85"/>
       <c r="O78" s="62">
         <v>1</v>
       </c>
@@ -4852,7 +4903,7 @@
         <v>48</v>
       </c>
       <c r="C83" s="28" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D83" s="59"/>
       <c r="E83" s="59"/>
@@ -4881,7 +4932,7 @@
         <v>48</v>
       </c>
       <c r="C84" s="28" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D84" s="59"/>
       <c r="E84" s="59"/>
@@ -4910,7 +4961,7 @@
         <v>48</v>
       </c>
       <c r="C85" s="28" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D85" s="59"/>
       <c r="E85" s="59"/>
@@ -4935,7 +4986,7 @@
         <v>48</v>
       </c>
       <c r="C86" s="28" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D86" s="59"/>
       <c r="E86" s="59"/>
@@ -5127,7 +5178,7 @@
       </c>
       <c r="B91" s="27"/>
       <c r="C91" s="28" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D91" s="59"/>
       <c r="E91" s="59"/>
@@ -5161,6 +5212,7 @@
       <c r="J92" s="62"/>
       <c r="K92" s="62"/>
       <c r="L92" s="62"/>
+      <c r="M92" s="85"/>
       <c r="N92" s="62"/>
       <c r="O92" s="62"/>
       <c r="P92" s="62"/>
@@ -5188,6 +5240,7 @@
       <c r="J93" s="62"/>
       <c r="K93" s="62"/>
       <c r="L93" s="62"/>
+      <c r="M93" s="85"/>
       <c r="N93" s="62">
         <v>1</v>
       </c>
@@ -5441,7 +5494,7 @@
         <v>3</v>
       </c>
       <c r="C102" s="21" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D102" s="59"/>
       <c r="E102" s="59"/>
@@ -5610,6 +5663,7 @@
       <c r="J108" s="62"/>
       <c r="K108" s="62"/>
       <c r="L108" s="62"/>
+      <c r="M108" s="85"/>
       <c r="N108" s="62"/>
       <c r="O108" s="62"/>
       <c r="P108" s="62"/>
@@ -5624,7 +5678,7 @@
         <v>3</v>
       </c>
       <c r="C109" s="12" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D109" s="59"/>
       <c r="E109" s="59"/>
@@ -5637,6 +5691,7 @@
       <c r="J109" s="62"/>
       <c r="K109" s="62"/>
       <c r="L109" s="62"/>
+      <c r="M109" s="85"/>
       <c r="N109" s="62"/>
       <c r="O109" s="62"/>
       <c r="P109" s="62"/>
@@ -5664,6 +5719,7 @@
       <c r="J110" s="62"/>
       <c r="K110" s="62"/>
       <c r="L110" s="62"/>
+      <c r="M110" s="85"/>
       <c r="N110" s="62"/>
       <c r="O110" s="62"/>
       <c r="P110" s="62"/>
@@ -5678,7 +5734,7 @@
         <v>48</v>
       </c>
       <c r="C111" s="12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D111" s="59"/>
       <c r="E111" s="59"/>
@@ -5689,7 +5745,7 @@
       <c r="J111" s="62"/>
       <c r="K111" s="62"/>
       <c r="L111" s="62"/>
-      <c r="M111" s="68">
+      <c r="M111" s="85">
         <v>1</v>
       </c>
       <c r="N111" s="62"/>
@@ -6089,6 +6145,7 @@
       <c r="L124" s="62">
         <v>1</v>
       </c>
+      <c r="M124" s="85"/>
       <c r="N124" s="62">
         <v>1</v>
       </c>
@@ -6105,7 +6162,7 @@
         <v>48</v>
       </c>
       <c r="C125" s="12" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D125" s="59"/>
       <c r="E125" s="59"/>
@@ -6124,6 +6181,7 @@
       <c r="L125" s="62">
         <v>1</v>
       </c>
+      <c r="M125" s="85"/>
       <c r="N125" s="62"/>
       <c r="O125" s="62"/>
       <c r="P125" s="62"/>
@@ -6157,7 +6215,7 @@
       <c r="L126" s="62">
         <v>1</v>
       </c>
-      <c r="M126" s="68">
+      <c r="M126" s="85">
         <v>1</v>
       </c>
       <c r="N126" s="62">
@@ -6176,7 +6234,7 @@
         <v>48</v>
       </c>
       <c r="C127" s="12" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D127" s="59"/>
       <c r="E127" s="59"/>
@@ -6187,6 +6245,7 @@
       <c r="J127" s="62"/>
       <c r="K127" s="62"/>
       <c r="L127" s="62"/>
+      <c r="M127" s="85"/>
       <c r="N127" s="62"/>
       <c r="O127" s="62"/>
       <c r="P127" s="62"/>
@@ -6201,7 +6260,7 @@
         <v>48</v>
       </c>
       <c r="C128" s="12" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D128" s="59"/>
       <c r="E128" s="59"/>
@@ -6246,7 +6305,7 @@
       <c r="Q129" s="60"/>
       <c r="R129" s="60"/>
       <c r="S129" s="73" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="130" spans="1:19" x14ac:dyDescent="0.2">
@@ -6282,7 +6341,7 @@
         <v>48</v>
       </c>
       <c r="C131" s="12" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D131" s="59"/>
       <c r="E131" s="59"/>
@@ -6382,7 +6441,7 @@
         <v>3</v>
       </c>
       <c r="C134" s="12" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D134" s="59"/>
       <c r="E134" s="59"/>
@@ -6407,7 +6466,7 @@
         <v>3</v>
       </c>
       <c r="C135" s="12" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D135" s="59"/>
       <c r="E135" s="59"/>
@@ -6567,7 +6626,7 @@
       <c r="Q140" s="60"/>
       <c r="R140" s="60"/>
       <c r="S140" s="73" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.2">
@@ -6734,7 +6793,7 @@
       <c r="Q145" s="60"/>
       <c r="R145" s="60"/>
       <c r="S145" s="73" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="146" spans="1:19" x14ac:dyDescent="0.2">
@@ -7022,7 +7081,7 @@
         <v>3</v>
       </c>
       <c r="C155" s="12" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D155" s="59"/>
       <c r="E155" s="59"/>
@@ -7058,6 +7117,7 @@
       <c r="J156" s="62"/>
       <c r="K156" s="62"/>
       <c r="L156" s="62"/>
+      <c r="M156" s="85"/>
       <c r="N156" s="62"/>
       <c r="O156" s="62"/>
       <c r="P156" s="62"/>
@@ -7239,7 +7299,7 @@
         <v>48</v>
       </c>
       <c r="C163" s="15" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D163" s="59"/>
       <c r="E163" s="59"/>
@@ -7293,7 +7353,7 @@
         <v>3</v>
       </c>
       <c r="C165" s="15" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D165" s="59"/>
       <c r="E165" s="59"/>
@@ -7366,7 +7426,7 @@
     </row>
     <row r="168" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A168" s="30" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B168" s="31" t="s">
         <v>3</v>
@@ -7399,7 +7459,7 @@
     </row>
     <row r="169" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A169" s="30" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B169" s="31" t="s">
         <v>3</v>
@@ -7430,7 +7490,7 @@
     </row>
     <row r="170" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A170" s="30" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B170" s="31" t="s">
         <v>48</v>
@@ -7447,6 +7507,7 @@
       <c r="J170" s="62"/>
       <c r="K170" s="62"/>
       <c r="L170" s="62"/>
+      <c r="M170" s="85"/>
       <c r="N170" s="62"/>
       <c r="O170" s="62"/>
       <c r="P170" s="62"/>
@@ -7547,6 +7608,7 @@
       <c r="J174" s="62"/>
       <c r="K174" s="62"/>
       <c r="L174" s="62"/>
+      <c r="M174" s="85"/>
       <c r="N174" s="62"/>
       <c r="O174" s="62"/>
       <c r="P174" s="62"/>
@@ -7602,7 +7664,7 @@
       <c r="Q176" s="60"/>
       <c r="R176" s="60"/>
       <c r="S176" s="68" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="177" spans="1:19" x14ac:dyDescent="0.2">
@@ -7647,7 +7709,7 @@
       <c r="J178" s="60"/>
       <c r="K178" s="60"/>
       <c r="L178" s="60"/>
-      <c r="M178" s="61"/>
+      <c r="M178" s="86"/>
       <c r="N178" s="60">
         <v>1</v>
       </c>
@@ -7656,7 +7718,7 @@
       <c r="Q178" s="60"/>
       <c r="R178" s="60"/>
       <c r="S178" s="68" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="179" spans="1:19" x14ac:dyDescent="0.2">
@@ -7678,7 +7740,7 @@
       <c r="J179" s="60"/>
       <c r="K179" s="60"/>
       <c r="L179" s="60"/>
-      <c r="M179" s="61"/>
+      <c r="M179" s="86"/>
       <c r="N179" s="60">
         <v>1</v>
       </c>
@@ -7687,7 +7749,7 @@
       <c r="Q179" s="60"/>
       <c r="R179" s="60"/>
       <c r="S179" s="73" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="180" spans="1:19" x14ac:dyDescent="0.2">
@@ -7711,6 +7773,7 @@
       <c r="J180" s="62"/>
       <c r="K180" s="62"/>
       <c r="L180" s="62"/>
+      <c r="M180" s="85"/>
       <c r="N180" s="62">
         <v>1</v>
       </c>
@@ -7738,6 +7801,7 @@
       <c r="J181" s="62"/>
       <c r="K181" s="62"/>
       <c r="L181" s="62"/>
+      <c r="M181" s="85"/>
       <c r="N181" s="62">
         <v>1</v>
       </c>
@@ -7765,6 +7829,7 @@
       <c r="J182" s="62"/>
       <c r="K182" s="62"/>
       <c r="L182" s="62"/>
+      <c r="M182" s="85"/>
       <c r="N182" s="62">
         <v>1</v>
       </c>
@@ -7792,6 +7857,7 @@
       <c r="J183" s="62"/>
       <c r="K183" s="62"/>
       <c r="L183" s="62"/>
+      <c r="M183" s="85"/>
       <c r="N183" s="62"/>
       <c r="O183" s="62"/>
       <c r="P183" s="62"/>
@@ -7806,7 +7872,7 @@
         <v>3</v>
       </c>
       <c r="C184" s="21" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D184" s="59"/>
       <c r="E184" s="59"/>
@@ -7817,6 +7883,7 @@
       <c r="J184" s="62"/>
       <c r="K184" s="62"/>
       <c r="L184" s="62"/>
+      <c r="M184" s="85"/>
       <c r="N184" s="62"/>
       <c r="O184" s="62"/>
       <c r="P184" s="62"/>
@@ -7842,6 +7909,7 @@
       <c r="J185" s="62"/>
       <c r="K185" s="62"/>
       <c r="L185" s="62"/>
+      <c r="M185" s="85"/>
       <c r="N185" s="62">
         <v>1</v>
       </c>
@@ -7869,6 +7937,7 @@
       <c r="J186" s="62"/>
       <c r="K186" s="62"/>
       <c r="L186" s="62"/>
+      <c r="M186" s="85"/>
       <c r="N186" s="62"/>
       <c r="O186" s="62"/>
       <c r="P186" s="62"/>
@@ -7894,6 +7963,7 @@
       <c r="J187" s="62"/>
       <c r="K187" s="62"/>
       <c r="L187" s="62"/>
+      <c r="M187" s="85"/>
       <c r="N187" s="62"/>
       <c r="O187" s="62"/>
       <c r="P187" s="62"/>
@@ -7921,6 +7991,7 @@
       <c r="J188" s="62"/>
       <c r="K188" s="62"/>
       <c r="L188" s="62"/>
+      <c r="M188" s="85"/>
       <c r="N188" s="62">
         <v>1</v>
       </c>
@@ -7939,7 +8010,7 @@
         <v>3</v>
       </c>
       <c r="C189" s="21" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D189" s="59"/>
       <c r="E189" s="59"/>
@@ -7950,6 +8021,7 @@
       <c r="J189" s="62"/>
       <c r="K189" s="62"/>
       <c r="L189" s="62"/>
+      <c r="M189" s="85"/>
       <c r="N189" s="62"/>
       <c r="O189" s="62"/>
       <c r="P189" s="62"/>
@@ -7975,6 +8047,7 @@
       <c r="J190" s="62"/>
       <c r="K190" s="62"/>
       <c r="L190" s="62"/>
+      <c r="M190" s="85"/>
       <c r="N190" s="62">
         <v>1</v>
       </c>
@@ -8002,7 +8075,7 @@
       <c r="J191" s="60"/>
       <c r="K191" s="60"/>
       <c r="L191" s="60"/>
-      <c r="M191" s="61"/>
+      <c r="M191" s="86"/>
       <c r="N191" s="60">
         <v>1</v>
       </c>
@@ -8011,7 +8084,7 @@
       <c r="Q191" s="60"/>
       <c r="R191" s="60"/>
       <c r="S191" s="68" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="192" spans="1:19" x14ac:dyDescent="0.2">
@@ -8033,6 +8106,7 @@
       <c r="J192" s="62"/>
       <c r="K192" s="62"/>
       <c r="L192" s="62"/>
+      <c r="M192" s="85"/>
       <c r="N192" s="62"/>
       <c r="O192" s="62"/>
       <c r="P192" s="62"/>
@@ -8040,29 +8114,33 @@
       <c r="R192" s="62"/>
     </row>
     <row r="193" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A193" s="19" t="s">
+      <c r="A193" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="B193" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C193" s="21" t="s">
+      <c r="B193" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="C193" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="D193" s="59"/>
-      <c r="E193" s="59"/>
-      <c r="F193" s="59"/>
-      <c r="G193" s="62"/>
-      <c r="H193" s="62"/>
-      <c r="I193" s="62"/>
-      <c r="J193" s="62"/>
-      <c r="K193" s="62"/>
-      <c r="L193" s="62"/>
-      <c r="N193" s="62"/>
-      <c r="O193" s="62"/>
-      <c r="P193" s="62"/>
-      <c r="Q193" s="62"/>
-      <c r="R193" s="62"/>
+      <c r="D193" s="44"/>
+      <c r="E193" s="44"/>
+      <c r="F193" s="44"/>
+      <c r="G193" s="60"/>
+      <c r="H193" s="60"/>
+      <c r="I193" s="60"/>
+      <c r="J193" s="60"/>
+      <c r="K193" s="60"/>
+      <c r="L193" s="60"/>
+      <c r="M193" s="86"/>
+      <c r="N193" s="60"/>
+      <c r="O193" s="60"/>
+      <c r="P193" s="60"/>
+      <c r="Q193" s="60"/>
+      <c r="R193" s="60"/>
+      <c r="S193" s="88" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="194" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A194" s="19" t="s">
@@ -8097,7 +8175,7 @@
         <v>3</v>
       </c>
       <c r="C195" s="15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D195" s="59"/>
       <c r="E195" s="59"/>
@@ -8153,7 +8231,7 @@
         <v>3</v>
       </c>
       <c r="C197" s="15" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D197" s="59"/>
       <c r="E197" s="59"/>
@@ -8323,7 +8401,7 @@
         <v>1</v>
       </c>
       <c r="S202" s="68" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="203" spans="1:19" x14ac:dyDescent="0.2">
@@ -8414,7 +8492,7 @@
         <v>3</v>
       </c>
       <c r="C206" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D206" s="59"/>
       <c r="E206" s="59"/>
@@ -8440,7 +8518,7 @@
         <v>48</v>
       </c>
       <c r="C207" s="50" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D207" s="44"/>
       <c r="E207" s="44"/>
@@ -8464,7 +8542,7 @@
         <v>1</v>
       </c>
       <c r="S207" s="76" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="208" spans="1:19" x14ac:dyDescent="0.2">
@@ -8511,7 +8589,7 @@
         <v>3</v>
       </c>
       <c r="C209" s="15" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D209" s="59"/>
       <c r="E209" s="59"/>
@@ -8565,7 +8643,7 @@
         <v>3</v>
       </c>
       <c r="C211" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D211" s="59"/>
       <c r="E211" s="59"/>
@@ -8591,7 +8669,7 @@
         <v>48</v>
       </c>
       <c r="C212" s="15" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D212" s="59"/>
       <c r="E212" s="59"/>
@@ -8665,7 +8743,7 @@
         <v>48</v>
       </c>
       <c r="C214" s="50" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D214" s="44"/>
       <c r="E214" s="44"/>
@@ -8684,8 +8762,8 @@
       <c r="P214" s="60"/>
       <c r="Q214" s="60"/>
       <c r="R214" s="60"/>
-      <c r="S214" s="80" t="s">
-        <v>456</v>
+      <c r="S214" s="77" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="215" spans="1:19" x14ac:dyDescent="0.2">
@@ -8696,7 +8774,7 @@
         <v>48</v>
       </c>
       <c r="C215" s="50" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D215" s="44"/>
       <c r="E215" s="44"/>
@@ -8715,8 +8793,8 @@
       <c r="P215" s="60"/>
       <c r="Q215" s="60"/>
       <c r="R215" s="60"/>
-      <c r="S215" s="80" t="s">
-        <v>456</v>
+      <c r="S215" s="77" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="216" spans="1:19" x14ac:dyDescent="0.2">
@@ -8746,8 +8824,8 @@
       <c r="P216" s="60"/>
       <c r="Q216" s="60"/>
       <c r="R216" s="60"/>
-      <c r="S216" s="80" t="s">
-        <v>456</v>
+      <c r="S216" s="77" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="217" spans="1:19" x14ac:dyDescent="0.2">
@@ -8782,7 +8860,7 @@
       </c>
       <c r="B218" s="14"/>
       <c r="C218" s="15" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D218" s="59"/>
       <c r="E218" s="59"/>
@@ -8878,7 +8956,7 @@
         <v>48</v>
       </c>
       <c r="C221" s="15" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D221" s="59"/>
       <c r="E221" s="59"/>
@@ -8908,7 +8986,7 @@
         <v>48</v>
       </c>
       <c r="C222" s="15" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D222" s="59"/>
       <c r="E222" s="59"/>
@@ -8934,7 +9012,7 @@
         <v>48</v>
       </c>
       <c r="C223" s="15" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D223" s="59"/>
       <c r="E223" s="59"/>
@@ -8960,7 +9038,7 @@
         <v>48</v>
       </c>
       <c r="C224" s="15" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D224" s="59"/>
       <c r="E224" s="59"/>
@@ -8986,7 +9064,7 @@
         <v>48</v>
       </c>
       <c r="C225" s="15" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D225" s="59"/>
       <c r="E225" s="59"/>
@@ -9012,7 +9090,7 @@
         <v>48</v>
       </c>
       <c r="C226" s="15" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D226" s="59"/>
       <c r="E226" s="59"/>
@@ -9394,7 +9472,7 @@
         <v>48</v>
       </c>
       <c r="C239" s="15" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D239" s="59"/>
       <c r="E239" s="59"/>
@@ -9438,7 +9516,7 @@
       <c r="Q240" s="62"/>
       <c r="R240" s="62"/>
     </row>
-    <row r="241" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A241" s="13" t="s">
         <v>208</v>
       </c>
@@ -9466,7 +9544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A242" s="13" t="s">
         <v>208</v>
       </c>
@@ -9494,7 +9572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A243" s="13" t="s">
         <v>208</v>
       </c>
@@ -9522,7 +9600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A244" s="13" t="s">
         <v>208</v>
       </c>
@@ -9548,7 +9626,7 @@
       <c r="Q244" s="62"/>
       <c r="R244" s="62"/>
     </row>
-    <row r="245" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A245" s="13" t="s">
         <v>208</v>
       </c>
@@ -9576,7 +9654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="246" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A246" s="13" t="s">
         <v>208</v>
       </c>
@@ -9602,7 +9680,7 @@
       <c r="Q246" s="62"/>
       <c r="R246" s="62"/>
     </row>
-    <row r="247" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A247" s="13" t="s">
         <v>208</v>
       </c>
@@ -9628,7 +9706,7 @@
       <c r="Q247" s="62"/>
       <c r="R247" s="62"/>
     </row>
-    <row r="248" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A248" s="13" t="s">
         <v>208</v>
       </c>
@@ -9666,7 +9744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A249" s="13" t="s">
         <v>208</v>
       </c>
@@ -9674,7 +9752,7 @@
         <v>48</v>
       </c>
       <c r="C249" s="15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D249" s="59"/>
       <c r="E249" s="59"/>
@@ -9691,8 +9769,9 @@
       <c r="P249" s="62"/>
       <c r="Q249" s="62"/>
       <c r="R249" s="62"/>
-    </row>
-    <row r="250" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S249" s="85"/>
+    </row>
+    <row r="250" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A250" s="13" t="s">
         <v>208</v>
       </c>
@@ -9730,7 +9809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A251" s="13" t="s">
         <v>208</v>
       </c>
@@ -9756,7 +9835,7 @@
       <c r="Q251" s="62"/>
       <c r="R251" s="62"/>
     </row>
-    <row r="252" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A252" s="13" t="s">
         <v>208</v>
       </c>
@@ -9794,7 +9873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A253" s="23" t="s">
         <v>30</v>
       </c>
@@ -9802,7 +9881,7 @@
         <v>3</v>
       </c>
       <c r="C253" s="25" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D253" s="59"/>
       <c r="E253" s="59"/>
@@ -9827,7 +9906,7 @@
       <c r="Q253" s="62"/>
       <c r="R253" s="62"/>
     </row>
-    <row r="254" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A254" s="23" t="s">
         <v>30</v>
       </c>
@@ -9852,7 +9931,7 @@
       <c r="Q254" s="62"/>
       <c r="R254" s="62"/>
     </row>
-    <row r="255" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A255" s="23" t="s">
         <v>30</v>
       </c>
@@ -9886,7 +9965,7 @@
       <c r="Q255" s="62"/>
       <c r="R255" s="62"/>
     </row>
-    <row r="256" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A256" s="23" t="s">
         <v>30</v>
       </c>
@@ -9986,7 +10065,7 @@
         <v>3</v>
       </c>
       <c r="C258" s="25" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D258" s="59"/>
       <c r="E258" s="59"/>
@@ -10270,6 +10349,7 @@
       <c r="J266" s="62"/>
       <c r="K266" s="62"/>
       <c r="L266" s="62"/>
+      <c r="M266" s="85"/>
       <c r="N266" s="62"/>
       <c r="O266" s="62"/>
       <c r="P266" s="62"/>
@@ -10301,6 +10381,7 @@
         <v>1</v>
       </c>
       <c r="L267" s="62"/>
+      <c r="M267" s="85"/>
       <c r="N267" s="62">
         <v>1</v>
       </c>
@@ -10317,7 +10398,7 @@
         <v>48</v>
       </c>
       <c r="C268" s="25" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D268" s="59"/>
       <c r="E268" s="59"/>
@@ -10332,6 +10413,7 @@
       <c r="L268" s="62">
         <v>1</v>
       </c>
+      <c r="M268" s="85"/>
       <c r="N268" s="62">
         <v>1</v>
       </c>
@@ -10365,6 +10447,7 @@
         <v>1</v>
       </c>
       <c r="L269" s="62"/>
+      <c r="M269" s="85"/>
       <c r="N269" s="62">
         <v>1</v>
       </c>
@@ -10432,7 +10515,7 @@
       <c r="Q271" s="60"/>
       <c r="R271" s="60"/>
       <c r="S271" s="68" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="272" spans="1:19" s="45" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -10465,7 +10548,7 @@
       <c r="Q272" s="60"/>
       <c r="R272" s="60"/>
       <c r="S272" s="68" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="273" spans="1:18" x14ac:dyDescent="0.2">
@@ -11225,7 +11308,7 @@
         <v>3</v>
       </c>
       <c r="C299" s="25" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D299" s="59"/>
       <c r="E299" s="59"/>
@@ -11292,7 +11375,7 @@
         <v>3</v>
       </c>
       <c r="C301" s="25" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D301" s="59"/>
       <c r="E301" s="59"/>
@@ -11692,6 +11775,7 @@
       <c r="J316" s="62"/>
       <c r="K316" s="62"/>
       <c r="L316" s="62"/>
+      <c r="M316" s="85"/>
       <c r="N316" s="62"/>
       <c r="O316" s="62"/>
       <c r="P316" s="62"/>
@@ -11719,7 +11803,7 @@
       <c r="J317" s="62"/>
       <c r="K317" s="62"/>
       <c r="L317" s="62"/>
-      <c r="M317" s="68">
+      <c r="M317" s="85">
         <v>1</v>
       </c>
       <c r="N317" s="62">
@@ -11913,7 +11997,7 @@
         <v>3</v>
       </c>
       <c r="C325" s="15" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D325" s="59"/>
       <c r="E325" s="59"/>
@@ -11979,7 +12063,7 @@
         <v>3</v>
       </c>
       <c r="C327" s="15" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D327" s="59"/>
       <c r="E327" s="59"/>
@@ -12020,7 +12104,7 @@
       <c r="Q328" s="60"/>
       <c r="R328" s="60"/>
       <c r="S328" s="68" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="329" spans="1:19" x14ac:dyDescent="0.2">
@@ -12031,7 +12115,7 @@
         <v>3</v>
       </c>
       <c r="C329" s="15" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D329" s="59"/>
       <c r="E329" s="59"/>
@@ -12125,7 +12209,7 @@
         <v>3</v>
       </c>
       <c r="C332" s="41" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D332" s="59"/>
       <c r="E332" s="59"/>
@@ -12161,6 +12245,7 @@
       <c r="J333" s="62"/>
       <c r="K333" s="62"/>
       <c r="L333" s="62"/>
+      <c r="M333" s="85"/>
       <c r="N333" s="62"/>
       <c r="O333" s="62"/>
       <c r="P333" s="62"/>
@@ -12184,6 +12269,7 @@
       <c r="J334" s="62"/>
       <c r="K334" s="62"/>
       <c r="L334" s="62"/>
+      <c r="M334" s="85"/>
       <c r="N334" s="62"/>
       <c r="O334" s="62"/>
       <c r="P334" s="62"/>
@@ -12213,6 +12299,7 @@
       <c r="J335" s="62"/>
       <c r="K335" s="62"/>
       <c r="L335" s="62"/>
+      <c r="M335" s="85"/>
       <c r="N335" s="62">
         <v>1</v>
       </c>
@@ -12240,6 +12327,7 @@
       <c r="J336" s="62"/>
       <c r="K336" s="62"/>
       <c r="L336" s="62"/>
+      <c r="M336" s="85"/>
       <c r="N336" s="62"/>
       <c r="O336" s="62"/>
       <c r="P336" s="62"/>
@@ -12265,6 +12353,7 @@
       <c r="J337" s="62"/>
       <c r="K337" s="62"/>
       <c r="L337" s="62"/>
+      <c r="M337" s="85"/>
       <c r="N337" s="62"/>
       <c r="O337" s="62"/>
       <c r="P337" s="62"/>
@@ -12279,7 +12368,7 @@
         <v>3</v>
       </c>
       <c r="C338" s="15" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D338" s="59"/>
       <c r="E338" s="59"/>
@@ -12423,7 +12512,7 @@
       <c r="Q342" s="60"/>
       <c r="R342" s="60"/>
       <c r="S342" s="68" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="343" spans="1:19" x14ac:dyDescent="0.2">
@@ -12485,7 +12574,7 @@
       <c r="R344" s="62"/>
     </row>
     <row r="345" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A345" s="84" t="s">
+      <c r="A345" s="80" t="s">
         <v>154</v>
       </c>
       <c r="B345" s="51" t="s">
@@ -12511,8 +12600,8 @@
         <v>1</v>
       </c>
       <c r="R345" s="60"/>
-      <c r="S345" s="80" t="s">
-        <v>456</v>
+      <c r="S345" s="77" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="346" spans="1:19" x14ac:dyDescent="0.2">
@@ -12944,7 +13033,7 @@
         <v>3</v>
       </c>
       <c r="C359" s="18" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D359" s="59"/>
       <c r="E359" s="59"/>
@@ -13019,7 +13108,7 @@
         <v>48</v>
       </c>
       <c r="C361" s="18" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D361" s="59"/>
       <c r="E361" s="59"/>
@@ -13807,7 +13896,7 @@
       <c r="L385" s="62">
         <v>1</v>
       </c>
-      <c r="M385" s="68">
+      <c r="M385" s="85">
         <v>1</v>
       </c>
       <c r="N385" s="62">
@@ -13830,7 +13919,7 @@
         <v>3</v>
       </c>
       <c r="C386" s="32" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D386" s="59"/>
       <c r="E386" s="59"/>
@@ -13841,6 +13930,7 @@
       <c r="J386" s="62"/>
       <c r="K386" s="62"/>
       <c r="L386" s="62"/>
+      <c r="M386" s="85"/>
       <c r="N386" s="62"/>
       <c r="O386" s="62"/>
       <c r="P386" s="62"/>
@@ -13874,7 +13964,7 @@
       <c r="L387" s="62">
         <v>1</v>
       </c>
-      <c r="M387" s="68">
+      <c r="M387" s="85">
         <v>1</v>
       </c>
       <c r="N387" s="62">
@@ -13930,7 +14020,7 @@
         <v>3</v>
       </c>
       <c r="C389" s="32" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D389" s="59"/>
       <c r="E389" s="59"/>
@@ -14092,7 +14182,7 @@
         <v>3</v>
       </c>
       <c r="C394" s="40" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D394" s="59"/>
       <c r="E394" s="59"/>
@@ -14163,7 +14253,7 @@
         <v>3</v>
       </c>
       <c r="C396" s="32" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D396" s="59"/>
       <c r="E396" s="59"/>
@@ -14188,7 +14278,7 @@
         <v>48</v>
       </c>
       <c r="C397" s="32" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D397" s="59"/>
       <c r="E397" s="59"/>
@@ -14846,63 +14936,71 @@
       <c r="C416" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="G416" s="68">
-        <v>1</v>
-      </c>
-      <c r="I416" s="68">
-        <v>1</v>
-      </c>
-      <c r="K416" s="68">
-        <v>1</v>
-      </c>
+      <c r="D416" s="84"/>
+      <c r="E416" s="84"/>
+      <c r="F416" s="84"/>
+      <c r="G416" s="85">
+        <v>1</v>
+      </c>
+      <c r="H416" s="85"/>
+      <c r="I416" s="85">
+        <v>1</v>
+      </c>
+      <c r="J416" s="85"/>
+      <c r="K416" s="85">
+        <v>1</v>
+      </c>
+      <c r="L416" s="85"/>
       <c r="M416" s="68">
         <v>1</v>
       </c>
-      <c r="N416" s="68">
-        <v>1</v>
-      </c>
-      <c r="O416" s="68">
-        <v>1</v>
-      </c>
-      <c r="Q416" s="68">
-        <v>1</v>
-      </c>
+      <c r="N416" s="85">
+        <v>1</v>
+      </c>
+      <c r="O416" s="85">
+        <v>1</v>
+      </c>
+      <c r="P416" s="85"/>
+      <c r="Q416" s="85">
+        <v>1</v>
+      </c>
+      <c r="R416" s="85"/>
     </row>
     <row r="417" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A417" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="B417" s="81" t="s">
-        <v>3</v>
-      </c>
-      <c r="C417" s="82" t="s">
+      <c r="B417" s="78" t="s">
+        <v>3</v>
+      </c>
+      <c r="C417" s="79" t="s">
         <v>285</v>
       </c>
-      <c r="D417" s="83"/>
-      <c r="E417" s="83"/>
-      <c r="F417" s="83"/>
-      <c r="G417" s="61"/>
-      <c r="H417" s="61"/>
-      <c r="I417" s="61">
-        <v>1</v>
-      </c>
-      <c r="J417" s="61"/>
-      <c r="K417" s="61"/>
-      <c r="L417" s="61"/>
+      <c r="D417" s="87"/>
+      <c r="E417" s="87"/>
+      <c r="F417" s="87"/>
+      <c r="G417" s="86"/>
+      <c r="H417" s="86"/>
+      <c r="I417" s="86">
+        <v>1</v>
+      </c>
+      <c r="J417" s="86"/>
+      <c r="K417" s="86"/>
+      <c r="L417" s="86"/>
       <c r="M417" s="61"/>
-      <c r="N417" s="61">
-        <v>1</v>
-      </c>
-      <c r="O417" s="61">
-        <v>1</v>
-      </c>
-      <c r="P417" s="61"/>
-      <c r="Q417" s="61">
-        <v>1</v>
-      </c>
-      <c r="R417" s="61"/>
-      <c r="S417" s="80" t="s">
-        <v>456</v>
+      <c r="N417" s="86">
+        <v>1</v>
+      </c>
+      <c r="O417" s="86">
+        <v>1</v>
+      </c>
+      <c r="P417" s="86"/>
+      <c r="Q417" s="86">
+        <v>1</v>
+      </c>
+      <c r="R417" s="86"/>
+      <c r="S417" s="77" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="418" spans="1:19" x14ac:dyDescent="0.2">
@@ -14915,18 +15013,28 @@
       <c r="C418" s="35" t="s">
         <v>284</v>
       </c>
-      <c r="I418" s="68">
-        <v>1</v>
-      </c>
-      <c r="N418" s="68">
-        <v>1</v>
-      </c>
-      <c r="O418" s="68">
-        <v>1</v>
-      </c>
-      <c r="Q418" s="68">
-        <v>1</v>
-      </c>
+      <c r="D418" s="84"/>
+      <c r="E418" s="84"/>
+      <c r="F418" s="84"/>
+      <c r="G418" s="85"/>
+      <c r="H418" s="85"/>
+      <c r="I418" s="85">
+        <v>1</v>
+      </c>
+      <c r="J418" s="85"/>
+      <c r="K418" s="85"/>
+      <c r="L418" s="85"/>
+      <c r="N418" s="85">
+        <v>1</v>
+      </c>
+      <c r="O418" s="85">
+        <v>1</v>
+      </c>
+      <c r="P418" s="85"/>
+      <c r="Q418" s="85">
+        <v>1</v>
+      </c>
+      <c r="R418" s="85"/>
     </row>
     <row r="419" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A419" s="19" t="s">
@@ -14938,18 +15046,28 @@
       <c r="C419" s="35" t="s">
         <v>283</v>
       </c>
-      <c r="I419" s="68">
-        <v>1</v>
-      </c>
-      <c r="N419" s="68">
-        <v>1</v>
-      </c>
-      <c r="O419" s="68">
-        <v>1</v>
-      </c>
-      <c r="Q419" s="68">
-        <v>1</v>
-      </c>
+      <c r="D419" s="84"/>
+      <c r="E419" s="84"/>
+      <c r="F419" s="84"/>
+      <c r="G419" s="85"/>
+      <c r="H419" s="85"/>
+      <c r="I419" s="85">
+        <v>1</v>
+      </c>
+      <c r="J419" s="85"/>
+      <c r="K419" s="85"/>
+      <c r="L419" s="85"/>
+      <c r="N419" s="85">
+        <v>1</v>
+      </c>
+      <c r="O419" s="85">
+        <v>1</v>
+      </c>
+      <c r="P419" s="85"/>
+      <c r="Q419" s="85">
+        <v>1</v>
+      </c>
+      <c r="R419" s="85"/>
     </row>
     <row r="420" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A420" s="19" t="s">
@@ -14961,18 +15079,28 @@
       <c r="C420" s="35" t="s">
         <v>286</v>
       </c>
-      <c r="I420" s="68">
-        <v>1</v>
-      </c>
-      <c r="N420" s="68">
-        <v>1</v>
-      </c>
-      <c r="O420" s="68">
-        <v>1</v>
-      </c>
-      <c r="Q420" s="68">
-        <v>1</v>
-      </c>
+      <c r="D420" s="84"/>
+      <c r="E420" s="84"/>
+      <c r="F420" s="84"/>
+      <c r="G420" s="85"/>
+      <c r="H420" s="85"/>
+      <c r="I420" s="85">
+        <v>1</v>
+      </c>
+      <c r="J420" s="85"/>
+      <c r="K420" s="85"/>
+      <c r="L420" s="85"/>
+      <c r="N420" s="85">
+        <v>1</v>
+      </c>
+      <c r="O420" s="85">
+        <v>1</v>
+      </c>
+      <c r="P420" s="85"/>
+      <c r="Q420" s="85">
+        <v>1</v>
+      </c>
+      <c r="R420" s="85"/>
     </row>
     <row r="421" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A421" s="19" t="s">
@@ -14984,18 +15112,28 @@
       <c r="C421" s="35" t="s">
         <v>287</v>
       </c>
-      <c r="I421" s="68">
-        <v>1</v>
-      </c>
-      <c r="N421" s="68">
-        <v>1</v>
-      </c>
-      <c r="O421" s="68">
-        <v>1</v>
-      </c>
-      <c r="Q421" s="68">
-        <v>1</v>
-      </c>
+      <c r="D421" s="84"/>
+      <c r="E421" s="84"/>
+      <c r="F421" s="84"/>
+      <c r="G421" s="85"/>
+      <c r="H421" s="85"/>
+      <c r="I421" s="85">
+        <v>1</v>
+      </c>
+      <c r="J421" s="85"/>
+      <c r="K421" s="85"/>
+      <c r="L421" s="85"/>
+      <c r="N421" s="85">
+        <v>1</v>
+      </c>
+      <c r="O421" s="85">
+        <v>1</v>
+      </c>
+      <c r="P421" s="85"/>
+      <c r="Q421" s="85">
+        <v>1</v>
+      </c>
+      <c r="R421" s="85"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:S421" xr:uid="{F00D01EA-5C3E-F64B-8B7F-2EE6141A689A}">
@@ -15056,7 +15194,7 @@
     <hyperlink ref="C185" r:id="rId46" display="https://aws.amazon.com/iot-events/" xr:uid="{09A17074-F045-D045-99F3-289DE651CC4B}"/>
     <hyperlink ref="C188" r:id="rId47" display="https://aws.amazon.com/greengrass/" xr:uid="{86C6B532-C282-AD49-84FC-E7151CC17562}"/>
     <hyperlink ref="C385" r:id="rId48" display="https://aws.amazon.com/kms/" xr:uid="{C0A6E0DF-7D93-854D-AF8E-5B9C19B8AF02}"/>
-    <hyperlink ref="C25" r:id="rId49" display="https://aws.amazon.com/lake-formation/" xr:uid="{8B1B5135-7A0D-7645-A701-475DDEBCFDA0}"/>
+    <hyperlink ref="C26" r:id="rId49" display="https://aws.amazon.com/lake-formation/" xr:uid="{8B1B5135-7A0D-7645-A701-475DDEBCFDA0}"/>
     <hyperlink ref="C67" r:id="rId50" display="https://aws.amazon.com/lambda/" xr:uid="{23B44498-C148-BD4C-86FE-EFAA00464E5B}"/>
     <hyperlink ref="C267" r:id="rId51" display="https://aws.amazon.com/license-manager/" xr:uid="{A80531A2-32DF-5E46-A8A2-AD514A9E876E}"/>
     <hyperlink ref="C110" r:id="rId52" display="https://aws.amazon.com/mp/" xr:uid="{83E81132-B5F9-A141-93D4-67826C5C6C2F}"/>
@@ -15128,7 +15266,7 @@
     <hyperlink ref="C384" r:id="rId118" display="https://aws.amazon.com/inspector/" xr:uid="{176BE9A8-3FF5-874F-8EFA-6BB4665C2F33}"/>
     <hyperlink ref="C124" r:id="rId119" display="https://aws.amazon.com/keyspaces/" xr:uid="{08537BC8-9E18-E341-B811-B357F4073FF5}"/>
     <hyperlink ref="C6" r:id="rId120" display="https://aws.amazon.com/kinesis/firehose/" xr:uid="{AB91BD64-7EBD-8A40-89D5-415AC999E5A7}"/>
-    <hyperlink ref="C24" r:id="rId121" display="https://aws.amazon.com/kinesis/streams/" xr:uid="{683B50F9-C9B3-9046-A380-EAD32C0551EC}"/>
+    <hyperlink ref="C25" r:id="rId121" display="https://aws.amazon.com/kinesis/streams/" xr:uid="{683B50F9-C9B3-9046-A380-EAD32C0551EC}"/>
     <hyperlink ref="C317" r:id="rId122" display="https://aws.amazon.com/kinesis/video-streams/" xr:uid="{92727233-FF93-4048-90C3-EB7CFF6B76A0}"/>
     <hyperlink ref="C68" r:id="rId123" display="https://amazonlightsail.com/" xr:uid="{5C26023E-C913-634E-BBA9-96985AD232E5}"/>
     <hyperlink ref="C170" r:id="rId124" display="https://aws.amazon.com/location" xr:uid="{3A5DA1F4-704B-4A4F-B42A-0132FA3F769F}"/>
@@ -15136,7 +15274,7 @@
     <hyperlink ref="C174" r:id="rId126" display="https://aws.amazon.com/lumberyard/" xr:uid="{0793FA7F-F861-E448-B351-2625AB793E29}"/>
     <hyperlink ref="C44" r:id="rId127" display="https://aws.amazon.com/amazon-mq/" xr:uid="{8F7E8190-F83B-7E45-9B55-465E1F7C79F3}"/>
     <hyperlink ref="C387" r:id="rId128" display="https://aws.amazon.com/macie/" xr:uid="{0A9A9C7B-64FF-4944-8B73-82D7A54412E2}"/>
-    <hyperlink ref="C27" r:id="rId129" display="https://aws.amazon.com/msk/" xr:uid="{46024F01-6B35-0740-B92F-18BA0D596F3D}"/>
+    <hyperlink ref="C28" r:id="rId129" display="https://aws.amazon.com/msk/" xr:uid="{46024F01-6B35-0740-B92F-18BA0D596F3D}"/>
     <hyperlink ref="C43" r:id="rId130" display="https://aws.amazon.com/managed-workflows-for-apache-airflow/" xr:uid="{E7D50CE9-B395-AE40-B3BD-7B31072C139C}"/>
     <hyperlink ref="C126" r:id="rId131" display="https://aws.amazon.com/neptune/" xr:uid="{35EB7CA9-2F10-7E4E-9B05-D1C561AFFA79}"/>
     <hyperlink ref="C219" r:id="rId132" display="https://aws.amazon.com/personalize/" xr:uid="{F1130D50-7EEE-8441-87AC-E48D5971C615}"/>
@@ -15361,7 +15499,7 @@
     <hyperlink ref="C96" r:id="rId351" xr:uid="{7477CB6A-F100-A34F-9008-B1BFB9967DA7}"/>
     <hyperlink ref="C357" r:id="rId352" xr:uid="{6AD92B4E-E0EB-1848-9442-69AFE2F3AE78}"/>
     <hyperlink ref="C17" r:id="rId353" xr:uid="{DF438ACC-C4F5-974D-96FC-A4F4FBD4D563}"/>
-    <hyperlink ref="C28" r:id="rId354" xr:uid="{567A6139-66F6-6E46-9546-8DDB94DE141F}"/>
+    <hyperlink ref="C24" r:id="rId354" display="Omics" xr:uid="{567A6139-66F6-6E46-9546-8DDB94DE141F}"/>
     <hyperlink ref="C57" r:id="rId355" xr:uid="{07941932-04CA-D14D-B516-833FCD650A67}"/>
     <hyperlink ref="C75" r:id="rId356" xr:uid="{438F4E0F-2656-3B4B-A75B-4361FF393940}"/>
     <hyperlink ref="C8" r:id="rId357" xr:uid="{3E5A0494-CA0B-014F-A243-AE4E024917C7}"/>
@@ -15401,7 +15539,7 @@
     <hyperlink ref="C209" r:id="rId391" xr:uid="{249561E9-79C6-BE48-97B5-47088052E20C}"/>
     <hyperlink ref="C132" r:id="rId392" display="https://aws.amazon.com/rds/" xr:uid="{52A384FE-5551-524F-8BE4-640C39EE59DB}"/>
     <hyperlink ref="C131" r:id="rId393" xr:uid="{C5C6C16C-2F05-5E43-A2AF-4B98DE5A08E2}"/>
-    <hyperlink ref="C26" r:id="rId394" display="Managed Service for Apache Flink" xr:uid="{3625922C-DB21-0444-B197-BA1C214B3BA9}"/>
+    <hyperlink ref="C27" r:id="rId394" display="Managed Service for Apache Flink" xr:uid="{3625922C-DB21-0444-B197-BA1C214B3BA9}"/>
     <hyperlink ref="C41" r:id="rId395" xr:uid="{47FA5F44-63ED-424F-8D67-3714160DBB93}"/>
     <hyperlink ref="C40" r:id="rId396" xr:uid="{E2FEFEBC-91F9-5243-A78E-89686A16F4AD}"/>
     <hyperlink ref="C42" r:id="rId397" xr:uid="{9AB559D5-E489-5645-8518-4F5B8DF3BBEF}"/>
@@ -15469,35 +15607,35 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="26" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="81" t="s">
         <v>320</v>
       </c>
-      <c r="B4" s="77"/>
+      <c r="B4" s="81"/>
     </row>
     <row r="5" spans="1:2" s="7" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="78" t="s">
+      <c r="A5" s="82" t="s">
         <v>319</v>
       </c>
-      <c r="B5" s="78"/>
+      <c r="B5" s="82"/>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="83" t="s">
         <v>318</v>
       </c>
-      <c r="B6" s="79"/>
+      <c r="B6" s="83"/>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="83" t="s">
         <v>317</v>
       </c>
-      <c r="B7" s="79"/>
+      <c r="B7" s="83"/>
     </row>
     <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="s">
+        <v>398</v>
+      </c>
+      <c r="B17" s="37" t="s">
         <v>399</v>
-      </c>
-      <c r="B17" s="37" t="s">
-        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>